<commit_message>
restructured code to use get_key_variables utility function
</commit_message>
<xml_diff>
--- a/docs/data-cleaning-requests/divest.xlsx
+++ b/docs/data-cleaning-requests/divest.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J214"/>
+  <dimension ref="A1:L214"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -412,7 +412,17 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>university</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>article_text</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>description_has_divest</t>
         </is>
       </c>
     </row>
@@ -453,10 +463,13 @@
           <t>University governance, admin, policies, programs, curriculum, Labor and work</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>After waiting for two years, Seattle University adjunct faculty were officially granted the right to unionize on Sept. 12. The National Labor Relations Board approved a long- standing petition to allow adjunct faculty to join the Service Employees International Union, making Seattle U one of just a few private Jesuit universities in the country to permit this change.&lt;br/&gt;Students and faculty march for unionization in April 2016.&lt;br/&gt;Students and faculty alike who were present to experience the swells of passion around the movement, including an organized walk-out protest in Feb. 2015, rejoice in this news in the hopes that it will mean positive changes both inside the classroom and within the Seattle U community.&lt;br/&gt;"I think it is a very good change. I think that adjunct professors should feel secure in their positions," said Wendall Tseng, a student and member of the Reignite the Mission club on campus. "And without giving adjunct equal benefits, I feel there is less incentive as a professor to build a community of the best curriculum. I do not see a valid instance in which this [unionization] shouldn't be allowed."&lt;br/&gt;The union has yet to begin its collective bargaining process, which includes negotiations between faculty and administrators. A unit will be formed by elected adjunct members who will work to alleviate issues within the non-tenure experience regarding wages, hours, work conditions and benefits. From there, they will work with Seattle U administrators to decide on regulations and legislation to protect these workers.&lt;br/&gt;All adjunct faculty will be subject to these future changes, with the exception of faculty working within departments of religion and theology, who are not permitted to unionize due to a rule regarding the separation of church and state.&lt;br/&gt;The road to unionization was not without its bumps, and resistance from some faculty and administrators halted the vote for over two years.&lt;br/&gt;The university argued that because it has increased minimum full-time faculty salaries over the past several years-from $24,600 to $45,000-a union would not be necessary in addressing faculty concerns.&lt;br/&gt;In 2014, University President Fr. Stephen Sundborg, S.J. released a video addressed to adjunct faculty strongly encouraging them to vote against the right to unionize. The video has since been removed from the university's website.&lt;br/&gt;In the video, Sundborg implied that the right to unionize would go against the university's mission statement, and stated it would be "nearly impossible" to work with faculty if they had to go through the Service Employees International. Some faculty felt differently about this point, including Emily Lieb, an assistant professor within the Matteo Ricci College.&lt;br/&gt;"Nothing is more consistent with the Jesuit mission of this university than having an organized faculty that is treated fairly and ethically and committed to their jobs," Lieb said.&lt;br/&gt;Sundborg went on to describe how happy students seem to be with their adjunct professors, and that student satisfaction should warrant not granting adjunct members the right to unionize. But as former Seattle U adjunct professor Larry Cushnie pointed out, there are several of aspects of teaching that go unseen to the average college student. Cushnie left Seattle U in 2015, and currently teaches at the University of Washington and Bellevue College.&lt;br/&gt;"I talked to other instructors, who even while they were teaching, were eligible for things like food stamps and public assistance," Cushnie said.&lt;br/&gt;The university's argument against unionization also referenced Catholic Social Teaching, a doctrine created by the Catholic Church that dictates the church's feelings and thoughts on the role of church and state, social organization and other forms of social justice. While some cited these teachings to support the campaign against unionization, Catholic social teaching explicitly allows and promotes the right to organize.&lt;br/&gt;But ultimately, the commitment of several faculty members and students to ignite a common governance for all hired adjuncts was able to win out over the university's defense.&lt;br/&gt;The union will specifically allow adjunct faculty to have a greater voice and role in the university's politics. For instance, they hope to have a larger say in how departments are run. Cushnie explained that when important, school-wide decisions on education are allocated to those who do not have the expertise to make those decisions, it can create dissonance between departments and how they function.&lt;br/&gt;"Decisions were being made to do things like cancel or nix some of the departments on campus...and then also adding new programs even as the university was experiencing budget problems, in terms of all- around education, and no one had a say about it-adjuncts especially," Cushnie said.&lt;br/&gt;Proponents of unionization have agreed that one of the most important reasons for unionization is the impact it can have on job security.&lt;br/&gt;"Being tenured, you have a lot of academic freedom as far as your curriculum because there is no fear of being chopped off the faculty line," Tseng said. "And in that way, job stability really helps you create the best kind of classroom because you can really have the most freedom to teach what you really want to teach, and really give students the best environment."&lt;br/&gt;A lack of job security in the past has greatly impacted the well-being of some Seattle U adjunct professors. Audrey Hudgins, a clinical instructor for the Matteo Ricci College, recounted having a class cancelled a week before it was meant to start.&lt;br/&gt;"You do a bunch of work you don't get compensated for, and then you don't get a check when your rent is due," Hudgins said.&lt;br/&gt;Lieb also emphasized the negative impacts this kind of last-minute planning can have.&lt;br/&gt;"The issue has been historically that people who are just teaching one class or two classes, there is no notice if they are going to cancel your class so you can show up the day before school starts and find you are not teaching," Lieb said.&lt;br/&gt;Creating equality of treatment where equality already exists is also a huge point of this movement.&lt;br/&gt;"In my view, there is no difference," Hudgins said. "There is the same level of academic training, the same credentials, the same disciplinary expertise, the same commitment to student success."&lt;br/&gt;With this new union, situations in which adjunct faculty have been given less rights and benefits as their tenured counterparts will hopefully be avoided to maintain the livelihood of all faculty, as well as that of the students they teach.&lt;br/&gt;Perhaps the demographic this change will affect the most are the students. Students are what make Seattle University the prestigious Jesuit college it is today. This of course could not have been achieved without the instruction and guidance of Seattle University professors. Cushnie illustrated the urgency of this system of checks and balances at Seattle U.&lt;br/&gt;"Universities in the last couple decades started organizing themselves in much more of a corporate-based structure. And you see this at SU; the hiring administration has skyrocketed and tenure track faculty have declined," Cushnie said. "If a tenure leaves for one reason or another...they tend to hire two to three adjuncts to make up for that since it is so much cheaper."&lt;br/&gt;At its core, the lack of unionization was taking its toll on the classroom experience.&lt;br/&gt;"At Seattle University my students were going into mass amounts of debt, and had no chance to form relationships with the adjuncts that were teaching the majority of their classes because they [the adjunct] had no idea if they would even be there the next quarter," Cushnie said.&lt;br/&gt;With the support of clubs campus-wide and a passion for justice brought forth by both students and faculty, some practices within university administration can now be halted and renegotiated to better fit the adjuncts being impacted.&lt;br/&gt;"If you want a healthy, Jesuit, social justice university, just look at the middle of campus, look at what types of protests and what students are involved in," Cushnie said.&lt;br/&gt;Students are the biggest supporters and drivers of social change on campus. Whether they're tackling issues of divestment or organizing occupations to take a stand against racism within their curriculum, Seattle U students continue every day to trailblaze and improve themselves, their campus and their community. This drive can be attributed to all the professors who have guided and educated students to profound bravery to stand up to their own university.&lt;br/&gt;Seattle U's character can be defined by its mission statement, and for many, unionization is just one step closer to a more just and humane world.&lt;br/&gt;The author may be reached at</t>
         </is>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -501,10 +514,13 @@
           <t>Anti-racism</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>Ada Throckmorton&lt;br/&gt;Staff Writer&lt;br/&gt;By: Ada Throckmorton | Staff Writer&lt;br/&gt;A group of local alumni joined the sit-in on Thursday and marched to the Alumni Center to say that they would not donate if the University continues to invest in fossil fuels.(McKENZIE LYNCH/The Stanford Daily)&lt;br/&gt;At the site of the Fossil Free Stanford sit-in outside the president and provost's office, wakeup times are staggered as the sun rises. Some participants, in tents, sleep longer. Others, in sleeping bags under the Main Quad arcades, begin to wake earlier. Most begin to pull out laptops, starting their work for the day.&lt;br/&gt;When most of the sit-in protesters are awake, Yari Greanley '15 M.S.'16 gathers the group for their morning meeting. In a typical day, the participants meet all together twice - once in the morning and once in the evening. Sitting in a circle on the quad, they share announcements, discuss their emotions as the sit-in continues and conclude each meeting in song.&lt;br/&gt;Greanley herself has been with FFS since its conception three years ago. An earth systems undergraduate and coterminal student, Greanley has experienced the impacts of climate change firsthand with widespread forest fires and lowering reservoir levels near her home in Redding, California. For Greanley, these experiences have reinforced the need for urgency in climate action - something FFS doesn't feel the Stanford administration has taken into account.&lt;br/&gt;"Toward the end of last year, we were realizing that the University might not follow through on its commitment to act quickly," Greanley said. "When our mentor at 350.org asked if we would be interested in escalating to nonviolent direct action, we began to plan."&lt;br/&gt;As the sit-in has progressed, Greanley said the conflict between University administration and the Stanford community has become more apparent as the community has shown "overwhelming support" over the past week of the sit-in.&lt;br/&gt;There are common activities from day to day of the sit-in: homework, teach-ins, film screenings, music, art. Food is brought in from co-ops or just friends of the participants. One alumnus brought hot chocolate to warm up protesters late Wednesday night, and on Thursday afternoon more alumni walked up carrying pizzas.&lt;br/&gt;Many of the amenities brought to the protesters are offered to the police standing watch at the door to Building 10 as well. Most of the time, the officers decline the offers of coffee or granola bars, but the relationship between the officers and the sit-in participants is a comfortable one.&lt;br/&gt;Chris LeBoa '19, a freshman who heard about FFS during Admit Weekend last year, has been particularly interactive with the police.&lt;br/&gt;"The police officers are there because they have to be, but they have a lot of stories too," LeBoa said. "Carol, who's working now, actually lived on a boat... Chris, the guy in the morning, is a surfer who lives in the Santa Cruz mountains. Israel wakes up at 4 a.m. to get his kids ready for school."&lt;br/&gt;According to LeBoa, the main "sacrifice" he has made to the sit-in is that his parents haven't been supportive of the idea. They've told him that they didn't intend to raise an activist.&lt;br/&gt;"But for the first time, I'm not just doing what I'm told but doing what I think is right," LeBoa said.&lt;br/&gt;Students as well as protestors, the sit-in participants are frequently doing work to try and minimize the academic "sacrifice." For some, this means getting a little distance (sitting 50 yards away from the main campsite) and getting some reading done. For others, this means pulling out a whiteboard and forming a Computation and Mathematics Engineering 100 study group.&lt;br/&gt;Some of the participants hardly leave the site, while others continue to attend classes and other functions.&lt;br/&gt;According to Zhanpei Fang '19, an intended physics major who joined the sit-in because she felt powerless as a student in the "Stanford bubble" and saw the sit-in as having real cultural impact, the sit-in has been calm enough to get homework done. Nonetheless, she hasn't stayed on-site at all times.&lt;br/&gt;"I have been going to classes because I don't want to fail," Fang said. "And I went back to my dorm once to shower."&lt;br/&gt;In addition to individual studying, some of the teach-ins have taken the form of classes that either relocated to the site of the sit-in or classes that allowed students to attend via Skype in order to not miss out on learning opportunities.&lt;br/&gt;Sijo Smith '18, who Skyped into Earth Systems 112 with seven other classmates from outside Building 10, indicated that many professors have been very accommodating of students participating in the sit-in.&lt;br/&gt;"It's been great working with professors who have allowed students to make up classes one way or the other," Smith said.&lt;br/&gt;Throughout the day, work and learning tends to be broken up by musical interludes. On Wednesday alone, the sit-in was visited by Occupella, a Bay Area pacifist music group; the Stanford Collaborative Orchestra; and the University Singers.&lt;br/&gt;Much of the music, however, is more impromptu. Walking through the arcades, songs are hummed under students' breath. One student pulls out a ukulele, and a group surrounding her breaks into an impromptu cover of Vance Joy's "Riptide."&lt;br/&gt;The most frequent instances of music, however, have been the songs of the protest itself. With simple songs about building power and expressing confidence in this power to effect change, the students sing both at meetings and at various other times during the week, such as when Smith presented FFS's response letter to the administration's warning letter.&lt;br/&gt;Smith, who has been a member of FFS since her freshman year, said she came to the sit-in with a strong group of friends, but also with people she didn't know as well or had never met.&lt;br/&gt;In fact, participants in the sit-in have differing levels of connection to Fossil Free Stanford and the rest of the environmental community at the University. Fang, for instance, decided to come to the event after reading about it on several email lists, but she didn't know anyone doing it particularly well.&lt;br/&gt;"I have had my friends visit me though," Fang said. "They've been very supportive of the cause."&lt;br/&gt;FFS organizers have also encouraged participants to attend other activist events on campus. On Tuesday, this meant a rally in the courtyard of Old Union to uplift Muslim and Arab voices in the wake of Islamophobia following the Paris attacks. On Wednesday, this meant a #StudentBlackout rally in White Plaza to stand in solidarity with students protesting racism at campuses across the country such as Mizzou, Yale, Claremont McKenna and all other educational spaces where discrimination occurs.&lt;br/&gt;While the fossil fuel divestment movement is not directly about these racial discrimination issues, the global environmental justice implications of fossil fuels is heavily emphasized in the FFS campaign.&lt;br/&gt;Gabriela Leslie '15 M.S.'17 was one of the people that led the charge on an art project underscoring the way that the fossil fuel industry has impacted communities across the globe. The project was a large trifold structure placed first off the main quad facing the oval, then moved back to the site of the sit-in after being notified by the University that it would otherwise be taken down by workers.&lt;br/&gt;The idea of the work, according to Leslie, is to "shine a spotlight on the high profile cases of global communities that have been directly affected by the negligence of the fossil fuel industry." The piece specifically features stories from the Chevron oil spill in Ecuador, the threat of sea level rise in Tuvalu and the drought in California, among others.&lt;br/&gt;"The two main criteria that institutions typically ask when deciding to divest is [one,] whether the product creates substantial societal harm and two, whether there are alternatives to the product or service readily available," Leslie said. "We wanted to tackle this first question in particular."&lt;br/&gt;"[The project] really brings the moral issue to the absolute forefront in a place where the University can't turn a blind eye," she added.&lt;br/&gt;Other actions have included the response letter presented back to the administration and an op-ed written by Andrea Martinez '15 M.S. '15 in response to an article published in The Stanford Review.&lt;br/&gt;For the protesters, the work and the music and the visitors are all just part of the now natural sit-in routine. The final shakeup of this routine, however, may come when the group has a rally on Friday at 11 a.m. and a tentative public meeting with President John Hennessy at an undetermined time on Friday. While FFS organizers have met with Hennessy in the past, this will be the first time it will occur in a public setting.&lt;br/&gt;Going into Friday, Greanley emphasizes the importance of attitude of the group.&lt;br/&gt;In the words of Greanley, the students intend to show Hennessy just how "passionate and persistent, hopeful and determined" they are, as they once again make their case for fossil fuel divestment.&lt;br/&gt;Editor's note: Ada Throckmorton is an embedded reporter at the sit-in.&lt;br/&gt;Contact Ada Throckmorton at adastat 'at' stanford.edu.</t>
         </is>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -544,10 +560,13 @@
           <t>Anti-racism, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>Ada Throckmorton&lt;br/&gt;Staff Writer&lt;br/&gt;By: Ada Throckmorton | Staff Writer&lt;br/&gt;A group of local alumni joined the sit-in on Thursday and marched to the Alumni Center to say that they would not donate if the University continues to invest in fossil fuels.(McKENZIE LYNCH/The Stanford Daily)&lt;br/&gt;At the site of the Fossil Free Stanford sit-in outside the president and provost's office, wakeup times are staggered as the sun rises. Some participants, in tents, sleep longer. Others, in sleeping bags under the Main Quad arcades, begin to wake earlier. Most begin to pull out laptops, starting their work for the day.&lt;br/&gt;When most of the sit-in protesters are awake, Yari Greanley '15 M.S.'16 gathers the group for their morning meeting. In a typical day, the participants meet all together twice - once in the morning and once in the evening. Sitting in a circle on the quad, they share announcements, discuss their emotions as the sit-in continues and conclude each meeting in song.&lt;br/&gt;Greanley herself has been with FFS since its conception three years ago. An earth systems undergraduate and coterminal student, Greanley has experienced the impacts of climate change firsthand with widespread forest fires and lowering reservoir levels near her home in Redding, California. For Greanley, these experiences have reinforced the need for urgency in climate action - something FFS doesn't feel the Stanford administration has taken into account.&lt;br/&gt;"Toward the end of last year, we were realizing that the University might not follow through on its commitment to act quickly," Greanley said. "When our mentor at 350.org asked if we would be interested in escalating to nonviolent direct action, we began to plan."&lt;br/&gt;As the sit-in has progressed, Greanley said the conflict between University administration and the Stanford community has become more apparent as the community has shown "overwhelming support" over the past week of the sit-in.&lt;br/&gt;There are common activities from day to day of the sit-in: homework, teach-ins, film screenings, music, art. Food is brought in from co-ops or just friends of the participants. One alumnus brought hot chocolate to warm up protesters late Wednesday night, and on Thursday afternoon more alumni walked up carrying pizzas.&lt;br/&gt;Many of the amenities brought to the protesters are offered to the police standing watch at the door to Building 10 as well. Most of the time, the officers decline the offers of coffee or granola bars, but the relationship between the officers and the sit-in participants is a comfortable one.&lt;br/&gt;Chris LeBoa '19, a freshman who heard about FFS during Admit Weekend last year, has been particularly interactive with the police.&lt;br/&gt;"The police officers are there because they have to be, but they have a lot of stories too," LeBoa said. "Carol, who's working now, actually lived on a boat... Chris, the guy in the morning, is a surfer who lives in the Santa Cruz mountains. Israel wakes up at 4 a.m. to get his kids ready for school."&lt;br/&gt;According to LeBoa, the main "sacrifice" he has made to the sit-in is that his parents haven't been supportive of the idea. They've told him that they didn't intend to raise an activist.&lt;br/&gt;"But for the first time, I'm not just doing what I'm told but doing what I think is right," LeBoa said.&lt;br/&gt;Students as well as protestors, the sit-in participants are frequently doing work to try and minimize the academic "sacrifice." For some, this means getting a little distance (sitting 50 yards away from the main campsite) and getting some reading done. For others, this means pulling out a whiteboard and forming a Computation and Mathematics Engineering 100 study group.&lt;br/&gt;Some of the participants hardly leave the site, while others continue to attend classes and other functions.&lt;br/&gt;According to Zhanpei Fang '19, an intended physics major who joined the sit-in because she felt powerless as a student in the "Stanford bubble" and saw the sit-in as having real cultural impact, the sit-in has been calm enough to get homework done. Nonetheless, she hasn't stayed on-site at all times.&lt;br/&gt;"I have been going to classes because I don't want to fail," Fang said. "And I went back to my dorm once to shower."&lt;br/&gt;In addition to individual studying, some of the teach-ins have taken the form of classes that either relocated to the site of the sit-in or classes that allowed students to attend via Skype in order to not miss out on learning opportunities.&lt;br/&gt;Sijo Smith '18, who Skyped into Earth Systems 112 with seven other classmates from outside Building 10, indicated that many professors have been very accommodating of students participating in the sit-in.&lt;br/&gt;"It's been great working with professors who have allowed students to make up classes one way or the other," Smith said.&lt;br/&gt;Throughout the day, work and learning tends to be broken up by musical interludes. On Wednesday alone, the sit-in was visited by Occupella, a Bay Area pacifist music group; the Stanford Collaborative Orchestra; and the University Singers.&lt;br/&gt;Much of the music, however, is more impromptu. Walking through the arcades, songs are hummed under students' breath. One student pulls out a ukulele, and a group surrounding her breaks into an impromptu cover of Vance Joy's "Riptide."&lt;br/&gt;The most frequent instances of music, however, have been the songs of the protest itself. With simple songs about building power and expressing confidence in this power to effect change, the students sing both at meetings and at various other times during the week, such as when Smith presented FFS's response letter to the administration's warning letter.&lt;br/&gt;Smith, who has been a member of FFS since her freshman year, said she came to the sit-in with a strong group of friends, but also with people she didn't know as well or had never met.&lt;br/&gt;In fact, participants in the sit-in have differing levels of connection to Fossil Free Stanford and the rest of the environmental community at the University. Fang, for instance, decided to come to the event after reading about it on several email lists, but she didn't know anyone doing it particularly well.&lt;br/&gt;"I have had my friends visit me though," Fang said. "They've been very supportive of the cause."&lt;br/&gt;FFS organizers have also encouraged participants to attend other activist events on campus. On Tuesday, this meant a rally in the courtyard of Old Union to uplift Muslim and Arab voices in the wake of Islamophobia following the Paris attacks. On Wednesday, this meant a #StudentBlackout rally in White Plaza to stand in solidarity with students protesting racism at campuses across the country such as Mizzou, Yale, Claremont McKenna and all other educational spaces where discrimination occurs.&lt;br/&gt;While the fossil fuel divestment movement is not directly about these racial discrimination issues, the global environmental justice implications of fossil fuels is heavily emphasized in the FFS campaign.&lt;br/&gt;Gabriela Leslie '15 M.S.'17 was one of the people that led the charge on an art project underscoring the way that the fossil fuel industry has impacted communities across the globe. The project was a large trifold structure placed first off the main quad facing the oval, then moved back to the site of the sit-in after being notified by the University that it would otherwise be taken down by workers.&lt;br/&gt;The idea of the work, according to Leslie, is to "shine a spotlight on the high profile cases of global communities that have been directly affected by the negligence of the fossil fuel industry." The piece specifically features stories from the Chevron oil spill in Ecuador, the threat of sea level rise in Tuvalu and the drought in California, among others.&lt;br/&gt;"The two main criteria that institutions typically ask when deciding to divest is [one,] whether the product creates substantial societal harm and two, whether there are alternatives to the product or service readily available," Leslie said. "We wanted to tackle this first question in particular."&lt;br/&gt;"[The project] really brings the moral issue to the absolute forefront in a place where the University can't turn a blind eye," she added.&lt;br/&gt;Other actions have included the response letter presented back to the administration and an op-ed written by Andrea Martinez '15 M.S. '15 in response to an article published in The Stanford Review.&lt;br/&gt;For the protesters, the work and the music and the visitors are all just part of the now natural sit-in routine. The final shakeup of this routine, however, may come when the group has a rally on Friday at 11 a.m. and a tentative public meeting with President John Hennessy at an undetermined time on Friday. While FFS organizers have met with Hennessy in the past, this will be the first time it will occur in a public setting.&lt;br/&gt;Going into Friday, Greanley emphasizes the importance of attitude of the group.&lt;br/&gt;In the words of Greanley, the students intend to show Hennessy just how "passionate and persistent, hopeful and determined" they are, as they once again make their case for fossil fuel divestment.&lt;br/&gt;Editor's note: Ada Throckmorton is an embedded reporter at the sit-in.&lt;br/&gt;Contact Ada Throckmorton at adastat 'at' stanford.edu.</t>
         </is>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -588,10 +607,13 @@
           <t>University governance, admin, policies, programs, curriculum, Anti-racism, Campus climate, Racist/racialized symbols</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>ShareTweetSharePrintPhoto by Yuhkai Lin |The ChronicleThe recent protests on campus have not occurred in isolation.Across the country, college students have been protesting about issues ranging from minority representation to budget transparency. Students in North Carolina have focused their efforts on the recently-passed House Bill 2, which resicted access to restrooms based on "biological sex" and repealed local non-discrimination ordinances.North Carolina responseMany students at University of North Carolina schools have expressed disappointment with new UNC System President Margaret Spellings' decision to comply with the law.Students from several UNC schools gathered at a Board of Governors meeting Friday to show their opposition to Spellings' decision. They also expressed complaints that the BOG has reduced funding for historically black colleges and universities, according to an article in The Daily Tar Heel last Friday. Some student leaders, however, noted that Spelling has promised to take some steps to counteract the law and that UNC schools will not change their anti-discrimination policies. "Despite the intentions and perceived hate promoted by this bill, I believe President Spellings is taking calculated action to ensure that the UNC system continues to become an ever more welcoming place for all," wrote Houston Summers, the former UNC-Chapel Hill student body president, in an email.&lt;br/&gt;"There is much to be done even in the face of adversity."However, students and advocacy groups-including the American Civil Liberties Union of North Carolina, Equality North Carolina and Lambda Legal-criticized Spellings' decision, arguing that House Bill 2 violates federal law by discriminating against ansgender individuals. Appalachian State Student Power, a student advocacy group, occupied the BB Dougherty administration building from April 8 to 13. The group left after a statement from Chancellor Sheri Everts condemned the bill, meeting the group's major demand, according to an article in the Asheville Citizen-Times April 13. Duke has called for a repeal of the law in a statement issued by President Richard Brodhead, Provost Sally Kornbluth and Chancellor for Health Affairs Dr. A. Eugene Washington Monday. The law has created problems for the University, said Michael Schoenfeld, vice president for public affairs and government relations. "There are a growing number of scholars from public universities in states that have a specific ban on travel to North Carolina who have not been able to attend conferences and meetings at Duke," he explained. "I'm aware of at least two national conferences that were supposed to take place at Duke that are now reconsidering their decision."Schoenfeld said that several parents and students have also reached out to express concern. "Those who are interested in and care about Duke recognize that Duke didn't create this problem and that both Duke and Durham are places that place a high premium on diversity, inclusion and tolerance for all communities," he said.Protests around the nationStudents attending the University of California-Davis occupied their campus administration building for five weeks to demand the resignation of Chancellor Linda P.B. Katehi for a lack of responsiveness to students. They also called her prior service on the board of DeVry Education Group, which is now under federal investigation, a conflict of interest, according to The Sacramento Bee. Although they left the building April 15, students said they plan to look for other ways to force Katehi's removal. At Clemson University, five students-known by the hashtag "Clemson5"-were arrested and charged with espassing for occupying Sikes Hall, a main administration building, last week. The sit-in began after a series of racist incidents on campus, including the discovery of bananas hanging from a sign celebrating Clemson's African-American history, according to an article in The Atlantic last Friday. The students then began occupying the steps to the building and have reiterated demands for increased minority inclusion, which they initially issued in January. Earlier this month, students at Ohio State University attempted to stage a sit-in of Bricker Hall, an administrative building, but ultimately disbanded after they were threatened with arrest and expulsion by campus administrators, said Caitlin Pitt, an OSU senior who was not involved with the sit-in. The students had issued a list of demands calling for budget transparency and requesting administrators to either divest from companies involved in human rights abuses, refuse to outsource employees or provide more sustainable food options. Since leaving the building, the protestors have continued their activism by hosting teach-ins and have gained support from faculty and alumni, Pitt said. Pitt noted that he thinks students at OSU know about the protests at Duke."We've been very aware, and we stand in solidarity with you guys," he said.Carbon divestment campaign heats upOther groups are demanding their universities divest from fossil fuels.At New York University, students ended a 33-hour occupation of an elevator leading to administrative offices Tuesday. They claimed the administration failed to live up to its earlier promises to divest, according to an article in the Washington Square News Tuesday. Students at Columbia University have occupied Low Library, which houses administrative offices, since Thursday and plan to do so until their president makes a statement in support of divestment. The protestors noted that their actions are situated within a larger history."Our first thought wasn't just to sit-in," junior Cristian Padilla, who is occupying the building, said. "This is a campaign that has been going on for three and a half years at this point."Senior Jennifer Tang, another occupier, said she hopes the action can have a broader impact. "Asking a university to divest its funds is mostly a symbolic act, but when taken as a collective movement across campuses and around the world it does add up to a lot of actual money that can then hopefully be invested elsewhere," she said. Presidential candidate Bernie Sanders showed solidarity with the movement from his Twitter account Monday with the hashtag "keepitintheground." Let us stand in solidarity with the students at Columbia and NYU for demanding their schools divest from fossil fuels. #KeepItInTheGroundConnections to DukeDuke Students and Workers in Solidarity, the organization that led the occupation of the Allen Building, has backed several of the student movements across the country. Anastasia Karklina, Trinity '14, a Ph.D. student in literature and African and African-American studies and a media liaison for DSWS, noted that social media has helped connect students across campuses. "I cannot speak to any direct actions sparking elsewhere in direct response to our sit-in, since I'm not aware of any," she said. "I do think, however, that seeing a growing student movement spreading across campuses has been a source of inspiration and moral support for many, myself included."Karklina noted that DSWS has received messages from activists at the University of Texas at Austin, Washington University in St. Louis, Harvard University and Appalachian State University. The connections provide a support system for protestors, she said. "It seems to me that there is a common understanding-between student organizers across campuses-about the kind of emotional, psychological and physical weight this work carries for many of us," Karklina explained.</t>
         </is>
+      </c>
+      <c r="L5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -636,10 +658,13 @@
           <t>University governance, admin, policies, programs, curriculum, Anti-racism</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>Ohio University students joined campuses nationwide Thursday as part of the Million Student March, where students came together for the Rally for Campus Democracy.&lt;br/&gt;More than 80 people attended the event hosted by the OU Student Union, including members of student groups BLAC, Sierra Student Coalition, OU's NAACP chapter and Bobcats for Bernie Sanders.&lt;br/&gt;The rally began at the top of Baker Center, and went down Morton Hill before stopping at the amphitheater in front of the four new residence halls on South Green.&lt;br/&gt;The mission of the Million Student March, a national movement for college students, includes three demands: tuition-free public college, cancellation of all student debt and a $15 minimum wage for all campus workers. But the march was not limited to those topics of discussion, as protesters brought up issues including racial inequality, divestment from fossil fuels and prisons, "real food" and sexual assault on campus.&lt;br/&gt;NAACP members Jasmyn Pearl and Mateo Dillard spoke about disadvantages students of color face.&lt;br/&gt;"It wasn't until 1954 ... that our parents and grandparents were allowed to sit at a desk next to white people," Dillard, a freshman studying business pre-law, said.&lt;br/&gt;Pearl, a freshman studying journalism, cited an article from Forbes stating that white households have 16 times more wealth than black households, adding that a small percentage of scholarships nationwide are exclusively for black students.&lt;br/&gt;"Without (scholarships) being increased, the struggle for equal education for blacks will never change," Pearl said.&lt;br/&gt;Julie White, associate professor of women's, gender and sexuality studies, spoke about professors' salaries at OU.&lt;br/&gt;"You need to think about how much you're paying for that class, and how little of it is going to your instructors," White said.&lt;br/&gt;OU students Rachel Komich and Daniel Kington talked about the Real Food Challenge, a national campaign advocating for improved food on college campuses.&lt;br/&gt;"It's basically just an allocation of power," Komich, a junior studying English, said. "McDavis has to sign the commitment, but the students do all the work."&lt;br/&gt;The challenge aims to have 20 percent "real food" in college dining halls, including OU's, by 2020.&lt;br/&gt;"It's not only a reallocation of our resources into a real food economy, it's a reallocation of our power to give it away from those with no vested interest and place it in the hands of students and community members." Kington, a Post columnist and sophomore studying English, said.&lt;br/&gt;Graduate Student Senate President Carl Edward Smith III spoke about graduate student worker wages, adding that graduate students want to be able to opt out of part of OU's general fee. Smith said he met with President Roderick McDavis Thursday morning about general fee concerns.&lt;br/&gt;"President McDavis ... told the room full of impoverished graduate students that the graduate students were focusing on the wrong issue and should instead make more use of general fee supported units and attend more football games," Smith said. "This sickens me. Football games don't buy food or medical insurance."&lt;br/&gt;Jazzmine Hardges, a sophomore studying communication studies, said more faculty members should have to take cultural competency courses.&lt;br/&gt;"If you're not going to be an African-American studies professor or if you're not a professor of something like that ... you don't have to take any kind of cultural sensitivity (classes)," she said.&lt;br/&gt;Will Klatt, an OU alumnus and employee of the union ASFME Council 8, said inequality is evident on OU's campus.&lt;br/&gt;"When there are corporate, unaccountable presidents, who refuse to listen to the demands of the students, they can get the boot," Klatt said.&lt;br/&gt;Bobby Walker, a junior studying women's, gender and sexuality studies, spoke on the importance of OU's divestment from prisons and said that the system of mass incarceration puts people of color at a disadvantage.&lt;br/&gt;"When you're in a class with 100 people and you only have five students of color ... it's not because black kids aren't smart. It's not because people of color can't get into colleges," she said. "It's because they're ... trapped in cages."&lt;br/&gt;Bobby Sunderhaus, a senior studying Latin American studies and environmental studies and a member of Sierra Student Coalition, spoke on the environmental effects of fossil fuels.&lt;br/&gt;"We are currently living in a time of climate chaos," he said, adding that SSC demands that OU publicly divest from fossil fuels within five years' time.&lt;br/&gt;No one has officially filed for the seat to be vacated by Rep. Debbie Phillips, D-Albany, at the end of her term in 2016.&lt;br/&gt;Rachel Baker, a sophomore studying social work and a member of F--kRapeCulture, spoke about problems with a campus climate survey OU plans to distribute.&lt;br/&gt;"It is a very valuable moment to ask the right questions about the problems students are facing on campus about racial harassment, sexual harassment, harassment based on gender identity and sexual orientation," Baker said. "The survey is designed in a way that they're not going to get any answers they don't like."&lt;br/&gt;Ryan Powers, a ·junior studying philosophy and a member of the OU Student Union, encouraged collective action among the group.&lt;br/&gt;"What it took to bring down (Missouri's) president was collective action," he said. "That's why we need to continue to organize ourselves. We have more power when we act together."&lt;br/&gt;@megankhenry&lt;br/&gt;mh573113@ohio.edu&lt;br/&gt;@taymaple&lt;br/&gt;tm255312@ohio.edu</t>
         </is>
+      </c>
+      <c r="L6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -684,10 +709,13 @@
           <t>Campus climate, Hate speech</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>Photo courtesy of SDSU&lt;br/&gt;Last Wednesday, several student activist groups protested San Diego State President Elliot Hirshman's response to posters displaying anti-Muslim sentiments posted around the school's campus. Student leaders specifically asked Hirshman for an apology regarding an email that, according to them, did not sufficiently address the posters, which identified specific SDSU students by name as Palestinian terrorists who perpetuate anti-Semitism.&lt;br/&gt;Hirshman's initial email response to the posters recognized the right to freedom of speech and the accountability that comes with taking political positions. Students were unsatisfied with this and took the opportunity to surround Hirshman in a police cruiser as he was leaving an event.&lt;br/&gt;They demanded an apology for the inadequate administrative response, to which Hirshman offered a formal meeting with those students who were named on the posters to discuss their concerns about the original email's lack of action.&lt;br/&gt;This past Monday, SDSU students and members of the Students for Justice in Palestine Osama Alkhawaja and Rachel Beck met with Hirshman in person to discuss the incident. Beck recalled the events of the meeting, emphasizing how Hirschman likened SJP's goals to that of a terrorist group's.&lt;br/&gt;"The president was saying [we appeared to be] 'allied' [with terrorists], because the fliers say that we're allied with terrorist groups," Beck told the UCSD Guardian. "He defines allied as 'a common cause or goal' and he said that terrorists have a common cause or goal with us and that goal is [Boycott, Divest and Sanction] ... because they support BDS, and because [we] support BDS, I guess that's how we're allied."&lt;br/&gt;An email was sent out to students yesterday regarding the discussion that occurred as a joint statement from both university representatives as well as student leaders, explaining the actions that will be taken.&lt;br/&gt;"Creating the appropriate balance between freedom of expression and protecting members of our community from harassment, as in the current case where students were named individually on a flyer posted on our campus, poses a significant challenge," the statement read. "The parties have agreed that in collaboration with A.S. and under the aegis of the University Senate, they will undertake a review of university policies to ensure we are balancing freedom of expression and protection from harassment.&lt;br/&gt;Beck expressed frustration with the administration's unsupportive response toward the severity of the situation, contrasting her own experience with that of her friends.&lt;br/&gt;"For me, my biggest concern is just the fact that when I Google my name, the first thing that immediately comes up are [things] that are calling me a terrorist ... If a prospective employer looks me up [and sees these websites], that's my biggest concern," Beck told the UCSD Guardian. "Most of the students are either Arab, Muslim or both, and a lot of them have been scared, whereas I'm white, European, not affiliated with any religion, so I don't fit the common racist perception of what a terrorist looks like. I'm not [personally] very scared, but I'm scared for them - it makes me mad that the president doesn't understand this very real fear that students have as a Muslim student on campus."&lt;br/&gt;The posters were created by the David Horwitz Center for Freedom whose mission is to "combat the efforts of the radical left and its Islamist allies to destroy American values and disarm this country as it attempts to defend itself in a time of terror" by focusing on college campus activism.&lt;br/&gt;The DHCF has made appearances at other campuses including UC Berkeley, UC Irvine and UCSD. In particular, UCSD's Young Americans for Freedom organization hosted Horowitz, a conservative Jewish author, in 2010 for a dialogue between Muslims and Jews.&lt;br/&gt;This Thursday evening Horowitz is slated to speak at an SDSU College Republicans event titled "David Horowitz on Fighting Anti-Semitism on College Campuses." According to the Facebook event, the SDSU Muslim Student Union is planning on holding a 100-person march on the day of the event, though Beck recently informed the Guardian that no protest would happen. The SDSU College Republicans have made the event open only to those who are on the guest list. SHARE Facebook Twitter tweet Rebecca Chong</t>
         </is>
+      </c>
+      <c r="L7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -727,10 +755,13 @@
           <t>Campus climate, Anti-racism, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>January 28, 2016 Filed under Columnists, OPINION&lt;br/&gt;Whitman has historically been an overwhelmingly white college. There is a lack of racial diversity on this campus and, as with all the race-related events occurring in the nation, the issue is becoming increasingly more pertinent. More people are realizing that it is wrong to acknowledge the problem but stand by in inaction. If Whitman continues to lack diversity, will it be able to sustain itself as an institution? The protests catalyzed by Whitman's lack of racial diversity seriously challenge the college's future.&lt;br/&gt;In these past several years at Whitman, there has been a steady increase in protests over racial and economic diversity. Divest Whitman organized demonstrations and put up signs and art installations last year to protest the removal of needs-blind admission. The mascot, constant micro-aggressions, cultural appropriation and racial profiling are race-related issues that have been increasingly protested this year as well. The struggles that Whitman minority students experience and the general non-responsiveness of the racial majority were brought up many times this November during the Mizzou protests. What worked about this protest at Whitman was its disruptive nature. There were 250 Whitman students in front of the library at 7:00p.m., blocking its entrance during one of its busiest times. This disruption and objection challenge the reputation of Whitman as a place of abundant happiness and down-to-earth perfection.&lt;br/&gt;The internet also can take disruption and threats to reputation to a whole new level. People can post videos of protests on websites such as YouTube or Facebook. There is at least one Whitman protest online right now located at https://www.youtube.com/watch?v=-vwx9LyWn2A. In this protest, the diversity club F.U.B.U. marched into President Bridges' office in December 2014. They reported an incident of a Latino student during Thanksgiving break being accused by a Whitman security officer of breaking into the French house even though he was living there. The president was dumbfounded, confused and unsure of what to do. The online depiction of this event at Whitman is very different from the way Whitman wants to depict itself - a safe place where all ethnicities and groups of people come together and study in a welcome environment. The internet gives protests more influence because when these videos get shared to countless pages, they easily reach prospective students, alumni and other groups, conveying a more realistic image of the school.&lt;br/&gt;The appropriation, isolation, racial profiling and micro-aggressions minority students deal with would decrease if this school was more racially varied. This is not the only solution but it is definitely a piece of the puzzle. As a result of the racial climate outside of Whitman and the amount of protest clubs that students as a whole have organized, we have more momentum than ever to persevere and continue to disrupt Whitman's reputation and catalyze a reexamination of the progressive identity of this campus. Whitman depends on its "unpretentious" reputation to attract new students and maintain a steady flow of alumni donations. Continuing to share protest videos online, as well as protesting in real time, will force Whitman to stop ignoring these disruptions and act like everything is okay. Because these protests will continue to affect the current and perspective students, faculty and the administration, something will eventually have to be done in order to alleviate these issues. Overall, this bad state of campus diversity is not sustainable and these disruptive protests will continue to be our main tool in pursuing change and threatening the facade of Whitman's reputation.</t>
         </is>
+      </c>
+      <c r="L8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -770,10 +801,13 @@
           <t>University governance, admin, policies, programs, curriculum, Anti-racism</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>January 28, 2016 Filed under Columnists, OPINION&lt;br/&gt;Whitman has historically been an overwhelmingly white college. There is a lack of racial diversity on this campus and, as with all the race-related events occurring in the nation, the issue is becoming increasingly more pertinent. More people are realizing that it is wrong to acknowledge the problem but stand by in inaction. If Whitman continues to lack diversity, will it be able to sustain itself as an institution? The protests catalyzed by Whitman's lack of racial diversity seriously challenge the college's future.&lt;br/&gt;In these past several years at Whitman, there has been a steady increase in protests over racial and economic diversity. Divest Whitman organized demonstrations and put up signs and art installations last year to protest the removal of needs-blind admission. The mascot, constant micro-aggressions, cultural appropriation and racial profiling are race-related issues that have been increasingly protested this year as well. The struggles that Whitman minority students experience and the general non-responsiveness of the racial majority were brought up many times this November during the Mizzou protests. What worked about this protest at Whitman was its disruptive nature. There were 250 Whitman students in front of the library at 7:00p.m., blocking its entrance during one of its busiest times. This disruption and objection challenge the reputation of Whitman as a place of abundant happiness and down-to-earth perfection.&lt;br/&gt;The internet also can take disruption and threats to reputation to a whole new level. People can post videos of protests on websites such as YouTube or Facebook. There is at least one Whitman protest online right now located at https://www.youtube.com/watch?v=-vwx9LyWn2A. In this protest, the diversity club F.U.B.U. marched into President Bridges' office in December 2014. They reported an incident of a Latino student during Thanksgiving break being accused by a Whitman security officer of breaking into the French house even though he was living there. The president was dumbfounded, confused and unsure of what to do. The online depiction of this event at Whitman is very different from the way Whitman wants to depict itself - a safe place where all ethnicities and groups of people come together and study in a welcome environment. The internet gives protests more influence because when these videos get shared to countless pages, they easily reach prospective students, alumni and other groups, conveying a more realistic image of the school.&lt;br/&gt;The appropriation, isolation, racial profiling and micro-aggressions minority students deal with would decrease if this school was more racially varied. This is not the only solution but it is definitely a piece of the puzzle. As a result of the racial climate outside of Whitman and the amount of protest clubs that students as a whole have organized, we have more momentum than ever to persevere and continue to disrupt Whitman's reputation and catalyze a reexamination of the progressive identity of this campus. Whitman depends on its "unpretentious" reputation to attract new students and maintain a steady flow of alumni donations. Continuing to share protest videos online, as well as protesting in real time, will force Whitman to stop ignoring these disruptions and act like everything is okay. Because these protests will continue to affect the current and perspective students, faculty and the administration, something will eventually have to be done in order to alleviate these issues. Overall, this bad state of campus diversity is not sustainable and these disruptive protests will continue to be our main tool in pursuing change and threatening the facade of Whitman's reputation.</t>
         </is>
+      </c>
+      <c r="L9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -818,10 +852,13 @@
           <t>Indigenous issues</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>The David Horowitz Freedom Center a conservative activist group, took responsibility Friday for posting fliers around the SF State campus that depicted a professor as a terrorist sympathizer, according to a press release issued by the center.  &lt;br/&gt;"Our goal in placing these posters on prominent campuses across America is to expose the true motivations and allegiances of these groups who have chosen to join forces with terrorists, to challenge their lies and to expose the financial and organizational supports which allow them to pursue their genocidal agenda," David Horowitz said in a press release.&lt;br/&gt;In a statement released today, SF State President Les Wong condemned the actions of those responsible for the posters, saying that "a line has been crossed."&lt;br/&gt;SF State has been the latest school in a group of California universities that has been targeted in the "Stop the Jew Hatred on Campus" poster campaign.  Other universities that were targeted were UC Berkeley, UCLA, San Diego State and UC Irvine.  &lt;br/&gt;One of the posters depicts an illustration of Rabab Ibrahim Abdulhadi, an associate professor in the ethnic studies program, with the statement next to it, "a leader of the Hamas BDS campaign; collaborator with terrorists; San Francisco State professor." BDS stands for the Boycott, Divestment and Sanctions movement, which calls for an international effort to put economic pressure on Israel for its treatments of Palestinians.   &lt;br/&gt;"Flyers were posted by an outside extremist group in numerous locations, singling out one of our faculty members, our students and vandalizing our campus,"  Wong said.  "We know that this group is not affiliated with San Francisco State University."&lt;br/&gt;Wong goes on to say that even though "we disagree on many issues, we must defend each other from personalized attacks that serve no purpose but to incite fear and promote division."&lt;br/&gt;In an article released by frontpagemag.com -- a website operated by the David Horowitz Freedom Center --  stated that "SF State has repeatedly enabled the most extreme actions of its General Union of Palestinian Students ." The article goes into describing recent SF State events involving GUPS, such as an April protest of the Jerusalem Mayor Nir Barkat, which led the University to implement a five-step protocol, after heavy scrutiny according to an article released by the Golden Gate Xpress.  &lt;br/&gt;SF State has been at the center of ongoing controversy involving Jewish and Palestinian relations, when a petition went out in September questioning the University's partnership with An-Najah National University.&lt;br/&gt;"Let me be clear, this is not an issue of free speech; this is bullying behavior that is unacceptable and will not be tolerated on our campus,"  Wong said.  &lt;br/&gt;Share this:&lt;br/&gt;EmailFacebookTwitterGoogleMoreRedditTumblrPinterestLinkedIn Tags:SF StateSFSU</t>
         </is>
+      </c>
+      <c r="L10" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -861,10 +898,13 @@
           <t>University governance, admin, policies, programs, curriculum, Transgender issues (For)</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>ShareTweetSharePrintPhoto by Yuhkai Lin |The ChronicleThe recent protests on campus have not occurred in isolation.Across the country, college students have been protesting about issues ranging from minority representation to budget transparency. Students in North Carolina have focused their efforts on the recently-passed House Bill 2, which resicted access to restrooms based on "biological sex" and repealed local non-discrimination ordinances.North Carolina responseMany students at University of North Carolina schools have expressed disappointment with new UNC System President Margaret Spellings' decision to comply with the law.Students from several UNC schools gathered at a Board of Governors meeting Friday to show their opposition to Spellings' decision. They also expressed complaints that the BOG has reduced funding for historically black colleges and universities, according to an article in The Daily Tar Heel last Friday. Some student leaders, however, noted that Spelling has promised to take some steps to counteract the law and that UNC schools will not change their anti-discrimination policies. "Despite the intentions and perceived hate promoted by this bill, I believe President Spellings is taking calculated action to ensure that the UNC system continues to become an ever more welcoming place for all," wrote Houston Summers, the former UNC-Chapel Hill student body president, in an email.&lt;br/&gt;"There is much to be done even in the face of adversity."However, students and advocacy groups-including the American Civil Liberties Union of North Carolina, Equality North Carolina and Lambda Legal-criticized Spellings' decision, arguing that House Bill 2 violates federal law by discriminating against ansgender individuals. Appalachian State Student Power, a student advocacy group, occupied the BB Dougherty administration building from April 8 to 13. The group left after a statement from Chancellor Sheri Everts condemned the bill, meeting the group's major demand, according to an article in the Asheville Citizen-Times April 13. Duke has called for a repeal of the law in a statement issued by President Richard Brodhead, Provost Sally Kornbluth and Chancellor for Health Affairs Dr. A. Eugene Washington Monday. The law has created problems for the University, said Michael Schoenfeld, vice president for public affairs and government relations. "There are a growing number of scholars from public universities in states that have a specific ban on travel to North Carolina who have not been able to attend conferences and meetings at Duke," he explained. "I'm aware of at least two national conferences that were supposed to take place at Duke that are now reconsidering their decision."Schoenfeld said that several parents and students have also reached out to express concern. "Those who are interested in and care about Duke recognize that Duke didn't create this problem and that both Duke and Durham are places that place a high premium on diversity, inclusion and tolerance for all communities," he said.Protests around the nationStudents attending the University of California-Davis occupied their campus administration building for five weeks to demand the resignation of Chancellor Linda P.B. Katehi for a lack of responsiveness to students. They also called her prior service on the board of DeVry Education Group, which is now under federal investigation, a conflict of interest, according to The Sacramento Bee. Although they left the building April 15, students said they plan to look for other ways to force Katehi's removal. At Clemson University, five students-known by the hashtag "Clemson5"-were arrested and charged with espassing for occupying Sikes Hall, a main administration building, last week. The sit-in began after a series of racist incidents on campus, including the discovery of bananas hanging from a sign celebrating Clemson's African-American history, according to an article in The Atlantic last Friday. The students then began occupying the steps to the building and have reiterated demands for increased minority inclusion, which they initially issued in January. Earlier this month, students at Ohio State University attempted to stage a sit-in of Bricker Hall, an administrative building, but ultimately disbanded after they were threatened with arrest and expulsion by campus administrators, said Caitlin Pitt, an OSU senior who was not involved with the sit-in. The students had issued a list of demands calling for budget transparency and requesting administrators to either divest from companies involved in human rights abuses, refuse to outsource employees or provide more sustainable food options. Since leaving the building, the protestors have continued their activism by hosting teach-ins and have gained support from faculty and alumni, Pitt said. Pitt noted that he thinks students at OSU know about the protests at Duke."We've been very aware, and we stand in solidarity with you guys," he said.Carbon divestment campaign heats upOther groups are demanding their universities divest from fossil fuels.At New York University, students ended a 33-hour occupation of an elevator leading to administrative offices Tuesday. They claimed the administration failed to live up to its earlier promises to divest, according to an article in the Washington Square News Tuesday. Students at Columbia University have occupied Low Library, which houses administrative offices, since Thursday and plan to do so until their president makes a statement in support of divestment. The protestors noted that their actions are situated within a larger history."Our first thought wasn't just to sit-in," junior Cristian Padilla, who is occupying the building, said. "This is a campaign that has been going on for three and a half years at this point."Senior Jennifer Tang, another occupier, said she hopes the action can have a broader impact. "Asking a university to divest its funds is mostly a symbolic act, but when taken as a collective movement across campuses and around the world it does add up to a lot of actual money that can then hopefully be invested elsewhere," she said. Presidential candidate Bernie Sanders showed solidarity with the movement from his Twitter account Monday with the hashtag "keepitintheground." Let us stand in solidarity with the students at Columbia and NYU for demanding their schools divest from fossil fuels. #KeepItInTheGroundConnections to DukeDuke Students and Workers in Solidarity, the organization that led the occupation of the Allen Building, has backed several of the student movements across the country. Anastasia Karklina, Trinity '14, a Ph.D. student in literature and African and African-American studies and a media liaison for DSWS, noted that social media has helped connect students across campuses. "I cannot speak to any direct actions sparking elsewhere in direct response to our sit-in, since I'm not aware of any," she said. "I do think, however, that seeing a growing student movement spreading across campuses has been a source of inspiration and moral support for many, myself included."Karklina noted that DSWS has received messages from activists at the University of Texas at Austin, Washington University in St. Louis, Harvard University and Appalachian State University. The connections provide a support system for protestors, she said. "It seems to me that there is a common understanding-between student organizers across campuses-about the kind of emotional, psychological and physical weight this work carries for many of us," Karklina explained.</t>
         </is>
+      </c>
+      <c r="L11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -909,10 +949,13 @@
           <t>Anti-racism</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>ShareTweetSharePrintPhoto by Yuhkai Lin |The ChronicleThe recent protests on campus have not occurred in isolation.Across the country, college students have been protesting about issues ranging from minority representation to budget transparency. Students in North Carolina have focused their efforts on the recently-passed House Bill 2, which resicted access to restrooms based on "biological sex" and repealed local non-discrimination ordinances.North Carolina responseMany students at University of North Carolina schools have expressed disappointment with new UNC System President Margaret Spellings' decision to comply with the law.Students from several UNC schools gathered at a Board of Governors meeting Friday to show their opposition to Spellings' decision. They also expressed complaints that the BOG has reduced funding for historically black colleges and universities, according to an article in The Daily Tar Heel last Friday. Some student leaders, however, noted that Spelling has promised to take some steps to counteract the law and that UNC schools will not change their anti-discrimination policies. "Despite the intentions and perceived hate promoted by this bill, I believe President Spellings is taking calculated action to ensure that the UNC system continues to become an ever more welcoming place for all," wrote Houston Summers, the former UNC-Chapel Hill student body president, in an email.&lt;br/&gt;"There is much to be done even in the face of adversity."However, students and advocacy groups-including the American Civil Liberties Union of North Carolina, Equality North Carolina and Lambda Legal-criticized Spellings' decision, arguing that House Bill 2 violates federal law by discriminating against ansgender individuals. Appalachian State Student Power, a student advocacy group, occupied the BB Dougherty administration building from April 8 to 13. The group left after a statement from Chancellor Sheri Everts condemned the bill, meeting the group's major demand, according to an article in the Asheville Citizen-Times April 13. Duke has called for a repeal of the law in a statement issued by President Richard Brodhead, Provost Sally Kornbluth and Chancellor for Health Affairs Dr. A. Eugene Washington Monday. The law has created problems for the University, said Michael Schoenfeld, vice president for public affairs and government relations. "There are a growing number of scholars from public universities in states that have a specific ban on travel to North Carolina who have not been able to attend conferences and meetings at Duke," he explained. "I'm aware of at least two national conferences that were supposed to take place at Duke that are now reconsidering their decision."Schoenfeld said that several parents and students have also reached out to express concern. "Those who are interested in and care about Duke recognize that Duke didn't create this problem and that both Duke and Durham are places that place a high premium on diversity, inclusion and tolerance for all communities," he said.Protests around the nationStudents attending the University of California-Davis occupied their campus administration building for five weeks to demand the resignation of Chancellor Linda P.B. Katehi for a lack of responsiveness to students. They also called her prior service on the board of DeVry Education Group, which is now under federal investigation, a conflict of interest, according to The Sacramento Bee. Although they left the building April 15, students said they plan to look for other ways to force Katehi's removal. At Clemson University, five students-known by the hashtag "Clemson5"-were arrested and charged with espassing for occupying Sikes Hall, a main administration building, last week. The sit-in began after a series of racist incidents on campus, including the discovery of bananas hanging from a sign celebrating Clemson's African-American history, according to an article in The Atlantic last Friday. The students then began occupying the steps to the building and have reiterated demands for increased minority inclusion, which they initially issued in January. Earlier this month, students at Ohio State University attempted to stage a sit-in of Bricker Hall, an administrative building, but ultimately disbanded after they were threatened with arrest and expulsion by campus administrators, said Caitlin Pitt, an OSU senior who was not involved with the sit-in. The students had issued a list of demands calling for budget transparency and requesting administrators to either divest from companies involved in human rights abuses, refuse to outsource employees or provide more sustainable food options. Since leaving the building, the protestors have continued their activism by hosting teach-ins and have gained support from faculty and alumni, Pitt said. Pitt noted that he thinks students at OSU know about the protests at Duke."We've been very aware, and we stand in solidarity with you guys," he said.Carbon divestment campaign heats upOther groups are demanding their universities divest from fossil fuels.At New York University, students ended a 33-hour occupation of an elevator leading to administrative offices Tuesday. They claimed the administration failed to live up to its earlier promises to divest, according to an article in the Washington Square News Tuesday. Students at Columbia University have occupied Low Library, which houses administrative offices, since Thursday and plan to do so until their president makes a statement in support of divestment. The protestors noted that their actions are situated within a larger history."Our first thought wasn't just to sit-in," junior Cristian Padilla, who is occupying the building, said. "This is a campaign that has been going on for three and a half years at this point."Senior Jennifer Tang, another occupier, said she hopes the action can have a broader impact. "Asking a university to divest its funds is mostly a symbolic act, but when taken as a collective movement across campuses and around the world it does add up to a lot of actual money that can then hopefully be invested elsewhere," she said. Presidential candidate Bernie Sanders showed solidarity with the movement from his Twitter account Monday with the hashtag "keepitintheground." Let us stand in solidarity with the students at Columbia and NYU for demanding their schools divest from fossil fuels. #KeepItInTheGroundConnections to DukeDuke Students and Workers in Solidarity, the organization that led the occupation of the Allen Building, has backed several of the student movements across the country. Anastasia Karklina, Trinity '14, a Ph.D. student in literature and African and African-American studies and a media liaison for DSWS, noted that social media has helped connect students across campuses. "I cannot speak to any direct actions sparking elsewhere in direct response to our sit-in, since I'm not aware of any," she said. "I do think, however, that seeing a growing student movement spreading across campuses has been a source of inspiration and moral support for many, myself included."Karklina noted that DSWS has received messages from activists at the University of Texas at Austin, Washington University in St. Louis, Harvard University and Appalachian State University. The connections provide a support system for protestors, she said. "It seems to me that there is a common understanding-between student organizers across campuses-about the kind of emotional, psychological and physical weight this work carries for many of us," Karklina explained.</t>
         </is>
+      </c>
+      <c r="L12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -952,10 +995,13 @@
           <t>Anti-racism, University governance, admin, policies, programs, curriculum, Campus climate</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>By ALEXA ESKENAZI&lt;br/&gt;Cries of "the students united will not be defeated!" filled Ho Plaza Thursday afternoon when nearly a hundred students banded together for the Million Student March and demanded tuition-free public college, cancellation of all student debt, a $15 minimum wage for campus workers and immediate divestment from fossil fuel corporations.&lt;br/&gt;Despite a student's post on social media calling for its cancellation, students gathered on the steps of Willard Straight Hall at 3 p.m. for the march, which was organized by the Cornell Independent Students' Union for a national event with more than 100 participating colleges.&lt;br/&gt;Cornell Independent Students' Union member Alec Desbordes '17 holds a sign during a march on Ho Plaza Thursday. (Cameron Pollack / Sun Senior Photographer)&lt;br/&gt;An hour before the march, a student posted on the Facebook event page a screenshot of a CISU statement of the union's demands, underlining a portion of the sentence, "Alongside students, faculty must demand that low-income and colored people traditionally excluded by the status quo, are invited into the university system."&lt;br/&gt;Pointing to the phrase "colored people," the student said in her post that she found it insensitive.&lt;br/&gt;"This is NOT okay. CISU needs to be held accountable. Students of color will not be tokenized by this organization," the student posted.&lt;br/&gt;In a comment on the Facebook post, CISU said it was "an unacceptable error" and that they planned to issue a public apology and "work hard to repair" it.&lt;br/&gt;Later in a post on the event page, Allison Lapehn '17 called for the protest to be cancelled, stating that CISU "cannot host an event promoting student power and solidarity when a group of students on campus no longer feel safe under your representation."&lt;br/&gt;She later told The Sun that she had called for the member of CISU responsible for the "racially insensitive" phrase to "step forward and formally apologize," but that the student union chose to collectively accept the blame, a decision that she said she believes should result in their dissolution.&lt;br/&gt;"It is unfortunate that progressive movements still do not realize the full meaning and importance of inclusion and promotion of all voices," Lapehn said.&lt;br/&gt;Despite the social media posts, the march continued as planned with multiple students shouting their demands and opinions.&lt;br/&gt;"Fifty percent of Cornell undergraduate students are employed by Cornell. One out of two of us is employed by this institution because we cannot afford to go here," said Alec Desbordes '17, a member of the Cornell Independent Students' Union. "This is ridiculous. There needs to be a change."&lt;br/&gt;Other students highlighted the importance of presenting a united fight in order to create a ripple effect that would motivate change regarding an array of issues.&lt;br/&gt;"We need to unite workers, students and full-time workers together because we work together, we strive together to make this campus work, and through our unity, we can bring change with an actual living wage and the possibility for us to not be under pressure and have an education how we should have it - free from any constraints," Desbordes said.&lt;br/&gt;Many protesters took pen to paper, canvas and cardboard, displaying signs to demonstrate their solidarity with messages that read "We have nothing to lose but our chains," "Total liberation from domination" and "Divest!"&lt;br/&gt;At approximately 3:35 p.m., the crowd marched towards Day Hall, streaming through Campus Road and East Avenue, which were both blocked off by campus police.&lt;br/&gt;"Whose school? Our school! Whose money? Our money! Whose future? Our future! Whose power? Our power!" protesters chanted.&lt;br/&gt;Alternating between cheering and chanting as they rounded street corners, protesters continued until they arrived in front of Day Hall, where they blocked off the intersection of Tower Road and East Avenue, and stood in a circle.&lt;br/&gt;There, students made impromptu speeches, acknowledging how privileged they are to attend Cornell with students from diverse backgrounds, who they said all have the right to protest in front of Day Hall. This, many reiterated, is a continuation of a movement against inequality. To continue the spread of the movement, protesters said they must make all students and faculty feel they are a part of the same cause.&lt;br/&gt;While the demands presented by all the schools participating in the Million Student March did not include divestment from fossil fuels, a demand made specifically by CISU for Cornell's administration, protesters still said it was equally important to the other issues.&lt;br/&gt;"Fossil fuels are a very important issue, but the real problem is that it is invested in with our tuition money without our consent," Desbordes said. "We do not think it is acceptable that the money we pay for education should be invested in corporations that are killing the world. We should be in control of where our money goes."&lt;br/&gt;Cornell's protest follows on the heels of demonstrations on college campuses across the nation. On Tuesday, hundreds of Ithaca College students and faculty participated in a walk out, accusing their president of mishandling racial incidents on campus and calling for his resignation. Students have also protested at the University of Missouri, Yale University, Smith College and Claremont McKenna.&lt;br/&gt;"We are out here trying to create a culture of student activism voice, democracy, and standing in solidarity as a community with faculty and students together," said Julien Morgan '19, a member of CISU.&lt;br/&gt;Before parting ways at around 4 p.m., many of those standing in the circle raised their fists in the air as a symbol of solidarity.&lt;br/&gt;While CISU is unsure what their next step will be, they plan to escalate in a Cornell-specific direction, bringing yearly tuition increases and divestment from fossil fuels to the spotlight, Desbordes said.&lt;br/&gt;"It is a powerful demonstration of student activism and how, as students, we collectively work as allies to target specific issues," said Ilse Paniagua '16, another CISU member. "Changes get made because students, faculty and workers, not the central administration or the trustees, are the ones that have fundamental power. So when we mobilize together, that's when change happens."&lt;br/&gt;Share this:&lt;br/&gt;Click to share on Twitter (Opens in new window)Share on Facebook (Opens in new window)Click to share on Google+ (Opens in new window)</t>
         </is>
+      </c>
+      <c r="L13" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -995,10 +1041,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>In anticipation of the United Nations Climate Change Conference scheduled to begin this November in Paris, University students gathered on the Diag on Friday to draw attention to climate change.&lt;br/&gt;The rally was sponsored by the University's chapter of Know Tomorrow, a student-led campaign launched by Cool Globes, a national nonprofit organization working to raise awareness and spur action on climate change.&lt;br/&gt;Members of Know Tomorrow held a banner urging students to stand on the "right side of history." The banner included information about recent gains in the climate change movement, including President Barack Obama's August announcement of the Clean Power Plan, which set new regulations for reducing carbon emissions from power plants.&lt;br/&gt;LSA junior Samantha Ginsburg, president of the University's chapter of Know Tomorrow, said she hoped the rally would help amplify and synchronize youth voices calling for action on climate change.&lt;br/&gt;"We know what tomorrow looks like," Ginsburg said. "The science is clear - there is no more debate. We want action because we know what our future looks like."&lt;br/&gt;Know Tomorrow chapters at 60 campuses across the country also held similar climate rallies Friday as part of the national day of action. Some events had high profile speakers such as Sen. Edward Markey at Harvard University and Robert F. Kennedy, Jr. at the University of Southern California.&lt;br/&gt;Don Scavia, a Graham Family Professor of Sustainability and director of the University's Graham Sustainability Institute, spoke at the rally on campus. Scavia urged students to combat climate change, at the personal and institutional levels.&lt;br/&gt;"There are lots of things you can do as individuals to reduce your own consumption," Scavia said. "Those individual actions, though, won't be enough - we need policy changes at the local, state and federal government levels."&lt;br/&gt;The Michigan Marching Band and Jugglers on Campus, a student organization, both performed at the event. Planet Blue and the Divest and Invest campaign also had tables distributing information.&lt;br/&gt;Engineering senior RJ Nakkula said students should join the University in its efforts to combat climate change.&lt;br/&gt;"The University is making steps in the right direction, but everyone needs to do their share," Nakkula said. "It's not just the University's part, it comes down to students, too."&lt;br/&gt;LSA freshman Noah Lowenstein, a member of Know Tomorrow, said the climate rally is an important step toward uniting millennials around climate change goals.&lt;br/&gt;"We are the millennials," Lowenstein said. "We are the ones who will be living on this Earth far beyond the policy makers today."</t>
         </is>
+      </c>
+      <c r="L14" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1038,10 +1087,13 @@
           <t>Trump and/or his administration (For), Tuition, fees, financial aid, _Other Issue</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>Photo by: Daryl Ontiveros | Multimedia EditorKristoffer Ian Celera, also known as Donald Tramp around campus, counter protests the Million Student March April 13 in front of the Vaquero Statue. Chants against student debt and championing the concept of free tuition echoed across campus from Old Main to the LBJ Student Center Wednesday as students protested in the Million Student March.The widespread movement is divided between national and campus goals and focuses on calling for free tuition and giving students the opportunity to have a say in how their tuition dollars are spent."We think that education is a right," said Kennedy Swift, studio art freshman, who took part in the march.The march wound around most of central campus and even went in to the student center itself, with students shouting slogans such as, "Banks got bailed out, students got sold out!" through megaphones."We want transparency on how tuition money is being spent," said Victoria Politte, communication disorders sophomore.&lt;br/&gt;"We don't want our money going towards wow factors like new fancy buildings."Some of the campus goals created by students for the Million Student Movement at Texas State involve a complete freeze in tuition rates and fees, a halt on all spending projects they feel are frivolous and the creation of a student tuition advisory board.The national goals of the movement are tuition-free public college, elimination of all student debt, $15 minimum wage for all campus workers and divestment from private prisons by all colleges and universities.Kristoffer Celera, computer science junior, said there are ways students can get a free education without demanding the government give it to them. Celera, who is a member of Young Americans for Liberty, did not support the protest.Celera was dressed up as his alter ego "Donald Tramp" during the march. Donald Tramp has garnered substantial attention on social media, as Celera wears Donald Trump-esque wig, a suit jacket and no pants.Throughout the march Celera could be seen dancing and siking various provocative poses holding a sign stating, "Your debt, your choice." Celera was not the only outspoken protestor against the march, as other Trump supporters made themselves heard at the end of the procession in the amphitheater.There were also other students present at the beginning of the march and at the end who did not take part, but voiced concerns over the goals of the movement, discussing their views with its members.Robert McAlmon, a mathematics graduate student, said he agrees with some of their points, but thinks it is more important students know where tuition is going and how it is used."I think we should make school officials more accountable for where our money is going," McAlmon said. "I know that a lot of our money goes to sports and overpaying administrators which I don't think is right.</t>
         </is>
+      </c>
+      <c r="L15" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1081,10 +1133,13 @@
           <t>University governance, admin, policies, programs, curriculum, Environmental</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>More than 50 protesters - brandishing expressive signs and miniature handmade windmills - gathered at Sample Gates to march and deliver a letter to the office of President Michael McRobbie, calling for University administrators to take a leadership role in the fight against ?climate change.&lt;br/&gt;"Support Clean Energy," "Indiana For Clean Air," "We are all concerned for the world" and "Stop Global Warming, Green Peace" were a few of the requests written on the protesters' signs and clothing.&lt;br/&gt;The protest was organized by Reinvest IU, an organization seeking to persuade the IU Foundation to divest from fossil fuel companies and reinvest in more sustainable forms of energy.&lt;br/&gt;Ben Brabson, a professor of physics at IU, speaks to a group of about 50 protestors Thursday evening at Showalter Fountain. Brabson applauded IU for their energy efficient buildings but challenged the University to distance itself from the fossil fuel industry.&lt;br/&gt;Students, alumni, faculty, concerned community members and a band marched into Bryan Hall, up a flight of stairs and into McRobbie's office in a uniform motion.&lt;br/&gt;The protesters crammed into his office, overflowing into the ?hallway.&lt;br/&gt;McRobbie was unavailable, so the letter was delivered to Kelly Kish, deputy chief of staff to McRobbie. The crowd fell silent and looked on intently as the letter was read out loud before it was handed to Kish.&lt;br/&gt;"The letter is just pointing out that climate change is important to not only the lives of future students but students here right now," said Ross E. Martinie Eiler, co-coordinator of Reinvest IU. "You can't in good conscience say we're trying to be a leader in dealing with the reality of climate change if we continue to pump all this money into corporations that are responsible for climate change."&lt;br/&gt;After receiving the letter, Kish declined to comment about the protest.&lt;br/&gt;"We'll just receive it, and we appreciate the students taking the time to come over," she said.&lt;br/&gt;Some students said they felt empowered after delivering the letter to IU's ?administration.&lt;br/&gt;"I think it is powerful to have a large crowd come in and support this cause," junior Melissa Bergsneider Serrano said. "We, the students, can have an impact on an issue like climate change and encourage the administration to take leadership on this issue."&lt;br/&gt;After delivering the letter to Kish, the protesters departed Bryan Hall and marched around campus before stopping at Showalter Fountain.&lt;br/&gt;Bystanders marveled as the crowd of protesters marched to the tune of one electric guitar, two saxophones and two drums.&lt;br/&gt;Sophomore Arielle Moir said the IU Foundation investing in fossil fuels is ?discouraging.&lt;br/&gt;"Investing in dirty energy like coal, oil and natural gas studies have shown that that's a harbinger of climate change," Moir said. "That affects all people, all creatures, including students here at IU not only in the present tense but future generations."&lt;br/&gt;In addition to the IU-Bloomington students present, there was a coterie of IU-Purdue University Indianapolis students carrying a placard reading "IUPUI Supports a Cleaner Future."&lt;br/&gt;"We're seeking to start a committee for climate change in Indianapolis," IUPUI senior Emma Fletcher said.&lt;br/&gt;Fletcher also said she hopes to get the attention of IUPUI Chancellor Charles Bantz and garner his support.&lt;br/&gt;At Showalter Fountain, physics professor Ben ?Brabson delivered a speech highlighting the progress and shortcomings of IU.&lt;br/&gt;"On one hand, IU is building energy efficient buildings and promoting research in climate," Brabson said. "On the other hand, IU is part owner of many of the fossil fuel producing and burning industries."&lt;br/&gt;Eiler said he hopes IU's administration will initiate dialogue with the IU Foundation about divesting in fossil fuels.&lt;br/&gt;"We think it's important to make moral investments with the University's money, and those moral investments include not jeopardizing the health of the planet," he said.</t>
         </is>
+      </c>
+      <c r="L16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1124,10 +1179,13 @@
           <t>University governance, admin, policies, programs, curriculum, Tuition, fees, financial aid, Environmental, Economy/inequality, Labor and work, Pro-Palestine/BDS</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>UNM students gathered in front of Zimmerman Library on Thursday as part of a nationwide movement calling for abolishing student debt, raising the minimum wage and providing free tuition at public universities.&lt;br/&gt;Marisa Trujillo, a sophomore business administration major, said the rally gave financially struggling students a way to voice their frustrations with peers in similar situations.&lt;br/&gt;"People talk about it, but it's too quiet; people are brushing it under the rug, the school is hiding it," she said. "That's why we put this on, we gave students a chance to stand with us and not to have any fear and to basically let their voices be heard."&lt;br/&gt;Trujillo said UNM is just one of hundreds of schools nationwide participating in rallies like Thursday's in hopes that the U.S. can model itself after other countries that offer free education, such as Denmark.&lt;br/&gt;"When people come and tell us that it's impossible, it's really possible, and it's simpler than people think," she said. "The thing is, people are afraid to stand up against it because they think that the authority of the school is going to shut them down. Which they might, but we're still going to speak out, because it's something we deserve."&lt;br/&gt;UNM was one of hundreds of schools nationwide that had students participating in the movement, called the Million Student March. Several students held signs that read "Kicking ass 4 the working class" and "Education Is A Human Rights Issue," among others.&lt;br/&gt;It was endorsed by several UNM student groups, including the Feminist Majority Leadership Alliance, Generation Justice and the Red-Student Faction.&lt;br/&gt;Micheáilín Buitléir, a junior American studies major, said that the movement's three goals are intertwined in a mission to partake in the assets that UNM collects from students.&lt;br/&gt;"This is just a pyramid scheme to mass-accumulate wealth," he said. "What we want is, instead of the wealth going into the hands of the one percent, we want the wealth to go to all of us, to redistribute that wealth to invest in our future. Like our sign says, 'The present is struggle, but the future is ours.'"&lt;br/&gt;Buitléir said that in addition to the core demands, the rally at UNM added a fourth: divestment of the indirect support of the occupation of Palestine, as well as the reliance on fossil fuels.&lt;br/&gt;"(It) is one of the biggest issues we're facing right now - the extinction of our species. So taking that money and starting to invest it in education and higher wages, investing it in healthcare and jobs and those sorts of things," he said.&lt;br/&gt;Another supporter said that UNM is being hypocritical in calling itself a public university, and that the University is essentially robbing students by continuing to raise tuition "in the second Great Depression of this nation's history."&lt;br/&gt;"I think, if we can work through the setup structure, that would be great because it gives us a good dialogue and a good forum to actually sit down and make a change," Graves said. "This raises awareness and it gets people thinking about it, but it doesn't drive the policy change we need."&lt;br/&gt;Not all UNM students approve of such policy change, however, including more conservative representatives from Young Americans for Liberty, a new organization at UNM this semester.&lt;br/&gt;"Before us, the liberal agenda (on campus) kind of had its way. It was never challenged; people just kind of walked around it and ignored it if they didn't agree with it," said Michael Aguilar, president of the group's UNM chapter. "So we decided to mobilize the conservative cohort that we do have on campus...and we made sure that the liberal agenda didn't go unchecked."&lt;br/&gt;Aguilar said that the demands of the Million Student March are not feasible, economically or otherwise, and that someone will have to bear the burden.&lt;br/&gt;"There's no such thing as a free lunch. Someone's going to get the bill, and they're going to realize that the one percent can't pay for everything," Aguilar said.&lt;br/&gt;While representatives from the two sides argued at the rally for some time, Aguilar said before his peers left the event, he and Graves agreed that they should hold an organized debate in the SUB.&lt;br/&gt;Such an event would accurately inform students about the issues at hand, something that Aguilar said he always advocates.&lt;br/&gt;"I think that, whether it be a rally like we had today, a counter-protest or a forum, any way (we can) engage the students and get them involved in the political process... I think that's beneficial for everyone involved," he said.&lt;br/&gt;Although Trujillo said that the rally's opponents were there just "to be against us," she also said a debate is the more appropriate route to discuss the issues at hand between the two parties.&lt;br/&gt;"We want to get stuff done, and shouting at each other isn't going to get anything done. Whether we agree on everything, or anything at all for that matter, we can still talk and be civil about it and get somewhere," she said.&lt;br/&gt;David Lynch is the news editor at the Daily Lobo. Contact him at news@dailylobo.com or on Twitter @RealDavidLynch.</t>
         </is>
+      </c>
+      <c r="L17" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1167,10 +1225,13 @@
           <t>Labor and work</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>After waiting for two years, Seattle University adjunct faculty were officially granted the right to unionize on Sept. 12. The National Labor Relations Board approved a long- standing petition to allow adjunct faculty to join the Service Employees International Union, making Seattle U one of just a few private Jesuit universities in the country to permit this change.&lt;br/&gt;Students and faculty march for unionization in April 2016.&lt;br/&gt;Students and faculty alike who were present to experience the swells of passion around the movement, including an organized walk-out protest in Feb. 2015, rejoice in this news in the hopes that it will mean positive changes both inside the classroom and within the Seattle U community.&lt;br/&gt;"I think it is a very good change. I think that adjunct professors should feel secure in their positions," said Wendall Tseng, a student and member of the Reignite the Mission club on campus. "And without giving adjunct equal benefits, I feel there is less incentive as a professor to build a community of the best curriculum. I do not see a valid instance in which this [unionization] shouldn't be allowed."&lt;br/&gt;The union has yet to begin its collective bargaining process, which includes negotiations between faculty and administrators. A unit will be formed by elected adjunct members who will work to alleviate issues within the non-tenure experience regarding wages, hours, work conditions and benefits. From there, they will work with Seattle U administrators to decide on regulations and legislation to protect these workers.&lt;br/&gt;All adjunct faculty will be subject to these future changes, with the exception of faculty working within departments of religion and theology, who are not permitted to unionize due to a rule regarding the separation of church and state.&lt;br/&gt;The road to unionization was not without its bumps, and resistance from some faculty and administrators halted the vote for over two years.&lt;br/&gt;The university argued that because it has increased minimum full-time faculty salaries over the past several years-from $24,600 to $45,000-a union would not be necessary in addressing faculty concerns.&lt;br/&gt;In 2014, University President Fr. Stephen Sundborg, S.J. released a video addressed to adjunct faculty strongly encouraging them to vote against the right to unionize. The video has since been removed from the university's website.&lt;br/&gt;In the video, Sundborg implied that the right to unionize would go against the university's mission statement, and stated it would be "nearly impossible" to work with faculty if they had to go through the Service Employees International. Some faculty felt differently about this point, including Emily Lieb, an assistant professor within the Matteo Ricci College.&lt;br/&gt;"Nothing is more consistent with the Jesuit mission of this university than having an organized faculty that is treated fairly and ethically and committed to their jobs," Lieb said.&lt;br/&gt;Sundborg went on to describe how happy students seem to be with their adjunct professors, and that student satisfaction should warrant not granting adjunct members the right to unionize. But as former Seattle U adjunct professor Larry Cushnie pointed out, there are several of aspects of teaching that go unseen to the average college student. Cushnie left Seattle U in 2015, and currently teaches at the University of Washington and Bellevue College.&lt;br/&gt;"I talked to other instructors, who even while they were teaching, were eligible for things like food stamps and public assistance," Cushnie said.&lt;br/&gt;The university's argument against unionization also referenced Catholic Social Teaching, a doctrine created by the Catholic Church that dictates the church's feelings and thoughts on the role of church and state, social organization and other forms of social justice. While some cited these teachings to support the campaign against unionization, Catholic social teaching explicitly allows and promotes the right to organize.&lt;br/&gt;But ultimately, the commitment of several faculty members and students to ignite a common governance for all hired adjuncts was able to win out over the university's defense.&lt;br/&gt;The union will specifically allow adjunct faculty to have a greater voice and role in the university's politics. For instance, they hope to have a larger say in how departments are run. Cushnie explained that when important, school-wide decisions on education are allocated to those who do not have the expertise to make those decisions, it can create dissonance between departments and how they function.&lt;br/&gt;"Decisions were being made to do things like cancel or nix some of the departments on campus...and then also adding new programs even as the university was experiencing budget problems, in terms of all- around education, and no one had a say about it-adjuncts especially," Cushnie said.&lt;br/&gt;Proponents of unionization have agreed that one of the most important reasons for unionization is the impact it can have on job security.&lt;br/&gt;"Being tenured, you have a lot of academic freedom as far as your curriculum because there is no fear of being chopped off the faculty line," Tseng said. "And in that way, job stability really helps you create the best kind of classroom because you can really have the most freedom to teach what you really want to teach, and really give students the best environment."&lt;br/&gt;A lack of job security in the past has greatly impacted the well-being of some Seattle U adjunct professors. Audrey Hudgins, a clinical instructor for the Matteo Ricci College, recounted having a class cancelled a week before it was meant to start.&lt;br/&gt;"You do a bunch of work you don't get compensated for, and then you don't get a check when your rent is due," Hudgins said.&lt;br/&gt;Lieb also emphasized the negative impacts this kind of last-minute planning can have.&lt;br/&gt;"The issue has been historically that people who are just teaching one class or two classes, there is no notice if they are going to cancel your class so you can show up the day before school starts and find you are not teaching," Lieb said.&lt;br/&gt;Creating equality of treatment where equality already exists is also a huge point of this movement.&lt;br/&gt;"In my view, there is no difference," Hudgins said. "There is the same level of academic training, the same credentials, the same disciplinary expertise, the same commitment to student success."&lt;br/&gt;With this new union, situations in which adjunct faculty have been given less rights and benefits as their tenured counterparts will hopefully be avoided to maintain the livelihood of all faculty, as well as that of the students they teach.&lt;br/&gt;Perhaps the demographic this change will affect the most are the students. Students are what make Seattle University the prestigious Jesuit college it is today. This of course could not have been achieved without the instruction and guidance of Seattle University professors. Cushnie illustrated the urgency of this system of checks and balances at Seattle U.&lt;br/&gt;"Universities in the last couple decades started organizing themselves in much more of a corporate-based structure. And you see this at SU; the hiring administration has skyrocketed and tenure track faculty have declined," Cushnie said. "If a tenure leaves for one reason or another...they tend to hire two to three adjuncts to make up for that since it is so much cheaper."&lt;br/&gt;At its core, the lack of unionization was taking its toll on the classroom experience.&lt;br/&gt;"At Seattle University my students were going into mass amounts of debt, and had no chance to form relationships with the adjuncts that were teaching the majority of their classes because they [the adjunct] had no idea if they would even be there the next quarter," Cushnie said.&lt;br/&gt;With the support of clubs campus-wide and a passion for justice brought forth by both students and faculty, some practices within university administration can now be halted and renegotiated to better fit the adjuncts being impacted.&lt;br/&gt;"If you want a healthy, Jesuit, social justice university, just look at the middle of campus, look at what types of protests and what students are involved in," Cushnie said.&lt;br/&gt;Students are the biggest supporters and drivers of social change on campus. Whether they're tackling issues of divestment or organizing occupations to take a stand against racism within their curriculum, Seattle U students continue every day to trailblaze and improve themselves, their campus and their community. This drive can be attributed to all the professors who have guided and educated students to profound bravery to stand up to their own university.&lt;br/&gt;Seattle U's character can be defined by its mission statement, and for many, unionization is just one step closer to a more just and humane world.&lt;br/&gt;The author may be reached at</t>
         </is>
+      </c>
+      <c r="L18" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1210,10 +1271,13 @@
           <t>Faith-based discrimination</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="K19" t="inlineStr">
         <is>
           <t>More than 5,000 people signed a petition, started last November, to ban Students for Justice in Palestine chapters in CUNY.&lt;br/&gt;Andrea Karshan, a student at the College of Staten Island, started the petition after members at different campuses chanted allegedly anti-Semitic comments at Jewish students during the Million Student March in November. One sign called for CUNY to divest from "Israeli apartheid."&lt;br/&gt;SJP began in 1993 at the University of California at Berkeley. Since then, there are chapters across the country, including at CUNY colleges. The organization is controversial for criticizing Israel's presence in Palestine. One tactic it uses is BDS, which means boycott, divest and sanctions.&lt;br/&gt;Karshan declined questions from The Knight News, but wrote an article on her blog defending the petition. She described the backlash from students and the support she received too.&lt;br/&gt;"I don't regret starting the petition," she wrote. "It was something that needed to be done. Our voices needed to be heard."&lt;br/&gt;Karshan worked at The Banner newspaper when she created the petition. But she was dismissed by the Editor-in-Chief. After a new one was appointed, she returned.&lt;br/&gt;The Banner newspaper sent a statement to The Knight News explaining why removing her was wrong.&lt;br/&gt;"While it was not right for Andrea to become a part of the story she was reporting on, the editors handled the situation appropriately by taking her off the assignment," it reads. "Her dismissal was quite literally against the Banner's constitution as we're obliged to be a welcoming place to all students at the College of Staten Island, no matter their beliefs or convictions."&lt;br/&gt;But Sarah Aly, president of the SJP chapter at Brooklyn College, said Karshan's petition cannot work.&lt;br/&gt;"There is no way that these demonstrations actually can be used to suspend any SJPs," Aly said. "The CUNY-wide demonstration was organized by NYC SJP, which is an off-campus organization not tied to a campus."&lt;br/&gt;Aly added Karshan did not get along with Muslim students and caused problems with SJP chapters too.&lt;br/&gt;"She complained that the prayer room on campus was 'too Muslim.' [She] forced Muslim students to clear the room of prayer rugs and Qurans, while Bibles and other religious items were left alone. She has also been known to harass CSI's chapter of SJP in person and online," Aly said.&lt;br/&gt;CUNY Chancellor James Milliken said, in response to the allegations, that the remarks were not suitable and denounced them.&lt;br/&gt;"While we will always embrace this openness to many voices, intolerant, hateful and bigoted speech, while it may be legally protected, is anathema to our values," he said. "Those voices," stop rather than encourage the dialogue and real debate that makes us stronger."&lt;br/&gt;In response to the Chancellor's comments, Aly said there were Islamophobic remarks and found it troubling that he did not address that. She brought up the New York Police Department's spying on Muslim students as something he does not comment on.&lt;br/&gt;"This has been the trend recently [where] issues affecting students and faculty of color are being pushed to the side and ignored," Aly said.&lt;br/&gt;The New York Civil Liberties Union released the NYPD's handbook on spying on MSAs at CUNY. At Queens College, officers are told to look at online profiles of members and even follow them.&lt;br/&gt;At QC, Aadil Ilyas, an alum, felt the backlash against SJP. He worked to make a chapter at the college.&lt;br/&gt;Ilyas posted a status on Facebook calling Israeli Prime Minister Benjamin Netanyahu a monkey. A Jewish student took a screenshot of his status and gave it to a staff member. Ilyas was told not to make the chapter after this and because the national "negative attention" toward the group.&lt;br/&gt;"I left [the person's] office in disbelief," Ilyas said. "I was so angry. I know why I started SJP, and QC is the perfect place to start it."&lt;br/&gt;But Ilyas said several club leaders supported his decision and starting the chapter.&lt;br/&gt;"I had a presentation to do for SJP [in front of QC officials], since it was a new club, and I did great," Ilyas said. "They had no choice but to approve it."&lt;br/&gt;Only the board of trustees can decide to ban SJP, but doing so is illegal, said Radhika Sainath, a staff attorney at Palestine Legal.&lt;br/&gt;"CUNY absolutely may not shut down SJP because some New Yorkers disagree with the group's message supporting justice for Palestinians. To do so would violate the First Amendment," Sainath said.</t>
         </is>
+      </c>
+      <c r="L19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1253,10 +1317,13 @@
           <t>Anti-racism, Police violence</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="K20" t="inlineStr">
         <is>
           <t>Last night, Student Government's General Assembly voted to indefinitely table a resolution reaffirming the University's commitment to free expression. Specifically, it referred to recent instances of speakers interrupted by protesters, including Anita Alvarez and Bassem Eid.&lt;br/&gt;Following extensive debate, General Assembly, which is comprised of the College Council and Graduate Council , first voted on a motion to reject the resolution. Eight students voted in favor of rejection, 10 voted against rejection, and eight abstained. In response, multiple members introduced a motion to table the resolution indefinitely, and only six members voted against the second motion allowing the tabling to pass.&lt;br/&gt;The resolution was proposed by second-year Matthew Foldi. This resolution calls on the University administration to condemn any student who "obstructs or disrupts" free speech, including making threats to speakers on campus, and to enforce such condemnation. It cited the University's Report of the Committee on Freedom of Expression and alluded to two campus events disrupted by student protesters earlier this year.&lt;br/&gt;In his presentation to the General Assembly, Foldi explained that he wrote the resolution in response to February events with Cook County State Attorney Anita Alvarez and Bassem Eid, a Palestinian human rights activist and critic of the Boycott, Divest, and Sanctions movement. Both events ended early after student protesters drowned out the speakers.&lt;br/&gt;Foldi added that the Foundation for Individual Rights in Education , a group that advocates for free speech on college campuses, awarded the University its highest rating for protection of free speech earlier this year.&lt;br/&gt;"In 2016 alone...18 speakers have been shut down or uninvited from college campuses, and two of those events are the ones stressed by this resolution," he said. "We are looked upon as an example by other institutions who adopt our speech policies and as such I think it's important to affirm the importance of free inquiry at the University of Chicago." 136 people signed the resolution, including 52 professors and Ph.D. students from a wide range of departments and 83 undergraduates, graduate students, and alumni.&lt;br/&gt;Foldi also co-sponsored two resolutions last week calling on the University to divest from China and the investment RSO Blue Chips to divest from Israeli companies listed in CC's April 12 resolution.&lt;br/&gt;In debating the resolution, several General Assembly members referenced the event with Anita Alvarez, who has been widely criticized for her office's role in delaying the release of a video of a Chicago Police Department officer shooting 17-year-old Laquan McDonald.&lt;br/&gt;"I do think that at a university, a variety of viewpoints are supposed to be put in front of us," said Class of 2018 CC Representative Calvin Cottrell. "I was going to show up [to the Alvarez event] and ask very tough questions about what had happened in her office and I think many people were denied the opportunity to ask those questions."&lt;br/&gt;Class of 2018 Representative Cosmo Albrecht disagreed. "I don't think we should use this idea of elected officials being...banned from speaking as evidence that free speech is under attack," he said. "If you're an elected official you should be willing to face the consequences of your actions.... I think these protests are a necessary part of a democracy."&lt;br/&gt;SG President Tyler Kissinger explained that while he does not usually speak on these issues, he urged General Assembly members to vote against the resolution. "As a public official it is my obligation not to run out of the room. I was at the Anita Alvarez event, an event with someone whose office has consistently refused to meet with black and Latino communities that her office has over-policed and I don't think that's right," he said. "I think it is well within the rights of people to protest events particularly for public officials...and I urge a no vote."&lt;br/&gt;After voting against the motion to reject the resolution, multiple SG members motioned to table the resolution indefinitely. Following the passage of this motion, Class of 2017 Representative Mark Sands made a point of order, saying, "postponing indefinitely is the lowest priority motion and I had another motion so it should've been voted on first." In response, Kissinger said, "I didn't hear the motion," and adjourned the meeting.&lt;br/&gt;The indefinite tabling of the resolution means that the resolution may be brought up for discussion in future academic quarters.</t>
         </is>
+      </c>
+      <c r="L20" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1296,10 +1363,13 @@
           <t>Anti-racism, Police violence</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="K21" t="inlineStr">
         <is>
           <t>Over the course of the school year, the Institute of Politics hosted many events featuring high-profile speakers, including several that attracted protests and controversy.&lt;br/&gt;High-Profile Speakers&lt;br/&gt;On September 28, Democratic presidential candidate Bernie Sanders (A.B. '64) spoke at Rockefeller Chapel to a crowd of more than 1,800 people. In addition to discussing his views on issues such as women's rights, criminal justice reform, and campaign finance, Sanders spoke about his time at UChicago. Coming from a low-income background, Sanders struggled to adjust to UChicago, where many students came from wealthy backgrounds. This experience shaped Sanders's commitment to socioeconomic equality.&lt;br/&gt;On October 16, IOP Director David Axelrod moderated a discussion with House Minority Leader Nancy Pelosi (D-CA) at the International House (I-House) Assembly Hall. Axelrod and Pelosi discussed the then-vacant Speaker of the House position in light of John Boehner's resignation. Pelosi argued that the lack of a clear successor to Boehner indicated that the Republican Party is an "anti-governance party."&lt;br/&gt;On April 7, President Barack Obama, a former constitutional law professor at the University, returned to the Law School to discuss the resistance to his nomination of Judge Merrick Garland to the Supreme Court. Obama argued that Senate Republicans' refusal to consider his nomination of Garland represents a failure of the Senate to fulfill its constitutional duty and the infringement of party politics on the judicial branch.&lt;br/&gt;On May 9, former Daily Show host Jon Stewart spoke in Rockefeller Chapel for a live recording of Axelrod's podcast, The Axe Files. Stewart and Axelrod discussed the 2016 election, with a particular focus on Donald Trump and Hillary Clinton. Stewart stated that Trump's reputation for "telling it like it is" and battling against political correctness is unwarranted because of Trump's sensitivity to criticism. Stewart also criticized Clinton for not clearly expressing her convictions.&lt;br/&gt;On May 12, whistleblower Edward Snowden addressed a crowd at Ida Noyes Hall over a video call. Snowden said that he had taken an oath to uphold the U.S. Constitution and that he believed he had an obligation to the Constitution's principles in spite of the illegality of his actions. Snowden also advocated for a simpler internal complaint system at government agencies.&lt;br/&gt;Protests&lt;br/&gt;On February 17, Cook County State's Attorney Anita Alvarez left 20 minutes into a talk at the IOP after vocal protests by representatives from several organizations, including Black Lives Matter Chicago. Alvarez has been heavily criticized in light of the release of a video showing 17-year-old Laquan McDonald being shot 16 times by a police officer, which reignited discussions and protests regarding police brutality against black people nationwide. Protesters held signs and chanted "Anita Alvarez does not believe that black lives matter," prompting Alvarez's exit. Following the incident, Axelrod wrote a Letter to the Editor published in The Maroon on February 18 denouncing the protests and arguing that "free and open debate should not be muzzled by government, university administrations, or angry mobs."&lt;br/&gt;On February 18, police intervened in a talk by Palestinian human rights activist Bassem Eid at I-House after disagreements between Eid and the audience. Eid has vehemently criticized the Boycott, Divestment, and Sanctions movement, which aims to put pressure on Israel to alter its policies towards Palestinians. A Palestinian audience member questioned "what brought Palestinians to a place where they have to go work for their occupiers," leading to a tense argument between Eid and the audience member. After the audience member was ushered away by I-House staff, others asked similar questions and questioned Eid's status as a Palestinian and human rights activist. University of Chicago Police Department officers then intervened, removing the two audience members and Eid, and ended the event.&lt;br/&gt;On April 25, members of the Armenian Students Organization, Students for Justice in Palestine, and the Hellenic Students Association protested a lecture by University of Louisville professor Justin McCarthy, who they say denies the Armenian Genocide, at I-House. McCarthy, who claims that the events deemed genocide were part of a civil war between the Ottoman Empire and Armenian rebels, has been accused of Armenian Genocide denialism by the International Association of Genocide Scholars. Protesters filled the second and third rows of the audience and placed red tape over their mouths. McCarthy asked the protestors to sit down, but they refused and then exited the room to applause.</t>
         </is>
+      </c>
+      <c r="L21" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1344,10 +1414,13 @@
           <t>Hate speech</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="K22" t="inlineStr">
         <is>
           <t>Students hang banners in Arts and Letters Hall Wednesday decrying hate speech a week after conservative MIlo Yiannopoulos visited campus. (Brenden Moore/The DePaulia)&lt;br/&gt;Student activists decried hate speech as they dropped banners, one stating "Hate speech ? free speech" and the other asking "What would Vinny do?",  from the third and fourth floor balconies of Arts and Letters Hall this afternoon.&lt;br/&gt;The act comes after a week which saw political and racial tensions float to the surface following conservative writer Milo Yiannopoulos' visit to campus and incidents that include the drawing of an anti-Mexican slur on the Quad and the reported finding of a noose the sidewalk near a residence hall.&lt;br/&gt;Around 20 student activists, split by floor, dropped the banners around 12:50 p.m. and started chants that included, "Hate speech ain't free speech", "Can't stop the revolution" and "Black Lives Matter".&lt;br/&gt;Sources said the event had been in the works for nearly a week and that it may have been the effort of a sociology class applying the events of last week to curriculum in the classroom.&lt;br/&gt;About 10 minutes in, a university maintenance worker attempted to take the banners down, which led to chants of "Let the banner hang!" and then cheers when he indeed quit his effort.&lt;br/&gt;"Let the banner hang!" pic.twitter.com/P1mMjhqfuO&lt;br/&gt;- Brenden Moore (@brendenmoore13) June 1, 2016&lt;br/&gt;The event would continue for another 10 minutes when Public Safety eventually took the banner down. The students then marched outside the building and dispersed.&lt;br/&gt;The university appeared to have a heads up as an assortment of officials, including vice president for facilities operations Bob Janis, vice president for student affairs Gene Zdziarski and associate vice president for diversity Rico Tyler were quickly on the scene. This is the fourth banner drop in recent years. One in April 2014 brought attention to the alleged rape culture in the athletic department, one in Spring 2014 called for DePaul to divest in companies that supported Israel's occupation of Palestine by dropping a Palestinian flag and one in the Student Center two weeks ago called for former Chicago Police officer Dante Servin to be denied his pension after he killed Rekia Boyd.</t>
         </is>
+      </c>
+      <c r="L22" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1387,10 +1460,13 @@
           <t>_Other Issue</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
+      <c r="K23" t="inlineStr">
         <is>
           <t>Over the course of the school year, the Institute of Politics hosted many events featuring high-profile speakers, including several that attracted protests and controversy.&lt;br/&gt;High-Profile Speakers&lt;br/&gt;On September 28, Democratic presidential candidate Bernie Sanders (A.B. '64) spoke at Rockefeller Chapel to a crowd of more than 1,800 people. In addition to discussing his views on issues such as women's rights, criminal justice reform, and campaign finance, Sanders spoke about his time at UChicago. Coming from a low-income background, Sanders struggled to adjust to UChicago, where many students came from wealthy backgrounds. This experience shaped Sanders's commitment to socioeconomic equality.&lt;br/&gt;On October 16, IOP Director David Axelrod moderated a discussion with House Minority Leader Nancy Pelosi (D-CA) at the International House (I-House) Assembly Hall. Axelrod and Pelosi discussed the then-vacant Speaker of the House position in light of John Boehner's resignation. Pelosi argued that the lack of a clear successor to Boehner indicated that the Republican Party is an "anti-governance party."&lt;br/&gt;On April 7, President Barack Obama, a former constitutional law professor at the University, returned to the Law School to discuss the resistance to his nomination of Judge Merrick Garland to the Supreme Court. Obama argued that Senate Republicans' refusal to consider his nomination of Garland represents a failure of the Senate to fulfill its constitutional duty and the infringement of party politics on the judicial branch.&lt;br/&gt;On May 9, former Daily Show host Jon Stewart spoke in Rockefeller Chapel for a live recording of Axelrod's podcast, The Axe Files. Stewart and Axelrod discussed the 2016 election, with a particular focus on Donald Trump and Hillary Clinton. Stewart stated that Trump's reputation for "telling it like it is" and battling against political correctness is unwarranted because of Trump's sensitivity to criticism. Stewart also criticized Clinton for not clearly expressing her convictions.&lt;br/&gt;On May 12, whistleblower Edward Snowden addressed a crowd at Ida Noyes Hall over a video call. Snowden said that he had taken an oath to uphold the U.S. Constitution and that he believed he had an obligation to the Constitution's principles in spite of the illegality of his actions. Snowden also advocated for a simpler internal complaint system at government agencies.&lt;br/&gt;Protests&lt;br/&gt;On February 17, Cook County State's Attorney Anita Alvarez left 20 minutes into a talk at the IOP after vocal protests by representatives from several organizations, including Black Lives Matter Chicago. Alvarez has been heavily criticized in light of the release of a video showing 17-year-old Laquan McDonald being shot 16 times by a police officer, which reignited discussions and protests regarding police brutality against black people nationwide. Protesters held signs and chanted "Anita Alvarez does not believe that black lives matter," prompting Alvarez's exit. Following the incident, Axelrod wrote a Letter to the Editor published in The Maroon on February 18 denouncing the protests and arguing that "free and open debate should not be muzzled by government, university administrations, or angry mobs."&lt;br/&gt;On February 18, police intervened in a talk by Palestinian human rights activist Bassem Eid at I-House after disagreements between Eid and the audience. Eid has vehemently criticized the Boycott, Divestment, and Sanctions movement, which aims to put pressure on Israel to alter its policies towards Palestinians. A Palestinian audience member questioned "what brought Palestinians to a place where they have to go work for their occupiers," leading to a tense argument between Eid and the audience member. After the audience member was ushered away by I-House staff, others asked similar questions and questioned Eid's status as a Palestinian and human rights activist. University of Chicago Police Department officers then intervened, removing the two audience members and Eid, and ended the event.&lt;br/&gt;On April 25, members of the Armenian Students Organization, Students for Justice in Palestine, and the Hellenic Students Association protested a lecture by University of Louisville professor Justin McCarthy, who they say denies the Armenian Genocide, at I-House. McCarthy, who claims that the events deemed genocide were part of a civil war between the Ottoman Empire and Armenian rebels, has been accused of Armenian Genocide denialism by the International Association of Genocide Scholars. Protesters filled the second and third rows of the audience and placed red tape over their mouths. McCarthy asked the protestors to sit down, but they refused and then exited the room to applause.</t>
         </is>
+      </c>
+      <c r="L23" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1430,10 +1506,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
+      <c r="K24" t="inlineStr">
         <is>
           <t>On the first day of Parents' Weekend last Friday, something out of the ordinary occurred outside of Commons during peak lunch hour. Onlookers observed as a whistle blew and a group of students suddenly dropped to the ground. Another student then drew chalk outlines around the bodies playing dead on the pavement. Next, student protestors formed a line and held up signs with messages such as "Climate Change Kills" and "Invest In Our Future."&lt;br/&gt;Members of BEAM, the Bates Energy Action Movement, organized the rally as part of the Bates College Divestment Movement. The "dead" bodies were representative of the expected 300,000 deaths per year in result of various hazards created by climate change.&lt;br/&gt;Fossil fuels, or natural fuels such as coal and gas, play a dangerous role in global warming, and time is running out. In order for a stable climate to be secured, 80% of all the fossil fuel reserves need to be left underground. BEAM believes that Bates must do its part in reducing fossil fuel usage.&lt;br/&gt;Last May, a member of the group met with the Bates Board of Trustees. While the Board responded favorably to BEAM's conviction and claimed that Bates has the "moral justification" to divest, they also maintained that Bates would never be a leader in this movement.&lt;br/&gt;BEAM Co-President Ben Breger '14 explains that the objective behind the rally was "to shine a spotlight on the human impact of climate change, rather than only the ecological impact," and ultimately "to actually build something from this rally."&lt;br/&gt;The rally was a method of drawing attention to the ongoing online petition against Bates' donations going toward investments in fossil fuel companies.&lt;br/&gt;For a year now, BEAM has been executing a campaign that puts pressure on the Bates Board of Trustees to divest completely from the fossil fuel industry. BEAM proposes that Bates execute a "five year faze out" from relationships with fossil fuel companies and total divestment from coal companies in two years, hoping to offer some flexibility.&lt;br/&gt;The online petition created by BEAM petitions directly for the Board of Trustees to divest from fossil fuel, and calls upon each individual signer to pledge not to contribute to Bates if such investments are still being made. The petition is directed at the Advancement Office with hopes that the Advancement Office will then put pressure on the Board or Trustees to take action.&lt;br/&gt;The introduction to the petition reads: "As a Bates College graduate, and a member of the extended Bates community, I share and cherish Bates' commitment to social responsibility. The growing climate crisis is a call to action to uphold this commitment in impactful ways." The ultimate message of the petition is the concluding pledge: "By signing this petition I agree to not donate to Bates College until the Board of Trustees commits to divesting from the fossil fuel industry."&lt;br/&gt;The BEAM club at Bates does not act alone in its fossil fuel divestment efforts. Co-President Breger explains, "The movement has become international, becoming active at over three-hundred college campuses, twenty cities and towns, numerous religious organizations." Two colleges in Maine, Unity College and The College of the Atlantic, are the only two Maine colleges to completely divest from fossil fuel companies.&lt;br/&gt;Members of BEAM, in addition to other Bates students, faculty, and community members, hope that Bates can follow Unity College and The College of the Atlantic by divesting investments of the fossil fuel industry.&lt;br/&gt;Breger criticized Bates' current stance on the refusal to divest from fossil fuel industries by citing the college's mission statement; BEAM believes that if Bates is serious about its pledge to "engage the transformative power of our differences, cultivating intellectual discovery and informed civic action," then the Advancement Office should take action to invest more responsibility in light of pressing issues of climate change.&lt;br/&gt;BEAM members will continue to be involved in climate change issues during the upcoming October break, when they will travel to Pittsburgh, Pennsylvania to attend the Power Shift Conference.&lt;br/&gt;"The conference is a great way for students to learn about organizing campaigns and learn about important issues like hydraulic fracking," explains BEAM co-President Bora Kim '14. Spots are still available for Bates students interested in attending the conference.by</t>
         </is>
+      </c>
+      <c r="L24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1473,10 +1552,13 @@
           <t>Labor and work, University governance, admin, policies, programs, curriculum, Economy/inequality</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="K25" t="inlineStr">
         <is>
           <t>Photo: Alexandra Davis.Students walk down the street during the protest to democratize the University holding various posters.&lt;br/&gt;IIRON-once the Illinois-Indiana Regional Organizing Network-has linked University students with opportunities to advocate on behalf of local and national issues for years. This year, the IIRON Student Network has brought its activism to campus with a series of attention-grabbing protests. Many of the University's most important advocacy groups joined under ISN's banner for a series of actions which escalated as the end of the year neared.&lt;br/&gt;On November 2, four University of Chicago students and two alumni were arrested along with 38 other protesters at the Chicago Board of Trade. The protest, organized by the Fair Economy Illinois coalition, demanded a "LaSalle Street Tax" on corporations and higher income taxes on the rich to balance the state's budget. Southside Solidarity Network , a UChicago student organization, and UChicago Climate Action Network both sent protesters. Hundreds of protesters marched from Thompson Center to the Chicago Board of Trade, where they blocked entrances and staged a die-in.&lt;br/&gt;On February 26, 60 students from Fair Budget UChicago protested to demand that the University raise the minimum wage on campus to $15 an hour. The protest included a march from Regenstein Library across the main quad to Edward H. Levi Hall.&lt;br/&gt;The protesters gathered in the fifth-floor waiting room outside Provost Eric D. Isaacs's office to deliver a petition with more than 1,000 signatures calling for a higher wage for University employees. When Isaacs was not found in his office, protesters asked the Dean-on-Call to commit to delivering the petition to Isaacs. Initially the Dean-on-Call stated that she could not promise to deliver the petition because she didn't have the authority to ensure that Isaacs would see the petition. Later she stated that she would make an effort to deliver the petition to Isaacs. University spokesman Jeremy Manier later confirmed that the provost had received the petition.&lt;br/&gt;More than a month later, on April 2, students and activists gathered outside the Chicago Symphony Orchestra to protest higher-education budget cuts before the Saturday 8 p.m. orchestra performance. Students from FBU participated in the protest directed at two University trustees along with the IIRON Student Network.&lt;br/&gt;A public meeting, organized by IIRON and attended by over 50 student activists from IIRON and Phoenix Survivors Alliance , was held in Reynolds Club on May 2. The meeting aimed to provide a forum at which students could express their concerns over administrative policies and advocate for increased transparency and communication with undergraduates. The meeting was initially organized as a town hall meeting that Isaacs, incoming Provost Daniel Diermeier, Vice President and Secretary of the University Darren Reisberg, and Dean of Students in the College John "Jay" Ellison were invited to attend. However, no administrators attended.&lt;br/&gt;A week later, on May 9, three University of Chicago students, among many protesters unaffiliated with the University, were arrested for blocking the entrance to Citadel Headquarters, a hedge fund based in downtown Chicago. The students were participating in a rally led by FEI and IIRON against the Illinois budget crisis and Governor Bruce Rauner. The protest, urging advocacy for higher education funding, was directed at Sam Zell, James S. Crown, and Kenneth C. Griffin, significant donors to Rauner's super PAC and to the CSO.&lt;br/&gt;In response to the administration's lack of attendance at the May 2 public meeting, IIRON organized a protest on May 19. According to protest organizers, more than 150 students, staff members, and alumni participated in the rally calling for increased accountability and democratization of the University. Issues ranging from equitable policing to the University's divestment from fossil fuels were discussed.&lt;br/&gt;The protest consisted of a three-block march on the street from outside Ratner Athletics Center, through Hull Gate across the main quad, to Levi Hall. Before the protest, a group of 34 students and alumni had gathered to occupy the administrative lobby outside Isaacs's office once again until a meeting with the Provost was arranged. The sit-in lasted over an hour, and at 5 p.m. the participants joined the rally outside after the UCPD told them they could face disciplinary action up to suspension and expulsion or arrest if they remained, and escorted them out of the building.&lt;br/&gt;At Monday's Student Government General Assembly meeting, IIRON was finally able to speak to a top-level administrator. When Isaacs appeared before the General Assembly, activists associated with IIRON were ready with questions. They demanded yes or no answers, which Isaacs refused to supply. After a tense half-hour, Isaacs left. As for IIRON, the participants in the sit-in chanted "we'll be back" after they were expelled from Levi Hall on May 19, and this seems more than likely.</t>
         </is>
+      </c>
+      <c r="L25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1516,10 +1598,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="K26" t="inlineStr">
         <is>
           <t>Fifteen members of Reinvest Montana were cited with criminal espassing Tuesday after refusing to leave Gilkey Hall at its 5 p.m. closing time. The non-violent sit-in was in protest of the University's choice to continue using fossil fuels.&lt;br/&gt; As 5 p.m. rolled around the protesters began chanting and singing songs that became louder as closing time grew closer. Some chants called out Mack Clapp, chairman of the investment committee, although he wasn't in the building all day.About five police officers were in different parts of the building supervising the event.UM Police Chief Marty Ludemann said the sit-in was mostly legal because Gilkey is a public space but it isn't open to the public after hours.&lt;br/&gt;Chanting loudly is also not allowed in most buildings on campus."They've been pretty good all day so we're letting it go," Ludemann said. "But what they're doing right now is disrupting a business. If it would've been like this all day this would've been over at 9 a.m."At exactly 5, Ludemann stood in front of the protesters and asked them to leave. Ludemann said anyone who stayed past closing could receive criminal espassing citations as well as disorderly conduct citations, depending on the situation.Ludemann gave the group two minutes to decide whether they would leave or stay. Many students left after one final group hug from which someone shouted, "It smells like hippies!" Fifteen stayed behind to receive criminal espassing citations. Raphael Hagen, a senior at UM, was one of those protestors. Hagen said staying behind to get a citation showed how serious people are about divesting from fossil fuels. "This is important to us," he said. "It affects not just us, or some political group or some minority group, but everyone on the planet. I feel like this is the one social issue of our time that connects everybody."Although there has been no response from the UM Foundation or Mack Klapp so far, Justine Bright, with Reinvest Montana, said the group plans to stay firm with their request that UM divests from the top 200 fossil fuel companies and reinvest in more local and sustainable practices.Bright said Reinvest Montana has spent two years ying to affect change through the University's institutional channels. Bright said all the meetings and voting have gotten a response, but no actual changes have been made."We need to move past those institutional channels and take more direct action," Bright said. kasey.bubnash@umontana.edu@KBubnash</t>
         </is>
+      </c>
+      <c r="L26" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1559,10 +1644,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
+      <c r="K27" t="inlineStr">
         <is>
           <t>Holding signs reading "Carbon emissions - air pollution -  8 million deaths a year" and "Rhonda Cohen -  Board of Glenmede Trust -  $1 billion in Fossil Fuel Industry," 18 members of Mountain Justice, accompanied by Professor of Religion, Mark Wallace, staged a demonstration at the Philadelphia offices of investment and wealth management firm Glenmede Trust on Wednesday morning. Their aim was to expose the conflict of interest that they allege has unjustly clouded the ability of Rhonda Cohen '76, member of the college's Board of Managers, to impartially adjudicate on whether the college should divest from fossil fuels. Since 2008, Cohen has served on the Board of Directors of Glenmede Trust, which holds more than $1 billion in assets in the fossil fuel industry as well as $297 million in the Exxon Mobil Corporation. The Mountain Justice activists were escorted out of the Glenmede's lobby by the building's security, but continued their demonstration outside.&lt;br/&gt;"After finding out that several board members have direct ties to the fossil fuel industry, we felt that we needed to shed light on the situation, not only for transparency but because it is unjust that these persons were allowed to sit in on the decision making process last spring and stop divestment from fossil fuels at Swarthmore from going forward," explained Christopher Malafronti '18, a member of Mountain Justice. "This action was a direct result of those board members from refusing to recuse themselves from future conversations on divestment ... We were hoping to bring continued pressure on the board, specifically Rhonda Cohen, one of the board members with significant ties to the fossil fuel industry."&lt;br/&gt;Last fall, Mountain Justice's core organizers received information from Lil Sis, a free knowledge database, which indicated that Cohen, as well as Harold "Koof" Kalkstein and Samuel Hayes III, are tied to investment firms that hold a collective $3.6 billion dollars in assets in fossil fuel companies. Since then, the group since has staged several demonstrations at board meetings on campus, demanding that Cohen, Kalkstein, and Hayes III recuse themselves from all future board votes on divestment at the college in order to enable objectivity in the college's decision-making process. Despite Mountain Justice's efforts, however, neither Cohen, Kalkstein, nor Hayes III have stepped down.&lt;br/&gt;"Swarthmore's Board even has a conflict of interest policy stating that they should not vote on issues when they have financial conflicts of interest invested in the outcome," explained Sophia Zaia '18, a member of Mountain Justice. "It is unconscionable for board members like Rhonda Cohen to vote on divestment at Swarthmore ... This leaves us no choice but to escalate and ensure that the conversation on divestment from fossil fuels, an issue that leaves us literally without a moment to lose, are transparent and free from compromising financial conflicts of interest."&lt;br/&gt;Choosing Cohen as the target of their protest due to the close proximity of her office in Philadelphia, the 19 demonstrators assembled in the lobby of One Liberty Place, displaying their signs. Some were in costume for the theatrical interpretation of the alleged conflict of interest that the group planned to display, while others held signs or carried leaflets.&lt;br/&gt;"We knew we couldn't get upstairs ... so we were just going to do it in the lobby, but the security guards immediately came up to us and were like 'What are you doing? You can't do this here, we're going to call the police,'" Zaia explained. "I tried to talk to him, but he just immediately was like 'We're going to call the police' and we had told everyone that it wasn't an arrestable action or anything, so we went outside, and we just did the theatrical piece on the sidewalk."&lt;br/&gt;As a video livestreamed from the demonstration on Mountain Justice's Facebook page shows, demonstrators played out a scene in which Swarthmore students ask investigators why the board will not divest from fossil fuels, given the environmental damage caused by the fossil fuel industry.&lt;br/&gt;"It's not just a moral necessity, it's a financial one," says Jeremy Seitz-Brown '18, playing the role of a Swarthmore student. "Divesting will protect our endowment from plummeting fossil fuel stocks. We just don't understand why Swarthmore won't make this obvious choice that the Rockefeller's, the nation of Norway, and Stanford University have already made."&lt;br/&gt;As the scene plays out, other members of Mountain Justice playing the roles of investigators come to the conclusion that the Board's refusal to divest from fossil fuels is the product of its inability to impartially consider the issue, given Cohen's professional ties to the fossil fuel industry.&lt;br/&gt;"Board members can't make an objective decision on divestment if they have a personal financial stake in the fossil fuel industry," May Dong '18 says. "It is unconscionable for board members like Rhonda Cohen to vote on divestment at Swarthmore."&lt;br/&gt;"Swarthmore's bylaws say that Board members with conflicts of interest should recuse themselves from the vote," adds Shana Herman '19. "The fact that Rhonda Cohen sits on the board of a company with such large investments in the fossil fuel industry certainly appears to constitute a conflict of interest."&lt;br/&gt;The performance concludes with all of the Mountain Justice demonstrators shouting in unison, "Board member Cohen, recuse yourself!"&lt;br/&gt;Demonstrators then returned to the lobby of One Liberty Place - this time undisturbed by security guards - and sang two popular movement songs about climate change, which are often used by activists at larger demonstrations. The group concluded their demonstration, chanting "I believe that we will win," as suited professionals passed by, baffled.&lt;br/&gt;"This action was important because we continued to leverage the power built up last year to show the board that we are fully committed to divestment and are not going away," Malafronti explained.&lt;br/&gt;Zaia agreed, explaining that Mountain Justice planned to send Cohen a message about their demonstration in order to make sure that she was made aware of what took place in her firm's lobby.&lt;br/&gt;"I don't know how she'll react, but I would hope that she would take seriously the commitment that students have to ensuring that the conversation on divestment continues in a transparent way free of conflict of interest," Zaia explained. "But obviously, I really don't know how she'll react."&lt;br/&gt;The next meeting of the Board of Managers will take place on the weekend of May 6th and 7th, marking the one year anniversary of the board's decision to not divest last spring, but whether or not the board intends to vote on, or even discuss, divestment remains unknown. Neither the college administration nor the Board of Managers have yet to respond to Wednesday's demonstration, however, Zaia and her fellow Mountain Justice members hope that Cohen, Kalkstein, and Hays III heed the group's plea for increased fairness and objectivity on the board.&lt;br/&gt;"Climate change is one of the most urgent issues of our generation, threatening the lives of frontlines community members each day and actively making our planet uninhabitable," Zaia explained. "We cannot sit idly by as our college continues to align itself with an industry that is literally incompatible with our future on this planet, despite a mandate from our community and the clear urgency of ceasing to legitimize companies who ... lie and deceive the public."</t>
         </is>
+      </c>
+      <c r="L27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1602,10 +1690,13 @@
           <t>Trump and/or his administration (Against)</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
+      <c r="K28" t="inlineStr">
         <is>
           <t>Nearly a thousand people gathered on the Diag and marched through University of Michigan buildings for a student walk-out protest against racism on campus following President-elect Donald Trump's upset win Wednesday afternoon, briefly shutting down traffic. &lt;br/&gt;The walkout, which was organized by the student organization Students4Justice, was also attended by civil rights activist Rev. Jesse Jackson and was part of a national movement of walkouts across the country. &lt;br/&gt;"This walkout is a national movement that is happening in response to the election, as well as the increase in hate crimes and other forms of violence against marginalized (folks)." the event description says. "We are doing this to hold President Schlissel and our Regents at the University of Michigan accountable for their claims of valuing diversity and student safety and well-being."&lt;br/&gt;Prior to the event, Students4Justice also released a list of demands that they hoped to achieve from the protest.&lt;br/&gt;Protest crowded into @MichiganRoss pic.twitter.com/3dynl46Gm1&lt;br/&gt;- Emma Richter (@emma__richter) November 16, 2016&lt;br/&gt;The demands include calls for University action to protect underrepresented minority students by re-channeling resources, as well as a call for the University to become an immigrant sanctuary site, to double its commitment to rejecting racial harassment, to divest from unethical corporations and to remove all symbols and fliers associated with the alt-right movement and those encouraging white supremacy.&lt;br/&gt;LSA junior Lakyrra Magee, one of the event organizers, highlighted the call to make the University a sanctuary campus - a designation that would empower the University to limit institutional cooperation with federal immigration officers seeking undocumented students- as among the most significant demands.&lt;br/&gt;"Thanks for standing up and fighting back" - Rev. Jesse Jackson pic.twitter.com/4AAYdNvx3A&lt;br/&gt;- Matt Harmon (@MattHarmon20) November 16, 2016&lt;br/&gt;Protesters also cited a number of recent campus concerns during the walkout, including the two hate crimes in downtown Ann Arbor that have been reported to police since Trump's presidential win last week. On Friday, a woman was threatened and forced to remove her hijab. On Saturday, a woman was pushed down a hill and verbally harassed. Additionally, many speakers discussed anti-Black, anti-LGBTQ and anti-Muslim posters, many of them promoting themes of white supremacy, that have been found posted on campus several times in the past few months.&lt;br/&gt;LSA junior Alyiah Al-Bonijim spoke to the crowd about her frustrations with Islamophobic comments triggered by her choice to wear a hijab.&lt;br/&gt;"For what? Because you want to see my hair? Is that what is important to these fucking white people?" Al-Bonijim asked the cheering crowd, saying that forcing a woman to take off her clothing, including the hijab, was sexual assault.&lt;br/&gt;University student on hate crimes towards Muslims wearing hijabs from last week @michigandaily pic.twitter.com/VzchH4CHEK&lt;br/&gt;- Nisa Khan (@mnisakhan) November 16, 2016&lt;br/&gt;Protesters also touched on the failure of a Central Student Government resolution Tuesday night to divest from corporations that have allegedly committed human rights violations against Palestinians. Many in the crowd yelled negative chants about CSG during the walkout. &lt;br/&gt;"You don't represent me." Palestinian student criticize @umcsg for not passing #umdivest resolution last night. pic.twitter.com/ePE4Q3JLBZ&lt;br/&gt;- Nisa Khan (@mnisakhan) November 16, 2016&lt;br/&gt;Following their initial assembly on the Diag at 3 p.m., with many students walking directly out of classes, the protesters marched throughout Central Campus, also entering buildings and encouraging others to join them.  &lt;br/&gt;As the march moved through campus, student organizers, as well as Jackson, led the crowd in a number of chants condemning racism, sexism, islamophobia and xenophobia.&lt;br/&gt;Chants included slogans such as: "No justice, no peace," "Hey Hey, Ho Ho, these racist folks have got to go," "No Alt-Right, no KKK, no fascist USA" and "Black Lives Matter."&lt;br/&gt;"Thanks for stepping up and fighting back," Jackson told the crowd. "Do not let any election oppress your dreams ... Red, yellow, black and white, you are all precious in God's sight. We must learn to live together. This land is a land of multiculturalism."&lt;br/&gt;Chanting with the crowd, he expressed solidarity with individuals who have felt marginalized in the past months, including Black, Muslim and Mexican-American students.&lt;br/&gt;"We are all sanctuary," he said. "We love each other. We care for each other. You take one of us, you must take all of us. We are not going anywhere. This land is our land. We will outlast the meanness, we will outlast hate. We will outlast violence. Love will conquer hate."&lt;br/&gt;After walking through several buildings, a brief moment of silence was held at Burton Memorial Tower, during which students told stories about their own personal struggles. At the end of the walkout, organizers asked for white supporters to block State Street so protesters could safely gather at Angell Hall for a speakout.&lt;br/&gt;Students blocking road, car honking and surrounded pic.twitter.com/ZmcLxNsazZ&lt;br/&gt;- Emma Richter (@emma__richter) November 16, 2016&lt;br/&gt;During the protest, white students were asked by organizers to peacefully block the roads and talk to the police to protect the lives of brown and Black people, who organizers said were more likely to be targeted at student gatherings. Rackham student Vikrant Garg, a walkout organizer, asked for a nonviolent protest and for all students involved to march peacefully.&lt;br/&gt;"We see a lot of white folks here," he said. "We need you on the sidelines to protect us ... there are going to be parts where we shut down the street. We need you all to be there to protect us. This is nonviolence, we recognize that violent acts you may commit will, in the end, hurt us the most."&lt;br/&gt;The walkout is one of the largest events to take place after the election on campus. On election night, an impromptu vigil consisting of roughly 30 students coalesced on the Diag at about 3 a.m., an hour after Trump was declared victorious. The next night, a vigil attended by about 1,000 students took place, during which University President Mark Schlissel and CSG President David Schafer, an LSA senior, called for campus unity and inclusivity. Multiple protests against the president-elect and in reaction to the hate crimes has since occurred. &lt;br/&gt;At the walkout, LSA junior Victoria Johnson said she came to the event to help draw the administration's attention about the problems facing minorities on campus.&lt;br/&gt;"These problems have been boiling up for a long time - this isn't anything new," she said. "But I think the election, I think what happened, has been tipping the scale. Now these people who have always been against the rights for me and my rights and who I stand as a person, my identity. They feel empowered to speak out and act on these hateful feelings they have. And that's why I am here, because my rights are at stake. And not just my rights, but my safety. And I feel like it's important to make the University be held accountable for it all." </t>
         </is>
+      </c>
+      <c r="L28" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1645,10 +1736,13 @@
           <t>University governance, admin, policies, programs, curriculum, Anti-racism, Campus climate</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="K29" t="inlineStr">
         <is>
           <t>In the past two years, the University of Michigan has seen several acts of hate targeted at people of color and minority groups across campus.&lt;br/&gt;In September 2016, flyers advocating white supremacy were found on campus posting walls. In February, engineering students received racist and anti-Semitic emails from hacked email accounts. This September, the Rock, a campus landmark, was found graffitied with anti-Latino and pro-Trump expressions. In October, racist slurs were found on the residence hall doors of three Black students in West Quad Residence Hall.   &lt;br/&gt;In the aftermath of these incidents, campus communities have not stood idly by. Hundreds of students have rallied against racist flyering, graffiti and a variety of other attacks. In late September, Rackham student Dana Greene knelt in the Diag for 21 hours to protest racism on campus and across the country; dozens of other students joined the peaceful protest.    &lt;br/&gt;The University administration has taken steps to respond to acts of hate and its historically low minority enrollment. In October 2016, the University launched its five-year Diversity, Equity and Inclusion strategic plan, which aims to foster a diverse and inclusive campus, while also supporting inclusive scholarship and teaching. Diversity has been especially difficult in the University, since practicing affirmative action has been banned in the state since 2014 despite the University's attempts to appeal the vote.  &lt;br/&gt;When the plan was implemented, then-Provost Martha Pollack, who is now the president of Cornell University, said the recent racist incidents only emphasized the need for the plan.&lt;br/&gt;"It's only human to respond with anger and sometimes with fear, emotions that have been felt deeply on this campus," she said. "I share the grief and outrage felt by our students, faculty and staff. We must cling to the vision of what the world must be ... and that is what the Diversity, Equity and Inclusion plan is all about."&lt;br/&gt;However, also pertinent to DEI, the University ranked last in terms of socioeconomic mobility and diversity among top public universities. According to a report by the Equality of Opportunity Project, which was highlighted by The Upshot - a data analytics section of the New York Times- 66 percent of students come from the top 20 percent of the income distribution and students have the highest median family income of 27 "highly selective" public colleges.&lt;br/&gt;The DEI plan has been criticized for failing to foster a diverse environment and for failing to put a stop to racist incidents. After the racist emails were sent out in February, students protested outside University President Mark Schlissel's house calling for "action, not emails," referencing the University's digital statement, which showed its support for those attacked, but no further action.&lt;br/&gt;"Schissel WYA" is a common rally of for University students, criticizing University President Mark Schlissel's response to the incidents. In mid-September, students gathered in front of the president's home and posted flyers on his door. Schlissel was at a family event during this time.&lt;br/&gt;Postdoctoral fellow Austin McCoy was not surprised by the University's response.&lt;br/&gt;"From the administration, I anticipate them sending out probably an email and saying that they condemn the acts and then that they're investigating, but other than that, I don't know what else the administration plans to do," he said in February. &lt;br/&gt;However, such incidences and responses are not unique to the University of Michigan campus. Post-election, campus climate and rallying students have been points of debate across the country.&lt;br/&gt;Conservative criticism refers to liberal students as too sensitive and ignorant of free speech - worried for conservative students and their lack of voice on more Democratic campuses. The University of Chicago even shut down the concept of "safe spaces" - sparking what some call a clear rebuke of political correctness. Liberal students, however, hope to protest the turn of the administration along with the fear of rhetoric that they deem bigotry and do not wish to give such thought a platform.&lt;br/&gt;This article is part one of a series in which The Michigan Daily looks at colleges similar to the University of Michigan on the issue of reacting in a tense campus climate. As the University administration and students face their own numerous bias incidents, The Daily will look at other schools to compare and contrast in incidents, administration response and student activism, whether it is a difference in religion, culture, politics or policies.&lt;br/&gt;Cornell University&lt;br/&gt;Juliana Rosana Montejo graduated from Cornell University in May 2017. Montejo is Guatemalan and came from a predominantly white high school. She said when she entered the university in 2013, she wasn't really aware of incidents on campus.&lt;br/&gt;"Long story short, every semester there has been something," she said.&lt;br/&gt;Cornell University, located in Ithaca, N.Y. - a blue state - ranks similarly to the University of Michigan in terms of the Upshot's SES status - albeit in the private school category among other Ivy Leagues. Out of 14,907 undergraduate students, Cornell has 6,462 students of color - 43.34 percent. In the graduate program, it is 17.94 percent. Cornell also uses affirmative action in admission.  &lt;br/&gt;In fall 2013, a campus organization that promotes Cornell sporting events attempted to increase support for an upcoming football game by creating a "Cinco de Octubre" event, which incorporated racist caricature depictions of Mexican Americans. Montejo said there was a prize given to whoever dressed up as the "best Mexican."&lt;br/&gt;Since then, Montejo said, there have been a variety of incidents that have primarily targeted Black people and people of color generally. She said she met many people involved with activism at Cornell and in her senior year, she served as vice president of diversity and inclusion on the Cornell Student Assembly.&lt;br/&gt;"A big part of why I started getting more involved was that there had just been a lot of things building up, and I think we were kind of at a culmination of, 'Oh there were some of these undertones there already,' and now it's kind of coming to a point where it's kind of exacerbated," she said.&lt;br/&gt;Montejo also said such hateful incidents became more prevalent after the 2016 election. She explained Cornell is known to be a liberal school; subsequently, there is a claim that conservative ideas are oppressed on campus.&lt;br/&gt;"The conversation wasn't automatically, 'What can we do for people of color?'" she said. "A lot of it became, 'Look at these poor conservative students who aren't able to speak their minds.'"&lt;br/&gt;She said at the end of 2016 and in early 2017, there were two resolutions brought before the student assembly to create task forces to investigate why there are so many liberal professors at the school. There have also been calls for the university to do more to protect conservative speakers who come to campus. She said there have been more visibly proactive actions to help conservative students.&lt;br/&gt;Montejo also said that whereas prior to the election, there seemed to be one or two major acts of hate every semester, there is now something happening all the time.&lt;br/&gt;Last month, a Cornell student was arrested by Ithaca police for a hate crime, according to the The Cornell Daily Sun. A Black student, who asked to remain anonymous, told the Sun he confronted four or five white men who were shouting racist slurs at him; they then proceeded to beat him.&lt;br/&gt;In Michigan, during one of the protests after the racist vandalism, an individual was punched by a white man who also called them racial slurs.&lt;br/&gt;Black Students United at Cornell released a statement saying the perpetrators were members of the Psi Upsilon fraternity, which already had its recognition revoked on campus. The building is to be remade into a multicultural center.&lt;br/&gt;Pollack, now Cornell's president, released a statement in response to the incident - and others preceding it - citing steps the administration will take to create a more equitable and inclusive campus. Among them was a promise to take disciplinary action against the perpetrators of the aforementioned attack and a commitment to not reinstating the fraternity.&lt;br/&gt;"I will not tell you 'this is not who we are,' as the events of the past few weeks belie that. But it is absolutely not who we want to be," the statement read. "The leadership team and I have been working throughout the weekend, and we will continue to do so, to develop and implement steps to be a more equitable, inclusive and welcoming university."&lt;br/&gt;Meanwhile, Black Students United declared a "state of emergency for black students" in response to the incident. The group blamed the university for creating the Campus Code of Conduct, which protects white supremacists' hate speech. They recognized it would be difficult to change the policy but felt it would be possible with help from the greater university community.&lt;br/&gt;In mid-September 2016, Black Students United handed a list of demands to Pollack, including racial sensitivity training for all employees and a space for Black students on campus.  &lt;br/&gt;Prior to creating an official list, Black Students United members met with Dean of Students Vijay Pendakur right after the assault. They were frustrated Pollack did not reach out to them until three days after the assault; they were also frustrated that many of the ideas they brought up in their meeting with Pendakur were presented in Pollack's letter, without recognition. &lt;br/&gt;Anti-Semitic posters have also been seen on Cornell's campus and Pollack has denounced these incidents as well.&lt;br/&gt;Looking at responses to acts of hate on Cornell's campus overall, Montejo said there appears to be a lot of support.&lt;br/&gt;"In terms of climate change I think to your face it seems like there's a lot of support," she said. "But behind the scenes, there's a lot of weird antagonism that's going on."&lt;br/&gt;Beth Garrett, Cornell's thirteenth president, passed away after a battle with colon cancer in March 2016. However, according to Montejo, when Garrett came into office she hired Ryan Lombardi, vice president for student and campus life. According to Montejo, Lombardi re-envisioned the Office of the Dean of Students and the dean of students position as one that would be very focused on diversity and inclusion issues.&lt;br/&gt;Additionally, she said Cornell has used polls to gauge how students feel about diversity and inclusion issues - the University has also had campus climate polls - and has always addressed campus climate even without major incidents occurring. Cornell has diversity officers through its Diversity and Inclusion initiative to better promote a welcoming and inclusive campus, as well as a bias reporting program.&lt;br/&gt;Montejo explained the administration always sends out statements to the campus community in response.&lt;br/&gt;Montejo noted Ivy League schools are definitely targeted. In November 2015, for example, hundreds of members of the Yale University community marched in support of minority students who felt they were not fully included on campus. According to The Washington Post, protesters rallied in support of women of color, faculty of color and ethnic studies; one person carried a sign that read: "Your move Yale."&lt;br/&gt;The theory that prominent, progressive schools are being targeted has floated around before - especially with Washtenaw as a blue county in a newly turned red state. In an earlier interview with The Daily, Schlissel said there might not be a way to mitigate the target on the University's back.&lt;br/&gt;"I think that part of being a prominent university, taking clear positions on things, having large numbers of very successful graduates out there in the world, being on TV all the time, being in the media all the time means that what happens here gets noticed," he said. "That's the sort of other side of this double-edged sword of being famous and prominent. ... It's because of our prominence that provocateurs realize they can use us as a platform that the national media will pay attention to, to spread their terrible, thoughtless, degrading, awful ideas. They're using us."&lt;br/&gt;Montejo said she believes Cornell is generally diverse. According to Cornell's Composition Dashboard from fall 2016, 39.5 percent of undergraduates were white, while 42.3 percent were from minority groups. Despite that, she said groups that have disproportionate power on campus include those that are white, including the Interfraternity Council.&lt;br/&gt;"I felt really compelled and pushed to join a Panhellenic sorority, and while I had a great experience there, it did kind of feel like there was a disproportionate amount of influence of power in that structure because of its whiteness," she said.  &lt;br/&gt;Though the administration has taken a lot of positive steps, Montejo said there are gaps that need to be filled. She said she feels there is a lot of movement on reactive measures but not nearly as much around proactive members.&lt;br/&gt;In an email response, Cornell's Media Relations Office pointed The Daily to several of its official statements.&lt;br/&gt;University of California at Berkeley&lt;br/&gt;Some say Berkeley has been the poster child of college campus activism this year - the pushback against controversial speakers has been widely documented in the media. Notably, while activism has escalated to violence, much of it has occurred in the campus vicinity, not specifically at the university.&lt;br/&gt;Billy Curtis is the director of the Gender Equity Resource Center at University of California at Berkeley. Strictly in terms of reports, Curtis said, there has been an uptick, but quickly explained that like with incidents of sexual violence, as there are increases in education and awareness, there are more reports. It's unclear whether there are more incidents or more reports.&lt;br/&gt;Another challenge UC-Berkeley faces, according to Curtis, has to do with protocols for a response. Many victims and members of communities that are targeted feel the chancellor needs to respond.&lt;br/&gt;"We're trying to figure out always, when does the chancellor respond? What does that response look like? How do people feel cared for, seen, heard, tended to?" he said. "I think that's the biggest challenge because too often what we're really dealing with isn't necessarily just a campus climate issue, we're dealing with our sociological problems of the United States."&lt;br/&gt;UC-Berkeley is taking steps to make the campus more inclusive and address the needs of students from marginalized communities. The Division of Equity &amp; Inclusion provides a variety of programs and services.&lt;br/&gt;On Sept. 1, the division launched the Campus Climate, Community Engagement and Transformation unit, whose mission is to focus on "reshaping and influencing policies and practices that increase opportunities, advance social justice and create equitable experiences for all groups, with a special focus on marginalized and underserved populations."&lt;br/&gt;The initiative's website also highlights results of a spring 2013 campus climate survey, which showed 1 in 4 community members have experienced exclusion on campus. It also showed undergraduates who are not African American overestimate the inclusivity of the climate for the group. For instance, 89 percent of Asian students and 87 percent of white students rated the climate as "respectful" or "very respectful" for African Americans; African Americans rated the climate as 47 percent for the categories. Additionally, on the survey, a top concern was not having channels through which to report discrimination and the notion that faculty judge students based on their perceived identities.    &lt;br/&gt;That being said, in fall 2017, 2.9 percent of enrolled freshmen at UC-Berkeley were African American or Black, 9.9 percent were Mexican American or Chicano, 3.7 percent were labeled "other Hispanic/Latino." White students constituted 24.5 percent of the freshman class.&lt;br/&gt;Other initiatives through UC-Berkeley's diversity division include a Campus Climate Speaker Series, which brings scholars and activists to campus to address related issues, and Innovation Grants, which provide funding for projects focused on increasing equity and inclusion on campus.&lt;br/&gt;Still, UC-Berkeley has seen hate acts in the past year. In September, posters listing 13 specific community members and identifying them as "terrorist supporters" were found on campus, according to The Daily Californian. Some of the victims in the past had vocalized their support for Palestinian divestment from Israel.&lt;br/&gt;In a statement sent to the university community, UC-Berkeley Chancellor Carol Christ condemned the acts. She highlighted the school's Principles of Community, among which are a commitment to respect the differences and commonalities of all people.&lt;br/&gt;"Berkeley is better than what these incidents reflect," the statement read. "Many things contribute to the fact that we are the nation's number one public university, and a strong component is the care, respect and esteem which we have for our fellow campus community members. As we move into the events of next week, please join me in upholding these values."&lt;br/&gt;Four days after the posters were found, conservative writer Milo Yiannopoulos spoke at Berkeley. According to The Daily Californian, Yiannopoulos was originally invited to speak by the student group the Berkeley Patriot - a conservative group on campus - as part of the "Free Speech Week," in which several conservative speakers were coming to campus. Amid confusion surrounding the event and the Berkeley Patriot actually filing a complaint with the Department of Justice, claiming Berkeley was infringing free speech rights, the event was canceled. Still, Yiannopoulos - and other speakers - came to campus and were met by a crowd of protesters.&lt;br/&gt;In an interview with The Daily Californian, Pranav Jandhyala - a news editor for the Berkeley Patriot and who founded the organization that invited Ann Coulter - explained the situation became too complicated and the group had to pull out of the event.&lt;br/&gt;"It became a situation that we just had to get out of because of the complications," Jandhyala said.&lt;br/&gt;Meanwhile, the Yvette Felarca, an organizer for Berkeley's By Any Means Necessary pointed to the need for a sanctuary space.&lt;br/&gt;"To protect the community (and make) it a sanctuary campus, that means actively defending it," Felarca said.&lt;br/&gt;The University faced its own slew of controversial speakers - the latest being Charles Murray, known for "The Bell Curve," which argues the correlation of IQ and race. McCoy said speakers like Murray use student anger as a platform.&lt;br/&gt;"I'm not really going to say much about what's his name -- Charles Murray -- I don't really care about Charles Murray, I think he's irrelevant," he said. "I think he's just trying to use protests, I think he's trying to use student anger to rebuild his career. So, think about this. He has to use students to get a come-up."&lt;br/&gt;LSA senior Ben Decatur, co-chair of the AEI Executive Council at the University, defended Murray's right to speak on campus.&lt;br/&gt;"If the hosts of tonight's program, in collaboration with University representatives, believe that the protesters are interfering unduly with the speaker's freedom of expression, those protesters will be warned by a University administrator," Decatur said. "If warnings are not heeded and interference continues, the individuals responsible may be removed from the building."&lt;br/&gt;Berkeley freshman Justin Kim serves on the Hall Association at UC-Berkeley. In an interview with The Daily, he described the controversy surrounding Yiannopoulos's visit to campus. He said there were police and blockades for the entire week around Sproul Plaza, where the event took place.&lt;br/&gt;In terms of how the school responds, Kim explained the Berkeley Police Department and administration have worked together to send email advisories about crimes on campus to the community.&lt;br/&gt;"During Free Speech Week, or when it was supposed to happen ... even leading up to it, we got notifications to avoid the area," he said.&lt;br/&gt;He noted that Christ released a statement, which stated the university is committed to free speech, as exemplified by the speakers on campus, even though they put forth ideals that "run counter" to those of the university.&lt;br/&gt;"To provide the security necessary to protect the community, we have had to close buildings, relocate students and workers, bring to campus a police presence that some find intimidating, and spend money that we would have much rather put toward our academic and research mission," the statement read.&lt;br/&gt;Kim explained earlier in the fall there was an event in which UC-Berkeley students could ask Christ any question. There is also a way for students to write letters to the chancellor, which are directly delivered by the president of the Associated Students of the University of California - the UC-Berkeley student government.&lt;br/&gt;Regarding hate acts and the reactions they prompt, Curtis explained the campus climate shifts based on the level to which the incident rises.&lt;br/&gt;"Someone writing something on a residence board in a residence hall on one floor, I may be aware of it, but it usually doesn't rise to the level of impacting a larger community because it's a one-off - unless there are enough instances in the residence halls that are targeting folks, and students are feeling like, 'Wow, there's a lot of racist things, or a lot of anti-Semitic things said,' and that's happened over the years," he said. "But all of a sudden it starts to bubble up."&lt;br/&gt;Graffiti on a building, he explained, will rise to different levels because it is far more public and more people see it. He said it creates a different level of response.&lt;br/&gt;Curtis also noted UC-Berkeley has been in the media as a result of certain speakers coming to campus and impacting the campus climate. Students, for example, can report that they feel unsafe and unwelcome on the campus in response to an event like that.   &lt;br/&gt;He explained that while many programs and offices work to educate the campus and make it more safe, inclusive and accessible for marginalized groups, racism and other forms of bigotry are still prevalent in the United States. Due to a variety of reasons, he explained, the campus climate changes.&lt;br/&gt;"It's not static, we're not working in a place where everyone remains the same forever more, or there's little turnover," he said. "We have large turnover because our student body turns over, and they're coming from their communities and their experiences ... and in the modern era - the modern era of information and social media - we're now impacted by things that happen in the virtual world. The things we may create on campus don't necessarily stop or even mitigate the stuff around hate and bias acts; (the two) can work in concert but I've not seen it stop."</t>
         </is>
+      </c>
+      <c r="L29" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1688,10 +1782,13 @@
           <t>University governance, admin, policies, programs, curriculum, Environmental, Police violence/anti-law enforcement/criminal justice</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
+      <c r="K30" t="inlineStr">
         <is>
           <t>Group will present the board with a petition demanding the College divest from fossil fuels.&lt;br/&gt;Students will demonstrate from 5-7 p.m. this evening in the Peirce Dining Hall atrium, urging the College to divest from fossil fuels and pledge to never invest in private prisons. The rally, organized by DivestKenyon - a group that advocates divestment from fossil fuels and private prisons - will involve speeches by members of various social justice organizations, live music by Kenyon a capella groups and the recitation of pro-divestment chants. &lt;br/&gt;The demonstration's intended audience is the Board of Trustees, which is gathering on campus today and tomorrow for their annual spring meeting. Joseph Lipscomb '87, the chair of the budget, finance and audit trustee committee and vice chair of the executive trustee committee, is meeting with the Kenyon Democrats to discuss investments at 4 p.m.  today in the Alumni Dining Room. He will emerge from this meeting into the student-organized protest.&lt;br/&gt;"The point is that it'll be too big to miss and to show that students care about fossil fuel divestment and not investing in private prisons," Matt Meyers '17, a leader of the DivestKenyon movement, said.&lt;br/&gt;During the meeting with Lipscomb, representatives of DivestKenyon also plan to deliver a petition demanding that Kenyon remove investments from the top 200 fossil fuel companies and formally agree to not invest in the top two private prison corporations, the GEO Group and Corrections Corporation of America. The petition had received more than 790 signatures as of Wednesday evening; twenty-two of these signatures are professors and administrators.&lt;br/&gt;Following the protest, approximately 50 students will camp out overnight on Ransom Lawn in front of Peirce.&lt;br/&gt;"All school rules will be followed," Katherine King '17, another leader of the DivestKenyon movement, said. "There's going to be opportunities there for people to learn more about divestment."&lt;br/&gt;DivestKenyon members presented their proposal to divest from fossil fuels last October during a meeting with the Investment Committee.&lt;br/&gt;Lipscomb, who is a co-founder and partner at Arborview Capital LLC, an organization that invests in clean energy and sustainability companies, attended the meeting. He said he appreciates students' enthusiasm about climate change, but does not feel divestment is a productive approach to solving the issue.&lt;br/&gt;"I just don't think that we're at a point where that's feasible today for a small endowment like Kenyon," Lipscomb said. "We basically have $360 million of investable assets."&lt;br/&gt;Approximately seven percent of the College's endowment is invested in the energy industry, according to Vice President for Finance Todd Burson. CornerStone Partners, the College's endowment manager, declined to comment for this article, but Burson agreed to send questions from the Collegian to the firm.&lt;br/&gt;"They will not be able to secure a list of all of the individual investments, as some investment managers keep that information confidential," Burson wrote in an email to the Collegian.&lt;br/&gt;"What we have been told is that, in 2016, we had about five percent of our endowment invested in fossil fuel infrastructure and another three percent in fossil fuel companies," Meyers wrote in an email to the Collegian. "If we were to divest from fossil fuels, the board and our investments managers would make a plan to negatively screen fossil fuel investments out of our investment portfolio."&lt;br/&gt;Meyers said this does not mean the College would lose eight percent of its endowment: The money would be reallocated to other investments.&lt;br/&gt;The Collegian was unable to verify these numbers, but President Sean Decatur stated that the College does invest in some funds that have holdings in the fossil fuel industry.&lt;br/&gt;Lipscomb supports investing in green initiatives rather than pulling money out of fossil fuel investments. Despite the board's decision not to discuss divestment, they will examine future investments in environmental initiatives.&lt;br/&gt;A group of students and student interns working with Director of Green Initiatives David Heithaus presented suggestions for a "Green Revolving Fund," which would set aside funds for green initiatives across campus, to Decatur and senior faculty Monday, April 10. The board will not discuss this during their meetings, according to Decatur.&lt;br/&gt;"The next step is for us to refine the proposal's details - which projects to pursue ... as well as a plan to finance them," Decatur wrote in an email to the Collegian.&lt;br/&gt;Heithaus does not see divestment and the proposed GRF as mutually exclusive projects. "Divestment would be one of many ways money could be raised or allocated to seed a GRF," Heithaus said.&lt;br/&gt;King and Meyers want to emphasize that DivestKenyon's mission is linked with a larger national divestment movement aimed at changing the behavior of corporations.&lt;br/&gt;"The purpose of divestment is to stigmatize these corporations," King said. "You do divestment in conjunction with major movements. We're doing fossil fuels and private prison divestments because that's what ... the energy is building around."&lt;br/&gt;Burson noted that Investment Committee members have discussed green initiatives at length.&lt;br/&gt;"In April 2013, a group of students met with the Investment Committee to express their desire for divestment of fossil fuel companies," Burson said. "[The Committee] decided at the end that it would not be appropriate to divest but that the students and the College should continue its focus on making structural changes on the campus."&lt;br/&gt;Spurred by this conversation, the College spent $7.5 million on campus-wide energy conservation efforts to reduce use of water, gas and electricity. The College also began to compost food waste and require that recent building projects are LEED certified, meaning they use fewer resources and reduce greenhouse gas emissions.</t>
         </is>
+      </c>
+      <c r="L30" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1731,10 +1828,13 @@
           <t>Pro-Palestine/BDS</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
+      <c r="K31" t="inlineStr">
         <is>
           <t xml:space="preserve">When students launched the Barnard Columbia Solidarity Network last year, they sought to put into practice principles of solidarity between movements and work against forms of oppression using an intersectional framework. The guiding principle of this coalition was that all forms of oppression operate in interrelated ways and thus must be fought together. Although BCSN sought to foster solidarity among campus activists, its inclusion of Students for Justice in Palestine and Jewish Voice for Peace incurred virulent criticism as some argued that the pro-Palestinian groups created a hostile environment for students who support Israel.&lt;br/&gt;We, members of Columbia University Apartheid Divest , were left asking: why should recognition of intersectionality exclude Palestinians? How could one, in good conscience, ignore racism, sexual violence, environmental racism, and colonialism in the context of Israel/Palestine? When students are made aware of this double standard, they will often say that they simply don't know enough to take a stance. This widespread belief-that entitlement to an opinion requires exhaustive knowledge of the Israeli occupation of Palestine-keeps many students out of the conversations we in CUAD try to encourage on campus.&lt;br/&gt;Moreover, the misleading and divisive narrative of "us vs. them" that attends dominant discourses surrounding Israel/Palestine activism intimidates students and activists with the implied accusation that any engagement at all amounts to full endorsement of one side or the other. Either afraid of negotiating or believing themselves unable to negotiate these polarizing stances, students retreat to a position of presumed "neutrality," a non-stance amounting to little more than tacit support for the status quo: occupation, dispossession, and apartheid. "Neutral" silence has become a powerful tool wielded by Zionists in their effort to bolster the hegemony of Israeli apartheid and dissuade dissenting voices. From hard-right Zionist groups such as AIPAC to student Hillel chapters, the discourse about Israel/Palestine at Columbia is in need of dramatic recalibration.&lt;br/&gt;We put on events for Israeli Apartheid Week to create a space for learning and growing, not hostility. Activism is a process, one that is shared between all groups organizing against oppression and one that asks for the participation-at whatever capacity-of those who might not call themselves "activists." Without engaged people seeking new information, dialogue on campus becomes a repetitive cycle of attack between the "two sides."&lt;br/&gt;As part of our work this Israeli Apartheid Week, CUAD will present a resolution to CCSC calling for divestment from companies that participate in Israel's occupation of Palestine and the government's continued human rights abuses. If 10 percent of the CC student body signs our petition supporting the resolution, CCSC will be obligated to put the resolution to a vote for the entire Columbia College student body. The resolution seeks to end our University's support for corporations that engage in and profit from human rights violations in Israel/Palestine.&lt;br/&gt;Education and dialogue during Israeli Apartheid week are essential to the resolution vote. This is our way of honoring the Palestinian call to BDS (Boycott, Divestment, Sanctions). BDS, with its three simple demands, is an effective tactic for pressuring the Israeli government into abiding by international law. It is a tangible way to empower everyone, from consumer to politician, to end apartheid.&lt;br/&gt;There is a new administration in Washington, and a staunch supporter of illegal settlement building has been nominated to be the new US Ambassador to Israel. Now more than ever it is incumbent upon us to fight for institutional support in the struggle to end the well-documented violations of human rights in Palestine. To do so means both to learn and to act simultaneously. We hope Israeli Apartheid Week will serve this purpose. This week, featuring events every night, and our mock Apartheid wall on Low Plaza every day, is an essential moment in our movement and an excellent opportunity for students to learn about Israel/Palestine.&lt;br/&gt;The United States has witnessed the consolidation of power by some of the country's most overtly corporate, racist, and authoritarian forces in the past few months. The supposedly neutral stance on Israel/Palestine may have felt comfortable for people in the past, but it now becomes impossible to uphold if we are at all opposed to what is happening in the United States-the Muslim ban, the Dakota Access Pipeline, police brutality and the reinstatement of Jim Crow-era voting laws in some states. It has been heartening to see so many in the United States come together-in the streets, at town hall meetings, on campuses-to reaffirm our basic principles of equal protection under the law. Right here in Morningside Heights, students, faculty, staff, and administrators have recommitted to the principles of sanctuary. In this fraught moment, it is especially important that we affirm our insistence that basic human rights are not limited by zip code, religion, or national identity, but that they are fundamental rights for all individuals. This is what we, as CUAD members, fight for this week and every week.&lt;br/&gt;Columbia University Apartheid Divest is a coalition between Students for Justice in Palestine and Jewish Voice for Peace .&lt;br/&gt;To respond to this op-ed, or to submit an op-ed, contact </t>
         </is>
+      </c>
+      <c r="L31" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1774,10 +1874,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr">
+      <c r="K32" t="inlineStr">
         <is>
           <t xml:space="preserve">Tents were pitched in front of Wilson Hall on the Quad while students played guitar, enacted skits and talked through the night. The last time students camped out on the Quad, they were trying to get on TV for College GameDay. This week, students did it in the name of protest.&lt;br/&gt;Amelia Morrison, a junior geographic science major, was one of these students. Morrison's the community outreach chair in the Climate Justice Coalition, a group that was protesting JMU's investment in fossil fuels. &lt;br/&gt;"When I'm out here educating people, getting people aware and going to marches, doing civil disobedience - I feel like I'm doing something, and that makes me feel less powerless," Morrison said.&lt;br/&gt;The Climate Justice Coalition was originally founded to formally encourage JMU to stop using money from its endowment for fossil fuels.  &lt;br/&gt;The endowment consists of donations individuals give to the university, not including tuition, and is supposed to be used to grow and improve the university.&lt;br/&gt;"Our stance is that we don't want the university to be growing off of the profits of the fossil fuel industry, because it's destructive to people and the planet," Morrison said.&lt;br/&gt;As the most recent event in a series of protests, the Climate Justice Coalition staged a campout on the Quad this week, with intentions to stay there from Monday morning until whenever they were asked to leave. Camping on campus is a violation of the student code of conduct. &lt;br/&gt;They tried to camp out Sunday night, but were asked to leave by JMU police around 1 a.m., so they got formal permission for Monday night's campout. The JMU police periodically checked on them throughout the night to make sure they were safe.&lt;br/&gt;The Climate Justice Coalition chose CHOICES, April 10, for their protest to gain the attention of both current students and prospective students.&lt;br/&gt;"I think it actually had a positive impact for our families," Anna Boley, the visitor relations coordinator, said. "I think it was great for them to kind of see involvement of some of our students. It was a great display of how a passionate group of students is taking action and sharing their opinions on campus, and we definitely encourage that and welcome that on campus."&lt;br/&gt;In addition to this protest, the Climate Justice Coalition held a campaign asking people not to participate on JMU Giving Day until the university divested. The organization hoped that campaigns like this would raise awareness of JMU's investments.&lt;br/&gt;Paul Campbell, the senior assistant director of admissions, witnessed the protest from Wilson Hall on Monday during CHOICES. He thought the protest was done with respect and without any intent to disrupt CHOICES. &lt;br/&gt;"I think the thing all our students have in common is they love JMU and they want the best for it," Campbell said. "I think part of that is they understand the recruitment part of what we do."&lt;br/&gt;While the organization didn't have any apparent malicious intent toward CHOICES events, they've been working toward this goal for about two years. The Climate Justice Coalition recently gave presentations to the JMU Foundation, proposing that they stop investing in fossil fuels. &lt;br/&gt;"Last month in March, we received a formal rejection of our proposal," Morrison said. "Over the past month, we've been doing actions to continue the momentum and show that, like, we're not accepting that answer." &lt;br/&gt;Bill Wyatt, the director of communications and university spokesperson, believes the university focused on being environmentally responsible, despite the protests.&lt;br/&gt;"I think we share mutual goals with the students who are protesting," Wyatt said. "The university fundamentally believes in the principle of environmental stewardship and is constantly looking for ways to reduce our carbon footprint ... we're trying to reduce the footprint but also educate students on its importance."&lt;br/&gt;Members of the Climate Justice Coalition have noticed efforts made by the university to be more environmentally conscious, including compost opportunities in dining halls, LEDE certified buildings and a riparian buffer lining a stream on East Campus.&lt;br/&gt;According to Morrison, these efforts are noticed and appreciated, but don't appear consistent. &lt;br/&gt;"They do a lot of good things, but I think that their decision not to divest kind of weakens those things that they've already done," Morrison said. "It was only like one or two percent of their endowment that was invested in fossil fuels, so the fact that they chose not to make this decision I think says a little bit about how true to those efforts they really are."&lt;br/&gt;Wyatt felt that the Foundation offered the students a plan that could still help to reduce JMU's carbon footprint, but that the students involved decided to go in a different direction. &lt;br/&gt;The Climate Justice Coalition plans to continue its efforts to eliminate JMU's investments in fossil fuels, even if its methods of protest change. &lt;br/&gt;"We don't want to give up on this issue, but we also need to find new ways to continue pursuing it since we've kind of exhausted our routes with the administration," Morrison said. "Now we have to find other ways of getting people aware."&lt;br/&gt;Morrison expressed that she didn't expect a change to come immediately after the Quad protest, nor does she necessarily expect a change will come during her time at JMU. She still thinks the organization has to maintain its efforts.&lt;br/&gt;"You may get pushed back and back again, but everything that you're doing is building momentum and building support, building membership," Morrison said. "It takes a long time to build power from a grassroots level, but eventually when you have enough commitment from people, the democratic process kicks back in. That's what we're hoping for." &lt;br/&gt;Contact Abby Church and Emma Korynta at </t>
         </is>
+      </c>
+      <c r="L32" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1817,10 +1920,13 @@
           <t>Faith-based discrimination</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
+      <c r="K33" t="inlineStr">
         <is>
           <t>More than 5,000 people signed a petition, started last November, to ban Students for Justice in Palestine chapters in CUNY.&lt;br/&gt;Andrea Karshan, a student at the College of Staten Island, started the petition after members at different campuses chanted allegedly anti-Semitic comments at Jewish students during the Million Student March in November. One sign called for CUNY to divest from "Israeli apartheid."&lt;br/&gt;SJP began in 1993 at the University of California at Berkeley. Since then, there are chapters across the country, including at CUNY colleges. The organization is controversial for criticizing Israel's presence in Palestine. One tactic it uses is BDS, which means boycott, divest and sanctions.&lt;br/&gt;Karshan declined questions from The Knight News, but wrote an article on her blog defending the petition. She described the backlash from students and the support she received too.&lt;br/&gt;"I don't regret starting the petition," she wrote. "It was something that needed to be done. Our voices needed to be heard."&lt;br/&gt;Karshan worked at The Banner newspaper when she created the petition. But she was dismissed by the Editor-in-Chief. After a new one was appointed, she returned.&lt;br/&gt;The Banner newspaper sent a statement to The Knight News explaining why removing her was wrong.&lt;br/&gt;"While it was not right for Andrea to become a part of the story she was reporting on, the editors handled the situation appropriately by taking her off the assignment," it reads. "Her dismissal was quite literally against the Banner's constitution as we're obliged to be a welcoming place to all students at the College of Staten Island, no matter their beliefs or convictions."&lt;br/&gt;But Sarah Aly, president of the SJP chapter at Brooklyn College, said Karshan's petition cannot work.&lt;br/&gt;"There is no way that these demonstrations actually can be used to suspend any SJPs," Aly said. "The CUNY-wide demonstration was organized by NYC SJP, which is an off-campus organization not tied to a campus."&lt;br/&gt;Aly added Karshan did not get along with Muslim students and caused problems with SJP chapters too.&lt;br/&gt;"She complained that the prayer room on campus was 'too Muslim.' [She] forced Muslim students to clear the room of prayer rugs and Qurans, while Bibles and other religious items were left alone. She has also been known to harass CSI's chapter of SJP in person and online," Aly said.&lt;br/&gt;CUNY Chancellor James Milliken said, in response to the allegations, that the remarks were not suitable and denounced them.&lt;br/&gt;"While we will always embrace this openness to many voices, intolerant, hateful and bigoted speech, while it may be legally protected, is anathema to our values," he said. "Those voices," stop rather than encourage the dialogue and real debate that makes us stronger."&lt;br/&gt;In response to the Chancellor's comments, Aly said there were Islamophobic remarks and found it troubling that he did not address that. She brought up the New York Police Department's spying on Muslim students as something he does not comment on.&lt;br/&gt;"This has been the trend recently [where] issues affecting students and faculty of color are being pushed to the side and ignored," Aly said.&lt;br/&gt;The New York Civil Liberties Union released the NYPD's handbook on spying on MSAs at CUNY. At Queens College, officers are told to look at online profiles of members and even follow them.&lt;br/&gt;At QC, Aadil Ilyas, an alum, felt the backlash against SJP. He worked to make a chapter at the college.&lt;br/&gt;Ilyas posted a status on Facebook calling Israeli Prime Minister Benjamin Netanyahu a monkey. A Jewish student took a screenshot of his status and gave it to a staff member. Ilyas was told not to make the chapter after this and because the national "negative attention" toward the group.&lt;br/&gt;"I left [the person's] office in disbelief," Ilyas said. "I was so angry. I know why I started SJP, and QC is the perfect place to start it."&lt;br/&gt;But Ilyas said several club leaders supported his decision and starting the chapter.&lt;br/&gt;"I had a presentation to do for SJP [in front of QC officials], since it was a new club, and I did great," Ilyas said. "They had no choice but to approve it."&lt;br/&gt;Only the board of trustees can decide to ban SJP, but doing so is illegal, said Radhika Sainath, a staff attorney at Palestine Legal.&lt;br/&gt;"CUNY absolutely may not shut down SJP because some New Yorkers disagree with the group's message supporting justice for Palestinians. To do so would violate the First Amendment," Sainath said.</t>
         </is>
+      </c>
+      <c r="L33" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1865,10 +1971,13 @@
           <t>Anti-racism, Campus climate, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J34" t="inlineStr">
+      <c r="K34" t="inlineStr">
         <is>
           <t>"The people, united, will never be defeated."&lt;br/&gt;This chant-led by Alexis Yeboah-Kodie, CC '16, and repeated by a crowd of about 120 students at a rally on Monday afternoon-was the principal message expressed by the Barnard Columbia Solidarity Network, a new coalition of activist groups that has come together to protest the ways its members say the University puts "profit over people."&lt;br/&gt;The coalition includes Barnard Divest, Columbia Divest for Climate Justice, the International Socialist Organization, Lucha, No Red Tape, Student-Worker Solidarity, and Mobilized African Diaspora, which was participating in its first public rally.&lt;br/&gt;During the rally, BCSN organizers said that interlocking systems of oppression connect the issues they are looking to tackle-including sexual violence, labor inequality, and climate change-through their six core demands. In particular, activists underscored the importance of racial justice and securing the well-being of black people on campus and in the surrounding neighborhood.&lt;br/&gt;"We, the Barnard Columbia Solidarity Network, mobilize in a common struggle for liberation," Barnard Divest member Maya Garfinkel, BC '19, said, reading a statement from the network at the rally. "Columbia University, as a historically and structurally oppressive institution, actively obstructs each of our movements."&lt;br/&gt;Fainan Lakha, CDCJ member chanting during the really.&lt;br/&gt;Mobilized African Diaspora began a speak-out at the rally by calling on the University to hire more faculty of color and allocate more space and funding for centers and institutes that explore marginalized identities.&lt;br/&gt;"MAD is a collection of concerned black students who understand that we are complicit in the oppression that this University facilitates against all black people," MAD organizer Courtney Okeke, CC '16, said during the rally. "We understand and we believe we will not be the marker of diversity for this racist campus. We understand and believe that our bodies are valuable."&lt;br/&gt;As MAD organizers presented three of BCSN's six core demands-including the hiring of more faculty of color and the addition of Introduction to African-American Studies and Introduction to Ethnic Studies as required courses in the Core Curriculum-they emphasized that fighting for black students will benefit all black people as well as all students.&lt;br/&gt;"We are here today not because it's about black issues. We are here today because it's about Columbia's campus as a whole," MAD organizer Ron Busby, CC '17, said. "When black students thrive, all of us do better."&lt;br/&gt;BCSN also called on Columbia to prepare a public report "detailing the complexities of black student life," establish a pantry on campus to combat food insecurity, and asked the University to admit and retain more black students, especially those who are low-income and from local areas.&lt;br/&gt;Last fall, Columbia launched a scholarship program that provides need-based grants for up to 40 undergraduate students each year who grew up or went to school in Harlem, Washington Heights, or the South Bronx.&lt;br/&gt;Activists also emphasized the University's relationship with the surrounding neighborhood, calling on Columbia to invest in jobs and housing for local residents affected by the Manhattanville expansion.&lt;br/&gt;"We are not a group of black students who organize just for black students, because all black people are connected," Okeke said during the rally. "In that, all black people are affected by every single one of these campaigns and the issues they are campaigning against."&lt;br/&gt;Wendi Lu / Staff Designer&lt;br/&gt;For its portion of the speak-out, Lucha deferred to Taylonn Murphy, an anti-violence activist from West Harlem, who is campaigning for the creation of a crisis management center that would provide GED training, online college classes, and other services to local youth.&lt;br/&gt;"Columbia not letting that money trickle down into the community and the people that really need those services is actually strangling the community," Murphy said. "Diversity is one thing when people are living at a certain level where everybody can succeed, but gentrification is actually pushing out people that have been here for years."&lt;br/&gt;At the rally, Columbia Divest for Climate Justice reiterated its demand that the University divest from the top 200 publicly-traded fossil fuel companies, saying that climate change disproportionately affects communities of color.&lt;br/&gt;"Climate change and the exploitation of the earth cannot be dissociated from the exploitation that occurs in our society," CDCJ organizer Iliana Salazar-Dodge, CC '16, said. "The only reason the fossil fuel industry can thrive is because of its reliance on the belief that some lands and some lives are worth sacrificing."&lt;br/&gt;David Alexander CC '16.&lt;br/&gt;After the group's proposal was rejected by the Advisory Committee on Socially Responsible Investing last month, CDCJ collected over 200 pledges from students to engage in civil disobedience, which had originally been planned for this week to mark the COP-21 talks in Paris.&lt;br/&gt;"We were ready to escalate and engage in civil disobedience this semester," Salazar-Dodge said. "Instead, we decided to postpone our action and unite with our fellow activists on campus to build even more power."&lt;br/&gt;Members of Student-Worker Solidarity called on Columbia to raise pay for all work-study and casual employment jobs to $15 an hour, while No Red Tape demanded the creation of a 24-hour rape crisis center. Both groups have been campaigning for their respective causes since September, with No Red Tape explicitly taking on an increased focus on intersectionality.&lt;br/&gt;While each of the seven groups at the rally addressed different causes from the full list, BCSN organizers all expressed optimism for the future of this newly created united front against what they called "interlocked systems of oppression."&lt;br/&gt;"We have a network because we're not divided," MAD organizer David Alexander, CC '16, said. "The University administration will not listen to us. They will not listen to us. But together we will get the change that we want. Know that."&lt;br/&gt;teo.armus@columbiaspectator.com | @teoarmus</t>
         </is>
+      </c>
+      <c r="L34" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1913,10 +2022,13 @@
           <t>Prison/mass incarceration</t>
         </is>
       </c>
-      <c r="J35" t="inlineStr">
+      <c r="K35" t="inlineStr">
         <is>
           <t>AboutStaffAdvertiseClassifiedsNEWSUniversity NewsCity NewsDiversity at NYU2031 ExpansionCrime LogFEATURESBeauty &amp; StyleDiningFashion WeekAbroadARTSBooksEntertainmentFilmTribeca 2016MusicTheaterSPORTSOPINIONMultimediaSpecial EditionsBlogsThe HighlighterUnder the ArchViolet VisionExposureHOUSINGLexi Faunce, News Writer May 2, 2016&lt;br/&gt;As the school year draws to a close, WSN takes a look at some of the most impactful events that took place on campus during the spring semester.&lt;br/&gt;Jake Quan&lt;br/&gt;Hayden Renamed to Lipton Hall&lt;br/&gt;March 22 - The university officially confirmed that Hayden Residence Hall will be renamed to Lipton Hall this June. The change honors NYU School of Law alumnus Martin Lipton, who now resides as chairman to the Board of Trustees. As the second name change of an NYU institution this academic year, students hope that its dining hall cookies don't change along with the building's title.&lt;br/&gt;Anne Cruz&lt;br/&gt;IEC's 36-Hour Sit-In at the Kimmel Center&lt;br/&gt;March 25-26 - The Incarceration to Education Coalition occupied the Kimmel Grand Staircase for 36 hours to draw attention to their Ban the Box initiative. The IEC demanded that the university take action to remove the box on its undergraduate Common Application that requests potential students to disclose prior criminal history and disciplinary action. On April 25, the IEC met with President Hamilton to discuss how the movement would move forward - a demand granted during their sit-in.&lt;br/&gt;Hannah Shulman&lt;br/&gt;Taxi Hits Woman Outside Weinstein Hall&lt;br/&gt;April 7 - A woman was struck by a taxi on the sidewalk near the intersection of University Place and 8th Street, just outside of Weinstein Hall. Some witnesses reported that the incident was caused by brake failure, though this was never confirmed. The NYFD was first to arrive on the scene and immediately evacuated the victim.&lt;br/&gt;Anna Letson&lt;br/&gt;Bernie Sanders Came to Washington Square Park&lt;br/&gt;April 13 - Democratic presidential candidate Bernie Sanders spoke at a rally of more than 27,000 people in Washington Square Park. The Vermont senator was introduced by a variety of celebrities, including a performance by Vampire Weekend. The event followed a voter-registration drive in support of Sanders led by Danny DeVito and Susan Sarandon a few weeks prior. Sanders addressed topics of particular interest to the youthful crowd in preparation for the New York Primary on April 19.&lt;br/&gt;Hannah Shulman&lt;br/&gt;Divest's Occupation of the Executive Elevator in Bobst Library&lt;br/&gt;April 18 - NYU Divest organizers occupied the administrative elevator in Bobst Library for more than 33 hours. The sit-in was in response to the university's failure to grant the organization a meeting with the full Board of Trustees, a demand promised to them by former President John Sexton. Presidential candidate Bernie Sanders tweeted a statement of support to the group and their cause midway through the occupation. While 18 students remained overnight in the library, the occupation ended the following afternoon after university administrators informed the students they would face immediate suspension if the protest continued.&lt;br/&gt;A version of this article appeared in the Monday, May 1 print edition. Email Lexi Faunce at [email protected]</t>
         </is>
+      </c>
+      <c r="L35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1933,10 +2045,13 @@
           <t>Know Tomorrow, a student-led campaign launched by Cool Globes, a national nonprofit organization working to raise awareness and spur action on climate change. Rallies were held by Know Tomorrow chapters at 60 campuses across the country as part of a national day of action in October 2015. The national day of action came in anticipation of the United Nations Climate Change Conference scheduled to begin November in Paris, hoping to raise awareness and spur action on climate change.</t>
         </is>
       </c>
-      <c r="J36" t="inlineStr">
+      <c r="K36" t="inlineStr">
         <is>
           <t>In anticipation of the United Nations Climate Change Conference scheduled to begin this November in Paris, University students gathered on the Diag on Friday to draw attention to climate change.&lt;br/&gt;The rally was sponsored by the University's chapter of Know Tomorrow, a student-led campaign launched by Cool Globes, a national nonprofit organization working to raise awareness and spur action on climate change.&lt;br/&gt;Members of Know Tomorrow held a banner urging students to stand on the "right side of history." The banner included information about recent gains in the climate change movement, including President Barack Obama's August announcement of the Clean Power Plan, which set new regulations for reducing carbon emissions from power plants.&lt;br/&gt;LSA junior Samantha Ginsburg, president of the University's chapter of Know Tomorrow, said she hoped the rally would help amplify and synchronize youth voices calling for action on climate change.&lt;br/&gt;"We know what tomorrow looks like," Ginsburg said. "The science is clear - there is no more debate. We want action because we know what our future looks like."&lt;br/&gt;Know Tomorrow chapters at 60 campuses across the country also held similar climate rallies Friday as part of the national day of action. Some events had high profile speakers such as Sen. Edward Markey at Harvard University and Robert F. Kennedy, Jr. at the University of Southern California.&lt;br/&gt;Don Scavia, a Graham Family Professor of Sustainability and director of the University's Graham Sustainability Institute, spoke at the rally on campus. Scavia urged students to combat climate change, at the personal and institutional levels.&lt;br/&gt;"There are lots of things you can do as individuals to reduce your own consumption," Scavia said. "Those individual actions, though, won't be enough - we need policy changes at the local, state and federal government levels."&lt;br/&gt;The Michigan Marching Band and Jugglers on Campus, a student organization, both performed at the event. Planet Blue and the Divest and Invest campaign also had tables distributing information.&lt;br/&gt;Engineering senior RJ Nakkula said students should join the University in its efforts to combat climate change.&lt;br/&gt;"The University is making steps in the right direction, but everyone needs to do their share," Nakkula said. "It's not just the University's part, it comes down to students, too."&lt;br/&gt;LSA freshman Noah Lowenstein, a member of Know Tomorrow, said the climate rally is an important step toward uniting millennials around climate change goals.&lt;br/&gt;"We are the millennials," Lowenstein said. "We are the ones who will be living on this Earth far beyond the policy makers today."</t>
         </is>
+      </c>
+      <c r="L36" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1981,10 +2096,13 @@
           <t>Indigenous issues</t>
         </is>
       </c>
-      <c r="J37" t="inlineStr">
+      <c r="K37" t="inlineStr">
         <is>
           <t>Around 200 people gathered on the Green Friday afternoon to protest construction of the Dakota Access Pipeline on the Standing Rock Indian Reservation. Critics say the pipeline threatens to harm the water supply of many Native tribes while also cutting across their sacred lands and burial grounds.&lt;br/&gt;Several Dartmouth students shared their stories about why they were opposing the pipeline. Charli Fool Bear-Vetter '15 spoke about her family's experiences dealing with the threat of contaminated water, something she said she can never forget. The DAPL does not care about such threats to the Missouri River, she said, criticizing the use of attack dogs and mace in Standing Rock against protesters.&lt;br/&gt;Students gather on the green to protest the Dakota Access Pipeline.&lt;br/&gt;Augusta Terkildsen '19, who is from North Dakota, shared her experiences in Standing Rock this summer. She encouraged people to spread the word about the situation there and expressed gratitude that awareness about the DAPL has increased recently.&lt;br/&gt;"We deserve to live too, just as much as anyone else," she said.&lt;br/&gt;Terkildsen spoke out against stereotypes of Native Americans as alcoholics, or the usage of statistical drinking rates to try and dismiss other Native health concerns. Several of her relatives in North Dakota who have never drank have still become sick, an outcome she blamed on water conditions there. She said she felt torn between her obligations as a student and to help her family and people.&lt;br/&gt;Kalae Trask-Sharpe '18, an indigenous Hawaiian student, discussed protests in Hawaii against the Thirty Meter Telescope, a proposed observatory that was intended to be built on lands considered sacred to Hawaiians. He talked about the importance of solidarity against such acts, including the DAPL.&lt;br/&gt;The a cappella group the Rockapellas, of which Fool Bear-Vetter is a member, sang "Bury My Heart at Wounded Knee" and "Ella's Song" at the rally.&lt;br/&gt;The Rockapellas sing at the #rally for the #NorthDakotaPipeline #water #Dartmouth pic.twitter.com/34Beq56PJm&lt;br/&gt;- The Dartmouth (@thedartmouth) September 16, 2016&lt;br/&gt;In an interview after the event, Terkildsen said that she began planning the event a few weeks before she came back to campus, with most of the event coming together in the last two or three weeks. She said that she felt great about the turnout, and was pleased that the attendees were not only Native or people of color.&lt;br/&gt;Moving forward, Terkildsen said she and other organizers will be working to raise money in support of Standing Rock. She directed those interested in learning more towards the Sacred Stone Facebook group.&lt;br/&gt;More members of the community share their stories and feelings on #WaterIsLife and the #NorthDakotaPipeline pic.twitter.com/XuJ7W6bkUP&lt;br/&gt;- The Dartmouth (@thedartmouth) September 16, 2016&lt;br/&gt;Eliza Rockefeller '17 said that she came to the rally because she supported what the Native students there were doing from both environmental and social justice perspectives. She described the people at the event as "lovely."&lt;br/&gt;Connor Gibson '16 said that the DAPL is an important issue that everyone should support. While he was pleased with the level of turnout, he said that there could always stand to be more.&lt;br/&gt;Emily Hardwell '16, who was the president of the Native Americans at Dartmouth last year, said that she thought the rally had a good turnout, especially given how few Native students attend Dartmouth. She said the College itself should work to raise money in support of Standing Rock.&lt;br/&gt;Divest Dartmouth, a group that advocates divesting from companies that extract fossil fuels, also joined the demonstration to show their solidarity with the NAD.&lt;br/&gt;Megan Larkin '19, who is an organizer for Divest Dartmouth, said that about 15 members from the group were present at the protest. She said Divest Dartmouth recognizes that the fossil fuel industry "not only contributes to climate change in the future, but also has [negative] impacts right now, such as building pipelines in Native communities."&lt;br/&gt;Larkin said that given the College's status as a prominent institution, protests that occur on Dartmouth's campus are more likely to receive national media coverage.&lt;br/&gt;Hailey Jiang contributed reporting.</t>
         </is>
+      </c>
+      <c r="L37" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -2024,10 +2142,13 @@
           <t>University governance, admin, policies, programs, curriculum, Affirmative action (For), Campus climate, Anti-racism</t>
         </is>
       </c>
-      <c r="J38" t="inlineStr">
+      <c r="K38" t="inlineStr">
         <is>
           <t>Over 150 people attended Monday's faculty of arts and sciences meeting in Alumni Hall, including around 50 protesters supporting Native American studies professor N. Bruce Duthu '80's appointment as dean of the faculty. by Erin Lee / The Dartmouth Senior Staff&lt;br/&gt;Yesterday afternoon, over 150 faculty members and around 50 student demonstrators gathered at Alumni Hall for the termly faculty of arts and sciences meeting. The meeting followed College President Phil Hanlon's campus-wide email earlier yesterday afternoon announcing that N. Bruce Duthu '80 had declined his appointment to dean of faculty of arts and sciences following weeks of discussion surrounding his appointment.&lt;br/&gt;Student demonstrators attended the meeting in support of Duthu, carrying signs that read "Fight 4 Faculty of Color" and "This is Why Faculty of Color Leave Dartmouth," among other messages. Julian Nathan&lt;br/&gt;Protestors made signs and brought them to Monday's faculty of arts and science meeting.&lt;br/&gt;At the beginning of the meeting, Hanlon said that Duthu had his "unwavering support" and that opposition to Duthu's appointment originated from "external" sources, not from individuals on campus.&lt;br/&gt;During the meeting, several faculty members said that the administration should have done more to communicate its support for Duthu, comments that received applause from faculty and students alike. Italian language and literature professor Graziella Parati said during the meeting that it was important for Dartmouth faculty to show their support for Duthu to demonstrate their commitment to diversity.&lt;br/&gt;After Hanlon's statement, current dean of faculty of arts and sciences Michael Mastanduno addressed the audience. He began by saying that he had "deep respect" for Duthu, who was to succeed Mastanduno on July 1, and said that Duthu's credentials were "impeccable." Mastanduno added that Duthu found himself in a "difficult" situation, and Mastanduno was "not interested in debating" whether or not Duthu was at fault for signing a declaration calling for the boycott of Israeli academic institutions in 2013. At certain points, faculty members and students alike interrupted Mastanduno with interjections supporting Duthu's qualifications for the position.&lt;br/&gt;"I may be in full agreement with any of your signs, but please have the respect to allow the faculty to do its business," Mastanduno responded at one point to an interrupting student.&lt;br/&gt;After Mastanduno made the majority of his remarks regarding Duthu's decision, one faculty member proposed a motion to vote to urge Duthu to reconsider declining his appointment. After the motion was seconded by another faculty member, Hanlon asked the faculty members present at the meeting if they were willing to vote on the motion. The vast majority of faculty members raised their hands in favor of voting on the motion while none raised their hands in opposition. Since at least two-thirds of the faculty were in favor of voting on the motion, Hanlon then asked faculty members to vote for or against urging Duthu to reconsider his resignation. After more than two-thirds of the faculty voiced their support again, Hanlon announced that the measure passed but did not specify further how Duthu would be notified of this motion.&lt;br/&gt;Julie Solomon '17, who attended the meeting with a sign that read "Don't Do DartMYTH," said that she learned of the faculty meeting through friends, not through any campus organizations. She said that while she respected Duthu's decision to refuse his appointment, she was upset because she believed that opposition to Duthu's appointment undermined the College's stated goal to employ a diverse faculty. Solomon also added that she does not believe that Duthu's stance on Boycott, Divest, Sanctions amounts to anti-Semitism.&lt;br/&gt;Classics professor Lindsey Whaley, who voted in favor of the motion, said in an interview that Duthu's appointment had "tremendous faculty support" and that the controversy surrounding the appointment upset most faculty members. He added that despite his belief that Duthu is well qualified for this position, he respects Duthu's decision to refuse his appointment.&lt;br/&gt;In an interview after the meaning, Parati said that "it would be naive to think that race had nothing to do with the opposition [to Duthu's appointment]." Parati, who was a member of the search committee for the dean of the faculty position, said she believes that Duthu is an ideal choice. She added that she was glad that faculty had the opportunity to vote on the resolution because it gave them the chance to "send a strong message" of support for Duthu's appointment. She said she believes that faculty members, and not "external forces," have the right to decide who would represent them as their dean.&lt;br/&gt;Hanlon and Provost Carolyn Dever announced Duthu's appointment on March 27. On May 3, economics professor Alan Gustman sent a faculty-wide email raising concerns about Duthu's co-authorship of the Native American and Indigenous Studies Association's 2013 "Declaration of Support for the Boycott of Israeli Academic Institutions." Gustman argued that Duthu's involvement implied support for the Boycott, Divest, Sanctions movement, which Gustman called anti-Semitic.&lt;br/&gt;Duthu responded to "recent charges" in a May 9 faculty-wide meeting, noting that he "condemn[s] anti-Semitism" and supports the "right of private citizens to express criticism of any country's government policies." Gustman responded to this email on May 9, saying that Duthu did not clearly repudiate the BDS movement.</t>
         </is>
+      </c>
+      <c r="L38" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -2067,10 +2188,13 @@
           <t>Public funding for higher education, Labor and work, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J39" t="inlineStr">
+      <c r="K39" t="inlineStr">
         <is>
           <t>Photo: Alexandra Davis.Students walk down the street during the protest to democratize the University holding various posters.&lt;br/&gt;IIRON-once the Illinois-Indiana Regional Organizing Network-has linked University students with opportunities to advocate on behalf of local and national issues for years. This year, the IIRON Student Network has brought its activism to campus with a series of attention-grabbing protests. Many of the University's most important advocacy groups joined under ISN's banner for a series of actions which escalated as the end of the year neared.&lt;br/&gt;On November 2, four University of Chicago students and two alumni were arrested along with 38 other protesters at the Chicago Board of Trade. The protest, organized by the Fair Economy Illinois coalition, demanded a "LaSalle Street Tax" on corporations and higher income taxes on the rich to balance the state's budget. Southside Solidarity Network , a UChicago student organization, and UChicago Climate Action Network both sent protesters. Hundreds of protesters marched from Thompson Center to the Chicago Board of Trade, where they blocked entrances and staged a die-in.&lt;br/&gt;On February 26, 60 students from Fair Budget UChicago protested to demand that the University raise the minimum wage on campus to $15 an hour. The protest included a march from Regenstein Library across the main quad to Edward H. Levi Hall.&lt;br/&gt;The protesters gathered in the fifth-floor waiting room outside Provost Eric D. Isaacs's office to deliver a petition with more than 1,000 signatures calling for a higher wage for University employees. When Isaacs was not found in his office, protesters asked the Dean-on-Call to commit to delivering the petition to Isaacs. Initially the Dean-on-Call stated that she could not promise to deliver the petition because she didn't have the authority to ensure that Isaacs would see the petition. Later she stated that she would make an effort to deliver the petition to Isaacs. University spokesman Jeremy Manier later confirmed that the provost had received the petition.&lt;br/&gt;More than a month later, on April 2, students and activists gathered outside the Chicago Symphony Orchestra to protest higher-education budget cuts before the Saturday 8 p.m. orchestra performance. Students from FBU participated in the protest directed at two University trustees along with the IIRON Student Network.&lt;br/&gt;A public meeting, organized by IIRON and attended by over 50 student activists from IIRON and Phoenix Survivors Alliance , was held in Reynolds Club on May 2. The meeting aimed to provide a forum at which students could express their concerns over administrative policies and advocate for increased transparency and communication with undergraduates. The meeting was initially organized as a town hall meeting that Isaacs, incoming Provost Daniel Diermeier, Vice President and Secretary of the University Darren Reisberg, and Dean of Students in the College John "Jay" Ellison were invited to attend. However, no administrators attended.&lt;br/&gt;A week later, on May 9, three University of Chicago students, among many protesters unaffiliated with the University, were arrested for blocking the entrance to Citadel Headquarters, a hedge fund based in downtown Chicago. The students were participating in a rally led by FEI and IIRON against the Illinois budget crisis and Governor Bruce Rauner. The protest, urging advocacy for higher education funding, was directed at Sam Zell, James S. Crown, and Kenneth C. Griffin, significant donors to Rauner's super PAC and to the CSO.&lt;br/&gt;In response to the administration's lack of attendance at the May 2 public meeting, IIRON organized a protest on May 19. According to protest organizers, more than 150 students, staff members, and alumni participated in the rally calling for increased accountability and democratization of the University. Issues ranging from equitable policing to the University's divestment from fossil fuels were discussed.&lt;br/&gt;The protest consisted of a three-block march on the street from outside Ratner Athletics Center, through Hull Gate across the main quad, to Levi Hall. Before the protest, a group of 34 students and alumni had gathered to occupy the administrative lobby outside Isaacs's office once again until a meeting with the Provost was arranged. The sit-in lasted over an hour, and at 5 p.m. the participants joined the rally outside after the UCPD told them they could face disciplinary action up to suspension and expulsion or arrest if they remained, and escorted them out of the building.&lt;br/&gt;At Monday's Student Government General Assembly meeting, IIRON was finally able to speak to a top-level administrator. When Isaacs appeared before the General Assembly, activists associated with IIRON were ready with questions. They demanded yes or no answers, which Isaacs refused to supply. After a tense half-hour, Isaacs left. As for IIRON, the participants in the sit-in chanted "we'll be back" after they were expelled from Levi Hall on May 19, and this seems more than likely.</t>
         </is>
+      </c>
+      <c r="L39" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -2110,10 +2234,13 @@
           <t>Public funding for higher education, _Other Issue</t>
         </is>
       </c>
-      <c r="J40" t="inlineStr">
+      <c r="K40" t="inlineStr">
         <is>
           <t>Photo: Alexandra Davis.Students walk down the street during the protest to democratize the University holding various posters.&lt;br/&gt;IIRON-once the Illinois-Indiana Regional Organizing Network-has linked University students with opportunities to advocate on behalf of local and national issues for years. This year, the IIRON Student Network has brought its activism to campus with a series of attention-grabbing protests. Many of the University's most important advocacy groups joined under ISN's banner for a series of actions which escalated as the end of the year neared.&lt;br/&gt;On November 2, four University of Chicago students and two alumni were arrested along with 38 other protesters at the Chicago Board of Trade. The protest, organized by the Fair Economy Illinois coalition, demanded a "LaSalle Street Tax" on corporations and higher income taxes on the rich to balance the state's budget. Southside Solidarity Network , a UChicago student organization, and UChicago Climate Action Network both sent protesters. Hundreds of protesters marched from Thompson Center to the Chicago Board of Trade, where they blocked entrances and staged a die-in.&lt;br/&gt;On February 26, 60 students from Fair Budget UChicago protested to demand that the University raise the minimum wage on campus to $15 an hour. The protest included a march from Regenstein Library across the main quad to Edward H. Levi Hall.&lt;br/&gt;The protesters gathered in the fifth-floor waiting room outside Provost Eric D. Isaacs's office to deliver a petition with more than 1,000 signatures calling for a higher wage for University employees. When Isaacs was not found in his office, protesters asked the Dean-on-Call to commit to delivering the petition to Isaacs. Initially the Dean-on-Call stated that she could not promise to deliver the petition because she didn't have the authority to ensure that Isaacs would see the petition. Later she stated that she would make an effort to deliver the petition to Isaacs. University spokesman Jeremy Manier later confirmed that the provost had received the petition.&lt;br/&gt;More than a month later, on April 2, students and activists gathered outside the Chicago Symphony Orchestra to protest higher-education budget cuts before the Saturday 8 p.m. orchestra performance. Students from FBU participated in the protest directed at two University trustees along with the IIRON Student Network.&lt;br/&gt;A public meeting, organized by IIRON and attended by over 50 student activists from IIRON and Phoenix Survivors Alliance , was held in Reynolds Club on May 2. The meeting aimed to provide a forum at which students could express their concerns over administrative policies and advocate for increased transparency and communication with undergraduates. The meeting was initially organized as a town hall meeting that Isaacs, incoming Provost Daniel Diermeier, Vice President and Secretary of the University Darren Reisberg, and Dean of Students in the College John "Jay" Ellison were invited to attend. However, no administrators attended.&lt;br/&gt;A week later, on May 9, three University of Chicago students, among many protesters unaffiliated with the University, were arrested for blocking the entrance to Citadel Headquarters, a hedge fund based in downtown Chicago. The students were participating in a rally led by FEI and IIRON against the Illinois budget crisis and Governor Bruce Rauner. The protest, urging advocacy for higher education funding, was directed at Sam Zell, James S. Crown, and Kenneth C. Griffin, significant donors to Rauner's super PAC and to the CSO.&lt;br/&gt;In response to the administration's lack of attendance at the May 2 public meeting, IIRON organized a protest on May 19. According to protest organizers, more than 150 students, staff members, and alumni participated in the rally calling for increased accountability and democratization of the University. Issues ranging from equitable policing to the University's divestment from fossil fuels were discussed.&lt;br/&gt;The protest consisted of a three-block march on the street from outside Ratner Athletics Center, through Hull Gate across the main quad, to Levi Hall. Before the protest, a group of 34 students and alumni had gathered to occupy the administrative lobby outside Isaacs's office once again until a meeting with the Provost was arranged. The sit-in lasted over an hour, and at 5 p.m. the participants joined the rally outside after the UCPD told them they could face disciplinary action up to suspension and expulsion or arrest if they remained, and escorted them out of the building.&lt;br/&gt;At Monday's Student Government General Assembly meeting, IIRON was finally able to speak to a top-level administrator. When Isaacs appeared before the General Assembly, activists associated with IIRON were ready with questions. They demanded yes or no answers, which Isaacs refused to supply. After a tense half-hour, Isaacs left. As for IIRON, the participants in the sit-in chanted "we'll be back" after they were expelled from Levi Hall on May 19, and this seems more than likely.</t>
         </is>
+      </c>
+      <c r="L40" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -2158,10 +2285,13 @@
           <t>Police violence, _Other Issue</t>
         </is>
       </c>
-      <c r="J41" t="inlineStr">
+      <c r="K41" t="inlineStr">
         <is>
           <t>Students hang banners in Arts and Letters Hall Wednesday decrying hate speech a week after conservative MIlo Yiannopoulos visited campus. (Brenden Moore/The DePaulia)&lt;br/&gt;Student activists decried hate speech as they dropped banners, one stating "Hate speech ? free speech" and the other asking "What would Vinny do?",  from the third and fourth floor balconies of Arts and Letters Hall this afternoon.&lt;br/&gt;The act comes after a week which saw political and racial tensions float to the surface following conservative writer Milo Yiannopoulos' visit to campus and incidents that include the drawing of an anti-Mexican slur on the Quad and the reported finding of a noose the sidewalk near a residence hall.&lt;br/&gt;Around 20 student activists, split by floor, dropped the banners around 12:50 p.m. and started chants that included, "Hate speech ain't free speech", "Can't stop the revolution" and "Black Lives Matter".&lt;br/&gt;Sources said the event had been in the works for nearly a week and that it may have been the effort of a sociology class applying the events of last week to curriculum in the classroom.&lt;br/&gt;About 10 minutes in, a university maintenance worker attempted to take the banners down, which led to chants of "Let the banner hang!" and then cheers when he indeed quit his effort.&lt;br/&gt;"Let the banner hang!" pic.twitter.com/P1mMjhqfuO&lt;br/&gt;- Brenden Moore (@brendenmoore13) June 1, 2016&lt;br/&gt;The event would continue for another 10 minutes when Public Safety eventually took the banner down. The students then marched outside the building and dispersed.&lt;br/&gt;The university appeared to have a heads up as an assortment of officials, including vice president for facilities operations Bob Janis, vice president for student affairs Gene Zdziarski and associate vice president for diversity Rico Tyler were quickly on the scene. This is the fourth banner drop in recent years. One in April 2014 brought attention to the alleged rape culture in the athletic department, one in Spring 2014 called for DePaul to divest in companies that supported Israel's occupation of Palestine by dropping a Palestinian flag and one in the Student Center two weeks ago called for former Chicago Police officer Dante Servin to be denied his pension after he killed Rekia Boyd.</t>
         </is>
+      </c>
+      <c r="L41" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -2201,10 +2331,13 @@
           <t>Pro-Palestine/BDS, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J42" t="inlineStr">
+      <c r="K42" t="inlineStr">
         <is>
           <t>Crowds gathered around Sather Gate on Tuesday afternoon to watch a mock checkpoint demonstration presented by Students for Justice in Palestine, or SJP, which aimed to illustrate Israeli-Palestinian border relations.&lt;br/&gt;SJP placed painted wooden barriers in front of Sather Gate to symbolize the walls erected between parts of Palestine and Israel. The barriers were guarded by two students in faux Israeli military attire who carried cardboard cutout guns.&lt;br/&gt;The checkpoint demonstration was intended to educate Berkeley students on the "implications and realities" of Palestinian occupation, according to SJP member and campus graduate student David McCleary.&lt;br/&gt;"We wanted to show Berkeley students what the average Palestinian has to go through traversing these checkpoints," McCleary said. "We are just showing all of the ways people are treated differently and treated unequally. That is the driving force of our group."&lt;br/&gt;Throughout the afternoon, SJP members acted out scenes based on video footage of checkpoint interactions, according to McCleary. As part of the demonstration, students with colored visas engaged with the guards and tried to pass through the barriers.&lt;br/&gt;According to campus graduate student and SJP member Kumars Salehi, the checkpoint event was also intended to protest UC Berkeley's investments in companies that allegedly profit from Palestinian occupation. Salehi noted that while SJP's efforts have been successful so far, more pressure on the UC Board of Regents is necessary to ensure divestment.&lt;br/&gt;Near the SJP event, Tikvah, a campus Zionist group, staged a counter-protest. Members of Tikvah held Israeli flags and signs that brought attention to recent stabbings in Israel.&lt;br/&gt;"We were standing in solidarity with victims of terror and standing up against terrorism that is directed towards innocent civilians," said Michaela Fried, president of Tikvah, adding that Tikvah was not trying to infringe upon SJP's free speech.&lt;br/&gt;"Our demonstration today was not an attempt to silence SJP, but rather an effort to have our narrative represented as well," Fried said in an email.&lt;br/&gt;McCleary mentioned that while SJP was fine with Tikvah's presence, he was offended by some of the signs held by Tikvah protesters. He emphasized that SJP is an explicitly non-violent group and does not condone stabbings or terrorism.&lt;br/&gt;"To imply that we are okay with Jews being stabbed in Israel is offensive and wrong," McCleary said.&lt;br/&gt;Becca Berman, president of Bears for Israel, said the demonstration presented a false image of what occurs at checkpoints and wishes broader context was given during SJP's demonstration.&lt;br/&gt;Student observers, such as campus sophomore Ismael Chamu, said they thought the visuals were helpful in understanding the issue. The presence of both campus groups, he said, helped frame the issue of Israeli-Palestinian conflict.&lt;br/&gt;"Each side has its own arguments but it brings them to light so that other folks on campus can talk about it, analyze the situation and know where the roots of this problem are and where it exists," Chamu said.&lt;br/&gt;This event was part of SJP's Palestine Awareness Week, which is a week of events intended to educate students on Palestinian affairs. SJP's next event will be a march and die-in in Downtown Berkeley on Thursday.&lt;br/&gt;Contact Maya Eliahou and Roann Pao at [email protected].</t>
         </is>
+      </c>
+      <c r="L42" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -2244,10 +2377,13 @@
           <t>Pro-Israel/Zionism</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr">
+      <c r="K43" t="inlineStr">
         <is>
           <t>Crowds gathered around Sather Gate on Tuesday afternoon to watch a mock checkpoint demonstration presented by Students for Justice in Palestine, or SJP, which aimed to illustrate Israeli-Palestinian border relations.&lt;br/&gt;SJP placed painted wooden barriers in front of Sather Gate to symbolize the walls erected between parts of Palestine and Israel. The barriers were guarded by two students in faux Israeli military attire who carried cardboard cutout guns.&lt;br/&gt;The checkpoint demonstration was intended to educate Berkeley students on the "implications and realities" of Palestinian occupation, according to SJP member and campus graduate student David McCleary.&lt;br/&gt;"We wanted to show Berkeley students what the average Palestinian has to go through traversing these checkpoints," McCleary said. "We are just showing all of the ways people are treated differently and treated unequally. That is the driving force of our group."&lt;br/&gt;Throughout the afternoon, SJP members acted out scenes based on video footage of checkpoint interactions, according to McCleary. As part of the demonstration, students with colored visas engaged with the guards and tried to pass through the barriers.&lt;br/&gt;According to campus graduate student and SJP member Kumars Salehi, the checkpoint event was also intended to protest UC Berkeley's investments in companies that allegedly profit from Palestinian occupation. Salehi noted that while SJP's efforts have been successful so far, more pressure on the UC Board of Regents is necessary to ensure divestment.&lt;br/&gt;Near the SJP event, Tikvah, a campus Zionist group, staged a counter-protest. Members of Tikvah held Israeli flags and signs that brought attention to recent stabbings in Israel.&lt;br/&gt;"We were standing in solidarity with victims of terror and standing up against terrorism that is directed towards innocent civilians," said Michaela Fried, president of Tikvah, adding that Tikvah was not trying to infringe upon SJP's free speech.&lt;br/&gt;"Our demonstration today was not an attempt to silence SJP, but rather an effort to have our narrative represented as well," Fried said in an email.&lt;br/&gt;McCleary mentioned that while SJP was fine with Tikvah's presence, he was offended by some of the signs held by Tikvah protesters. He emphasized that SJP is an explicitly non-violent group and does not condone stabbings or terrorism.&lt;br/&gt;"To imply that we are okay with Jews being stabbed in Israel is offensive and wrong," McCleary said.&lt;br/&gt;Becca Berman, president of Bears for Israel, said the demonstration presented a false image of what occurs at checkpoints and wishes broader context was given during SJP's demonstration.&lt;br/&gt;Student observers, such as campus sophomore Ismael Chamu, said they thought the visuals were helpful in understanding the issue. The presence of both campus groups, he said, helped frame the issue of Israeli-Palestinian conflict.&lt;br/&gt;"Each side has its own arguments but it brings them to light so that other folks on campus can talk about it, analyze the situation and know where the roots of this problem are and where it exists," Chamu said.&lt;br/&gt;This event was part of SJP's Palestine Awareness Week, which is a week of events intended to educate students on Palestinian affairs. SJP's next event will be a march and die-in in Downtown Berkeley on Thursday.&lt;br/&gt;Contact Maya Eliahou and Roann Pao at [email protected].</t>
         </is>
+      </c>
+      <c r="L43" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -2287,10 +2423,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J44" t="inlineStr">
+      <c r="K44" t="inlineStr">
         <is>
           <t>In anticipation of the United Nations Climate Change Conference scheduled to begin this November in Paris, University students gathered on the Diag on Friday to draw attention to climate change.&lt;br/&gt;The rally was sponsored by the University's chapter of Know Tomorrow, a student-led campaign launched by Cool Globes, a national nonprofit organization working to raise awareness and spur action on climate change.&lt;br/&gt;Members of Know Tomorrow held a banner urging students to stand on the "right side of history." The banner included information about recent gains in the climate change movement, including President Barack Obama's August announcement of the Clean Power Plan, which set new regulations for reducing carbon emissions from power plants.&lt;br/&gt;LSA junior Samantha Ginsburg, president of the University's chapter of Know Tomorrow, said she hoped the rally would help amplify and synchronize youth voices calling for action on climate change.&lt;br/&gt;"We know what tomorrow looks like," Ginsburg said. "The science is clear - there is no more debate. We want action because we know what our future looks like."&lt;br/&gt;Know Tomorrow chapters at 60 campuses across the country also held similar climate rallies Friday as part of the national day of action. Some events had high profile speakers such as Sen. Edward Markey at Harvard University and Robert F. Kennedy, Jr. at the University of Southern California.&lt;br/&gt;Don Scavia, a Graham Family Professor of Sustainability and director of the University's Graham Sustainability Institute, spoke at the rally on campus. Scavia urged students to combat climate change, at the personal and institutional levels.&lt;br/&gt;"There are lots of things you can do as individuals to reduce your own consumption," Scavia said. "Those individual actions, though, won't be enough - we need policy changes at the local, state and federal government levels."&lt;br/&gt;The Michigan Marching Band and Jugglers on Campus, a student organization, both performed at the event. Planet Blue and the Divest and Invest campaign also had tables distributing information.&lt;br/&gt;Engineering senior RJ Nakkula said students should join the University in its efforts to combat climate change.&lt;br/&gt;"The University is making steps in the right direction, but everyone needs to do their share," Nakkula said. "It's not just the University's part, it comes down to students, too."&lt;br/&gt;LSA freshman Noah Lowenstein, a member of Know Tomorrow, said the climate rally is an important step toward uniting millennials around climate change goals.&lt;br/&gt;"We are the millennials," Lowenstein said. "We are the ones who will be living on this Earth far beyond the policy makers today."</t>
         </is>
+      </c>
+      <c r="L44" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -2330,10 +2469,13 @@
           <t>_Other Issue</t>
         </is>
       </c>
-      <c r="J45" t="inlineStr">
+      <c r="K45" t="inlineStr">
         <is>
           <t>UNM students gathered in front of Zimmerman Library on Thursday as part of a nationwide movement calling for abolishing student debt, raising the minimum wage and providing free tuition at public universities.&lt;br/&gt;Marisa Trujillo, a sophomore business administration major, said the rally gave financially struggling students a way to voice their frustrations with peers in similar situations.&lt;br/&gt;"People talk about it, but it's too quiet; people are brushing it under the rug, the school is hiding it," she said. "That's why we put this on, we gave students a chance to stand with us and not to have any fear and to basically let their voices be heard."&lt;br/&gt;Trujillo said UNM is just one of hundreds of schools nationwide participating in rallies like Thursday's in hopes that the U.S. can model itself after other countries that offer free education, such as Denmark.&lt;br/&gt;"When people come and tell us that it's impossible, it's really possible, and it's simpler than people think," she said. "The thing is, people are afraid to stand up against it because they think that the authority of the school is going to shut them down. Which they might, but we're still going to speak out, because it's something we deserve."&lt;br/&gt;UNM was one of hundreds of schools nationwide that had students participating in the movement, called the Million Student March. Several students held signs that read "Kicking ass 4 the working class" and "Education Is A Human Rights Issue," among others.&lt;br/&gt;It was endorsed by several UNM student groups, including the Feminist Majority Leadership Alliance, Generation Justice and the Red-Student Faction.&lt;br/&gt;Micheáilín Buitléir, a junior American studies major, said that the movement's three goals are intertwined in a mission to partake in the assets that UNM collects from students.&lt;br/&gt;"This is just a pyramid scheme to mass-accumulate wealth," he said. "What we want is, instead of the wealth going into the hands of the one percent, we want the wealth to go to all of us, to redistribute that wealth to invest in our future. Like our sign says, 'The present is struggle, but the future is ours.'"&lt;br/&gt;Buitléir said that in addition to the core demands, the rally at UNM added a fourth: divestment of the indirect support of the occupation of Palestine, as well as the reliance on fossil fuels.&lt;br/&gt;"(It) is one of the biggest issues we're facing right now - the extinction of our species. So taking that money and starting to invest it in education and higher wages, investing it in healthcare and jobs and those sorts of things," he said.&lt;br/&gt;Another supporter said that UNM is being hypocritical in calling itself a public university, and that the University is essentially robbing students by continuing to raise tuition "in the second Great Depression of this nation's history."&lt;br/&gt;"I think, if we can work through the setup structure, that would be great because it gives us a good dialogue and a good forum to actually sit down and make a change," Graves said. "This raises awareness and it gets people thinking about it, but it doesn't drive the policy change we need."&lt;br/&gt;Not all UNM students approve of such policy change, however, including more conservative representatives from Young Americans for Liberty, a new organization at UNM this semester.&lt;br/&gt;"Before us, the liberal agenda (on campus) kind of had its way. It was never challenged; people just kind of walked around it and ignored it if they didn't agree with it," said Michael Aguilar, president of the group's UNM chapter. "So we decided to mobilize the conservative cohort that we do have on campus...and we made sure that the liberal agenda didn't go unchecked."&lt;br/&gt;Aguilar said that the demands of the Million Student March are not feasible, economically or otherwise, and that someone will have to bear the burden.&lt;br/&gt;"There's no such thing as a free lunch. Someone's going to get the bill, and they're going to realize that the one percent can't pay for everything," Aguilar said.&lt;br/&gt;While representatives from the two sides argued at the rally for some time, Aguilar said before his peers left the event, he and Graves agreed that they should hold an organized debate in the SUB.&lt;br/&gt;Such an event would accurately inform students about the issues at hand, something that Aguilar said he always advocates.&lt;br/&gt;"I think that, whether it be a rally like we had today, a counter-protest or a forum, any way (we can) engage the students and get them involved in the political process... I think that's beneficial for everyone involved," he said.&lt;br/&gt;Although Trujillo said that the rally's opponents were there just "to be against us," she also said a debate is the more appropriate route to discuss the issues at hand between the two parties.&lt;br/&gt;"We want to get stuff done, and shouting at each other isn't going to get anything done. Whether we agree on everything, or anything at all for that matter, we can still talk and be civil about it and get somewhere," she said.&lt;br/&gt;David Lynch is the news editor at the Daily Lobo. Contact him at news@dailylobo.com or on Twitter @RealDavidLynch.</t>
         </is>
+      </c>
+      <c r="L45" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -2373,10 +2515,13 @@
           <t>University governance, admin, policies, programs, curriculum, Tuition, fees, financial aid</t>
         </is>
       </c>
-      <c r="J46" t="inlineStr">
+      <c r="K46" t="inlineStr">
         <is>
           <t>Approximately 20 students gathered to protest the University of California Board of Regents vote to raise tuition, which occurred earlier today. UCSD Students Against Tuition Hikes also organized the protest to demand free UC tuition, to make UC campuses sanctuary campuses, to encourage prison and energy transfer partner divestment, to advocate that the UC endorse Proposition 13 reform and that, overall, the UC become more democratized.&lt;br/&gt;In-state tuition is expected to rise by 2.5 percent, or $282 per student, with an additional $54 increase in student services fees, totaling $11,502 for the 2017-18 academic year. Out-of-state students will experience a total increase of $1,668 resulting from the overall 2.5 percent increase, in addition to five percent more in supplemental tuition - an overall cost of $28,014 for the next school year. This is the first tuition increase the UC system has seen in six years.&lt;br/&gt;Protesters marched down Library Walk and through Price Center chanting, "Hey hey ho ho, tuition hikes have got to go," among other phrases including, "Tuition is going up on a Thursday and the chancellor's getting a pay raise," and stopping briefly to discuss why the tuition hikes are making it difficult for students to continue studying at the university.&lt;br/&gt;Students, including some who finance their own education, explained the struggle of working multiple jobs to meet the tuition and the high cost of living in La Jolla. These students are concerned that increasing tuition would make it even more difficult to balance academic, social and work life.&lt;br/&gt;Ricardo Vazquez, the director of media relations at the University of California Office of the President told the UCSD Guardian that two out of three UC students will still be covered by financial aid and will not have to pay the tuition increase.&lt;br/&gt;"One-third of the increase in revenue will be added to the financial aid fund," he added. "The rest of the revenue will go to campus priorities and to things that will directly benefit students. [Things that] the students themselves have told us [ they want], and others [that are] are a very high priority for them in terms of the quality of education."&lt;br/&gt;Priorities vary from campus to campus but include hiring more faculty to combat the increasing enrollment, hiring more TAs and lowering the student-to-faculty ratio. Most of the increase in the student services fee will go to improving mental health facilities for students.&lt;br/&gt;"The revenue from the tuition and fee increase [will provide UC students] with more than $540 million, including more than $250 million directly from the university to help pay for educational expenses [aside from] tuition," Vazquez told the Guardian.&lt;br/&gt;Students covered by financial aid will also receive funds to pay for expenses besides tuition, such as books, housing, and transportation.&lt;br/&gt;Associated Student Council President Daniel Juarez, who participated in the protest, spoke to the Guardian about her thoughts on the tuition hikes as a response to inflation.&lt;br/&gt;"I understand that money is needed for the [University of California]," she explained. "The UC [system] is in a place where it needs to be sustained financially; I understand and agree with that 100 percent. I don't agree with the fact that students need to pay for it because we have been paying for the increases for over a decade."&lt;br/&gt;Ly Nguyen, a graduate student from the ethnic studies department attending the protest today also expressed concerns that the UC system is becoming increasingly privatized.&lt;br/&gt;"I don't want to use this myth of the golden time when education is free because every historical era has its own flaws," she clarified. "But the fact that the UC system is gradually becoming privatized, and [it is] investing in a lot of national projects like the prison industry and the private banking system and things like that, while students have to pay the price. I think it's important for students to realize that this is the battle they are going to have to fight now."&lt;br/&gt;Juarez also pointed out that, although state officials helped ensure tuition would not rise in 2014, they have not provided adequate support for higher education over the past couple of years.&lt;br/&gt;"Addressing UC's accountability issue as an excuse to not fund higher education properly is no longer an acceptable excuse, I would argue," Juarez said. "Because that's the excuse that's been given to us in the past you know. Students mobilized and we worked with the state in 2014...they were supposed to be the ally that we had in terms of higher education funding and then we were let down."&lt;br/&gt;With regards to preventing tuition hikes now and in the future, Juarez discussed that she would be looking for different ways to mobilize and unite students while also finding alternative ways to fund higher education, including starting conversations about rolling back tuition.&lt;br/&gt;"I am going to use my position to keep pushing the student narrative that's valuable that we need to hear, I really hope to keep doing that," Juarez said. "I think that at the administration's level, it'll be expressing that we're discontent with this decision. Also, trying to mobilize other students as a whole by partnering with our graduate students and our faculty. I think together we have a lot of similar interests and we are really powerful. At the state level, I think we are going to have to lobby the state...at the rate that the state is funding us, this [raising tuition] is not going to be uncommon. We need to start talking about what we can do to get a tuition rollback ... understand what is necessary to do that and do it or do something to make higher education more affordable ... there's a lot that could be done and we need the money but we also need the priorities from those higher up to commit to our needs."&lt;br/&gt;The UC Board of Regents previously voted to approve a tuition hike in 2014 that would have increased tuition by up to five percent annually through the 2019-2020 academic year. The proposal resulted in protests across the UC campuses, and, following negotiations with the state to provide more funding, the increase was ultimately not enforced.&lt;br/&gt;Additional reporting by Tina Butoiu and Lauren Holt&lt;br/&gt;TAGSA.S. CouncilasucsdCaliforniaGovernor BrownTuitiontuition hikeUC Board of RegentsUC System SHARE Facebook Twitter tweet Promita Nandy</t>
         </is>
+      </c>
+      <c r="L46" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -2423,10 +2568,13 @@
           <t>Anti-racism, Racist/racialized symbols</t>
         </is>
       </c>
-      <c r="J47" t="inlineStr">
+      <c r="K47" t="inlineStr">
         <is>
           <t>Protesters Shut Down Jewish Defense League at World Social Forum&lt;br/&gt;Far-right Jewish Group Drove from Toronto to Oppose Palestine-Solidarity&lt;br/&gt;News by Jon Milton — Published August 11, 2016 | Comments&lt;br/&gt;Follow @514jon&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Around 10 members of the far-right Jewish Defense League were confronted by over 100 anti-racist protesters on Wednesday. Photo: Cori Marshall&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Around 10 members of the far-right Jewish Defense League were confronted by over 100 anti-racist protesters on Wednesday. Photo: Cori Marshall&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;“Send your little punk over here, we’ll go one-on-one,” the middle-aged man shouted angrily, from behind police lines, at the group of anti-racist protesters.&lt;br/&gt;The man was one of about ten members of the Jewish Defense League, who had driven to Montreal from Toronto with the intention of disrupting Palestine solidarity events at the ongoing World Social Forum. &lt;br/&gt;The JDL’s Toronto branch had specifically created plans to disrupt a workshop given by Canadian Friends of Sabeel, an organization which describes itself as “standing in solidarity with Palestinians, and raising awareness in Canada of the struggle of Palestinian Christians.” The subject of the workshop was “Divesting your Church or Denomination 101 (BDS for peace and justice in Palestine/Israel),” and was scheduled to take place at 1 p.m at Cegep du Vieux Montreal.&lt;br/&gt;A callout to prevent the JDL’s disruption was initially made through Treyf, a podcast and blog run by Jewish leftists in Montreal. The callout was answered by Solidarity Across Borders, a migrant solidarity group, which helped to organize and publicize the action.&lt;br/&gt;“We felt it was important to call for immediate opposition to the JDL, who have already attempted to create links with other fascist groups in [Montreal] like PEGIDA,” said David Zinman, one of the authors of the original Treyf callout.&lt;br/&gt;“As Jewish people, we know that our liberation and safety is tied to that of the Palestinian people, and we adamantly refuse the logic of anti-Arab racism that the JDL peddles,” he continued.&lt;br/&gt;The JDL is a group that was formed in 1968 in New York City, under the leadership of Rabbi Meir Kahane. It was initially formed as a vigilante-style street patrol in the city’s Jewish neighborhoods, specifically targeting black people and Puerto Ricans.&lt;br/&gt;The organization grew throughout the United States, and began to focus more principally on targeting Arabs. In 1994, JDL member Baruch Goldstein murdered 29 Muslims in a mosque in the West Bank—a move which was later celebrated by the JDL.&lt;br/&gt;In 2000, the FBI designated the JDL a right-wing terrorist organization.&lt;br/&gt;“Alerta, Alerta, Antifascista!”&lt;br/&gt;By the time the workshop was set to begin, around 100 anti-racist activists gathered in front of the school where it was taking place, waiting to prevent the JDL from disrupting the event. Music playing on the loudspeakers was cut at 2 p.m., and an organizer announced that ten people in JDL shirts were a few blocks away.&lt;br/&gt;The crowd began to move, and turned the corner from Ontario St. onto St. Laurent Blvd. to find a van and a group of people with Israeli flags and JDL shirts. A JDL member—a middle aged woman—was carrying a stack of pamphlets which juxtaposed two separate photos of a keffiyeh-wearing Palestinian and a member of the KKK, with the words “the face of terror” emblazoned underneath.&lt;br/&gt;One protester attempted to grab the pamphlets, only to be shoved by a man wearing a JDL shirt. The pamphlets were scattered on the ground, and the increasingly angry man from the JDL was punched in the face by an anti-fascist demonstrator after shoving more counter-protesters.&lt;br/&gt;Within seconds, the police arrived. They quickly formed a line in between the two groups, and a tense silence prevailed. Soon, the anti-JDL protesters began chanting slogans such as “alerta, alerta, antifascista!” which are common in anti-fascist and anti-racist demonstrations.&lt;br/&gt;“The [Service de Police de la Ville de Montreal] is here… to make sure no one gets hurt and that nothing happens between the two groups arguing with each other,” said SPVM media relations officer Manuel Couture.&lt;br/&gt;Both sides brought out megaphones, and attempted to give speeches from behind police lines. Whenever the member of the JDL attempted to speak, however, they were drowned out by the chants of the anti-racist protesters. This back-and-forth lasted approximately an hour and a half.&lt;br/&gt;There was a sizable contingent of Jewish participants on the anti-JDL side, who sometimes attempted to chant slogans in Yiddish. &lt;br/&gt;Once the Friends of Sabeel workshop was finished, the JDL members decided to leave. Their van was escorted by police as they drove southbound on St. Laurent Blvd., a one-way street which heads north. &lt;br/&gt;Correction: In a previous iteration of this article, we published quotes anonymously suggesting that Jewish voices weren’t centered in the resistance again the JDL. Organizers from the protest have since been contacted and said that multiple anti-JDL Jewish protesters spoke using the megaphone. The quotes have been removed due to an unjustified anonymity. The Link regrets the error.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;By commenting on this page you agree to the terms of our Comments Policy.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Please enable JavaScript to view the comments powered by Disqus.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Related Reading&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;UPDATE: BDS Movement Question Altered to Exclude Mention of Israeli Human Rights Violations&lt;br/&gt;Jonathan Caragay-Cook&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Opinions&lt;br/&gt;Editorial: New PM, Same Song and Dance&lt;br/&gt;The Link&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;BDS Movement Question Altered to Exclude Israeli Human Rights Violations&lt;br/&gt;Jonathan Caragay-Cook&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;CSU to Endorse November Anti-Racism Protest&lt;br/&gt;Franca G. Mignacca</t>
         </is>
+      </c>
+      <c r="L47" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -2468,10 +2616,13 @@
           <t>Pro-Palestine/BDS</t>
         </is>
       </c>
-      <c r="J48" t="inlineStr">
+      <c r="K48" t="inlineStr">
         <is>
           <t>On Wednesday, November 9, an Artists 4 Israel event on Lower Field of campus organized by Chabad McGill attracted protesters who denounced what they perceived to be the event’s insensitive concept and erasure of Palestinian voices.&lt;br/&gt;In an event which has subsequently been removed from Facebook, members of the organization Artists 4 Israel erected a temporary wall on Lower Field, decorated it with Canadian and Israeli flags, and the word ‘peace’ in Hebrew and English, and invited passers-by to add their own graffiti to the installation.&lt;br/&gt;They also displayed banners listing statements about Israel, and distributed free refreshments and t-shirts. Initially, Palestinian people, along with any Palestinian flags or symbols, were entirely absent from the event.&lt;br/&gt;Soon however, the installation began to attract opposition. A small crowd of protesters gathered on Lower Field, carrying banners and placards which denounced Israel’s ongoing violence against Palestinian people, and appropriation of Palestinian land. The demonstrators spread out in a line, standing in front of the Artists 4 Israel installation.&lt;br/&gt;Speaking to The Daily at the protest, George Ghabrial, a member of McGill Students in Solidarity with Palestinian Human Rights (SPHR), explained what prompted him and other students to protest the event.&lt;br/&gt;“Me and a couple friends were [at] the Y [intersection], we were all going to class, and we saw this structure […] and then we saw an Israeli flag. […] We went up to some of these student organizers, asked them what was going on, they said it was an event called ‘Artists 4 Israel,’” he explained.&lt;br/&gt;“So SPHR […] said that we should do something – there’s no representation of Palestine, there’s no mention of Palestine, there’s no […] mention of the occupation,” he continued. “It’s an implicitly political event that does not make explicit the occupation of Palestine. […] So we went and got our banners […] and came down to Lower Field.”&lt;br/&gt;“On the surface, it’s supposed to be apolitical,” Ghabrial explained. “I don’t know very much about Chabad as an organization, but I’d say that the event is very normalizing about the occupation. […] And there’s a very strong connotation about who the antagonizers to peace are.”&lt;br/&gt;A member of Artists 4 Israel spoke with The Daily about the intended purpose of the event.&lt;br/&gt;“Artists 4 Israel was brought here by Chabad, Stand With Us, Size Doesn’t Matter and AEπ and […] Hasbara Fellowships, in order to paint a mural about peace and coexistence, and try to bridge all the […] diverse cultures that are here together, and of course express their pride in their own Jewish heritage and sense of Israel with that larger culture of the campus.”&lt;br/&gt;When asked about the response to the protest, he said: “Instead of their protest […] they’ve all been offered the opportunity to spray-paint with us and to have shirts made, the same way the entire student body has been allowed. That they chose to separate themselves and segregate themselves from an event that’s supposed to be about inclusiveness […] I think speaks for itself as to what their true intentions are. We would have loved them to be part of it.”&lt;br/&gt;In a comment sent to The Daily by email, however, Julie, a member of Boycott, Divestment &amp; Sanctions (BDS) McGill said that she had been present at the protest for more than an hour, and had never been invited to write on the installation.&lt;br/&gt;The protesters partly took issue with the statements about Israel on display beside the art installation, which portrayed the nation as a place of tolerance and equality. One section, in particular, alleged that non-Jewish Israelis “enjoy equal rights and freedoms.” In fact, Israel has drawn criticism from minority voices internally, and from the international community for the systemic discrimination that many non-Jewish citizens face.&lt;br/&gt;However, event organizer, Eva Chorna, objected to this characterization, saying, “To have that [statement] on the board I think is very representative of the essence that is Israel, because if there is one country that understands what it’s like to be a refugee, I think it’s Israel.”&lt;br/&gt;“Israel isn’t a perfect society,” she continued, “as no society is, but there are so many instances where they try to be inclusive towards the Palestinians, towards the Israeli Arabs in society, towards all the different religions.”&lt;br/&gt;However, protesters also took issue with the concept of the installation.&lt;br/&gt;“The board itself resembles the Apartheid Wall that runs in the West Bank and restricts access to medical resources and water supplies of Palestinians that live there,” said Julie in her email to The Daily. “The idea of graffiti-ing the ‘canvas’ mocks and appropriates the forms of Palestinian resistance that appear on the Apartheid Wall.”&lt;br/&gt;“Furthermore, the ‘graffiti’ displayed the word peace next to the Israeli flag alongside the Canadian flag as well as the McGill Martlet, which completely disregards the settler-colonial history tied to all three of these,” she continued.&lt;br/&gt;She added that she “was asked to move multiple times.” She was also “asked to leave because they claimed this art (that resembled the Apartheid Wall with flags of Israel, Canada, and the McGill martlet) was not political.”</t>
         </is>
+      </c>
+      <c r="L48" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -2511,10 +2662,13 @@
           <t>Labor and work, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J49" t="inlineStr">
+      <c r="K49" t="inlineStr">
         <is>
           <t>To the Editors:&lt;br/&gt;Broader Context:&lt;br/&gt;Since May Day is a national day of action for labor rights in the U.S., members of the Student Labor Action Coalition and other interested students chose May 1 to make a stand for workers' rights on campus. We wanted to both make a statement on campus while also recognizing the increasing attacks on labor that have continued for decades. The Trump administration's nomination of Secretary of Labor Alexander Acosta and its targeting of immigrant and specifically non-white workers further emphasize the need for solidarity within the labor movement both in Northeastern Ohio and nationwide. Historically, the labor movement has privileged exclusively white men over the rest of the global workforce. May Day must be a moment of truly intersectional activism that works in the interests of the working class beyond the historical recipients of labor's benefits. The labor movement must be the immigrant rights movement, it must be the anti-imperialist movement, it must be the anti-racist movement and it must support gender equality and self-determination. For too long the labor movement has been complicit in its own destruction, because it has prioritized its corporate interests over international and domestic solidarity.&lt;br/&gt;Two weeks ago, SLAC held a labor panel with United Auto Workers members in attendance who expressed their outrage at Bon Appétit Management Company's management policies, its role in CDS employment decisions such as position eliminations, and its treatment of CDS staff. Bon Appétit's managers have consistently been disrespectful and dismissive of CDS staff, sometimes to the point of harassment. Dean Holliday, [the Bon Appetit executive chef] at Oberlin, was accused on multiple occasions of sexual misconduct but was never fired by Bon Appétit. Instead, he was moved to Case Western University.&lt;br/&gt;The boycott itself was inspired by the early 2000 "Not With Our Money" divestment campaign, which was originated by the Prison Moratorium Project. In 2001, Oberlin, students led a series of actions, which included a boycott of CDS, to pressure the College to end its contract with Sodexho Marriott Services, the College's previous dining management company. Their objections were based on Sodexho's ties to private prisons, its terrible food quality and its exploitative labor practices. Students intended to pressure the College into replacing Sodexho with worker self-managed dining halls; instead, Oberlin replaced it with Bon Appétit. However, like Sodexho, Bon Appétit has ties to fossil fuel industries, military contractors and private prisons.&lt;br/&gt;The parent company of Bon Appétit is Compass Group, a majority stakeholder in the prison services vendor Trinity Services. Compass Group has been involved with numerous controversies in recent years, including underpaying their workers in the U.S. Senate kitchens, overcharging the New York public school system for school lunches, serving Listeria-contaminated food in Canadian prison and serving undeclared horse meat in schools in the U.K., France and Sweden. Compass Group has also been responsible for providing dining and construction services for U.N. Peacekeepers, U.S. Armed Forces in Kuwait and Iraq, as well as major defense contractors including Fluor, RMS, Bechtel, Blackwater and KBR (a subsidiary of Halliburton). According to its own website, Compass Group subsidiary Eurest Support Services "leads the market in providing food and support services to major companies operating in the oil and gas, mining, construction and defence sectors." ESS has also been investigated multiple times for bribery and fraud. Although campus dining halls may appear isolated from these broader conditions, the dynamics of subcontracting at the macro-level informs and is relevant to their behavior on campus.&lt;br/&gt;Workers have voiced concerns about the quality of food purchased by Bon Appétit, which markets itself as using ethically sourced and sustainable products but buys in bulk from Tyson Chicken, a corporation that has been accused of wage theft and animal cruelty. According to a report by the Environmental Protection Agency, Tyson also dumps more pollution into waterways each year than even Exxonmobil. Oberlin must end its financial support of the environmental devastation and economic exploitation that Tyson Foods perpetuates.&lt;br/&gt;Schools that directly compete with Oberlin - including Occidental College, Amherst College, Bowdoin College, University of California, Los Angeles and recently Pomona College - all have independent dining services with much higher food rankings than Oberlin. Given the College's current financial difficulties, it would be extremely beneficial for dining halls to be more economical with their purchasing as well as their food preparation. Oberlin's dining halls throw away pounds and pounds of food at every meal due to poor product quality as well as large amounts of leftovers. Allowing chefs to determine their own recipes and making them responsible for food preparation and cooking allows them greater control over the amount of food they produce, leading to both better food and less food waste.&lt;br/&gt;Clarifications:&lt;br/&gt;Given the amount of information that has been circulating in the past week, we would like to clarify the origins and scope of the boycott. The action was planned in solidarity with workers' wish for self-management. While we did run it by the union, this specific action was not asked for or planned by the unions themselves. The boycott was planned only for lunch because we were only able to provide food for one meal, and we didn't want anyone to go hungry. Some people did organize alternative plans for dinner, but we were not involved in those decisions. However, we are incredibly grateful for their support and generosity.&lt;br/&gt;We did not ask either students or CDS workers to leave their shifts. We wanted to state our opposition to Bon Appétit, but we didn't want anyone to risk their jobs or place extra burdens on those who didn't feel comfortable walking off the job. This picnic was not just an isolated call for Oberlin to switch to worker self-management in its dining halls; it is also intended as the beginning of a continuing dialogue surrounding student and worker solidarity on Oberlin's campus.&lt;br/&gt;Vision for the Future of Oberlin Dining:&lt;br/&gt;The Oberlin May Day Coalition is calling for worker self-management in dining services. We do not want Oberlin to replace Bon Appétit with another outside management company, as it did after Sodexho. All of the other private contractors are just as bad as Bon Appétit. Aramark is one of the primary suppliers of prison food within Ohio and worldwide. Chartwells is also owned by Compass Group, and students already got rid of Sodexho. We are calling for a self-managed dining service where workers are able to make decisions regarding the management of the dining halls and are able to represent themselves to the administration, instead of an unrepresentative, corrupt third party. Oberlin students and workers must be represented in decision-making during the current restructuring process to allow for greater equity and accessibility across the board.&lt;br/&gt;- Jeeva Muhil&lt;br/&gt;SLAC co-chair&lt;br/&gt;- Eliza Guinn&lt;br/&gt;SLAC co-chair&lt;br/&gt;- Michael Kennedy&lt;br/&gt;SLAC treasurer</t>
         </is>
+      </c>
+      <c r="L49" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -2559,10 +2713,13 @@
           <t>Immigration (For)</t>
         </is>
       </c>
-      <c r="J50" t="inlineStr">
+      <c r="K50" t="inlineStr">
         <is>
           <t xml:space="preserve">As a single student, you may feel frustrated that you cannot impact world affairs, or that even if you really tried to, the time commitment would take away from your future career. My experience says differently. Student advocates can make an enormous impact with much less effort than any activist outside college, while still building valuable skills for their own futures.&lt;br/&gt;College advocates can have a high impact-to-effort ratio. For example, this past summer, the Princeton Student Climate Initiative wrote a white paper on a carbon fee &amp; dividend proposal in New Jersey. Such a policy could have a substantial impact on mitigating climate change impacts, like hurricane risk or agricultural losses, on top of stimulating the economy. We have been working with Assemblyman Zwicker to get a bill into the state legislature, and we believe it would have a good chance of passing: carbon pricing is supported by most economists, both parties, and even fossil fuel giants. How much effort did it take to propose this important economic reform for a state of nine million people, with a GDP of $465 billion? Surprisingly, only three hours of work per week, for a bit over a month.&lt;br/&gt;Climate change is not the only issue in which you can have a large, immediate impact. Consider the Immigration Day of Action in February, which mobilized over 500 students mailing postcards and letters to protest the first Muslim immigration ban. This was the work of the Princeton Muslim Advocates for Social Justice and Individual Dignity and Princeton Advocates for Justice . Or consider the Day of Action in March, organized by Princeton Citizen Scientists and PAJ, where nearly 1,500 people attended over 64 teach-ins on subjects ranging from nuclear proliferation to information censorship, and interacted with 13 University and community organizations promoting causes such as social justice and reducing the impact of money on politics. Or consider the fundraising work by Princeton Latinos y Amigos and Princeton DREAM Team, which raised $2,700 for undocumented high school students in the Trenton Area. Of all the issues that you could have an impact on here at Princeton, I am just getting started.&lt;br/&gt;If this recent advocacy still seems unimpressive, consider that student advocacy has often led to fundamental shifts in the course of history. The Voting Rights Act of 1965 outlawing racial segregation and discrimination was passed in large part due to the sit-ins and voter registration efforts by the Student Nonviolent Coordinating Committee. Korean student demonstrations were crucial in the June Struggle, which forced the South Korean government to transition from a military regime to a true democracy. Student activists, Princeton's included, pushed their own universities to divest from South Africa, which contributed to the dismantling of their apartheid system.&lt;br/&gt;Of all people, students can have particularly high impact per effort because of the college network. Where else in the world can one simply walk into the office of an international expert on climate change (Michael Oppenheimer), or human rights (Stanley Katz), or nuclear disarmament (Zia Mian)? When else would one be surrounded by thousands of other young, curious, and excited people? Who else is not overloaded with responsibilities like a family or full-time job?&lt;br/&gt;Furthermore, many University organizations, like the Pace Center for Civic Engagement, Fields Center for Equality &amp; Cultural Understanding, Office of Sustainability, and Student Government, are explicitly dedicated to supporting our projects. Because of them, we do not have to worry about logistical issues such as paying for posters, meeting places, websites, listservs, or food. This frees us to focus on what matters the most: brainstorming and implementing the most effective ways to impact issues.&lt;br/&gt;Above all, advocacy is a crucial skill to have whatever career you choose. The advocacy that convinces a peer to write a letter or a Republican to fight climate change is the same one that convinces a patient to follow a treatment plan or an investor to fund your project. And everyone can learn it. Take me for an example: a computer science major, I had taken zero classes related to effective political advocacy prior to starting the Princeton Student Climate Initiative last semester. But once the group started moving, once we started reading more on the topic, learning from other student groups and speaking with professors, I gained these advocacy skills. If I could do it, so can you.&lt;br/&gt;The Civic Engagement Fair is Friday, September 15 from 12-3 p.m. outside Dillon Gymnasium. Princeton's motto is "In the nation's service and the service of humanity." If they're just words to you, fine. Otherwise, I will see you there.&lt;br/&gt;Jonathan Lu is a senior in Computer Science from Fremont, Calif. He can be reached at </t>
         </is>
+      </c>
+      <c r="L50" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2607,10 +2764,13 @@
           <t>Indigenous issues, University governance, admin, policies, programs, curriculum, Anti-racism</t>
         </is>
       </c>
-      <c r="J51" t="inlineStr">
+      <c r="K51" t="inlineStr">
         <is>
           <t>Members of the Brown and Providence community gathered Wednesday afternoon to protest Citizens Bank's involvement in funding the Dakota Access Pipeline and other pipeline projects.&lt;br/&gt;Through its partnership with Sunoco Logistics Partners, Citizens Bank indirectly funds the Dakota Access Pipeline, according to an open letter that protestors wrote to President Christina Paxson P'19. Sunoco Logistics Partners also has an agreement with Energy Transfer Partners, and both of "these companies are building the Dakota Access, Bayou Bridge, Mariner East and Trans-Pecos pipelines," all of which "are neither moral nor sustainable," according to the open letter. These pipelines are responsible for "releasing a total of 111,000 gallons of oil into the environment" and threatening "the drinking water for the Standing Rock Sioux and 17 million others living downstream" while also violating infringing on "Lakota burial grounds in violation of treaty agreements," according to the letter.&lt;br/&gt;The letter urges the University to end its contract with Citizens Bank until the bank closes its line of credit with Sunoco Logistics Partners. The letter currently has over 100 signatures from members of the Brown community.&lt;br/&gt;Alejandro Subiotto&lt;br/&gt;Alejandro Subiotto&lt;br/&gt;Around 20 people stood outside Citizens Bank on Waterman Street chanting "shame on Citizens, shame on Brown," "stand with Standing Rock, Brown give up on your Citizens stock" and "Citizens Bank, you can't hide, divest now from genocide" while hoisting signs displaying phrases such as "Citizens: Stop funding violence against indigenous people," "No trans-pecos" and "#ShameOnCitizens."&lt;br/&gt;Before protesting outside the bank, protesters began their demonstration on the Quiet Green and then moved onto the Main Green to read the open letter aloud.&lt;br/&gt;Paxson plans to address the Brown community on "exploring strategies and actions Brown may undertake aligned with Brown's values," soon in response to a separate proposal submitted by the Advisory Committee on Corporate Responsibility in Investment Policies, wrote Vice President of Communications Cass Cliatt in an email to The Herald.&lt;br/&gt;The protest against Citizens Bank was hosted by both Environmental Justice at Brown and the Shame on Citizens Bank campaign, according to the protest's Facebook page. The protest was also held in collaboration with the FANG Collective, according to one of the event's organizers. The FANG Collective is a community group with several campaigns in the Northeast working against fracking.&lt;br/&gt;Ling, a supporter of the FANG Collective who chose not to provide The Herald with her last name, participated in the protest because she supports FANG's "intersectionality of eco-justice and racial justice" and appreciates that FANG is "very supportive of ... spaces" meant for people of color.&lt;br/&gt;The protest was just one of many actions taken by these groups to boycott Citizens Bank. Each week, the Shame on Citizens Bank campaign helps members of the community close their accounts with the bank, said Anusha Alles, a member of the Shame on Citizens Bank campaign. Citizens Bank indirectly funds "violence against indigenous people" and projects that are "destroying our climate," according to the campaign's Facebook page.&lt;br/&gt;The FANG Collective has also already hosted several protests against Citizens Bank, including a protest during which members of FANG locked themselves to the doors of the downtown headquarters of Citizens Bank.&lt;br/&gt;The relatively peaceful protest ended in an altercation, when several protesters got into an argument with a passerby who repeatedly yelled, "Trump, Trump, Trump" and insisted "If you don't like America, you can leave."&lt;br/&gt;Correction: A previous version of this article misstated that the open letter to President Christina Paxson P'19 said the Dakota Access, Bayou Bridge, Mariner East and Trans-Pecos pipelines is responsible for "releasing a total of 111,000 gallons of oil into the environment." In fact, the letter said Sunoco Logistics and Energy Transfer Partners were responsible for the spillage. In addition, the article misstated that the letter said the four pipelines are responsible for desecrating Lakota burial grounds. In fact, the letter said the Dakota Access Pipeline is responsible for threatening Lakota burial grounds. The Herald regrets the errors.  Share on Facebook Share on Twitter</t>
         </is>
+      </c>
+      <c r="L51" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -2650,10 +2810,13 @@
           <t>Public funding for higher education</t>
         </is>
       </c>
-      <c r="J52" t="inlineStr">
+      <c r="K52" t="inlineStr">
         <is>
           <t>This past week, Rutgers students, faculty, staff and alumni signed aletterof support with the students on strike at the University of Puerto Rico . The UPR student body concerns echo a resistance to a larger series of austerity measures imposed by the United States Congress with the passage of the 2016 PROMESA Bill. The legislation codified the Fiscal Oversight and Management Board the authority to manage Puerto Rico's $72 billion debt to the United States government. United States oversight of the debt has led to a $500 million cut to the UPR budget. Slashing roughly one-third of the public university's budget not only causes a detriment to the foundation of education for Puerto Rico, but sets a precedent for further permeation of United States fiscal intervention.&lt;br/&gt;To provide some historical context, a series of United States Supreme Court opinions known as the Insular Cases had claimed territories after the Spanish-American War in 1901, including Puerto Rico as "foreign in a domestic sense." Thus, while Puerto Ricans are citizens of the United States, they do not benefit from many of the rights outlined by the Constitution. Puerto Ricans cannot vote in elections or incur any of the benefits of a representational democracy and yet the United States' legal and monetary structures have made their mark of sovereignty on the island at multiple levels. Although to be dealt at a national level, the complicities occur at local levels as well. For example, Rutgers University has its own investment in the financial institutions that have bought Puerto Rico's debt in the form of bonds, which now wreak havoc on its economy. At a local level, the hedge fund divestment campaign that the Rutgers One coalition has spearheaded will continue as an ongoing effort to untie the exploitative economic binds that our own University has supported through its practices. Although this is reason enough for solidarity, the relationship between U.S. and Puerto Rican student activism should not be limited to dismantling market interests. A deeper question regarding an ethics of recognition probes the U.S. University consciousness.&lt;br/&gt;Thus even before laying out a much-needed criticism of the kind of exploitative mingling that the general legal and monetary schema allows at institutional levels of power, the call for solidarity must be explained. Graduate student organizers and UPR alumni Mario Mercado Diaz and Isabel Guzzardo wrote and circulated a Rutgers University affiliated letter of solidarity during a one-week strike in which students barricaded themselves inside the campus, halting classes for a week. The list of demands was outlined and disseminated to the departments, union staff and student organizations supportive of the cause.&lt;br/&gt;Members of the Rutgers Community must be concerned with what is going on in order to uphold democratic values worldwide. I would go further to say the imposition of democratic values runs into its own set of problems. Nonetheless, the blatant silence from many mainstream news outlets proves to contradict past consumption practices of an American reading public of national protests abroad. Perhaps the way in which we as a reading public wish to relate to publics in the Middle East during the region's own string of protests speaks more to the types of intervention tactics used by United States power. Insofar, the silence on Puerto Rico's crisis remains distant, while the strife of a Turkish or Iranian public is deemed an unacceptable violation of human rights, the representation speaks to the desires of an American public. Such desires support what kind of interventions are deemed responsible for spreading democracy through war or intervention. The spotlight that is not being shined on UPR reveals more about the United States notion of its citizenry as well as who it accepts as recognizable within its publics. Tuition hikes prove to be a relatable point among all universities, particularly state universities in the United States, like Rutgers, our own student body should provide greater solidarity to the efforts at UPR. Their struggle, though silenced by greater outlets, indeed speaks to a greater attack on public services and livability. The Rutgers University solidarity campaign proves to be necessary for this reason, and above all the else, we demand the students of UPR be recognized.&lt;br/&gt;Meryem Uzumcu is a School of Arts and Sciences senior majoring in planning and public policy, Middle Eastern studies and women's and gender studies. Her column, "Fahrenheit 250," runs on alternate Tuesdays.&lt;br/&gt;YOUR VOICE | The Daily Targum welcomes submissions from all readers. Due to space limitations in our print newspaper, letters to the editor must not exceed 500 words. Guest columns and commentaries must be between 700 and 850 words. All authors must include their name, phone number, class year and college affiliation or department to be considered for publication. Please submit via email to  by 4 p.m. to be considered for the following day's publication. Columns, cartoons and letters do not necessarily reflect the views of the Targum Publishing Company or its staff.</t>
         </is>
+      </c>
+      <c r="L52" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2693,10 +2856,13 @@
           <t>Tuition, fees, financial aid, Trump and/or his administration (Against)</t>
         </is>
       </c>
-      <c r="J53" t="inlineStr">
+      <c r="K53" t="inlineStr">
         <is>
           <t>A small group of students entered Chancellor Patrick Gallagher's office Tuesday morning with a letter of 15 demands, including disarming University police.&lt;br/&gt;The letter also demanded the University vocally endorse a graduate student union, divest from fossil fuels, install a $15 Pitt-wide minimum wage and freeze tuition.&lt;br/&gt;One student protester said Gallagher was not present to receive the letter and Pitt police came to remove the student protesters from the office despite peacefully protesting.&lt;br/&gt;According to University spokesperson Joe Miksch, the students were given the option to speak with another senior administrator, but they declined the invitation. After sitting in the middle of a "working reception area," Pitt police asked the students to leave, which Miksch said they did "without incident."&lt;br/&gt;The students then went to a small enclave on the Cathedral's second floor. They plan to occupy the space day and night "until their demands are met" or until Friday - when the group plans to protest on Towers Patio.&lt;br/&gt;The Towers "occupation" will feature speakers from groups such as Pitt's United Students Against Sweatshops chapter and Campus Anti-Fascist Network: Pittsburgh. Protesters said the rally is being held to coincide with the first anniversary of a protest last November against Donald Trump and student debt. Pitt police arrested two people during last year's protest after an altercation.</t>
         </is>
+      </c>
+      <c r="L53" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2736,10 +2902,13 @@
           <t>Tuition, fees, financial aid, Trump and/or his administration (Against)</t>
         </is>
       </c>
-      <c r="J54" t="inlineStr">
+      <c r="K54" t="inlineStr">
         <is>
           <t>A group of students marched throughout Oakland Friday afternoon waving flags and signs with slogans such as "Disarm the police, arm your desire" and chanting "A.C.A.B., all cops are bastards."&lt;br/&gt;Their words elicited varying reactions from observers.&lt;br/&gt;"Go home commies!" someone yelled from a window in Holland Hall.&lt;br/&gt;"They're making fools of themselves," a man outside of Noodles and Company said.&lt;br/&gt;Another man standing outside of Uncle Sam's Sandwich Bar cheered them on and sang along with their chant.&lt;br/&gt;"I could get in on this!" he shouted.&lt;br/&gt;The march - which began on Fifth Avenue, went through Schenley Quad onto Forbes and ended on Oakland Avenue - was the aftermath of a rally staged Friday afternoon by about 40 students and community members.&lt;br/&gt;The rally marked the end of an "occupation" of the Cathedral of Learning which began Tuesday. The "occupation" began with a small group of students who went to Chancellor Patrick Gallagher's office early Tuesday morning with a letter of 15 demands, including disarming the Pitt police, divesting from fossil fuels and implementing a University-wide $15 minimum wage.&lt;br/&gt;According to a rally organizer, who didn't want to be named, the four-day occupation and Friday rally were held to coincide with the first anniversary of a protest last November against student debt and President Donald Trump. Pitt police arrested two people during the protest last year after an altercation took place in Towers lobby.&lt;br/&gt;"We wanted to show [the University and Pitt police that] we are still here, still taking action," the organizer said.&lt;br/&gt;Students and community members marched in protest of police brutality Friday afternoon. (Photo by Christian Snyder | Contributing Editor)&lt;br/&gt;Associate Dean of Students Linda Williams Moore and Dean of Students Kenyon Bonner were present to observe the rally. About 10 to 15 Pitt police officers stood inside Towers lobby while four to five stood outside the entrance of Towers. Several police cars were parked across on Thackeray Avenue. Unlike last year, there were no violent confrontations between rally attendees and the police.&lt;br/&gt;Prior to the rally, Bonner approached the protesters with some "ground rules" for the event, including that they could not go into Towers lobby and that they would face repercussions if the rally turned into anything confrontational.&lt;br/&gt;"I just told them policies and protocol. This is a reservable space, they need to reserve the space for a protest here," he said of Towers lobby. "There's plenty of places off-campus where they can protest, just not this place."&lt;br/&gt;Students and community members - several clad in "Black Lives Matter" shirts or with their mouths covered by bandanas - joined hands and formed a circle in front of Tower B around 4 p.m.&lt;br/&gt;Several individuals spoke at the rally - including a Pitt alum who recounted their experience at last year's protest and another student who read an account said to be from one of the individuals arrested at the protest last November. The first speaker reminded attendees that the demonstration was being held to protest against the Pitt police.&lt;br/&gt;Each rally attendee asked refused to provide names to The Pitt News.&lt;br/&gt;The Pitt alum, who was present at last year's protest and witnessed and filmed the incident between students and police, said the police's action were "brutal and unjust" and blamed the University for allowing it to happen.&lt;br/&gt;"I love this University, I grew so much here," they said. "But in my experience they only care about what you have to say if it aligns with their goals of power, prestige and profit."&lt;br/&gt;Another rally attendee spoke about deaths of people of color by the hands of police, citing individuals such as 14-year-old Jason Pero, an eighth grader who died on the Bad River Band of Lake Superior Chippewa's reservation less than two weeks ago after police shot Pero.&lt;br/&gt;"All these cops are stealing life every day, it's their job to do that," they said.&lt;br/&gt;A student who wished to remain anonymous said he wasn't involved with the group that organized the rally but joined it halfway through because he wanted to show support for their views. He was unsure if some of the messages of the group were well conveyed, though.&lt;br/&gt;"The chanting was good, but I don't know if it was productive," he said of the "group of white people" chanting anti-police slogans.&lt;br/&gt;The student said plenty of cops do have their priorities in the wrong place, but there are many who just "want to make a living."&lt;br/&gt;"I don't think the right response is to dehumanize the administration," he said.&lt;br/&gt;The students and community members ended their march on Oakland Avenue around 5 p.m. Several broke off to go elsewhere. Others hung around and engaged in a discussion with Cameron Hallihan, a sophomore neuroscience major and member of the Pitt College Republicans who came to the rally to ask its attendees about their political views and goals.&lt;br/&gt;"I think they're misguided and I disagree, but I don't disagree with their right to free speech," Hallihan said.&lt;br/&gt;Another rally attendee said they thought the rally served its purpose in showing continued opposition to the Pitt police's actions last year and their involvement in "defending capitalism."&lt;br/&gt;"More needs to be done, but it says something that there were less than 50 of us and like 20 cop cars were around that place. It shows the University's scared of us," they said. "It went well, but it's not over."</t>
         </is>
+      </c>
+      <c r="L54" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -2784,10 +2953,13 @@
           <t>Indigenous issues</t>
         </is>
       </c>
-      <c r="J55" t="inlineStr">
+      <c r="K55" t="inlineStr">
         <is>
           <t>(Courtesy Earthstar Geographies Esri, HERE, DeLorme)&lt;br/&gt;Two Ryerson students were arrested yesterday on Parliament Hill while protesting the Kinder Morgan Trans Mountain expansion project, according to Divest Ryerson’s Facebook page.&lt;br/&gt;The students were identified as Ben Donato-Woodger and Emma Beattie who were among more than 200 people from all across Canada to call on Prime Minister Justin Trudeau to reject the Kinder Morgan pipeline that will run from the Alberta oilsands to the Burrard Inlet in Burnaby, B.C.&lt;br/&gt;According to Donato-Woodger, protesters marched from the University of Ottawa to Parliament Hill to hold the government accountable for its decision regarding the pipeline’s construction. The police had barricaded entrances into the House of Commons, but the protesters were insistent on getting inside. &lt;br/&gt;“They [police] warned that if we crossed, we would be arrested,” said Donato-Woodger. From the crowd, 99 students who crossed the barricades were arrested. While they were not criminally charged or ticketed, they received a notice for trespassing. &lt;br/&gt;The focus of the demonstration was to delay the approval of the expansion of the pipeline, a decision the Liberals have to make by mid-December. &lt;br/&gt;However, the larger goal was to call on Trudeau to keep his word on Canada’s international emissions-cutting promises, according to Donato-Woodger. &lt;br/&gt;“We know we can turn a delay into a rejection but it looks like Trudeau will fast-track the approval,” said Donato-Woodger. “The tar sands are the biggest growing sector of emissions. We would be meeting our international obligation if it wasn’t for that. We wanted to send a message that he [Trudeau] needs to reject pipelines and get serious about climate change.” &lt;br/&gt;Tamara Jones, the vice-president of equity at the Ryerson Students’ Union, says this was the largest act of student climate civil disobedience, the protest has and will bring attention to the problems people see in the pipeline construction. &lt;br/&gt;“I feel like they went there knowing that this would happen,” said Jones. “I also feel like the photos and video that have been gotten from this opportunity are going to be shared very widely and get a lot of attention so I think in some respects that’s what they were looking for.”</t>
         </is>
+      </c>
+      <c r="L55" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -2832,10 +3004,13 @@
           <t>Indigenous issues</t>
         </is>
       </c>
-      <c r="J56" t="inlineStr">
+      <c r="K56" t="inlineStr">
         <is>
           <t>99 Arrests At Climate Protest in Ottawa&lt;br/&gt;Former Concordia Student and Current CSU Executive Among Those Arrested&lt;br/&gt;News by Claire Loewen — Published October 30, 2016 | Comments&lt;br/&gt;Follow @@clairelwn&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Photo Courtesy Saffron Blaze&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Growing tension towards the Liberal government’s backtracking on climate policy promises caused around 200 protesters to march in Ottawa on Monday, Oct. 24. &lt;br/&gt;They marched from the University of Ottawa campus to Parliament Hill, where the majority of the group attempted to enter the building through the front entrance, near the Eternal Flame on Wellington St. &lt;br/&gt;Ninety-nine protesters were arrested and issued citations for trespassing from the RCMP for climbing police barricades. The notices will last for three months, according to RCMP media relations officer Cpl. Annie Delisle. &lt;br/&gt;Among the group were CSU Loyola Coordinator and member of Divest Concordia Marcus Peters and former Concordia student Kyle Ritchie. Both agreed that in comparison to Montreal protests, the RCMP national division was relatively non-confrontational in handling protesters. &lt;br/&gt;“The RCMP […] remains in constant contact with the organizers of any planned demonstration to ensure the safety and security of the protestors, Parliamentarians, employees and visitors to the grounds of Parliament Hill,” said Delisle in an email.&lt;br/&gt;The main issue at hand during the protest was the Kinder Morgan Trans Mountain oil pipeline, construction for which has yet to be approved by the Liberal government. The decision should be made by mid-December, according to the Liberals. The group was also demonstrating against various pipeline projects, like the Energy East Pipeline &lt;br/&gt;“I’m very passionate about these issues because I’ve been involved in environmental activism at Concordia for a few years and they just keep popping up,” Peters said. &lt;br/&gt;For Peters, the point of the protest was to “counter the image of [Prime Minister Justin Trudeau] having all that support from youth and from activists.” &lt;br/&gt;“We need to start putting the pressure […] to show the stark contrast between the words and actions,” he said.&lt;br/&gt;He added that protesters wanted to create a space in the media to talk about backtracking on the part of the Liberal government, which he believes is not discussed enough. &lt;br/&gt;The protest and arrests were covered by a variety of mainstream news organizations, from the Huffington Post to the Globe and Mail. &lt;br/&gt;The protest was organized by 350.org, a grassroots climate organization aiming to hold global leaders accountable “to the realities of science and the principles of justice,” according to the website. &lt;br/&gt;Former Concordia student Kyle Ritchie was among those issued trespassing citations. For him, the protest was about pushing the government towards a sense of urgency and crisis when it comes to climate change. &lt;br/&gt;“This isn’t a 100 year slow transition, this is an immediate crisis that they need to start working on,” he said. &lt;br/&gt;According to a survey released by Abacus Data in April, the Liberal government won the Oct. 19, 2015 election largely due to the millennial vote. Forty-five per cent of Canadians between 18 and 25 voted Liberal, and more young people voted for the Liberals in every region of the country than for any other party. &lt;br/&gt;“Millennials in plurality definitely voted for Justin Trudeau, and a lot of them care about the environment,” said Ritchie, adding that he believes it’s important to show that the trouble and conflict will only increase if the government does not uphold its promises on climate change. &lt;br/&gt;Liberal promises from 2015 claimed they would “provide national leadership and join with the provinces and territories to take action on climate change, put a price on carbon, and reduce carbon pollution.” &lt;br/&gt;Their campaign platform also criticized former Prime Minister Stephen Harper for failing to take action on climate change. &lt;br/&gt;“We will end the cycle of federal parties—of all stripes—setting arbitrary targets without a real federal/provincial/territorial plan in place,” the platform states. &lt;br/&gt;The day after the protest, Trudeau attended a youth labour forum in Ottawa. Many attending delegates turned their backs on the Prime Minister, and some “heckled” him, according to the Globe and Mail. Others held signs reading “Keep The Promise,” according to iPolitics.ca&lt;br/&gt;These actions reflected anger towards Liberal support for the Trans Pacific Partnership trade deal, and comments from Finance Minister Bill Morneau that were called arrogant by Conservatives and New Democrats, who accused Morneau of misunderstanding Canada’s youth unemployment problem. &lt;br/&gt;While these issues are not directly related to climate change policy, Tuesday’s events show that at least some millennials are unhappy with the Liberal government’s ability to abide by its platform in totality. &lt;br/&gt;Trudeau has pushed women’s and LGBTQ issues into the spotlight since taking office by making public appearances at various Pride events and publicly stating that he is a feminist. &lt;br/&gt;But Ritchie believes many people “lent” the Liberals their vote strategically, in order to kick Stephen Harper out of the running. &lt;br/&gt;“So we’re seeing after about a year or so that people’s patience is wearing off,” he said. &lt;br/&gt;“I think the honeymoon’s over at this point. It’s been about a year, and they haven’t done much to impress millennials or anyone else who voted for them for more progressive reasons.”&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;By commenting on this page you agree to the terms of our Comments Policy.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Please enable JavaScript to view the comments powered by Disqus.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Related Reading&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;Montrealers Protest Against Fossil Fuels&lt;br/&gt;Erika Morris&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Special Issue&lt;br/&gt;Recapping Climate Welcome&lt;br/&gt;John Saigle&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;Quebec gets peek  at president’s tuition plan&lt;br/&gt;Justin Giovannetti&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Opinions&lt;br/&gt;Editorial&lt;br/&gt;Julia Wolfe</t>
         </is>
+      </c>
+      <c r="L56" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -2880,10 +3055,13 @@
           <t>Indigenous issues</t>
         </is>
       </c>
-      <c r="J57" t="inlineStr">
+      <c r="K57" t="inlineStr">
         <is>
           <t>Select U of O students banned from Parliament for three months&lt;br/&gt;On Oct. 24, approximately 200 members of the Ottawa community, including 100 youth and students from across the country, rallied on Parliament Hill to protest the Kinder Morgan pipeline—only to be met with arrests by police.&lt;br/&gt;The existing 1,150 km pipeline, built in 1953, has been approved for a 980 km expansion between Strathcona County, Alta., and Burnaby, B.C. However, many groups are in opposition to the pipeline since it will pass through the land of several Indigenous communities.&lt;br/&gt;Aside from the effects this will have on First Nations groups, concerns also arose due to the potential effects of the pipeline on marine life, along with other environmental concerns. According to the group 350.org, Sophie Birks, a student from McGill University who attended the rally, summed up the event by saying, “climate leaders don’t build pipelines.”&lt;br/&gt;The Oct. 24 rally began at the University of Ottawa campus, where students, Indigenous groups, and other community members marched to Parliament Hill.&lt;br/&gt;Lisa Gunn, a masters student in international development with women’s studies, was one of the students present at the rally who was arrested.&lt;br/&gt;“Everyone was excited to be there, to take a stand on something we believe in and care about,” said Gunn, recalling how she had originally found out about the protest during a previous conference on pipelines organized by the 350.org.&lt;br/&gt;According to Gunn, “there were a couple points when (the protesters) were interacting with police,” which involved intentionally crossing a police barricade.&lt;br/&gt;Approximately 100 students ended up crossing the barricade, and Gunn said that she was among the last 10 to do so.&lt;br/&gt;Following their arrest, Gunn said that the police took her and the other protesters to the side, took down their names, read them their rights, and issued trespassing warrants. Now, Gunn and the others arrested at the protest are banned from Parliament Hill for the next three months.&lt;br/&gt;The Oct. 24 protest has been called “the largest act of youth-led climate civil disobedience in Canadian history” by 350.org and despite the arrests, Gunn is hopeful about further steps to take on the issue.&lt;br/&gt;“I know that there will be follow-up action, just to hammer home the (Kinder Morgan) pipeline,” she said.&lt;br/&gt;Gunn believes that there will be a lot of pressure on the federal government regarding the pipeline, since 350.org is now asking all the protesters who were arrested to write a letter to Prime Minister Justin Trudeau on the back of their trespassing warrants, in response to the protest and in opposition to the pipeline.&lt;br/&gt;“We (the youth) were one of the main demographics that brought the Liberal government into power,” Gunn said. And because of this, she hopes that this demographic will have their voices heard.&lt;br/&gt;For students wishing to get involved with this initiative, and others of the same nature, Gunn suggests joining local divestment  groups like Fossil Free uOttawa.&lt;br/&gt;Share this:Click to share on Twitter (Opens in new window)Click to share on Facebook (Opens in new window)Click to share on Google+ (Opens in new window)</t>
         </is>
+      </c>
+      <c r="L57" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -2923,10 +3101,13 @@
           <t>Public funding for higher education</t>
         </is>
       </c>
-      <c r="J58" t="inlineStr">
+      <c r="K58" t="inlineStr">
         <is>
           <t>This past week, Rutgers students, faculty, staff and alumni signed aletterof support with the students on strike at the University of Puerto Rico . The UPR student body concerns echo a resistance to a larger series of austerity measures imposed by the United States Congress with the passage of the 2016 PROMESA Bill. The legislation codified the Fiscal Oversight and Management Board the authority to manage Puerto Rico's $72 billion debt to the United States government. United States oversight of the debt has led to a $500 million cut to the UPR budget. Slashing roughly one-third of the public university's budget not only causes a detriment to the foundation of education for Puerto Rico, but sets a precedent for further permeation of United States fiscal intervention.&lt;br/&gt;To provide some historical context, a series of United States Supreme Court opinions known as the Insular Cases had claimed territories after the Spanish-American War in 1901, including Puerto Rico as "foreign in a domestic sense." Thus, while Puerto Ricans are citizens of the United States, they do not benefit from many of the rights outlined by the Constitution. Puerto Ricans cannot vote in elections or incur any of the benefits of a representational democracy and yet the United States' legal and monetary structures have made their mark of sovereignty on the island at multiple levels. Although to be dealt at a national level, the complicities occur at local levels as well. For example, Rutgers University has its own investment in the financial institutions that have bought Puerto Rico's debt in the form of bonds, which now wreak havoc on its economy. At a local level, the hedge fund divestment campaign that the Rutgers One coalition has spearheaded will continue as an ongoing effort to untie the exploitative economic binds that our own University has supported through its practices. Although this is reason enough for solidarity, the relationship between U.S. and Puerto Rican student activism should not be limited to dismantling market interests. A deeper question regarding an ethics of recognition probes the U.S. University consciousness.&lt;br/&gt;Thus even before laying out a much-needed criticism of the kind of exploitative mingling that the general legal and monetary schema allows at institutional levels of power, the call for solidarity must be explained. Graduate student organizers and UPR alumni Mario Mercado Diaz and Isabel Guzzardo wrote and circulated a Rutgers University affiliated letter of solidarity during a one-week strike in which students barricaded themselves inside the campus, halting classes for a week. The list of demands was outlined and disseminated to the departments, union staff and student organizations supportive of the cause.&lt;br/&gt;Members of the Rutgers Community must be concerned with what is going on in order to uphold democratic values worldwide. I would go further to say the imposition of democratic values runs into its own set of problems. Nonetheless, the blatant silence from many mainstream news outlets proves to contradict past consumption practices of an American reading public of national protests abroad. Perhaps the way in which we as a reading public wish to relate to publics in the Middle East during the region's own string of protests speaks more to the types of intervention tactics used by United States power. Insofar, the silence on Puerto Rico's crisis remains distant, while the strife of a Turkish or Iranian public is deemed an unacceptable violation of human rights, the representation speaks to the desires of an American public. Such desires support what kind of interventions are deemed responsible for spreading democracy through war or intervention. The spotlight that is not being shined on UPR reveals more about the United States notion of its citizenry as well as who it accepts as recognizable within its publics. Tuition hikes prove to be a relatable point among all universities, particularly state universities in the United States, like Rutgers, our own student body should provide greater solidarity to the efforts at UPR. Their struggle, though silenced by greater outlets, indeed speaks to a greater attack on public services and livability. The Rutgers University solidarity campaign proves to be necessary for this reason, and above all the else, we demand the students of UPR be recognized.&lt;br/&gt;Meryem Uzumcu is a School of Arts and Sciences senior majoring in planning and public policy, Middle Eastern studies and women's and gender studies. Her column, "Fahrenheit 250," runs on alternate Tuesdays.&lt;br/&gt;YOUR VOICE | The Daily Targum welcomes submissions from all readers. Due to space limitations in our print newspaper, letters to the editor must not exceed 500 words. Guest columns and commentaries must be between 700 and 850 words. All authors must include their name, phone number, class year and college affiliation or department to be considered for publication. Please submit via email to  by 4 p.m. to be considered for the following day's publication. Columns, cartoons and letters do not necessarily reflect the views of the Targum Publishing Company or its staff.</t>
         </is>
+      </c>
+      <c r="L58" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -2966,10 +3147,13 @@
           <t>University governance, admin, policies, programs, curriculum, Labor and work</t>
         </is>
       </c>
-      <c r="J59" t="inlineStr">
+      <c r="K59" t="inlineStr">
         <is>
           <t>Members of the Barnard contingent faculty union and roughly 20 students demonstrated their discontent with Barnard President Debora Spar on Wednesday night during an event at which she was speaking.&lt;br/&gt;The panel featured Spar, Anna Quindlen, Writer-in-Residence Jennifer Finney Boylan, writer Lizzie Skurnick, and writer and editor Cathi Hanauer, who read selections from the new book "The Bitch is Back." The book-which all of the panelists contributed material to-explores how societal ideas about women, feminism, and aging have changed in the last 10 years.&lt;br/&gt;Although the student demonstrators remained in their seats during other panelists' speeches, they stood in the aisles when Spar took to the podium, silently holding posters with phrases critical of what they saw as Spar's lack of engagement with other pertinent issues, such as the ongoing negotiations with the contingent faculty union, race relations, and fossil fuel divestment, among other issues.&lt;br/&gt;One sign reading "President Spar: For Poor Women Botox Isn't "There For The Picking" responded to an essay published by Spar in The New York Times last Sunday titled "Aging and My Beauty Dilemma," which is included in "The Bitch is Back."&lt;br/&gt;The essay was critiqued by some readers who felt that Spar's emphasis on appearance and cosmetic surgery was problematic, especially given her position at Barnard.&lt;br/&gt;Ella Merrill, BC '18, who was one of the silent demonstrators, said that although the panel was "good for what it was," it was not representative of the views of Barnard's students and community members.&lt;br/&gt;"I think, especially after her [Spar's] New York Times op-ed, a lot of us are frustrated that this is what she is using her position of power to discuss," she said. "Why not talk about the many issues facing the Barnard community at large?"&lt;br/&gt;Shortly before the event, members of the contingent faculty union-which was not involved in the student demonstration-also addressed Spar's essay in leaflets that they distributed outside of the Event Oval, which also called attention to their ongoing contract negotiations.&lt;br/&gt;"Feminist issues Barnard alumnae consider a very high priority: health care and fair pay for women faculty," the flier read. "'Feminist-leaning' issues Barnard alumnae consider very low priority: the 'beauty' dilemmas of the 1%."&lt;br/&gt;English lecturer Sonam Singh, a member of the contingent faculty union's bargaining committee, said that having a presence at the event was a way for the union to try and engage with Spar, who he said has been absent from the negotiating table.&lt;br/&gt;"We've had a hard time getting her attention. While she's certainly directing negotiations on behalf of the college, she's never spoken with us," he said. "As negotiations drag out, we do want to get her attention."&lt;br/&gt;Singh also said that although the union, who recently delivered an alumnae petition in support of the union to Spar's office last Tuesday, would have distributed flyers regardless of whether Spar's essay had been published or not, he found her op-ed to be "frustrating."&lt;br/&gt;"Since you are the president of a very important college, and you have this platform, we would like you to focus on issues that matter in a more significant way," he said.&lt;br/&gt;Ginger Mayo, BC '20, a member of Divest Barnard who demonstrated at the event, said that she found the essay to be "tone-deaf," particularly as it was published the same week as the 20th anniversary of the clerical worker's strike.&lt;br/&gt;"I don't think that the group [of student demonstrators] had a particular issue with the content of the piece, but with the tone and with using this very important platform to talk about something extremely artificial and very inaccessible to most women," she said.&lt;br/&gt;But regardless of Spar's controversial essay, student demonstrators said they believed that Spar's position as the leader and public figurehead of the college meant that she had the responsibility to use her platform to discuss issues facing the larger Barnard community.&lt;br/&gt;"Debora Spar does represent us, and we think her role is important," Merrill said.&lt;br/&gt; | @ACBandrowski</t>
         </is>
+      </c>
+      <c r="L59" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -3009,10 +3193,13 @@
           <t>University governance, admin, policies, programs, curriculum, Labor and work</t>
         </is>
       </c>
-      <c r="J60" t="inlineStr">
+      <c r="K60" t="inlineStr">
         <is>
           <t>Members of the Barnard contingent faculty union and roughly 20 students demonstrated their discontent with Barnard President Debora Spar on Wednesday night during an event at which she was speaking.&lt;br/&gt;The panel featured Spar, Anna Quindlen, Writer-in-Residence Jennifer Finney Boylan, writer Lizzie Skurnick, and writer and editor Cathi Hanauer, who read selections from the new book "The Bitch is Back." The book-which all of the panelists contributed material to-explores how societal ideas about women, feminism, and aging have changed in the last 10 years.&lt;br/&gt;Although the student demonstrators remained in their seats during other panelists' speeches, they stood in the aisles when Spar took to the podium, silently holding posters with phrases critical of what they saw as Spar's lack of engagement with other pertinent issues, such as the ongoing negotiations with the contingent faculty union, race relations, and fossil fuel divestment, among other issues.&lt;br/&gt;One sign reading "President Spar: For Poor Women Botox Isn't "There For The Picking" responded to an essay published by Spar in The New York Times last Sunday titled "Aging and My Beauty Dilemma," which is included in "The Bitch is Back."&lt;br/&gt;The essay was critiqued by some readers who felt that Spar's emphasis on appearance and cosmetic surgery was problematic, especially given her position at Barnard.&lt;br/&gt;Ella Merrill, BC '18, who was one of the silent demonstrators, said that although the panel was "good for what it was," it was not representative of the views of Barnard's students and community members.&lt;br/&gt;"I think, especially after her [Spar's] New York Times op-ed, a lot of us are frustrated that this is what she is using her position of power to discuss," she said. "Why not talk about the many issues facing the Barnard community at large?"&lt;br/&gt;Shortly before the event, members of the contingent faculty union-which was not involved in the student demonstration-also addressed Spar's essay in leaflets that they distributed outside of the Event Oval, which also called attention to their ongoing contract negotiations.&lt;br/&gt;"Feminist issues Barnard alumnae consider a very high priority: health care and fair pay for women faculty," the flier read. "'Feminist-leaning' issues Barnard alumnae consider very low priority: the 'beauty' dilemmas of the 1%."&lt;br/&gt;English lecturer Sonam Singh, a member of the contingent faculty union's bargaining committee, said that having a presence at the event was a way for the union to try and engage with Spar, who he said has been absent from the negotiating table.&lt;br/&gt;"We've had a hard time getting her attention. While she's certainly directing negotiations on behalf of the college, she's never spoken with us," he said. "As negotiations drag out, we do want to get her attention."&lt;br/&gt;Singh also said that although the union, who recently delivered an alumnae petition in support of the union to Spar's office last Tuesday, would have distributed flyers regardless of whether Spar's essay had been published or not, he found her op-ed to be "frustrating."&lt;br/&gt;"Since you are the president of a very important college, and you have this platform, we would like you to focus on issues that matter in a more significant way," he said.&lt;br/&gt;Ginger Mayo, BC '20, a member of Divest Barnard who demonstrated at the event, said that she found the essay to be "tone-deaf," particularly as it was published the same week as the 20th anniversary of the clerical worker's strike.&lt;br/&gt;"I don't think that the group [of student demonstrators] had a particular issue with the content of the piece, but with the tone and with using this very important platform to talk about something extremely artificial and very inaccessible to most women," she said.&lt;br/&gt;But regardless of Spar's controversial essay, student demonstrators said they believed that Spar's position as the leader and public figurehead of the college meant that she had the responsibility to use her platform to discuss issues facing the larger Barnard community.&lt;br/&gt;"Debora Spar does represent us, and we think her role is important," Merrill said.&lt;br/&gt; | @ACBandrowski</t>
         </is>
+      </c>
+      <c r="L60" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -3052,10 +3239,13 @@
           <t>University governance, admin, policies, programs, curriculum, Labor and work</t>
         </is>
       </c>
-      <c r="J61" t="inlineStr">
+      <c r="K61" t="inlineStr">
         <is>
           <t>Members of the Barnard contingent faculty union and roughly 20 students demonstrated their discontent with Barnard President Debora Spar on Wednesday night during an event at which she was speaking.&lt;br/&gt;The panel featured Spar, Anna Quindlen, Writer-in-Residence Jennifer Finney Boylan, writer Lizzie Skurnick, and writer and editor Cathi Hanauer, who read selections from the new book "The Bitch is Back." The book-which all of the panelists contributed material to-explores how societal ideas about women, feminism, and aging have changed in the last 10 years.&lt;br/&gt;Although the student demonstrators remained in their seats during other panelists' speeches, they stood in the aisles when Spar took to the podium, silently holding posters with phrases critical of what they saw as Spar's lack of engagement with other pertinent issues, such as the ongoing negotiations with the contingent faculty union, race relations, and fossil fuel divestment, among other issues.&lt;br/&gt;One sign reading "President Spar: For Poor Women Botox Isn't "There For The Picking" responded to an essay published by Spar in The New York Times last Sunday titled "Aging and My Beauty Dilemma," which is included in "The Bitch is Back."&lt;br/&gt;The essay was critiqued by some readers who felt that Spar's emphasis on appearance and cosmetic surgery was problematic, especially given her position at Barnard.&lt;br/&gt;Ella Merrill, BC '18, who was one of the silent demonstrators, said that although the panel was "good for what it was," it was not representative of the views of Barnard's students and community members.&lt;br/&gt;"I think, especially after her [Spar's] New York Times op-ed, a lot of us are frustrated that this is what she is using her position of power to discuss," she said. "Why not talk about the many issues facing the Barnard community at large?"&lt;br/&gt;Shortly before the event, members of the contingent faculty union-which was not involved in the student demonstration-also addressed Spar's essay in leaflets that they distributed outside of the Event Oval, which also called attention to their ongoing contract negotiations.&lt;br/&gt;"Feminist issues Barnard alumnae consider a very high priority: health care and fair pay for women faculty," the flier read. "'Feminist-leaning' issues Barnard alumnae consider very low priority: the 'beauty' dilemmas of the 1%."&lt;br/&gt;English lecturer Sonam Singh, a member of the contingent faculty union's bargaining committee, said that having a presence at the event was a way for the union to try and engage with Spar, who he said has been absent from the negotiating table.&lt;br/&gt;"We've had a hard time getting her attention. While she's certainly directing negotiations on behalf of the college, she's never spoken with us," he said. "As negotiations drag out, we do want to get her attention."&lt;br/&gt;Singh also said that although the union, who recently delivered an alumnae petition in support of the union to Spar's office last Tuesday, would have distributed flyers regardless of whether Spar's essay had been published or not, he found her op-ed to be "frustrating."&lt;br/&gt;"Since you are the president of a very important college, and you have this platform, we would like you to focus on issues that matter in a more significant way," he said.&lt;br/&gt;Ginger Mayo, BC '20, a member of Divest Barnard who demonstrated at the event, said that she found the essay to be "tone-deaf," particularly as it was published the same week as the 20th anniversary of the clerical worker's strike.&lt;br/&gt;"I don't think that the group [of student demonstrators] had a particular issue with the content of the piece, but with the tone and with using this very important platform to talk about something extremely artificial and very inaccessible to most women," she said.&lt;br/&gt;But regardless of Spar's controversial essay, student demonstrators said they believed that Spar's position as the leader and public figurehead of the college meant that she had the responsibility to use her platform to discuss issues facing the larger Barnard community.&lt;br/&gt;"Debora Spar does represent us, and we think her role is important," Merrill said.&lt;br/&gt; | @ACBandrowski</t>
         </is>
+      </c>
+      <c r="L61" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -3095,10 +3285,13 @@
           <t>University governance, admin, policies, programs, curriculum, Labor and work</t>
         </is>
       </c>
-      <c r="J62" t="inlineStr">
+      <c r="K62" t="inlineStr">
         <is>
           <t>Members of the Barnard contingent faculty union and roughly 20 students demonstrated their discontent with Barnard President Debora Spar on Wednesday night during an event at which she was speaking.&lt;br/&gt;The panel featured Spar, Anna Quindlen, Writer-in-Residence Jennifer Finney Boylan, writer Lizzie Skurnick, and writer and editor Cathi Hanauer, who read selections from the new book "The Bitch is Back." The book-which all of the panelists contributed material to-explores how societal ideas about women, feminism, and aging have changed in the last 10 years.&lt;br/&gt;Although the student demonstrators remained in their seats during other panelists' speeches, they stood in the aisles when Spar took to the podium, silently holding posters with phrases critical of what they saw as Spar's lack of engagement with other pertinent issues, such as the ongoing negotiations with the contingent faculty union, race relations, and fossil fuel divestment, among other issues.&lt;br/&gt;One sign reading "President Spar: For Poor Women Botox Isn't "There For The Picking" responded to an essay published by Spar in The New York Times last Sunday titled "Aging and My Beauty Dilemma," which is included in "The Bitch is Back."&lt;br/&gt;The essay was critiqued by some readers who felt that Spar's emphasis on appearance and cosmetic surgery was problematic, especially given her position at Barnard.&lt;br/&gt;Ella Merrill, BC '18, who was one of the silent demonstrators, said that although the panel was "good for what it was," it was not representative of the views of Barnard's students and community members.&lt;br/&gt;"I think, especially after her [Spar's] New York Times op-ed, a lot of us are frustrated that this is what she is using her position of power to discuss," she said. "Why not talk about the many issues facing the Barnard community at large?"&lt;br/&gt;Shortly before the event, members of the contingent faculty union-which was not involved in the student demonstration-also addressed Spar's essay in leaflets that they distributed outside of the Event Oval, which also called attention to their ongoing contract negotiations.&lt;br/&gt;"Feminist issues Barnard alumnae consider a very high priority: health care and fair pay for women faculty," the flier read. "'Feminist-leaning' issues Barnard alumnae consider very low priority: the 'beauty' dilemmas of the 1%."&lt;br/&gt;English lecturer Sonam Singh, a member of the contingent faculty union's bargaining committee, said that having a presence at the event was a way for the union to try and engage with Spar, who he said has been absent from the negotiating table.&lt;br/&gt;"We've had a hard time getting her attention. While she's certainly directing negotiations on behalf of the college, she's never spoken with us," he said. "As negotiations drag out, we do want to get her attention."&lt;br/&gt;Singh also said that although the union, who recently delivered an alumnae petition in support of the union to Spar's office last Tuesday, would have distributed flyers regardless of whether Spar's essay had been published or not, he found her op-ed to be "frustrating."&lt;br/&gt;"Since you are the president of a very important college, and you have this platform, we would like you to focus on issues that matter in a more significant way," he said.&lt;br/&gt;Ginger Mayo, BC '20, a member of Divest Barnard who demonstrated at the event, said that she found the essay to be "tone-deaf," particularly as it was published the same week as the 20th anniversary of the clerical worker's strike.&lt;br/&gt;"I don't think that the group [of student demonstrators] had a particular issue with the content of the piece, but with the tone and with using this very important platform to talk about something extremely artificial and very inaccessible to most women," she said.&lt;br/&gt;But regardless of Spar's controversial essay, student demonstrators said they believed that Spar's position as the leader and public figurehead of the college meant that she had the responsibility to use her platform to discuss issues facing the larger Barnard community.&lt;br/&gt;"Debora Spar does represent us, and we think her role is important," Merrill said.&lt;br/&gt; | @ACBandrowski</t>
         </is>
+      </c>
+      <c r="L62" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -3143,10 +3336,13 @@
           <t>Immigration (For)</t>
         </is>
       </c>
-      <c r="J63" t="inlineStr">
+      <c r="K63" t="inlineStr">
         <is>
           <t>A week after Donald J. Trump's presidential victory, over 400 students walked out of classes and gathered on Low Steps on Wednesday afternoon to demand that the University provide sanctuary for undocumented immigrants.&lt;br/&gt;They chanted, "Education, not deportation" and "What do we want? Sanctuary campus. When do we want it? Now."&lt;br/&gt;The protest followed a week in which two petitions signed by students, faculty, and alumni were circulated, calling on the University to support undocumented students financially and secure them from deportation. Trump, during the course of his campaign, repeatedly threatened to repeal Deferred Action for Childhood Arrivals, an executive order signed by President Barack Obama, CC '83, that protects young undocumented immigrants from deportation and permits them to work.&lt;br/&gt;The demonstrators urged the University to ban immigration officials from campus, block immigration officials from obtaining student information, and make a public statement asking the government to protect students currently under DACA as well as support a path to permanent resident status for them.&lt;br/&gt;Despite increasing pressure on Columbia to address the uncertain future of these undocumented students, the University has yet to comment on what provisions it will make, if any, though a University spokesperson said that financial aid will not change for undocumented students, regardless of DACA status.&lt;br/&gt;During the demonstration on Wednesday, Cesar Zamudio, CC '20, described his personal experiences as an undocumented immigrant.&lt;br/&gt;"I learned when I was eight years old that I was undocumented when my dad lost his job because he didn't have the right paperwork to work," Zamudio said. "It didn't really affect me that much until I realized I wanted to go somewhere in life, because that's why my parents came here-to give me a better life."&lt;br/&gt;Jessica Bennett, GS '17 and organizer of the rally, said that mobilization of both undocumented migrants and citizens is necessary to effect change.&lt;br/&gt;"Our people are not criminals. The law has criminalized them," Bennett said. "We're calling on our supporters. We're calling on our allies. We're calling on people who, according to the United States, have representation. That means y'all can vote. And look what the fuck that got y'all-a tangerine."&lt;br/&gt;Numerous student groups read their statements of support for the movement, including the South Asian Feminisms Alliance, Party for Socialism and Liberation, Columbia Divest for Climate Justice, International Socialist Organization, Columbia Queer Alliance, and Apartheid Divest. Four New York Police Department officers stood on College Walk during the demonstration.&lt;br/&gt;In addition to leading the demonstration, the student group Undocumented Students Initiative also hosted a panel discussion in partnership with the Office of Multicultural Affairs on Wednesday night. Undocumented students shared their personal stories in hopes that they would help other students understand the struggles that they have faced.&lt;br/&gt;"When you talk about immigrants and immigration, it isn't just numbers. It isn't just laws. It is people," Genesis Garfio, CC '17, said during the discussion. "Because yes, I can give you all the statistics. Yes, I can give you all the facts. But I want you to remember that this is not something that's foreign to Columbia. Your fellow peers are experiencing this."&lt;br/&gt;If DACA were to be repealed, many students would lose the legal protections that they have now.&lt;br/&gt;"For most students who have DACA, they don't have any other pathway to regularize their status, so they don't usually have access to work permits, driver's licenses, even professional licenses," Alyshia Galvez, CC '95, said. Galvez is a CUNY professor who primarily researches Mexican migration in New York City.&lt;br/&gt;Galvez believes that undocumented migrants have much to contribute to society, particularly those protected by DACA.&lt;br/&gt;"When we look at it as a society, these are our children. These are children that were raised in our country, that were shaped by our institutions, that often are bilingual, that are well-versed and very capable navigators of our institutions and our civic life," Galvez said. "And so it's really unfair that, because they don't have a social security number, they're excluded and at risk of deportation."&lt;br/&gt;Aaron Holmes contributed reporting.&lt;br/&gt; | @canwenxu</t>
         </is>
+      </c>
+      <c r="L63" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -3195,10 +3391,13 @@
           <t>Immigration (For), University governance, admin, policies, programs, curriculum, Hate crimes/Anti-minority violence</t>
         </is>
       </c>
-      <c r="J64" t="inlineStr">
+      <c r="K64" t="inlineStr">
         <is>
           <t>Hundreds of Students Stage Walkout to Declare NYU a 'Sanctuary Campus'&lt;br/&gt;Alex Bazeley&lt;br/&gt;Students filled Washington Square Park on Wednesday to show their support for students who may feel vulnerable in the wake of Donald Trump's election as president.&lt;br/&gt;Natasha Roy, Deputy News Editor&lt;br/&gt;November 16, 2016&lt;br/&gt;Students held a school-wide walkout on Wednesday as part of the #SanctuaryCampus movement to protest Donald Trump's election as president and his discriminatory rhetoric. Hundreds of students left their classes at noon and convened in Washington Square Park - later moving to Bobst Library - to stand in solidarity with marginalized and vulnerable groups on campus.&lt;br/&gt;Leaders of the protest explained that they were calling on NYU to be a Sanctuary Campus for students and faculty who feel marginalized or attacked by those who support Trump's rhetoric. The walkout was part of a nationwide movement which saw more than 100 universities asking their schools to provide a safe place for students who feel attacked for their religion, gender, race, legal status or sexual orientation.&lt;br/&gt;Protesters gathered in the fountain to hear speakers tell their stories and lead chants from its center. The protest's organizers asked people who felt most marginalized to stand closer to the center.&lt;br/&gt;CAS junior Mariyamou Drammeh said she hopes NYU will act on students' anger and fear that came about after Trump's election.&lt;br/&gt;"I'm hoping the NYU administration will, first of all, realize that we have a say as a student population," Drammeh said. "Not only that we have a say but that our voices matter and that they will take that into consideration in terms of providing safe spaces for undocumented folks and also other marginalized communities."&lt;br/&gt;Chants included ones like "the people united will never be defeated" and "I believe that we will win."&lt;br/&gt;NYU Student Walk Out in Washington Sq Park: Students announce creation of "NYU Rising" movement @nyunews pic.twitter.com/GxkNllKu4y&lt;br/&gt;- Bobby Wagner (@bwags1121) November 16, 2016&lt;br/&gt;The rally came in response to numerous accounts of violent acts across the nation against minorities. Drammeh said she came to the walkout to help represent the Muslim Students Association. She identified with many of the issues students were speaking out about at the walkout.&lt;br/&gt;"I have a lot of undocumented family and friends," Drammeh said. "I'm Muslim, so a lot of Trump's rhetoric affects me and my family. I'm also African-American, low-income, and so I feel like a lot of Trump's policies and a lot of the things he says all kind of are directed towards people in my community."&lt;br/&gt;While Drammeh's class happened to be released early, meaning she didn't have to miss any class, she said she had planned to walk out of her class and was not worried about the repercussions.&lt;br/&gt;While some professors did not directly encourage the walkout, they said they respected whatever decision their students chose to make in light of the protest. CAS freshman Anna Sang left her Writing the Essay class and said that her professor, Jen Hyde, had emailed the class the day before outlining what students who were protesting would miss.&lt;br/&gt;"She made it okay, and she's always made it okay for us to express our opinions," Sang said. "I think that's why she's letting us walk out. She wants to make it a good space for us to express our opinions."&lt;br/&gt;Students leave the park to head into Bobst. NYPD is standing by. pic.twitter.com/6Hn5OKr8Oy&lt;br/&gt;- Washington Sq. News (@nyunews) November 16, 2016&lt;br/&gt;Following the hour-long rally in the park, students headed to Bobst to stand for a 10 minute moment of silence, with students overflowing onto the street.&lt;br/&gt;CAS freshman Wenqi Qiu also walked out of Hyde's Writing the Essay class and said he hopes this more formally organized movement is more effective in creating change.&lt;br/&gt;"This is, I think, one of the first more officially organized rallies," Qiu said. "I feel like this will be less incendiary speech, like 'fuck Donald Trump,' and be more about acceptance and love."&lt;br/&gt;The rally also saw a few scattered Trump supporters clad in the signature red "Make America Great Again" hat, but confrontations were largely civilized, with a few rally attendees simply demanding that they leave the safe space that was being nurtured.&lt;br/&gt;Protesters said a main goal of the rally was to provide solidarity and a sense of community for all fearful students after the election.&lt;br/&gt;"I'm here to support all students, all speakers and show that I'm here in solidarity with all the communities because we're only going to persevere if we come together as one," Drammeh said.&lt;br/&gt;Email Natasha Roy at [email protected]&lt;br/&gt;Related Stories&lt;br/&gt;Fight Against Islamophobia Continues at Tandon Rally Comic Films Sacrifice Story for the Big Screen Divest Rallies With National Standing Rock Movement</t>
         </is>
+      </c>
+      <c r="L64" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -3238,10 +3437,13 @@
           <t>Social services and welfare, Public funding for higher education, _Other Issue</t>
         </is>
       </c>
-      <c r="J65" t="inlineStr">
+      <c r="K65" t="inlineStr">
         <is>
           <t>Students, Teachers Gather Outside Senator Schumer's Office to Protest Education Rights&lt;br/&gt;Miranda Levingston, Deputy News Editor&lt;br/&gt;January 31, 2017&lt;br/&gt;Elementary school children waved signs proclaiming "Public School Students Are Watching" and "Reject DeVos, Reject Hate" from the windows of Senator Chuck Schumer's (D-NY) office.&lt;br/&gt;A diverse group of approximately 300 parents, elementary-aged students, teachers and other concerned bystanders attended the event organized by Public School Watchdogs - a parent education organization based in New York. The event was launched on Facebook five days ago, with over 700 people showing interest in attending.&lt;br/&gt;The event was organized in response to Schumer's recent statements opposing Betsy DeVos' possible appointment as secretary of education. Schumer disagrees with DeVos's plans to privatize education, enforce daily prayer in school and her refusal to divest from her companies. Schumer has also voiced his concerns on his Twitter account.&lt;br/&gt;Betsy DeVos would single-handedly decimate our public education system if she were confirmed. I will vote "No" &amp; I will do it proudly.&lt;br/&gt;- Chuck Schumer (@SenSchumer) January 26, 2017&lt;br/&gt;Protesters called for Schumer to act on his previous intentions to block DeVos's appointment. Chants of "Teachers; not billionaires," "Betsy DeVos is not the boss" and "Withhold consent - 100%" echoed around the midtown block. The event's organizers also asked protesters to thank Senators Gillibrand and Schumer for their promised votes against DeVos.&lt;br/&gt;Tisch freshman Meagen Tajalle said that she was particularly alarmed by DeVos's plan to privatize education, because she personally benefits from federal financial aid, federal grants and federal work-study. She said that DeVos's policies could financially limit college students' opportunities.&lt;br/&gt;"I'm worried by the thought of someone like DeVos to be confirmed, because of the way that I benefit from federal funding and higher education," said Tajalle. "I hope someone more qualified for the department is confirmed - someone who doesn't have ulterior motives like she does, as a millionaire."&lt;br/&gt;Annie Lederman, a comedian on "Chelsea Lately" and on MTV's "Girl Code," said that at the moment, DeVos's policies primarily affect children in grades K-12, but because today's children will become tomorrow's leaders, these policies will eventually affect everyone.&lt;br/&gt;"This affects our children; this is the future of this country, and there's nothing more to it than that," Lederman said. "This is not what Schumer says he stands for, and so it's time to spine up.  I hope that Schumer votes 'No."&lt;br/&gt;Public school teacher Emily Gadd said that teachers need to keep their eyes on elected officials and advocate for their students.&lt;br/&gt;"As teachers, we know more than most about public education," Gadd said. "We have politicians, like DeVos, who are trying to make decisions based on profit and not on what's best for student learning."&lt;br/&gt;Email Miranda Levingston at [email protected]&lt;br/&gt;Related Stories&lt;br/&gt;Protestors in Battery Park Respond to JFK Detainees NYU Student Organizes Love Rally in the Park Protesters Flood the Streets, Head to Trump Tower</t>
         </is>
+      </c>
+      <c r="L65" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -3281,10 +3483,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J66" t="inlineStr">
+      <c r="K66" t="inlineStr">
         <is>
           <t>Members of a student organization called Reinvest IU and others armed with protest signs advocated against fossil fuels Monday as they paraded to IU President Michael McRobbie's office.&lt;br/&gt;Protesters staged a walkout and a march from Showalter Fountain to McRobbie's office as part of a national movement to end the use of fossil fuels. The group included 14 members.&lt;br/&gt;"IU is representative of the student population," junior Kara Duval-Fowler said. "We should have a say. This is a matter of survival."&lt;br/&gt;Reinvest IU is an organization dedicated to ensuring IU divests from fossil fuels and reinvests in cleaner resources. It works closely with organizations such as 350.org, IU Student Sustainability Council, and other Bloomington and University groups.&lt;br/&gt;Duval-Fowler and second-year graduate student Linus Platzer both said Reinvest IU has been in close contact with the IU Foundation in one-on-one meetings, but the meetings have never led to action.&lt;br/&gt;On Monday students were unable to speak directly with McRobbie. Participants Wes Cammenga, Platzer and Duval-Fowler gave short speeches to McRobbie's two receptionists.&lt;br/&gt;"Given currently existing political and scientific realities, it is pretty clear to us that this is not just something McRobbie might want to do, it's what he should do," Cammenga said.&lt;br/&gt;The letter asks McRobbie to make a public statement urging the IU Foundation to refrain from the use of fossil fuels.&lt;br/&gt;IU has a history of resisting the pressure to become more environmentally friendly despite the ?example of many Indiana schools, Platzer said.&lt;br/&gt;He said the University's refusal to sign the American College and University Presidents' Climate Commitment is one example of its refusal to think carefully about the ?environment.&lt;br/&gt;He also said it's difficult to find an explanation online behind IU's choice to neglect environmental issues. He said he believes there can be only two explanations: The information is so bad the University can't disclose it or IU decision makers don't want to talk.&lt;br/&gt;He said he wanted to know why.&lt;br/&gt;"Students feel IU is not fulfilling the promise," Platzer said. "Climate change happens."&lt;br/&gt;Duval-Fowler said climate change is not just a matter to be conscious of, but, instead, is an issue of life or death everyone should acknowledge.&lt;br/&gt;"There is not a future where we do not divest from fossil fuels, where we don't shift to renewable energy," Duval-Fowler said. "There simply is no future, and we ask that President McRobbie considers what he is leaving the rest of us."&lt;br/&gt;Cammenga discussed the moral obligation to face climate change in his speech.&lt;br/&gt;He said he didn't want McRobbie to support the letter only because Reinvest IU encouraged him to but because it was in the best interest of everyone for him to do so.&lt;br/&gt;"What we are asking him to doing do, though, is to read this letter we have here very carefully and to think very carefully about whether what we are saying in this letter is correct," Cammenga said.&lt;br/&gt;Rebecca Mahan, an IU alumna and retired IU professor who taught for 27 years, was in attendance, even though she was surrounded by students younger than 25.&lt;br/&gt;She was sent an email about Student Divestment Network's national Day of Action, and she said she wants to work alongside Reinvest IU.&lt;br/&gt;Mahan, who taught English to international students, said the parade and letter-delivering was exciting to her because marches occurred daily when she was in college, in stark contrast to now.&lt;br/&gt;She said it was refreshing to see a group of students raising awareness to their peers, especially on a topic she valued.&lt;br/&gt;"I had thousands of students from over 50 countries, and, although they disagreed on other issues, they all agreed on the importance of climate change," Mahan said.</t>
         </is>
+      </c>
+      <c r="L66" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -3324,10 +3529,13 @@
           <t>Sexual assault/violence, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J67" t="inlineStr">
+      <c r="K67" t="inlineStr">
         <is>
           <t>Rachael Folland on December 5, 2016 at 5:00 pm&lt;br/&gt;The Dalai Lama Visits the U&lt;br/&gt;In June the Dalai Lama made a long-awaited appearance at the U. Thousands of people filed into the Huntsman Center to hear the&lt;br/&gt;Buddhist leader deliver his speech. He spoke of compassion, peace and universal responsibility. The event caused political controversy, as some Utah lawmakers were concerned that meeting with the Dalai Lama would damage relations between the state and China. Nonetheless, Governor Gary Herbert and Salt Lake City Mayor Jackie Biskupski met with the 14th Dalai Lama, Tenzin Gyatso, during his visit to Utah.&lt;br/&gt;ASUU Elections&lt;br/&gt;Students Leading Change won this year's ASUU election by 500 votes. Jack Bender is the president elect, and he, along with the rest of SLC, have major plans for ASUU. Their platform includes reducing student fees, increasing involvement and creating a new face for ASUU.&lt;br/&gt;Halloween Sexual Assault on Campus&lt;br/&gt;On Halloween, a female student was held at gunpoint in the back seat of her car and sexually assaulted by a masked man. The assault happened in broad daylight. Throughout 2016, light has been shed on incidents of sexual assault that have plagued students at the U. The Salt Lake Tribune hosted a discussion about rape culture at the U later that week. Students reacted to the assault by protesting administration's response to sexual violence on campus.&lt;br/&gt;U Opts Not to Divest From Fossil Fuels&lt;br/&gt;In May the Academic Senate voted on whether or not to divest from fossil fuels. For several years the U has invested in resources to reduce its carbon print on the environment. The vote would make a political statement, as U receives a lot of funding from its investments in fossil fuels. The senate voted to divest, but according to the Salt Lake Tribune, the board of trustees rejected the decision and the U will continue to invest in fossil fuels.&lt;br/&gt;Mitt Romney Denounces Trump in Speech at the U&lt;br/&gt;During the presidential primary elections, Mitt Romney took to the podium at Libby Gardner Hall to denounce Donald Trump as the Republican presidential nominee. Romney reaffirmed that he would not be running in the 2016 election and did not endorse any candidates at the event. In his speech, Romney attacked Trump's moral character and foreign and economic policies. He argued that Trump's nomination would result in a Clinton presidency. Trump responded in a speech later that day, calling Romney a "failed candidate."&lt;br/&gt;Jeremih Brings Females on Stage During Redfest&lt;br/&gt;Jeremih performing at the University of Utah 2016 Redfest at the Student Union building plaza on Friday, September 16, 2016&lt;br/&gt;At this year's Redfest, headliner Jeremih brought two female students onto the stage and attempted to kiss them, while another woman got on stage and flashed the audience. Jeremih is known for bringing girls onto stages at his concerts, but ASUU stated they had no knowledge of his intentions. Both of the women brought on stage said they were not traumatized by what took place.&lt;br/&gt;Student Protest at Commencement&lt;br/&gt;Students and community members gathered at this year's commencement to protest and honorary degree given to Lynette Nielsen Gay. Many people were upset about the degree because of her involvement with two hate groups that target the LGBT community. Protesters believed that this decision could lead to further mistreatment of the LGBT community. Gay later resigned from one of the organizations she was associated with.&lt;br/&gt;Jimmy Fallon and the U Hat&lt;br/&gt;Jimmy Fallon wore a U hat after being challenged by Jan Krystkowiak, wife of Utes basketball coach Larry Krystkowiak, to wear the hat if the Utes beat the Duke Blue Devils. Fallon wore the hat during an interview with KSL sports-anchor and BYU fan Mike Headrick. An image of Fallon in the hat posted on the U's Facebook page garnered more than 4,000 "likes."&lt;br/&gt;Posters Vandalized with Anti-Islam Messages&lt;br/&gt;In the heat of the presidential primaries, posters in the OSH building advertising an event about Islamophobia and&lt;br/&gt;bigotry fueled by the race were defaced with Islamophobic language. Among the phrases was "F- Islam" written in black marker. U police investigated the incident as a hate crime.&lt;br/&gt;Share This:</t>
         </is>
+      </c>
+      <c r="L67" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -3367,10 +3575,13 @@
           <t>Trump and/or his administration (Against)</t>
         </is>
       </c>
-      <c r="J68" t="inlineStr">
+      <c r="K68" t="inlineStr">
         <is>
           <t>This semester has been unlike any other for most universities. The 2016 presidential election season is finally coming to a close, and just as the country will soon move past these presidential races, students will, too.&lt;br/&gt;Every student body demonstrates activism in its own way. The editorial boards from GW's The Hatchet, NYU's Washington Square News and Penn State's The Daily Collegian considered student activism in higher education on their individual campuses and collectively throughout this election season.&lt;br/&gt;Our universities are clearly different, but this semester has been equally political on each of our campuses. Before we all headed back to school this fall, we expected the political activity on our campuses to be high - after all, this is the only presidential election most of us will be in college for. But we didn't know just how divisive the election would be.&lt;br/&gt;Regardless of where we go to school, we believe in the political activity throughout the campaigns, and we believe it's important that students at any university stay politically aware long after Election Day.&lt;br/&gt;Student organizations have gotten into the election spirit on all three of our campuses - we've all had debate watch parties, NYU and Penn State have hosted mass rallies for candidates on their respective campuses and membership in GW's political student organizations is at an all-time high.&lt;br/&gt;While it's great to watch university Democrats and university Republicans around the country debate about the candidates, hopefully we'll see these groups come together on Wednesday, Nov. 9. But of course, not all discourse is civil. At NYU, the presidential election has been a source of some anxiety. Students have clashed in the past, when some Trump-supporting students felt intimidated by NYU's liberal atmosphere. NYU, academically and socially, tends to skew towards the left of the political spectrum.&lt;br/&gt;Conservatives at NYU may sometimes feel marginalized, but that does not mean they do not have a voice on campus. College Republicans, for example, are an active participant in campus debates and represent a broad cross section of conservative viewpoints.&lt;br/&gt;And just last week, members of the Penn State Bull-Moose Party erected a "wall" around the American flag pole on the Old Main lawn, and soon enough, Students for Hillary arrived in response. There wasn't a violent clash between the two groups, but it was symbolic of a larger issue in the divisiveness of this campaign.&lt;br/&gt;At a scheduled debate between the Bull-Moose Party and Students for Hillary, tensions rose before the debate even began, with the Bull-Moose representative claiming that Students for Hillary pulled out of the debate. While the debate still took place, the two debating representatives traded blows all night.&lt;br/&gt;Similarly, GW's College Republicans and College Democrats were set to debate Nov. 1, but just two days before the event, the College Republicans withdrew from the debate. After a confusing night of Facebook statuses from both student groups, College Democrats implored any Republican at GW to debate them. Eventually, the College Republicans issued an apology, writing on Facebook that misinformation provoked them to pull out of the debate and retract their statement.&lt;br/&gt;or tags on article template page. The placement should appear just "below-the-fold", meaning that a user needs to scroll down slightly to see the video. Be sure that if you article page also has an "inline" ad unit that plays within the text that the two ad units do not overlap. */ --&gt;&lt;br/&gt;While this election cycle has been divisive on all of our campuses, we have good reason to hope and expect that our student bodies will come together Wednesday and focus their political energy on campus issues.&lt;br/&gt;Student activism is a trademark of college life on all three of our campuses. At NYU, students have identified and protested several causes that affect their life on campus. One of the most well-documented demonstrations was a sit-in staged by NYU's Incarceration to Education Coalition - a group that advocates against penalizing prospective students with criminal records. NYU Divest, which aims to pressure the Board of Trustees to divest from fossil fuels, organized a protest in the library. And recently after student protest, the university committed to providing free menstrual health products.&lt;br/&gt;GW students have found similar success in protesting University policies. In 2015, GW's Students Against Sexual Assault marched to officials' offices to demand mandatory sexual assault and prevention training for students. They succeeded: Freshmen are now mandated to complete trainings during orientation. And after years of protest coupled with effective Student Association leadership in 2014, the University's student health center was moved to campus.&lt;br/&gt;And at Penn State, the relative isolation of Happy Valley creates the perfect environment for political and social activism, as it breeds a range of opinions. Penn State welcomed its largest freshman class in recent years and has consistently seen a varying population of international students, so together this draws the student body toward different types of issues. Civil issues of race and gender equality have resulted in protests and awareness campaigns on campus. Raising awareness of sexual assault and bystander intervention have created leadership roundtables, inspired HUB - Penn State's main student center - takeovers, marches and increased the overall visibility of it on campus.&lt;br/&gt;It makes sense that college students have made this semester into a political marathon. But just like any fad, the interest in this presidential election will fade. Students should remember the causes they fought for this semester and continue advocating after Election Day.&lt;br/&gt;And hopefully, students can apply their excitement about national political activity to their own campuses to make tangible changes.&lt;br/&gt;This staff editorial was written by The Hatchet's opinions editor Melissa Holzberg, Washington Square News' opinions editor Emily Fong and The Daily Collegian's opinions editor Lauren Davis. The opinions expressed are based on conversations with the editorial boards of The Hatchet, Washington Square News and The Daily Collegian.</t>
         </is>
+      </c>
+      <c r="L68" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -3410,10 +3621,13 @@
           <t>Trump and/or his administration (For)</t>
         </is>
       </c>
-      <c r="J69" t="inlineStr">
+      <c r="K69" t="inlineStr">
         <is>
           <t>This semester has been unlike any other for most universities. The 2016 presidential election season is finally coming to a close, and just as the country will soon move past these presidential races, students will, too.&lt;br/&gt;Every student body demonstrates activism in its own way. The editorial boards from GW's The Hatchet, NYU's Washington Square News and Penn State's The Daily Collegian considered student activism in higher education on their individual campuses and collectively throughout this election season.&lt;br/&gt;Our universities are clearly different, but this semester has been equally political on each of our campuses. Before we all headed back to school this fall, we expected the political activity on our campuses to be high - after all, this is the only presidential election most of us will be in college for. But we didn't know just how divisive the election would be.&lt;br/&gt;Regardless of where we go to school, we believe in the political activity throughout the campaigns, and we believe it's important that students at any university stay politically aware long after Election Day.&lt;br/&gt;Student organizations have gotten into the election spirit on all three of our campuses - we've all had debate watch parties, NYU and Penn State have hosted mass rallies for candidates on their respective campuses and membership in GW's political student organizations is at an all-time high.&lt;br/&gt;While it's great to watch university Democrats and university Republicans around the country debate about the candidates, hopefully we'll see these groups come together on Wednesday, Nov. 9. But of course, not all discourse is civil. At NYU, the presidential election has been a source of some anxiety. Students have clashed in the past, when some Trump-supporting students felt intimidated by NYU's liberal atmosphere. NYU, academically and socially, tends to skew towards the left of the political spectrum.&lt;br/&gt;Conservatives at NYU may sometimes feel marginalized, but that does not mean they do not have a voice on campus. College Republicans, for example, are an active participant in campus debates and represent a broad cross section of conservative viewpoints.&lt;br/&gt;And just last week, members of the Penn State Bull-Moose Party erected a "wall" around the American flag pole on the Old Main lawn, and soon enough, Students for Hillary arrived in response. There wasn't a violent clash between the two groups, but it was symbolic of a larger issue in the divisiveness of this campaign.&lt;br/&gt;At a scheduled debate between the Bull-Moose Party and Students for Hillary, tensions rose before the debate even began, with the Bull-Moose representative claiming that Students for Hillary pulled out of the debate. While the debate still took place, the two debating representatives traded blows all night.&lt;br/&gt;Similarly, GW's College Republicans and College Democrats were set to debate Nov. 1, but just two days before the event, the College Republicans withdrew from the debate. After a confusing night of Facebook statuses from both student groups, College Democrats implored any Republican at GW to debate them. Eventually, the College Republicans issued an apology, writing on Facebook that misinformation provoked them to pull out of the debate and retract their statement.&lt;br/&gt;or tags on article template page. The placement should appear just "below-the-fold", meaning that a user needs to scroll down slightly to see the video. Be sure that if you article page also has an "inline" ad unit that plays within the text that the two ad units do not overlap. */ --&gt;&lt;br/&gt;While this election cycle has been divisive on all of our campuses, we have good reason to hope and expect that our student bodies will come together Wednesday and focus their political energy on campus issues.&lt;br/&gt;Student activism is a trademark of college life on all three of our campuses. At NYU, students have identified and protested several causes that affect their life on campus. One of the most well-documented demonstrations was a sit-in staged by NYU's Incarceration to Education Coalition - a group that advocates against penalizing prospective students with criminal records. NYU Divest, which aims to pressure the Board of Trustees to divest from fossil fuels, organized a protest in the library. And recently after student protest, the university committed to providing free menstrual health products.&lt;br/&gt;GW students have found similar success in protesting University policies. In 2015, GW's Students Against Sexual Assault marched to officials' offices to demand mandatory sexual assault and prevention training for students. They succeeded: Freshmen are now mandated to complete trainings during orientation. And after years of protest coupled with effective Student Association leadership in 2014, the University's student health center was moved to campus.&lt;br/&gt;And at Penn State, the relative isolation of Happy Valley creates the perfect environment for political and social activism, as it breeds a range of opinions. Penn State welcomed its largest freshman class in recent years and has consistently seen a varying population of international students, so together this draws the student body toward different types of issues. Civil issues of race and gender equality have resulted in protests and awareness campaigns on campus. Raising awareness of sexual assault and bystander intervention have created leadership roundtables, inspired HUB - Penn State's main student center - takeovers, marches and increased the overall visibility of it on campus.&lt;br/&gt;It makes sense that college students have made this semester into a political marathon. But just like any fad, the interest in this presidential election will fade. Students should remember the causes they fought for this semester and continue advocating after Election Day.&lt;br/&gt;And hopefully, students can apply their excitement about national political activity to their own campuses to make tangible changes.&lt;br/&gt;This staff editorial was written by The Hatchet's opinions editor Melissa Holzberg, Washington Square News' opinions editor Emily Fong and The Daily Collegian's opinions editor Lauren Davis. The opinions expressed are based on conversations with the editorial boards of The Hatchet, Washington Square News and The Daily Collegian.</t>
         </is>
+      </c>
+      <c r="L69" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -3453,10 +3667,13 @@
           <t>Pro-Israel/Zionism</t>
         </is>
       </c>
-      <c r="J70" t="inlineStr">
+      <c r="K70" t="inlineStr">
         <is>
           <t>The David Horowitz Freedom Center a conservative activist group, took responsibility Friday for posting fliers around the SF State campus that depicted a professor as a terrorist sympathizer, according to a press release issued by the center.  &lt;br/&gt;"Our goal in placing these posters on prominent campuses across America is to expose the true motivations and allegiances of these groups who have chosen to join forces with terrorists, to challenge their lies and to expose the financial and organizational supports which allow them to pursue their genocidal agenda," David Horowitz said in a press release.&lt;br/&gt;In a statement released today, SF State President Les Wong condemned the actions of those responsible for the posters, saying that "a line has been crossed."&lt;br/&gt;SF State has been the latest school in a group of California universities that has been targeted in the "Stop the Jew Hatred on Campus" poster campaign.  Other universities that were targeted were UC Berkeley, UCLA, San Diego State and UC Irvine.  &lt;br/&gt;One of the posters depicts an illustration of Rabab Ibrahim Abdulhadi, an associate professor in the ethnic studies program, with the statement next to it, "a leader of the Hamas BDS campaign; collaborator with terrorists; San Francisco State professor." BDS stands for the Boycott, Divestment and Sanctions movement, which calls for an international effort to put economic pressure on Israel for its treatments of Palestinians.   &lt;br/&gt;"Flyers were posted by an outside extremist group in numerous locations, singling out one of our faculty members, our students and vandalizing our campus,"  Wong said.  "We know that this group is not affiliated with San Francisco State University."&lt;br/&gt;Wong goes on to say that even though "we disagree on many issues, we must defend each other from personalized attacks that serve no purpose but to incite fear and promote division."&lt;br/&gt;In an article released by frontpagemag.com -- a website operated by the David Horowitz Freedom Center --  stated that "SF State has repeatedly enabled the most extreme actions of its General Union of Palestinian Students ." The article goes into describing recent SF State events involving GUPS, such as an April protest of the Jerusalem Mayor Nir Barkat, which led the University to implement a five-step protocol, after heavy scrutiny according to an article released by the Golden Gate Xpress.  &lt;br/&gt;SF State has been at the center of ongoing controversy involving Jewish and Palestinian relations, when a petition went out in September questioning the University's partnership with An-Najah National University.&lt;br/&gt;"Let me be clear, this is not an issue of free speech; this is bullying behavior that is unacceptable and will not be tolerated on our campus,"  Wong said.  &lt;br/&gt;Share this:&lt;br/&gt;EmailFacebookTwitterGoogleMoreRedditTumblrPinterestLinkedIn Tags:SF StateSFSU</t>
         </is>
+      </c>
+      <c r="L70" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -3496,10 +3713,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J71" t="inlineStr">
+      <c r="K71" t="inlineStr">
         <is>
           <t xml:space="preserve">ROBERT DURRELL / UC DAVIS FILE PHOTO&lt;br/&gt;UC Regents members review possible tuition increase, sexual harassment&lt;br/&gt;On Nov. 16 and 17, UC Regents met at the San Francisco Mission Bay Conference Center to discuss pressing issues with regard to faculty, students and staff.&lt;br/&gt;On Nov. 16, UC Santa Cruz and UC Berkeley students from Fossil Free UC, a UC systemwide, student-led organization, asked the regents to divest from fossil fuels. Students from UC Berkeley presented a letter to the board of regents which was signed by more than 650 faculty members from across the UC system, urging members to take action against the use of fossil fuels like other universities have.&lt;br/&gt;"By choosing not to lead with us, Regent Sherman, you are spreading a diseased lie about the impact of the oil industry, on the climate and on people," said Sam Weinstein, a UC Santa Cruz student. "This issue is not going away, and we are not going away."&lt;br/&gt;Students stated this topic was especially relevant in light of Donald Trump winning the presidential election, as he has denied climate change and global warming and also appointed a climate change skeptic to direct the Environmental Protection Agency.&lt;br/&gt;Jasmine Marshall Armstrong, a doctoral candidate at UC Merced, also addressed the presidential election and the impact it had on students the night Donald Trump was won the presidency.&lt;br/&gt;Armstrong stated that many members of the UC system, especially LGBT+ students, students of color and undocumented students are fearful of hate crimes and deliberate violence. Armstrong herself received a death threat from a white nationalist due to her support of minority groups.&lt;br/&gt;"We all need to feel safe, valued and protected," Armstrong said. "I ask you to live up to our motto of 'let there be light.' Let California be the light in this moment of darkness."&lt;br/&gt;The UC Board of Regents also addressed and approved a policy change requiring board members to comply with ethical conduct and sexual harassment policy in private as well as public life. This policy change comes after controversial issues pertaining to sexual harassment, including an incident in which Regent Norman Pattiz asked a female colleague if he could touch her breasts during the public airing of a recording, as well as an incident in which Pattiz was accused of saying to a female "If I wasn't married I'd be chasing you down the hallway."&lt;br/&gt;The new policy will require regents to complete sexual harassment prevention training.&lt;br/&gt;Pattiz, who sits on the Governance and Compensation Committee and was present at the meeting, said he had already begun the mandated sexual harassment training.&lt;br/&gt;The board voted on reducing the number of standing committees from 10 to six and will also allow committee meetings to be held concurrently. Committee chair Regent Russell Gould stated these changes would allow each committee to be more engaged and effective during meetings.&lt;br/&gt;The six renamed and standing committees are Academic and Student Affairs, Compliance and Audit, Finance and Capital Strategies, Governance and Compensation, Health Services and Public Engagement and Development.&lt;br/&gt;The regents also discussed potential tuition increases.&lt;br/&gt;UC chief financial officer Nathan Brostrom pointed out the existing gap between the $7 billion received from UC tuition and state funding and the $30 billion operational budget. Brostrom proposed an increase in tuition of about $300. He addressed the system's preliminary 2017 to 2018 budget, which included growth of undergraduate and graduate student enrollment, resulting in mandatory cost increases.&lt;br/&gt;"There was discussion of potential tuition increases, but we don't know at this point in time," said Regent Hadi Makarechian.&lt;br/&gt;Makarechian presented a report by the Finance and Capital Strategies Committee explaining that further consideration of tuition hikes would occur in January.&lt;br/&gt;The regents approved a three year financial sustainability plan, which includes cost-saving alternative revenues.&lt;br/&gt;This discussion lead to protests on the second day of meetings, where more than 50 students protested tuition hikes outside the conference center, marching around the driveway and insisting that the regents not only freeze tuition but also to roll back existing fees.&lt;br/&gt;Students moved into the meeting room and spoke over regents numerous times in the ensuing discussion. Vice Chair Bonnie Reiss gave several warnings, threatening police intervention if there were continued disruptions. Students entered at 10:30 a.m., and left the meeting room and continued to protest outside by 1 p.m.&lt;br/&gt;The meeting adjourned around 3 p.m. on Nov. 17.&lt;br/&gt;Written by: Demi Caceres  - </t>
         </is>
+      </c>
+      <c r="L71" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -3539,10 +3759,13 @@
           <t>Tuition, fees, financial aid, University governance, admin, policies, programs, curriculum, Economy/inequality</t>
         </is>
       </c>
-      <c r="J72" t="inlineStr">
+      <c r="K72" t="inlineStr">
         <is>
           <t xml:space="preserve">ROBERT DURRELL / UC DAVIS FILE PHOTO&lt;br/&gt;UC Regents members review possible tuition increase, sexual harassment&lt;br/&gt;On Nov. 16 and 17, UC Regents met at the San Francisco Mission Bay Conference Center to discuss pressing issues with regard to faculty, students and staff.&lt;br/&gt;On Nov. 16, UC Santa Cruz and UC Berkeley students from Fossil Free UC, a UC systemwide, student-led organization, asked the regents to divest from fossil fuels. Students from UC Berkeley presented a letter to the board of regents which was signed by more than 650 faculty members from across the UC system, urging members to take action against the use of fossil fuels like other universities have.&lt;br/&gt;"By choosing not to lead with us, Regent Sherman, you are spreading a diseased lie about the impact of the oil industry, on the climate and on people," said Sam Weinstein, a UC Santa Cruz student. "This issue is not going away, and we are not going away."&lt;br/&gt;Students stated this topic was especially relevant in light of Donald Trump winning the presidential election, as he has denied climate change and global warming and also appointed a climate change skeptic to direct the Environmental Protection Agency.&lt;br/&gt;Jasmine Marshall Armstrong, a doctoral candidate at UC Merced, also addressed the presidential election and the impact it had on students the night Donald Trump was won the presidency.&lt;br/&gt;Armstrong stated that many members of the UC system, especially LGBT+ students, students of color and undocumented students are fearful of hate crimes and deliberate violence. Armstrong herself received a death threat from a white nationalist due to her support of minority groups.&lt;br/&gt;"We all need to feel safe, valued and protected," Armstrong said. "I ask you to live up to our motto of 'let there be light.' Let California be the light in this moment of darkness."&lt;br/&gt;The UC Board of Regents also addressed and approved a policy change requiring board members to comply with ethical conduct and sexual harassment policy in private as well as public life. This policy change comes after controversial issues pertaining to sexual harassment, including an incident in which Regent Norman Pattiz asked a female colleague if he could touch her breasts during the public airing of a recording, as well as an incident in which Pattiz was accused of saying to a female "If I wasn't married I'd be chasing you down the hallway."&lt;br/&gt;The new policy will require regents to complete sexual harassment prevention training.&lt;br/&gt;Pattiz, who sits on the Governance and Compensation Committee and was present at the meeting, said he had already begun the mandated sexual harassment training.&lt;br/&gt;The board voted on reducing the number of standing committees from 10 to six and will also allow committee meetings to be held concurrently. Committee chair Regent Russell Gould stated these changes would allow each committee to be more engaged and effective during meetings.&lt;br/&gt;The six renamed and standing committees are Academic and Student Affairs, Compliance and Audit, Finance and Capital Strategies, Governance and Compensation, Health Services and Public Engagement and Development.&lt;br/&gt;The regents also discussed potential tuition increases.&lt;br/&gt;UC chief financial officer Nathan Brostrom pointed out the existing gap between the $7 billion received from UC tuition and state funding and the $30 billion operational budget. Brostrom proposed an increase in tuition of about $300. He addressed the system's preliminary 2017 to 2018 budget, which included growth of undergraduate and graduate student enrollment, resulting in mandatory cost increases.&lt;br/&gt;"There was discussion of potential tuition increases, but we don't know at this point in time," said Regent Hadi Makarechian.&lt;br/&gt;Makarechian presented a report by the Finance and Capital Strategies Committee explaining that further consideration of tuition hikes would occur in January.&lt;br/&gt;The regents approved a three year financial sustainability plan, which includes cost-saving alternative revenues.&lt;br/&gt;This discussion lead to protests on the second day of meetings, where more than 50 students protested tuition hikes outside the conference center, marching around the driveway and insisting that the regents not only freeze tuition but also to roll back existing fees.&lt;br/&gt;Students moved into the meeting room and spoke over regents numerous times in the ensuing discussion. Vice Chair Bonnie Reiss gave several warnings, threatening police intervention if there were continued disruptions. Students entered at 10:30 a.m., and left the meeting room and continued to protest outside by 1 p.m.&lt;br/&gt;The meeting adjourned around 3 p.m. on Nov. 17.&lt;br/&gt;Written by: Demi Caceres  - </t>
         </is>
+      </c>
+      <c r="L72" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -3582,10 +3805,13 @@
           <t>Labor and work, University governance, admin, policies, programs, curriculum, Economy/inequality</t>
         </is>
       </c>
-      <c r="J73" t="inlineStr">
+      <c r="K73" t="inlineStr">
         <is>
           <t>The UC Board of Regents convened Wednesday at UCSF Mission Bay for the first time this year, marking the first regents meeting held during President Donald Trump's presidency.&lt;br/&gt;Items discussed included the new position of a systemwide Title IX coordinator, the expansion of AB 540 nonresident tuition exemption, the protection of Deferred Action for Childhood Arrivals, or DACA, students and UC sustainable practices.&lt;br/&gt;Prior to the meeting, an open session was held for public comment at 9 a.m. Though the public comment period was allotted 20 minutes, it did not conclude until 9:50 a.m. Among the various speakers was a stronghold of members from Teamsters Local 2010, the union representing 14,000 UC employees. The Teamsters' last speaker, Secretary-Treasurer Jason Rabinowitz, urged the regents to grant UC workers contracts. According to Rabinowitz, 70 percent of university workers suffer from food insecurity.&lt;br/&gt;"What do we want - contracts! When do we want - now! If we don't get it, shut it down!" Teamsters chanted, as regents chair Monica Lozano attempted to end the public comment session. Police stationed themselves between the Teamsters and the regents, and the protesters began to exit the room, chanting, "No contracts! No peace!"&lt;br/&gt;On Jan. 12, Kathleen Salvaty, former UCLA Title IX coordinator, was appointed to a systemwide version of the position, reporting directly to UC President Janet Napolitano.&lt;br/&gt;"(The position is meant) to ensure policies on sexual violence, sexual assault and sexual harassment are implemented effectively and consistently, and all members of our UC community feel safe and respected," Napolitano said in her opening remarks. "It's all about a climate of respect. With progress also comes opportunities - everyday, at every campus."&lt;br/&gt;The Academic and Student Affairs Committee heard an update from the working group on undocumented members of the UC community that was established in November, the day after the presidential election. The work group's first action was taken Nov. 30 when the university issued its Statement of Principles in Support of Undocumented Members of the UC Community.&lt;br/&gt;UC Office of the President Deputy General Counsel Julia Friedlander spoke at the meeting on behalf of the working group. According to Friedlander, the work group's four basic principles are that students will be admitted to the university based solely on merit, UCPD will work only to maintain student safety, the university will protect student privacy and UC medical centers will treat any patient regardless of documentation.&lt;br/&gt;"When the university receives requests for records that implicate the privacy rights of individuals, the Office of General Counsel will work closely with our clients to protect the privacy of community members, as we are required to do - unless there is a countervailing law that requires us to make disclosures," Friedlander said.&lt;br/&gt;The future of undocumented UC students was also addressed by Lozano during her opening remarks.&lt;br/&gt;"DACA students' ... actions have been entirely consistent with the university's core values," Lozano said.&lt;br/&gt;Lozano added that the university will protect and support undocumented DACA students who may feel threatened with deportation.&lt;br/&gt;"(Trump) has certain views on immigration, DACA. We are going to be opposite of him on many issues," said regent George Kieffer.&lt;br/&gt;Five UC Berkeley students attended Wednesday's meeting to discuss the university's investment in fossil fuel industries and the UC Retirement Plan, which holds bonds in two companies building on the Dakota Access Pipeline, with UC Chief Investment Officer Jagdeep Singh Bachher.&lt;br/&gt;The students questioned why the UC system has not completely divested from fossil fuels, while other similarly sized research universities, such as the University of Massachusetts and the University of Oregon, have done so.&lt;br/&gt;"While the political climate has changed drastically, the commitment and actions of the university has not," said DAPL protester and campus junior Camille Fassett.&lt;br/&gt;The board will reconvene Thursday to vote on a new operating budget plan, which includes tuition hikes for in-state and out-of-state students.&lt;br/&gt;Audrey McNamara is the lead higher education reporter. Contact her at [email protected] and follow her on Twitter at @McNamaraAud.</t>
         </is>
+      </c>
+      <c r="L73" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -3620,10 +3846,13 @@
           <t>Sexual assault/violence, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J74" t="inlineStr">
+      <c r="K74" t="inlineStr">
         <is>
           <t>Continuing its criticism of Columbia's policy prohibiting students from recording gender-based misconduct proceedings, No Red Tape held its first rally of the semester on Low Steps on Friday and demanded that the University give students the right to record.&lt;br/&gt;Last month, the activist group published an online petition arguing that the policy violates New York State's campus anti-sexual violence bill, Enough is Enough. That law states that universities must require students access to the investigation records the institution keeps-it does not specify a type of record that must be maintained.&lt;br/&gt;Administrators have continued to defend the policy, warning that most students feel uncomfortable with having their testimony recorded and that rescinding the policy would create a chilling effect.&lt;br/&gt;About 30 students attended the rally, during which survivors of sexual assault spoke about their experiences undergoing Columbia's gender-based misconduct investigations. Two survivors elected to play recordings they had created of their interviews with the University's investigators, with one survivor admitting to recording the exchange despite the policy. According to the survivors, the recordings are proof that investigators misconstrued their testimonies or handled their cases improperly.&lt;br/&gt;"This policy leaves students without an effective means of record-keeping to hold the University accountable for its practices and outcomes," activists chanted in unison.&lt;br/&gt;Administrators have pushed back, arguing that the investigation model Columbia uses-ensuring that two investigators interview and take notes during proceedings and allowing students to review those notes and suggest changes-acts as a safeguard.&lt;br/&gt;A series of student groups including Students for Justice in Palestine, International Socialist Organization, Columbia Queer Alliance, and Columbia Divest for Climate Justice, expressed their support for No Red Tape by sponsoring the event.&lt;br/&gt;The rally also featured Birgit Brander Rasmussen, an assistant professor at Binghamton University, and Anne McClintock, a feminist scholar and public intellectual.&lt;br/&gt;"The right to record is crucial, and we all know this because we just heard Donald Trump brag about grabbing women by the crotch. And we know this because someone recorded it. If it wasn't for that recording, Trump could grab crotches all the way to the White House," Brander Rasmussen said. "Like he said, you can get away with it. You can get away with it unless there is a recording."&lt;br/&gt; | @CatieEdmondson</t>
         </is>
+      </c>
+      <c r="L74" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -3658,10 +3887,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J75" t="inlineStr">
+      <c r="K75" t="inlineStr">
         <is>
           <t>Demonstrators call on Harvard to divest its endowment from fossil fuels in 2014, arguing the move will help mitigate climate change. Courtesy of Rick Colson&lt;br/&gt;University President Drew G. Faust signed a statement Monday affirming Harvard's commitment to combatting climate change in the wake of President Donald Trump's decision to withdraw the United States from the Paris Agreement.&lt;br/&gt;In the statement, Faust and the presidents of six other Ivy League universities as well as Duke, Georgetown, Johns Hopkins, MIT, and Stanford promise to "slow, and ultimately prevent, the rise in the global average temperature and to facilitate the transition to a clean energy economy." It comes days after Trump announced that the United States would withdraw from the Paris Agreement, an international accord aimed at limiting the greenhouse gas emissions and the rise of global temperatures.&lt;br/&gt;The university leaders write that their commitment is "consistent with the Paris Agreement."&lt;br/&gt;But some students and faculty are calling on Harvard to also to make further public commitments and join a coalition led by former New York City Mayor Michael Bloomberg that pledges to meet the United States' greenhouse gas emissions target under the Paris Agreement.&lt;br/&gt;More than 1200 American signatories, including governors, mayors, businesses, investors, and institutions of higher education have joined that coalition, according to a statement published Monday afternoon. Harvard is not among the 183 colleges and universities that were signatories, and some faculty members and students are calling on Harvard to take what they say is a stronger stance.&lt;br/&gt;James M. Recht, a Clinical Assistant Professor of Psychiatry at Harvard Medical School and a leader of Harvard Faculty for Divest, said he is disappointed with the University's current stance.&lt;br/&gt;Comparing Harvard's pledge with that of the larger coalition, he said there was a "glaring omission" of "any acknowledgement of the dangerous and really reprehensible actions and behavior of Trump and the Trump administration."&lt;br/&gt;"This statement about support for the Paris Accord loses meaning because it's put out there without any political context. We had a right as members of the Harvard community to expect quite a bit more," he said.&lt;br/&gt;Recht said he and other members of Harvard Faculty for Divest circulated a petition among several hundred Harvard faculty Sunday afternoon, receiving 78 signatures. They sent a brief letter to Faust Sunday evening with the faculty signatures, but Recht said they have yet to receive a response.&lt;br/&gt;Students have also encouraged Faust to join the Bloomberg-led coalition. Members of the Harvard College Conservation Society drafted an open letter, which has dozens of signatory student groups as of Tuesday afternoon, including the Harvard Democrats, members of the Undergraduate Council, performing arts organizations, and other affinity groups.&lt;br/&gt;Katherine A. Culbertson '18, president of Harvard College Conservation Society, said she has been "so excited to see much support for a wide range of student organizations and students."&lt;br/&gt;"To see that solidarity has been really an incredible thing, especially after having been so down about the decision on Thursday," she said.&lt;br/&gt;HCCS also launched an online petition Monday evening and received more than 250 individual signatures in the first day, according to Andrés M. López-Garrido '18, Advocacy Project Leader of HCCS.&lt;br/&gt;López-Garrido, whose position was created following the success of the open letter campaign, said the group plans to keep gathering signatures in the coming weeks and applying student pressure on administrators to take stronger action.&lt;br/&gt;Culbertson said she hopes to continue the conversation and for Faust to respond to the students' open letter.&lt;br/&gt;"This has instilled in all of us working on the letter with a new sense of vigor and a feeling that maybe we can actually do something in a time where so many of us have felt so powerless," Culbertson said.&lt;br/&gt;-Staff writer Sarah Wu can be reached at  Follow her on Twitter @sarah_wu_.Want to keep up with breaking news? Subscribe to our email newsletter.&lt;br/&gt;Read more in University News Manning, Professor and Constitutional Law Scholar, Named Law School Dean</t>
         </is>
+      </c>
+      <c r="L75" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -3701,10 +3933,13 @@
           <t>Pro-Palestine/BDS</t>
         </is>
       </c>
-      <c r="J76" t="inlineStr">
+      <c r="K76" t="inlineStr">
         <is>
           <t>On Sept. 12, it was announced that Israeli Prime Minister Benjamin Netanyahu and Palestinian Authority President Mahmoud Abbas would potentially be meeting in Luxembourg to further negotiate a peace settlement. This is a potential step toward further diplomacy and peace between the two sides. However, within our own gates, the value and importance we grant to open and constructive dialogue came under protest Sept. 8.&lt;br/&gt;The Center for Jewish Civilization hosted an event titled "The Netanyahu Premiership: A Retrospective," with the hopes of exploring the policies and politics currently surrounding the soon-to-be longest-serving prime minister in Israeli history. The event hosted a panel of speakers, including academics, journalists and former bureaucrats, to dissect and explore the nuances of Netanyahu's leadership while facilitating questions from the audience into the discussion.&lt;br/&gt;Regardless of one's feelings about Netanyahu and his policies, the event was not meant to heap unchallenged support and praise for the prime minister, but rather to earnestly discuss and criticize aspects of his tenure. The event presented itself as an example of what dialogue at Georgetown could look like when experts and students come together to learn and listen from one another on contentious topics.&lt;br/&gt;Yet during the open question section of the event, various protesters began disrupting the event. According to present students, a few individuals pushed past other attendees to ask questions while others unveiled a banner before chanting "From the river to the sea, Palestine will be free." Eventually they were escorted out of the event by security, with a few able to linger for a few minutes longer before chanting different pro-Palestinian phrases, with one protester yelling "The panel lies to you" before being escorted out as well.&lt;br/&gt;Nowhere in America should one's freedom of speech and expression be more defended than on a college campus, where academic life pushes us to new intellectual curiosities and ideas while encouraging us to confront opinions with which we may disagree. Yet the issue with Thursday's protest is in its conduct and procedure. Students essentially protested an open panel and dialogue, where a free expression of ideas was welcome, but disruption was certainly not.&lt;br/&gt;While the event was interrupted only momentarily and the question-and-answer session was eventually able to continue, the protesters interrupted others' ability to ask questions, momentarily preventing concrete dialogue from occurring on a contentious topic. Protests can be valuable tools and outlets for making points when other forms of expression fall on deaf ears. Yet when protests prevent dialogue from happening, they can become protests of the dialogue itself as opposed to the original issue. The chief problem is that this protest of dialogue strips the ability of others to develop their own freely created opinion on any issue.&lt;br/&gt;A similar situation occurred in March 2015, when members of GU Fossil Free protested and interrupted a visit by President of the World Bank Group Jim Yong Kim. The protesters, who unfurled a banner on the stage where Kim was about to take questions from audience members, called for Georgetown to divest its endowment from companies in fossil fuel industries.&lt;br/&gt;While the group succeeded in capturing momentary public attention, Kim's whole talk focused on addressing the dangers of ignoring climate change and promoting concrete action - an issue in line with the very motives of the protesters themselves. Kim even praised the work of GU Fossil Free, claiming it has given a positive contribution by forcing the question of divestment onto a college campus. By the event's end, it seemed the protesters, while eye-catching, would have made a greater contribution to the issue and conversation by asking questions when the opportunity presented itself rather than causing disruption to others' learning and engagement.&lt;br/&gt;The same could be said of those protestors at the Netanyahu panel. Our campus community should, as a whole, understand that freedom of speech and expression is a two-way street. Using speech as a silencer expresses a disbelief in others' ability to engage in conversation. It would be best for future protesters to consider whether their actions further constructive dialogue or merely hamper students' abilities to develop their own opinions after having the opportunity to hear both sides.&lt;br/&gt;Have a reaction to this article? Write a letter to the editor.Tags: Dialouge, fossil free, Free Expression, free speech, netanyahu, protest</t>
         </is>
+      </c>
+      <c r="L76" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -3749,10 +3984,13 @@
           <t>Indigenous issues</t>
         </is>
       </c>
-      <c r="J77" t="inlineStr">
+      <c r="K77" t="inlineStr">
         <is>
           <t>Students are pushing back on the Trump administration's recent approval of completing the Dakota Access Pipeline by protesting more than 1,000 miles away.&lt;br/&gt;Native American and environmental activists have resisted the pipeline, which would go through Standing Rock Reservation in South Dakota, since April because of concerns about potential water contamination and disturbance of sacred tribal ground. Students who have protested against the pipeline said while the decision to complete the project is a setback, they will continue to protest in D.C. and hold phone banking sessions to lobby companies funding the construction to shut it down a second time.&lt;br/&gt;Construction on the pipeline was initially blocked in December by the U.S. Army Corps of Engineers. But on Jan. 24, President Donald Trump signed an executive order to resume construction.&lt;br/&gt;Green GW, a student organization focused on environmental issues, posted the names and contact information of banks that are funding the construction of the pipeline on Facebook, asking students to call the banks to pull their support for the project.&lt;br/&gt;Isabelle Moody, vice president of Green GW, said the post is part of Green GW's newest protest strategy to encourage students to divest their money from the pipeline.&lt;br/&gt;"If we shift our focus from one of broader education on campus to a mission that's more in line with environmental justice, I think we can make an even bigger impact," Moody said.&lt;br/&gt;Moody said that although her group recognized the environmental impact of the pipeline, members believe the spotlight should be on the Native Americans most affected by the project.&lt;br/&gt;"What it comes down to is remembering that it's about them," Moody said. "The environmental movement is largely white and historically hasn't paid attention to these kinds of issues. We really need to speak up."&lt;br/&gt;Kate Cooper, a sophomore and Eastern Band Cherokee, said she spent months protesting against the pipeline.&lt;br/&gt;"When I first heard of Trump's decision I was heartbroken," Cooper said. "In his first days of presidency, he had managed to undo almost a year's worth of selfless people putting their lives on the line."&lt;br/&gt;She said constructing pipeline was a human rights issue in that it puts sacred Native American land in jeopardy and could potentially pollute local water sources.&lt;br/&gt;"Can you imagine being removed from land that was once yours, knowing that your ancestors were buried there, and then being told that a giant pipeline of oil was being drilled right through it? Let that sink in," Cooper said.&lt;br/&gt;More than 400 students marched from the White House to Rice Hall in November to protest Trump's rhetoric supporting the pipeline, which included speaking out against his support for completing the pipeline. Students in the walkout called out the Lakota chant, "Mni wiconi, water is life."&lt;br/&gt;Cooper said she has participated in marches and demonstrations against the pipeline and found that people often didn't know much about the pipeline's impact.&lt;br/&gt;"I feel like toward the end of 2016, there were still so many people who didn't really understand 'NoDAPL' to its full extent," Cooper said. "As uncomfortable as it can be, sometimes all you can do is try your absolute hardest to make sure that every person knows what's really going on."&lt;br/&gt;Despite Trump's decision, she said activists should continue the fight through in-person and online activism, as well as calling the companies that fund the construction.&lt;br/&gt;"I soon realized that there was no point for feeling sorry and acting defeated," Cooper said. "The fight isn't over-now is the time to fight harder than ever."&lt;br/&gt;This article appeared in the February 23, 2017 issue of the Hatchet.</t>
         </is>
+      </c>
+      <c r="L77" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -3792,10 +4030,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J78" t="inlineStr">
+      <c r="K78" t="inlineStr">
         <is>
           <t>Protesters call for Chico State to cut ties with banks lending to North Dakota Access pipeline&lt;br/&gt;Nicole Henson&lt;br/&gt;February 19, 2017&lt;br/&gt;Filed under Campus, Community, News&lt;br/&gt;After Seattle voted to cut ties with Wells Fargo because of its ties to the Dakota Access Pipeline, Chico protesters are asking Chico State to do the same.&lt;br/&gt;Chico State was the first public university in the United States to fully sever ties with fossil fuel companies in 2014. This raises concern as to if the current divestment plan from fossil fuels coincides to working with organizations who are helping fund projects such as installing a crude oil pipeline.&lt;br/&gt;The University's website states the divestment plan in fossil fuel companies is an effort to use every opportunity to move toward an environmentally sustainable future.&lt;br/&gt;Local activists and members of the Mechoopda tribe held organized protests the week of Feb. 6 in favor of people and administrations divesting in big banks such as Wells Fargo. Protesters said they believe that if this becomes an ongoing trend across the nation, then these banks may divest in funding the installment of a pipeline that could lead to water contamination.&lt;br/&gt;Chris Howell, Chico resident and Sioux tribal member, began protesting near campus Feb. 7. He had received word from the Indigenous Support Collaborative NorCal that the day would be a collective call to action against funding of the pipeline.&lt;br/&gt;"I know Chico State uses banks who fund DAPL," Howell said. "They don't have a divestment plan, but we are starting to unify because we are not alone. Since Seattle did it, I felt strongly that Chico State could do it too."&lt;br/&gt;Samuel White Swan-Perkins, an organizer with Indigenous Support Collaborative NorCal, said he believes the first step in Chico residents supporting this movement is recognizing native territory.&lt;br/&gt;"Begin by recognizing that all of us who are not of Mechoopda heritage reside on occupied Mechoopda Territory and that this land was taken from them," White-Swan Perkins said. "Without this acknowledgement, particularly from the non-Native Americans, non-people of color who live in Butte County, the genocide that was forced upon the local Nations is perpetuated."&lt;br/&gt;The Mechoopda tribe has a plan in progress that will propose that Chico State sever ties with banks funding the pipeline.&lt;br/&gt;"While the exact details of the plan are in the works, I can share that we have a varied group of professionals from the Native American and allied community working together to to address this issue," White Swan-Perkins said.&lt;br/&gt;Until this plan is mobilized, students can learn more about supporting this cause at .&lt;br/&gt;Nicole Henson can be reached at  or @nicohenson on Twitter.&lt;br/&gt;If you want a picture to show with your comment, go get a gravatar.&lt;br/&gt;Name (required)&lt;br/&gt;Email Address (required)&lt;br/&gt;XHTML: You can use these tags:&lt;br/&gt;Speak your mind&lt;br/&gt;Click to cancel reply</t>
         </is>
+      </c>
+      <c r="L78" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -3835,10 +4076,13 @@
           <t>Labor and work, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J79" t="inlineStr">
+      <c r="K79" t="inlineStr">
         <is>
           <t>Student activists who pushed Georgetown University to commit not to invest in private prison companies now say the university is unfairly taking the credit for their activism in an Oct. 5 news release announcing the new policy.&lt;br/&gt;The university announced the policy after a committee of the university's board of directors accepted a March recommendation of the Committee on Investments and Social Responsibility, which makes recommendations to the board on ethical investment policies. Under the new policy, the university will encourage its external investment managers to avoid investments in private prison companies.&lt;br/&gt;What the university's announcement mentioned only briefly, however, was how the proposal came to the CISR in the first place: It was submitted by Eman Abdelfadeel (COL '17), Sophie Bauerschmidt Sweeney (COL '17) and Salma Khamis (SFS '17), and accompanied by a three-month campaign launched last December by the student group Georgetown University Forming a Radically Ethical Endowment.FILE PHOTO: JEANINE SANTUCCI/THE HOYA Students at a 2016 rally organized by activist student group GU F.R.E.E.&lt;br/&gt;Abdelfadeel said the university's statement took credit for the change while only briefly alluding to student involvement.&lt;br/&gt;"Understating the fact that this was a call from students is indicative of a trend of the administration being unresponsive to the demands of the wider community and then taking credit for the work once it has become socially and/or financially appropriate for them to do the right things," Abdelfadeel said.&lt;br/&gt;The release made one reference to the students' involvement, saying the CISR "reviewed a student proposal that included a request that the university divest from the private prison industry."&lt;br/&gt;"After finding investing in the private prison industry to be inconsistent with Georgetown's commitment to socially responsible investing - which is reflected in the new SRI policy, CISR submitted a recommendation to the board that supported this strategy," the release said.&lt;br/&gt;A discussion of the activism that led up to the decision is lacking from the campus conversation, according to Christian Morris (COL '19), a student organizer for GU F.R.E.E.&lt;br/&gt;"I feel like it was worked for," Morris said. "I want to bring it back to the fact that student activism, student pressure and conversations are happening. I haven't heard anything about the demonstrations we did last year, or the events that we disrupted, or the proposal we submitted through Georgetown's bureaucratic loopholes."&lt;br/&gt;A university spokesperson did not respond to requests for comment.&lt;br/&gt;This is not the first time students have criticized the university for taking credit for activists' efforts.&lt;br/&gt;Lily Ryan (COL '18), a member of the workers' rights student activist group Georgetown Solidarity Committee, said the administration failed to acknowledge GSC's role in a 2016 dispute with the university over its licensing contract with Nike.&lt;br/&gt;Students associated with the GSC staged a 35-hour sit-in last December in the office of University President John J. DeGioia, demanding the university cut its contract with Nike unless the company agreed to allow independent workers' rights inspections of its factories. After hours of negotiations between students and university administrators, the university ultimately agreed to the students' demands and allowed the contract to expire at the end of the year. The parties struck a new contract in August which included an agreement to allow regular, independent inspections of Nike supplier factories.&lt;br/&gt;A university news release announcing the new contract in August does not mention GSC, the sit-in or student activism. One line in the eighth paragraph of the release notes the university "engaged with faculty and student leaders" while negotiating the contract.&lt;br/&gt;Ryan said the framing of the university's statement disregards the pivotal role of student activists in pressuring the university to negotiate the new contract.&lt;br/&gt;"What troubles me is that, as usual, there is no mention of the extensive efforts that students put into pushing Georgetown into a decision," Ryan wrote in an email to The Hoya. "While I can't speak for all students or student activists on campus, I don't think we do it for the glamor or for the recognition by university administrators but I think it erases the work done by students, in the case of GU F.R.E.E., it was work done in large part by queer students and students of color."&lt;br/&gt;Ryan said the way the university represents student activism is important for reasons other than conferring credit.&lt;br/&gt;"The stories we tell about victories and failures are important and it can be hard to tell stories about student activism when the activists are left out of the narrative," Ryan wrote. "I knew when the statement was released about private prisons that it had taken time and effort on the part of a committed group of students, but I know that so many students don't know, and that can be detrimental to promoting a culture in which students can engage in activism."&lt;br/&gt;As for the future, Abdelfadeel noted the work of divestment advocates is unfinished. The original group's 2016 proposal to the CISR was more broad than the one enacted by the board of directors this month, also including a request for divestment from companies invested in private prisons, rather than only private prisons themselves.&lt;br/&gt;"The original proposal to the CISR proposed divestment from private prisons and the wider industry that sustains it," Abdelfadeel said. "It would be great to see a commitment from the university regarding the wider private prison industry."&lt;br/&gt;The proposal also called on the university to divest from any companies that benefitted financially from the Israeli occupation of Palestine, a request that was rejected by the CISR.&lt;br/&gt;Abdelfaleel said there are common threads in the social implications of private prisons and the occupation.&lt;br/&gt;"We found common themes of state violence - black people living and dying under the United States' white supremacy and Palestinians living and dying under Israeli settler colonialism and apartheid. Moreover, there is an overlap in companies that empower the private prison industry and the illegal occupation," Abdelfaleel said.&lt;br/&gt;GU F.R.E.E. also continues to call for greater transparency in Georgetown's investment records and promotes general public consciousness of the university's investment policies.&lt;br/&gt;Morris, meanwhile, said he hoped that this decision would prompt the university to look at other instances of state violence and adapt its investment policies accordingly.&lt;br/&gt;"I hope there is something sustaining from the divestment of prisons, not like, 'OK, we did it; it's done,'" Morris said. "This should only be the beginning of Georgetown's broader divestment movement."&lt;br/&gt;Have a reaction to this article? Write a letter to the editor. Tags: activism, divestment, georgetown solidarity committee, GU F.R.E.E.</t>
         </is>
+      </c>
+      <c r="L79" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -3878,10 +4122,13 @@
           <t>Immigration (For), University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J80" t="inlineStr">
+      <c r="K80" t="inlineStr">
         <is>
           <t>By: Hannah Knowles | Managing Editor of News&lt;br/&gt;At an Admit Weekend event Thursday, student activists pushing "sanctuary campus" measures protested onstage with signs (Courtesy of Doris Rodriguez).&lt;br/&gt;As Admit Weekend kicked off Thursday, students from four campus activist groups took the stage at the University's official Welcome event in Memorial Auditorium to protest for increased University support for undocumented students.&lt;br/&gt;About a dozen students from Stanford Sanctuary Now , Students for the Liberation of All People , MEChA de Stanford and the Stanford Student and Labor Alliance stepped onstage bearing cardboard signs as Provost Persis Drell addressed prospective freshmen (ProFros) and their families.&lt;br/&gt;The students remained onstage for roughly an hour through a series of administrators' speeches, staying silent during the talks but chanting during intermissions and taking up a mantra of their own when Dean of Admission and Financial Aid Richard Shaw tried to lead admits in a chant.&lt;br/&gt;"It's really about accountability," said Doris Rodriguez '20, one of the activists and a recently elected ASSU senator. "We were there to show our presence, to show the ProFros [who are] being told this school is perfect... there's a lot that Stanford needs to do better, and we're not afraid to call Stanford out on that."&lt;br/&gt;The protesters have called for a variety of  University actions related to immigration. SSN's agenda, supported by the other groups demonstrating, advocates measures ranging from Stanford's divestment from private prisons to a pledge to fully fund deportation defense for students, workers and their families.&lt;br/&gt;Earlier this year, SSN led an unsuccessful push for Stanford to declare itself a "sanctuary campus"- the University equivalent of "sanctuary cities," which generally refuse to enforce federal immigration laws with local funding. Although the University declined the official sanctuary label, it has promised to keep students' and employees' records private unless legally forced and is providing immigration-related legal help to community members. Stanford spokesperson E.J. Miranda said the University cannot directly cover families' legal needs, but will help them find other pro bono resources.&lt;br/&gt;Amid the protest, administrators proceeded with their speeches and did not attempt to remove the students onstage, though Miranda later said the University was "disappointed" with the activists' methods. Briefly addressing the situation during the event, Vice Provost Harry Elam told the crowd that the demonstration was unexpected but "shows something about Stanford," according to Miranda and students present at the event.&lt;br/&gt;"These students love Stanford," Elam said, according to Miranda. "They may want something different of Stanford. They're going to hold us to account, and we understand that. That is one of the things that makes this place so special."&lt;br/&gt;Rodriguez said that most of the audience was receptive to the protest, at some points cheering the demonstrators on. However, she said, one attendee who appeared to be a parent responded to one of their chants by calling out, "legal immigrants are welcome here."&lt;br/&gt;"All immigrants are welcome here," the protesters chanted back, according to Rodriguez.&lt;br/&gt;The activists exited the stage right before a student panel.&lt;br/&gt;Miranda wrote in an email to The Daily that the University empathizes with the students' concerns but takes issue with the protesting groups' venue choice of Thursday's central Admit Weekend event.&lt;br/&gt;"These students have previously raised these issues and we have already extensively discussed them during in-person meetings and in other settings, so it is disappointing that they chose to disrupt an event that was so important to those attending," Miranda wrote.&lt;br/&gt;Miranda noted that the University is currently considering some of SSN's priorities: For example, he said, a request to divest from private prisons is moving through the Advisory Panel on Investment Responsibility and Licensing .&lt;br/&gt;However, Rodriguez argued Stanford still has work to do to fully support the undocumented community, noting that Georgetown University, for example, has a center specifically for undocumented students. SSN's demands call for increased University support for local undocumented immigrants, expanded professional opportunities and protections for Stanford immigrant workers and more.&lt;br/&gt;Prospective students who attended the Welcome event had a variety of opinions on the protest.&lt;br/&gt;"I'm glad they protested," said Peter Caroline '21. "More people, especially incoming freshmen, needed to see the difference they can make or should make."&lt;br/&gt;Hannes Boehning '21, on the other hand, wished that the activists had protested outside the building. At first, he said, many ProFros thought the demonstration was part of the official event. He found the protest "irritating" because it distracted from the day's speeches.&lt;br/&gt;Rodriguez believed many ProFros were heartened by the demonstration. She recalled how one ProFro approached her and her fellow activists after the event to say he was "glad Stanford was a place where people speak up."&lt;br/&gt;"The biggest goal of today was bringing the conversation out for the incoming class," Rodriguez said. "A lot of the time the activists graduate out. We want to keep the conversation going on with the incoming classes."&lt;br/&gt;Contact Hannah Knowles at hknowles 'at' stanford.edu.</t>
         </is>
+      </c>
+      <c r="L80" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -3928,10 +4175,13 @@
           <t>Immigration (For), University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J81" t="inlineStr">
+      <c r="K81" t="inlineStr">
         <is>
           <t>In the wake of the presidential election earlier this month, student organizing and activism on campus has swelled to address the concerns brought about by the proposed policies of the president-elect.&lt;br/&gt;On Nov. 15, over 100 students crowded into the Scheuer Room for the first of two interest meetings dedicated to coalition building and strategizing about avenues for action both on campus and beyond. The second of these meetings took place two days after the first. The organizers of the meeting, Priya Dieterich '18 and Aru Shiney-Ajay '20, hoped that these gatherings would provide a space to effectively channel the fervor for action that has grown within the student body in recent weeks and generate ideas about how to fortify the college community for the coming years.&lt;br/&gt;"Aru and I independently had the idea of holding a meeting to connect different students who want to organize.  When I found out about her meeting, we joined forces and co-facilitated these two meetings.  I have seen and heard about - and personally felt - so much anger, frustration, and energy in the last week or so, and I wanted to help us collectively make the step towards concrete action," Dieterich said.&lt;br/&gt;In her description of the event on Facebook, Shiney-Ajay emphasized the intersectional focus of the meeting and the diverse motivations that brought students into that space.&lt;br/&gt;"People from vastly different political and personal backgrounds stand against Trump - from groups focused on identity to groups focused on party politics. In order to effectively organize, we must, at least, be aware of various efforts. Tactical disagreement is encouraged," she wrote.&lt;br/&gt;A brainstorming session among the entire group was followed by small-group discussions in which more concrete action plans were formulated. Topics raised in these discussions included an increased institutional support for college staff, a student-led course derived from reading lists released by Black Lives Matter and the Standing Rock Sioux Tribe, a renewed campaign for fossil fuel divestment, and a social justice academic distribution requirement.&lt;br/&gt;"A lot of really great ideas were brought up at the meetings: [ideas] about how we can organize both on campus and off, about how to leverage our power and privilege as students, about how to responsibly and respectfully plug into existing activist work in our communities, about how to honor our commitments to social justice as an institution," Dieterich said.&lt;br/&gt;Among the plans voiced at the Nov. 15 meeting was a school-wide walkout scheduled for Wednesday, Nov. 17 at noon. Swarthmore joined over 80 other colleges across the country in campus-wide walkouts, which were organized by students in coordination with Movimiento Cosecha, a nonviolent movement dedicated to protecting the rights of immigrant populations in the United States.&lt;br/&gt;At Swarthmore on Wednesday, hundreds of students gathered in front of Parrish Hall to demand that the college become a Sanctuary Campus, thereby providing institutional support to undocumented community members. The specific stipulations of a Sanctuary Campus include measures such as a special advisor for undocumented students, financial support for legal procedures that undocumented students may need to undergo, and a commitment to protecting undocumented community members from law enforcement officials such as U.S. Immigrations and Customs Enforcement.&lt;br/&gt;Just after noon, in front of an audience of students, faculty, staff, and other community members, Jordan Reyes '19 led the group in chants and served as a sort of moderator for the student speakers at the event, all of whom drew upon personal experiences as undocumented or Latinx people whose security is directly endangered by the Trump administration.&lt;br/&gt;"This event was, more than anything, a showing of solidarity and support for any group that may be targeted in the coming months and years, more specifically the Latinx community and undocumented students," Reyes said, following the event.&lt;br/&gt;Wednesday's walkout was just one of a series of actions that students have undertaken to pressure the college to become a Sanctuary Campus.&lt;br/&gt;Killian McGinnis '19 was responsible for drafting the petition for a Sanctuary Campus that has, at the point of publication, garnered nearly 2,000 signatures from students, faculty, staff, alumni, and other community members. The petition will be presented to the Board of Managers at their upcoming meeting this Saturday, Dec. 2.&lt;br/&gt;McGinnis says that the she is hopeful about the prospect of a Sanctuary Campus at Swarthmore.&lt;br/&gt;"Students, faculty members, and administrators alike have devoted time and collaborative energy to thinking critically about what it would mean to make Swarthmore a Sanctuary Campus, and I would be surprised and disappointed if the Board's decision didn't reflect the widespread community support of the initiative," said McGinnis.&lt;br/&gt;In addition to creating the petition, McGinnis has been collaborating with a group of students who identify as undocumented and Latinx, co-led by Miguel Gutierrez '18 and Ivan Lomeli '19,&lt;br/&gt;to formulate a faculty resolution to support the movement for a Sanctuary Campus. According to Lomeli, this resolution outlines the ways in which members of the faculty and staff at the college can continue to support the undocumented student population.&lt;br/&gt;Lomeli underscored that the effort to make the college a Sanctuary Campus is critical to alleviate the acute threat that a Trump administration will pose to undocumented students, specifically pointing to the vulnerability of students who are protected by Presidents Barack Obama's Deferred Action for Childhood Arrivals, which President-elect Trump has denounced as an unconstitutional overreach of executive power, and which he has publicly promised to overturn. DACA allows undocumented young people who entered the U.S. before the age of 16 to obtain a protected status, work permit, and social security number for two years at a time after a lengthy application process that costs $465 and is most often underwent without an attorney.&lt;br/&gt;"The undocumented population on campus, of which most but not all, benefit from DACA, worried about what would happen if their benefits were taken away. Many, including myself, were discouraged from studying abroad to prevent being stuck outside of the country in case DACA was removed," Lomeli said.&lt;br/&gt;Furthermore, DACA impacts a student's life beyond their tenure at the college. Lomeli pointed out that, were DACA to be repealed, its beneficiaries would no longer be able to work legally in the United States.&lt;br/&gt;"The list of workplaces that sponsor employees to citizenship is very small and not at all promising," he said.&lt;br/&gt;Lomeli stressed that the walkout, the petition, and the faculty resolution affirmed a feeling of support and solidarity from the college that was much appreciated, and he, like McGinnis, hoped that this support would translate into a formal decision by the Board of Managers on Saturday.&lt;br/&gt;"The faculty and staff, along with the many people whose energy and hope have been put into this Sanctuary Campus movement, await the response of the Board of Managers. If the Board of Managers chooses to ignore our plea, it will have to silence more than just the undocumented students on campus as there is a community standing behind us," he said.&lt;br/&gt;In addition to the movement for a Sanctuary Campus, a diverse array of student groups on campus have organized other solidarity actions in direct response to the presidential election and in support of those who will be most affected by the election.&lt;br/&gt;In one such display of solidarity, students and several members of the administration met on Wednesday to participate in a national day of Jewish resistance declared by IfNotNow, a movement of American Jewish youth dedicated to progressive political causes. Marissa Cohen '17 and Mira Revesz '17, who organized the action, stated that it was meant to call on the Jewish establishment, the U.S. government, and any other institution claiming to represent the interests of young American Jews to prioritize human rights and dignity above all else.&lt;br/&gt;"We stood as Jewish students and allies to uphold the lesson of 'never again' for every targeted community and challenged our communal institutions to do the same. We ask these institutions to condemn Trump and Bannon and stand up against anti-Semitism and white supremacy of any kind," said Cohen and Revesz in a joint statement.&lt;br/&gt;While the spike in student mobilization is discernible to many in the college community, it is not without precedent. Professor of sociology Lee Smithey drew connections between the kind of energy he is currently witnessing to the spring of 2013, often called the "Spring of Discontent," which was also marked by heightened student mobilization and activism, saying that he sees the two periods as united by a distinct sense of fear and threat. However, Smithey was careful to note that the stakes and the particular political conditions of the two periods are markedly different.&lt;br/&gt;"The presidential election is a much higher profile, really world-historical event, so the concern and even fear among many people is more widespread. It has stirred concerns about student experiences as well as larger national political concerns. President-elect Trump's rhetoric about ending DACA, for example, has brought these worlds together: our daily life at the college and national politics," Smithey said.&lt;br/&gt;Smithey also emphasized that this period of student organizing in the face of the election is still in its infancy, and will likely evolve to meet the urgent needs and concerns of that will become more apparent as Donald Trump takes office.&lt;br/&gt;"It feels a little early to characterize what student mobilization, or faculty or staff mobilization for that matter, is really like or is going to be like," Smithey said.&lt;br/&gt;However, while acknowledging that the full picture of student activism has yet to come into focus, Smithey expressed cautious optimism at the ability of the student body and the Swarthmore community at large to address these needs in an intersectional, multidimensional way.&lt;br/&gt;"I do recall being impressed during that first organizing meeting at what seemed to be a real willingness among the students there to work in cooperation with one another across different groups and different interests and different concerns. That will take careful work - to continue with that kind of strategic care - and I think it will be really interesting to see if we can sustain that."&lt;br/&gt;In the final weeks of the semester, the work of student organizers will continue to include, among other endeavors, phone banking against the construction of the Dakota Access Pipeline and the state-sponsored violence against the Standing Rock Sioux Tribe, a solidarity march through the town of Swarthmore, and, no matter what the decision of the Board of Managers, the realization of a Sanctuary Campus at the college. Thus, while it remains to be seen how student organizing will adjust and respond to the impending presidential administration, the current climate of activism shows no signs of cooling in the immediate future.</t>
         </is>
+      </c>
+      <c r="L81" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -3978,10 +4228,13 @@
           <t>Immigration (For), University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J82" t="inlineStr">
+      <c r="K82" t="inlineStr">
         <is>
           <t>There is no shortage of public outcry across the country in protest of the newly established Trump administration. As recently as Monday, January 23rd, members of Swarthmore Mountain Justice, in collaboration with over 50 other colleges across the country, organized a walk-out / teach-in aimed at calling attention to the environmentally-threatening rhetoric of the Trump administration.&lt;br/&gt;The walk-out / teach-in, though student run and organized, was a collective effort between Mountain Justice and appointed faculty to rally the general college population to reject climate denialism. A walk-out is a form of protests where participants walk out of their workplace or classroom to gather for a rally; a teach-in refers to a somewhat casual lecture made by expects aimed at educating protest participants.  For Mountain Justice, an organization whose main focus is to push the college to divest their endowment from fossil fuel companies, the proposed policies of the Trump administration are especially troubling as they hinder environmental justice on a larger scale.&lt;br/&gt;Stephen O'Hanlon '17, a longtime member and coordinator of Mountain Justice, spoke about how the Trump administration's policies conflict with the cause.&lt;br/&gt;"[On Friday,] Donald Trump was inaugurated as president of the United States. At noon, when I guess he officially took office, all of the information on climate science was taken off of the White House webpage. He's nominated Rex Tillerson, the former CEO of Exxon ... Companies like Exxon have been imperiling communities around the world and the very future of our generation, and now, they have [a] huge influence in this administration," he said.&lt;br/&gt;Trump's nomination of Rex Tillerson for Secretary of State has been hotly contested because of his 40-year leadership role in ExxonMobil, an American oil and gas company attributed with the exploitation and ill-treatment of marginalized communities, as well as his well documented climate science denialism.&lt;br/&gt;One example of this was a statement made by Tillerson during a 2013 annual shareholders meeting where he denied the existence of climate change, a phenomenon scientists have been consistently providing evidence for since the 1970s.&lt;br/&gt;"If you examine the temperature record of the last decade, it really hadn't changed ... I know you will like to hear that as it don't comport to some of the views of others, but last ten years' temperatures had been relatively flat," he purported.&lt;br/&gt;Aru Shiney-Ajay '20, Coordinator for Mountain Justice, called for Swarthmore to be proactive in its efforts to be socially and environmentally conscious.&lt;br/&gt;"It's a message to the Swarthmore community and board that, in an era of Trump's administration with climate denialism so rampant, that Swarthmore can no longer afford to be neutral," she said.&lt;br/&gt;Protesting the Trump administration on different fronts is not new for Swarthmore's population. In November, a few short weeks after Trump's election, students organized a walk-out where hundreds of students, faculty, and staff joined in solidarity with immigrant populations to advocate for their rights and safety. This included the demand, which was eventually met, of the college becoming a Sanctuary Campus. Again, the pro-activism sentiments shared by many at the college was evidenced by the number of students participating in the Women's March on Washington and Philadelphia to advocate for women's rights in addition to healthcare, environmental justice, and the rights of marginalized groups.&lt;br/&gt;Melissa Tier '14, Sustainability Program Manager, lent her support to the students during the walk-out/teach-in, praising the efforts made by the students to protest.&lt;br/&gt;"I certainly think that interacting, having a conversation, taking action against the climate denialism of our current administration is essential. That takes a lot of different forms; a teach-in is fantastic way to go about it, it's one of many and I hope it continues," she said.&lt;br/&gt;On the topic of campus protest, Tier also spoke about the history of protest at Swarthmore and campus activism, noting that she thought that mass participation from the campus community was wonderful.&lt;br/&gt;"A teach-in is an excellent approach, one that's actually not new to Swarthmore...during my time as a student at Swarthmore, we definitely had teach-ins, some of them focused on sustainability and climate justice. I'm always in favor of multi-pronged approaches, both because they can address topics in different ways, and because they can attract different people. I think the more people you can get involved with a topic, the better," she said.&lt;br/&gt;The news of protests both on and off campus have served to mobilize many students; but some admittedly do not share the same fervor.&lt;br/&gt;Ibrahim Tamale '20 offered his opinion on participating in protests and why he doesn't.&lt;br/&gt;"I have not felt any effect socially, or any injustice done against me to go and protest or to take any action. I believe actions should be taken as a reaction to something, but if nothing's being done to you personally or as a society, then I don't see why you should be moving forward to take action. Actions should have goals, ... and if there are no goals, I don't see any precedence for taking action at the moment," he said.&lt;br/&gt;What warrants protest, in Tamale's opinion, is tied to how deeply one's sentiments runs for the cause they are protesting for.&lt;br/&gt;"I believe people should only attend rallies and protests if they deeply align with the goals and the motives of those rallies and protests. Based on the friends that I have that have participated in protests in Egypt and Tunisia, I believe it's all about willing to die for that cause ... If people are deeply aligned with the cause and do believe that their rallying and protesting is not going to stop until their cause has been fulfilled, then yes. But if they're going to do it for one to two weeks then stop, then no," he said.&lt;br/&gt;Mountain Justice Lead Organizer Abigail Saul '19 explained the importance of engaging in protest against climate denialism.&lt;br/&gt;"We all have a stake in this issue, and the stake looks different for everyone. Climate justice affects everyone, but it is an inequality multiplier, so it affects certain populations a lot more than it affects others. So, I think it's important that we all recognize that and stand together with each other, as well as with communities that are going to be most affected by these issues," she said.&lt;br/&gt;Associate Professor of Sociology and Peace and Conflict Studies Professor Lee Smithey made mention of some of the things he commented on during the event.&lt;br/&gt;"One of my fields of study is social movements; I talked for a couple of minutes about micromobilization ... I then said that the calls for divestment shared by students, faculty, staff and alumni is a perfectly reasonable request under the circumstances ... The fossil fuel companies' dangerous business model is to try and make as much profit as they possibly can off of their product even if it means rejecting climate science ... by extension, through our investments here at the college, we're participating in the same plan. I challenged us all to ask really serious questions about that plan," he said.&lt;br/&gt;Smithey also spoke about the support provided by faculty and staff.&lt;br/&gt;"I think that we are in a historic moment right now with the new administration. I think that there is wide concern among many faculty, staff and students because there are so many different fronts that are under threat at the moment ... I counted at least 25 faculty and staff there. I think we should acknowledge that 20 minutes of sacrificing class time is not insignificant in a busy semester, and the fact that many faculty and staff turned out signaled support for the walk-out," he said.&lt;br/&gt;O'Hanlon asserted that it was imperative for the students and the college to take action in the wake of the new administration.&lt;br/&gt;"As young people, we need to stand up for our futures, for communities around the world, and we need to call on our institution, Swarthmore, as an institution that espouses social justice values, to really stand with our generation, to stand with communities around the world, and to stand for basic science," O'Hanlon asserted.&lt;br/&gt;Eric Jensen, Professor of Astronomy, made a statement during the event which resonated with many participants, receiving the Swat-famous snaps of approval.&lt;br/&gt;"Just because you don't know exactly what to do, doesn't mean you should choose to do nothing," he said.&lt;br/&gt;In this time of confusion and fear for many across the country, many students glean strength from the support of their peers. On the same token, with the same fear and outrage, many take it upon themselves to mobilize and actively rally against injustices. The pro-activism sentiments at Swarthmore have yet to dwindle and, in the coming years and policy changes introduced by the Trump administration, it remains to be seen what next students will participate in. (Visited 3 times, 3 visits today)</t>
         </is>
+      </c>
+      <c r="L82" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -4021,10 +4274,13 @@
           <t>Immigration (For), University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J83" t="inlineStr">
+      <c r="K83" t="inlineStr">
         <is>
           <t>In the wake of the presidential election earlier this month, student organizing and activism on campus has swelled to address the concerns brought about by the proposed policies of the president-elect.&lt;br/&gt;On Nov. 15, over 100 students crowded into the Scheuer Room for the first of two interest meetings dedicated to coalition building and strategizing about avenues for action both on campus and beyond. The second of these meetings took place two days after the first. The organizers of the meeting, Priya Dieterich '18 and Aru Shiney-Ajay '20, hoped that these gatherings would provide a space to effectively channel the fervor for action that has grown within the student body in recent weeks and generate ideas about how to fortify the college community for the coming years.&lt;br/&gt;"Aru and I independently had the idea of holding a meeting to connect different students who want to organize.  When I found out about her meeting, we joined forces and co-facilitated these two meetings.  I have seen and heard about - and personally felt - so much anger, frustration, and energy in the last week or so, and I wanted to help us collectively make the step towards concrete action," Dieterich said.&lt;br/&gt;In her description of the event on Facebook, Shiney-Ajay emphasized the intersectional focus of the meeting and the diverse motivations that brought students into that space.&lt;br/&gt;"People from vastly different political and personal backgrounds stand against Trump - from groups focused on identity to groups focused on party politics. In order to effectively organize, we must, at least, be aware of various efforts. Tactical disagreement is encouraged," she wrote.&lt;br/&gt;A brainstorming session among the entire group was followed by small-group discussions in which more concrete action plans were formulated. Topics raised in these discussions included an increased institutional support for college staff, a student-led course derived from reading lists released by Black Lives Matter and the Standing Rock Sioux Tribe, a renewed campaign for fossil fuel divestment, and a social justice academic distribution requirement.&lt;br/&gt;"A lot of really great ideas were brought up at the meetings: [ideas] about how we can organize both on campus and off, about how to leverage our power and privilege as students, about how to responsibly and respectfully plug into existing activist work in our communities, about how to honor our commitments to social justice as an institution," Dieterich said.&lt;br/&gt;Among the plans voiced at the Nov. 15 meeting was a school-wide walkout scheduled for Wednesday, Nov. 17 at noon. Swarthmore joined over 80 other colleges across the country in campus-wide walkouts, which were organized by students in coordination with Movimiento Cosecha, a nonviolent movement dedicated to protecting the rights of immigrant populations in the United States.&lt;br/&gt;At Swarthmore on Wednesday, hundreds of students gathered in front of Parrish Hall to demand that the college become a Sanctuary Campus, thereby providing institutional support to undocumented community members. The specific stipulations of a Sanctuary Campus include measures such as a special advisor for undocumented students, financial support for legal procedures that undocumented students may need to undergo, and a commitment to protecting undocumented community members from law enforcement officials such as U.S. Immigrations and Customs Enforcement.&lt;br/&gt;Just after noon, in front of an audience of students, faculty, staff, and other community members, Jordan Reyes '19 led the group in chants and served as a sort of moderator for the student speakers at the event, all of whom drew upon personal experiences as undocumented or Latinx people whose security is directly endangered by the Trump administration.&lt;br/&gt;"This event was, more than anything, a showing of solidarity and support for any group that may be targeted in the coming months and years, more specifically the Latinx community and undocumented students," Reyes said, following the event.&lt;br/&gt;Wednesday's walkout was just one of a series of actions that students have undertaken to pressure the college to become a Sanctuary Campus.&lt;br/&gt;Killian McGinnis '19 was responsible for drafting the petition for a Sanctuary Campus that has, at the point of publication, garnered nearly 2,000 signatures from students, faculty, staff, alumni, and other community members. The petition will be presented to the Board of Managers at their upcoming meeting this Saturday, Dec. 2.&lt;br/&gt;McGinnis says that the she is hopeful about the prospect of a Sanctuary Campus at Swarthmore.&lt;br/&gt;"Students, faculty members, and administrators alike have devoted time and collaborative energy to thinking critically about what it would mean to make Swarthmore a Sanctuary Campus, and I would be surprised and disappointed if the Board's decision didn't reflect the widespread community support of the initiative," said McGinnis.&lt;br/&gt;In addition to creating the petition, McGinnis has been collaborating with a group of students who identify as undocumented and Latinx, co-led by Miguel Gutierrez '18 and Ivan Lomeli '19,&lt;br/&gt;to formulate a faculty resolution to support the movement for a Sanctuary Campus. According to Lomeli, this resolution outlines the ways in which members of the faculty and staff at the college can continue to support the undocumented student population.&lt;br/&gt;Lomeli underscored that the effort to make the college a Sanctuary Campus is critical to alleviate the acute threat that a Trump administration will pose to undocumented students, specifically pointing to the vulnerability of students who are protected by Presidents Barack Obama's Deferred Action for Childhood Arrivals, which President-elect Trump has denounced as an unconstitutional overreach of executive power, and which he has publicly promised to overturn. DACA allows undocumented young people who entered the U.S. before the age of 16 to obtain a protected status, work permit, and social security number for two years at a time after a lengthy application process that costs $465 and is most often underwent without an attorney.&lt;br/&gt;"The undocumented population on campus, of which most but not all, benefit from DACA, worried about what would happen if their benefits were taken away. Many, including myself, were discouraged from studying abroad to prevent being stuck outside of the country in case DACA was removed," Lomeli said.&lt;br/&gt;Furthermore, DACA impacts a student's life beyond their tenure at the college. Lomeli pointed out that, were DACA to be repealed, its beneficiaries would no longer be able to work legally in the United States.&lt;br/&gt;"The list of workplaces that sponsor employees to citizenship is very small and not at all promising," he said.&lt;br/&gt;Lomeli stressed that the walkout, the petition, and the faculty resolution affirmed a feeling of support and solidarity from the college that was much appreciated, and he, like McGinnis, hoped that this support would translate into a formal decision by the Board of Managers on Saturday.&lt;br/&gt;"The faculty and staff, along with the many people whose energy and hope have been put into this Sanctuary Campus movement, await the response of the Board of Managers. If the Board of Managers chooses to ignore our plea, it will have to silence more than just the undocumented students on campus as there is a community standing behind us," he said.&lt;br/&gt;In addition to the movement for a Sanctuary Campus, a diverse array of student groups on campus have organized other solidarity actions in direct response to the presidential election and in support of those who will be most affected by the election.&lt;br/&gt;In one such display of solidarity, students and several members of the administration met on Wednesday to participate in a national day of Jewish resistance declared by IfNotNow, a movement of American Jewish youth dedicated to progressive political causes. Marissa Cohen '17 and Mira Revesz '17, who organized the action, stated that it was meant to call on the Jewish establishment, the U.S. government, and any other institution claiming to represent the interests of young American Jews to prioritize human rights and dignity above all else.&lt;br/&gt;"We stood as Jewish students and allies to uphold the lesson of 'never again' for every targeted community and challenged our communal institutions to do the same. We ask these institutions to condemn Trump and Bannon and stand up against anti-Semitism and white supremacy of any kind," said Cohen and Revesz in a joint statement.&lt;br/&gt;While the spike in student mobilization is discernible to many in the college community, it is not without precedent. Professor of sociology Lee Smithey drew connections between the kind of energy he is currently witnessing to the spring of 2013, often called the "Spring of Discontent," which was also marked by heightened student mobilization and activism, saying that he sees the two periods as united by a distinct sense of fear and threat. However, Smithey was careful to note that the stakes and the particular political conditions of the two periods are markedly different.&lt;br/&gt;"The presidential election is a much higher profile, really world-historical event, so the concern and even fear among many people is more widespread. It has stirred concerns about student experiences as well as larger national political concerns. President-elect Trump's rhetoric about ending DACA, for example, has brought these worlds together: our daily life at the college and national politics," Smithey said.&lt;br/&gt;Smithey also emphasized that this period of student organizing in the face of the election is still in its infancy, and will likely evolve to meet the urgent needs and concerns of that will become more apparent as Donald Trump takes office.&lt;br/&gt;"It feels a little early to characterize what student mobilization, or faculty or staff mobilization for that matter, is really like or is going to be like," Smithey said.&lt;br/&gt;However, while acknowledging that the full picture of student activism has yet to come into focus, Smithey expressed cautious optimism at the ability of the student body and the Swarthmore community at large to address these needs in an intersectional, multidimensional way.&lt;br/&gt;"I do recall being impressed during that first organizing meeting at what seemed to be a real willingness among the students there to work in cooperation with one another across different groups and different interests and different concerns. That will take careful work - to continue with that kind of strategic care - and I think it will be really interesting to see if we can sustain that."&lt;br/&gt;In the final weeks of the semester, the work of student organizers will continue to include, among other endeavors, phone banking against the construction of the Dakota Access Pipeline and the state-sponsored violence against the Standing Rock Sioux Tribe, a solidarity march through the town of Swarthmore, and, no matter what the decision of the Board of Managers, the realization of a Sanctuary Campus at the college. Thus, while it remains to be seen how student organizing will adjust and respond to the impending presidential administration, the current climate of activism shows no signs of cooling in the immediate future.</t>
         </is>
+      </c>
+      <c r="L83" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -4069,10 +4325,13 @@
           <t>White supremacy (Against)</t>
         </is>
       </c>
-      <c r="J84" t="inlineStr">
+      <c r="K84" t="inlineStr">
         <is>
           <t>In the wake of the presidential election earlier this month, student organizing and activism on campus has swelled to address the concerns brought about by the proposed policies of the president-elect.&lt;br/&gt;On Nov. 15, over 100 students crowded into the Scheuer Room for the first of two interest meetings dedicated to coalition building and strategizing about avenues for action both on campus and beyond. The second of these meetings took place two days after the first. The organizers of the meeting, Priya Dieterich '18 and Aru Shiney-Ajay '20, hoped that these gatherings would provide a space to effectively channel the fervor for action that has grown within the student body in recent weeks and generate ideas about how to fortify the college community for the coming years.&lt;br/&gt;"Aru and I independently had the idea of holding a meeting to connect different students who want to organize.  When I found out about her meeting, we joined forces and co-facilitated these two meetings.  I have seen and heard about - and personally felt - so much anger, frustration, and energy in the last week or so, and I wanted to help us collectively make the step towards concrete action," Dieterich said.&lt;br/&gt;In her description of the event on Facebook, Shiney-Ajay emphasized the intersectional focus of the meeting and the diverse motivations that brought students into that space.&lt;br/&gt;"People from vastly different political and personal backgrounds stand against Trump - from groups focused on identity to groups focused on party politics. In order to effectively organize, we must, at least, be aware of various efforts. Tactical disagreement is encouraged," she wrote.&lt;br/&gt;A brainstorming session among the entire group was followed by small-group discussions in which more concrete action plans were formulated. Topics raised in these discussions included an increased institutional support for college staff, a student-led course derived from reading lists released by Black Lives Matter and the Standing Rock Sioux Tribe, a renewed campaign for fossil fuel divestment, and a social justice academic distribution requirement.&lt;br/&gt;"A lot of really great ideas were brought up at the meetings: [ideas] about how we can organize both on campus and off, about how to leverage our power and privilege as students, about how to responsibly and respectfully plug into existing activist work in our communities, about how to honor our commitments to social justice as an institution," Dieterich said.&lt;br/&gt;Among the plans voiced at the Nov. 15 meeting was a school-wide walkout scheduled for Wednesday, Nov. 17 at noon. Swarthmore joined over 80 other colleges across the country in campus-wide walkouts, which were organized by students in coordination with Movimiento Cosecha, a nonviolent movement dedicated to protecting the rights of immigrant populations in the United States.&lt;br/&gt;At Swarthmore on Wednesday, hundreds of students gathered in front of Parrish Hall to demand that the college become a Sanctuary Campus, thereby providing institutional support to undocumented community members. The specific stipulations of a Sanctuary Campus include measures such as a special advisor for undocumented students, financial support for legal procedures that undocumented students may need to undergo, and a commitment to protecting undocumented community members from law enforcement officials such as U.S. Immigrations and Customs Enforcement.&lt;br/&gt;Just after noon, in front of an audience of students, faculty, staff, and other community members, Jordan Reyes '19 led the group in chants and served as a sort of moderator for the student speakers at the event, all of whom drew upon personal experiences as undocumented or Latinx people whose security is directly endangered by the Trump administration.&lt;br/&gt;"This event was, more than anything, a showing of solidarity and support for any group that may be targeted in the coming months and years, more specifically the Latinx community and undocumented students," Reyes said, following the event.&lt;br/&gt;Wednesday's walkout was just one of a series of actions that students have undertaken to pressure the college to become a Sanctuary Campus.&lt;br/&gt;Killian McGinnis '19 was responsible for drafting the petition for a Sanctuary Campus that has, at the point of publication, garnered nearly 2,000 signatures from students, faculty, staff, alumni, and other community members. The petition will be presented to the Board of Managers at their upcoming meeting this Saturday, Dec. 2.&lt;br/&gt;McGinnis says that the she is hopeful about the prospect of a Sanctuary Campus at Swarthmore.&lt;br/&gt;"Students, faculty members, and administrators alike have devoted time and collaborative energy to thinking critically about what it would mean to make Swarthmore a Sanctuary Campus, and I would be surprised and disappointed if the Board's decision didn't reflect the widespread community support of the initiative," said McGinnis.&lt;br/&gt;In addition to creating the petition, McGinnis has been collaborating with a group of students who identify as undocumented and Latinx, co-led by Miguel Gutierrez '18 and Ivan Lomeli '19,&lt;br/&gt;to formulate a faculty resolution to support the movement for a Sanctuary Campus. According to Lomeli, this resolution outlines the ways in which members of the faculty and staff at the college can continue to support the undocumented student population.&lt;br/&gt;Lomeli underscored that the effort to make the college a Sanctuary Campus is critical to alleviate the acute threat that a Trump administration will pose to undocumented students, specifically pointing to the vulnerability of students who are protected by Presidents Barack Obama's Deferred Action for Childhood Arrivals, which President-elect Trump has denounced as an unconstitutional overreach of executive power, and which he has publicly promised to overturn. DACA allows undocumented young people who entered the U.S. before the age of 16 to obtain a protected status, work permit, and social security number for two years at a time after a lengthy application process that costs $465 and is most often underwent without an attorney.&lt;br/&gt;"The undocumented population on campus, of which most but not all, benefit from DACA, worried about what would happen if their benefits were taken away. Many, including myself, were discouraged from studying abroad to prevent being stuck outside of the country in case DACA was removed," Lomeli said.&lt;br/&gt;Furthermore, DACA impacts a student's life beyond their tenure at the college. Lomeli pointed out that, were DACA to be repealed, its beneficiaries would no longer be able to work legally in the United States.&lt;br/&gt;"The list of workplaces that sponsor employees to citizenship is very small and not at all promising," he said.&lt;br/&gt;Lomeli stressed that the walkout, the petition, and the faculty resolution affirmed a feeling of support and solidarity from the college that was much appreciated, and he, like McGinnis, hoped that this support would translate into a formal decision by the Board of Managers on Saturday.&lt;br/&gt;"The faculty and staff, along with the many people whose energy and hope have been put into this Sanctuary Campus movement, await the response of the Board of Managers. If the Board of Managers chooses to ignore our plea, it will have to silence more than just the undocumented students on campus as there is a community standing behind us," he said.&lt;br/&gt;In addition to the movement for a Sanctuary Campus, a diverse array of student groups on campus have organized other solidarity actions in direct response to the presidential election and in support of those who will be most affected by the election.&lt;br/&gt;In one such display of solidarity, students and several members of the administration met on Wednesday to participate in a national day of Jewish resistance declared by IfNotNow, a movement of American Jewish youth dedicated to progressive political causes. Marissa Cohen '17 and Mira Revesz '17, who organized the action, stated that it was meant to call on the Jewish establishment, the U.S. government, and any other institution claiming to represent the interests of young American Jews to prioritize human rights and dignity above all else.&lt;br/&gt;"We stood as Jewish students and allies to uphold the lesson of 'never again' for every targeted community and challenged our communal institutions to do the same. We ask these institutions to condemn Trump and Bannon and stand up against anti-Semitism and white supremacy of any kind," said Cohen and Revesz in a joint statement.&lt;br/&gt;While the spike in student mobilization is discernible to many in the college community, it is not without precedent. Professor of sociology Lee Smithey drew connections between the kind of energy he is currently witnessing to the spring of 2013, often called the "Spring of Discontent," which was also marked by heightened student mobilization and activism, saying that he sees the two periods as united by a distinct sense of fear and threat. However, Smithey was careful to note that the stakes and the particular political conditions of the two periods are markedly different.&lt;br/&gt;"The presidential election is a much higher profile, really world-historical event, so the concern and even fear among many people is more widespread. It has stirred concerns about student experiences as well as larger national political concerns. President-elect Trump's rhetoric about ending DACA, for example, has brought these worlds together: our daily life at the college and national politics," Smithey said.&lt;br/&gt;Smithey also emphasized that this period of student organizing in the face of the election is still in its infancy, and will likely evolve to meet the urgent needs and concerns of that will become more apparent as Donald Trump takes office.&lt;br/&gt;"It feels a little early to characterize what student mobilization, or faculty or staff mobilization for that matter, is really like or is going to be like," Smithey said.&lt;br/&gt;However, while acknowledging that the full picture of student activism has yet to come into focus, Smithey expressed cautious optimism at the ability of the student body and the Swarthmore community at large to address these needs in an intersectional, multidimensional way.&lt;br/&gt;"I do recall being impressed during that first organizing meeting at what seemed to be a real willingness among the students there to work in cooperation with one another across different groups and different interests and different concerns. That will take careful work - to continue with that kind of strategic care - and I think it will be really interesting to see if we can sustain that."&lt;br/&gt;In the final weeks of the semester, the work of student organizers will continue to include, among other endeavors, phone banking against the construction of the Dakota Access Pipeline and the state-sponsored violence against the Standing Rock Sioux Tribe, a solidarity march through the town of Swarthmore, and, no matter what the decision of the Board of Managers, the realization of a Sanctuary Campus at the college. Thus, while it remains to be seen how student organizing will adjust and respond to the impending presidential administration, the current climate of activism shows no signs of cooling in the immediate future.</t>
         </is>
+      </c>
+      <c r="L84" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -4117,10 +4376,13 @@
           <t>Indigenous issues</t>
         </is>
       </c>
-      <c r="J85" t="inlineStr">
+      <c r="K85" t="inlineStr">
         <is>
           <t>A group of students and community members gathered on the UA Mall on Feb. 10, chanting "water is life," to demand the UA divest from Wells Fargo bank, a financier of the Dakota Access Pipeline.&lt;br/&gt;"Today we are announcing the launch of a campaign to get the UA to divest from Wells Fargo, to end its contract and end its relationship," said Magdalena Rios, a member of the Chukson/Tucson Water Protectors.&lt;br/&gt;The campaign, which will involve marches, rallies and teach-ins, plans to show solidarity with members of the Standing Rock Indian Reservation and pressure the Arizona Board of Regents and the UA to end relationships will all organizations supporting damaging projects such as the Dakota Access Pipeline.&lt;br/&gt;"Water is life for all of us, and the sovereign rights of Native Americans have been violated, and when their rights are violated mine and your rights are violated," said Najima Rainey, a representative of Tucson's Black Lives Matter.&lt;br/&gt;Rainey told the crowd the future will need water more than corporations or corporate interests and demanded the UA take a stand.&lt;br/&gt;RELATED: Hundreds rally in Tucson in support of Oak Flat&lt;br/&gt;"This isn't just an institution for people to learn something and leave to get a job," Rainey said. "This is a place where we shape young people to mean something and bring something into this world."&lt;br/&gt;According to Rainey, no university should conduct businesses with institutions who have forgotten we are all human beings.&lt;br/&gt;The protests come in response to two recent executive orders signed by President Donald Trump, which grant approval for the construction of the Dakota Access and Keystone XL oil pipelines.&lt;br/&gt;The orders directly contrast efforts by former President Barack Obama to halt construction of the pipelines in coordination with massive public dissent against the pipelines.&lt;br/&gt;Protesters have renewed their efforts to amplify the voice of their concern following statements made by Trump on Tuesday, Feb. 7, that he neither believes the pipelines are controversial, nor has he received phone calls condemning the pipeline.&lt;br/&gt;Sal Amdor, Tucson Water Protector, protests with other organizers against the Dakota Access Pipeline on the UA campus on Feb 2. Several political groups met to hold a press conference and to protest Wells Fargo in solidarity with the Dakota Access Pipeline protest.&lt;br/&gt;State Rep. Sally Ann Gonzales, D-Tucson, told the crowd, "I stand here with you to continue the fight because this fight is important."&lt;br/&gt;Gonzales wants to fight for clean air and water in order to secure the future for her children and her community.&lt;br/&gt;"It is the greed that money brings to people that make them think they are allowed to do this to anybody here in the United States," Gonzales said of the pipeline.&lt;br/&gt;She plans to continue to fight for the rights of indigenous communities and all Arizonans at the state legislature.&lt;br/&gt;"Are you devoted to your students, the future of this country, or are you devoted to money and just the ones who can pay?" Rios asked the UA.&lt;br/&gt;RELATED: UA students walk out in protest of President Trump's climate change vision&lt;br/&gt;Rios remains devoted to organizing a fight against the Dakota Access Pipeline on the UA campus and believes the cause will succeed no matter how long it takes because water does not know time.&lt;br/&gt;Michelle Cook, a UA alumna from the Gender and Women's studies program, travelled to the protest site at Standing Rock in North Dakota. She said the UA prides itself on being one of the first institutions to offer a program focused on Native American studies.&lt;br/&gt;"Now, is the university going to contribute to the destruction of indigenous people by funding a bank that is responsible for gross human rights violations?" Cook asked.&lt;br/&gt;Cook described images of individuals covered in bite marks from dogs from her time protesting the pipeline in North Dakota.&lt;br/&gt;Robert Mclane protests on the UA campus on Feb. 2 against the Dakota Access Pipeline. Several political groups met to hold a press conference and to protest Wells Fargo in solidarity with the Dakota Access Pipeline protest.&lt;br/&gt;Cook called on everyone on the mall to join the resistance and cut off the money funding projects endangering the environment and violating the rights of indigenous communities.&lt;br/&gt;The UA also has a relationship with Bank of America, another financier of the Dakota Access Pipeline. JPMorgan Chase, Citi Bank, and 14 other banks provided capital for the Dakota Access Pipeline.&lt;br/&gt;The Seattle City Council recently voted to divest from Wells Fargo over Dakota Access Pipeline concerns. Rios demanded UA do the same and put human beings before their financial relationships.&lt;br/&gt;Follow Randall Eck on Twitter.</t>
         </is>
+      </c>
+      <c r="L85" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -4160,10 +4422,13 @@
           <t>Trump and/or his administration (Against)</t>
         </is>
       </c>
-      <c r="J86" t="inlineStr">
+      <c r="K86" t="inlineStr">
         <is>
           <t>For the past several months, protestors have been gathering at the Standing Rock Indian Reservation in North Dakota to oppose the construction of a segment of the Dakota Access Pipeline. This segment would threaten the safety of the tribe's waters and destroy burial sites sacred to the Standing Rock Sioux. Unarmed water protectors at the site faced brutal treatment by law enforcement, especially in recent weeks. As temperatures dropped below freezing, law enforcement blocked road access and threatened to arrest newcomers in an attempt to prevent supplies and warm weather gear from reaching the protestors.&lt;br/&gt;The Standing Rock protests demonstrate the remarkable power of protest to change the course of policy. Refusing to bow to the government's attempts to remove them from the site of the pipeline construction, the water protectors won a victory: the Army Corps of Engineers will not grant the final permit necessary to build through the reservation, although they do plan to reroute it through another area of North Dakota. Despite the continued threat to their lands and water, the Standing Rock protestors served as an excellent example of the efficacy of nonviolent resistance, when aimed towards accomplishing an explicit goal.&lt;br/&gt;Since the election of Donald Trump to the Presidency of the United States, many more protests have erupted all over the country. Yet, these acts of resistance have noticeably lacked the kind of clear objective characterized by the Standing Rock protests, and instead seem intended to comfort the protestors themselves, who feel obligated to take some form of action. While this sort of self-affirming protest can occasionally help to build community and foster solidarity after a crisis, ultimately, the purpose of a protest should be to accomplish some concrete change.&lt;br/&gt;The day after the 2016 election, the Colorado College community organized a protest intended to affirm our love, unity, and solidarity. Through it began as an on-campus rally, the protest soon transitioned into a full-blown march, with students blocking traffic on a busy midday Nevada Ave. Although we who participated in the march, myself included, felt powerful and empowered as we shouted messages of love and strength, the drivers we obstructed certainly were not feeling the love we claimed to profess. Instead of starting a conversation with the politically diverse city in which we find ourselves, we shouted our own truth at the top of our lungs. It felt good, but nobody was listening. And nobody had a reason to listen - we weren't asking for anything. We merely wanted to feel that ask a group, we were acting.&lt;br/&gt;A protest needs a purpose if it wants to accomplish anything positive outside of in-group solidarity. The purpose of the protests at Standing Rock was to halt the construction of the Dakota Access Pipeline, and it has succeeded, for now. The purpose of the protests at CC, on the other hand, was ambiguous at best. If the purpose was to spread a message of love and acceptance into Colorado Springs, it may have succeeded for the Palmer High School students who joined the march. However, it certainly did not for the driver screaming, "Please just let me get home to my children!" as I and other protestors swarmed in front of her car on Nevada Ave. If the purpose of the protest was to somehow impact the results of the election, it failed. But if the purpose was to make the participating CC students feel like they had accomplished something, had taken some sort of direct action rather that just sitting back and letting the results of this election pass unmarked, then it undoubtedly succeeded.&lt;br/&gt;Maybe that feeling of accomplishment was necessary for us at the time. Our participation among the larger movement of post-election college protests certainly caught the attention of the media. But there are only so many self-affirming protests we can hold before we begin to embody that worst of millennial stereotypes: wanting acknowledgement without achievement. If we are going to parade down to City Hall, we need to be asking for something, trying to accomplish something. It is not enough for us to merely make our presence known. When they ask, "Okay, I see you, so what?" we need to have an answer ready. An answer like, "So make Colorado Springs a sanctuary city." "So pledge not to revoke the rights granted to the LGBTQ community." "So set goals for carbon neutrality and invest more in renewable energy for the city." It doesn't matter what we choose for our answer, but we must have one if we want to be taken seriously. We need to set an attainable goal, and we need to invite our fellow Colorado Springs residents to join us, not alienate them.&lt;br/&gt;Are we trying to start a movement? If so, we need a direction. Just like the water protectors at Standing Rock, we have the power to create change with our action, but only if we decide what we want that change to be. We can ask our college to divest from fossil fuels, to commit to being a sanctuary school, or to take more seriously charges of sexual assault and other forms of harassment. We can ask the same of our city. This means we cannot just protest to protest, march to march, act to say that we have acted. We must ask for change, and protest with a purpose.</t>
         </is>
+      </c>
+      <c r="L86" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -4203,10 +4468,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J87" t="inlineStr">
+      <c r="K87" t="inlineStr">
         <is>
           <t xml:space="preserve">The Mizzou Energy Action Coalition will be presenting its campaign for the UM System to divest from fossil fuels to President Mun Choi on May 3.&lt;br/&gt;The divestment resolution that passed unanimously in joint session calls for the UM System to "pursue total divestment of fossil fuel stock by 2020." The University of Missouri currently has $10 million invested in fossil fuel stock and 45 companies. The MU System Endowment is $1.4 billion, and the resolution calls for 0.8 percent of the total endowment to be divested.&lt;br/&gt;MU Chief Communication Officer John Fougere said in an email he is proud MU is a national leader in matters of environmental sustainability, but "it would be nearly impossible to function as an institution or as a society without the energy provided by fossil fuels."&lt;br/&gt;MEAC, previously called Coal Free Mizzou, successfully petitioned to the UM System Board of Curators in 2013 to switch MU's primary energy source from the coal-burning power plant to renewable energy, a petition that was supported by 3,000 signatures. However, Fougere believes fossil fuels are too crucial to campus for the UM System to divest from.&lt;br/&gt;"The dependency on energy provided by fossil fuels will continue to exist for some time, and it is our belief that disengaging from a large segment of the world economy is not in the best interests of the UM System," Fougere said.&lt;br/&gt;The divestment targets the Endowment Pool, which is not used to buy energy nor run the power plant or for any university operations. The Endowment Pool is invested in both publicly and privately traded stocks and bonds, including investments in fossil fuel companies.If the money gets divested, the MEAC has no suggestions as to which other companies the Endowment Pool would invest in.&lt;br/&gt;"Directly, [the divestment] has nothing to do with our power plant," MEAC president Frankie Hawkins said. "So by 'divesting from fossil fuels,' the university is agreeing to sell its stock in fossil fuel companies and invest in other companies."&lt;br/&gt;At least $3.5 million of the MU System investment is in companies regarded by The Carbon Underground, an environmental organization, as some of top carbon emitters and most environmentally hazardous companies in history, including Gazprom Neft, one of Russia's largest oil producers and distributors, and CNOOC. This resolution, if accepted by Board of Curators, would make MU one of 16 schools to commit to divestment.&lt;br/&gt;"This movement shows student solidarity with other larger movements of social justice," Hawkins said. "It draws attention to the threat of climate change. We want to send a signal to fossil fuel companies that we are not in favor of cooking the earth five times over."&lt;br/&gt;The Missouri Energy Action Coalition, founded in 2008, presented its divestment movement initiative to Missouri Students Association April 12, and the resolution was passed in that night's full Senate with an 18-6 vote. MEAC representatives met with UM System Curator Steelman and said he showed positive reception to this divestment. MEAC originally began its divestment campaign in 2013.&lt;br/&gt;Hawkins said, with the support of joint session, their organization is taking the divestment proposal to a meeting with President Choi and UM System officials next week. On April 18, MEAC began a petition through change.org to get donations and a goal of 500 student signatures; the organization currently has 291.&lt;br/&gt;"A unanimous vote from joint session took my breath away," Hawkins said. "Going forward, it's great to know we have the student body behind us. We have proof to bring to President Choi and UM System officials that people care."&lt;br/&gt;Joint session is composed of 11 student governments on campus. Each government receives one vote on joint session legislation.&lt;br/&gt;The MEAC hosted a rally for "fossil fuels and climate injustice" on April 29 in Middlebush Auditorium. Many members of the community gathered for the rally which featured music, poetry from OneMic, various activists and speakers.&lt;br/&gt;"Our planet is being threatened by corporations and governments," MU senior and environmental activist Mallory Brown said. "We need to work for justice. It's important to ask if we are we doing our best to commit to environmental justices in our community."&lt;br/&gt;Activists and residents spoke on the increasing issue of climate change, specifically in this political climate, as well as environmental action. Hawkins spoke at the rally and encouraged residents of Columbia to sign the petition and get involved in the movement on campus.&lt;br/&gt;"I've signed MEAC's petition because it's an important thing," MU sophomore Rachel Peterson said. "It's a really good way for our university to demonstrate that we are not about climate change or fossil fuels."&lt;br/&gt;Edited by Sarah Hallam | </t>
         </is>
+      </c>
+      <c r="L87" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -4241,10 +4509,13 @@
           <t>University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J88" t="inlineStr">
+      <c r="K88" t="inlineStr">
         <is>
           <t>National and sometimes international political movements often find homes on college campuses, but lately, students are aiming their protest signs at their own universities.&lt;br/&gt;Students at Davidson College, a private, liberal arts college in North Carolina, began circulating a digital petition late last month calling for more access to their board. Their main demand is for at least 20 percent of Davidson's 45-person board to attend twice-annual town halls open to students. A similar movement at Salem College, a women's college in North Carolina, is calling for board members to participate in mandatory diversity training.&lt;br/&gt;Neither of these events exists in isolation, either. In a growing trend across the country, students are demanding greater access to members of their university's board of trustees, as opposed to going through channels such as deans and professors to relay messages. Although we've seen a plethora of student activism and involvement in many important issues this semester, we're missing a similar shift at Pitt.&lt;br/&gt;While there are certainly issues with Pitt's board - namely, a lack of diversity of thought, as we've noted in past editorials - we can't criticize it too harshly for failing to take student concerns into consideration because the student groups actively working to lobby the board are few and far between.&lt;br/&gt;And we're doubtful the reasons behind this are due to a lack of frustrated or disgruntled Pitt students who feel like the administration doesn't listen to them. With students facing issues from education funding to diversity and inclusion to rising student debt, it's probably quite the opposite.&lt;br/&gt;While the chancellor is the one tasked with dealing with the administrative, academic and management authorities of the University, the board holds the ultimate power over all University affairs. If students want to lobby an issue of relatively minor consequence, they're probably better off going through Student Government Board or the dean's office. More substantial issues, especially ones dealing with the economics or finances of the University - such as concerns about tuition and student loans, adjunct professors or minimum wage for University workers and employees - is where the Board would most likely come in.&lt;br/&gt;There are student groups who have made effective changes, or attempts, when it comes to lobbying and working with the board at Pitt. No Sweat: Pitt Coalition Against Sweatshops - a conglomerate of student organizations committed to banning sweatshops worldwide - was the last group to garner substantial success with the board. Pitt began requiring its apparel licensees to sign documents agreeing not to manufacture products in unsafe working environments in 2014, after a year of student push on the matter.&lt;br/&gt;Pitt's Fossil Free Coalition - a similar conglomeration of more than 35 student groups pushing for Pitt to divest from the fossil fuel industry - is the only recent example of a student group making any progress with the board. The push for faculty and graduate student unions have likewise garnered support and interest at an administrative level, but other than these select groups, few students have taken advantage of channels that could lead directly to institutional change.&lt;br/&gt;Even if you're not interested in initiating change at Pitt, you should still know what's going on with the group of people running the University - transparency is an issue we should all rally behind.&lt;br/&gt;And there's a lot of confusion about how change actually happens at a university. Maybe it's because students don't know how the board actually works or what it does. So let us tell you:&lt;br/&gt;First of all, while the board has a lot of power, it also has a lot of restraints. Rarely do trustees get involved in Pitt's day to day.&lt;br/&gt;Next, the board doesn't make most of its decisions based on morality - it's literally a line written into its constitution. The board can, however, vote to go against that code in extreme circumstances. In the 1980s, for example, the board voted to divest from companies that were aiding apartheid in South Africa.&lt;br/&gt;So, if you're going to lobby to the board, do your research. Come with the numbers crunched, ready to show the higher-ups that there's an economic imperative for whatever change it is that you want. Or, be willing to make a really insightful argument about the ethical implications of the issue you're trying to bring to light.&lt;br/&gt;The board is made up of 36 voting members, including 12 commonwealth, 17 term, six alumni trustees and the Chancellor. Additionally, there are 12 special and numerous emeritus members of the board who have all the same rights of any board member except the right to vote.&lt;br/&gt;The Alumni Association nominates those to be elected as alumni trustees, and the commonwealth trustees are nominated by the state governor, the President Pro Tempore of the state Senate and the Speaker of the state House. And the governor, the Secretary of Education of the Commonwealth and the mayor of Pittsburgh all serve as nonvoting members on the board as well.&lt;br/&gt;So if you want to start at the most basic level of lobbying, all the individual names of both voting and nonvoting members of the board can be found online. But if you're unable to contact these members personally, the nomination process for each of them presents a clear path where students can insert their input as well through the Alumni Association or through the mayor or governor's office. Even though they don't vote, they still have the power to speak to the Board members at meetings.&lt;br/&gt;The board holds at least three meetings, including the annual meeting, each year. These meetings are open for public viewing but not public comments. If you want to speak with board members, you typically have to wait until after the meeting is over.&lt;br/&gt;Since most board members are hard for students to reach, perhaps the most effective way to communicate with the board is through Chancellor Gallagher, since he serves "as the representative of the students, staff, faculty, and administration to the board" - although he's been known to say otherwise. But Gallagher doesn't meet with students very often, so your cause would need to have garnered a significant amount of support already in order to catch his attention. If it hasn't, going through someone else in his office - such as Dean of Students Kenyon Bonner or Vice Chancellor Kathy Humphrey - is likely the next best option.&lt;br/&gt;Student Government Board, the student group on campus with the most power to lobby the Chancellor and the board for what students wants, began holding monthly town-hall-style meetings, in addition to their weekly meetings, this semester. The town halls were supposed to be an avenue for more Pitt students to voice concerns to SGB, but they've garnered starkingly low turnout rates.&lt;br/&gt;Next year, this should change. Standing on street corners yelling at passing cars is fine, but if you're looking to enact change at the university level, go to the people who can make that happen.&lt;br/&gt;Pitt students who feel underrepresented should look to Davidson and Salem as prime examples of what students can do to actively push the administration for change.&lt;br/&gt;We won't know if the board is willing to listen unless we start talking.</t>
         </is>
+      </c>
+      <c r="L88" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -4289,10 +4560,13 @@
           <t>Immigration (For)</t>
         </is>
       </c>
-      <c r="J89" t="inlineStr">
+      <c r="K89" t="inlineStr">
         <is>
           <t>As University of Wisconsin rang in the new year and kickstarted yet another semester, students witnessed the passage of a historic divestment resolution, one of the largest women's rights marches nationwide and the "alt-right" movements' introduction, and disappearance, from campus.&lt;br/&gt;The Badger Herald news team recounts these events and more in a recap of the biggest stories from this semester.&lt;br/&gt;Campus&lt;br/&gt;Adding to the tense racial climate President Donald Trump's election created, one University of Wisconsin student made moves to bring the "alt-right" movement to campus to advocate against what he described as "anti-white racism."&lt;br/&gt;The "alt-right" is a movement based on right-wing ideology and white identity that aims to reject political correctness. UW student Daniel Dropik began a club promoting the movement on campus late January. His club has been described as a "political and racial advocacy student club promoting Western European American students and traditional values."&lt;br/&gt;Dropik has a criminal record for racially motivated arson from about a decade ago. But he said his group was about making people feel welcome on campus, not about hate.&lt;br/&gt;"We want to support students who have been harassed and heckled for having beliefs which challenge academic orthodoxy of race and other topics on this campus," Dropik said in an email to The Badger Herald.&lt;br/&gt;UW student wants to bring alt-right movement to campusLooking down at the small piece of paper that barely fit between his thumb and index finger, two phrases glared Read...&lt;br/&gt;The "alt-right" has frequently been characterized as a neo-Nazi movement, with the Anti-Defamation League citing it as a hate group. Both liberal and conservative groups on campus openly denounced the movement, stating they support free speech but not what Dropik is promoting.&lt;br/&gt;Conservative, liberal student organizations denounce 'alt-right' movementIn a moment of unity on the University of Wisconsin campus, student organizations from both the liberal and conservative camps have Read...&lt;br/&gt;But Dropik said his group is not motivated by hate. Both white and nonwhite students have been interested in joining UW alt-right, he said.&lt;br/&gt;In a statement, UW Chancellor Rebecca Blank said the possibility of this type of activity on campus is "concerning." But she said it was not illegal for Dropik to hand out political information and express objectionable, even hateful, viewpoints.&lt;br/&gt;Approximately 70 students protested the "alt-right" on Bascom Hill in January, calling on their peers to fight against white supremacy. They interrupted a shared governance meeting where Blank was present and demanded she take action against it. Though Blank stated several times Dropik's words and actions are "personally offensive," she stood firm in her conviction that unless violence is directly incited, he is allowed to speak freely.&lt;br/&gt;UW students protest 'alt-right,' call on chancellor to condemn hate speechOne week after a University of Wisconsin student attempted to start an "alt-right" group on campus, students and community members Read...&lt;br/&gt;Associated Students of Madison also called out Blank to label the group as a white supremacy group.&lt;br/&gt;Blank said she will ask the UW System Board of Regents to review their admissions policy, which does not allow universities to review a student's criminal history, in light of Dropik's past crimes.&lt;br/&gt;Blank stands her ground on confronting 'alt-right' movementUniversity of Wisconsin Chancellor Rebecca Blank's appearance at a Tuesday shared governance meeting was met with protests against white supremacy Read...&lt;br/&gt;After facing strong opposition from the student body and administration, Dropik dropped his plans to start a chapter of the American Freedom Party on campus in early February.&lt;br/&gt;ASM unanimously votes to divest despite UW administration disapproval&lt;br/&gt;Associated Students of Madison proposed and passed a resolution for the University of Wisconsin to divest from corporations complicit in alleged human rights violations in late March.&lt;br/&gt;In a March 29 meeting, more than 60 students spoke at an ASM open forum about the resolution. The students who spoke in favor of the resolution said it would bring more transparency to the UW Foundation and the student body, and take away funds from corporations that profit off human rights abuses.&lt;br/&gt;Those who spoke in opposition said the resolution was too similar to the Boycott, Divest, Sanction movement, which asks entities to withdraw support from Israel and Israeli companies.&lt;br/&gt;ASM indefinitely postpones divestment resolution after hours of heated debateAfter six hours of heated debate, the University of Wisconsin Associated Students of Madison voted 13-12-1 to postpone a resolution demanding the Read...&lt;br/&gt;In six hours of heated debate, the legislation was tabled indefinitely in a 13-12-1 vote.&lt;br/&gt;But in an April 26 ASM meeting, the legislation was brought up again, this time without some of the more contentious previsions. ASM representatives cut down the legislation from its original 13 pages to one to appease the opposition's requests.&lt;br/&gt;Representatives from Badgers United Against Hate said they were pleased with how ASM took Israeli and Jewish students concerns into consideration with the new legislation.&lt;br/&gt;Others said the updated resolution was "watered down" and was made for the "comfort of ... oppressors."&lt;br/&gt;ASM unanimously approves contentious divestment proposal to mixed reactions from campusAfter five hours of debate and nearly 50 people appearing before open forum, the University of Wisconsin Associated Students of Read...&lt;br/&gt;After the open forum ended, ASM representatives added new amendments to reflect the resolution proposed in the March 29 meeting. The amendments named specific Israeli companies, prompting two members of ASM to leave.&lt;br/&gt;The updated resolution, now four pages, was passed in a 24-0-2 vote.&lt;br/&gt;In a statement, Chancellor Blank said the university will not divest from corporations, citing ASM doesn't control UW. The statement said UW was concerned with how ASM handled the issue, saying it was "undemocratic" and "not transparent."&lt;br/&gt;Amid backlash, Walker introduces proposal to opt out of segregated fees&lt;br/&gt;Gov. Scott Walker's contentious proposal to allow students to decide whether or not to pay segregated fees to fund certain student organizations reached a temporary resolution in April.&lt;br/&gt;Walker and other Republican supporters of the opt-out proposal said it would cut costs for families struggling to pay for college. But ASM and a host of student organizations said it would throw funding for necessary student services into question.&lt;br/&gt;The Joint Finance Committee determined the opt-out was a nonfiscal item, and therefore could not be included in the governor's state budget. But the issue could potentially re-emerge if a state legislator introduces it as an individual bill separate from the budget.&lt;br/&gt;Joint Finance Committee eliminates proposal allowing students to opt out of segregated feesFollowing much backlash from students throughout the University of Wisconsin System about the possibility of being able to opt out of allocable Read...&lt;br/&gt;The Associated Students of Madison and other students quickly responded to the opt out prevision when Walker proposed it in February. ASM is responsible for allocating student fee dollars at the University of Wisconsin.&lt;br/&gt;Students throughout the UW System came together to pass a resolution opposing the opt out, with representatives from 18 UW campuses participating in the vote.&lt;br/&gt;"I am glad that we all are united on fighting for our campuses and the UW System," ASM Chair Carmen Goséy said. "ASM always tries to best represent our student voices and we're excited to move forward with our efforts."&lt;br/&gt;UW System representatives express opposition to allocable fee opt-out proposalStudent representatives from across the UW System passed a resolution Monday expressing opposition to Gov. Scott Walker's proposal to make allocable Read...&lt;br/&gt;UW Dean of Students Lori Berquam also urged JFC to remove the provision, saying it would have had a "significant impact" on important services and programs like transportation, health care and veteran support.&lt;br/&gt;Student groups unite in effort to oppose contentious budget proposalUniversity of Wisconsin students considered what a future with reduced segregated fees would look like in light of a proposal Read...&lt;br/&gt;City&lt;br/&gt;Tony Robinson's family receives historic $3.35 million settlementAlmost two years after a white Madison police officer shot biracial 19-year-old Tony Robinson, his family received a federal civil rights settlement of $3.35 million.&lt;br/&gt;The settlement was the highest amount paid in state history for an officer-related shooting.&lt;br/&gt;But Kenny was cleared of any wrongdoing by Dane County District Attorney Ismael Ozanne. After an internal investigation, MPD also found Kenny had acted within the department's code of conduct.&lt;br/&gt;Tony Robinson's family reaches record $3.35 million settlement for fatal shootingNearly two years after the fatal shooting of 19-year-old Tony Robinson, his family has finally settled a $3.35 million federal Read...&lt;br/&gt;The police department said it found the settlement "outrageous" because Kenny "did [his] job in accordance with their training and the law."&lt;br/&gt;MPD also said the settlement was likely to hurt its morale.&lt;br/&gt;Despite the settlement being the largest in state history, Robinson's family still feels a void from their loss.&lt;br/&gt;Despite historically large settlement, family still 'feels void' from Tony Robinson's deathAlmost two years have passed since Madison Police Officer Matt Kenny fatally shot 19-year-old Tony Robinson Jr., and today the late teen's Read...&lt;br/&gt;For Robinson's mother said the sum of the money didn't matter. She wanted to go through with the trail, but didn't want to put her children through that process.&lt;br/&gt;Racial just group Racial Justice Tipping Point created a petition calling for MPD to fire Kenny.&lt;br/&gt;According to the petition, firing Kenny would be one step closer toward accountability for him and the department.&lt;br/&gt;Racial justice group calls for officer who shot Tony Robinson to be firedAs the two-year anniversary of Tony Robinson's death approaches, Racial Justice Tipping Point has created a petition calling for Madison Read...&lt;br/&gt;In response to the petition, MPD said the investigation was already conducted and they found Kenny acted within his rights and therefore will not fire him.&lt;br/&gt;In response to the settlement, the city of Madison has made policy changes regarding backup in policing situations, which will hopefully save lives, MPD officials said.&lt;br/&gt;Dane County paves path for immigration reform&lt;br/&gt;The year began with many federal actions regarding immigration and immense pushback from communities around the country, including Madison and Dane County.&lt;br/&gt;Dane County Executive Joe Parisi announced in February that the county would be creating an immigration assistance fund. The Dane County Board later approved a resolution in April to give the fund $150,000.&lt;br/&gt;Dane County Board carves path for undocumented immigrants hoping to become citizensAs conversation on immigration reform at the federal level intensifies, the Dane County Board of Supervisors moved forward with programs aimed Read...&lt;br/&gt;The resolution also seeks to help immigrants by reaching out to several legal service providers in the area to help develop emergency immigration assistance.&lt;br/&gt;The legal service providers will work with the Madison Community Foundation to help decide how money from the fund will be spent.&lt;br/&gt;Dane County Executive announces plan to help residents attain citizenshipDane County Executive Joe Parisi announced a two-pronged plan to help Dane County residents gain citizenship at a news conference Read...&lt;br/&gt;Sup. Jenni Dye, District 33, said many organization have spoken in favor of the resolution.&lt;br/&gt;"We don't often do thing like this," Dye said. "I'm really proud to be on a body and with my community where we can come together to do the right thing and help the people that need it."&lt;br/&gt;The board also created an amendment in March to help keep immigrants' information private.&lt;br/&gt;Dane County Board moves to amend ordinance to protect immigrant communityShortly after President Donald Trump issued a second executive order with regard to immigrant and refugee entry, the Dane County Board planned to Read...&lt;br/&gt;The amendment itself further clarified what information falls under the category of "confidential information" and says which county employees cannot disclose this information.&lt;br/&gt;"We're looking at the art of the possible - what do we have control over, how can we help, how can we meet the needs of our community?" Parisi said. "And at the same time, reflecting the values of the people who live in this community, because this isn't just about people who are immigrants who are looking for that path to citizenship."&lt;br/&gt;Dane County spearheads initiatives to help homeless&lt;br/&gt;After months of debate between the Mayor Paul Soglin and City Council over a panhandling ordinance, numerous homeless initiatives, including creation of new housing and homeless owned on-call company, are on the way.  &lt;br/&gt;Homeless Issues Committee votes against ordinance prohibiting sleeping on public sidewalksCity officials unanimously voted against a resolution prohibiting individuals from sleeping or lying down on public sidewalks during a Homeless Read...&lt;br/&gt;The Homeless Issues Committee voted against a resolution prohibiting individuals from sleeping in Central Business District Area.&lt;br/&gt;County Sup. Heidi Wegleitner, District 2, said though no lawful alternatives exist, the city needs to address homelessness in more humane ways.&lt;br/&gt;The 2017 Dane County budget also prioritized reducing homelessness by bolstering funding for existing initiatives and starting funding for new ones, totaling $2 million.     &lt;br/&gt;Parisi prioritizes homelessness, opioid epidemic in 2017 budgetWith a focus on investing in the county's future, Dane County Executive Joe Parisi announced several expansions in social services Read...&lt;br/&gt;In a joint project between the city and county, $3 million will be used to develop a single-housing unit complex and affordable housing.&lt;br/&gt;Dane County Board votes to expand housing for homelessIn an effort to expand affordable housing for low-income families in Madison, the Dane County Board approved a resolution Thursday to Read...&lt;br/&gt;Madison residents also established initiatives to employ more homeless people. Resident Henry Johnson started the Homeless Entrepreneurship Initiative to hire homeless people for jobs ranging from moving to hauling scrap metal.&lt;br/&gt;Madison resident begins initiative to help city's homeless empower themselvesMadison resident Henry Johnson found that as a homeless man for nearly three years, there are few resources to help Read...&lt;br/&gt;State&lt;br/&gt;Legislators move to legalize lifesaving CBD oil&lt;br/&gt;Gov. Scott Walker signed a mostly bipartisan bill legalizing a cannabis oil extract in April.&lt;br/&gt;CBD oil has been effective at treating various seizure-causing illnesses. Several families spoke at a public hearing about the need for their children to have CBD oil to help with their seizures.&lt;br/&gt;A Wisconsin grandmother said her 2-year-old granddaughter suffers from seizures. The grandmother said she has to go to another state to purchase CBD oil and bring it back to Wisconsin.&lt;br/&gt;Rep. Scott Krug, R-Wisconsin Rapids, who co-authored the bill, discussed the need for this legislation in Wisconsin at a news conference in March.&lt;br/&gt;Assembly passes bill to legalize possession of medical marijuana extractAfter passing the Wisconsin state Senate, the Assembly unanimously voted 98-0 to legalize the possession of a medical marijuana extract oil. Read...&lt;br/&gt;"As we move forward with the CBD issues in the state of Wisconsin, for me, it's bittersweet because we've seen hundreds of families come through and talk to us about the need for a bill that works and is effective and now we're able to deliver," Krug said.&lt;br/&gt;The legislation includes a 30-day provision to help avoid problems with the U.S. Drug Enforcement Agency's classification of CBD oil as a Schedule 1 drug. The provision makes it so if the federal government changes CBD's classification, Wisconsin will follow suit in 30 days.&lt;br/&gt;Wisconsin families continue emotional fight in push for medical marijuana extract billThe sound of people holding back tears peppered a public hearing in the State Capitol Wednesday as legislators considered a Read...&lt;br/&gt;Assembly Speaker Robin Vos, R-Rochester, praised the bipartisan support of this legislation at the March news conference.&lt;br/&gt;"Today is a day that I could not be prouder to serve as the leader of the Assembly," Vos said.&lt;br/&gt;Wisconsin rallies with the world to support women&lt;br/&gt;Protesters have made their voices heard on the steps of the state Capitol for a variety of issues in the past months, but especially women's rights.&lt;br/&gt;Madison community marches in solidarity with women around the country and worldThe footsteps of women in Madison echoed those from around the world as they marched in solidarity Saturday to protest the upcoming presidency Read...&lt;br/&gt;Sporting pink hats and signs showing solidarity with women, Madisonians joined demonstrations around the world to oppose Trump's inauguration in January and again in March as part of International Women's Day.&lt;br/&gt;A Day Without Women: Madison community marches to advocate for women's rightsWomen from across the state battled strong winds atop the steps of the State Capitol building as they marched to discuss a Read...&lt;br/&gt;Madison Police Department estimated the crowd peaked at approximately 100,000 people for Madison's Women's March, which began at Library Mall. Those marching took issue with the normalization of Trump's "misogynistic behavior" and welcomed a host of local politicians urging organization and information seeking.&lt;br/&gt;As demonstrators continued to call for community control and political engagement, people from different walks of life found common ground. At the "Day Without A Woman" strike, speakers encouraged attendees to "show up" for each other.&lt;br/&gt;One speaker, Zon Muas, said her goal with the protests was to speak up on behalf of minority women.&lt;br/&gt;"It was very important that we really spoke about solidarity and unity and showing up, because a lot of time women's issues are just thought of as reproductive, but it is so much more than that," Muas said.&lt;br/&gt;Trump's immigration ban affects more than 100 students&lt;br/&gt;President Donald Trump's executive order, which suspended entry of refugees and travelers,particularly those from a host of Muslim-majority countries, impacted 115 University of Wisconsin faculty and staff in January.&lt;br/&gt;Trump executive order impacts at least 88 in UW communityUniversity of Wisconsin officials announced Monday there are 115 faculty, students and staff impacted by President Donald Trump's executive order Read...&lt;br/&gt;UW Chancellor Rebecca Blank officially added UW to the list of universities calling for Trump to reconsider the executive order.&lt;br/&gt;"These actions affect real people - researchers, scholars, students and staff - who are essential to our goals of providing a world-class education," Blank said.&lt;br/&gt;Opponents of the order, including more than 200 students of various religious backgrounds, spoke out their supports for refugees at the top of Bascom Hill.&lt;br/&gt;Executive order impacts students, faculty, researchers on campus, forcing many to speak outStanding in front of a crowd of 200, Zahiah Hammad introduced the ways President Donald Trump's executive order on immigration Read...&lt;br/&gt;The city board approved a resolution to fund the citizenship assistance services. Dane County granted $150,000 and reached out to local legal service providers such as UW Law School Immigration Justice Center and Jewish Social Services of Madison for their assistance with immigration issues.&lt;br/&gt;Dane County Board carves path for undocumented immigrants hoping to become citizensAs conversation on immigration reform at the federal level intensifies, the Dane County Board of Supervisors moved forward with programs aimed Read...</t>
         </is>
+      </c>
+      <c r="L89" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -4337,10 +4611,13 @@
           <t>White supremacy (Against)</t>
         </is>
       </c>
-      <c r="J90" t="inlineStr">
+      <c r="K90" t="inlineStr">
         <is>
           <t>As University of Wisconsin rang in the new year and kickstarted yet another semester, students witnessed the passage of a historic divestment resolution, one of the largest women's rights marches nationwide and the "alt-right" movements' introduction, and disappearance, from campus.&lt;br/&gt;The Badger Herald news team recounts these events and more in a recap of the biggest stories from this semester.&lt;br/&gt;Campus&lt;br/&gt;Adding to the tense racial climate President Donald Trump's election created, one University of Wisconsin student made moves to bring the "alt-right" movement to campus to advocate against what he described as "anti-white racism."&lt;br/&gt;The "alt-right" is a movement based on right-wing ideology and white identity that aims to reject political correctness. UW student Daniel Dropik began a club promoting the movement on campus late January. His club has been described as a "political and racial advocacy student club promoting Western European American students and traditional values."&lt;br/&gt;Dropik has a criminal record for racially motivated arson from about a decade ago. But he said his group was about making people feel welcome on campus, not about hate.&lt;br/&gt;"We want to support students who have been harassed and heckled for having beliefs which challenge academic orthodoxy of race and other topics on this campus," Dropik said in an email to The Badger Herald.&lt;br/&gt;UW student wants to bring alt-right movement to campusLooking down at the small piece of paper that barely fit between his thumb and index finger, two phrases glared Read...&lt;br/&gt;The "alt-right" has frequently been characterized as a neo-Nazi movement, with the Anti-Defamation League citing it as a hate group. Both liberal and conservative groups on campus openly denounced the movement, stating they support free speech but not what Dropik is promoting.&lt;br/&gt;Conservative, liberal student organizations denounce 'alt-right' movementIn a moment of unity on the University of Wisconsin campus, student organizations from both the liberal and conservative camps have Read...&lt;br/&gt;But Dropik said his group is not motivated by hate. Both white and nonwhite students have been interested in joining UW alt-right, he said.&lt;br/&gt;In a statement, UW Chancellor Rebecca Blank said the possibility of this type of activity on campus is "concerning." But she said it was not illegal for Dropik to hand out political information and express objectionable, even hateful, viewpoints.&lt;br/&gt;Approximately 70 students protested the "alt-right" on Bascom Hill in January, calling on their peers to fight against white supremacy. They interrupted a shared governance meeting where Blank was present and demanded she take action against it. Though Blank stated several times Dropik's words and actions are "personally offensive," she stood firm in her conviction that unless violence is directly incited, he is allowed to speak freely.&lt;br/&gt;UW students protest 'alt-right,' call on chancellor to condemn hate speechOne week after a University of Wisconsin student attempted to start an "alt-right" group on campus, students and community members Read...&lt;br/&gt;Associated Students of Madison also called out Blank to label the group as a white supremacy group.&lt;br/&gt;Blank said she will ask the UW System Board of Regents to review their admissions policy, which does not allow universities to review a student's criminal history, in light of Dropik's past crimes.&lt;br/&gt;Blank stands her ground on confronting 'alt-right' movementUniversity of Wisconsin Chancellor Rebecca Blank's appearance at a Tuesday shared governance meeting was met with protests against white supremacy Read...&lt;br/&gt;After facing strong opposition from the student body and administration, Dropik dropped his plans to start a chapter of the American Freedom Party on campus in early February.&lt;br/&gt;ASM unanimously votes to divest despite UW administration disapproval&lt;br/&gt;Associated Students of Madison proposed and passed a resolution for the University of Wisconsin to divest from corporations complicit in alleged human rights violations in late March.&lt;br/&gt;In a March 29 meeting, more than 60 students spoke at an ASM open forum about the resolution. The students who spoke in favor of the resolution said it would bring more transparency to the UW Foundation and the student body, and take away funds from corporations that profit off human rights abuses.&lt;br/&gt;Those who spoke in opposition said the resolution was too similar to the Boycott, Divest, Sanction movement, which asks entities to withdraw support from Israel and Israeli companies.&lt;br/&gt;ASM indefinitely postpones divestment resolution after hours of heated debateAfter six hours of heated debate, the University of Wisconsin Associated Students of Madison voted 13-12-1 to postpone a resolution demanding the Read...&lt;br/&gt;In six hours of heated debate, the legislation was tabled indefinitely in a 13-12-1 vote.&lt;br/&gt;But in an April 26 ASM meeting, the legislation was brought up again, this time without some of the more contentious previsions. ASM representatives cut down the legislation from its original 13 pages to one to appease the opposition's requests.&lt;br/&gt;Representatives from Badgers United Against Hate said they were pleased with how ASM took Israeli and Jewish students concerns into consideration with the new legislation.&lt;br/&gt;Others said the updated resolution was "watered down" and was made for the "comfort of ... oppressors."&lt;br/&gt;ASM unanimously approves contentious divestment proposal to mixed reactions from campusAfter five hours of debate and nearly 50 people appearing before open forum, the University of Wisconsin Associated Students of Read...&lt;br/&gt;After the open forum ended, ASM representatives added new amendments to reflect the resolution proposed in the March 29 meeting. The amendments named specific Israeli companies, prompting two members of ASM to leave.&lt;br/&gt;The updated resolution, now four pages, was passed in a 24-0-2 vote.&lt;br/&gt;In a statement, Chancellor Blank said the university will not divest from corporations, citing ASM doesn't control UW. The statement said UW was concerned with how ASM handled the issue, saying it was "undemocratic" and "not transparent."&lt;br/&gt;Amid backlash, Walker introduces proposal to opt out of segregated fees&lt;br/&gt;Gov. Scott Walker's contentious proposal to allow students to decide whether or not to pay segregated fees to fund certain student organizations reached a temporary resolution in April.&lt;br/&gt;Walker and other Republican supporters of the opt-out proposal said it would cut costs for families struggling to pay for college. But ASM and a host of student organizations said it would throw funding for necessary student services into question.&lt;br/&gt;The Joint Finance Committee determined the opt-out was a nonfiscal item, and therefore could not be included in the governor's state budget. But the issue could potentially re-emerge if a state legislator introduces it as an individual bill separate from the budget.&lt;br/&gt;Joint Finance Committee eliminates proposal allowing students to opt out of segregated feesFollowing much backlash from students throughout the University of Wisconsin System about the possibility of being able to opt out of allocable Read...&lt;br/&gt;The Associated Students of Madison and other students quickly responded to the opt out prevision when Walker proposed it in February. ASM is responsible for allocating student fee dollars at the University of Wisconsin.&lt;br/&gt;Students throughout the UW System came together to pass a resolution opposing the opt out, with representatives from 18 UW campuses participating in the vote.&lt;br/&gt;"I am glad that we all are united on fighting for our campuses and the UW System," ASM Chair Carmen Goséy said. "ASM always tries to best represent our student voices and we're excited to move forward with our efforts."&lt;br/&gt;UW System representatives express opposition to allocable fee opt-out proposalStudent representatives from across the UW System passed a resolution Monday expressing opposition to Gov. Scott Walker's proposal to make allocable Read...&lt;br/&gt;UW Dean of Students Lori Berquam also urged JFC to remove the provision, saying it would have had a "significant impact" on important services and programs like transportation, health care and veteran support.&lt;br/&gt;Student groups unite in effort to oppose contentious budget proposalUniversity of Wisconsin students considered what a future with reduced segregated fees would look like in light of a proposal Read...&lt;br/&gt;City&lt;br/&gt;Tony Robinson's family receives historic $3.35 million settlementAlmost two years after a white Madison police officer shot biracial 19-year-old Tony Robinson, his family received a federal civil rights settlement of $3.35 million.&lt;br/&gt;The settlement was the highest amount paid in state history for an officer-related shooting.&lt;br/&gt;But Kenny was cleared of any wrongdoing by Dane County District Attorney Ismael Ozanne. After an internal investigation, MPD also found Kenny had acted within the department's code of conduct.&lt;br/&gt;Tony Robinson's family reaches record $3.35 million settlement for fatal shootingNearly two years after the fatal shooting of 19-year-old Tony Robinson, his family has finally settled a $3.35 million federal Read...&lt;br/&gt;The police department said it found the settlement "outrageous" because Kenny "did [his] job in accordance with their training and the law."&lt;br/&gt;MPD also said the settlement was likely to hurt its morale.&lt;br/&gt;Despite the settlement being the largest in state history, Robinson's family still feels a void from their loss.&lt;br/&gt;Despite historically large settlement, family still 'feels void' from Tony Robinson's deathAlmost two years have passed since Madison Police Officer Matt Kenny fatally shot 19-year-old Tony Robinson Jr., and today the late teen's Read...&lt;br/&gt;For Robinson's mother said the sum of the money didn't matter. She wanted to go through with the trail, but didn't want to put her children through that process.&lt;br/&gt;Racial just group Racial Justice Tipping Point created a petition calling for MPD to fire Kenny.&lt;br/&gt;According to the petition, firing Kenny would be one step closer toward accountability for him and the department.&lt;br/&gt;Racial justice group calls for officer who shot Tony Robinson to be firedAs the two-year anniversary of Tony Robinson's death approaches, Racial Justice Tipping Point has created a petition calling for Madison Read...&lt;br/&gt;In response to the petition, MPD said the investigation was already conducted and they found Kenny acted within his rights and therefore will not fire him.&lt;br/&gt;In response to the settlement, the city of Madison has made policy changes regarding backup in policing situations, which will hopefully save lives, MPD officials said.&lt;br/&gt;Dane County paves path for immigration reform&lt;br/&gt;The year began with many federal actions regarding immigration and immense pushback from communities around the country, including Madison and Dane County.&lt;br/&gt;Dane County Executive Joe Parisi announced in February that the county would be creating an immigration assistance fund. The Dane County Board later approved a resolution in April to give the fund $150,000.&lt;br/&gt;Dane County Board carves path for undocumented immigrants hoping to become citizensAs conversation on immigration reform at the federal level intensifies, the Dane County Board of Supervisors moved forward with programs aimed Read...&lt;br/&gt;The resolution also seeks to help immigrants by reaching out to several legal service providers in the area to help develop emergency immigration assistance.&lt;br/&gt;The legal service providers will work with the Madison Community Foundation to help decide how money from the fund will be spent.&lt;br/&gt;Dane County Executive announces plan to help residents attain citizenshipDane County Executive Joe Parisi announced a two-pronged plan to help Dane County residents gain citizenship at a news conference Read...&lt;br/&gt;Sup. Jenni Dye, District 33, said many organization have spoken in favor of the resolution.&lt;br/&gt;"We don't often do thing like this," Dye said. "I'm really proud to be on a body and with my community where we can come together to do the right thing and help the people that need it."&lt;br/&gt;The board also created an amendment in March to help keep immigrants' information private.&lt;br/&gt;Dane County Board moves to amend ordinance to protect immigrant communityShortly after President Donald Trump issued a second executive order with regard to immigrant and refugee entry, the Dane County Board planned to Read...&lt;br/&gt;The amendment itself further clarified what information falls under the category of "confidential information" and says which county employees cannot disclose this information.&lt;br/&gt;"We're looking at the art of the possible - what do we have control over, how can we help, how can we meet the needs of our community?" Parisi said. "And at the same time, reflecting the values of the people who live in this community, because this isn't just about people who are immigrants who are looking for that path to citizenship."&lt;br/&gt;Dane County spearheads initiatives to help homeless&lt;br/&gt;After months of debate between the Mayor Paul Soglin and City Council over a panhandling ordinance, numerous homeless initiatives, including creation of new housing and homeless owned on-call company, are on the way.  &lt;br/&gt;Homeless Issues Committee votes against ordinance prohibiting sleeping on public sidewalksCity officials unanimously voted against a resolution prohibiting individuals from sleeping or lying down on public sidewalks during a Homeless Read...&lt;br/&gt;The Homeless Issues Committee voted against a resolution prohibiting individuals from sleeping in Central Business District Area.&lt;br/&gt;County Sup. Heidi Wegleitner, District 2, said though no lawful alternatives exist, the city needs to address homelessness in more humane ways.&lt;br/&gt;The 2017 Dane County budget also prioritized reducing homelessness by bolstering funding for existing initiatives and starting funding for new ones, totaling $2 million.     &lt;br/&gt;Parisi prioritizes homelessness, opioid epidemic in 2017 budgetWith a focus on investing in the county's future, Dane County Executive Joe Parisi announced several expansions in social services Read...&lt;br/&gt;In a joint project between the city and county, $3 million will be used to develop a single-housing unit complex and affordable housing.&lt;br/&gt;Dane County Board votes to expand housing for homelessIn an effort to expand affordable housing for low-income families in Madison, the Dane County Board approved a resolution Thursday to Read...&lt;br/&gt;Madison residents also established initiatives to employ more homeless people. Resident Henry Johnson started the Homeless Entrepreneurship Initiative to hire homeless people for jobs ranging from moving to hauling scrap metal.&lt;br/&gt;Madison resident begins initiative to help city's homeless empower themselvesMadison resident Henry Johnson found that as a homeless man for nearly three years, there are few resources to help Read...&lt;br/&gt;State&lt;br/&gt;Legislators move to legalize lifesaving CBD oil&lt;br/&gt;Gov. Scott Walker signed a mostly bipartisan bill legalizing a cannabis oil extract in April.&lt;br/&gt;CBD oil has been effective at treating various seizure-causing illnesses. Several families spoke at a public hearing about the need for their children to have CBD oil to help with their seizures.&lt;br/&gt;A Wisconsin grandmother said her 2-year-old granddaughter suffers from seizures. The grandmother said she has to go to another state to purchase CBD oil and bring it back to Wisconsin.&lt;br/&gt;Rep. Scott Krug, R-Wisconsin Rapids, who co-authored the bill, discussed the need for this legislation in Wisconsin at a news conference in March.&lt;br/&gt;Assembly passes bill to legalize possession of medical marijuana extractAfter passing the Wisconsin state Senate, the Assembly unanimously voted 98-0 to legalize the possession of a medical marijuana extract oil. Read...&lt;br/&gt;"As we move forward with the CBD issues in the state of Wisconsin, for me, it's bittersweet because we've seen hundreds of families come through and talk to us about the need for a bill that works and is effective and now we're able to deliver," Krug said.&lt;br/&gt;The legislation includes a 30-day provision to help avoid problems with the U.S. Drug Enforcement Agency's classification of CBD oil as a Schedule 1 drug. The provision makes it so if the federal government changes CBD's classification, Wisconsin will follow suit in 30 days.&lt;br/&gt;Wisconsin families continue emotional fight in push for medical marijuana extract billThe sound of people holding back tears peppered a public hearing in the State Capitol Wednesday as legislators considered a Read...&lt;br/&gt;Assembly Speaker Robin Vos, R-Rochester, praised the bipartisan support of this legislation at the March news conference.&lt;br/&gt;"Today is a day that I could not be prouder to serve as the leader of the Assembly," Vos said.&lt;br/&gt;Wisconsin rallies with the world to support women&lt;br/&gt;Protesters have made their voices heard on the steps of the state Capitol for a variety of issues in the past months, but especially women's rights.&lt;br/&gt;Madison community marches in solidarity with women around the country and worldThe footsteps of women in Madison echoed those from around the world as they marched in solidarity Saturday to protest the upcoming presidency Read...&lt;br/&gt;Sporting pink hats and signs showing solidarity with women, Madisonians joined demonstrations around the world to oppose Trump's inauguration in January and again in March as part of International Women's Day.&lt;br/&gt;A Day Without Women: Madison community marches to advocate for women's rightsWomen from across the state battled strong winds atop the steps of the State Capitol building as they marched to discuss a Read...&lt;br/&gt;Madison Police Department estimated the crowd peaked at approximately 100,000 people for Madison's Women's March, which began at Library Mall. Those marching took issue with the normalization of Trump's "misogynistic behavior" and welcomed a host of local politicians urging organization and information seeking.&lt;br/&gt;As demonstrators continued to call for community control and political engagement, people from different walks of life found common ground. At the "Day Without A Woman" strike, speakers encouraged attendees to "show up" for each other.&lt;br/&gt;One speaker, Zon Muas, said her goal with the protests was to speak up on behalf of minority women.&lt;br/&gt;"It was very important that we really spoke about solidarity and unity and showing up, because a lot of time women's issues are just thought of as reproductive, but it is so much more than that," Muas said.&lt;br/&gt;Trump's immigration ban affects more than 100 students&lt;br/&gt;President Donald Trump's executive order, which suspended entry of refugees and travelers,particularly those from a host of Muslim-majority countries, impacted 115 University of Wisconsin faculty and staff in January.&lt;br/&gt;Trump executive order impacts at least 88 in UW communityUniversity of Wisconsin officials announced Monday there are 115 faculty, students and staff impacted by President Donald Trump's executive order Read...&lt;br/&gt;UW Chancellor Rebecca Blank officially added UW to the list of universities calling for Trump to reconsider the executive order.&lt;br/&gt;"These actions affect real people - researchers, scholars, students and staff - who are essential to our goals of providing a world-class education," Blank said.&lt;br/&gt;Opponents of the order, including more than 200 students of various religious backgrounds, spoke out their supports for refugees at the top of Bascom Hill.&lt;br/&gt;Executive order impacts students, faculty, researchers on campus, forcing many to speak outStanding in front of a crowd of 200, Zahiah Hammad introduced the ways President Donald Trump's executive order on immigration Read...&lt;br/&gt;The city board approved a resolution to fund the citizenship assistance services. Dane County granted $150,000 and reached out to local legal service providers such as UW Law School Immigration Justice Center and Jewish Social Services of Madison for their assistance with immigration issues.&lt;br/&gt;Dane County Board carves path for undocumented immigrants hoping to become citizensAs conversation on immigration reform at the federal level intensifies, the Dane County Board of Supervisors moved forward with programs aimed Read...</t>
         </is>
+      </c>
+      <c r="L90" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -4385,10 +4662,13 @@
           <t>Immigration (For)</t>
         </is>
       </c>
-      <c r="J91" t="inlineStr">
+      <c r="K91" t="inlineStr">
         <is>
           <t>Hundreds gathered at the Capitol Monday for International Workers' Day to call for a higher minimum wage, better working conditions and an end to attacks on unions.&lt;br/&gt;For this year's International Workers' Day, in light of President Donald Trump's administration's immigration policy reforms, the march rallied specifically for marginalized community members in "A Day without Immigrants and Refugees."&lt;br/&gt;The marchers gathered in two locations: University of Wisconsin Library Mall and Brittingham Park. UW and high school students gathered largely at Library Mall, while community members gathered at Brittingham Park.&lt;br/&gt;Marchers ended at the Capitol to express their dismay over current workers' rights issues to state legislators.&lt;br/&gt;Madison leaders call new immigration executive order unconstitutionalIn light of a recent executive order on immigration from President Donald Trump's administration, Madison city officials have voiced their support Read...&lt;br/&gt;About 400 assembled for the march without incident, according to a Madison Police Department incident report.&lt;br/&gt;Over 20 artists, performers and community leaders delivered messages to the marchers, emphasizing social welfare and workers' rights.&lt;br/&gt;In the opening speech, Claudia Gonzalez from the Immigrant Workers Union expressed the need to raise the minimum wage to $15.&lt;br/&gt;"We can see that in one way or another things haven't changed because the 1 percent has always quieted us with false promises," Gonzalez said. "[The 1 percent] want [immigrants] to survive with the minimum wage pay, having us to work two to three jobs because it's impossible to survive with the minimum wage pay of $7.25 per hour."&lt;br/&gt;Alex Gillas, one of the lead organizers of the march, said the main objective was to raise awareness that the public is tired of policies benefitting corporations, not people.&lt;br/&gt;ASM unanimously approves contentious divestment proposal to mixed reactions from campusAfter five hours of debate and nearly 50 people appearing before open forum, the University of Wisconsin Associated Students of Read...&lt;br/&gt;Gillas said he expected public discontentment with Trump's stances toward immigrants to boost the rally's attendance since immigrants feel the effects of these discriminatory policies.&lt;br/&gt;"This year is more important than many others because President Trump said he has decided to do things better for us, but it's actually way worse," Gillas said. "It's true we don't have any legislation right now... [but] just the rhetoric involving the wall is dangerous to society."&lt;br/&gt;Activist Shadayra Kilfoy-Flores said she came to the march because many of her family members also experience discrimination in Madison.&lt;br/&gt;But Kilfoy-Flores said she still believes the Madison community can change.&lt;br/&gt;"I feel that it's my responsibility, because I'm documented, to stand up for those who are not," Kilfoy-Flores said.</t>
         </is>
+      </c>
+      <c r="L91" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -4423,10 +4703,13 @@
           <t>University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J92" t="inlineStr">
+      <c r="K92" t="inlineStr">
         <is>
           <t>The 2015-16 school year marked the University of Chicago's 125th anniversary, which Dean Boyer commemorated by dropping a 700-page tome on the history of the University. What's missing: the chapter that we as students are helping to write right now. Below is a rundown of the major stories from '15-'16 to get you up to speed and ready to jump into '16-'17.&lt;br/&gt;The first news of the year came in early September, before classes had even begun. After years of pressure from the Trauma Center Coalition , the University announced that it would partner with Sinai Health System to build a Level I adult trauma center at Holy Cross Hospital on the South Side. In December, the University announced a change of course: the trauma center would no longer be built at Holy Cross, but at the UCMC instead. The $269 million plan was approved by the Illinois Health Facilities and Services Review Board in May, and the trauma center is slated to open in 2018.&lt;br/&gt;Back in May of 2015, the South Side got some other big news when the Obama Foundation announced that Washington Park or Jackson Park would be the future home of the Barack Obama Presidential Center. Though signs initially pointed to Washington Park, the foundation announced its pick of Jackson Park in July. The center will open its doors in 2020 or 2021 and will be designed by the same firm responsible for the Logan Center for the Arts.&lt;br/&gt;A University posting policy violation in October foreshadowed a tense year for students on both sides of the Israel-Palestine debate. Students for Justice in Palestine at the University of Chicago filed a complaint with the Office of Campus and Student Life after flyers they had put up across campus for a "Day of Action" were vandalized with handwritten graffiti that included "Six million Jews were murdered during the Holocaust," and "Stop Venerating Terror." Unsigned flyers also appeared, one of which played on the SJP acronym with "Stabbing Jews for Peace."&lt;br/&gt;Campus stood still at the end of fall quarter when President Robert J. Zimmer announced via a university-wide e-mail that all classes and activities would be canceled on November 30. The reason: a gun threat posted as a comment on worldstarhiphop.com that read: "This is my only warning. At 10 AM Monday morning, I'm going to the campus quad of the University of Chicago. I will be armed with an M-4 carbine and two desert eagles, all fully loaded. I will execute approximately 16 white male students and/or staff, which is the same number of times [Laquan] McDonald was killed. I will then die killing white policemen in the process. This is not a joke." The man who posted the threat, a University of Illinois at Chicago student named Jabari Dean, was identified and arrested by the FBI around midday on November 30. Though nothing came of the threat, Zimmer announced in a follow-up e-mail that the University would beef up security around campus for the remainder of fall quarter.&lt;br/&gt;An alleged sexual assault was reported at Delta Upsilon fraternity in October, setting the stage for a debate about Greek life and sexual assault that would amplify as the year continued. In March, rumors circulated on Yik Yak about another alleged sexual assault that had been reported at the Psi Upsilon (Psi U) fraternity in August of 2015 but garnered little attention at the time. The rumors prompted the complainant to set the story straight on the public Facebook group Overheard at UChicago. Just hours later, another UChicago student revealed on Overheard that she too was assaulted at Psi U in April of 2015.&lt;br/&gt;In early February, The New York Times reported that Dr. Jason Lieb, a UChicago professor in the Department of Human Genetics, resigned following allegations that he sexually assaulted a student while she was under the influence of alcohol. Lieb had taken a leave of absence in November of 2015 after the University began investigating the allegations, and formally resigned on January 21. The resignation raised questions about how and why Lieb was hired in the first place, given that he faced similar accusations during his tenure at the University of North Carolina at Chapel Hill.&lt;br/&gt;In 2014, the U.S. Department of Education's Office of Civil Rights launched a campus-wide investigation into a potential breach of Title IX, which prohibits discrimination on the basis of sex in education programs or activities. This February, the ORC opened two new investigations into the University for possible violations of federal law over the handling of sexual violence and harassment complaints.&lt;br/&gt;Students responded to the frequent and public allegations of sexual assault by pressuring the administration and Greek life to more strictly enforce disciplinary measures for perpetrators and bolster awareness and prevention efforts.&lt;br/&gt;But the University finds itself stuck between a rock and a hard place. Last month, a male student twice investigated for sexual assault by the University sued the school for violating Title IX by creating a "gender-based, hostile environment against males." The suit is one of several recent?and typically unsuccessful?instances of male students across the country suing their universities for favoring females over males as a result of public pressure to eradicate their campuses of sexual assault. Last month, however, a federal appeals court ruled in favor of a similar suit against Columbia University.&lt;br/&gt;The same week The New York Times broke the news about professor Lieb's resignation, BuzzFeed News published an article with leaked racist, Islamophobic, and misogynistic e-mails that had been circulated to the listhost of Alpha Epsilon Pi (AEPi), a historically Jewish fraternity, between 2011 and 2015. Administrators sent an e-mail condemning the language of the AEPi e-mails, but many students were displeased with their lack of action. College Council passed a resolution authored by members of the Muslim Students Association , Organization of Black Students , and Students for Justice in Palestine and endorsed by 42 student groups demanding that the University suspend all ties with AEPi and mandate yearly sensitivity training on diversity and sexual assault for members of Greek life. AEPi released an apology on Facebook and has said it is taking steps to combat intolerance.&lt;br/&gt;That same week, The Maroon received a tip from an alumnus and former brother of Phi Delta Theta (Phi Delt) that the fraternity's UChicago chapter would be suspended and eventually "recolonized" on account of unspecified "risk management policy violations." This summer, a rising third-year and former Phi Delt pledge filed a lawsuit against the Phi Delt fraternity, the Illinois Beta chapter at UChicago, and 13 students who were members of the chapter. He alleges in the suit that he was the victim of hazing and physical assault in the chapter house during spring pledge week of 2015. Phi Delt has not commented on whether the incidents presented in the suit are related to the charter suspension.&lt;br/&gt;Though administrators remained hands-off and close-lipped throughout the Greek life controversies, they urged students to complete the upcoming Campus Climate Survey, promising to work toward long-term solutions for issues of diversity and inclusion. The University launched its campus climate project in 2015 in response to complaints and concerns raised during the 2014-2015 school year about the safety of UChicago campus life. It circulated the first survey at the end of 2015, which was focused on issues of sexual assault and misconduct, and the second this April, focused on the experiences of underrepresented and potentially marginalized groups. About thirty two percent of students completed the first survey, which found that "UChicago students experience sexual misconduct, including sexual assault, at rates similar to those reported by other institutions." The results of the 2015 survey were used to redesign O-Week programming and improve training for undergraduate and graduate students. Twenty nine percent of students completed the second survey, the results of which will be released during the upcoming year.&lt;br/&gt;In January at Bartlett Dining Hall, a student cut into her grilled chicken to behold a screw. She notified UChicago Dining, which investigated the incident and found Aramark, the University's food supplier of 27 years, responsible. At the time the screw was discovered, the University was in the process of renegotiating its contract with Aramark and was considering proposals from two other companies, Sodexo and Bon Appétit. Bon Appétit, which has the highest food service ratings of the three providers, ultimately won out and took over on July 1. Most students are happy about the change, but not members of the Fight for Just Food , a group that advocates for in-house, or self-operated, dining services. FJF argues that the University supports mass incarceration because it contracts with food suppliers who profit from serving food in prisons. Though Bon Appétit, unlike Aramark, does not directly provide food to prisons, its parent company owns other food providers that do. The group organized a rally and a day-long hunger strike after the University announced its pick of Bon Appétit, and later proposed a resolution to CC calling for self-operation that failed.&lt;br/&gt;At the beginning of spring quarter, a group called U of C Divest launched an effort?in response to the "Boycott, Divestment, and Sanctions" movement?to get the University to divest from 10 companies it sees as complicit in Israeli human rights abuses against Palestinians. U of C Divest presented a resolution to CC that passed after heated debate at an unusually crowded meeting where audio and video recording were prohibited. The resolution divided campus not only over the Israel-Palestine conflict, but also over the question of whether Student Government should represent the student body on controversial political issues. The administration responded to the passage of the resolution by saying that it would not divest from the listed companies, citing the 1967 Kalven Report, which maintains that the University stay politically and socially neutral. The University has refused to divest from fossil fuel companies for the same reason, despite sustained efforts by the UChicago Climate Action Network .&lt;br/&gt;When SG elections rolled around in the spring, United Progress was elected to the executive slate for the third year in a row, this time without Tyler Kissinger, who graduated in June after serving two consecutive years as student body president. Third-year Eric Holmberg took his place, joined by graduate student Cody Jones as vice president for student affairs and second-year Salma Elkhaoudi as vice president for administration. United Progress beat out three other slates: Our Campus, Unite and Support, and DU's satirical Moose slate. Our Campus won the overall College vote, but United Progress's pro-grad student unionization platform earned it all but two graduate divisions: Booth and the Law School.&lt;br/&gt;Both the outgoing and incoming United Progress slates made graduate issues a priority at the end of the year, with the main focus on grad student unionization. Graduate Students United , a group of around 700 graduate students that has been advocating for graduate students' rights since 2007, intensified its fight for unionization after non-tenure track faculty successfully unionized in December. GSU had a major win in August when the National Labor Relations Board ruled that graduate students are workers under the National Labor Relations Act and have the right to unionize at private universities. However, administrators and other graduate students worry that unionization will inevitably shift the professor-student relationship from mentor-mentee to employer-employee, redefining and perhaps jeopardizing the graduate student experience.&lt;br/&gt;The outgoing United Progress executive slate made a final push in May to leave its mark on SG. It proposed a plan to pay future members of the executive cabinet using $16,979 in rollover funds from the 2015-2016 budget. The proposal failed after two representatives walked out of an extraordinary session of General Assembly that had been called by petition to discuss the plan, denying quorum and preventing a vote. Also unsuccessful was United Progress's attempt to streamline the way graduate students vote for their divisions' representatives, in accordance with SG's election code. The majority of graduate student representatives argued that the diverse processes suit the individual needs of the various divisions and schools, and GA voted to pass an amendment officially allowing Graduate Council to determine the electoral process of its members on a division- or school-specific basis.&lt;br/&gt;To the dismay of many students and alumni, College Housing sold satellite dorms Broadview, Maclean, and Blackstone at the end of the year to 3L real estate, which is leasing out rooms for 2016-17. Broadview, Maclean, and Blackstone's house names, along with New Grad's house names, were retired and the houses moved into Campus North, the megalodon of dorms that your class will christen. North Campus follows in the footsteps of Max P and Granville-Grossman as part of the University's effort to centralize student housing and retain students after their first year. Dean Boyer even suggested at a CC meeting in April that another dorm south of the Midway may be on the horizon.&lt;br/&gt;Cut to finals week in June, when everyone dropped their textbooks and picked up The New York Times to read an article entitled "University of Chicago Student President Faces Expulsion on His Eve of Graduation." Tyler Kissinger was indeed summoned to a disciplinary hearing, but only received disciplinary probation and was allowed to graduate with the rest of the Class of 2016. He was summoned for "creating an unsafe situation" when he used his status as SG president to gain entry into the building under false pretenses and prop the door open for protesters to enter and hold a sit-in outside Provost Eric Isaacs's office. The May 14 sit-in was an extension of a "Rally to Democratize the University," organized by the IIRON Student Network (now called Chicago Student Action), of which Kissinger was a member. A change.org petition petition calling on the University to drop charges gained over 3,000 signatures as students expressed concern that the administration was contradicting its values by discouraging freedom of protest.&lt;br/&gt;The "Rally to Democratize the University" was the largest campus protest of the year, with more than 150 participants. IIRON, the social justice umbrella network that coordinated it, is made up of organizations including Fair Budget UChicago , the Campaign for Equitable Policing , Students for Disability Justice , and UChicago Climate Action Network . The protest covered a range of issues, from a living wage to UCPD accountability to fossil fuel divestment. It was organized in response to administrators' failure to meet with student activists on numerous occasions throughout the year.&lt;br/&gt;IIRON frequently targeted Isaacs, who left his post to become Executive Vice President for Research, Innovation, and National Laboratories at the end of the year (He is succeeded by Daniel Diermeier, whose academic work has focused on politics, the interaction of politics and business, public perception, and crisis management). During winter quarter, 60 students from Fair Budget UChicago, one of IIRON's member organizations that advocates for a $15 per hour minimum wage for campus workers, organized a march across the quad. The march ended outside Isaacs's office in Levi Hall with the delivery of a petition signed by over 1,000 people calling for a higher wage for University workers.&lt;br/&gt;Fair Budget UChicago also participated in a protest over higher-education budget cuts in April outside the Chicago Symphony Orchestra, where two University trustees were in attendance. That month, the University announced that it would roll out a Shared Services program over the next two years. Shared Services is a cost-cutting initiative meant to consolidate administrative services between departments. Similar programs have faced opposition at other universities in recent years from groups like FBU that argue they hurt workers and waste money.&lt;br/&gt;Perhaps the biggest controversy of all came last: Dean Ellison's letter to you, the Class of 2020, delivered on August 24. The letter affirmed the University's commitment to academic freedom, but in so doing denounced trigger warnings and safe spaces. Some, who felt that the administration was taking a needed stand against a culture of political correctness in higher education, praised the letter, while others condemned it, claiming that the administration was unfairly conflating trigger warnings and safe spaces with speaker silencing.&lt;br/&gt;Academic freedom always looms large at UChicago, but this year it will be at the forefront of the conversation like never before. Last year was marked by controversy after Black Lives Matter protesters shouted Anita Alvarez off the stage at the Institute of Politics and the UCPD shut down an event featuring Bassem Eid after a Q&amp;A session turned heated. This year's dialogue is sure to be influenced by trigger warnings and safe spaces thanks to Ellison's letter. Lying dormant in the background is a free speech resolution with 136 signatures that was tabled indefinitely by CC in the spring. The resolution, which calls on the University to condemn any student who "obstructs or disrupts" free speech and to enforce such condemnation, may be brought up again for discussion at any time.&lt;br/&gt;Here's to another action-packed year at the third highest-ranked college in the country (well, tied with Yale).</t>
         </is>
+      </c>
+      <c r="L92" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -4466,10 +4749,13 @@
           <t>University governance, admin, policies, programs, curriculum, Labor and work</t>
         </is>
       </c>
-      <c r="J93" t="inlineStr">
+      <c r="K93" t="inlineStr">
         <is>
           <t>By Adam Duke&lt;br/&gt;Editor in Chief&lt;br/&gt;Following a year in which students experienced problems with Canisius' travel agent, Travel Team, the Griffs' hockey team won the Atlantic Hockey Conference for the first time in program history, and the administration struggled with Gov. Cuomo's Excelsior Scholarship Program, Canisius faced new problems, but also experienced new triumphs in the 2017-18 school year.&lt;br/&gt;The year started with 553 freshmen going through orientation. This was a drop from last year's class of 600, which sparked an issue of rightsizing, with decreasing enrollment throughout the school. In September, Student Life developed "Today@Canisius," which consolidates all of the club event announcements into one email to prevent the need for mass emails cluttering students' inboxes. Sophomore senator Emily Augugliaro organized Reddy Bike bike rides through the city, as the bikes increased in popularity amongst students, with a new bike rack outside Old Main. To round out the month, The Griffin profiled Gabrielle Walter, current Miss New York and Canisius alumna, who graduated in 2015.&lt;br/&gt;Come Oct. 2, Canisius had its "Great to be a Griff" day, where administration announced the Excellence Within Reach campaign, which reduced tuition from nearly $35,000 to $27,000 to provide more of an incentive for incoming students to enroll at Canisius. With this announcement, scholarships were also reduced, which created a commotion amongst students.&lt;br/&gt;Later in the month, Canisius' Afro-American Society began its celebration of its 50th anniversary. The club was formed to give African American students a voice on campus and to create a diverse atmosphere. This year, the club held events such as the poetry and fashion art exhibit, the soul food dinner, and the annual Afro-American Society Ball, which was held last week. In addition, the school saw activism on the Griffs' volleyball team as three players took a knee for the national anthem for several games, inspired by the movement begun by former San Francisco 49ers quarterback Colin Kaepernick, who was displeased with police brutality and oppression of people of color in the United States.&lt;br/&gt;Following the impact of Hurricane Maria later in the month, the entire volleyball team rallied together to assist teammate Andrea Díaz López, her family, and the island of Puerto Rico.&lt;br/&gt;November brought forth talks of divestment, as Augugliaro spoke with Canisius' vice president of business and finance, Marco Benedetti at USA's first meeting of the month, about letting go of unethical or morally ambiguous investments. November also sparked what would become the issue The Griffin covered most in-depth throughout the year, the authorization of a strike by facilities workers after the contract dispute between their union and Canisius administration. Talks of possible strike began when the union's labor contract expired in May. Due to lower enrollment, resources including facilities' benefits, particularly retirement benefits, had to be cut. Canisius president and former Griffin editor John J. Hurley said that returning retirement benefits was a "top priority."&lt;br/&gt;Facilities disputes continued through December, as students and faculty joined the unionized workers in a rally at 9 Hughes Ave. early in the month. The rally spurred a march to President Hurley's office, where the workers delivered a letter that expressed their concerns.&lt;br/&gt;Over winter break, a soft serve ice cream machine was implemented in the dining hall.&lt;br/&gt;The new semester began with the extension of negotiations for facilities workers, which remained at a standstill until February, as both the Service Employees International Union and Hurley released statements on the contract, showing opposing views on it. The semester also brought the enforcement of a 2017 travel policy, which requires clubs and teams traveling on school-funded trips to limit one student per bed in hotel rooms. This created frustration in club leaders, who had to have more student funds allocated to be spent on additional hotel rooms.&lt;br/&gt;Following The Griffin's "Pillars" February editorial about USA and student apathy, Maddie Reed '18, spoke to USA about this lack of student involvement in club events. This began talks in USA requiring senators to attend these events to support their school. From these discussions, the School Spirit Committee was established by USA president Amelia Greenan.&lt;br/&gt;March began with the first ever Community Week, from March 11 to March 17, beginning with Mass on Sunday and concluding with the Day of Service. Each day featured a new event that allowed students to learn about opportunities to get involved in the community. That same week, Dylan McLaughlin of Canisius hockey was named a top 10 finalist for the Hobey Baker Award on March 14, the second Griff to do so in the past two years. He was also named the AHC Player of the Year the next day. Canisius also had a school walkout that week, in solidarity with those across the nation walking out in support of stricter gun laws, due to the school shooting in Parkland, Fla.&lt;br/&gt;This month, the College's director of public safety, H. Wil Johnson, announced his retirement April 10. After three years as head of the department, he will be stepping down as director on May 19. On April 11, sophomore Isaiah Reese of the Canisius basketball team entered his name into the 2018 NBA draft. The following day, freshman Takal Molson also made the announcement that he would be entering his name into the draft, after a season that Griffin sports editor Marshall Haim described as featuring "the best team in two decades." On April 13, The Griffin reported on rodents found in the freshman dorms, specifically on the fourth floor of Bosch. Students were charged an additional fee to move from the dorm and expressed their frustrations. The month concluded with USA elections, in which Matthew Smardz won president and Olivia Owens won VP. Senate election results were released last night via USA's twitter account.</t>
         </is>
+      </c>
+      <c r="L93" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -4509,10 +4795,13 @@
           <t>Gun control</t>
         </is>
       </c>
-      <c r="J94" t="inlineStr">
+      <c r="K94" t="inlineStr">
         <is>
           <t>By Adam Duke&lt;br/&gt;Editor in Chief&lt;br/&gt;Following a year in which students experienced problems with Canisius' travel agent, Travel Team, the Griffs' hockey team won the Atlantic Hockey Conference for the first time in program history, and the administration struggled with Gov. Cuomo's Excelsior Scholarship Program, Canisius faced new problems, but also experienced new triumphs in the 2017-18 school year.&lt;br/&gt;The year started with 553 freshmen going through orientation. This was a drop from last year's class of 600, which sparked an issue of rightsizing, with decreasing enrollment throughout the school. In September, Student Life developed "Today@Canisius," which consolidates all of the club event announcements into one email to prevent the need for mass emails cluttering students' inboxes. Sophomore senator Emily Augugliaro organized Reddy Bike bike rides through the city, as the bikes increased in popularity amongst students, with a new bike rack outside Old Main. To round out the month, The Griffin profiled Gabrielle Walter, current Miss New York and Canisius alumna, who graduated in 2015.&lt;br/&gt;Come Oct. 2, Canisius had its "Great to be a Griff" day, where administration announced the Excellence Within Reach campaign, which reduced tuition from nearly $35,000 to $27,000 to provide more of an incentive for incoming students to enroll at Canisius. With this announcement, scholarships were also reduced, which created a commotion amongst students.&lt;br/&gt;Later in the month, Canisius' Afro-American Society began its celebration of its 50th anniversary. The club was formed to give African American students a voice on campus and to create a diverse atmosphere. This year, the club held events such as the poetry and fashion art exhibit, the soul food dinner, and the annual Afro-American Society Ball, which was held last week. In addition, the school saw activism on the Griffs' volleyball team as three players took a knee for the national anthem for several games, inspired by the movement begun by former San Francisco 49ers quarterback Colin Kaepernick, who was displeased with police brutality and oppression of people of color in the United States.&lt;br/&gt;Following the impact of Hurricane Maria later in the month, the entire volleyball team rallied together to assist teammate Andrea Díaz López, her family, and the island of Puerto Rico.&lt;br/&gt;November brought forth talks of divestment, as Augugliaro spoke with Canisius' vice president of business and finance, Marco Benedetti at USA's first meeting of the month, about letting go of unethical or morally ambiguous investments. November also sparked what would become the issue The Griffin covered most in-depth throughout the year, the authorization of a strike by facilities workers after the contract dispute between their union and Canisius administration. Talks of possible strike began when the union's labor contract expired in May. Due to lower enrollment, resources including facilities' benefits, particularly retirement benefits, had to be cut. Canisius president and former Griffin editor John J. Hurley said that returning retirement benefits was a "top priority."&lt;br/&gt;Facilities disputes continued through December, as students and faculty joined the unionized workers in a rally at 9 Hughes Ave. early in the month. The rally spurred a march to President Hurley's office, where the workers delivered a letter that expressed their concerns.&lt;br/&gt;Over winter break, a soft serve ice cream machine was implemented in the dining hall.&lt;br/&gt;The new semester began with the extension of negotiations for facilities workers, which remained at a standstill until February, as both the Service Employees International Union and Hurley released statements on the contract, showing opposing views on it. The semester also brought the enforcement of a 2017 travel policy, which requires clubs and teams traveling on school-funded trips to limit one student per bed in hotel rooms. This created frustration in club leaders, who had to have more student funds allocated to be spent on additional hotel rooms.&lt;br/&gt;Following The Griffin's "Pillars" February editorial about USA and student apathy, Maddie Reed '18, spoke to USA about this lack of student involvement in club events. This began talks in USA requiring senators to attend these events to support their school. From these discussions, the School Spirit Committee was established by USA president Amelia Greenan.&lt;br/&gt;March began with the first ever Community Week, from March 11 to March 17, beginning with Mass on Sunday and concluding with the Day of Service. Each day featured a new event that allowed students to learn about opportunities to get involved in the community. That same week, Dylan McLaughlin of Canisius hockey was named a top 10 finalist for the Hobey Baker Award on March 14, the second Griff to do so in the past two years. He was also named the AHC Player of the Year the next day. Canisius also had a school walkout that week, in solidarity with those across the nation walking out in support of stricter gun laws, due to the school shooting in Parkland, Fla.&lt;br/&gt;This month, the College's director of public safety, H. Wil Johnson, announced his retirement April 10. After three years as head of the department, he will be stepping down as director on May 19. On April 11, sophomore Isaiah Reese of the Canisius basketball team entered his name into the 2018 NBA draft. The following day, freshman Takal Molson also made the announcement that he would be entering his name into the draft, after a season that Griffin sports editor Marshall Haim described as featuring "the best team in two decades." On April 13, The Griffin reported on rodents found in the freshman dorms, specifically on the fourth floor of Bosch. Students were charged an additional fee to move from the dorm and expressed their frustrations. The month concluded with USA elections, in which Matthew Smardz won president and Olivia Owens won VP. Senate election results were released last night via USA's twitter account.</t>
         </is>
+      </c>
+      <c r="L94" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -4552,10 +4841,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J95" t="inlineStr">
+      <c r="K95" t="inlineStr">
         <is>
           <t>Over 70 students and community members formed a "Human Oil Spill" in Hirst Lounge Tuesday afternoon to protest the Dakota Access Pipeline -a 1,172-mile underground pipeline designed to transport crude oil from the North Dakota Bakken region into Illinois-and UR's investments in the fossil fuel industry.&lt;br/&gt;Protesters dressed in black from head to toe and lay on the floor for 15 minutes with posters that read "Respect Existence or Expect Resistance" and "We are Water," while members of Grassroots and Students for a Democratic Society spoke to the crowd.&lt;br/&gt;Sophomore and Grassroots Activism Chair Henry Scharfe had two messages to deliver-one to President-elect Donald Trump, the other to University President Joel Seligman.&lt;br/&gt;"We refuse to be complacent," he said, addressing Trump. "You represent the entire nation now. We expect you to protect environmental laws. We expect you to respect the Paris Climate Agreement. We expect you to respect and acknowledge indigenous land."&lt;br/&gt;To Seligman, he added, "The time has come for you to do the same."&lt;br/&gt;The demonstration was one of many protests nationwide in observance of #NoDAPL Day of Action, a day of solidarity to support the Standing Rock Sioux Tribe, which contends that its sacred land and water supply could be compromised by the pipeline's construction.&lt;br/&gt;Sophomore and Vice-President of the Native American Student Association Ruth Dan empathized with the tribe.&lt;br/&gt;"I am a Yupik person," she said. "We are indigenous to the west part of Alaska, and we have lived there for thousands of years. As ice melts, we lose more and more of our shoreline, thus communities are being forced to move. They are the United States' first climate change refugees."&lt;br/&gt;Junior and SDS Co-President Laura Cowie-Haskell called on students to stand up against social injustice.&lt;br/&gt;"Kicking people out of the land they owned and live on is not emblematic of University policies," she said.&lt;br/&gt;To further encourage UR to divest from the fossil fuel industry, Grassroots and SDS have formed the group UR Fossil Free. The group plans on reaching out to alumni and students to receive support and raise awareness of its goal.&lt;br/&gt;"We were very pleased with the turnout, particularly because there were so many community members, something we weren't expecting," said Julianne Kapner, a sophomore and Grassroots fall programming chair. "We hope not to let this momentum die."</t>
         </is>
+      </c>
+      <c r="L95" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -4608,10 +4900,13 @@
           <t>Immigration (For), Hate speech, Anti-racism</t>
         </is>
       </c>
-      <c r="J96" t="inlineStr">
+      <c r="K96" t="inlineStr">
         <is>
           <t>Last week, noted troll Milo Yiannopoulous was scheduled to speak at U.C. Berkeley, the home of our favorite hippie arch rivals and noted free speech enthusiasts across the bay. To the surprise of absolutely no one, people turned out - not to hear Milo speak, but to protest the extension of a public platform to a deliciously punchable platinum-haired douche. This protest was then hijacked by one of the many radical anarchist groups that have made the Bay Area their home since America's Golden Age of Terrorism.&lt;br/&gt;As predictable as the protests against Milo was the outrage spewed against the protestors from left, right and center. Most articles condemning their actions structured their argument along the following lines: central to liberalism is protection of individual liberty, including freedom of speech; freedom of speech must necessarily include protection for speech that is not palatable or agreeable to the majority (or minority); Milo, however unpleasant or unpalatable his opinions might be, must therefore be accorded the same free speech protections as anyone else speaking at a college campus, i.e., he ought to be granted a platform to express his views and that violent action in protest is a form of censorship that ought not to be tolerated.&lt;br/&gt;The typical American liberal response to this, as summed up by my friend and fellow columnist Nick Pether, is that a constitutionally guaranteed right to free speech is strictly a right to express your views without the threat of physical or material violence, or censorship on the part of the state. Expressions of dissent towards controversial viewpoints, including termination of employment, withdrawal of speaking invitations, internet petitions and peaceful protest or civil disobedience, are also forms of protected speech. Therefore, protecting the espouser of a controversial viewpoint from people actively expressing their displeasure through non-violent means infringes on the free speech rights of those dissenting. Under this framework, had the protesters at Berkeley been completely non-violent, they would be in the clear.&lt;br/&gt;Nick goes on to argue that this free speech framework is dangerous because of its framing of free speech as a negative right, i.e. a protection against violence or deprivation. This, he goes on to say, is a typically libertarian or right-wing mindset, which tends to prioritize protection of what an individual already has, and in doing so, reinforces existing social inequities and injustices. Contrast this with what Nick calls positive rights, i.e. rights to proactively access and benefit from something - healthcare, education, a social safety net, etc. The latter viewpoint intends to empower the underprivileged, improve their status within society and provide support to artists, activists and others who typically might not succeed in the free-market-driven society that we live in. Framing free speech as a negative right therefore opens up the field to an extremely slippery slope of arguments advancing regressive goals, Nick concludes - including slashing public funding of universities for teaching leftist material, defunding of abortion providers like Planned Parenthood and discriminating against LGBTQ individuals on the grounds of religious freedom. After all, if U.C. Berkeley can tell Milo to shove it, then why can't conservatives, who currently control 25 state governments and the federal government, decide to defund universities for spending resources on the arts and identity politics?&lt;br/&gt;The implication, of course, is that maybe woke progressives on university campuses shouldn't try to shut down a right-wing provocateur like Milo because the cackling supervillains on the right will in turn try to shut them down by withdrawing funding or declaring criticism of police a hate crime. This is a major cause for concern, specifically given the right's attempts to censor and undermine academic freedom recently.&lt;br/&gt;However, there are three things that critics of college protestors constantly seem to get wrong. The first is that all speech of conservative figures like Milo is protected speech. While this is true for issues that are implicitly part of public debate (e.g. gay marriage, abortion rights, etc.), there is a rich history of exceptions to free speech within liberal democracy that most reasonable people would agree to. These include incitement, libel and provocation or fighting words. Key to all of these exceptions is a reasonable expectation of violent or harmful outcomes from the speech as well as the personal targeting of individuals. So when Milo goes on stage and calls people 'retards' and worse, or publicly humiliates a trans woman for no good reason, then it is nearly impossible to characterize what he says as protected speech - liberally insulting people for shits and giggles isn't exactly a conservative viewpoint. This is further compounded by the fact that Milo himself admits that this behavior is done entirely to provoke and incite protesters, giving credence under the Fighting Words doctrine to those who want to either shut him down or protest him. It's not so much about stopping the free flow of ideas as much as it is about calling out a bully.&lt;br/&gt;The second thing that liberal critics of college leftists get wrong is that conservatives are somehow marginalized and wield little influence in the world, implying that colleges should therefore go out of their way to accommodate viewpoints that are not typically liberal, even idiotic ones like climate change denial. The truth is that Republicans now dominate U.S. politics, business and wealth. Sure, while encased in the bubbles of academia and urban America, it might be easy to think that progressivism has won and that our main task at hand is to keep the excesses of the left in check. Many of us on campus railed against the divest from Palestine movement for being too extreme, while conveniently forgetting about the many ways in which legitimate criticism of Israel has been thrown aside wholesale as anti-Semitism.&lt;br/&gt;More often than not civil disobedience or artistic expression is the only way for liberals, particularly those from marginalized communities, to express their dissent against the more destructive ideas coming from the right. If free speech is supposed to be a positive right, then platforms that enable speech have an obligation to help prop up the voices of those who typically have been excluded from the main channels of expression - and those tend to be the very people protesting Milo. At the end of the day, Milo/Tomi Lahren/insert troll here still get to spew vitriol on Breitbart and the Blaze and make appearances on the Daily Show, while a trans student activist has to drop out of college because Milo publicly humiliated her.&lt;br/&gt;Finally, there is this notion that students on the left are simply "snowflakes" that do not want to engage with ideas or people that make them uncomfortable. Evidence for this is given by the withdrawal of several high-profile commencement speakers from universities, usually after social media campaigns highlighting their past history with homophobia, neoliberal economics or wars of questionable legality. Further evidence is also compounded by concepts such as trigger warnings, which critics deride as methods of protecting students from uncomfortable or controversial ideas.&lt;br/&gt;This is a load of hokum. Protests at colleges are probably older than your parents. The difference was that academics and politicians didn't run away because a few not-fully-formed adults told them that their career had promoted global oppression. People, including leftists, have disagreed and railed against members of the establishment for decades. One would expect noted academics like Condoleezza Rice and Christine Lagarde not to bow down to a few hundred anonymous signatures on the internet. Indeed, even those Smith college students who protested the choice of Lagarde as a commencement speaker were dismayed by her decision to withdraw, since it robbed them off the chance to raise awareness about the perceived harms of neoliberal economics.&lt;br/&gt;Similarly, trigger warnings are nothing new - we just used to say things like 'parental advisory', 'rated R' or 'viewer discretion advised.' The reason these labels were attached to music and movies was because they contained material that people might find shocking or alarming - such as gratuitous violence. When professors freely choose to warn students about content that might be graphic as part of their course material, it's not because they think students are too fragile to study colonialism - it's mainly because we live in a society where we are more mindful of trauma and mental health issues, whether they are faced by survivors of rape, war veterans, or bystanders of terrorist attacks.&lt;br/&gt;If free speech is to be a positive right, then it ought to serve its end goal of bringing in marginalized and non-mainstream voices. But let's put the blame where it ought to lie, and not at the feet of students who are rightfully angry about a platinum-blonde creep doxxing their classmates.&lt;br/&gt;Contact Arnav Mariwala at arnavm 'at' stanford.edu.&lt;br/&gt;While you're here...&lt;br/&gt;We're a student-run organization committed to providing hands-on experience in journalism, digital media and business for the next generation of reporters. Your support makes a difference in helping give staff members from all backgrounds the opportunity to develop important professional skills and conduct meaningful reporting. All contributions are tax-deductible. Support the Daily $25 $50 $100 $500 $1,000</t>
         </is>
+      </c>
+      <c r="L96" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -4664,10 +4959,13 @@
           <t>Immigration (For), Hate speech, Anti-racism</t>
         </is>
       </c>
-      <c r="J97" t="inlineStr">
+      <c r="K97" t="inlineStr">
         <is>
           <t>Divest Dartmouth organized a demonstration against the Keystone XL pipeline. Source: Courtesy of Catherine Rocchi&lt;br/&gt;This article was featured in the 2017 Freshman Issue.&lt;br/&gt;"Dartmouth College has a problem," declared Linda Chavez in a widely-read April 2014 New York Post opinion column. Student protesters, she wrote, had occupied President Phil Hanlon's office and demanded increased faculty diversity, gender-neutral bathrooms and coverage of sex change operations under student health insurance plans.&lt;br/&gt;It can be difficult to ignore sensational articles published by major news outlets following instances of student-led political activism at the College. However, student activists in Divest Dartmouth, Turning Point USA and other groups view their work as more than just fodder for national headlines. Some, like Jesus Franco '20, say that rather than being "a problem," political activism is a powerful instrument of change on campus.&lt;br/&gt;Franco is the co-director of Dartmouth Coalition for Immigration Reform, Equality and DREAMers, or CoFIRED, a campus organization that gathers resources for undocumented students. Franco said that he became involved in CoFIRED last fall as a freshman because he wanted to make a difference on campus. He added that he felt connected to CoFIRED in particular because he comes from a "mixed status" family - while Franco has legal status in the United States, his parents are undocumented immigrants.&lt;br/&gt;CoFIRED's fall 2016 programming included hosting students from Freedom University, an Atlanta-based school for undocumented youth that was founded in 2011 after the Georgia Board of Regents banned undocumented students from attending Georgia's top public universities and removed in-state tuition eligibility for undocumented students. The group hosted students from Freedom University to raise awareness for issues affecting undocumented youth, he said.&lt;br/&gt;Additionally, some of CoFIRED's previous work has received national recognition, such as the group's successful 2016 petition which helped to replace the term "illegal alien" with "undocumented immigrant" in the Library of Congress classification system.&lt;br/&gt;Franco said that since Donald Trump's election to the U.S. presidency, CoFIRED has been "acting pre-emptively" to reassure undocumented students at Dartmouth that the College is prepared to support them in any way possible in the event that the Trump administration phases out Deferred Action for Childhood Arrivals, an Obama-era policy that allows undocumented immigrants who entered the country as minors to receive renewable deferral from deportation.&lt;br/&gt;"Dartmouth has a long history of political activism ... and no student should be complacent when they [notice issues at the College]," he said.&lt;br/&gt;Divest Dartmouth member Alex Miller '20 echoed Franco's sentiment that student-initiated political advocacy is an important source of positive change on campus, saying that he especially appreciated how many of the College's faculty members encouraged students to become politically involved in issues that interest them.&lt;br/&gt;Miller added that he enjoys his work with Divest Dartmouth because there is a strong sense of progress in the organization and its small size allows him to take a more active role in the group's operations.&lt;br/&gt;For example, he helped to coordinate a Keystone pipeline protest, in which Divest members strung together empty Keystone Light beer cans and placed them around the administrative building, Parkhurst Hall, to protest the construction of the Keystone XL and Dakota Access pipelines. Miller said that Divest intends to plan more visible projects, similar to the Keystone pipeline protest, to bring more awareness to the organization and its mission.Miller expects membership in Divest to increase as a result of more visible activism techniques, adding that increased membership would improve the organization's ability to attract attention from the College administration. He also said that he is optimistic that Divest will realize its goal of convincing College officials to divest from certain fossil fuel companies because of changes within the Board of Trustees. Miller added that newer, younger trustees seem more interested in Divest Dartmouth's mission than previous trustees.&lt;br/&gt;Founder of Dartmouth's chapter of Turning Point USA, a right-wing non-profit organization, Tyler Baum '20 said that political activism on campus allows students to learn from their peers' perspectives. Turning Point USA is known for its founder, conservative activist Charlie Kirk, and its Professor Watchlist - on which Dartmouth's women's, gender and sexuality studies professor Eng-Beng Lim is listed. The group seeks to promote fiscal responsibility, free markets and limited government through campus activist programming.&lt;br/&gt;Dartmouth students and Hanover community members canvass for the 2016 New Hampshire Senate election.&lt;br/&gt;Baum said that he founded Dartmouth's chapter of Turning Point USA because he was disappointed with how political discussions in other organizations sometimes devolved into partisan debates.&lt;br/&gt;"Turning Point USA is for people to come together regardless of party or ideology...[before I created Turning Point USA] there wasn't really a place where people from both sides of the aisle could come together and talk about issues," he said.&lt;br/&gt;Baum said that in having non-partisan discussions with his peers, he has at times adapted his own views.&lt;br/&gt;"As a conservative on campus, [it's important for me to learn] from people I may not agree with," he said.&lt;br/&gt;Baum said that in addition to hosting guest speakers, Dartmouth's chapter of Turning Point USA intends to address issues affecting college students, such as free speech on campus and the student debt crisis. He said that Turning Point USA is planning to organize a "free speech ball" event during the fall term in which students can write whatever they want on a large beach ball.&lt;br/&gt;President of the College Democrats Jennifer West '20 said that she became more politically involved than she expected she would be during her first year at Dartmouth because the College's culture is "a breeding ground for political activism."&lt;br/&gt;West added that she was "overwhelmed" with the student body's strong interest in attending the Women's March on Washington in January 2017 after posting about the event in the Dartmouth Class of 2020 Facebook page. Some students, she said, created their own groups to attend the march together following her post.&lt;br/&gt;She explained that political activism is an especially powerful force at the College because as other universities grapple with issues of free speech, Dartmouth seems "relatively isolated" from the controversy surrounding this issue. Instead, West said, she and her peers feel free to speak their minds and disagree with each other in a civil, productive way.&lt;br/&gt;"I have friends with political views that could not be more different than mine, and I think that it is because of Dartmouth that we are able to have productive conversations," West said. "This school really does foster a great sense of community and respect among students."&lt;br/&gt;She added that a debate between the College Republicans and the College Democrats during the spring term successfully maintained a strong policy focus, and that participants did not resort to making snide remarks or ad hominem attacks that have recently become a fixture of national politics.&lt;br/&gt;West also said that while she disagrees with Milo Yiannopoulos, a political commentator closely associated with the alt-right movement, she was glad that he had the opportunity to speak to Dartmouth students without interruption when he visited campus in November 2016. Yiannopoulos's visits to college campuses were the subject of intense media scrutiny in February 2017 when the University of California, Berkeley canceled his talk after 150 student protesters caused $100,000 worth of damage ahead of his scheduled appearance.&lt;br/&gt;West said that she supports the right of an individual to express their opinion peacefully, adding that in this regard, "Dartmouth is really a model for other campuses to follow."&lt;br/&gt;Miller echoed this sentiment, saying "There has never been a part of me that feels I am being silenced."</t>
         </is>
+      </c>
+      <c r="L97" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -4707,10 +5005,13 @@
           <t>Police violence, Anti-racism</t>
         </is>
       </c>
-      <c r="J98" t="inlineStr">
+      <c r="K98" t="inlineStr">
         <is>
           <t>Share on TwitterCourtesy Claudrena Harold, Black Fire U.Va.&lt;br/&gt;Students at a rally in the early 1980s.&lt;br/&gt;Assoc. Prof. Claudrena Harold said the University's Black Student Alliance is "without question" the most important organization on Grounds.&lt;br/&gt;The University's history with racial integration and equality has been a complex one - one that the Black Student Alliance has been at the forefront of since its inception in the 1968-69 academic year.&lt;br/&gt;The first black students at the University&lt;br/&gt;The first black student to attend the University was Gregory H. Swanson, who was admitted to the Law School in 1950 only after he filed a legal suit to gain entry.&lt;br/&gt;The Board of Visitors originally rejected Swanson's application on the basis that "the Constitution and the laws of the State of Virginia provide that white and colored shall not be taught in the same schools," according to their written response.&lt;br/&gt;Despite eventually being granted entry into the Law School, the twenty-five year old did not graduate due to the racial hostility and isolation he experienced while on Grounds. The University's first black graduate was Walter N. Ridley, who was accepted in 1951 and received his degree in 1953.&lt;br/&gt;The BSA was created more than a decade later to represent the growing population of black students on Grounds. Originally known as the Black Students for Freedom, the BSF was a student initiative which has had a variety of goals related to both the University community and the broader Charlottesville community.&lt;br/&gt;"There can be no understanding of the integration of African-Americans into this University without looking at the Black Students for Freedom and the BSA," Harold said. "They are central to the story of racial transformation at U.Va."&lt;br/&gt;BSA's beginnings&lt;br/&gt;College graduate John Charles Thomas was one of the first presidents of the BSA during his undergraduate years from 1968 to 1972, and was actively involved in instituting some of the original programs of the BSA.&lt;br/&gt;"We looked at ourselves as a voice that needed to be asserted at U.Va.," Thomas said. "So we were always at the forefront at arguing for black courses, black professors and more black students. We were pushing for integrating U.Va."&lt;br/&gt;Though Thomas said he remembers having a positive relationship with many faculty members and the administration - who he recalls as being receptive to many of the broad goals of the BSA - the University was not always as progressive as it hoped to be.&lt;br/&gt;A University-wide referendum in the early 1970s indicated most students would endorse, or go on strike for, increasing the percentage of black students to 20 percent, but in 1969 the University was only 1.3 percent black.&lt;br/&gt;"I can remember basically demanding that U.Va. change," Thomas said.&lt;br/&gt;The BSA worked actively to recruit more black students and professors, institute an African-American studies program and also address particular issues around Grounds.&lt;br/&gt;When the Cavaliers scored a touchdown during football games, students would first sing the Southern song "Dixie" before the "The Good Ol' Song" and a man mounted on a horse would carry a Confederate flag around the stadium.&lt;br/&gt;Thomas said he and BSA members were vocal in adamantly protesting the use of the Confederate flag, which they argued has an irrevocable tie to slavery and racial segregation. By the time Thomas graduated in 1972, he said this particular tradition was obsolete.&lt;br/&gt;The BSA was also active in traveling to local and Virginia high schools to encourage young black high school students to apply to and attend the University.&lt;br/&gt;Thomas said he was formally hired by the administration to visit schools - where he would meet with guidance counselors and speak at assemblies in an effort to recruit future black students.&lt;br/&gt;"U.Va. was very well educated and very international. We had scholars from all over the world," Thomas said. "These people in Charlottesville - they were interested in changing the world and I was just one of the young kids who they happened to come upon in that moment who might play a role in that."&lt;br/&gt;Great leaders become great figures&lt;br/&gt;After graduating from the College in 1972, Thomas attended the University's Law School. Upon earning his J.D., Thomas practiced law with a private firm for several years before being appointed to the Virginia Supreme Court.&lt;br/&gt;Thomas was the first African-American justice to sit on Virginia's highest court and also the youngest. His portrait currently hangs in the atrium of the Law School.&lt;br/&gt;But Thomas is only one of the BSA's distinguished and esteemed alumni - a fact which Harold has emphasized as one of the greatest legacies of the BSA.&lt;br/&gt;"Like any organization the Black Student Alliance has experienced its share of changes [and] transformations," Harold said. "It has at times been reflective of the times and it is at times transcended the times. It has pushed the University, but it has also been a critical training ground for African-American leaders who have gone on to do some amazing things."&lt;br/&gt;Like Thomas, Leroy R. Hassell, a 1977 College graduate and BSA member, became a justice on the Virginia Supreme Court. Hassell was the court's first black Chief Justice, serving two terms from 2003 to 2011.&lt;br/&gt;Deborah Saunders-White, who was the president of the BSA in the 1970s, became the first female Chancellor at North Carolina Central University, a historically black college, in 2013.&lt;br/&gt;"The thing about the history of BSA is I am always finding these figures of import," Harold said.&lt;br/&gt;Current BSA President Bryanna Miller, a fourth-year College student, said she feels some of the most exciting events are ones that engage underclassmen to build leadership skills.&lt;br/&gt;For example, the BSA recently hosted its second Black Leadership Academy - a four-day-long retreat targeted at underclassmen to participate in student run workshops. Future programs are then designed by those attendees of the academy, like the Black Man Brunch or charity functions for the homeless.&lt;br/&gt;"Those are the most exciting because it's coming from the next generation of students that are going to lead at the University," Miller said.&lt;br/&gt;The BSA today&lt;br/&gt;According to 2016 figures, the University's undergraduate student body is 6.4 percent black, which equals a little more than 1,000 students. Every black student at the University is a member of the BSA, although regular attendance to meetings and events varies, Miller said.&lt;br/&gt;The BSA has several subcommittees focused on topics like academic and career development, leadership development and political action. The organization has dozens of events on Grounds each academic year - ranging from small study groups to leadership programs to the Black Ball, which boasts more than 400 attendees.&lt;br/&gt;One particular annual event, Black Culture Week, has been put on annually by the BSA since 1970. It celebrated its 45th anniversary in 2015.&lt;br/&gt;The BSA has also participated in several major protests in recent months - another legacy of the organization which remains strong both here on Grounds and in the greater Charlottesville community.&lt;br/&gt;From Thomas's protest of the use of the Confederate flag during his time at the University to current initiatives, the BSA has always had an active voice in shaping the social climate on Grounds.&lt;br/&gt;In the 1970s, the BSA was a key student organization protesting for divestment of the University from its stockholdings in South Africa during apartheid and advocating in support of affirmative action. The BSA has also episodically been involved in protesting for a higher living wage for workers at the University for decades as well as against instances of police brutality against blacks.&lt;br/&gt;In response to the violent arrest of then-third-year College student Martese Johnson in March 2015, Black Dot - with the support of the BSA - rallied hundreds of students, faculty and community members in protest of the discord between law enforcement and black people in both locally and nationally.&lt;br/&gt;In September 2016, the BSA staged a die-in outside of Old Cabell Hall to protest police brutality and show support for the national Black Lives Matter movement.&lt;br/&gt;The BSA also frequently co-sponsors events with other organizations and engages with other student voices to combat specific social or political concerns.&lt;br/&gt;Overall, Miller said she thinks black students need to be engaged and actively supported here by not only other students, but faculty and administration as well.&lt;br/&gt;"Black students need to be reassured that they matter and that their issues matter," Miller said. "Their issues are being valued, their accomplishments are being valued."&lt;br/&gt;The BSA for decades now has been a central part of connecting and engaging students. The BSA is the anchor of black U.Va. and the wider University community, Harold said.&lt;br/&gt;"That an organization can celebrate 48 years of history and can say that there has never been a year or there has been an extended period where they have not been in existence - is remarkable," Harold added.</t>
         </is>
+      </c>
+      <c r="L98" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -4750,10 +5051,13 @@
           <t>Tuition, fees, financial aid, Public funding for higher education, Labor and work</t>
         </is>
       </c>
-      <c r="J99" t="inlineStr">
+      <c r="K99" t="inlineStr">
         <is>
           <t>For University of Montana freshman Jake Aguirre, a tuition increase poses such a risk to his education that he slept on the grass in the Oval in protest.&lt;br/&gt;Aguirre brought his sleeping bag, computer and backpack full of books to continue doing his schoolwork. He joined over 20 students in tents as part of a two-day protest led by the Missoula Community-Campus Coalition against impending budget cuts and layoffs.&lt;br/&gt;"They are threatening to up tuition, and if they do, I'll have to leave," Aguirre said. He said his major, ecological restoration, isn't offered in many other places, and he has become attached to UM.&lt;br/&gt;"I don't want to leave," he said. "I like it here."&lt;br/&gt;Due to dropping enrollment (26 percent in the past six years), and an expected decrease of Montana University System funds by around $11 million, UM is faced with upcoming cuts to faculty, staff and possibly entire programs prior to fall of 2018.&lt;br/&gt;UM's budget for the upcoming 2017-18 school year, is about $3 million lower than this year's. This particular cut, however, is mostly due to a loss of tuition revenue, as the Office of the Commissioner of Higher Education and the Board of Regents are expected to give UM the same amount of state funding as they did last year, essentially floating the University through a "transition year." It isn't until fall of 2018 that the legislative cuts will hit, meaning UM's 2018-19 budget will likely take a far bigger dip.&lt;br/&gt;Vice President for Administration and Finance Michael Reid has said in budget committee meetings that he doesn't expect any tuition increases that will entirely make up for a decrease in state revenue. Reid's department estimates that a 1 percent increase in resident tuition results in around $300,000 in revenue, so resident tuition would have to increase by roughly 10 percent to account for this year's decrease.&lt;br/&gt;Decisions about a tuition increase won't be made until the Board of Regents meeting in May. Students, faculty, staff and community members gathered on the Oval at noon on Tuesday to protest large increases and suggest alternatives.&lt;br/&gt;Standing in front of Main Hall before a crowd of about 50 people, Hannah Gale outlined three demands. She called for tuition to increase only by single digits (somewhere between 3 to 5 percent), for cuts to be distributed equally across programs instead of targeting specific ones, and to increase state financial support for the University from 40 percent to 50 percent.&lt;br/&gt;History professor Mehrdad Kia followed with a speech that called for different groups on campus to speak up for each other and stand united. He made his point with a slightly altered version of a well-known poem:&lt;br/&gt;"They first came for the staff, and I didn't say anything because I wasn't a member of the UM staff. Then they came for the adjuncts and the lecturers, and I didn't say anything because I was neither an adjunct nor a lecturer. Then they came for senior faculty, and they offered them early retirement packages, and I didn't say anything because I was not a senior faculty member. And then they came for me, and there was no one left to speak on my behalf." +1&lt;br/&gt;Professor Mehrdad Kia, standing beside protest organizers, spoke out against program defunding and what he believes to be unfair actions against students, at the Occupy the Oval demonstration April 4, 2017.  Isabella Grannis / Montana Kaimin@isabellagrannis&lt;br/&gt;The administration has made clear that employee cuts are inevitable. Currently UM spends 81 percent of its budget on personnel. Administrators have stated that they are aiming for a 18-to-1 faculty-to-student ratio. If UM's enrollment decreases to 11,000 students, as officials expect it will, personnel spending would make up 68 percent of the University's budget.&lt;br/&gt;Curtis Schiwal, a humanities student and member of the Missoula Campus-Community Coalition, International Workers of the World and Divest UM, said 12 different campus groups joined together for the two-day event. He said it's a moral and ethical problem to place the budget crisis burden on the backs of students, especially low-income students who can't afford a tuition increase.&lt;br/&gt;"Those double-digit tuition raises, which would raise tuition by $600 to $1,000 for in-state students, is something that couldn't really be coped with," Schiwal said. "And it's something that is unfair as well."&lt;br/&gt;Program prioritization, which will rank UM's academic programs based on a set of to-be-determined metrics, is also not the way to handle a budget crisis, Schiwal said. Distributing cuts equally across campus would help preserve smaller programs that might not fare well in a ranking system, he said.&lt;br/&gt;Schiwal has shared the MCCC's three demands with Interim President Sheila Stearns and Commissioner of Higher Education Clayton Christian, who agreed with the group's desire to mitigate damage to students and programs. Schiwal said Stearns and Christian are doing the best they can in a tough situation, though he doesn't think students should be complacent throughout the process.&lt;br/&gt;"This group and myself have learned to be mistrustful of the administration," Schiwal said. "So while we think that they are doing their best, we're going to remain vigilant. People can slip up, and people can lose sight of what's actually important here. Be it balancing the budget, or actually caring about students and their futures."&lt;br/&gt;Stearns and UM Director of Communications Paula Short could not be reached for comment before the publishing of this article.</t>
         </is>
+      </c>
+      <c r="L99" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -4793,10 +5097,13 @@
           <t>Anti-racism, Campus climate, University governance, admin, policies, programs, curriculum, Hate speech, Hate crimes/Anti-minority violence</t>
         </is>
       </c>
-      <c r="J100" t="inlineStr">
+      <c r="K100" t="inlineStr">
         <is>
           <t>In the past two years, the University of Michigan has seen several acts of hate targeted at people of color and minority groups across campus.&lt;br/&gt;In September 2016, flyers advocating white supremacy were found on campus posting walls. In February, engineering students received racist and anti-Semitic emails from hacked email accounts. This September, the Rock, a campus landmark, was found graffitied with anti-Latino and pro-Trump expressions. In October, racist slurs were found on the residence hall doors of three Black students in West Quad Residence Hall.   &lt;br/&gt;In the aftermath of these incidents, campus communities have not stood idly by. Hundreds of students have rallied against racist flyering, graffiti and a variety of other attacks. In late September, Rackham student Dana Greene knelt in the Diag for 21 hours to protest racism on campus and across the country; dozens of other students joined the peaceful protest.    &lt;br/&gt;The University administration has taken steps to respond to acts of hate and its historically low minority enrollment. In October 2016, the University launched its five-year Diversity, Equity and Inclusion strategic plan, which aims to foster a diverse and inclusive campus, while also supporting inclusive scholarship and teaching. Diversity has been especially difficult in the University, since practicing affirmative action has been banned in the state since 2014 despite the University's attempts to appeal the vote.  &lt;br/&gt;When the plan was implemented, then-Provost Martha Pollack, who is now the president of Cornell University, said the recent racist incidents only emphasized the need for the plan.&lt;br/&gt;"It's only human to respond with anger and sometimes with fear, emotions that have been felt deeply on this campus," she said. "I share the grief and outrage felt by our students, faculty and staff. We must cling to the vision of what the world must be ... and that is what the Diversity, Equity and Inclusion plan is all about."&lt;br/&gt;However, also pertinent to DEI, the University ranked last in terms of socioeconomic mobility and diversity among top public universities. According to a report by the Equality of Opportunity Project, which was highlighted by The Upshot - a data analytics section of the New York Times- 66 percent of students come from the top 20 percent of the income distribution and students have the highest median family income of 27 "highly selective" public colleges.&lt;br/&gt;The DEI plan has been criticized for failing to foster a diverse environment and for failing to put a stop to racist incidents. After the racist emails were sent out in February, students protested outside University President Mark Schlissel's house calling for "action, not emails," referencing the University's digital statement, which showed its support for those attacked, but no further action.&lt;br/&gt;"Schissel WYA" is a common rally of for University students, criticizing University President Mark Schlissel's response to the incidents. In mid-September, students gathered in front of the president's home and posted flyers on his door. Schlissel was at a family event during this time.&lt;br/&gt;Postdoctoral fellow Austin McCoy was not surprised by the University's response.&lt;br/&gt;"From the administration, I anticipate them sending out probably an email and saying that they condemn the acts and then that they're investigating, but other than that, I don't know what else the administration plans to do," he said in February. &lt;br/&gt;However, such incidences and responses are not unique to the University of Michigan campus. Post-election, campus climate and rallying students have been points of debate across the country.&lt;br/&gt;Conservative criticism refers to liberal students as too sensitive and ignorant of free speech - worried for conservative students and their lack of voice on more Democratic campuses. The University of Chicago even shut down the concept of "safe spaces" - sparking what some call a clear rebuke of political correctness. Liberal students, however, hope to protest the turn of the administration along with the fear of rhetoric that they deem bigotry and do not wish to give such thought a platform.&lt;br/&gt;This article is part one of a series in which The Michigan Daily looks at colleges similar to the University of Michigan on the issue of reacting in a tense campus climate. As the University administration and students face their own numerous bias incidents, The Daily will look at other schools to compare and contrast in incidents, administration response and student activism, whether it is a difference in religion, culture, politics or policies.&lt;br/&gt;Cornell University&lt;br/&gt;Juliana Rosana Montejo graduated from Cornell University in May 2017. Montejo is Guatemalan and came from a predominantly white high school. She said when she entered the university in 2013, she wasn't really aware of incidents on campus.&lt;br/&gt;"Long story short, every semester there has been something," she said.&lt;br/&gt;Cornell University, located in Ithaca, N.Y. - a blue state - ranks similarly to the University of Michigan in terms of the Upshot's SES status - albeit in the private school category among other Ivy Leagues. Out of 14,907 undergraduate students, Cornell has 6,462 students of color - 43.34 percent. In the graduate program, it is 17.94 percent. Cornell also uses affirmative action in admission.  &lt;br/&gt;In fall 2013, a campus organization that promotes Cornell sporting events attempted to increase support for an upcoming football game by creating a "Cinco de Octubre" event, which incorporated racist caricature depictions of Mexican Americans. Montejo said there was a prize given to whoever dressed up as the "best Mexican."&lt;br/&gt;Since then, Montejo said, there have been a variety of incidents that have primarily targeted Black people and people of color generally. She said she met many people involved with activism at Cornell and in her senior year, she served as vice president of diversity and inclusion on the Cornell Student Assembly.&lt;br/&gt;"A big part of why I started getting more involved was that there had just been a lot of things building up, and I think we were kind of at a culmination of, 'Oh there were some of these undertones there already,' and now it's kind of coming to a point where it's kind of exacerbated," she said.&lt;br/&gt;Montejo also said such hateful incidents became more prevalent after the 2016 election. She explained Cornell is known to be a liberal school; subsequently, there is a claim that conservative ideas are oppressed on campus.&lt;br/&gt;"The conversation wasn't automatically, 'What can we do for people of color?'" she said. "A lot of it became, 'Look at these poor conservative students who aren't able to speak their minds.'"&lt;br/&gt;She said at the end of 2016 and in early 2017, there were two resolutions brought before the student assembly to create task forces to investigate why there are so many liberal professors at the school. There have also been calls for the university to do more to protect conservative speakers who come to campus. She said there have been more visibly proactive actions to help conservative students.&lt;br/&gt;Montejo also said that whereas prior to the election, there seemed to be one or two major acts of hate every semester, there is now something happening all the time.&lt;br/&gt;Last month, a Cornell student was arrested by Ithaca police for a hate crime, according to the The Cornell Daily Sun. A Black student, who asked to remain anonymous, told the Sun he confronted four or five white men who were shouting racist slurs at him; they then proceeded to beat him.&lt;br/&gt;In Michigan, during one of the protests after the racist vandalism, an individual was punched by a white man who also called them racial slurs.&lt;br/&gt;Black Students United at Cornell released a statement saying the perpetrators were members of the Psi Upsilon fraternity, which already had its recognition revoked on campus. The building is to be remade into a multicultural center.&lt;br/&gt;Pollack, now Cornell's president, released a statement in response to the incident - and others preceding it - citing steps the administration will take to create a more equitable and inclusive campus. Among them was a promise to take disciplinary action against the perpetrators of the aforementioned attack and a commitment to not reinstating the fraternity.&lt;br/&gt;"I will not tell you 'this is not who we are,' as the events of the past few weeks belie that. But it is absolutely not who we want to be," the statement read. "The leadership team and I have been working throughout the weekend, and we will continue to do so, to develop and implement steps to be a more equitable, inclusive and welcoming university."&lt;br/&gt;Meanwhile, Black Students United declared a "state of emergency for black students" in response to the incident. The group blamed the university for creating the Campus Code of Conduct, which protects white supremacists' hate speech. They recognized it would be difficult to change the policy but felt it would be possible with help from the greater university community.&lt;br/&gt;In mid-September 2016, Black Students United handed a list of demands to Pollack, including racial sensitivity training for all employees and a space for Black students on campus.  &lt;br/&gt;Prior to creating an official list, Black Students United members met with Dean of Students Vijay Pendakur right after the assault. They were frustrated Pollack did not reach out to them until three days after the assault; they were also frustrated that many of the ideas they brought up in their meeting with Pendakur were presented in Pollack's letter, without recognition. &lt;br/&gt;Anti-Semitic posters have also been seen on Cornell's campus and Pollack has denounced these incidents as well.&lt;br/&gt;Looking at responses to acts of hate on Cornell's campus overall, Montejo said there appears to be a lot of support.&lt;br/&gt;"In terms of climate change I think to your face it seems like there's a lot of support," she said. "But behind the scenes, there's a lot of weird antagonism that's going on."&lt;br/&gt;Beth Garrett, Cornell's thirteenth president, passed away after a battle with colon cancer in March 2016. However, according to Montejo, when Garrett came into office she hired Ryan Lombardi, vice president for student and campus life. According to Montejo, Lombardi re-envisioned the Office of the Dean of Students and the dean of students position as one that would be very focused on diversity and inclusion issues.&lt;br/&gt;Additionally, she said Cornell has used polls to gauge how students feel about diversity and inclusion issues - the University has also had campus climate polls - and has always addressed campus climate even without major incidents occurring. Cornell has diversity officers through its Diversity and Inclusion initiative to better promote a welcoming and inclusive campus, as well as a bias reporting program.&lt;br/&gt;Montejo explained the administration always sends out statements to the campus community in response.&lt;br/&gt;Montejo noted Ivy League schools are definitely targeted. In November 2015, for example, hundreds of members of the Yale University community marched in support of minority students who felt they were not fully included on campus. According to The Washington Post, protesters rallied in support of women of color, faculty of color and ethnic studies; one person carried a sign that read: "Your move Yale."&lt;br/&gt;The theory that prominent, progressive schools are being targeted has floated around before - especially with Washtenaw as a blue county in a newly turned red state. In an earlier interview with The Daily, Schlissel said there might not be a way to mitigate the target on the University's back.&lt;br/&gt;"I think that part of being a prominent university, taking clear positions on things, having large numbers of very successful graduates out there in the world, being on TV all the time, being in the media all the time means that what happens here gets noticed," he said. "That's the sort of other side of this double-edged sword of being famous and prominent. ... It's because of our prominence that provocateurs realize they can use us as a platform that the national media will pay attention to, to spread their terrible, thoughtless, degrading, awful ideas. They're using us."&lt;br/&gt;Montejo said she believes Cornell is generally diverse. According to Cornell's Composition Dashboard from fall 2016, 39.5 percent of undergraduates were white, while 42.3 percent were from minority groups. Despite that, she said groups that have disproportionate power on campus include those that are white, including the Interfraternity Council.&lt;br/&gt;"I felt really compelled and pushed to join a Panhellenic sorority, and while I had a great experience there, it did kind of feel like there was a disproportionate amount of influence of power in that structure because of its whiteness," she said.  &lt;br/&gt;Though the administration has taken a lot of positive steps, Montejo said there are gaps that need to be filled. She said she feels there is a lot of movement on reactive measures but not nearly as much around proactive members.&lt;br/&gt;In an email response, Cornell's Media Relations Office pointed The Daily to several of its official statements.&lt;br/&gt;University of California at Berkeley&lt;br/&gt;Some say Berkeley has been the poster child of college campus activism this year - the pushback against controversial speakers has been widely documented in the media. Notably, while activism has escalated to violence, much of it has occurred in the campus vicinity, not specifically at the university.&lt;br/&gt;Billy Curtis is the director of the Gender Equity Resource Center at University of California at Berkeley. Strictly in terms of reports, Curtis said, there has been an uptick, but quickly explained that like with incidents of sexual violence, as there are increases in education and awareness, there are more reports. It's unclear whether there are more incidents or more reports.&lt;br/&gt;Another challenge UC-Berkeley faces, according to Curtis, has to do with protocols for a response. Many victims and members of communities that are targeted feel the chancellor needs to respond.&lt;br/&gt;"We're trying to figure out always, when does the chancellor respond? What does that response look like? How do people feel cared for, seen, heard, tended to?" he said. "I think that's the biggest challenge because too often what we're really dealing with isn't necessarily just a campus climate issue, we're dealing with our sociological problems of the United States."&lt;br/&gt;UC-Berkeley is taking steps to make the campus more inclusive and address the needs of students from marginalized communities. The Division of Equity &amp; Inclusion provides a variety of programs and services.&lt;br/&gt;On Sept. 1, the division launched the Campus Climate, Community Engagement and Transformation unit, whose mission is to focus on "reshaping and influencing policies and practices that increase opportunities, advance social justice and create equitable experiences for all groups, with a special focus on marginalized and underserved populations."&lt;br/&gt;The initiative's website also highlights results of a spring 2013 campus climate survey, which showed 1 in 4 community members have experienced exclusion on campus. It also showed undergraduates who are not African American overestimate the inclusivity of the climate for the group. For instance, 89 percent of Asian students and 87 percent of white students rated the climate as "respectful" or "very respectful" for African Americans; African Americans rated the climate as 47 percent for the categories. Additionally, on the survey, a top concern was not having channels through which to report discrimination and the notion that faculty judge students based on their perceived identities.    &lt;br/&gt;That being said, in fall 2017, 2.9 percent of enrolled freshmen at UC-Berkeley were African American or Black, 9.9 percent were Mexican American or Chicano, 3.7 percent were labeled "other Hispanic/Latino." White students constituted 24.5 percent of the freshman class.&lt;br/&gt;Other initiatives through UC-Berkeley's diversity division include a Campus Climate Speaker Series, which brings scholars and activists to campus to address related issues, and Innovation Grants, which provide funding for projects focused on increasing equity and inclusion on campus.&lt;br/&gt;Still, UC-Berkeley has seen hate acts in the past year. In September, posters listing 13 specific community members and identifying them as "terrorist supporters" were found on campus, according to The Daily Californian. Some of the victims in the past had vocalized their support for Palestinian divestment from Israel.&lt;br/&gt;In a statement sent to the university community, UC-Berkeley Chancellor Carol Christ condemned the acts. She highlighted the school's Principles of Community, among which are a commitment to respect the differences and commonalities of all people.&lt;br/&gt;"Berkeley is better than what these incidents reflect," the statement read. "Many things contribute to the fact that we are the nation's number one public university, and a strong component is the care, respect and esteem which we have for our fellow campus community members. As we move into the events of next week, please join me in upholding these values."&lt;br/&gt;Four days after the posters were found, conservative writer Milo Yiannopoulos spoke at Berkeley. According to The Daily Californian, Yiannopoulos was originally invited to speak by the student group the Berkeley Patriot - a conservative group on campus - as part of the "Free Speech Week," in which several conservative speakers were coming to campus. Amid confusion surrounding the event and the Berkeley Patriot actually filing a complaint with the Department of Justice, claiming Berkeley was infringing free speech rights, the event was canceled. Still, Yiannopoulos - and other speakers - came to campus and were met by a crowd of protesters.&lt;br/&gt;In an interview with The Daily Californian, Pranav Jandhyala - a news editor for the Berkeley Patriot and who founded the organization that invited Ann Coulter - explained the situation became too complicated and the group had to pull out of the event.&lt;br/&gt;"It became a situation that we just had to get out of because of the complications," Jandhyala said.&lt;br/&gt;Meanwhile, the Yvette Felarca, an organizer for Berkeley's By Any Means Necessary pointed to the need for a sanctuary space.&lt;br/&gt;"To protect the community (and make) it a sanctuary campus, that means actively defending it," Felarca said.&lt;br/&gt;The University faced its own slew of controversial speakers - the latest being Charles Murray, known for "The Bell Curve," which argues the correlation of IQ and race. McCoy said speakers like Murray use student anger as a platform.&lt;br/&gt;"I'm not really going to say much about what's his name -- Charles Murray -- I don't really care about Charles Murray, I think he's irrelevant," he said. "I think he's just trying to use protests, I think he's trying to use student anger to rebuild his career. So, think about this. He has to use students to get a come-up."&lt;br/&gt;LSA senior Ben Decatur, co-chair of the AEI Executive Council at the University, defended Murray's right to speak on campus.&lt;br/&gt;"If the hosts of tonight's program, in collaboration with University representatives, believe that the protesters are interfering unduly with the speaker's freedom of expression, those protesters will be warned by a University administrator," Decatur said. "If warnings are not heeded and interference continues, the individuals responsible may be removed from the building."&lt;br/&gt;Berkeley freshman Justin Kim serves on the Hall Association at UC-Berkeley. In an interview with The Daily, he described the controversy surrounding Yiannopoulos's visit to campus. He said there were police and blockades for the entire week around Sproul Plaza, where the event took place.&lt;br/&gt;In terms of how the school responds, Kim explained the Berkeley Police Department and administration have worked together to send email advisories about crimes on campus to the community.&lt;br/&gt;"During Free Speech Week, or when it was supposed to happen ... even leading up to it, we got notifications to avoid the area," he said.&lt;br/&gt;He noted that Christ released a statement, which stated the university is committed to free speech, as exemplified by the speakers on campus, even though they put forth ideals that "run counter" to those of the university.&lt;br/&gt;"To provide the security necessary to protect the community, we have had to close buildings, relocate students and workers, bring to campus a police presence that some find intimidating, and spend money that we would have much rather put toward our academic and research mission," the statement read.&lt;br/&gt;Kim explained earlier in the fall there was an event in which UC-Berkeley students could ask Christ any question. There is also a way for students to write letters to the chancellor, which are directly delivered by the president of the Associated Students of the University of California - the UC-Berkeley student government.&lt;br/&gt;Regarding hate acts and the reactions they prompt, Curtis explained the campus climate shifts based on the level to which the incident rises.&lt;br/&gt;"Someone writing something on a residence board in a residence hall on one floor, I may be aware of it, but it usually doesn't rise to the level of impacting a larger community because it's a one-off - unless there are enough instances in the residence halls that are targeting folks, and students are feeling like, 'Wow, there's a lot of racist things, or a lot of anti-Semitic things said,' and that's happened over the years," he said. "But all of a sudden it starts to bubble up."&lt;br/&gt;Graffiti on a building, he explained, will rise to different levels because it is far more public and more people see it. He said it creates a different level of response.&lt;br/&gt;Curtis also noted UC-Berkeley has been in the media as a result of certain speakers coming to campus and impacting the campus climate. Students, for example, can report that they feel unsafe and unwelcome on the campus in response to an event like that.   &lt;br/&gt;He explained that while many programs and offices work to educate the campus and make it more safe, inclusive and accessible for marginalized groups, racism and other forms of bigotry are still prevalent in the United States. Due to a variety of reasons, he explained, the campus climate changes.&lt;br/&gt;"It's not static, we're not working in a place where everyone remains the same forever more, or there's little turnover," he said. "We have large turnover because our student body turns over, and they're coming from their communities and their experiences ... and in the modern era - the modern era of information and social media - we're now impacted by things that happen in the virtual world. The things we may create on campus don't necessarily stop or even mitigate the stuff around hate and bias acts; (the two) can work in concert but I've not seen it stop."</t>
         </is>
+      </c>
+      <c r="L100" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -4841,10 +5148,13 @@
           <t>Anti-racism, Campus climate, Immigration (For), Hate speech, White supremacy (Against)</t>
         </is>
       </c>
-      <c r="J101" t="inlineStr">
+      <c r="K101" t="inlineStr">
         <is>
           <t>In the past two years, the University of Michigan has seen several acts of hate targeted at people of color and minority groups across campus.&lt;br/&gt;In September 2016, flyers advocating white supremacy were found on campus posting walls. In February, engineering students received racist and anti-Semitic emails from hacked email accounts. This September, the Rock, a campus landmark, was found graffitied with anti-Latino and pro-Trump expressions. In October, racist slurs were found on the residence hall doors of three Black students in West Quad Residence Hall.   &lt;br/&gt;In the aftermath of these incidents, campus communities have not stood idly by. Hundreds of students have rallied against racist flyering, graffiti and a variety of other attacks. In late September, Rackham student Dana Greene knelt in the Diag for 21 hours to protest racism on campus and across the country; dozens of other students joined the peaceful protest.    &lt;br/&gt;The University administration has taken steps to respond to acts of hate and its historically low minority enrollment. In October 2016, the University launched its five-year Diversity, Equity and Inclusion strategic plan, which aims to foster a diverse and inclusive campus, while also supporting inclusive scholarship and teaching. Diversity has been especially difficult in the University, since practicing affirmative action has been banned in the state since 2014 despite the University's attempts to appeal the vote.  &lt;br/&gt;When the plan was implemented, then-Provost Martha Pollack, who is now the president of Cornell University, said the recent racist incidents only emphasized the need for the plan.&lt;br/&gt;"It's only human to respond with anger and sometimes with fear, emotions that have been felt deeply on this campus," she said. "I share the grief and outrage felt by our students, faculty and staff. We must cling to the vision of what the world must be ... and that is what the Diversity, Equity and Inclusion plan is all about."&lt;br/&gt;However, also pertinent to DEI, the University ranked last in terms of socioeconomic mobility and diversity among top public universities. According to a report by the Equality of Opportunity Project, which was highlighted by The Upshot - a data analytics section of the New York Times- 66 percent of students come from the top 20 percent of the income distribution and students have the highest median family income of 27 "highly selective" public colleges.&lt;br/&gt;The DEI plan has been criticized for failing to foster a diverse environment and for failing to put a stop to racist incidents. After the racist emails were sent out in February, students protested outside University President Mark Schlissel's house calling for "action, not emails," referencing the University's digital statement, which showed its support for those attacked, but no further action.&lt;br/&gt;"Schissel WYA" is a common rally of for University students, criticizing University President Mark Schlissel's response to the incidents. In mid-September, students gathered in front of the president's home and posted flyers on his door. Schlissel was at a family event during this time.&lt;br/&gt;Postdoctoral fellow Austin McCoy was not surprised by the University's response.&lt;br/&gt;"From the administration, I anticipate them sending out probably an email and saying that they condemn the acts and then that they're investigating, but other than that, I don't know what else the administration plans to do," he said in February. &lt;br/&gt;However, such incidences and responses are not unique to the University of Michigan campus. Post-election, campus climate and rallying students have been points of debate across the country.&lt;br/&gt;Conservative criticism refers to liberal students as too sensitive and ignorant of free speech - worried for conservative students and their lack of voice on more Democratic campuses. The University of Chicago even shut down the concept of "safe spaces" - sparking what some call a clear rebuke of political correctness. Liberal students, however, hope to protest the turn of the administration along with the fear of rhetoric that they deem bigotry and do not wish to give such thought a platform.&lt;br/&gt;This article is part one of a series in which The Michigan Daily looks at colleges similar to the University of Michigan on the issue of reacting in a tense campus climate. As the University administration and students face their own numerous bias incidents, The Daily will look at other schools to compare and contrast in incidents, administration response and student activism, whether it is a difference in religion, culture, politics or policies.&lt;br/&gt;Cornell University&lt;br/&gt;Juliana Rosana Montejo graduated from Cornell University in May 2017. Montejo is Guatemalan and came from a predominantly white high school. She said when she entered the university in 2013, she wasn't really aware of incidents on campus.&lt;br/&gt;"Long story short, every semester there has been something," she said.&lt;br/&gt;Cornell University, located in Ithaca, N.Y. - a blue state - ranks similarly to the University of Michigan in terms of the Upshot's SES status - albeit in the private school category among other Ivy Leagues. Out of 14,907 undergraduate students, Cornell has 6,462 students of color - 43.34 percent. In the graduate program, it is 17.94 percent. Cornell also uses affirmative action in admission.  &lt;br/&gt;In fall 2013, a campus organization that promotes Cornell sporting events attempted to increase support for an upcoming football game by creating a "Cinco de Octubre" event, which incorporated racist caricature depictions of Mexican Americans. Montejo said there was a prize given to whoever dressed up as the "best Mexican."&lt;br/&gt;Since then, Montejo said, there have been a variety of incidents that have primarily targeted Black people and people of color generally. She said she met many people involved with activism at Cornell and in her senior year, she served as vice president of diversity and inclusion on the Cornell Student Assembly.&lt;br/&gt;"A big part of why I started getting more involved was that there had just been a lot of things building up, and I think we were kind of at a culmination of, 'Oh there were some of these undertones there already,' and now it's kind of coming to a point where it's kind of exacerbated," she said.&lt;br/&gt;Montejo also said such hateful incidents became more prevalent after the 2016 election. She explained Cornell is known to be a liberal school; subsequently, there is a claim that conservative ideas are oppressed on campus.&lt;br/&gt;"The conversation wasn't automatically, 'What can we do for people of color?'" she said. "A lot of it became, 'Look at these poor conservative students who aren't able to speak their minds.'"&lt;br/&gt;She said at the end of 2016 and in early 2017, there were two resolutions brought before the student assembly to create task forces to investigate why there are so many liberal professors at the school. There have also been calls for the university to do more to protect conservative speakers who come to campus. She said there have been more visibly proactive actions to help conservative students.&lt;br/&gt;Montejo also said that whereas prior to the election, there seemed to be one or two major acts of hate every semester, there is now something happening all the time.&lt;br/&gt;Last month, a Cornell student was arrested by Ithaca police for a hate crime, according to the The Cornell Daily Sun. A Black student, who asked to remain anonymous, told the Sun he confronted four or five white men who were shouting racist slurs at him; they then proceeded to beat him.&lt;br/&gt;In Michigan, during one of the protests after the racist vandalism, an individual was punched by a white man who also called them racial slurs.&lt;br/&gt;Black Students United at Cornell released a statement saying the perpetrators were members of the Psi Upsilon fraternity, which already had its recognition revoked on campus. The building is to be remade into a multicultural center.&lt;br/&gt;Pollack, now Cornell's president, released a statement in response to the incident - and others preceding it - citing steps the administration will take to create a more equitable and inclusive campus. Among them was a promise to take disciplinary action against the perpetrators of the aforementioned attack and a commitment to not reinstating the fraternity.&lt;br/&gt;"I will not tell you 'this is not who we are,' as the events of the past few weeks belie that. But it is absolutely not who we want to be," the statement read. "The leadership team and I have been working throughout the weekend, and we will continue to do so, to develop and implement steps to be a more equitable, inclusive and welcoming university."&lt;br/&gt;Meanwhile, Black Students United declared a "state of emergency for black students" in response to the incident. The group blamed the university for creating the Campus Code of Conduct, which protects white supremacists' hate speech. They recognized it would be difficult to change the policy but felt it would be possible with help from the greater university community.&lt;br/&gt;In mid-September 2016, Black Students United handed a list of demands to Pollack, including racial sensitivity training for all employees and a space for Black students on campus.  &lt;br/&gt;Prior to creating an official list, Black Students United members met with Dean of Students Vijay Pendakur right after the assault. They were frustrated Pollack did not reach out to them until three days after the assault; they were also frustrated that many of the ideas they brought up in their meeting with Pendakur were presented in Pollack's letter, without recognition. &lt;br/&gt;Anti-Semitic posters have also been seen on Cornell's campus and Pollack has denounced these incidents as well.&lt;br/&gt;Looking at responses to acts of hate on Cornell's campus overall, Montejo said there appears to be a lot of support.&lt;br/&gt;"In terms of climate change I think to your face it seems like there's a lot of support," she said. "But behind the scenes, there's a lot of weird antagonism that's going on."&lt;br/&gt;Beth Garrett, Cornell's thirteenth president, passed away after a battle with colon cancer in March 2016. However, according to Montejo, when Garrett came into office she hired Ryan Lombardi, vice president for student and campus life. According to Montejo, Lombardi re-envisioned the Office of the Dean of Students and the dean of students position as one that would be very focused on diversity and inclusion issues.&lt;br/&gt;Additionally, she said Cornell has used polls to gauge how students feel about diversity and inclusion issues - the University has also had campus climate polls - and has always addressed campus climate even without major incidents occurring. Cornell has diversity officers through its Diversity and Inclusion initiative to better promote a welcoming and inclusive campus, as well as a bias reporting program.&lt;br/&gt;Montejo explained the administration always sends out statements to the campus community in response.&lt;br/&gt;Montejo noted Ivy League schools are definitely targeted. In November 2015, for example, hundreds of members of the Yale University community marched in support of minority students who felt they were not fully included on campus. According to The Washington Post, protesters rallied in support of women of color, faculty of color and ethnic studies; one person carried a sign that read: "Your move Yale."&lt;br/&gt;The theory that prominent, progressive schools are being targeted has floated around before - especially with Washtenaw as a blue county in a newly turned red state. In an earlier interview with The Daily, Schlissel said there might not be a way to mitigate the target on the University's back.&lt;br/&gt;"I think that part of being a prominent university, taking clear positions on things, having large numbers of very successful graduates out there in the world, being on TV all the time, being in the media all the time means that what happens here gets noticed," he said. "That's the sort of other side of this double-edged sword of being famous and prominent. ... It's because of our prominence that provocateurs realize they can use us as a platform that the national media will pay attention to, to spread their terrible, thoughtless, degrading, awful ideas. They're using us."&lt;br/&gt;Montejo said she believes Cornell is generally diverse. According to Cornell's Composition Dashboard from fall 2016, 39.5 percent of undergraduates were white, while 42.3 percent were from minority groups. Despite that, she said groups that have disproportionate power on campus include those that are white, including the Interfraternity Council.&lt;br/&gt;"I felt really compelled and pushed to join a Panhellenic sorority, and while I had a great experience there, it did kind of feel like there was a disproportionate amount of influence of power in that structure because of its whiteness," she said.  &lt;br/&gt;Though the administration has taken a lot of positive steps, Montejo said there are gaps that need to be filled. She said she feels there is a lot of movement on reactive measures but not nearly as much around proactive members.&lt;br/&gt;In an email response, Cornell's Media Relations Office pointed The Daily to several of its official statements.&lt;br/&gt;University of California at Berkeley&lt;br/&gt;Some say Berkeley has been the poster child of college campus activism this year - the pushback against controversial speakers has been widely documented in the media. Notably, while activism has escalated to violence, much of it has occurred in the campus vicinity, not specifically at the university.&lt;br/&gt;Billy Curtis is the director of the Gender Equity Resource Center at University of California at Berkeley. Strictly in terms of reports, Curtis said, there has been an uptick, but quickly explained that like with incidents of sexual violence, as there are increases in education and awareness, there are more reports. It's unclear whether there are more incidents or more reports.&lt;br/&gt;Another challenge UC-Berkeley faces, according to Curtis, has to do with protocols for a response. Many victims and members of communities that are targeted feel the chancellor needs to respond.&lt;br/&gt;"We're trying to figure out always, when does the chancellor respond? What does that response look like? How do people feel cared for, seen, heard, tended to?" he said. "I think that's the biggest challenge because too often what we're really dealing with isn't necessarily just a campus climate issue, we're dealing with our sociological problems of the United States."&lt;br/&gt;UC-Berkeley is taking steps to make the campus more inclusive and address the needs of students from marginalized communities. The Division of Equity &amp; Inclusion provides a variety of programs and services.&lt;br/&gt;On Sept. 1, the division launched the Campus Climate, Community Engagement and Transformation unit, whose mission is to focus on "reshaping and influencing policies and practices that increase opportunities, advance social justice and create equitable experiences for all groups, with a special focus on marginalized and underserved populations."&lt;br/&gt;The initiative's website also highlights results of a spring 2013 campus climate survey, which showed 1 in 4 community members have experienced exclusion on campus. It also showed undergraduates who are not African American overestimate the inclusivity of the climate for the group. For instance, 89 percent of Asian students and 87 percent of white students rated the climate as "respectful" or "very respectful" for African Americans; African Americans rated the climate as 47 percent for the categories. Additionally, on the survey, a top concern was not having channels through which to report discrimination and the notion that faculty judge students based on their perceived identities.    &lt;br/&gt;That being said, in fall 2017, 2.9 percent of enrolled freshmen at UC-Berkeley were African American or Black, 9.9 percent were Mexican American or Chicano, 3.7 percent were labeled "other Hispanic/Latino." White students constituted 24.5 percent of the freshman class.&lt;br/&gt;Other initiatives through UC-Berkeley's diversity division include a Campus Climate Speaker Series, which brings scholars and activists to campus to address related issues, and Innovation Grants, which provide funding for projects focused on increasing equity and inclusion on campus.&lt;br/&gt;Still, UC-Berkeley has seen hate acts in the past year. In September, posters listing 13 specific community members and identifying them as "terrorist supporters" were found on campus, according to The Daily Californian. Some of the victims in the past had vocalized their support for Palestinian divestment from Israel.&lt;br/&gt;In a statement sent to the university community, UC-Berkeley Chancellor Carol Christ condemned the acts. She highlighted the school's Principles of Community, among which are a commitment to respect the differences and commonalities of all people.&lt;br/&gt;"Berkeley is better than what these incidents reflect," the statement read. "Many things contribute to the fact that we are the nation's number one public university, and a strong component is the care, respect and esteem which we have for our fellow campus community members. As we move into the events of next week, please join me in upholding these values."&lt;br/&gt;Four days after the posters were found, conservative writer Milo Yiannopoulos spoke at Berkeley. According to The Daily Californian, Yiannopoulos was originally invited to speak by the student group the Berkeley Patriot - a conservative group on campus - as part of the "Free Speech Week," in which several conservative speakers were coming to campus. Amid confusion surrounding the event and the Berkeley Patriot actually filing a complaint with the Department of Justice, claiming Berkeley was infringing free speech rights, the event was canceled. Still, Yiannopoulos - and other speakers - came to campus and were met by a crowd of protesters.&lt;br/&gt;In an interview with The Daily Californian, Pranav Jandhyala - a news editor for the Berkeley Patriot and who founded the organization that invited Ann Coulter - explained the situation became too complicated and the group had to pull out of the event.&lt;br/&gt;"It became a situation that we just had to get out of because of the complications," Jandhyala said.&lt;br/&gt;Meanwhile, the Yvette Felarca, an organizer for Berkeley's By Any Means Necessary pointed to the need for a sanctuary space.&lt;br/&gt;"To protect the community (and make) it a sanctuary campus, that means actively defending it," Felarca said.&lt;br/&gt;The University faced its own slew of controversial speakers - the latest being Charles Murray, known for "The Bell Curve," which argues the correlation of IQ and race. McCoy said speakers like Murray use student anger as a platform.&lt;br/&gt;"I'm not really going to say much about what's his name -- Charles Murray -- I don't really care about Charles Murray, I think he's irrelevant," he said. "I think he's just trying to use protests, I think he's trying to use student anger to rebuild his career. So, think about this. He has to use students to get a come-up."&lt;br/&gt;LSA senior Ben Decatur, co-chair of the AEI Executive Council at the University, defended Murray's right to speak on campus.&lt;br/&gt;"If the hosts of tonight's program, in collaboration with University representatives, believe that the protesters are interfering unduly with the speaker's freedom of expression, those protesters will be warned by a University administrator," Decatur said. "If warnings are not heeded and interference continues, the individuals responsible may be removed from the building."&lt;br/&gt;Berkeley freshman Justin Kim serves on the Hall Association at UC-Berkeley. In an interview with The Daily, he described the controversy surrounding Yiannopoulos's visit to campus. He said there were police and blockades for the entire week around Sproul Plaza, where the event took place.&lt;br/&gt;In terms of how the school responds, Kim explained the Berkeley Police Department and administration have worked together to send email advisories about crimes on campus to the community.&lt;br/&gt;"During Free Speech Week, or when it was supposed to happen ... even leading up to it, we got notifications to avoid the area," he said.&lt;br/&gt;He noted that Christ released a statement, which stated the university is committed to free speech, as exemplified by the speakers on campus, even though they put forth ideals that "run counter" to those of the university.&lt;br/&gt;"To provide the security necessary to protect the community, we have had to close buildings, relocate students and workers, bring to campus a police presence that some find intimidating, and spend money that we would have much rather put toward our academic and research mission," the statement read.&lt;br/&gt;Kim explained earlier in the fall there was an event in which UC-Berkeley students could ask Christ any question. There is also a way for students to write letters to the chancellor, which are directly delivered by the president of the Associated Students of the University of California - the UC-Berkeley student government.&lt;br/&gt;Regarding hate acts and the reactions they prompt, Curtis explained the campus climate shifts based on the level to which the incident rises.&lt;br/&gt;"Someone writing something on a residence board in a residence hall on one floor, I may be aware of it, but it usually doesn't rise to the level of impacting a larger community because it's a one-off - unless there are enough instances in the residence halls that are targeting folks, and students are feeling like, 'Wow, there's a lot of racist things, or a lot of anti-Semitic things said,' and that's happened over the years," he said. "But all of a sudden it starts to bubble up."&lt;br/&gt;Graffiti on a building, he explained, will rise to different levels because it is far more public and more people see it. He said it creates a different level of response.&lt;br/&gt;Curtis also noted UC-Berkeley has been in the media as a result of certain speakers coming to campus and impacting the campus climate. Students, for example, can report that they feel unsafe and unwelcome on the campus in response to an event like that.   &lt;br/&gt;He explained that while many programs and offices work to educate the campus and make it more safe, inclusive and accessible for marginalized groups, racism and other forms of bigotry are still prevalent in the United States. Due to a variety of reasons, he explained, the campus climate changes.&lt;br/&gt;"It's not static, we're not working in a place where everyone remains the same forever more, or there's little turnover," he said. "We have large turnover because our student body turns over, and they're coming from their communities and their experiences ... and in the modern era - the modern era of information and social media - we're now impacted by things that happen in the virtual world. The things we may create on campus don't necessarily stop or even mitigate the stuff around hate and bias acts; (the two) can work in concert but I've not seen it stop."</t>
         </is>
+      </c>
+      <c r="L101" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -4889,10 +5199,13 @@
           <t>Anti-racism, Campus climate, Immigration (For), Hate speech, White supremacy (Against)</t>
         </is>
       </c>
-      <c r="J102" t="inlineStr">
+      <c r="K102" t="inlineStr">
         <is>
           <t>Each week, The Michigan Daily's news desk will be publishing a most-read wrap up of the previous week's most popular articles based on the number of online reads each article received. Here are the five most-read from Nov. 26 to Dec. 2:&lt;br/&gt;Hundreds walk out to protest Spencer event, march on campus&lt;br/&gt;Last Wednesday, hundreds of students walked out of their classes to protest the administration's decision to not deny white supremacist Richard Spencer's request to speak at the University of Michigan. This event was part of a larger collection of educational events and protests last week aimed at highlighting student and faculty resistance to Spencer's ideas.&lt;br/&gt;The new e-cigarette on campus: Juul use in campus facilities heightens&lt;br/&gt;Despite the implementation of a January 2015 "no electronic cigarette" policy in University libraries, students say the use of e-cigarettes on campus is on the rise. So far, there is only a ban against "combustible tobacco products" on the main University campus.&lt;br/&gt;"Spencer is somewhere laughing at us": Schlissel talks student strikes, #UMDivest, tax reform&lt;br/&gt;The Daily spoke with University President Mark Schlissel regarding the administration's decision to continue negotiations with Richard Spencer, the decision passed by Central Student Government on #UMDivest and the negative effects President Donald Trump's tax reform bill could have on students.&lt;br/&gt;University moves to schedule Spencer request to speak on campus&lt;br/&gt;After holding an emergency Board of Regents meeting Tuesday night, University President Mark Schlissel announced the University will begin deliberations with Richard Spencer's team regarding time, place and nature of Spencer's potential speaking event. Schlissel was clear that the event will not proceed if there is a risk to student safety.&lt;br/&gt;#StopSpencer speak out, teach-in held to protest University decision to consider Richard Spencer&lt;br/&gt;In connection with the student walk-out and protests against Richard Spencer last week, a crowd of students, faculty and community members gathered in the Diag to allow individuals to share their own frustrations with the administration's handling of Spencer's request. Public Health graduate student Dana Greene, who kneeled in the Diag for 21 hours in September to protest systematic white supremacy, was one of the speakers.</t>
         </is>
+      </c>
+      <c r="L102" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="103">
@@ -4937,10 +5250,13 @@
           <t>University governance, admin, policies, programs, curriculum, White supremacy (Against), Hate speech, Campus climate</t>
         </is>
       </c>
-      <c r="J103" t="inlineStr">
+      <c r="K103" t="inlineStr">
         <is>
           <t>Each week, The Michigan Daily's news desk will be publishing a most-read wrap up of the previous week's most popular articles based on the number of online reads each article received. Here are the five most-read from Nov. 26 to Dec. 2:&lt;br/&gt;Hundreds walk out to protest Spencer event, march on campus&lt;br/&gt;Last Wednesday, hundreds of students walked out of their classes to protest the administration's decision to not deny white supremacist Richard Spencer's request to speak at the University of Michigan. This event was part of a larger collection of educational events and protests last week aimed at highlighting student and faculty resistance to Spencer's ideas.&lt;br/&gt;The new e-cigarette on campus: Juul use in campus facilities heightens&lt;br/&gt;Despite the implementation of a January 2015 "no electronic cigarette" policy in University libraries, students say the use of e-cigarettes on campus is on the rise. So far, there is only a ban against "combustible tobacco products" on the main University campus.&lt;br/&gt;"Spencer is somewhere laughing at us": Schlissel talks student strikes, #UMDivest, tax reform&lt;br/&gt;The Daily spoke with University President Mark Schlissel regarding the administration's decision to continue negotiations with Richard Spencer, the decision passed by Central Student Government on #UMDivest and the negative effects President Donald Trump's tax reform bill could have on students.&lt;br/&gt;University moves to schedule Spencer request to speak on campus&lt;br/&gt;After holding an emergency Board of Regents meeting Tuesday night, University President Mark Schlissel announced the University will begin deliberations with Richard Spencer's team regarding time, place and nature of Spencer's potential speaking event. Schlissel was clear that the event will not proceed if there is a risk to student safety.&lt;br/&gt;#StopSpencer speak out, teach-in held to protest University decision to consider Richard Spencer&lt;br/&gt;In connection with the student walk-out and protests against Richard Spencer last week, a crowd of students, faculty and community members gathered in the Diag to allow individuals to share their own frustrations with the administration's handling of Spencer's request. Public Health graduate student Dana Greene, who kneeled in the Diag for 21 hours in September to protest systematic white supremacy, was one of the speakers.</t>
         </is>
+      </c>
+      <c r="L103" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="104">
@@ -4985,10 +5301,13 @@
           <t>White supremacy (Against), University governance, admin, policies, programs, curriculum, Anti-racism</t>
         </is>
       </c>
-      <c r="J104" t="inlineStr">
+      <c r="K104" t="inlineStr">
         <is>
           <t>Each week, The Michigan Daily's news desk will be publishing a most-read wrap up of the previous week's most popular articles based on the number of online reads each article received. Here are the five most-read from Nov. 26 to Dec. 2:&lt;br/&gt;Hundreds walk out to protest Spencer event, march on campus&lt;br/&gt;Last Wednesday, hundreds of students walked out of their classes to protest the administration's decision to not deny white supremacist Richard Spencer's request to speak at the University of Michigan. This event was part of a larger collection of educational events and protests last week aimed at highlighting student and faculty resistance to Spencer's ideas.&lt;br/&gt;The new e-cigarette on campus: Juul use in campus facilities heightens&lt;br/&gt;Despite the implementation of a January 2015 "no electronic cigarette" policy in University libraries, students say the use of e-cigarettes on campus is on the rise. So far, there is only a ban against "combustible tobacco products" on the main University campus.&lt;br/&gt;"Spencer is somewhere laughing at us": Schlissel talks student strikes, #UMDivest, tax reform&lt;br/&gt;The Daily spoke with University President Mark Schlissel regarding the administration's decision to continue negotiations with Richard Spencer, the decision passed by Central Student Government on #UMDivest and the negative effects President Donald Trump's tax reform bill could have on students.&lt;br/&gt;University moves to schedule Spencer request to speak on campus&lt;br/&gt;After holding an emergency Board of Regents meeting Tuesday night, University President Mark Schlissel announced the University will begin deliberations with Richard Spencer's team regarding time, place and nature of Spencer's potential speaking event. Schlissel was clear that the event will not proceed if there is a risk to student safety.&lt;br/&gt;#StopSpencer speak out, teach-in held to protest University decision to consider Richard Spencer&lt;br/&gt;In connection with the student walk-out and protests against Richard Spencer last week, a crowd of students, faculty and community members gathered in the Diag to allow individuals to share their own frustrations with the administration's handling of Spencer's request. Public Health graduate student Dana Greene, who kneeled in the Diag for 21 hours in September to protest systematic white supremacy, was one of the speakers.</t>
         </is>
+      </c>
+      <c r="L104" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -5033,10 +5352,13 @@
           <t>Immigration (For)</t>
         </is>
       </c>
-      <c r="J105" t="inlineStr">
+      <c r="K105" t="inlineStr">
         <is>
           <t>The 2016-2017 academic year was eventful at Tufts University, with everything from tension on campus in the aftermath of the 2016 presidential election to shakeups in the Greek life system. The following is a rundown of the biggest stories on the Hill from last year.&lt;br/&gt;September&lt;br/&gt;Tufts Student Services released the Tufts Mobile app in collaboration with Tufts Technology Services  and the Tufts Community Union Senate. The app provides students with features such as a university shuttle tracker and a laundry machine monitoring system.&lt;br/&gt;South Hall was renamed Harleston Hall, honoring former Professor of Psychology Bernard Harleston, Tufts' first African-American tenure-track faculty member and a former dean of the faculty of Arts and Sciences.&lt;br/&gt;October&lt;br/&gt;Almost half the members of Tufts' Alpha Omicron Pi Delta chapter dropped from the sorority, after AOII's international organization demurred to offer a bid to a transgender woman.&lt;br/&gt;Tufts announced that it will change its one course, one credit system to the widely-used semester-hour unit system, otherwise known as the credit-hour system, by fall 2018. &lt;br/&gt;November&lt;br/&gt;After Donald Trump's unexpected election as the 45th President of the United States, Tufts' political and activist student groups became energized. The election was followed by an anti-Trump rally in Boston and a post-election gathering on campus. &lt;br/&gt;Tufts janitors voted to accept a new four-year-long contract on Nov. 3. The contract guarantees lower health costs, a $1.80 hourly raise by Jan. 1, 2020 and higher pensions. &lt;br/&gt;Hundreds of students staged a walkout and gathered in front of Olin Center on Nov. 16, demanding that the university declare itself a "sanctuary campus," which would protect and support undocumented Tufts students and community members in these spaces. University President Anthony Monaco also attended the gathering and reassured attendees of the university's commitment to protect and support undocumented students, though he did not officially designate Tufts a sanctuary campus.&lt;br/&gt;The Tufts Observer published an article detailing hazing and sexual assault at a Tufts fraternity in January 2015. The piece sparked calls for the abolition of Greek life at Tufts. Many public discussions and debates on the subject continuedthroughout the year.&lt;br/&gt;December&lt;br/&gt;Following the Observer article and a subsequent wave of misconduct reports, recruitment for all Greek organizations, excluding organizations in the Multicultural Greek Council, was suspended for the spring semester. Additionally, fraternities and sororities voluntarily suspended all social events, a decision affirmed by the university.&lt;br/&gt;ResLife announced that the resident assistant position will be replaced with two new roles: first-year assistant and community development assistant .&lt;br/&gt;January&lt;br/&gt;In response to the Greek life controversy and the suspension of social events, Monacoappointed a Student Life Review Committee composed of faculty, students, staff, parents, alumni and representatives from the Medford and Somerville communities to holistically examine undergraduate student life at Tufts. &lt;br/&gt;A Boston Globe analysis revealed that the number of reported forcible sexual offenses on the Medford/Somerville campus had risen from 14 in 2014 to 25 in 2015, the most recent year for which data was available. Increased reporting was cited as the reason for this change.&lt;br/&gt;February&lt;br/&gt;Massachusetts Governor Charlie Baker visited Tufts to give a talk on civic engagement and public policy on Feb. 24. The event was disrupted by protests and walkouts.&lt;br/&gt;The linguistics minor was reinstated after a year-long hold.&lt;br/&gt;Four Greek life organizations regained the ability to recruit new members, though fraternities and sororities on cease-and-desist orders were not allowed to recruit in the spring. Later in the month, the Interfraternity Council and Panhellenic Council (Panhel) lifted their voluntary holds on social events for eligible Greek life organizations.&lt;br/&gt;Medford City Council unanimously passed the University and College Accountability ordinance on Feb. 28, requiring Tufts to provide an anonymous list of the addresses of students living off campus in Medford.&lt;br/&gt;March&lt;br/&gt;In a TCU Senate resolution, Students Advocating for Students claimed that Tufts' Title IX procedures are unfair towards alleged perpetrators of sexual misconduct. Senators decisively voted down the resolution, with many warning that it could threaten sexual misconduct survivors.&lt;br/&gt;School officials announced that tuition and fees will increase by 3.6 percent for the 2017-2018 academic year, which is the same rate of increase as the year prior. Members of Tufts Student Action criticized the planned increase, arguing that the university has given insufficient justification for continual increases in the cost of a Tufts education.&lt;br/&gt;April&lt;br/&gt;Tufts received a record number of 21,101 applications and saw a slight increase in the overall acceptance rate from last year's 14.3 percent to 14.8 percent.&lt;br/&gt;In an uncontested election, senior Benya Kraus was elected as TCU president for the 2016-2017 academic year.&lt;br/&gt;Tufts joined 30 other universities to file a joint amicus brief against Trump's revised travel ban enacted on March 31.&lt;br/&gt;T-Pain unexpectedly canceled his Spring Fling appearance eight days before the event, citing his son's birthday.&lt;br/&gt;Linda Furgala, an employee at Carmichael Dining Center who faced sudden dismissal from her job on April 19, returned to work after less than a week following an outpouring of student support.&lt;br/&gt;TCU Senate passed a controversial resolution calling for divestment from four companies allegedly involved in the Israeli occupation of the Palestinian territories on April 9. Shortly after the resolution's passage, Tufts announced that it would not divest from those companies, and raised concern that the resolution was passed at a Senate meeting immediately before Passover.&lt;br/&gt;R&amp;B artist Tinashe headlined the annual Spring Fling concert. Other performers included up-and-coming rapper Aminé and producer Metro Boomin.&lt;br/&gt;May&lt;br/&gt;The Peace and Justice Studies Program avoided cancellation, but saw a planned reorganization and the departure of Assistant Director Dale Bryan.&lt;br/&gt;A group called TuftsLeaks published confidential university documents online, including salary data for faculty, staff and students.&lt;br/&gt;Tufts graduate students employed by the School of Arts and Sciences voted to unionize and join Service Employees International Union Local #509. Tufts is now one of the few private universities where graduate students have successfully unionized. &lt;br/&gt;Screenwriter and "Black-ish," (2014-present) creator Kenya Barris delivered the 2017 Commencement address.</t>
         </is>
+      </c>
+      <c r="L105" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -5076,10 +5398,13 @@
           <t>University governance, admin, policies, programs, curriculum, Immigration (For)</t>
         </is>
       </c>
-      <c r="J106" t="inlineStr">
+      <c r="K106" t="inlineStr">
         <is>
           <t>The Class of 2017's years on the Hill were filled with changes to the university, impressive athletic feats and almost-constant political activism. In recognition of Tufts' newest graduating class, the Daily has looked back on the last four years, highlighting their most memorable events, speeches, policy changes and tumultuous moments.&lt;br/&gt;2013 to 2014&lt;br/&gt;The Class of 2013's first year on the Hill saw changes to Tufts' social and dining scenes, as well as student activism over the university's sexual assault policies and practices.&lt;br/&gt;Fall Gala and Winter Ball, rebranded in an effort to address alcohol-related issues at previous years' events, had earlier start times and fewer available tickets. Meanwhile, Tufts University Police Department (TUPD) cut short the fall show of Tufts Dance Collective due to multiple alcohol-related medical calls and unsafe and unsanitary conditions within Cohen Auditorium. Although many feared that this would mark the end of TDC, the spring show went ahead after its organizers also implemented changes.&lt;br/&gt;While several Tufts social traditions were restructured, Tufts welcomed a fourth sorority, Kappa Alpha Theta, onto campus. Theta initiated 77 charter members in September.&lt;br/&gt;Tufts Dining also saw several exciting additions. Former Tufts Community Union Senators Isabella Kahhalé (LA'17) and Christie Maciejewski (LA '14) spearheaded the introduction of late night dining at the Commons Deli and Grill. Starting in January, the Commons began accepting meal swipes from 9 p.m. to 2 a.m. on Fridays and Saturdays, until rowdy and disrespectful behavior prompted the closing time to be shifted forward to 1 a.m.&lt;br/&gt;The Pax Et Lox Kosher Deli on Nov. 3, 2014. (Nicholas Pfosi / The Tufts Daily Archive)&lt;br/&gt;Tufts also opened a kosher deli, later named Pax et Lox Glatt Kosher Deli. However, the Class of 2013 was the last class to take advantage of a practice known as 'trick turning,' in which students on unlimited meal plans could swipe into a dining hall and then swipe into Hodgdon Food-on-the-Run in the same meal period.&lt;br/&gt;The Tufts community bid farewell to a number of staff members. Associate Provost Mary Lee left Tufts after 27 years to assume the prestigious Kimitaka Kaga Professorship at the University of Tokyo's Graduate School of Medicine and Dean of the School of Arts and Sciences Joanne Berger-Sweeney left in June to become president of Trinity College. The university also mourned the deaths of Fletcher Professor of English Emeritus Jesper Rosenmeier and Assistant Director of Career Services Donna Milmore.&lt;br/&gt;In November, the Board of Trustees approved the T10 Strategic Plan, which created a framework for the university's goals over the next 10 years. The 45-page document focused on increasing diversity initiatives through funding gap years and financial aid as well as encouraging interdisciplinary learning with programs like Bridge Professorships. In February, the Committee on Student Life announced the reversal of its December 2012 "justified departure" policy. All organizations, including Religious and Philosophical Student Organizations, would now be required to adhere to the TCU Judiciary's non-discrimination policy.&lt;br/&gt;Additionally, issues surrounding sexual assault on campus were prevalent throughout the year. In the fall, University President Anthony Monaco announced the formation of a university-wide task force on sexual misconduct prevention. In the spring, students organized the first annual It Happens Here event, which provides a space for survivors of sexual assault to share narratives.&lt;br/&gt;Senior Vice President David Harris delivers the second half of the announcement after the noncompliance protest at the Stand with Survivors at Tufts: Rally for Title IX Compliance outside Ballou Hall on May 1, 2014. (Annie Levine / The Tufts Daily Archive)&lt;br/&gt;Later in April, the Department of Education's Office for Civil Rights announced that Tufts was in violation of Title IX as it inadequately supported students who reported campus sexual assault. Tufts then revoked its agreement to comply with OCR recommendations on how to improve the university's sexual assault policies and practices. This triggered the largest student protest since the late 1980s, as more than 100 students marched around Ballou Hall for several hours. After discussions between administrators and student organizers, the university promised to make changes that Monaco said would put Tufts back in compliance with Title IX.&lt;br/&gt;A number of high-profile speakers visited the Hill this year. Huffington Post founder Arianna Huffington spoke about modern media at the annual Edward R. Murrow Forum, while Kenan Thompson of "Saturday Night Live" headlined the Tufts Entertainment Board's spring comedy event. On the political front, Rwandan President Paul Kagame and the late Supreme Court Justice Antonin Scalia both sparked controversy with their visits - about 20 students protested Scalia's speech, the final of the Richard E. Snyder President's Lecture series.&lt;br/&gt;Within Tufts' student politics, the TCU presidential election saw a heated contest between Andrew Núñez (LA '15) and Robert Joseph (LA '15). However, a website and Facebook page for "Generic Candidate" were anonymously created by Ben Kurland (LA '15) to draw attention to what he noted were many similarities between the two platforms. After a 12-hour delay due to technical problems with TCU Election Commission's new online voting system, Joseph was announced as the next TCU president.&lt;br/&gt;2014 to 2015&lt;br/&gt;Between a "Snowpocalypse," two student sit-ins and unstoppable sports teams, 2014-2015 was a year of firsts and record-breaking events.&lt;br/&gt;Team members and students celebrate after the Tufts football 24-17 victory against Hamilton. (Nick Pfosi / The Tufts Daily Archive)&lt;br/&gt;Tufts football won its season opener against Hamilton, breaking the team's infamous 31-game losing streak. Attendees at the homecoming festivities crowded the field in celebration of the historic win.&lt;br/&gt;Also in the fall, men's soccer saw an unlikely run for the NCAA Div. III National Championship title. After making it through the quarterfinals and semifinals, Tufts clinched the championship against Wheaton College in a 4-2 win.&lt;br/&gt;Student activism reached new heights this year, with many students joining protests in Boston in response to several deaths of black Americans at the hands of police officers nationwide. A student group, Indict Tufts, also led protests against racial oppression of black Americans, including a march from campus to the Harvard Bridge over the Charles River.&lt;br/&gt;A Tufts custodian helps announce the start of a hunger strike to protest proposed cuts to the custodial staff on May 3, 2015. (Sophie Hecht / The Tufts Daily)&lt;br/&gt;Meanwhile, Tufts Labor Coalition responded to Tufts' proposed changes to and downsizing of the janitorial services staff with a 33-hour sit-in at Ballou Hall and a five-day hunger strike that made local and regional headlines. TLC also protested a new 5,000-pound bronze Jumbo statue, which was donated by alumni and unveiled in April. In addition to labor issues, the debate over fossil fuel divestment was invigorated when 33 students, mostly from Tufts Climate Action , held a sit-in at Ballou Hall to protest Tufts' investments in the fossil fuel industry.&lt;br/&gt;The spring semester was significantly affected by heavy snow, which led to a record-breaking five snow days. To make up for lost class time, professors rescheduled classes on Patriot's Day and during the first two days of reading period. This spring also saw computer science become the most popular major at Tufts, surpassing international relations as the program with the most declared majors. Professor Sol Gittleman also retired after more than 50 years at Tufts.&lt;br/&gt;Several student initiatives began this year, including the production "Not Your Mother's Monologues," a non-ciscentric, more inclusive version of "The Vagina Monologues" (1996). TED Talk-style lectures also came to campus through the student-led launch of TEDxTufts, which gives students an opportunity to share their ideas and passions. In April, Kesha headlined Tufts' first Spring Fling that featured exclusively female-led groups, including MisterWives and Lauren Lane.&lt;br/&gt;Tufts Community Union Senate saw a major first and a major controversy, with the first uncontested Senate presidential election in recent history leading to the election of Brian Tesser (LA '16). Earlier in the year, Senate's budgeting and club-funding decisions came under fire when some student groups, particularly Tufts Mock Trial, learned of new limitations on travel funding from Senate's budget.&lt;br/&gt;The house of Tufts fraternity Delta Tau Delta stood empty for more than a year after the double stabbing on May 31, 2015. (Sofie Hecht / The Tufts Daily)&lt;br/&gt;While Greek life grew in popularity, the brothers of Pi Delta, formerly known as Alpha Epsilon Pi, disaffiliated from their national chapter in response to differing interests and values between the Tufts and national chapters. In late May, a stabbing took place inside the house of Delta Tau Delta, leading to a temporary lockdown of the Medford/Somerville campus. The stabbing incident is still under investigation.&lt;br/&gt;Students saw their housing affected by Somerville's passing of the University Accountability Ordinance. This ordinance mandates that universities in Somerville - particularly Tufts - submit a report providing students' addresses to limit overcrowding in off-campus housing in accordance with an existing zoning ordinance. The ordinance came at a time when Tufts saw more applicants and more students choosing to attend the university, straining on-campus housing and forcing more upperclassmen to live off campus in increasingly expensive Medford and Somerville.&lt;br/&gt;George Stephanopoulos, ABC News Chief Anchor, speaks during the The 10th Annual Edward R. Murrow Forum on Issues in Journalism: "Who Can You Trust in the 24/7 Multimedia News Cycle?" in Cabot Auditorium on April 8, 2015. (Nicholas Pfosi / The Tufts Daily Archive)&lt;br/&gt;Several notable speakers, including the parents of Trayvon Martin, came to campus. Some student groups, especially the Pan-African Alliance and Black Student Union, criticized Hillel's choice to invite Martin's parents due to Hillel's stance on Israel, among other concerns. Additionally, ABC News anchor George Stephanopoulos spoke at the Edward P. Murrow Forum and Senator Elizabeth Warren delivered the Alan D. Solomont Lecture on Citizenship and Public Service, where about a dozen students protested Warren's previous pro-Israeli statements.&lt;br/&gt;2015 to 2016&lt;br/&gt;The 2015-2016 academic year saw notable changes and additions to the programs and majors offered at Tufts, lively student activism and progress made on several significant building projects.&lt;br/&gt;Perhaps the biggest academic news was Tufts' announcement of the acquisition of the School of the Museum of Fine Arts at the end of the year. Meanwhile, the School of Arts and Sciences began to offer a Portuguese minor in the spring. It also announced a film and media studies major; an environmental studies minor focusing on food systems and nutrition; and a science, technology and society co-major and minor, which all debuted in fall 2016. On the other hand, minors in linguistics and cognitive and brain sciences were terminated in fall 2015, although they returned in spring 2017.&lt;br/&gt;TLC members rally outside Ballou Hall on March 2, 2016 demanding the university hire union-only labor for construction projects. (Alex Knapp / The Tufts Daily Archive)&lt;br/&gt;Tufts saw the reopening of the Collaborative Learning and Innovation Complex at 574 Boston Ave., the completion of the renovated Memorial Steps, the start of construction work on a new Central Energy Plant and significant work completed on the Science and Engineering Complex . Construction workers, however, protested Tufts' use of non-union workers for these projects, with the Boston Building Trades Council using billboard trucks to communicate this message.&lt;br/&gt;Tufts Labor Coalition also supported union-only hiring efforts on campus and continued to push for better labor practices for Tufts janitors. Student organizers from TLC protested outside Gifford House, at town-hall meetings and during Jumbos Days.&lt;br/&gt;Other student activists continued to rally behind divestment from the fossil fuel industry. Tufts Climate Action hosted a two-day symposium on climate change in April and demonstrated outside a Board of Trustees meeting that month. Many faculty also showed support for fossil fuel divestment through a faculty resolution passed in May.&lt;br/&gt;Protesters march away from the Campus Center during the #thethreepercent rally on Tufts campus on Nov. 18, 2015. Students organized to protest anti-Black racism on Tufts' campus and other college campuses across the U.S. (Nicholas Pfosi / The Tufts Daily Archive)&lt;br/&gt;Other activist efforts included a march organized by #TheThreePercent in conjunction with nationwide protests against racism on campus. #TheThreePercent also released a list of demands to Tufts administrators, asking for better black student and faculty representation, increases to the Africana Center's budget and more mental health resources for black students. Students for Justice in Palestine also staged several protests and actions, including the disruption of Friends of Israel's annual Taste of Israel event, sparking a debate about the Israeli-Palestinian conflict, cultural appropriation in food and the nature of campus protests.&lt;br/&gt;The university hired its first chief diversity officer, Mark Brimhall-Vargas, who had begun working as associate provost in May 2015. In the fall, Brimhall-Vargas chaired the Diversity and Inclusion Working Group and later helped start a "Diversity Dashboard" to increase transparency in diversity issues.&lt;br/&gt;Several notable speakers came to campus last year, such as economist Lawrence Summers, television journalist David Gregory and activist and scholar Noam Chomsky. At the Edward P. Murrow Forum, television journalist Anderson Cooper spoke about his career and the 2016 presidential election. Congressman and civil rights activist John Lewis and political strategists David Axelrod and Beth Myers (J '79) also came to speak on the Hill.&lt;br/&gt;The Jonathan M. Tisch College of Citizenship and Public Service was renamed the Jonathan M. Tisch College of Civic Life to focus on civic engagement, after a donation from Jonathan (A '76) and Lizzie Tisch to the college.&lt;br/&gt;Lee Coffin, the former dean of undergraduate admissions, makes a snow angel on Feb. 12, 2016. (Evan Sayles / The Tufts Daily)&lt;br/&gt;Several longstanding administrative, admissions and student life positions were revised throughout the year. Dean of Undergraduate Admissions Lee Coffin ended his 13-year Tufts career at the end of the year to head admissions at Dartmouth College. Director of the Institute of Global Leadership Sherman Teichman also left his role after more than three decades. In December, Director of the Experimental College Robyn Gittleman retired after 40 years. Finally, Steph Gauchel left her position as director of the Women's Center to work at the Harvard Divinity School.&lt;br/&gt;Greek life organizations became increasingly popular this year, with 200 students accepting sorority bids and a potential new sorority, Alpha Gamma Delta, which ultimately did not form a chapter on campus. The fraternity Pi Rho Omega, formerly known as Sigma Phi Epsilon, disaffiliated from its national organization in January, citing differing values between the Tufts and national chapters.&lt;br/&gt;Firefighters extinguish a car fire in the parking lot of the Tufts University Health Service on May 9, 2016. (Evan Sayles / The Tufts Daily)&lt;br/&gt;Several campus safety issues came up throughout the year, including the ongoing investigation surrounding the stabbing at Delta Tau Delta's house in May 2015. Multiple sexual assaults and acts of misconduct were reported in Tufts dorms, prompting a public university response. Finally, spring semester final exams were postponed due to bomb threats and a car fire behind Health Service. &lt;br/&gt;Throughout the year, students also prepared for the 2016 presidential election, canvassing in New Hampshire, attending rallies and demonstrating at a rally held by then-presidential candidate Donald Trump in Massachusetts.&lt;br/&gt;2016 to 2017&lt;br/&gt;This year saw a rise in tension on campus in the aftermath of President Trump's election, which had unmistakable parallels to the atmosphere nationwide. The effects of this reverberated throughout the rest of the school year.&lt;br/&gt;Members of Tufts United for Immigrant Justice speak to students and community members during a rally demanding that Tufts become a sanctuary campus, following a campus-wide walkout on Nov. 16, 2016. (Evan Sayles / The Tufts Daily)&lt;br/&gt;One effect was a walkout and rally calling for Tufts to become a sanctuary campus in an effort to protect its undocumented students. Though never explicitly naming Tufts a sanctuary campus, Monaco pledged to support and protect undocumented students by keeping their information private from law enforcement officials and providing access to legal counsel.&lt;br/&gt;Simultaneously, the Tufts Observer published an explosive article detailing hazing and sexual assault at a fraternity in November. The piece sparked calls for the abolition of Greek life at Tufts, the suspension of spring recruitment of fraternities and sororities and the issuance of nine cease-and-desist orders. One Greek organization was dissolved and two more were suspended. Earlier in the fall, half of Alpha Omicron Pi sorority's members dropped out after the national organization hesitated to admit a transgender woman, and several members of Chi Omega sorority quit, citing discrimination by their own national organization. In light of this tumult, Monaco commissioned the Student Life Review Committee to assess all aspects of student life on campus.&lt;br/&gt;Ben Kesslen (center) protests against sorority recruitment events on March 30, 2016. (Ray Bernoff / The Tufts Daily)&lt;br/&gt;In the second uncontested election in three years, rising senior Benya Kraus was elected Tufts Community Union president. TCU Senate also debated controversial resolutions that called for changes to Tufts' Sexual Misconduct Policy and Title IX policies as well as divestment from four companies involved in the Israeli occupation of the Palestinian Territories.&lt;br/&gt;Labor issues continued this year, as janitors threatened to strike in the run-up to the deadline of their contract renegotiations, workers in Facilities Services filed a complaint against Tufts with the National Labor Review Board, part-time faculty rallied support for their contract renegotiation with Tufts and graduate students authorized a vote to unionize.&lt;br/&gt;Tufts continued its integration of the School of the Museum of Fine Arts  after its acquisition last summer. SMFA students went through Tufts orientation, the admissions of both schools were combined and SMFA students switched to a need-based, rather than merit-based, financial aid system.&lt;br/&gt;In September, South Hall was renamed Harleston Hall in honor of Bernard Harleston, former dean of the faculty of arts and sciences and the first African-American tenure-track professor at Tufts. Construction on the  Central Energy Plant and the Science and Engineering Complex  continued while it was announced the Boston Avenue/College Avenue intersection would be redesigned for pedestrian safety. Brown and Brew Coffee House will be closing in August, to be replaced by a cafe in the SEC. &lt;br/&gt;The Residential Strategies Working Group finished its work and recommended converting Tufts-owned wood-framed houses, currently used as office space and faculty housing, into student housing to ease tensions with Tufts' neighbors.&lt;br/&gt;Two students ask whether Massachusetts will be a sanctuary state during Gov. Charlie Baker's talk in Distler Auditorium on Feb. 23, 2016. (Seohyun Shim / The Tufts Daily)&lt;br/&gt;This year, Tufts saw a slew of interesting and sometimes controversial visitors, including former Secretary of State John Kerry, "NBC Nightly News" anchor Lester Holt, Senator Tim Kaine, former advisor to President Barack Obama David Axelrod, former host of "Meet the Press" David Gregory, who also taught a class through the Jonathan M. Tisch College of Civic Life in the fall, academic Judith Butler, NPR's Mara Liasson, former Governor of New Mexico Bill Richardson, Chief of Staff to President George W. Bush Andrew Card, President of CBS News David Rhodes and Massachusetts Governor Charlie Baker, whose presence provoked a protest and walkout. In March, actor and Cambridge native Matt Damon made two surprise appearances at the Steve Tisch Sports and Fitness Center.&lt;br/&gt;Tufts also said goodbye to several members of the faculty and staff, including Mark Brimhall Vargas, who left his post as chief diversity officer to become vice president for diversity, equity and inclusion at Brandeis University. LGBT Center Director Nino Testa and Latino Center Director Rubén Stern both left Tufts, as did Vice President of Operations Lynda Snyder, who retired.&lt;br/&gt;The year rounded out with Spring Fling performances from an all-black lineup of artists. The show was successful despite a last-minute cancellation from headliner T-Pain.&lt;br/&gt;Another end-of-year upset took the form of a leak of confidential information by a group called TuftsLeaks. The information included salary data for faculty, staff and students, and the investigation is ongoing.&lt;br/&gt;The leaks were done in the name of transparency in university spending. This was a common theme of this year as tuition, fees and other expenses topped $70,000. Yearly tuition increases prompted the creation of a #HaltTheHike campaign by Tufts Student Action, who demanded transparency and a freeze on increases.&lt;br/&gt;The Tufts University Men's Soccer Team cheers with the championship trophy after the match against Calvin College of the national NCAA Division III men's soccer tournament on Dec. 3, 2016. The Jumbos defeated the Knights 1 to 0 in double overtime. (Alonso Nichols / Tufts University)&lt;br/&gt;In happier news, Tufts celebrated its first Indigenous People's Day in October, and the men's soccer team closed out its season with its second NCAA Championship win in three years.</t>
         </is>
+      </c>
+      <c r="L106" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -5119,10 +5444,13 @@
           <t>University governance, admin, policies, programs, curriculum, Immigration (For)</t>
         </is>
       </c>
-      <c r="J107" t="inlineStr">
+      <c r="K107" t="inlineStr">
         <is>
           <t>The 2016-2017 academic year was eventful at Tufts University, with everything from tension on campus in the aftermath of the 2016 presidential election to shakeups in the Greek life system. The following is a rundown of the biggest stories on the Hill from last year.&lt;br/&gt;September&lt;br/&gt;Tufts Student Services released the Tufts Mobile app in collaboration with Tufts Technology Services  and the Tufts Community Union Senate. The app provides students with features such as a university shuttle tracker and a laundry machine monitoring system.&lt;br/&gt;South Hall was renamed Harleston Hall, honoring former Professor of Psychology Bernard Harleston, Tufts' first African-American tenure-track faculty member and a former dean of the faculty of Arts and Sciences.&lt;br/&gt;October&lt;br/&gt;Almost half the members of Tufts' Alpha Omicron Pi Delta chapter dropped from the sorority, after AOII's international organization demurred to offer a bid to a transgender woman.&lt;br/&gt;Tufts announced that it will change its one course, one credit system to the widely-used semester-hour unit system, otherwise known as the credit-hour system, by fall 2018. &lt;br/&gt;November&lt;br/&gt;After Donald Trump's unexpected election as the 45th President of the United States, Tufts' political and activist student groups became energized. The election was followed by an anti-Trump rally in Boston and a post-election gathering on campus. &lt;br/&gt;Tufts janitors voted to accept a new four-year-long contract on Nov. 3. The contract guarantees lower health costs, a $1.80 hourly raise by Jan. 1, 2020 and higher pensions. &lt;br/&gt;Hundreds of students staged a walkout and gathered in front of Olin Center on Nov. 16, demanding that the university declare itself a "sanctuary campus," which would protect and support undocumented Tufts students and community members in these spaces. University President Anthony Monaco also attended the gathering and reassured attendees of the university's commitment to protect and support undocumented students, though he did not officially designate Tufts a sanctuary campus.&lt;br/&gt;The Tufts Observer published an article detailing hazing and sexual assault at a Tufts fraternity in January 2015. The piece sparked calls for the abolition of Greek life at Tufts. Many public discussions and debates on the subject continuedthroughout the year.&lt;br/&gt;December&lt;br/&gt;Following the Observer article and a subsequent wave of misconduct reports, recruitment for all Greek organizations, excluding organizations in the Multicultural Greek Council, was suspended for the spring semester. Additionally, fraternities and sororities voluntarily suspended all social events, a decision affirmed by the university.&lt;br/&gt;ResLife announced that the resident assistant position will be replaced with two new roles: first-year assistant and community development assistant .&lt;br/&gt;January&lt;br/&gt;In response to the Greek life controversy and the suspension of social events, Monacoappointed a Student Life Review Committee composed of faculty, students, staff, parents, alumni and representatives from the Medford and Somerville communities to holistically examine undergraduate student life at Tufts. &lt;br/&gt;A Boston Globe analysis revealed that the number of reported forcible sexual offenses on the Medford/Somerville campus had risen from 14 in 2014 to 25 in 2015, the most recent year for which data was available. Increased reporting was cited as the reason for this change.&lt;br/&gt;February&lt;br/&gt;Massachusetts Governor Charlie Baker visited Tufts to give a talk on civic engagement and public policy on Feb. 24. The event was disrupted by protests and walkouts.&lt;br/&gt;The linguistics minor was reinstated after a year-long hold.&lt;br/&gt;Four Greek life organizations regained the ability to recruit new members, though fraternities and sororities on cease-and-desist orders were not allowed to recruit in the spring. Later in the month, the Interfraternity Council and Panhellenic Council (Panhel) lifted their voluntary holds on social events for eligible Greek life organizations.&lt;br/&gt;Medford City Council unanimously passed the University and College Accountability ordinance on Feb. 28, requiring Tufts to provide an anonymous list of the addresses of students living off campus in Medford.&lt;br/&gt;March&lt;br/&gt;In a TCU Senate resolution, Students Advocating for Students claimed that Tufts' Title IX procedures are unfair towards alleged perpetrators of sexual misconduct. Senators decisively voted down the resolution, with many warning that it could threaten sexual misconduct survivors.&lt;br/&gt;School officials announced that tuition and fees will increase by 3.6 percent for the 2017-2018 academic year, which is the same rate of increase as the year prior. Members of Tufts Student Action criticized the planned increase, arguing that the university has given insufficient justification for continual increases in the cost of a Tufts education.&lt;br/&gt;April&lt;br/&gt;Tufts received a record number of 21,101 applications and saw a slight increase in the overall acceptance rate from last year's 14.3 percent to 14.8 percent.&lt;br/&gt;In an uncontested election, senior Benya Kraus was elected as TCU president for the 2016-2017 academic year.&lt;br/&gt;Tufts joined 30 other universities to file a joint amicus brief against Trump's revised travel ban enacted on March 31.&lt;br/&gt;T-Pain unexpectedly canceled his Spring Fling appearance eight days before the event, citing his son's birthday.&lt;br/&gt;Linda Furgala, an employee at Carmichael Dining Center who faced sudden dismissal from her job on April 19, returned to work after less than a week following an outpouring of student support.&lt;br/&gt;TCU Senate passed a controversial resolution calling for divestment from four companies allegedly involved in the Israeli occupation of the Palestinian territories on April 9. Shortly after the resolution's passage, Tufts announced that it would not divest from those companies, and raised concern that the resolution was passed at a Senate meeting immediately before Passover.&lt;br/&gt;R&amp;B artist Tinashe headlined the annual Spring Fling concert. Other performers included up-and-coming rapper Aminé and producer Metro Boomin.&lt;br/&gt;May&lt;br/&gt;The Peace and Justice Studies Program avoided cancellation, but saw a planned reorganization and the departure of Assistant Director Dale Bryan.&lt;br/&gt;A group called TuftsLeaks published confidential university documents online, including salary data for faculty, staff and students.&lt;br/&gt;Tufts graduate students employed by the School of Arts and Sciences voted to unionize and join Service Employees International Union Local #509. Tufts is now one of the few private universities where graduate students have successfully unionized. &lt;br/&gt;Screenwriter and "Black-ish," (2014-present) creator Kenya Barris delivered the 2017 Commencement address.</t>
         </is>
+      </c>
+      <c r="L107" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -5167,10 +5495,13 @@
           <t>University governance, admin, policies, programs, curriculum, Police violence, Anti-racism</t>
         </is>
       </c>
-      <c r="J108" t="inlineStr">
+      <c r="K108" t="inlineStr">
         <is>
           <t>courtesy of lucas miranda&lt;br/&gt;The People's March for Justice brought together Hopkins students and Baltimore community members.&lt;br/&gt;Members of the Hopkins and Baltimore community joined a demonstration organized by the People's Power Assembly on Jan. 13. Officially named the People's March for Justice, the event addressed the protestor's concerns about the Baltimore Police Department infringing on the rights of community members and drawing city resources away from other public institutions like schools.&lt;br/&gt;The morning of the March, a group of Hopkins students gathered on the Beach. Representatives from several student groups spoke about their motivations for getting involved in the demonstration and told students how to respond if police showed up.&lt;br/&gt;Students for a Democratic Society and Tzedek (formerly known as Jews Giving a Fuck at Hopkins) created a Facebook event for interested students and coordinated efforts with PPA.&lt;br/&gt;Other student organizations who participated were Students for Justice in Palestine , the Black Student Union , Voice for Choice and Teachers and Researchers United .&lt;br/&gt;The Hopkins contingent joined Baltimore community members at McKeldin Square, where PPA leaders, Baltimore community members and Hopkins students made short speeches about the causes behind the March.&lt;br/&gt;The group then marched to the Police Administration Building on East Fayette and President Street, where organizers and community members made a few more speeches before the March disbanded.&lt;br/&gt;Protesters shouted chants such as "BPD, KKK, How many kids did you kill today?" and "Up up with education, down down with deportation" and held signs with anti-BPD slogans. Many others carried signs with the names of people killed in police shootings.&lt;br/&gt;Organizers did not collaborate with the police when planning the March, which involved walking through busy streets near the Inner Harbor and obstructing traffic.&lt;br/&gt;About 10 minutes after the March began, police cars and motorbikes began to follow the group. Several police officers told demonstrators to get off the street.&lt;br/&gt;According to SDS Co-President Mira Wattal, who witnessed a police officer grab a protester from the sidelines and question them, there were minimal altercations between police officers and protesters.&lt;br/&gt;"They were obviously trying to corral us in, they were yelling at us, but they didn't really break up the crowd. It was maybe one incident on the outskirts, one altercation," she said.&lt;br/&gt;Wattal attributed this to the presence of college students, specifically Hopkins students, at the demonstration.&lt;br/&gt;"Historically, when there are Hopkins students at an event in Baltimore, police presence is usually less aggressive," Wattal said. "As college students, we have the privilege of being treated differently by the law, which makes me angry, because not everyone else in Baltimore gets that same treatment."&lt;br/&gt;The People's March was initially organized in response to Mayor Catherine Pugh canceling the annual MLK Day Parade and replacing it with a day of service.&lt;br/&gt;Though Pugh eventually reinstated the parade in response to a citywide outcry, the PPA decided to go forward with the March.&lt;br/&gt;PPA Member Sharon Black explained why the PPA decided to continue with the March, emphasizing the BPD's occupation of Harlem Park after the fatal shooting of a homicide detective.&lt;br/&gt;"The PPA has been organizing around the issue of police racism and corruption, and particularly the occupation that took place in Harlem Park after the scandal of the officer who was killed, most likely by his own," she said. "Instead, the community was targeted for some time and [was placed] on lockdown."&lt;br/&gt;Black discussed how police brutality and infringement of Baltimore citizens' rights in Harlem Park called for some form of community action.&lt;br/&gt;"Our demonstration was against police corruption in Baltimore City. But then the mayor cancelled the original Dr. King parade, and we wanted to have a People's March," she said. "We've been fighting to divest money out of the police department and put it into education."&lt;br/&gt;Tzedek founding member Miranda Bachman agreed, further addressing the implications of the events in Harlem Park.&lt;br/&gt;"The Baltimore Police Department's illegal occupation of the Harlem Park neighborhood in West Baltimore is a clear example of how police departments - which are highly militarized, over-funded, and corrupt - terrorize poor black neighborhoods without any accountability," she wrote in an email to The News-Letter. "For almost a week, people were not let into their homes or allowed outside of them, they were held at checkpoints, they lost their jobs and wages. This cannot be ignored or condoned, and the city is doing just that."&lt;br/&gt;Bachman, along with the other student leaders at the event, was impressed with the amount of Hopkins students who attended.&lt;br/&gt;"I was really excited to see so many people come out, including many younger students who will be at Hopkins longer and can continue this work," she wrote. "One of the March organizers told me that when we got off the bus, we looked like the cavalry coming."&lt;br/&gt;SJP member Naisa Rahman felt that it was important for Hopkins students to get more involved in events organized by grassroots organizations in the Baltimore community.&lt;br/&gt;When addressing the group of Hopkins students on the Beach prior to the March, she noted the brutality of the Baltimore Police force in the context of their military-level training. She discussed the history of the BPD's relationship with the Israel Defense Forces that began in 2002.&lt;br/&gt;"The people of this city do not deserve for their money to be used to arm and militarize the police further," Rahman said. "SJP joins this March because we recognize that deadly police violence in Palestine is intricately tied to the physical abuse, shoot-to-kill policies, police murders, racial profiling, mass spying and surveillance, detention and excessive force we see by the BPD."&lt;br/&gt;Samantha Agarwal, a graduate student in the sociology department and member of TRU, spoke on the Beach about the Hopkins administration's reliance on contracted workers.&lt;br/&gt;"Through subcontracting, Hopkins pushes the responsibilities of being an employer on third parties, instead of hiring directly, allowing it to circumvent labor laws and pay lower wages," she said. "Subcontracted employees at Hopkins often have no benefits and have fewer job protections."&lt;br/&gt;Agarwal addressed the impact that Hopkins as an institution has had on Baltimore neighborhoods.&lt;br/&gt;"We look to Hopkins and we see a microcosm of the racial injustices which plague our society. This is seen in its appalling lack of black faculty and student body, its labor practices which disadvantage people of color and in its racist housing policies," she said. "While Hopkins is a major force for gentrification, it makes little to no attempt to create affordable housing."&lt;br/&gt;At the Police Administration Building, Sharon Black further discussed the idea of housing inequality and privatization in Baltimore, emphasizing the importance of young people in continuing the fight.&lt;br/&gt;"Forty percent of public housing in Baltimore City is being torn down and privatized. I don't think the mayor or any of the powers that be, the people that run this city, they don't give a damn," she said. "They don't care where these people go. Put them way out in the county where they can't get in touch with their families; let them starve; let them live in the streets."&lt;br/&gt;Black also discussed how some neighborhoods in Baltimore, including hers, had water shut off on certain blocks for up to five days, emphasizing the importance of direct action to hold City institutions accountable.&lt;br/&gt;In her speech before the March, Wattal talked about the responsibility Hopkins students have as members of the Baltimore community.&lt;br/&gt;"We're part of the problem because Hopkins students can and do conduct drone research and weapons research. Even though we're outsiders, we're Hopkins students and we're part of the problem, we might be a part of the solution," she said. "We're here today because we're not politically apathetic."&lt;br/&gt;BSU President Kwame Alston agreed, further addressing the part he believe Hopkins students need to play in helping and empowering the community. Drawing from his personal experience as a Baltimore native who went through the public school system, Alston talked about how education budget cuts endanger schools and families throughout the City.&lt;br/&gt;"When schools shut down, people's parents have to stay home from work, and they're threatened with losing their jobs because they have to take care of their kids," he said.&lt;br/&gt;Baltimore City, according to Alston, invests $15,000 per student in its schooling system, as opposed to Montgomery County, which invests $17,000 and other school districts across the country that invest over $20,000. He discussed the lack of infrastructure in Baltimore schools, which has been causing heating issues in schools for over a decade even though it just recently gained media attention.&lt;br/&gt;At the event in McKeldin Square, a Baltimore City Public School teacher shared her experience during the heating crisis that several public schools experienced earlier in January, which prompted outcry among teachers and parents.&lt;br/&gt;"The students looked at me and said 'do something, do something.' I couldn't do anything. I could not turn on the heat and keep them warm. I could not dismiss them to go home," she said.&lt;br/&gt;Alston added that even when heaters are introduced in Baltimore schools, the poor infrastructure causes fuses to break as a result of the power drawn by the heaters.&lt;br/&gt;"As you march today, just remember that as Hopkins students, we directly benefit from a lot of the reasons why there is not funding, we directly benefit from the development of Harbor East, we directly benefit from the gentrification of Remington," he said. "Keep those [BCPS] students in the back of your mind."</t>
         </is>
+      </c>
+      <c r="L108" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -5210,10 +5541,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J109" t="inlineStr">
+      <c r="K109" t="inlineStr">
         <is>
           <t xml:space="preserve">At the culmination of a two-week, student-led protest advocating for the University of Colorado Boulder to divest from fossil fuels, Fossil Free CU member P.D. Gantert said the group won the divestment fight despite the university's refusal to financially cut ties with the oil and gas industry.&lt;br/&gt;"It's absolutely miraculous what we've done in the last two weeks," Gantert said as he marched through the campus. "Now people on this campus actually know what this issue is. We've changed the conversation. We've won."&lt;br/&gt;The Friday rally started at the UMC Fountains and gathered about 30 students and community members who sang, unfurled banners and talked about being threatened with arrest for their weeklong occupation of the chancellor's office. From left the right, Fossil Free CU members Alex Koek, P.D. Gantert and Cha Cha Spinrad carry fake oil barrels during a protest by the group Friday on the University of Colorado Boulder campus. (Paul Aiken / Staff Photographer)&lt;br/&gt;CU police and a few members of administration stood off to the side of the rally and watched.&lt;br/&gt;"Our role is to make sure everybody's First Amendment rights are protected," said CUPD spokesman Scott Pribble. "We do this when we know there's going to be something going on. It's standard procedure."&lt;br/&gt;Climate scientists joined the students group, adding more venerable environmental advocates to the group of young activists.&lt;br/&gt;Kritee Kanko is a climate scientist, zen priest and member of Boulder Eco-Dharma Sangha. She felt she had no other option but to show up and support the cause.&lt;br/&gt;"If a university like CU can't divest, who can?" Kanko said. "I'm here because these students need intergenerational support. I feel inspired when I see them. All that we love is at stake."Advertisement&lt;br/&gt;Naropa University graduate student Jeff Au Green commanded a megaphone, talking about his university's success in fossil fuel divestment. Naropa is the only university in Colorado to divest from the oil and gas industry.&lt;br/&gt;"We sent a letter to your Board of Regents saying we did it, and you can do it, too," Au Green said.&lt;br/&gt;Because of the student protests, the Boulder Faculty Assembly passed a resolution Thursday to support continuing advocacy for CU to divest from fossil fuels in the coming months.&lt;br/&gt;"The BFA supports the students as they and we engage the issue of divestment from fossil fuels, and call for reasoned debate with Administration in the coming months," the resolution said.&lt;br/&gt;Gantert, who graduated in December, watched as his group members charged ahead of him, singing protest songs as passing students did double takes. He is passing the torch of leading the group to CU sophomore Lior Gross, who was kicked out of the chancellor's office during a sit-in on Wednesday.&lt;br/&gt;"It's my time to go," Gantert said. "I'm not a student anymore. This is the strongest team we've ever had."&lt;br/&gt;Elizabeth Hernandez: 303-473-1106, </t>
         </is>
+      </c>
+      <c r="L109" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -5253,10 +5587,13 @@
           <t>University governance, admin, policies, programs, curriculum, Environmental</t>
         </is>
       </c>
-      <c r="J110" t="inlineStr">
+      <c r="K110" t="inlineStr">
         <is>
           <t>After sleeping on the floor of the University of Colorado chancellor's office since Thursday night, students urging CU to divest from fossil fuels met with Chancellor Phil DiStefano on Tuesday and asked him to publicly support their cause.&lt;br/&gt;Five students from the advocacy group Fossil Free CU sat around a table in the Regent Administrative Center and shared what they described as a "level of grassroot support rarely seen on this campus."&lt;br/&gt;A reporter and a photographer from the Daily Camera were allowed to observe the closed-door meeting after originally being barred access to the protesters inside the building that houses the chancellor's office. University of Colorado Chancellor Phil DiStefano, left, listens as members of Fossil Free CU demand the university divest from fossil fuels, during a meeting Tuesday inside the Regent Administrative Center on the campus. (Jeremy Papasso / Staff Photographer)&lt;br/&gt;Since the protest began last week, group member and sophomore Lior Gross said Fossil Free CU has engaged at least 75 students who intermittently have joined in the student-led occupation of the chancellor's office, made protest art or otherwise contributed to raising awareness about the university's ties to the oil and gas industry.&lt;br/&gt;"It's been really incredible in terms of support," Gross said. "This is the most I've seen anybody engage with a campaign."&lt;br/&gt;During their meeting, group members told DiStefano they understood he, alone, could not make the decision to divest from fossil fuels. But they asked him to publicly pledge his support of the students' cause.Advertisement&lt;br/&gt;"We know you can't go around the Board of Regents," senior Rosellen Sell said. "But we want to see CU walk the walk and align itself with the image it has as an environmentally friendly institution."&lt;br/&gt;Pointing to the fatal Firestone house explosion last month that's been linked to a cut line from a well, the students said now is the time to act and cut ties with the oil and gas industry.&lt;br/&gt;"We're doing this because there's a lot on the line," group member P.D. Gantert said.&lt;br/&gt;The students passed DiStefano their requests in a letter, to which he said he would have to read it later and confer with his cabinet.&lt;br/&gt;"We're happy to sit while you read it and answer any questions you may have," Sell said.&lt;br/&gt;She mentioned concerns the group had about being pacified or ignored, and the group continued to pressure the chancellor to read their letter and talk it out.&lt;br/&gt;DiStefano thanked the students for their passion and, ultimately, said he'd need to discuss the matter further with his staff.&lt;br/&gt;"I'll get a response back to you very quickly," he said.&lt;br/&gt;Following the meeting, a group of Fossil Free CU students hauled "oil barrels" with painted slogans supporting their mission onto the grounds near the Dalton Trumbo Fountain outside the University Memorial Center.&lt;br/&gt;"This represents what we're fighting against," said Michaela Mujica-Steiner, who graduated from CU in 2016, as she pointed toward the barrels.&lt;br/&gt;In 2015, the regents voted 7-2 to reaffirm the university's current investment practices, claiming neutrality.&lt;br/&gt;Students have met with administrators and regents in the past, showing up at Board of Regents meetings to voice their concerns. Fossil Free CU claims they have been largely ignored.&lt;br/&gt;Elizabeth Hernandez: 303-473-1106,  or twitter.com/ehernandez</t>
         </is>
+      </c>
+      <c r="L110" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -5296,10 +5633,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J111" t="inlineStr">
+      <c r="K111" t="inlineStr">
         <is>
           <t>Corrections: Due to a reporting error, this story identified the sit-in as happening at 924 Broadway. It is happening next door in the University Administrative Center. The assistant dean of students' name is spelled Jennifer McDuffie.&lt;br/&gt;About seven CU Boulder students and alumni are staging a sit-in in a building on campus, urging Chancellor DiStefano to make a statement on the future of CU's investments in the fossil fuel industry. The sit-in began with about a dozen students at 12:45 p.m., and the chancellor came to the building at about 5:40 p.m., when he and the group went upstairs.&lt;br/&gt;At about 5 p.m., Colorado state Senator Steve Fenberg released a letter endorsing the sit-in that the group shared on Facebook.&lt;br/&gt;"I support bold action against the crisis of climate change," Fenberg said in the letter. "Today's young people are part of the generation that will be most impacted by the negative impacts of climate change, even though the public policy decisions that caused the crisis were not made by them."&lt;br/&gt;The group, called Fossil Free CU, continued to protest at the University Administrative Center after three days of sit-ins in Old Main. The students decided to move to the building after not receiving a response from the administration, according to group member P.D. Gantert. The students said that they will not leave until the university makes a statement about whether CU will divest its money from fossil fuels, and are willing to face arrest. They delivered a letter to the chancellor to the building. A police officer stopped by the scene but left and did not make arrests.&lt;br/&gt;Currently, CU says it maintains a politically neutral policy on where the almost $2.7 billion investment pool is invested, 3 to 4 percent of which is in the energy sector, as reported by the Daily Camera. &lt;br/&gt;"There's too much at risk right now for CU to stay neutral during the climate crisis," Gantert said. "We're tired of not getting answers after asking through so many forms."&lt;br/&gt;Gantert said that Jennifer McDuffie, assistant dean of students, came by the sit-in earlier in the day to offer the group meetings with other CU administrators. The students declined, waiting to hear from DiStefano directly.&lt;br/&gt;"We call for you to officially support the regents' divestment of our endowment from the top 200 carbon-holding corporations," the letter from Fossil Free CU to the chancellor read. "This is a call for investment in Colorado corporations and our future."&lt;br/&gt;Alana Wilson, a graduate student at CU, said she was at the protest because she wants to help mitigate climate change. She said she wants the administration to do more than make a statement about CU's commitment to environmentalism.&lt;br/&gt;While declining to change investment policy, a decision he said he does not to have control over, DiStefano applauded the student's passion in an letter sent to Fossil Free CU members on Wednesday.&lt;br/&gt;"I am proud to have you as students at this campus, expressing yourselves in a peaceful way and bringing attention to your position on these issues." DiStefano said in the letter.&lt;br/&gt;"These investments we have, the tens of millions of dollars invested in the fossil fuel industry, are another piece of the puzzle," Wilson said. "We talk the talk, but that's a way that our walk doesn't really line up with our talk."&lt;br/&gt;We will update this story as it develops.&lt;br/&gt;Contact CU Independent Copy Editor Carina Julig at  &lt;br/&gt;CU Independent Breaking News Editor Lucy Haggard contributed reporting.carbon Climate change DiStefano fossil free CU fossil fuel divestment sit-in2017-04-27Carina Julig</t>
         </is>
+      </c>
+      <c r="L111" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="112">
@@ -5339,10 +5679,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J112" t="inlineStr">
+      <c r="K112" t="inlineStr">
         <is>
           <t>Chancellor Phil DiStefano met with students belonging to Fossil Free CU to discuss the possibility of the University of Colorado's divestment from the fossil fuel industry. The group presented a letter, co-written with Regent Linda Shoemaker, asking the administration to acknowledge the effects of climate change and the influence that fossil fuels have on it. The meeting did not end with a definite resolution, although the group left feeling "hesitantly hopeful," according to P.D. Gantert, a recent CU Boulder graduate and one of the leaders of Fossil Free CU.&lt;br/&gt;The meeting got personal as DiStefano shared his experience of growing up in Steubenville, Ohio, and the harmful impact of the coal industry on the people around him and the local economy. The group, including CU Boulder student Lior Gross, acknowledged that the chancellor didn't have the power to override the Board of Regents, who control the CU system's investments. However, they held steady to their demand that the chancellor make a definitive statement encouraging divestment.&lt;br/&gt;"We are still looking to them to exhibit more leadership and so students are continuing to work with their office in order to come to a place of agreement," Gross said. They spoke to the CUI Tuesday night from the University Administrative Center, the site of the sit-in.&lt;br/&gt;"We know that the chancellor understands the threat that the fossil fuel industry poses to our communities and to our future. And that's why we are asking him to choose a side and to continue to lead with students, because while he remains declaring institutional neutrality, we know that the university investing in the fossil fuel industry is not a neutral position. And we understand that he comes from a place where he knows exactly how the fossil fuel industry threatens the community."&lt;br/&gt;Fossil Free CU is the primary student group on campus advocating for CU's divestment from fossil fuels. They have maintained the sit-in at the University Administrative Center since Thursday by rotating members in and out. Before settling into the UAC, they held sit-ins around campus last week, including at Old Main last Wednesday. They decided to move to the UAC to be more visible to the chancellor and his cabinet.&lt;br/&gt;In addition to working to talk with the Chancellor, the group has put increasing pressure on some of the CU Regents to act in accordance with divestment. On Monday, they met with Shoemaker, a Democrat representing Colorado's 2nd Congressional district. She was the first regent to work with Fossil Free CU, proposing a vote of divestment that did not pass the Board of Regents back in 2015.&lt;br/&gt;Shoemaker's office plans on releasing a formal statement on Wednesday. Members of Fossil Free CU who met with her said that the meeting was productive, solidifying their previous relationship with her as an advocate for a common goal.&lt;br/&gt;"We are looking to Regent Shoemaker to show leadership on the board and we know she'll do the right thing and stand with students for climate justice. And we're looking forward to working with her towards a vote in September [to move CU investment away from fossil fuels] at the Board of Regents meeting," Gross said.&lt;br/&gt;Fossil Free CU is currently working on contacting Regent Glen Gallegos, a Republican representing the 3rd Congressional district. They called him out numerous times on their Facebook page and have cited him as a necessary swing vote on the Board of Regents.&lt;br/&gt;The group also called out Regents Sue Sharkey and John Carson during an event they held Tuesday at the UMC fountains. Sharkey and Carson have both allegedly denied climate change. Fossil Free CU placed barrels with writing on them with statements like "students &gt; fossil fuel $" and "divest from destruction, invest in students' futures."&lt;br/&gt;Fossil Free CU planned the demonstration before the chancellor offered them a meeting. "[Divesting is] something we could do and something we should do," said Alex Koek, a member of the group and one of the organizers of the demonstration.&lt;br/&gt;Another demonstration organizer, Michaela Mujica-Steiner, emphasized the importance of calling out the specific regents.&lt;br/&gt;"People across Colorado have been building people power to resist the fossil fuel industry, and one of the main reasons that they have not been able to prevent fracking and these other projects is because of the entrenched money in our political system by the oil and gas industry," Mujica-Steiner said. "By being complacent and not choosing a side, Regent Gallegos is being complacent in the injustices and the exploitations of his own constituents on the Western slope."&lt;br/&gt;Tuesday was busy on other accounts as well. Earlier in the morning, a sign was posted on the outside of the UAC explicitly forbidding four reporters at the Daily Camera from entering the building. According to CU spokesperson Ryan Huff, the sign was unauthorized and a miscommunication between police, the third-party security staff hired to supervise the UAC while students sat in overnight and CU administration. The university apologized directly to the Camera as well as publicly.&lt;br/&gt;In the evening, Fossil Free CU held a public meeting in front of the UAC. Just over a dozen students gathered to discuss the current state of their campaign. Most were optimistic, having seen significant support from students and faculty over the past few days.&lt;br/&gt;The group will continue their sit-in for the sixth straight night. Calling from the sit-in, Gross said that though Fossil Free CU has made significant progress in their campaign since the beginning of the sit-in, they know there's a lot of work still to do.&lt;br/&gt;"I know this widespread support form the community is a very encouraging sign. We're in a position right now with the relationships we've been building with the regents and also the actions we've been taking on campus in order to get a vote. And I know that when students take action, we win on climate justice. So I feel confident that our university will do the right thing to side with students' futures instead of the fossil fuel industry."&lt;br/&gt;Contact CU Independent Breaking News Editor Lucy Haggard at &lt;br/&gt;CU Independent Staff Writers Devlin Thieke () and Stephanie Wood () contributed reporting.fossil free CU protest Regents sit-in2017-05-03Lucy Haggard</t>
         </is>
+      </c>
+      <c r="L112" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -5382,10 +5725,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J113" t="inlineStr">
+      <c r="K113" t="inlineStr">
         <is>
           <t>Just after 5 p.m. Wednesday, CU Boulder administration ended a sit-in by Fossil Free CU protesters in the University Administrative Center that lasted nearly seven nights.&lt;br/&gt;Fossil Free CU is a student group on campus advocating for CU's divestment, or removal of investments, from the fossil fuel industry. They maintained the sit-in at the University Administrative Center since Thursday by rotating members in and out. Before settling into the UAC, they held sit-ins around campus last week, including at Old Main last Wednesday. They decided to move to the UAC to be more visible to the chancellor and his cabinet.&lt;br/&gt;Dean of Students Akirah Bradley and Assistant Dean of Students Jennifer McDuffie presented a letter Wednesday from the chancellor to Lior Gross, one of the undergraduate student leaders of the activist group. The deans then told Gross, the only student at the sit-in at the time, that they had to leave immediately or risk arrest.&lt;br/&gt;CU Boulder police removed the possessions from the conference room where the group settled in for the protest. The students were not notified of the location of their belongings until 7:14 p.m., at which point they received an email detailing that they could be picked up at the UMC after showing photo identification.&lt;br/&gt;"We've had plenty of dialogue," said Ryan Huff, spokesperson for CU, adding his opinion that the students stayed in the building long enough and that the sit-in was disruptive of the building's functions.&lt;br/&gt;The letter administration gave the group was an edited version of the original letter that Fossil Free CU presented to the chancellor at their meeting Tuesday. The original letter, written in collaboration with Regent Linda Shoemaker, was formatted for the chancellor to modify and release to address Fossil Free CU to say definitively whether the university would remove its investments from the fossil fuel industry. The group's goal in protesting was to push the chancellor to publicly take a stand on that question. The edited, officially released letter by the chancellor said that CU supported students taking "non-violent direct action" to advocate for environmental justice. Additionally, it said that the chancellor supported that the group work with the board of regents on divestment.P.D. Gantert holds up the letter Fossil Free CU received shortly before CU administration removed them from the University Administrative Center May 4, 2017. (Lucy Haggard/CU Independent)&lt;br/&gt;The letter thanked students for the "peaceful and respectful way" they carried out the sit-in. The chancellor went on to encourage students to continue a dialogue with the regents on divestment, but he did not give direct support for that action in the way that the group had hoped.&lt;br/&gt;"[The chancellor] doesn't have the authority to do it and he's not the person in a position to make that decision," Huff said. "He's said that all along."&lt;br/&gt;After their meeting with the chancellor Tuesday, many members felt hopeful that a resolution could be reached that would please all parties. They understood that the chancellor could not directly make the choice to divest, but hoped that he could advise the regents to do so. Since the beginning of the protest, they planned to continue the sit-in until they received support of divestment from the chancellor.&lt;br/&gt;"This clearly shows me that the administration has chosen a side, and it's not the side of the students," Gross said. "After a lot of the work we've been doing, knowing we have the support of the campus behind us, and to have the administration treat students this way after all we've done is be respectful, without any notice or giving us time to pack up our stuff, that they could just kick us out - this was not expected at all."&lt;br/&gt;Fossil Free CU members said they think CU administration took advantage of the fact that Gross was the only student in the building at the time. The group also alleged that administration used Gross' status as an undergraduate student against them throughout the sit-in, starting with the group's action at Old Main last Wednesday.&lt;br/&gt;"They know Lior didn't want to be arrested," said P.D. Gantert, a recent CU graduate and a leader of Fossil Free CU. "The entire action they've been holding everything above Lior's head. They said as the main student leader, everything's on [Lior's] head, and [they] could be looking at university sanctions for activities here. They've threatened academic probation."&lt;br/&gt;Fossil Free CU plans to hold another action on Friday.&lt;br/&gt;Contact CU Independent Breaking News Editor Lucy Haggard at  broadway Breaking News campus Chancellor Chancellor DiStefano Climate change cu boulder divestment Environment fossil free fossil free CU fossil fuel industry Phil DiStefano protest sit-in university administrative buliding university of colorado2017-05-04Lucy Haggard</t>
         </is>
+      </c>
+      <c r="L113" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -5429,10 +5775,13 @@
           <t>Far Right/Alt Right (Against), Hate speech, _Other Issue</t>
         </is>
       </c>
-      <c r="J114" t="inlineStr">
+      <c r="K114" t="inlineStr">
         <is>
           <t>In the past two years, the University of Michigan has seen several acts of hate targeted at people of color and minority groups across campus.&lt;br/&gt;In September 2016, flyers advocating white supremacy were found on campus posting walls. In February, engineering students received racist and anti-Semitic emails from hacked email accounts. This September, the Rock, a campus landmark, was found graffitied with anti-Latino and pro-Trump expressions. In October, racist slurs were found on the residence hall doors of three Black students in West Quad Residence Hall.   &lt;br/&gt;In the aftermath of these incidents, campus communities have not stood idly by. Hundreds of students have rallied against racist flyering, graffiti and a variety of other attacks. In late September, Rackham student Dana Greene knelt in the Diag for 21 hours to protest racism on campus and across the country; dozens of other students joined the peaceful protest.    &lt;br/&gt;The University administration has taken steps to respond to acts of hate and its historically low minority enrollment. In October 2016, the University launched its five-year Diversity, Equity and Inclusion strategic plan, which aims to foster a diverse and inclusive campus, while also supporting inclusive scholarship and teaching. Diversity has been especially difficult in the University, since practicing affirmative action has been banned in the state since 2014 despite the University's attempts to appeal the vote.  &lt;br/&gt;When the plan was implemented, then-Provost Martha Pollack, who is now the president of Cornell University, said the recent racist incidents only emphasized the need for the plan.&lt;br/&gt;"It's only human to respond with anger and sometimes with fear, emotions that have been felt deeply on this campus," she said. "I share the grief and outrage felt by our students, faculty and staff. We must cling to the vision of what the world must be ... and that is what the Diversity, Equity and Inclusion plan is all about."&lt;br/&gt;However, also pertinent to DEI, the University ranked last in terms of socioeconomic mobility and diversity among top public universities. According to a report by the Equality of Opportunity Project, which was highlighted by The Upshot - a data analytics section of the New York Times- 66 percent of students come from the top 20 percent of the income distribution and students have the highest median family income of 27 "highly selective" public colleges.&lt;br/&gt;The DEI plan has been criticized for failing to foster a diverse environment and for failing to put a stop to racist incidents. After the racist emails were sent out in February, students protested outside University President Mark Schlissel's house calling for "action, not emails," referencing the University's digital statement, which showed its support for those attacked, but no further action.&lt;br/&gt;"Schissel WYA" is a common rally of for University students, criticizing University President Mark Schlissel's response to the incidents. In mid-September, students gathered in front of the president's home and posted flyers on his door. Schlissel was at a family event during this time.&lt;br/&gt;Postdoctoral fellow Austin McCoy was not surprised by the University's response.&lt;br/&gt;"From the administration, I anticipate them sending out probably an email and saying that they condemn the acts and then that they're investigating, but other than that, I don't know what else the administration plans to do," he said in February. &lt;br/&gt;However, such incidences and responses are not unique to the University of Michigan campus. Post-election, campus climate and rallying students have been points of debate across the country.&lt;br/&gt;Conservative criticism refers to liberal students as too sensitive and ignorant of free speech - worried for conservative students and their lack of voice on more Democratic campuses. The University of Chicago even shut down the concept of "safe spaces" - sparking what some call a clear rebuke of political correctness. Liberal students, however, hope to protest the turn of the administration along with the fear of rhetoric that they deem bigotry and do not wish to give such thought a platform.&lt;br/&gt;This article is part one of a series in which The Michigan Daily looks at colleges similar to the University of Michigan on the issue of reacting in a tense campus climate. As the University administration and students face their own numerous bias incidents, The Daily will look at other schools to compare and contrast in incidents, administration response and student activism, whether it is a difference in religion, culture, politics or policies.&lt;br/&gt;Cornell University&lt;br/&gt;Juliana Rosana Montejo graduated from Cornell University in May 2017. Montejo is Guatemalan and came from a predominantly white high school. She said when she entered the university in 2013, she wasn't really aware of incidents on campus.&lt;br/&gt;"Long story short, every semester there has been something," she said.&lt;br/&gt;Cornell University, located in Ithaca, N.Y. - a blue state - ranks similarly to the University of Michigan in terms of the Upshot's SES status - albeit in the private school category among other Ivy Leagues. Out of 14,907 undergraduate students, Cornell has 6,462 students of color - 43.34 percent. In the graduate program, it is 17.94 percent. Cornell also uses affirmative action in admission.  &lt;br/&gt;In fall 2013, a campus organization that promotes Cornell sporting events attempted to increase support for an upcoming football game by creating a "Cinco de Octubre" event, which incorporated racist caricature depictions of Mexican Americans. Montejo said there was a prize given to whoever dressed up as the "best Mexican."&lt;br/&gt;Since then, Montejo said, there have been a variety of incidents that have primarily targeted Black people and people of color generally. She said she met many people involved with activism at Cornell and in her senior year, she served as vice president of diversity and inclusion on the Cornell Student Assembly.&lt;br/&gt;"A big part of why I started getting more involved was that there had just been a lot of things building up, and I think we were kind of at a culmination of, 'Oh there were some of these undertones there already,' and now it's kind of coming to a point where it's kind of exacerbated," she said.&lt;br/&gt;Montejo also said such hateful incidents became more prevalent after the 2016 election. She explained Cornell is known to be a liberal school; subsequently, there is a claim that conservative ideas are oppressed on campus.&lt;br/&gt;"The conversation wasn't automatically, 'What can we do for people of color?'" she said. "A lot of it became, 'Look at these poor conservative students who aren't able to speak their minds.'"&lt;br/&gt;She said at the end of 2016 and in early 2017, there were two resolutions brought before the student assembly to create task forces to investigate why there are so many liberal professors at the school. There have also been calls for the university to do more to protect conservative speakers who come to campus. She said there have been more visibly proactive actions to help conservative students.&lt;br/&gt;Montejo also said that whereas prior to the election, there seemed to be one or two major acts of hate every semester, there is now something happening all the time.&lt;br/&gt;Last month, a Cornell student was arrested by Ithaca police for a hate crime, according to the The Cornell Daily Sun. A Black student, who asked to remain anonymous, told the Sun he confronted four or five white men who were shouting racist slurs at him; they then proceeded to beat him.&lt;br/&gt;In Michigan, during one of the protests after the racist vandalism, an individual was punched by a white man who also called them racial slurs.&lt;br/&gt;Black Students United at Cornell released a statement saying the perpetrators were members of the Psi Upsilon fraternity, which already had its recognition revoked on campus. The building is to be remade into a multicultural center.&lt;br/&gt;Pollack, now Cornell's president, released a statement in response to the incident - and others preceding it - citing steps the administration will take to create a more equitable and inclusive campus. Among them was a promise to take disciplinary action against the perpetrators of the aforementioned attack and a commitment to not reinstating the fraternity.&lt;br/&gt;"I will not tell you 'this is not who we are,' as the events of the past few weeks belie that. But it is absolutely not who we want to be," the statement read. "The leadership team and I have been working throughout the weekend, and we will continue to do so, to develop and implement steps to be a more equitable, inclusive and welcoming university."&lt;br/&gt;Meanwhile, Black Students United declared a "state of emergency for black students" in response to the incident. The group blamed the university for creating the Campus Code of Conduct, which protects white supremacists' hate speech. They recognized it would be difficult to change the policy but felt it would be possible with help from the greater university community.&lt;br/&gt;In mid-September 2016, Black Students United handed a list of demands to Pollack, including racial sensitivity training for all employees and a space for Black students on campus.  &lt;br/&gt;Prior to creating an official list, Black Students United members met with Dean of Students Vijay Pendakur right after the assault. They were frustrated Pollack did not reach out to them until three days after the assault; they were also frustrated that many of the ideas they brought up in their meeting with Pendakur were presented in Pollack's letter, without recognition. &lt;br/&gt;Anti-Semitic posters have also been seen on Cornell's campus and Pollack has denounced these incidents as well.&lt;br/&gt;Looking at responses to acts of hate on Cornell's campus overall, Montejo said there appears to be a lot of support.&lt;br/&gt;"In terms of climate change I think to your face it seems like there's a lot of support," she said. "But behind the scenes, there's a lot of weird antagonism that's going on."&lt;br/&gt;Beth Garrett, Cornell's thirteenth president, passed away after a battle with colon cancer in March 2016. However, according to Montejo, when Garrett came into office she hired Ryan Lombardi, vice president for student and campus life. According to Montejo, Lombardi re-envisioned the Office of the Dean of Students and the dean of students position as one that would be very focused on diversity and inclusion issues.&lt;br/&gt;Additionally, she said Cornell has used polls to gauge how students feel about diversity and inclusion issues - the University has also had campus climate polls - and has always addressed campus climate even without major incidents occurring. Cornell has diversity officers through its Diversity and Inclusion initiative to better promote a welcoming and inclusive campus, as well as a bias reporting program.&lt;br/&gt;Montejo explained the administration always sends out statements to the campus community in response.&lt;br/&gt;Montejo noted Ivy League schools are definitely targeted. In November 2015, for example, hundreds of members of the Yale University community marched in support of minority students who felt they were not fully included on campus. According to The Washington Post, protesters rallied in support of women of color, faculty of color and ethnic studies; one person carried a sign that read: "Your move Yale."&lt;br/&gt;The theory that prominent, progressive schools are being targeted has floated around before - especially with Washtenaw as a blue county in a newly turned red state. In an earlier interview with The Daily, Schlissel said there might not be a way to mitigate the target on the University's back.&lt;br/&gt;"I think that part of being a prominent university, taking clear positions on things, having large numbers of very successful graduates out there in the world, being on TV all the time, being in the media all the time means that what happens here gets noticed," he said. "That's the sort of other side of this double-edged sword of being famous and prominent. ... It's because of our prominence that provocateurs realize they can use us as a platform that the national media will pay attention to, to spread their terrible, thoughtless, degrading, awful ideas. They're using us."&lt;br/&gt;Montejo said she believes Cornell is generally diverse. According to Cornell's Composition Dashboard from fall 2016, 39.5 percent of undergraduates were white, while 42.3 percent were from minority groups. Despite that, she said groups that have disproportionate power on campus include those that are white, including the Interfraternity Council.&lt;br/&gt;"I felt really compelled and pushed to join a Panhellenic sorority, and while I had a great experience there, it did kind of feel like there was a disproportionate amount of influence of power in that structure because of its whiteness," she said.  &lt;br/&gt;Though the administration has taken a lot of positive steps, Montejo said there are gaps that need to be filled. She said she feels there is a lot of movement on reactive measures but not nearly as much around proactive members.&lt;br/&gt;In an email response, Cornell's Media Relations Office pointed The Daily to several of its official statements.&lt;br/&gt;University of California at Berkeley&lt;br/&gt;Some say Berkeley has been the poster child of college campus activism this year - the pushback against controversial speakers has been widely documented in the media. Notably, while activism has escalated to violence, much of it has occurred in the campus vicinity, not specifically at the university.&lt;br/&gt;Billy Curtis is the director of the Gender Equity Resource Center at University of California at Berkeley. Strictly in terms of reports, Curtis said, there has been an uptick, but quickly explained that like with incidents of sexual violence, as there are increases in education and awareness, there are more reports. It's unclear whether there are more incidents or more reports.&lt;br/&gt;Another challenge UC-Berkeley faces, according to Curtis, has to do with protocols for a response. Many victims and members of communities that are targeted feel the chancellor needs to respond.&lt;br/&gt;"We're trying to figure out always, when does the chancellor respond? What does that response look like? How do people feel cared for, seen, heard, tended to?" he said. "I think that's the biggest challenge because too often what we're really dealing with isn't necessarily just a campus climate issue, we're dealing with our sociological problems of the United States."&lt;br/&gt;UC-Berkeley is taking steps to make the campus more inclusive and address the needs of students from marginalized communities. The Division of Equity &amp; Inclusion provides a variety of programs and services.&lt;br/&gt;On Sept. 1, the division launched the Campus Climate, Community Engagement and Transformation unit, whose mission is to focus on "reshaping and influencing policies and practices that increase opportunities, advance social justice and create equitable experiences for all groups, with a special focus on marginalized and underserved populations."&lt;br/&gt;The initiative's website also highlights results of a spring 2013 campus climate survey, which showed 1 in 4 community members have experienced exclusion on campus. It also showed undergraduates who are not African American overestimate the inclusivity of the climate for the group. For instance, 89 percent of Asian students and 87 percent of white students rated the climate as "respectful" or "very respectful" for African Americans; African Americans rated the climate as 47 percent for the categories. Additionally, on the survey, a top concern was not having channels through which to report discrimination and the notion that faculty judge students based on their perceived identities.    &lt;br/&gt;That being said, in fall 2017, 2.9 percent of enrolled freshmen at UC-Berkeley were African American or Black, 9.9 percent were Mexican American or Chicano, 3.7 percent were labeled "other Hispanic/Latino." White students constituted 24.5 percent of the freshman class.&lt;br/&gt;Other initiatives through UC-Berkeley's diversity division include a Campus Climate Speaker Series, which brings scholars and activists to campus to address related issues, and Innovation Grants, which provide funding for projects focused on increasing equity and inclusion on campus.&lt;br/&gt;Still, UC-Berkeley has seen hate acts in the past year. In September, posters listing 13 specific community members and identifying them as "terrorist supporters" were found on campus, according to The Daily Californian. Some of the victims in the past had vocalized their support for Palestinian divestment from Israel.&lt;br/&gt;In a statement sent to the university community, UC-Berkeley Chancellor Carol Christ condemned the acts. She highlighted the school's Principles of Community, among which are a commitment to respect the differences and commonalities of all people.&lt;br/&gt;"Berkeley is better than what these incidents reflect," the statement read. "Many things contribute to the fact that we are the nation's number one public university, and a strong component is the care, respect and esteem which we have for our fellow campus community members. As we move into the events of next week, please join me in upholding these values."&lt;br/&gt;Four days after the posters were found, conservative writer Milo Yiannopoulos spoke at Berkeley. According to The Daily Californian, Yiannopoulos was originally invited to speak by the student group the Berkeley Patriot - a conservative group on campus - as part of the "Free Speech Week," in which several conservative speakers were coming to campus. Amid confusion surrounding the event and the Berkeley Patriot actually filing a complaint with the Department of Justice, claiming Berkeley was infringing free speech rights, the event was canceled. Still, Yiannopoulos - and other speakers - came to campus and were met by a crowd of protesters.&lt;br/&gt;In an interview with The Daily Californian, Pranav Jandhyala - a news editor for the Berkeley Patriot and who founded the organization that invited Ann Coulter - explained the situation became too complicated and the group had to pull out of the event.&lt;br/&gt;"It became a situation that we just had to get out of because of the complications," Jandhyala said.&lt;br/&gt;Meanwhile, the Yvette Felarca, an organizer for Berkeley's By Any Means Necessary pointed to the need for a sanctuary space.&lt;br/&gt;"To protect the community (and make) it a sanctuary campus, that means actively defending it," Felarca said.&lt;br/&gt;The University faced its own slew of controversial speakers - the latest being Charles Murray, known for "The Bell Curve," which argues the correlation of IQ and race. McCoy said speakers like Murray use student anger as a platform.&lt;br/&gt;"I'm not really going to say much about what's his name -- Charles Murray -- I don't really care about Charles Murray, I think he's irrelevant," he said. "I think he's just trying to use protests, I think he's trying to use student anger to rebuild his career. So, think about this. He has to use students to get a come-up."&lt;br/&gt;LSA senior Ben Decatur, co-chair of the AEI Executive Council at the University, defended Murray's right to speak on campus.&lt;br/&gt;"If the hosts of tonight's program, in collaboration with University representatives, believe that the protesters are interfering unduly with the speaker's freedom of expression, those protesters will be warned by a University administrator," Decatur said. "If warnings are not heeded and interference continues, the individuals responsible may be removed from the building."&lt;br/&gt;Berkeley freshman Justin Kim serves on the Hall Association at UC-Berkeley. In an interview with The Daily, he described the controversy surrounding Yiannopoulos's visit to campus. He said there were police and blockades for the entire week around Sproul Plaza, where the event took place.&lt;br/&gt;In terms of how the school responds, Kim explained the Berkeley Police Department and administration have worked together to send email advisories about crimes on campus to the community.&lt;br/&gt;"During Free Speech Week, or when it was supposed to happen ... even leading up to it, we got notifications to avoid the area," he said.&lt;br/&gt;He noted that Christ released a statement, which stated the university is committed to free speech, as exemplified by the speakers on campus, even though they put forth ideals that "run counter" to those of the university.&lt;br/&gt;"To provide the security necessary to protect the community, we have had to close buildings, relocate students and workers, bring to campus a police presence that some find intimidating, and spend money that we would have much rather put toward our academic and research mission," the statement read.&lt;br/&gt;Kim explained earlier in the fall there was an event in which UC-Berkeley students could ask Christ any question. There is also a way for students to write letters to the chancellor, which are directly delivered by the president of the Associated Students of the University of California - the UC-Berkeley student government.&lt;br/&gt;Regarding hate acts and the reactions they prompt, Curtis explained the campus climate shifts based on the level to which the incident rises.&lt;br/&gt;"Someone writing something on a residence board in a residence hall on one floor, I may be aware of it, but it usually doesn't rise to the level of impacting a larger community because it's a one-off - unless there are enough instances in the residence halls that are targeting folks, and students are feeling like, 'Wow, there's a lot of racist things, or a lot of anti-Semitic things said,' and that's happened over the years," he said. "But all of a sudden it starts to bubble up."&lt;br/&gt;Graffiti on a building, he explained, will rise to different levels because it is far more public and more people see it. He said it creates a different level of response.&lt;br/&gt;Curtis also noted UC-Berkeley has been in the media as a result of certain speakers coming to campus and impacting the campus climate. Students, for example, can report that they feel unsafe and unwelcome on the campus in response to an event like that.   &lt;br/&gt;He explained that while many programs and offices work to educate the campus and make it more safe, inclusive and accessible for marginalized groups, racism and other forms of bigotry are still prevalent in the United States. Due to a variety of reasons, he explained, the campus climate changes.&lt;br/&gt;"It's not static, we're not working in a place where everyone remains the same forever more, or there's little turnover," he said. "We have large turnover because our student body turns over, and they're coming from their communities and their experiences ... and in the modern era - the modern era of information and social media - we're now impacted by things that happen in the virtual world. The things we may create on campus don't necessarily stop or even mitigate the stuff around hate and bias acts; (the two) can work in concert but I've not seen it stop."</t>
         </is>
+      </c>
+      <c r="L114" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="115">
@@ -5472,10 +5821,13 @@
           <t>Environmental, Trump and/or his administration (Against)</t>
         </is>
       </c>
-      <c r="J115" t="inlineStr">
+      <c r="K115" t="inlineStr">
         <is>
           <t>A group of 60 CU students and high schoolers from Boulder's private Watershed School walked out of classes Monday to rally against President Donald Trump's plans to deregulate federal policy on the environment.&lt;br/&gt;The rally, called "Resist and Reject Denial," was organized by Fossil Free CU, an environmental awareness group that pushes for CU to divest its stocks and assets in the fossil fuel industry. But the rally brought in several environmental groups that focus on protecting the air, water supplies and anything that can combat climate change.&lt;br/&gt;"We're basically protesting banks that support fossil fuels and anyone who is saying they're going to support fossil fuels in the near future," said Ellie, a student from Watershed. "It's not a sustainable industry, and it's not something we can rely on."&lt;br/&gt;The group specifically targeted Wells Fargo and any local banks in Boulder that do business with it.&lt;br/&gt;PD Gantert, a CU graduate and former leader of Fossil Free CU, organized the event knowing the new presidential administration will shift policy on the environment compared with the previous Obama administration.&lt;br/&gt;"I think that it's imperative that people ask for what they need. And what they need right now is an administration that has their back in the time of Trump," Gantert said. "This rally is a really exciting opportunity to reconnect with the students that are also feeling the sadness and anger right now."&lt;br/&gt;The Trump administration has made it clear that combating climate change will not be a priority. As soon as the president was sworn in on Friday, the White House removed its page on climate change. Additionally, Trump's cabinet consists of several climate change deniers, including secretary of energy nominee Rick Perry, Environmental Protection Agency nominee Scott Pruitt, and secretary of state nominee Rex Tillerson  - the former CEO of oil corporation Exxon - indicating that the federal government could quickly shift from renewable energy efforts to more fossil fuel production with fewer environmental regulations to curb greenhouse gas emissions.&lt;br/&gt;In April 2015, Fossil Free CU lobbied the CU Board of Regents to exclude fossil fuels from its investment portfolio. That effort failed, but the current head of FFCU, Lior Gross, said they can still make a difference.&lt;br/&gt;"The reason they voted for our referendum in the first place is because our campaign pushed them to a point where they had to decide, and that just shows the power of our organizing," Gross said. Gross also said they would continue to get more students to join their cause and continue to press the regents for change.&lt;br/&gt;Other students like Xiuhtezcatl Martinez, a member of activist group Earth Guardians, is involved in suing the federal government for environmental degradation on constitutional grounds.&lt;br/&gt;"The constitution says that we have an inalienable right to life, liberty and property," Martinez said. "We believe that climate change is a violation of those inalienable constitutional rights and our government has failed us to protect us from the impacts of climate change." Martinez said the lawsuit is slated for Feb. 20.&lt;br/&gt;On Monday, The Trump administration announced cuts to the EPA by as much as $500 million. President Trump also stated during the presidential campaign that climate change is a hoax, and in July 2016 told a group of California farmers that there is no drought.&lt;br/&gt;Contact CU Independent Assistant Visuals Editor Jesse Hughes at  News Climate change demonstrationr donald trump Environment fossil free CU global warming News protest rally resist and reject denial Trump administration UMC umc fountain watershed school2017-01-24Jesse Hughes</t>
         </is>
+      </c>
+      <c r="L115" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -5520,10 +5872,13 @@
           <t>Immigration (For), Anti-racism</t>
         </is>
       </c>
-      <c r="J116" t="inlineStr">
+      <c r="K116" t="inlineStr">
         <is>
           <t>This week, we will stray from our standard editorial form. Instead, we provide you with a how-to guide for being politically active in a turbulent time when people's rights are at risk. This guide is woven from many similar online resources and contextualized by the advice of student and faculty activists here at Middlebury. In past weeks, we - and several op-ed writers - have extolled the virtues of speaking with others who differ from yourself, emotionally supporting those who are immediately harmed by the new administration's policies and being politically active and aware. But these general sentiments, while true and important, possess a false ring to them: They simply aren't actionable. As such, we hope to provide you with a sampling of tools to get working on our larger community goals and encourage everyone to become politically active.&lt;br/&gt;Everyone on this campus has the capacity to make a difference. The main tools we can access to do so include our financial resources, the press, public space and protest, our legally protected rights, our education and avenues for contacting our representatives. We will describe specific ways in which students can create an impact through each of these points. If we each engage in as many ways as we are able to, and as often as we are able to, our collective impact can be huge. Today, participation remains a fundamental key to success. Nia Robinson '19, president of the Black Student Union, emphasizes this aspect. "Activism is such a broad term, so we also suggest that people find the avenue that makes the most sense," Robinson told us. "Some people write, some can organize rallies, some are good with talking with people in power. Every action counts." Whether your own action entails donating a single dollar each month, taking five minutes a week to call your senators or spending eight hours out of a weekend at a rally - every action, no matter how big or small, counts.&lt;br/&gt;DONATIONS &amp; SPENDING&lt;br/&gt;First, let's talk money. Every one of us has at least one way to influence some flow of money. As students at Middlebury, we can exert such influence through the College by advocating for the school's divestment from industries we dislike and disagree with. For example, student groups have long lobbied the College to divest from oil and privatized prisons. More directly, we can donate to established organizations who are fighting discriminatory policies with their ample expertise and networks. For those with the means of doing so, you can convince family and friends to make personal contributions to these same causes. Besides the ACLU and Planned Parenthood, there exist many local organizations supporting refugees, LGBTQ youth and other people who are likely to be targeted by new legislation. Locally, for example, WomenSafe fights domestic and sexual violence and welcomes donations and volunteers.&lt;br/&gt;We can also use the capitalist, consumer system to generate pressure for change. There has been a flurry of activism surrounding the redistribution of money. For example, activists successfully harnessed the power of social media to boycott Uber after the rideshare company made a statement in support of President Trump. As a result of the boycott and the media it sparked, Uber has backtracked on its statement and vowed to hire more immigrants. Instagram is also full of less conscientious consumers who proudly claim to be an activist by spending $4.45 on a Grande Caramel Macchiato (because Starbucks, as an entity, has expressed disagreement with President Trump). We can have an impact by thoughtfully spending only at businesses whose views we condone, but determining the best way to spend requires another layer of research and thoughtfulness to be truly meaningful.&lt;br/&gt;THE PRESS&lt;br/&gt;You can use your money to be heard, but you can also use your voice. Here at the newspaper, we believe in the power of the press. President Trump has called the press "the enemy of the people" and slandered reputed news sources as "fake news." One way to support the free press is to activitely participate in and contribute to it. Submit letters to the editor (typically very short responses to previously published articles or current events) or op-eds (approximately 600-800 word think pieces about current issues) for your local newspaper or to this newspaper. (The Campus opinions editors will work with anyone who submits a piece to publish their work.) Use these platforms to call your representatives and fellow citizens to action.&lt;br/&gt;LOCAL EVENTS&lt;br/&gt;You can also make your voice heard at town halls or local rallies and protests. Here in Middlebury, Director of Chellis House Karin Hanta has organized a weekly Resistance Tuesday series, which held its kick-off event this past Tuesday. The open discussions will be held at the College Park (across from Sama's) every Tuesday at 12:30 p.m. According to Hanta, the events are a place to join with other activists "to discuss the issues of the day and find strength in solidarity." Chellis House is also organizing several events throughout the semester focusing on reproductive health and justice. The Gensler Symposium, held April 13 and 14, will be about "Sex and the State."&lt;br/&gt;Also on campus, Professor of Political Science Matt Dickinson runs a political lunch on Tuesdays, and the Middlebury's First 100 Days Facebook page posts events and resources for students. As we wrote last week, the Muslim Students Association recently hosted a rally against discriminatory immigration policy. Other student organizations will likely hold talks and rallies throughout this semester.&lt;br/&gt;Liz Dunn '18 from Women of Color advises students to attend socially oriented club meetings. "One of the most crucial things for people to do is begin to build solidarity with groups they don't necessarily belong to," Dunn told us. "Easy starting points could be going to meetings that are socially oriented, [like] WOC and other cultural orgs like Alianza, BSU [and] FAM have open meetings and are always open to people who are ready and willing to respectfully and honestly engage with these issues."&lt;br/&gt;KNOW YOUR RIGHTS&lt;br/&gt;When attending a protest, know your rights. There are many guides online that describe your rights in case of arrest at a protest. They typically recommend bringing the number of a lawyer and an emergency contact with you to the event, even writing them on your arm if you are concerned about your phone being confiscated or lost. If you are told you are being arrested, do not resist. Do not answer any questions and respond only with "Can I speak to an attorney?"&lt;br/&gt;Many online guides also share advice for immigrants targeted by the Immigration and Customs Enforcement office. If ICE officers come to your house or that of a family member, you are not required to let the officers in. Ask if they have a warrant. You are not required by law to let them into the house unless they can produce a physical copy of the warrant.&lt;br/&gt;GET EDUCATED&lt;br/&gt;Throughout this guide, we have referred often to online resources. There is a wealth of information online. Use these resources to inform yourself and your friends. Learn more about issues you care deeply about and also those you don't know little of. There is a lot to learn from other activists not only in terms of content about the issues but also in terms of activism strategies. Robinson also suggests learning about successful activism. "Look at history and recent accounts of what people have been doing. From teach-ins, to lectures, to art based events, there are ideas that will work for Midd and beyond." For example, the Tea Party was highly successful at influencing their representatives and creating waves in the Republican Party. Activists today can co-opt their strategies to similarly impact today's representatives.&lt;br/&gt;CONTACT YOUR PEOPLE&lt;br/&gt;Finally, perhaps most obviously, you can contact your representatives. Congress's phone lines have been ringing off the hook since the inauguration, and many activist groups want to continue the flood of feedback. In a political system where constituent preferences are often ignored in favor of donor interests, Representatives and Senators will be unable to ignore the huge volume of constituent feedback.&lt;br/&gt;The most direct way to contact your representatives is to call them at their state offices. Former Congressional Staffer Emily Ellsworth became Twitter-famous when she posted advice for calling your representatives. According to Ellsworth, Tweeting at your reps, or contacting them on Facebook is largely ineffective. She recommends calls to the state office or letters to the state office over contacting their Washington offices or using email. Keep your statement brief and concise: "Hello, I am a constituent from X. I support/do not support Y. Please do/do not support Z legislation relevant to this issue. Thank you."&lt;br/&gt;The massive constituent response to recent legislation has already had an impact in Congress. A proposal to abolish the House's Office of Congressional Ethics was trashed, two Republican senators voted against Betsy DeVos's Secretary of Education nomination and Rep. Jason Chaffetz (R-UT) pulled a bill to sell off federally owned lands after overwhelming feedback from voters.&lt;br/&gt;Whether or not you want to call yourself an "activist," there are many paths to fighting off the negative effects of Trump's malicious policies. Even from our small college on the hill, our actions can make a difference. In closing, we want to leave you with a final piece of advice: take care of yourself. We recommend picking three big issues to focus on, rather than spreading your energy thinly across many fronts. Choose two issues that are close to your heart and impact you the most, and one issue that affects someone else. Dedicate as much time and energy as you can afford to fighting harmful legislation around these issues and promoting a more just and open community, and then take a break. Experienced activists have noted the fatigue that can quickly set in after working for an intense and emotional cause; taking days off (especially away from the constant stream of negative news in our Facebook news feeds) can keep us energized for the long haul. And these four years are looking like they will be a very long haul.</t>
         </is>
+      </c>
+      <c r="L116" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="117">
@@ -5563,10 +5918,13 @@
           <t>University governance, admin, policies, programs, curriculum, Labor and work, _Other Issue</t>
         </is>
       </c>
-      <c r="J117" t="inlineStr">
+      <c r="K117" t="inlineStr">
         <is>
           <t>When, in a given system of governance, constituents petition their representatives to make a change and receive no response or reaction to their petition, what is their recourse?&lt;br/&gt;They could continue to have faith in the very system that failed them and try time and again to achieve incremental success. They could, miraculously, achieve total victory after a long, drawn-out battle. Or they could work outside the system and try to disrupt the status quo in their favor and send a strong message to those in charge.&lt;br/&gt;This latter approach consists of protesting, and it is precisely the tactic that the Student/Labor Dialogue has employed to combat the alleged mistreatment of campus dining workers, the supposed result of significant mismanagement and ignorance by the College and by Bon Appe?tit, Vassar's new food provider.&lt;br/&gt;In this week's column, as with many of my past columns and as I laid out in my first article of this year, I feel I have no choice but to scrutinize my own side on this issue. I ask the scores of progressive readers who have already begun formulating their angry comments to hold off on that for just a moment and hear me out. Here is why:&lt;br/&gt;About three weeks ago, I was extremely concerned both about the financial feasibility of a more labor-friendly budget-given the hits that the endowment has taken in recent years-as well as about the actual ability of this less-than-flashy protest movement to gain the support of the Vassar community. While I recognize that these concerns came from a vantage point of significant privilege, they were legitimate thoughts about the movement all the same, and I believe it is incredibly important that anything and everything in the public sphere be scrutinized appropriately. That being said, I no longer have those concerns.&lt;br/&gt;They were resolved for me at the Student/Labor Dialogue protest at the Deece on Friday, Sept. 15. Two things about that protest stood out to me and caused me to abandon my preconceived notions. For one thing, the turnout of hundreds of&lt;br/&gt;students representing a diverse range of student groups who were quite earnestly and passionately fighting against the disrespectful treatment of Vassar's kitchen workers showed me that this issue does indeed resonate with a significant number of students.&lt;br/&gt;What really shook me, however, was the passionate and powerful testimonial given by Cathy Bradford, an ACDC worker and a Service Employees International Union representative. Her speech at the rally was, quite simply, spectacular.&lt;br/&gt;She talked about a serious problem in a straightforward manner and with a very simple diagnosis, illustrating a stark and sensible correlation-causation relationship between the advent of Bon Appe?tit at Vassar and the consequent woes of the kitchen staff. She gave real, human examples of the hardships that Vassar employees have been facing and continue to face every day. She presented solid facts in support of her argument, gave reasonable context to the issues she was attempting to tackle and laid out both a pragmatic and concise agenda on just what needs to be done. All this was achieved, no less, while giving a speech that the crowd and I found deeply moving.&lt;br/&gt;Nevertheless, I felt I had to take a deeper look not at the intentions or ideology of SLD or Bradford, which are, to be sure, clear and admirable, but rather the effectiveness of their tactics in influencing Vassar's power structures. Their demands of the administration and of Bon Appe?tit are as follows: 1) that they ensure safe, stable working conditions, 2) that they post organized and regular work schedules and 3) that they maintain fair and transparent hiring processes.&lt;br/&gt;The Vassar administration has said, more or less, that it feels unmotivated to take action on this issue. Thus it appears that the SLD rally, despite its strong student turnout, has failed to sway them. According to a Miscellany News article about SLD and the rally, "Dean of College Christopher Roellke explained: 'We have been working diligently on these issues and will continue to work on them in earnest, in good faith and in alignment with our collective bargaining agreement'" ("Students, staff rally for better ACDC working conditions," The Miscellany News, 09.20.2017). While the language in that statement may sound supportive and promising, I sense a strong feeling of complacency in it. Nowhere does Roellke state that he has been moved or swayed by the protests in any way, nor does he make any mention of SLD's very reasonable demands. Roellke even went as far as to dismiss the act of protesting altogether saying, "My advice for students and workers is to continue to allow the dialogue to proceed as it should via the processes outlined in the collective bargaining agreement" (Miscellany News). It was clear from the outset that the administration's position on the SLD platform was simultaneously adversarial and complacent, and the protest does not seem to have changed that in any substantive way.&lt;br/&gt;Now, I should concede that I am about as much in the dark about precisely what has been going on with negotiations between dining staff and the administration as everybody else. The administration's comment, while somewhat off topic, was pretty edifying. I was informed that the administration's current position is that negotiations will only involve the administration, the workers and their representatives. Third-party involvement has not only been discouraged, but dismissed outright. There is no saying whether or not the ACDC workers will get their demands met in these closed-door meetings, but I find it unlikely.&lt;br/&gt;So what might change the administration's mind? To explore that question, we must consider how the administration is typically persuaded to change their stance on an issue. Why do administrations push back so hard against environmental and political divestment movements? Why does Vassar spend an exorbitant amount of money on frivolous alumnae/i amenities and events? Why do colleges across the country have such a difficult time bringing in student bodies from a diverse range of socioeconomic backgrounds?&lt;br/&gt;Simply put, it's because of money.&lt;br/&gt;Colleges tend to make their most unpopular decisions in order to secure their endowments and to keep the constant flow of alumnae/i money coming. After all, without an endowment, how can you fund a school? As the administration reiterates to donors, tuition alone doesn't come close to funding the school's operations. Of course, there are other factors that influence college administrators, but arguably none more so than money.&lt;br/&gt;Given this, the best strategy (and perhaps the only viable strategy) for SLD is to use their most valuable bargaining chip. Protests do not on their own sufficiently demonstrate that the cause will result in lost revenue for the school. The student organizers have to use their power to demonstrate to the school a threat to their funding by, for example, circulating a petition in which signers pledge to withhold donations to Vassar until SLD's demands are met.&lt;br/&gt;This would not only work from a strategic perspective, but would also bring a more principled approach to what has thus far been primarily a symbolic movement. Although the turnout for SLD's protest at the ACDC was surprising indeed, the methods have not been particularly effective-at least to date. Marching and chanting can be much more like checking the box and being contented with participation credit than creating actual change.&lt;br/&gt;Students at the ACDC protest clearly had the drive and enthusiasm necessary to effect change. The cause fits well into the narratives of long-overlooked and marginalized members of society that so strongly resonate with the Vassar community. There is much more that can be done to harness this energy, however. As was said at the protest, the fight is not over. Far from it, in fact.&lt;br/&gt;Without constant and persistent organizing, a protest movement might as well be dead. Only through the support of an impassioned movement can all the demands of SLD be guaranteed to workers on campus. That is exactly why SLD must take the steps outlined in this column.&lt;br/&gt;The way to have an effective protest is for the protesters to exercise power. They have the power; now it's simply a question of whether or not they will use it.</t>
         </is>
+      </c>
+      <c r="L117" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="118">
@@ -5606,10 +5964,13 @@
           <t>Immigration (For)</t>
         </is>
       </c>
-      <c r="J118" t="inlineStr">
+      <c r="K118" t="inlineStr">
         <is>
           <t>Can protest make a difference?&lt;br/&gt;On the last Tuesday of November, I found myself in Hinds Plaza looking for a spot to sit and enjoy the unusually warm weather. A large crowd was dispersing as I arrived, and I guessed there had been a rally. However, only when encountering a disturbing headline later on did I learn why this crowd had assembled: "ICE Arrests Came Hours Before Immigration Rally in Princeton." As it turned out, federal Immigration Customs Enforcement had swept up four people along Witherspoon not long before nearly 200 of their neighbors rallied around the block to call on Congress to pass a clean DREAM Act by Dec. 8. The aim of this legislaiton would be to protect the recipients of the now-terminated Deferred Action for Childhood Arrivals program.&lt;br/&gt;That Tuesday afternoon, as I was walking from Hinds Plaza to Dickinson Hall and the crowd of protesters was casually chatting and heading home, the lives of four Princeton community members were being completely overturned. It would be impossible to find out exactly where these individuals are now, but if unable to pay a bond they are most likely being detained while they await removal hearings. The article from the Princeton Patch did not make it clear whether the arrests inspired the rally.&lt;br/&gt;The everyday violence of immigrant detention and deportation might be hard to grasp in abstract terms, especially since this system takes in hundreds of thousands of individuals each year and has only grown since Trump's election. But the evidence of harmful, substandard conditions and frequent deaths in detention centers, where detainees are often cut off from access to family and legal representation, and the immediate danger that many deportees face, should compel us to grapple with the concrete, devastating human costs of detention and deportation.&lt;br/&gt;We cannot forget that human rights violations are occurring not only in distant war zones but right here in our own state. New Jersey ranks among the top five states with the largest number of people in immigrant detention. For example, a report on the Hudson County Jail in New Jersey, a county jail used by ICE to hold immigrant detainees, revealed a lack of outdoor space, nutritional food, and adequate access to family and legal representation.&lt;br/&gt;The arrests by ICE of our own neighbors are a clear reminder that our town is vulnerable to the everyday violence of our country's immigration system. Four of our neighbors were torn from their communities, homes, families, friends, jobs. Reflecting on the events of Nov. 28, it's difficult knowing how little distance and time separated the ICE arrests and the gathering of sign-waving protestors.&lt;br/&gt;I don't bring this up to shame those who participated in the Hines Plaza rally - I agree that the passage of the DREAM Act is incredibly urgent, and I wish that I had heard about the rally beforehand so that I could have attended myself. DACA was an incredibly important opportunity for 788,000 young immigrants, and its termination is a truly devastating blow for these individuals who have since feared that the information they provided to the government about their immigration status could now endanger them. As a community, we should lend our unequivocal support to efforts to preserve protections for DACA recipients - a struggle that is being led by one of our peers, María Perales '18, in a legal suit.&lt;br/&gt;However, let the ICE arrests serve as a reminder that if we are ever going to truly "show up" for all the undocumented members of our community, we must do more than speak up for the rights of DACA recipients. Unless the four individuals detained were DREAMers, the DREAM Act would have done nothing for them even if it had already been passed.&lt;br/&gt;We must, then, resoundingly assert that ICE, detention, and deportation should not exist whatsoever. We must welcome all immigrants, including students, childhood arrivals, older family members, people with criminal records, queer and trans immigrants. This position, which refuses to make distinctions between "good" or "bad" immigrants, should serve as the basis for networks of direct action. We should not only express support for the DREAM Act but also pressure our University to divest from the corporations that detain undocumented people of all different backgrounds in dehumanized conditions.&lt;br/&gt;Can we imagine a mode of collective action in which, rather than rallying several hours after a string of ICE arrests, community members were somehow immediately notified that federal immigration authorities were in town and began forming a crowd on the street as ICE agents were in the midst of knocking on doors and terrorizing families? What if, instead of simply carrying signs, protesters filmed and chanted down ICE agents until they left the community? It may sound unrealistic in the quiet and picturesque town of Princeton, but there have been plenty of cases of in which protesters have disrupted the work of ICE agents.&lt;br/&gt;Organizations like the DREAM Team have done much to build action networks, but there is only so much that small groups of activists can do alone. It's up to every community member to commit, unconditionally, to defending their undocumented neighbors and peers.&lt;br/&gt;Max Grear '18 is a senior columnist as well as a lead organizer of the Princeton Private Prison Divest Coalition.</t>
         </is>
+      </c>
+      <c r="L118" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -5649,10 +6010,13 @@
           <t>University governance, admin, policies, programs, curriculum, Sexual assault/violence</t>
         </is>
       </c>
-      <c r="J119" t="inlineStr">
+      <c r="K119" t="inlineStr">
         <is>
           <t>CW: sexual assault&lt;br/&gt;It's been less than 10 days since Organizing for Survivors, an activist group led by eight female and non-binary students, made their public debut on the steps of Parrish Hall on March 17. Everywhere from the bulletin boards in Parrish to the Sharples banner wall has become a hotbed of demonstration and discussion among students and faculty. Posters advocating for the resignations of Dean of Students Liz Braun, Dean Nathan Miller and Associate Director for Investigations Beth Pitts as well as the abolishment of frat housing, among other demands, have been put up and taken down within the same hour. The "Swat Protects Rapists" slogan and WordPress site have made a resurgence. Over 130 students of various gender identities attended a meeting following the rally on the night of March 18, where the O4S core team and other members planned further actions. Over 15 clubs and affiliation groups have released letters of support for the demands, including Resident Assistants, the Student Government Association and a group of student athletes.&lt;br/&gt;"We have been inspired and heartened by the abundance of support we've received from students and faculty alike and are excited to continue working with alongside all of those people," O4s wrote in an e-mail to the Phoenix.&lt;br/&gt;A week after the Parrish rally, President Valerie Smith addressed a letter to the college outlining policy changes and other responses to the O4S demands. To the demand that respondents (students who have had complaints filed against them) cannot serve as TAs or Residential Peer Leaders came in three parts: one, that due process requires that only students found responsible for a Title IX complaint will suffer consequences; two, that Provost Tom Stephenson will make the decision concerning TAs, as it is an academic position; and three, that "effective immediately," a student must be in good standing with the college in order for them to apply or serve as an RPL.&lt;br/&gt;O4S demanded that "Swarthmore must ensure that our right for Title IX to not proceedings exceed 60 days is protected." However, Under Betsy DeVos's federal guidelines, this is not a guaranteed right: "The department [of Education] says there is "no fixed time frame" under which a school must complete a Title IX investigation. The 2011 guidance stated that a "typical investigation" takes about 60 days after a complaint is made but said more complex cases could take longer," Inside Higher Ed reported.  President Smith wrote that the administration "will strive to complete" the adjudication process in 60 days.&lt;br/&gt;The preface to President Smith's letter, which President Smith, Dean Braun, Director of Public Safety Mike Hill, Dean Miller, Pitts, and Interim Title IX Coordinator Michelle D. Ray signed,  emphasized both recent changes and the need for improvement.&lt;br/&gt;"During the past five years the College has implemented a robust series of changes including adding staff, enhancing programming and training, and implementing new policies," President Smith wrote in the letter. "Despite this progress, more remains to be done, and we must continue to evaluate and reevaluate our practices based on our community members' experiences."&lt;br/&gt;As the preface mentions, this semester marks the fifth anniversary of "The Spring of Our Discontent," a period of intense, community-wide reckoning. By May 2013, two central activists, Hope Brinn '15 and Mia Ferguson '15, had spearheaded efforts to file two Federal complaints for violations of Title IX and the Clery Act, adding the college to a list of institutions of higher education that received negative, national attention for their handling of sexual assault cases. Other groups actively protesting during this period included those seeking divestment from fossil fuels, marginalized students who felt unsupported in STEM classes, and LGBTQ+ students who protested homophobia and the lack of queer mentors and faculty at the college.  The period resulted in an overhaul of the college's Title IX procedures and structure, from the establishment of the Title IX house and creation of the Title IX coordinator position to the firing of Tom Elverson. His position as advisor to the fraternities betrayed a conflict of interest in his position as a counselor for alcohol and drug use who also oversaw student misconduct, as the college's SHARE (Sexual Harassment/ Assault Resources and Education) website states. According to O4S, the group both takes inspiration and caution from this history.&lt;br/&gt;"We are very much informed by previous student activism of all types, including but not limited to the work that happened in the Spring of 2013," O4S core members wrote in an e-mail to the Phoenix. "We continue to look back at both the successes and missteps of previous organizing efforts in order to learn how we should move forward."&lt;br/&gt;This wave of renewed activism calls into question whether the college has resolved the issues that surfaced in 2013. Many members of the community, including alumni such as Jodie Goodman '16, who became progressively more involved in Title IX-related activism during her time at the college, believe that the college still does not do a satisfactory job of addressing sexual assault reports and complaints.&lt;br/&gt;"Fundamentally, the issue remains that Swarthmore still mistreats and silences survivors," Goodman said. "That is still at the heart of the activism."&lt;br/&gt;The changes that O4S demands are not only structural, but also involve the specific demand that Dean of Students Liz Braun, who has held her position since 2010, resign.&lt;br/&gt;"We demand the resignation of Dean of Students Liz Braun for her historic and ongoing unwillingness to meaningfully respond to student concerns about policy and practice, as well as her past inappropriate conduct as a participant in the adjudication of Title IX cases and other failures to protect students," O4S wrote in their demands.&lt;br/&gt;Students have criticized Dean Braun for similar issues in the past. In April 2016, the first year on which the college chose not to host a Clothesline Project event, the Daily Gazette reported that a red t-shirt was found taped to the sidewalk in front of Parrish that read, "Dean Braun is responsible for letting my rapist graduate. There is nothing else I can do but try to ignore it. Happy Sexual Assault 'Awareness' Month." The Phoenix reported in October 2013 of another incident in which a student found responsible for sexual assault and convicted by the Swarthmore police for attempted simple assault against a domestic partner would be permitted to return to the college  after a two-year suspension. According to the article, Dean Braun, who at that time handled Title IX appeals, denied the survivor's request for an appeal of the decision. It is unknown whether these incidents are the same, or related.&lt;br/&gt;"I think she has lost the trust of Swarthmore students," Goodman said. "She should apologize to the students she has hurt, and resign."&lt;br/&gt;Yet these issues coincide with concerns over high turnover of deans and college staff, such as the departure of the Intercultural Center Director, Dean Jason Rivera. President Smith chose to commission an external review of the Dean's Office, which occurs every 5 to 10 years, this year. In response to O4S's demands concerning the resignation of Dean Braun and Dean Miller, President Smith stated that she would publish the results of the external review report, but did not specify the date on which she would publish it. One finding from the external review of the college's compliance with Title IX and Clery Act regulations that then-President Rebecca Chopp commissioned in 2013: out of 11 people then mentioned as Title IX liaisons and resources, only six still work at the college.&lt;br/&gt;Adding to the intensity are concerns among students as well as within O4S about certain methods of activism. In the most recent turn of events, O4S addressed their use of posters with triggering content in a post on their WordPress site.&lt;br/&gt;"We knew that our slogans could be triggering-and that sometimes, the most triggering part of them is the fact that they are true," they wrote in the statement. "As we take responsibility and accountability, we also ask that you contextualize your critique in proportion to the structural mechanisms at play as we work through these contradictions: who is responsible for our shared frustration, and anxiety, at its core?"&lt;br/&gt;And then, around 6 p.m. on Tues., March 27, O4S announced that they would be temporarily ceasing activity and refocusing their message in a community forum that night.&lt;br/&gt;"We will be specifically addressing the harm caused by our organizing methods last week," the email said, which was distributed through Swarthmore Voices' email newsletter to students. "We believe that the best way to move forward is to focus on healing, on building trust within a network of people who have been harmed, and by centering the experiences of the most marginalized voices on campus, who are continuously ignored in the conversation on harm and violence universally. We got caught up in policy change and quick action and did not take the necessary time to reflect as a collective."&lt;br/&gt;O4S requested that press abstain from reporting on the happenings at the forum. However, they did apologize for their triggering postings multiple times, and dedicated most of the meeting to listening to community feedback. Though they have urged students outside of the group's core leadership to pause activity temporarily, they are hosting an informational meeting for faculty and instructional staff to learn about their campaign on Friday, March 30, according to biology professor Vince Formica.&lt;br/&gt;"Several faculty (myself included) passed on an invitation from O4S to the faculty and instructional staff to have an open gathering where they would answer questions about their demands and their experiences," Formica said.&lt;br/&gt;Two factors have likely driven O4S's decision to concentrate energy on the faculty as well as alumni. Firstly, faculty and instructional staff vote during monthly meetings on potential amendments and changes to the Faculty Procedures that the Committee on Faculty Procedures, the members of which are determined by vote, chooses.&lt;br/&gt;In addition, faculty and administration members have institutional memory that students' short term on campus prevents them from having. As every class present during the spring of 2013 has graduated by now, many current students do not know what happened that semester, or the divisive environment it created on campus.&lt;br/&gt;"Every week had some escalation, including the Intercultural Center being intentionally targeted by students who wanted to intimidate protesters. It's hard to argue that literally peeing on the doorstep of your ideological opponents is not heavily symbolic and gross," Goodman said. "Leaders of the movement to reform fraternities, like Hope Brinn and Mia Ferguson, were subjected to stalking, harassment, and violent threats on campus and online...Their testimony was alarming and upsetting to students on all sides of the issue," Goodman said. "Campus was divided in three: those passionately for reform, those passionately against reform, and those who thought the entire thing had gotten entirely out of hand and had opinions somewhere in the middle."&lt;br/&gt;Alumni, as well, have stock in this discussion. Alumni could choose to withhold donations unless the school addresses the concern, as alumni did in the late 80s to push the administration to divest from Apartheid South Africa.&lt;br/&gt;"All of the past Title IX advocates from Swarthmore that I've talked to are thrilled that the movement is growing and moving forward," Goodman said.&lt;br/&gt;According to O4S, they will release a public statement on their goals and mission as well as a statement on President Smith's response to their demands in the coming days. The Phoenix will cover the faculty information session and other developments.     &lt;br/&gt;How Clay Matthews Retro Alternate Jersey Boosted My Nfl Interest&lt;br/&gt;Although many MLB betting systems report that you do not need to understand baseball to bet. ... Learn more</t>
         </is>
+      </c>
+      <c r="L119" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -5692,10 +6056,13 @@
           <t>University governance, admin, policies, programs, curriculum, Sexual assault/violence</t>
         </is>
       </c>
-      <c r="J120" t="inlineStr">
+      <c r="K120" t="inlineStr">
         <is>
           <t>At 9:15 a.m. on Tuesday, May 1, over 30 students filed into Dean of Students Liz Braun's office on the first floor of Parrish Hall. As Braun rose from her seat, the students - members of Organizing for Survivors, a group that has protested Title IX handling at the college since early March - placed their backpacks on the floor beside them and announced their plans to stay there indefinitely.&lt;br/&gt;It is now over 50 hours later, and neither the students nor their belongings have moved. Dean Braun had picked up her bags and left silently after Shelby Dolch '21 delivered a statement on behalf of O4S, and by 5 p.m. on May 2, she had not returned to her office. No protesters have received citations.&lt;br/&gt;Dean Braun's office, its lobby and the hallway outside have been packed with students since. Provisions for the sit-in - coffee, Qdoba catering, Federal donuts, home-baked cakes, carrots - proliferate in the office space, most of which were either donated by professors or funded by sympathetic alumni through O4S's Venmo. Associate Dean of Diversity and Inclusion Shà Duncan Smith remained with students throughout the first day until around 2 a.m. and provided Chinese takeout for the group. By noon on the second day, over 175 students had participated in the sit-in and 17 students stayed overnight on the night of May 1.&lt;br/&gt;The group leading the sit-in, Organizing for Survivors, had not publicized the sit-in outside of private meetings and a Nonviolent Direct Action training meeting, hosted with help from Sunrise, a divestment advocacy group that staged a 32-day sit-in in Parrish last spring. For many, the sit-in is a response to growing dissatisfaction with the administration.&lt;br/&gt;"I feel like there's a narrative that it's not that bad or something, that this is the best administration can do, but I've really seen how jarring it is to be a survivor and feel like no one will support you and just have so many little things that happen that are institutional mistakes that shouldn't be there," Omene Addeh '21, who participated in the sit-in, said. "I think that the responses we've gotten from administration are just not satisfactory to me, and if this is what it takes, I'll do anything I can to help."&lt;br/&gt;At 9:55 p.m., as protesters prepared to spend the night, two Public Safety officers took down a banner from the Parrish hallway that read "Accountability looks like Beth Pitts resigning." Pitts is Associate Director of Investigations for Title IX cases. The officers cited a policy against "singling someone out" on banners and the policy that banners receive pre-approval five days before being hung, though the former policy is not listed in the student handbook and banners are not allowed in Parrish in the first place. They also removed two locked file cabinets from Braun's office around 11:00 p.m.&lt;br/&gt;"Per the Student Handbook, any language that is, 'harassing, demeaning or uncivil,' is grounds for removal. In this and other instances if the banner/poster or chalking specifically identifies a community member by name or position in a derogatory manner, it is considered 'harassment, demeaning, or uncivil,'" Public Safety Director Mike Hill wrote in an email to the Phoenix.&lt;br/&gt;Other administrators who have called O4S's methodology adversarial and uncivil include President Valerie Smith, who emailed students, faculty and staff of the college at 12:43 p.m. on May 1, alerting the community that the protesters' presence in Braun's office violated school policy because it prevented Braun and her staff from being able to work.&lt;br/&gt;"I will go to great lengths to protect our students' rights to peaceful protest and assembly," Smith wrote in an email to the Phoenix on May 2. "However, I can't support ad hominem attacks on individuals. We are capable of, and willing to allow for, disruptions of activities on campus, but no one should be prevented from doing their job, as our policies state plainly. At present, some of our students are in violation of those policies."&lt;br/&gt;Smith refers to Pitts, Braun and Dean Nathan Miller, from whom O4S has demanded resignations. At rallies during the sit-in, the group chanted songs such as "Hey hey, ho ho, ______ has got to go," for each of these administrators as well as for frat housing. But in contrast to Smith's assertion, O4S and supporters feels their demands are based on professional competence, not personality.&lt;br/&gt;For Dean Braun, O4S asks that she apologizes for her dismissal of student reports and concerns about sexual assault and mishandling of Title IX procedures. They believe that Dean Miller failed to correct violations of Title IX policies during Title IX adjudication processes, such as processes that lasted over 6 months. And they write that Beth Pitts asked victim-blaming questions and "belittled" complainants.&lt;br/&gt;"I am evaluating every allegation that has been brought against members of the staff," President Smith wrote to the Phoenix.&lt;br/&gt;O4S addressed those who disagree with their tactics at their Speak-Out rally on May 1. O4S core members Priya Dieterich '18 and Lydia Koku '18 feel that their movement is not unnecessarily combative towards administrators.&lt;br/&gt;"We think that we're being disruptive and that we're engaging in nonviolent direct action and we understand what comes with that," Dieterich said. "But sitting in is not adversarial, being public about our demands is not adversarial. We push back on the idea that just being loud and angry is necessarily adversarial. We have been committed to working collaboratively, we have not portrayed Val Smith as our adversary. If she's viewing us as adversaries, that's a decision on her part."&lt;br/&gt;"These are controversial demands and because of that people see them and our accompanying tactics as adversarial," Koku added.&lt;br/&gt;In addition to her update on the sit-in, President Smith's email included a copy of an email that Dean Braun had sent to O4S members after they met the week previous. O4S had not replied. In the email, Braun states that she will create a "student transition team" that will work with the new Title IX Coordinator and Violence Prevention Educator, that the ad hoc committee on wellbeing, belonging, and social life will release their report on the fraternity houses by July, and that she will oversee the creation of enhanced training during freshman orientation, among other updates.&lt;br/&gt;Yet according to O4S members, Braun's decision to create a student transition team does not solve the issues they've identified.&lt;br/&gt;"[The administration] has to decide that they're going to commit to shared governance with students," Dieterich said. "It's not just occasional committees or occasional invitations to the table, but permanently being at the table. And so I don't want the narrative to be that everything depends on who those people are, I don't think that that's true."&lt;br/&gt;O4S has consistently pushed back against administrative suggestions about committees and external reviews, asking instead for immediate action. At 8:45 a.m. on the second day of the sit-in, a handful of O4S members walked into a meeting of the same ad hoc committee to which Dean Braun referred in her email to ask questions directly to Deans Braun and Miller.&lt;br/&gt;"How many times will you make survivors retell their stories and retraumatize themselves to committee after committee year after year before it means enough for you to take action?" Anna Weber '19 said to the committee.&lt;br/&gt;The room was silent after O4S delivered their questions. "I think that's revealing," Dieterich said before leading the group out of the meeting.&lt;br/&gt;Afterwards, the protest intensified. At noon on May 2, over 150 students lined the Parrish hallway to hear a "special announcement" that O4S had publicized that morning on their Facebook page. They announced their decision to expand their sit-in to Dean Miller's office as a result of the events of that morning; they said they had planned to address Dean Miller, but could not, as he was out at lunch.&lt;br/&gt;Both The Philadelphia Inquirer and PhillyVoice published news stories online about O4S.NBC News Philadelphia continuously aired and posted two clips of video coverage of the sit-in. Students in the organization expressed anger after hearing that the college had removed NBC journalists from campus, as multiple students posted on the "Swarthmore Memes for Quaker Teens" page with memes about the "banning of free press" on campus.&lt;br/&gt;"This afternoon, after the news crew was done filming in Parrish, the officers met the reporters and advised them that they should leave, and the reporter complied," Hill confirmed."The media on hand were never interrupted during their reporting of the protest. Media access to campus is routinely requested, coordinated and approved through the College Communications office and neither of these visits followed that protocol. We are always happy to help accommodate media requests and do so fairly often."&lt;br/&gt;One of NBC's clips was titled "Swarthmore Students Stage Sit-In to Protest Sexual Violence." Yet what distinguishes O4S's protests from broader national movements such as #MeToo is its focus on the Swarthmore administration over cultural issues, according to Koku.&lt;br/&gt;"What I'd liked to do, or had hoped to do if we had had more time [and] more energy to do so, was connect with some of the other students, the other schools who are organizing specifically around the MeToo movement," she said. "We haven't explicitly discussed MeToo around our own organizing because it is so specific to Swarthmore and to transformative justice, but I think that the same challenges and impediments MeToo has experienced, we also have experiences as Organizing for Survivors."&lt;br/&gt;For Koku, leading O4S during her last semester at the college, despite the challenges she's faced - which included the fear that she would not receive her degree - changed how she viewed herself and administrators at the college.&lt;br/&gt;"This has made me find my voice in a more real and authentic way that I didn't have access to before," she said. "For me to say ... You were complicit in the harm that was caused to me and for that reason I need to fight not only for myself but for every single student who's gone through a similar experience and every single student that was subjected to those experiences and could be vulnerable to administrative harm."&lt;br/&gt;Because all of O4S's original core members except one are graduating seniors, the group made efforts to recruit underclassmen to take leadership for next year. Underclassmen such as Dolch held larger roles in the sit-in than they had previously. According to Dieterich, the timing of the sit-in, two weeks from the end of the year, worried her, but the turnout exceeded her expectations.&lt;br/&gt;"A lot of what we're doing and my willingness to do it publicly in this way is just that I want the concerns of people who are in my year not to be waited out and not to be buried," she said.&lt;br/&gt;"Seeing all of the people who came out today and especially the younger students who I haven't even met yet is incredibly heartening, and I have absolute faith that this is going to keep going next year and we'll all be watching and phoning it in and helping out as much as we can."&lt;br/&gt;As of the publication of this article, O4S has not announced an end date or condition for the sit-in.&lt;br/&gt;"I deeply regret any pain or burden students have borne unnecessarily due to our Title IX processes and procedures," President Smith wrote in her email to the Phoenix.&lt;br/&gt;Dieterich, too, regrets that students will continue to spend time on the movement.&lt;br/&gt;"I wish that the administration had listened all the times that these things had been raised in meetings so that students wouldn't have had to sacrifice so much of their energy, so much of their time, so much of their creativity and imagination and just all of their capacity and resources," she said. "That's on the administration."&lt;br/&gt;Sponsored: 20% off college storage!&lt;br/&gt;Learn more</t>
         </is>
+      </c>
+      <c r="L120" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="121">
@@ -5712,10 +6079,13 @@
           <t>The student group Organizing for Survivors held several protests at Swarthmore College over the handling of sexual assault issues on campus. Particularly the group is looking for procedural reform regarding sexual assault incidents.</t>
         </is>
       </c>
-      <c r="J121" t="inlineStr">
+      <c r="K121" t="inlineStr">
         <is>
           <t>CW: sexual assault&lt;br/&gt;It's been less than 10 days since Organizing for Survivors, an activist group led by eight female and non-binary students, made their public debut on the steps of Parrish Hall on March 17. Everywhere from the bulletin boards in Parrish to the Sharples banner wall has become a hotbed of demonstration and discussion among students and faculty. Posters advocating for the resignations of Dean of Students Liz Braun, Dean Nathan Miller and Associate Director for Investigations Beth Pitts as well as the abolishment of frat housing, among other demands, have been put up and taken down within the same hour. The "Swat Protects Rapists" slogan and WordPress site have made a resurgence. Over 130 students of various gender identities attended a meeting following the rally on the night of March 18, where the O4S core team and other members planned further actions. Over 15 clubs and affiliation groups have released letters of support for the demands, including Resident Assistants, the Student Government Association and a group of student athletes.&lt;br/&gt;"We have been inspired and heartened by the abundance of support we've received from students and faculty alike and are excited to continue working with alongside all of those people," O4s wrote in an e-mail to the Phoenix.&lt;br/&gt;A week after the Parrish rally, President Valerie Smith addressed a letter to the college outlining policy changes and other responses to the O4S demands. To the demand that respondents (students who have had complaints filed against them) cannot serve as TAs or Residential Peer Leaders came in three parts: one, that due process requires that only students found responsible for a Title IX complaint will suffer consequences; two, that Provost Tom Stephenson will make the decision concerning TAs, as it is an academic position; and three, that "effective immediately," a student must be in good standing with the college in order for them to apply or serve as an RPL.&lt;br/&gt;O4S demanded that "Swarthmore must ensure that our right for Title IX to not proceedings exceed 60 days is protected." However, Under Betsy DeVos's federal guidelines, this is not a guaranteed right: "The department [of Education] says there is "no fixed time frame" under which a school must complete a Title IX investigation. The 2011 guidance stated that a "typical investigation" takes about 60 days after a complaint is made but said more complex cases could take longer," Inside Higher Ed reported.  President Smith wrote that the administration "will strive to complete" the adjudication process in 60 days.&lt;br/&gt;The preface to President Smith's letter, which President Smith, Dean Braun, Director of Public Safety Mike Hill, Dean Miller, Pitts, and Interim Title IX Coordinator Michelle D. Ray signed,  emphasized both recent changes and the need for improvement.&lt;br/&gt;"During the past five years the College has implemented a robust series of changes including adding staff, enhancing programming and training, and implementing new policies," President Smith wrote in the letter. "Despite this progress, more remains to be done, and we must continue to evaluate and reevaluate our practices based on our community members' experiences."&lt;br/&gt;As the preface mentions, this semester marks the fifth anniversary of "The Spring of Our Discontent," a period of intense, community-wide reckoning. By May 2013, two central activists, Hope Brinn '15 and Mia Ferguson '15, had spearheaded efforts to file two Federal complaints for violations of Title IX and the Clery Act, adding the college to a list of institutions of higher education that received negative, national attention for their handling of sexual assault cases. Other groups actively protesting during this period included those seeking divestment from fossil fuels, marginalized students who felt unsupported in STEM classes, and LGBTQ+ students who protested homophobia and the lack of queer mentors and faculty at the college.  The period resulted in an overhaul of the college's Title IX procedures and structure, from the establishment of the Title IX house and creation of the Title IX coordinator position to the firing of Tom Elverson. His position as advisor to the fraternities betrayed a conflict of interest in his position as a counselor for alcohol and drug use who also oversaw student misconduct, as the college's SHARE (Sexual Harassment/ Assault Resources and Education) website states. According to O4S, the group both takes inspiration and caution from this history.&lt;br/&gt;"We are very much informed by previous student activism of all types, including but not limited to the work that happened in the Spring of 2013," O4S core members wrote in an e-mail to the Phoenix. "We continue to look back at both the successes and missteps of previous organizing efforts in order to learn how we should move forward."&lt;br/&gt;This wave of renewed activism calls into question whether the college has resolved the issues that surfaced in 2013. Many members of the community, including alumni such as Jodie Goodman '16, who became progressively more involved in Title IX-related activism during her time at the college, believe that the college still does not do a satisfactory job of addressing sexual assault reports and complaints.&lt;br/&gt;"Fundamentally, the issue remains that Swarthmore still mistreats and silences survivors," Goodman said. "That is still at the heart of the activism."&lt;br/&gt;The changes that O4S demands are not only structural, but also involve the specific demand that Dean of Students Liz Braun, who has held her position since 2010, resign.&lt;br/&gt;"We demand the resignation of Dean of Students Liz Braun for her historic and ongoing unwillingness to meaningfully respond to student concerns about policy and practice, as well as her past inappropriate conduct as a participant in the adjudication of Title IX cases and other failures to protect students," O4S wrote in their demands.&lt;br/&gt;Students have criticized Dean Braun for similar issues in the past. In April 2016, the first year on which the college chose not to host a Clothesline Project event, the Daily Gazette reported that a red t-shirt was found taped to the sidewalk in front of Parrish that read, "Dean Braun is responsible for letting my rapist graduate. There is nothing else I can do but try to ignore it. Happy Sexual Assault 'Awareness' Month." The Phoenix reported in October 2013 of another incident in which a student found responsible for sexual assault and convicted by the Swarthmore police for attempted simple assault against a domestic partner would be permitted to return to the college  after a two-year suspension. According to the article, Dean Braun, who at that time handled Title IX appeals, denied the survivor's request for an appeal of the decision. It is unknown whether these incidents are the same, or related.&lt;br/&gt;"I think she has lost the trust of Swarthmore students," Goodman said. "She should apologize to the students she has hurt, and resign."&lt;br/&gt;Yet these issues coincide with concerns over high turnover of deans and college staff, such as the departure of the Intercultural Center Director, Dean Jason Rivera. President Smith chose to commission an external review of the Dean's Office, which occurs every 5 to 10 years, this year. In response to O4S's demands concerning the resignation of Dean Braun and Dean Miller, President Smith stated that she would publish the results of the external review report, but did not specify the date on which she would publish it. One finding from the external review of the college's compliance with Title IX and Clery Act regulations that then-President Rebecca Chopp commissioned in 2013: out of 11 people then mentioned as Title IX liaisons and resources, only six still work at the college.&lt;br/&gt;Adding to the intensity are concerns among students as well as within O4S about certain methods of activism. In the most recent turn of events, O4S addressed their use of posters with triggering content in a post on their WordPress site.&lt;br/&gt;"We knew that our slogans could be triggering-and that sometimes, the most triggering part of them is the fact that they are true," they wrote in the statement. "As we take responsibility and accountability, we also ask that you contextualize your critique in proportion to the structural mechanisms at play as we work through these contradictions: who is responsible for our shared frustration, and anxiety, at its core?"&lt;br/&gt;And then, around 6 p.m. on Tues., March 27, O4S announced that they would be temporarily ceasing activity and refocusing their message in a community forum that night.&lt;br/&gt;"We will be specifically addressing the harm caused by our organizing methods last week," the email said, which was distributed through Swarthmore Voices' email newsletter to students. "We believe that the best way to move forward is to focus on healing, on building trust within a network of people who have been harmed, and by centering the experiences of the most marginalized voices on campus, who are continuously ignored in the conversation on harm and violence universally. We got caught up in policy change and quick action and did not take the necessary time to reflect as a collective."&lt;br/&gt;O4S requested that press abstain from reporting on the happenings at the forum. However, they did apologize for their triggering postings multiple times, and dedicated most of the meeting to listening to community feedback. Though they have urged students outside of the group's core leadership to pause activity temporarily, they are hosting an informational meeting for faculty and instructional staff to learn about their campaign on Friday, March 30, according to biology professor Vince Formica.&lt;br/&gt;"Several faculty (myself included) passed on an invitation from O4S to the faculty and instructional staff to have an open gathering where they would answer questions about their demands and their experiences," Formica said.&lt;br/&gt;Two factors have likely driven O4S's decision to concentrate energy on the faculty as well as alumni. Firstly, faculty and instructional staff vote during monthly meetings on potential amendments and changes to the Faculty Procedures that the Committee on Faculty Procedures, the members of which are determined by vote, chooses.&lt;br/&gt;In addition, faculty and administration members have institutional memory that students' short term on campus prevents them from having. As every class present during the spring of 2013 has graduated by now, many current students do not know what happened that semester, or the divisive environment it created on campus.&lt;br/&gt;"Every week had some escalation, including the Intercultural Center being intentionally targeted by students who wanted to intimidate protesters. It's hard to argue that literally peeing on the doorstep of your ideological opponents is not heavily symbolic and gross," Goodman said. "Leaders of the movement to reform fraternities, like Hope Brinn and Mia Ferguson, were subjected to stalking, harassment, and violent threats on campus and online...Their testimony was alarming and upsetting to students on all sides of the issue," Goodman said. "Campus was divided in three: those passionately for reform, those passionately against reform, and those who thought the entire thing had gotten entirely out of hand and had opinions somewhere in the middle."&lt;br/&gt;Alumni, as well, have stock in this discussion. Alumni could choose to withhold donations unless the school addresses the concern, as alumni did in the late 80s to push the administration to divest from Apartheid South Africa.&lt;br/&gt;"All of the past Title IX advocates from Swarthmore that I've talked to are thrilled that the movement is growing and moving forward," Goodman said.&lt;br/&gt;According to O4S, they will release a public statement on their goals and mission as well as a statement on President Smith's response to their demands in the coming days. The Phoenix will cover the faculty information session and other developments.     &lt;br/&gt;How Clay Matthews Retro Alternate Jersey Boosted My Nfl Interest&lt;br/&gt;Although many MLB betting systems report that you do not need to understand baseball to bet. ... Learn more</t>
         </is>
+      </c>
+      <c r="L121" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -5732,10 +6102,13 @@
           <t>The student group Organizing for Survivors held several protests at Swarthmore College over the handling of sexual assault issues on campus. Particularly the group is looking for procedural reform regarding sexual assault incidents.</t>
         </is>
       </c>
-      <c r="J122" t="inlineStr">
+      <c r="K122" t="inlineStr">
         <is>
           <t>At 9:15 a.m. on Tuesday, May 1, over 30 students filed into Dean of Students Liz Braun's office on the first floor of Parrish Hall. As Braun rose from her seat, the students - members of Organizing for Survivors, a group that has protested Title IX handling at the college since early March - placed their backpacks on the floor beside them and announced their plans to stay there indefinitely.&lt;br/&gt;It is now over 50 hours later, and neither the students nor their belongings have moved. Dean Braun had picked up her bags and left silently after Shelby Dolch '21 delivered a statement on behalf of O4S, and by 5 p.m. on May 2, she had not returned to her office. No protesters have received citations.&lt;br/&gt;Dean Braun's office, its lobby and the hallway outside have been packed with students since. Provisions for the sit-in - coffee, Qdoba catering, Federal donuts, home-baked cakes, carrots - proliferate in the office space, most of which were either donated by professors or funded by sympathetic alumni through O4S's Venmo. Associate Dean of Diversity and Inclusion Shà Duncan Smith remained with students throughout the first day until around 2 a.m. and provided Chinese takeout for the group. By noon on the second day, over 175 students had participated in the sit-in and 17 students stayed overnight on the night of May 1.&lt;br/&gt;The group leading the sit-in, Organizing for Survivors, had not publicized the sit-in outside of private meetings and a Nonviolent Direct Action training meeting, hosted with help from Sunrise, a divestment advocacy group that staged a 32-day sit-in in Parrish last spring. For many, the sit-in is a response to growing dissatisfaction with the administration.&lt;br/&gt;"I feel like there's a narrative that it's not that bad or something, that this is the best administration can do, but I've really seen how jarring it is to be a survivor and feel like no one will support you and just have so many little things that happen that are institutional mistakes that shouldn't be there," Omene Addeh '21, who participated in the sit-in, said. "I think that the responses we've gotten from administration are just not satisfactory to me, and if this is what it takes, I'll do anything I can to help."&lt;br/&gt;At 9:55 p.m., as protesters prepared to spend the night, two Public Safety officers took down a banner from the Parrish hallway that read "Accountability looks like Beth Pitts resigning." Pitts is Associate Director of Investigations for Title IX cases. The officers cited a policy against "singling someone out" on banners and the policy that banners receive pre-approval five days before being hung, though the former policy is not listed in the student handbook and banners are not allowed in Parrish in the first place. They also removed two locked file cabinets from Braun's office around 11:00 p.m.&lt;br/&gt;"Per the Student Handbook, any language that is, 'harassing, demeaning or uncivil,' is grounds for removal. In this and other instances if the banner/poster or chalking specifically identifies a community member by name or position in a derogatory manner, it is considered 'harassment, demeaning, or uncivil,'" Public Safety Director Mike Hill wrote in an email to the Phoenix.&lt;br/&gt;Other administrators who have called O4S's methodology adversarial and uncivil include President Valerie Smith, who emailed students, faculty and staff of the college at 12:43 p.m. on May 1, alerting the community that the protesters' presence in Braun's office violated school policy because it prevented Braun and her staff from being able to work.&lt;br/&gt;"I will go to great lengths to protect our students' rights to peaceful protest and assembly," Smith wrote in an email to the Phoenix on May 2. "However, I can't support ad hominem attacks on individuals. We are capable of, and willing to allow for, disruptions of activities on campus, but no one should be prevented from doing their job, as our policies state plainly. At present, some of our students are in violation of those policies."&lt;br/&gt;Smith refers to Pitts, Braun and Dean Nathan Miller, from whom O4S has demanded resignations. At rallies during the sit-in, the group chanted songs such as "Hey hey, ho ho, ______ has got to go," for each of these administrators as well as for frat housing. But in contrast to Smith's assertion, O4S and supporters feels their demands are based on professional competence, not personality.&lt;br/&gt;For Dean Braun, O4S asks that she apologizes for her dismissal of student reports and concerns about sexual assault and mishandling of Title IX procedures. They believe that Dean Miller failed to correct violations of Title IX policies during Title IX adjudication processes, such as processes that lasted over 6 months. And they write that Beth Pitts asked victim-blaming questions and "belittled" complainants.&lt;br/&gt;"I am evaluating every allegation that has been brought against members of the staff," President Smith wrote to the Phoenix.&lt;br/&gt;O4S addressed those who disagree with their tactics at their Speak-Out rally on May 1. O4S core members Priya Dieterich '18 and Lydia Koku '18 feel that their movement is not unnecessarily combative towards administrators.&lt;br/&gt;"We think that we're being disruptive and that we're engaging in nonviolent direct action and we understand what comes with that," Dieterich said. "But sitting in is not adversarial, being public about our demands is not adversarial. We push back on the idea that just being loud and angry is necessarily adversarial. We have been committed to working collaboratively, we have not portrayed Val Smith as our adversary. If she's viewing us as adversaries, that's a decision on her part."&lt;br/&gt;"These are controversial demands and because of that people see them and our accompanying tactics as adversarial," Koku added.&lt;br/&gt;In addition to her update on the sit-in, President Smith's email included a copy of an email that Dean Braun had sent to O4S members after they met the week previous. O4S had not replied. In the email, Braun states that she will create a "student transition team" that will work with the new Title IX Coordinator and Violence Prevention Educator, that the ad hoc committee on wellbeing, belonging, and social life will release their report on the fraternity houses by July, and that she will oversee the creation of enhanced training during freshman orientation, among other updates.&lt;br/&gt;Yet according to O4S members, Braun's decision to create a student transition team does not solve the issues they've identified.&lt;br/&gt;"[The administration] has to decide that they're going to commit to shared governance with students," Dieterich said. "It's not just occasional committees or occasional invitations to the table, but permanently being at the table. And so I don't want the narrative to be that everything depends on who those people are, I don't think that that's true."&lt;br/&gt;O4S has consistently pushed back against administrative suggestions about committees and external reviews, asking instead for immediate action. At 8:45 a.m. on the second day of the sit-in, a handful of O4S members walked into a meeting of the same ad hoc committee to which Dean Braun referred in her email to ask questions directly to Deans Braun and Miller.&lt;br/&gt;"How many times will you make survivors retell their stories and retraumatize themselves to committee after committee year after year before it means enough for you to take action?" Anna Weber '19 said to the committee.&lt;br/&gt;The room was silent after O4S delivered their questions. "I think that's revealing," Dieterich said before leading the group out of the meeting.&lt;br/&gt;Afterwards, the protest intensified. At noon on May 2, over 150 students lined the Parrish hallway to hear a "special announcement" that O4S had publicized that morning on their Facebook page. They announced their decision to expand their sit-in to Dean Miller's office as a result of the events of that morning; they said they had planned to address Dean Miller, but could not, as he was out at lunch.&lt;br/&gt;Both The Philadelphia Inquirer and PhillyVoice published news stories online about O4S.NBC News Philadelphia continuously aired and posted two clips of video coverage of the sit-in. Students in the organization expressed anger after hearing that the college had removed NBC journalists from campus, as multiple students posted on the "Swarthmore Memes for Quaker Teens" page with memes about the "banning of free press" on campus.&lt;br/&gt;"This afternoon, after the news crew was done filming in Parrish, the officers met the reporters and advised them that they should leave, and the reporter complied," Hill confirmed."The media on hand were never interrupted during their reporting of the protest. Media access to campus is routinely requested, coordinated and approved through the College Communications office and neither of these visits followed that protocol. We are always happy to help accommodate media requests and do so fairly often."&lt;br/&gt;One of NBC's clips was titled "Swarthmore Students Stage Sit-In to Protest Sexual Violence." Yet what distinguishes O4S's protests from broader national movements such as #MeToo is its focus on the Swarthmore administration over cultural issues, according to Koku.&lt;br/&gt;"What I'd liked to do, or had hoped to do if we had had more time [and] more energy to do so, was connect with some of the other students, the other schools who are organizing specifically around the MeToo movement," she said. "We haven't explicitly discussed MeToo around our own organizing because it is so specific to Swarthmore and to transformative justice, but I think that the same challenges and impediments MeToo has experienced, we also have experiences as Organizing for Survivors."&lt;br/&gt;For Koku, leading O4S during her last semester at the college, despite the challenges she's faced - which included the fear that she would not receive her degree - changed how she viewed herself and administrators at the college.&lt;br/&gt;"This has made me find my voice in a more real and authentic way that I didn't have access to before," she said. "For me to say ... You were complicit in the harm that was caused to me and for that reason I need to fight not only for myself but for every single student who's gone through a similar experience and every single student that was subjected to those experiences and could be vulnerable to administrative harm."&lt;br/&gt;Because all of O4S's original core members except one are graduating seniors, the group made efforts to recruit underclassmen to take leadership for next year. Underclassmen such as Dolch held larger roles in the sit-in than they had previously. According to Dieterich, the timing of the sit-in, two weeks from the end of the year, worried her, but the turnout exceeded her expectations.&lt;br/&gt;"A lot of what we're doing and my willingness to do it publicly in this way is just that I want the concerns of people who are in my year not to be waited out and not to be buried," she said.&lt;br/&gt;"Seeing all of the people who came out today and especially the younger students who I haven't even met yet is incredibly heartening, and I have absolute faith that this is going to keep going next year and we'll all be watching and phoning it in and helping out as much as we can."&lt;br/&gt;As of the publication of this article, O4S has not announced an end date or condition for the sit-in.&lt;br/&gt;"I deeply regret any pain or burden students have borne unnecessarily due to our Title IX processes and procedures," President Smith wrote in her email to the Phoenix.&lt;br/&gt;Dieterich, too, regrets that students will continue to spend time on the movement.&lt;br/&gt;"I wish that the administration had listened all the times that these things had been raised in meetings so that students wouldn't have had to sacrifice so much of their energy, so much of their time, so much of their creativity and imagination and just all of their capacity and resources," she said. "That's on the administration."&lt;br/&gt;Sponsored: 20% off college storage!&lt;br/&gt;Learn more</t>
         </is>
+      </c>
+      <c r="L122" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -5776,10 +6149,13 @@
           <t>Economy/inequality, Labor and work, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J123" t="inlineStr">
+      <c r="K123" t="inlineStr">
         <is>
           <t>Nathan A. Cummings Like many Harvard faculty members, History and Literature lecturer Timothy P. McCarthy '93 lines the walls of his office with towering stacks of books. But propped up against the window of his closet-sized Quincy House office is something more unusual: a sign touting UNITE HERE Local 26, the union that represents Harvard's dining hall workers.&lt;br/&gt;When the workers engaged in a three week-long strike in October, McCarthy was holding that sign on the picket lines. He's been agitating for social justice causes since he first arrived at Harvard as an undergraduate in 1989.&lt;br/&gt;As both a citizen and a scholar-he co-teaches "Culture and Belief 49: American Protest Literature from Tom Paine to Tupac"-activism has been a part of McCarthy's "whole adult life," he said. But McCarthy said this puts him in the minority among his colleagues.&lt;br/&gt;"I always laugh whenever there's kind of a caricature of Harvard as a kind of hotbed of faculty radicalism, you know the Kremlin on the Charles, and Harvard is filled with all of these radical insurgent revolutionary thinkers who don't respect authority and the status quo and institutions and so on," he said.&lt;br/&gt;McCarthy laughed. "That has not been my experience."&lt;br/&gt;While Harvard faculty may not be the radical cohort some imagine, McCarthy and other professors say they have noticed growing activist engagement among the faculty. Recently, faculty members have been involved in advocating for undocumented students and other marginalized groups following the election of President Donald Trump.&lt;br/&gt;"I have definitely noticed recently in the last year or so a growing chorus of critique and activism among a broader range of faculty members, which I welcome with open arms," McCarthy said.&lt;br/&gt;While many of Harvard's professors still prefer the lectern over the loudspeaker, in the age of Trump, a growing number of faculty members are signing petitions and joining protests.&lt;br/&gt;'The Usual Suspects'&lt;br/&gt;For John Stauffer, an English and African and African-American Studies professor who teaches "Culture and Belief 49" with McCarthy, activism is more of an intellectual pursuit.&lt;br/&gt;"I'm not on the front lines in a walk," he said. "I'm more interested in analyzing and understanding what leads to a position." Stauffer said he believes that many of his colleagues feel the same way.&lt;br/&gt;McCarthy said a small cohort of professors are regularly inclined to protest, though. He calls them "the usual suspects."&lt;br/&gt;For that small group, protests are a way to push for change at an institution that tends to tread cautiously on political issues.&lt;br/&gt;One of the "usual suspects" is Kennedy School lecturer Richard Parker, who has advocated for Harvard's divestment from fossil fuels and against the manufacture of Harvard-brand goods by sweatshops. Parker said he believes activism has influenced Harvard's history in a positive way.&lt;br/&gt;"Go look at the way in which modern Harvard was created, which was out of the so-called Unitarian revolt of the beginning of the 19th century or look at the protests that swept through Harvard in the 1930s over public policy issues or in the 1960s, the 1970s and they've all had an impact on the University," he said.&lt;br/&gt;History and Literature lecturer Timothy P. McCarthy '93 walked out of class during the dining workers' strike in the fall. Jason K. Thong Parker said he is not worried about consequences for speaking out against the administration's policies. McCarthy echoed this, although with a caveat.&lt;br/&gt;"I've never felt that an explicit encouragement to remain silent from anyone here at Harvard and no one's ever written to me and said to me and said you can't say this," he said. "I would say that there are certain people here who are probably not happy with the fact that I sometimes will be vocal about things in the world including certain policies that Harvard has implemented or certain positions that Harvard has taken or not taken."&lt;br/&gt;McCarthy said he had once had a dean question whether the outspoken professor must speak at "every rally."&lt;br/&gt;"I said I wouldn't have to if more people would," he said.&lt;br/&gt;Indeed, a small minority of faculty have often been the most involved in activism, and unsurprisingly-according to Organismic and Evolutionary Biology Department chair Elena M. Kramer- most come from the Social Sciences and Arts and Humanities divisions.&lt;br/&gt;It is frequently non-STEM professors who take to the microphone at Faculty meetings to critique administrative policies, draft petitions, or discuss heated political issues in the classroom. Kramer attributed the varying levels of activism to "different cultures in those departments" and geographic distance from undergraduates.&lt;br/&gt;"Those departments are more integrated into the Yard and the College," Kramer said in an interview from her office in the Biology Labs, one of the northernmost sectors of campus. "Because of that, they have a closer connection and investment in the undergraduate College."&lt;br/&gt;Dean of FAS Michael D. Smith, a current professor in SEAS, agreed that the topics discussed in STEM field usually aren't accompanied with fierce political debate.&lt;br/&gt;"I've learned a lot from listening to my students over time," Smith said. "Engineering is not all that political sometimes, but it can be."&lt;br/&gt;'A Different World'&lt;br/&gt;While political activism among Harvard's faculty has historically been muted, movements and events including the dining workers' strike, the January Women's March, and Trump's executive order on immigration have lit a fire in many faculty who have previously remained silent.&lt;br/&gt;"More people are engaged, more people are involved," Parker said. "It is not the case that 50 percent of the faculty or something are willing to march, I don't think even 20 percent might march, but for sure more active than the past."&lt;br/&gt;Activism among faculty members takes different forms. Petitions and letters remain efficient and common methods of protest for faculty members on a variety of topics from campus issues like the protection of undocumented students and the dining workers strike to Trump's executive order.&lt;br/&gt;"I've signed many petitions in the past months. I've been a huge petition-signer. I'm a huge fan of petitions and it's also just logistically easy," Stauffer said.&lt;br/&gt;Sometimes, though, faculty members engage in more overt methods of activism on and off campus. Suzanne P. Blier, an Art and Architecture and African and African American studies professor, can be found alongside Cambridge residents at weekly City Council meetings, fighting to preserve historical structures like the Out of Town News Kiosk and Abbot Building, which houses the world's Only Curious George Store.&lt;br/&gt;"I came to this in part through last year's primary. I had not been that active politically before then," Blier said of her political efforts. "I, like many others, came to realize that all politics is local."&lt;br/&gt;Following Trump's executive order on immigration, Economics department chair David I. Laibson '88 encouraged his students to attend a Copley Square protest if they felt strongly about the issue.&lt;br/&gt;Brandishing signs and flags, crowds rally in Boston's Copley Square in January after President Donald Trump's immigration order.</t>
         </is>
+      </c>
+      <c r="L123" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="124">
@@ -5819,10 +6195,13 @@
           <t>Tuition, fees, financial aid</t>
         </is>
       </c>
-      <c r="J124" t="inlineStr">
+      <c r="K124" t="inlineStr">
         <is>
           <t>"Hey hey, ho ho, student debt has got to go!" chanted University of California students at the UC Board of Regents meeting. While the midterm season is in full swing, students from across the ten campuses traveled to the University of California, San Francisco to protest the proposed tuition increase.&lt;br/&gt;According to a report from the Los Angeles Times, the increase, which would take effect in 2018-2019, would raise in-state tuition by 2.7%, or $342. Students who live outside of California were in for a worse fate as their nonresident tuition would increase by $978.&lt;br/&gt;Frustration over the continued rising costs of the university, students mobilized by protesting, calling their state representatives, and expressing their frustrations on social media. Elected representatives spoke out against the hike, including Governor Jerry Brown, Lieutenant Governor Gavin Newsom, and Speaker of the California State Assembly Anthony Rendon.&lt;br/&gt;As UC regents prepare to vote on a tuition hike, this just arrived from @JerryBrownGov pic.twitter.com/AqKc4DUDeF&lt;br/&gt;- Emily DeRuy (@Emily_DeRuy) January 24, 2018&lt;br/&gt;On Wednesday, January 24, much to the celebration of students across the state, it was announced by the UC Board of Regents that the vote would be postponed until the May meeting. Until then, the UC Board of Regents committed to lobbying the state legislature for additional funding, as the current state budget allocated $34 million less than what university administration expected to meet their financial needs.&lt;br/&gt;It's official. The UC Board of Regents will postpone it's vote on a tuition increase until May. This is unprecedented and was only possible because of student power.&lt;br/&gt;- Paul Monge (@paulmonge_SF) January 25, 2018&lt;br/&gt;While tuition in California was once free, the rising costs of tuition (paired with the ever-increasing costs of living) have students shaking their head.&lt;br/&gt;Last January, the UC Board of Regents voted to increase tuition by 2.5%, raising costs for the first time in six years. Four months later, a state audit revealed that the university hid $175 million in a rainy-day fund, while continually demanding more funding from the university. Further controversy erupted when it was discovered that Janet Napolitano, the president of the University of California, spent more than $4,000 on an employee's retirement party, $13,000 for a dinner party to honor two departing members of the Board and $862,000 spent on the president's apartment in Oakland.&lt;br/&gt;The state isn't blameless, either. While California is celebrated as a progressive state, the legislature continues to divest from higher education, providing less funding to meet the exponential need of college graduates within the state. From 2012-2013, tuition was a part of the core funding for the university, with $2.98 billion contributed solely from students. As state legislatures and university officials clash, often, it's at the expense of underresourced and over-paying students, causing spikes in tuition as substitutes for critical conversations and political negotiations.&lt;br/&gt;"The university and the state legislators can work together by putting aside their differences and work toward the goal of looking at the data together and coming up with a solution collaboratively," said Jonathan Abboud, graduate student at the University of California, Santa Barbara and one of the lead organizers behind The $48 Fix, an organization working to reclaim California's Master Plan for Higher Education.&lt;br/&gt;While students celebrate their well-deserved victory in postponing the vote, only time will tell what the final administrative decision will be. Only one thing is certain: that the voices of students will continue to be amplified, and unflinchingly demand a seat at the table for the decisionmaking processes toward the future of their university. And that, regardless of the vote, is something to celebrate.&lt;br/&gt;"I'm most excited for students to regain their agency," said Paul Monge, the UC Student Regent. "We are, in fact, partners of the university and of the state."&lt;br/&gt;The next UC Board of Regents meeting will be on March 15-16 at the University of California, San Francisco.</t>
         </is>
+      </c>
+      <c r="L124" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -5867,10 +6246,13 @@
           <t>Police violence</t>
         </is>
       </c>
-      <c r="J125" t="inlineStr">
+      <c r="K125" t="inlineStr">
         <is>
           <t>A group of students marched throughout Oakland Friday afternoon waving flags and signs with slogans such as "Disarm the police, arm your desire" and chanting "A.C.A.B., all cops are bastards."&lt;br/&gt;Their words elicited varying reactions from observers.&lt;br/&gt;"Go home commies!" someone yelled from a window in Holland Hall.&lt;br/&gt;"They're making fools of themselves," a man outside of Noodles and Company said.&lt;br/&gt;Another man standing outside of Uncle Sam's Sandwich Bar cheered them on and sang along with their chant.&lt;br/&gt;"I could get in on this!" he shouted.&lt;br/&gt;The march - which began on Fifth Avenue, went through Schenley Quad onto Forbes and ended on Oakland Avenue - was the aftermath of a rally staged Friday afternoon by about 40 students and community members.&lt;br/&gt;The rally marked the end of an "occupation" of the Cathedral of Learning which began Tuesday. The "occupation" began with a small group of students who went to Chancellor Patrick Gallagher's office early Tuesday morning with a letter of 15 demands, including disarming the Pitt police, divesting from fossil fuels and implementing a University-wide $15 minimum wage.&lt;br/&gt;According to a rally organizer, who didn't want to be named, the four-day occupation and Friday rally were held to coincide with the first anniversary of a protest last November against student debt and President Donald Trump. Pitt police arrested two people during the protest last year after an altercation took place in Towers lobby.&lt;br/&gt;"We wanted to show [the University and Pitt police that] we are still here, still taking action," the organizer said.&lt;br/&gt;Students and community members marched in protest of police brutality Friday afternoon. (Photo by Christian Snyder | Contributing Editor)&lt;br/&gt;Associate Dean of Students Linda Williams Moore and Dean of Students Kenyon Bonner were present to observe the rally. About 10 to 15 Pitt police officers stood inside Towers lobby while four to five stood outside the entrance of Towers. Several police cars were parked across on Thackeray Avenue. Unlike last year, there were no violent confrontations between rally attendees and the police.&lt;br/&gt;Prior to the rally, Bonner approached the protesters with some "ground rules" for the event, including that they could not go into Towers lobby and that they would face repercussions if the rally turned into anything confrontational.&lt;br/&gt;"I just told them policies and protocol. This is a reservable space, they need to reserve the space for a protest here," he said of Towers lobby. "There's plenty of places off-campus where they can protest, just not this place."&lt;br/&gt;Students and community members - several clad in "Black Lives Matter" shirts or with their mouths covered by bandanas - joined hands and formed a circle in front of Tower B around 4 p.m.&lt;br/&gt;Several individuals spoke at the rally - including a Pitt alum who recounted their experience at last year's protest and another student who read an account said to be from one of the individuals arrested at the protest last November. The first speaker reminded attendees that the demonstration was being held to protest against the Pitt police.&lt;br/&gt;Each rally attendee asked refused to provide names to The Pitt News.&lt;br/&gt;The Pitt alum, who was present at last year's protest and witnessed and filmed the incident between students and police, said the police's action were "brutal and unjust" and blamed the University for allowing it to happen.&lt;br/&gt;"I love this University, I grew so much here," they said. "But in my experience they only care about what you have to say if it aligns with their goals of power, prestige and profit."&lt;br/&gt;Another rally attendee spoke about deaths of people of color by the hands of police, citing individuals such as 14-year-old Jason Pero, an eighth grader who died on the Bad River Band of Lake Superior Chippewa's reservation less than two weeks ago after police shot Pero.&lt;br/&gt;"All these cops are stealing life every day, it's their job to do that," they said.&lt;br/&gt;A student who wished to remain anonymous said he wasn't involved with the group that organized the rally but joined it halfway through because he wanted to show support for their views. He was unsure if some of the messages of the group were well conveyed, though.&lt;br/&gt;"The chanting was good, but I don't know if it was productive," he said of the "group of white people" chanting anti-police slogans.&lt;br/&gt;The student said plenty of cops do have their priorities in the wrong place, but there are many who just "want to make a living."&lt;br/&gt;"I don't think the right response is to dehumanize the administration," he said.&lt;br/&gt;The students and community members ended their march on Oakland Avenue around 5 p.m. Several broke off to go elsewhere. Others hung around and engaged in a discussion with Cameron Hallihan, a sophomore neuroscience major and member of the Pitt College Republicans who came to the rally to ask its attendees about their political views and goals.&lt;br/&gt;"I think they're misguided and I disagree, but I don't disagree with their right to free speech," Hallihan said.&lt;br/&gt;Another rally attendee said they thought the rally served its purpose in showing continued opposition to the Pitt police's actions last year and their involvement in "defending capitalism."&lt;br/&gt;"More needs to be done, but it says something that there were less than 50 of us and like 20 cop cars were around that place. It shows the University's scared of us," they said. "It went well, but it's not over."</t>
         </is>
+      </c>
+      <c r="L125" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -5910,10 +6292,13 @@
           <t>Labor and work, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J126" t="inlineStr">
+      <c r="K126" t="inlineStr">
         <is>
           <t>Alec Vandenberg | Daily Trojan&lt;br/&gt;Last week, Aramark-subcontracted janitors at USC and their supporters marched from Trousdale Parkway to USC Village, imploring students to join their campus rally to advocate for higher wages, better benefits and more affordable health care. But even as they walked through the middle of campus past hundreds of students, they were generally met with indifference.&lt;br/&gt;I've dedicated a decent chunk of my column to waxing lyrical about the subpar state of engagement on campus. But these past few months have presented my peers and me with new opportunities for activism, and raised more questions and concerns about our inaction.&lt;br/&gt;Millennials may be painted as the most self-centered generation, but college itself revolves around the student. The pressures of academic course loads, extracurriculars, career development, job hunting and often the struggle to afford tuition, books and basic needs leave little time and energy for social and political activism.&lt;br/&gt;And yet, too rarely do we consider the obligations that we students owe to one another, and to our communities both on and off campus. Circling back to the custodial protest, ought we join USC workers, those who form the bedrock of our campus community and Trojan Family, in their struggle for basic rights and dignity? But more broadly, how should students engage with issues that ought to be solved by our administration, but often stem from our existence on this campus and fall on our shoulders?&lt;br/&gt;The continuing conversation surrounding gentrification represents an extension of this same conversation. USC housing pushed out local retailers and raised concerns about higher rent, and students living in housing around the campus raise the cost of living for community members sharing the surrounding, increasingly pricy housing developments.&lt;br/&gt;Grace Cillo | Daily Trojan&lt;br/&gt;Zumper, a housing rental website, revealed in 2015 average rent increased by over 15 percent in the area surrounding USC, and Rentcafe lists 90007, USC's regional zip code, as the second-most expensive zip code for rentals in Los Angeles County for 2015. Just last semester, property owners evicted more than 70 community members in an apartment complex off of Exposition Boulevard to open up their housing stock to wealthier student tenants.&lt;br/&gt;It's no surprise then when these community members and campus workers - whose lives are inextricably tied to and impacted by campus life - appeal to students when stymied by the administration. They reach out to students through flyering on Trousdale and reaching out to groups and clubs. Or, especially in the case of local evictions unrelated to USC policy, community members encourage students to join local causes to advocate for policy changes.&lt;br/&gt;We students can't change the unintended effects of our presence, but we can and must change our apathy and translate it into dialogue and action - otherwise we risk complicity by mere association of attending USC.&lt;br/&gt;The service worker rally provided students informational materials and easy ways of contacting the administration to advocate on their behalf. And local housing rights groups and neighborhood associations always look for student support in their conversations and workshops on tenant rights.&lt;br/&gt;But the dialogue and engagement extends further to issues beyond workers' rights and rent, as students can investigate our endowment to ensure that USC divests from any sin stocks, such as tobacco or arms companies, and we can encourage the transition to campus clean energy to reduce our carbon footprint. All of these examples illustrate how the financial decisions of our University send shockwaves, for better or worse, past the boundaries of our campus and the local community - and there are many ways for students to have impact.&lt;br/&gt;As students, we often feel overwhelmed by the pressures and gravity of inequality and other pressing issues, but also feel disempowered to be the change in addressing special interests, donor clout or other barriers.&lt;br/&gt;But external factors and internal hesitations cannot justify our inaction. Students taking action to rename the Von KleinSmid Center, a building named after a former USC president heavily involved with the eugenics movement; advocacy groups demanding safer working conditions for campus workers; and environmental groups pushing USC to adhere to their sustainability plans, show the commitment and power of our student body.&lt;br/&gt;Let's join these activists, our community and all members of the Trojan Family in this overarching push for greater progress and accountability. Because just as our collective action impacts lives, so, too, does our inaction.&lt;br/&gt;Alec Vandenberg is a sophomore majoring in public policy. His column,"It Takes a Village," runs every other Monday.</t>
         </is>
+      </c>
+      <c r="L126" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="127">
@@ -5953,10 +6338,13 @@
           <t>Pro-Palestine/BDS</t>
         </is>
       </c>
-      <c r="J127" t="inlineStr">
+      <c r="K127" t="inlineStr">
         <is>
           <t>Students Against Israeli Apartheid rally in Vari Hall March 27th. York slammed the door on the SAIA after numerous warmings. Photo courtesy of SAIA Facebook page.&lt;br/&gt;York alumnus and SAIA activist Hammam Farah has been banned from York property. After receiving warning letters, the Students Against Israeli Apartheid had their club status revoked for “repeated disruption of academic activities.”&lt;br/&gt;Students Against Israeli Apartheid’s status as an officially recognized student group at York was revoked by the university following a rally held in Vari Hall on March 27.&lt;br/&gt;Janet Morrison, vice-provost students, who makes decisions with respect to club statuses, de-listed SAIA as an official club until January 2014 for “repeated disruption of academic activities,” according to Joanne Rider of York media.&lt;br/&gt;“Specifically, SAIA will not be able to book space or otherwise access university resources directly or through another student organization,” says the notification letter from Morrison. SAIA is also “debarred from re-registering for official student group status” until January 1, 2014.&lt;br/&gt;Rider says this isn’t the first time that SAIA has “disrupted academic activities” during one of their rallies and that this action wasn’t taken lightly. The university follows a similar process with any student club, association, or organization when university policies are violated, she explains.&lt;br/&gt;“We followed due process including warning SAIA a number of times before we made the decision to sanction them,” says Rider.&lt;br/&gt;SAIA was notified on May 3 by York that their club status had been revoked via email and letter delivered by Morrison.&lt;br/&gt;Along with SAIA, a number of other groups were present at the rally, including the York University Black Students’ Association, York’s chapter of the Filipino Canadian Youth Alliance, the Middle Eastern Students’ Association, Ontario Public Interest Research Group-York, Independent Jewish Voices – Toronto, Fightback, and CUPE 3903.&lt;br/&gt;“An unprecedented attack on academic freedom and freedom of speech on the York University campus.” &lt;br/&gt;A few members of student groups involved in the rally received warning letters from the university.&lt;br/&gt;Excalibur obtained a copy of the letter sent from the university to Arshiya Lakhani, one of the students who spoke at the March 27 rally.&lt;br/&gt;“By this letter, the University is giving you notice that should you in future fail to comply with applicable regulations of the University […] York University may invoke disciplinary action against you in accordance with applicable University rules,” the letter said.&lt;br/&gt;Letters were also sent to the presidents of YUBSA and the Middle Eastern Students’ Association, among other students.&lt;br/&gt;“The warning letters sent from the university definitely felt threatening,” says SAIA member Huda Al-Sarraj.&lt;br/&gt;YUBSA and Rider were contacted concerning warning letters but were unable to be reached in time.&lt;br/&gt;“Receiving the letters and threatening us is problematic because all these clubs involved are fighting for fundamental rights, like YUBSA who fight against racial profiling and for black rights,” says Al-Sarraj.&lt;br/&gt;The rally in question took place one week after the York Federation of Students endorsed the Israel Boycott, Divestment, and Sanctions campaign at a board of directors’ meeting, joining York’s Graduate Students’ Association in their support of the movement.&lt;br/&gt;In a post on SAIA’s Facebook page, the group writes that the university’s decision to revoke their status is an “unprecedented attack on academic freedom and freedom of speech on the York University campus.”&lt;br/&gt;When asked for a response, Rider says, “York University encourages freedom of expression and debate of controversial issues, and values diverse perspectives.  The university does not permit such expression to compromise or disrupt classes or other academic activities.”&lt;br/&gt;“With the March 27 rally, we wanted to show that York didn’t have an ethical investment strategy and that we needed to push for that,” says Al-Sarraj. “We cooperated with York security, and we also had a security liaison and marshal keep things under control.”&lt;br/&gt;Following the same rally, York alumnus and SAIA activist Hammam Farah was banned from entering York property as of April 25.&lt;br/&gt;According to a letter sent to Farah by Gary Brewer, vp finance and administration, Farah was banned from campus because of his participation in two demonstrations — the first on November 29, 2012, and the other on on March 27, 2013,  — where he was observed by York security using an amplification device to speak to a gathering of students and others.&lt;br/&gt;Rider says Farah was banned for violating university policy.&lt;br/&gt;“Acting in violation of any York University policy or procedure may result in a review process,” says Rider. “Actions by the university as a result of the review may include banning an individual or group from campus.”&lt;br/&gt;This is the first incident since 2009 that a club has been sanctioned by the university.&lt;br/&gt;In 2009, SAIA and the Hasbara Fellowship were each suspended for 30 days and fined $1,000, the Tamil Students’ Association was suspended for 15 days and fined&lt;br/&gt;$500, and Hillel was fined $500 for “for their part in recent activities which disrupted classes adjacent to Vari Hall rotunda,” according to a York Media Relations press release.</t>
         </is>
+      </c>
+      <c r="L127" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="128">
@@ -5996,10 +6384,13 @@
           <t>Pro-Palestine/BDS</t>
         </is>
       </c>
-      <c r="J128" t="inlineStr">
+      <c r="K128" t="inlineStr">
         <is>
           <t>As a U of C student, it is likely that you have strong feelings about issues, and that you'll be interested in voicing those feelings in some kind of public gathering, or Q&amp;A with a famous speaker, or Facebook group. Over the years there have been a lot of controversies generated by students like you, ranging from divesting the University from Darfur (students lost, the investments remained), kicking Coca-Cola off campus and keeping Coca-Cola on campus (it's still here, so tie?), getting a pass for free trips on the CTA (too expensive, the students lost), and even against aMaroon writer whose opinion piece was deemed incendiary (students won! TheMaroon retracted the article).&lt;br/&gt;Two incidents really drove campus crazy last year, and both took place on 57th Street. The Harris School of Public Policy invited former Israeli Prime Minister Ehud Olmert to give a speech at Mandel Hall last October, a move that did not sit well with the University's Palestine advocates (and some activists from off-campus, too). Many protested outside the event, and others registered to attend. Once inside, they yelled so loudly and continuously that it took almost an hour and a half for Olmert to complete a planned 20-minute speech.</t>
         </is>
+      </c>
+      <c r="L128" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="129">
@@ -6039,10 +6430,13 @@
           <t>University governance, admin, policies, programs, curriculum, Anti-racism, Campus climate</t>
         </is>
       </c>
-      <c r="J129" t="inlineStr">
+      <c r="K129" t="inlineStr">
         <is>
           <t>More than 70 people rallied and marched for racial justice on Friday, demonstrating in front of Levi Hall before marching to Hutchinson Courtyard.&lt;br/&gt;The demonstration concluded a week of activism events regarding race at UChicago that was organized by a coalition of campus groups.&lt;br/&gt;Representatives of these groups, including Graduate Students United and UChicago Student Action , spoke on topics related to racial justice, as well as the recent campus unionization campaigns and a perceived crackdown on activism at the University.&lt;br/&gt;The nine organizing groups were GSU, UCSA, Students Working Against Prisons , UChicago for a Community Benefits Agreement (UC for a CBA), UChicago United, the UChicago chapter of the American Association of University Professors , Faculty Forward UChicago, Reparations at UChicago, and International Socialist Organization .&lt;br/&gt;The ralliers held signs with messages including "Reparations at UChicago" and chanted slogans including "Zimmer, Zimmer, you can't hide, we can see your corporate side" and "urban renewal is urban removal." The chants alluded to the University's involvement with the Obama Presidential Center and other South Side development projects, which critics fear will displace current residents.&lt;br/&gt;The center will be built on a 21-acre site in Jackson Park. One speaker, fourth-year Cindy Du with UC for a CBA, noted that the project will coincide with the University's construction of the Rubenstein Forum conference center and a 15-story for-profit hotel.&lt;br/&gt;Between rounds of chanting, attendees heard from 12 speakers representing different organizations.&lt;br/&gt;Nearly all of the speakers emphasized the University's alleged avoidance of racial issues, including a connection between the original Baptist University of Chicago and prominent Illinois politician Stephen Douglas, who took a morally ambivalent position on slavery in the run-up to the American Civil War. Some of the speakers mentioned a paper by a team of UChicago graduate students working at the Reparations at UChicago Working Group , which argues that Douglas was a direct financial beneficiary of slavery. The paper also argues that the old University of Chicago, which received the land for its campus from Douglas, should not be considered a separate entity from the modern University, as it traditionally has been.&lt;br/&gt;A student speaks at the racial justice rally on Sept. 29.&lt;br/&gt;Giovanna DeCastro / The Chicago MaroonDuring the second half of the rally, the group marched through the main quad to Hutchinson Court, near the plaque of Douglas outside of Mandel Hall in the Reynolds Club. Another commemoration of Douglas, a stone from Douglas Hall of the old University of Chicago, sits in the wall of the tunnel connecting the Classics Building and Wieboldt Hall.&lt;br/&gt;Ta-Nehisi Coates, prominent intellectual and public advocate for black reparations, attended the part of the rally outside the Reynolds Club, at one point filming the ralliers.&lt;br/&gt;Second-year Michelle Yang spoke on behalf of UChicago United, a coalition of multicultural RSOs: the Movimiento Estudiantial Chicanx de Aztlán (MEChA), the Organization of Latin American Students , the Organization of Black Students , the African Caribbean Students Association , the Arab Student Association , and the PanAsia Solidarity Coalition (PanAsia). Yang said large numbers of students at UChicago incorrectly believe that racism is not an issue on campus and called for more targeted measures to support minority students, including ethnic studies programs and a stronger bias response team. "We want the establishment of ethnic studies, black studies, Chicanx studies and Asian studies for core classes that don't only offer texts by dead white men, not only for students of color but for all students to understand the racist foundations that America was built on."&lt;br/&gt;Several of the speakers echoed the feeling that the University has resisted protecting and supporting activist members of the campus community. Mathematics Professor Denis Hirschfeldt, a member of AAUP and UChicago Resists, said that there has been an ongoing campaign by the University to make activists unwelcome. Hirschfeldt said, "Some of us are vocal, some of us are less vocal, but there are faculty here that want activists here."&lt;br/&gt;Several speakers stressed the importance of the upcoming vote on graduate student unionization, currently scheduled for October 17-18, and criticized the University administration for filing a motion that would further delay the vote.&lt;br/&gt;Other speakers mentioned the University's unwillingness to name and condemn the David Horowitz Freedom Center, which recently spread posters naming members of campus groups affiliated with the Boycott, Divestment, and Sanctions for the third time in the past two years.&lt;br/&gt;Fourth-year graduate student Alejandra Azuero Quijano, who spoke during the rally on behalf of UChicago Resists and is also a member of GSU, spoke about the University's free speech policies and a newly ratified disciplinary system for disruptive conduct in relation to attacks on students like those by the Horowitz Center.&lt;br/&gt;Speaking after the rally, Azuero Quijano said, "If you have an environment in which students are both being in some ways criminalized for protesting, and on the other hand, external speech is protected over speech coming from within campus, then you have an environment where the Horowitz [Center] can come and attack members of our community, and know that it will go not unnoticed, but not responded at with the same severity with which students are being met."&lt;br/&gt;Kamm Howard, a member of the National Coalition of Blacks for Reparations in America (N'COBRA) who spoke during the rally, said that he hopes the reparations campaign at UChicago could have nationwide influence. "What happens in Chicago, and of course at the University of Chicago, has national reverberations, so we're hopeful that what happens here can also affect some of the things that are going on around the country with universities admitting to their complicity, but also reconciling that past with reparations or reparative measures."</t>
         </is>
+      </c>
+      <c r="L129" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="130">
@@ -6082,10 +6476,13 @@
           <t>University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J130" t="inlineStr">
+      <c r="K130" t="inlineStr">
         <is>
           <t>The University of Chicago Medical Center opened the Center for Care and Discovery , its new hospital, on February 23, and its lack of a Level 1 trauma center became the most recent flashpoint for student activism on campus. While the late '60s were exceptionally tumultuous years for UChicago, with the two-week-long occupation of the Administration Building by student protesters, recent events on campus and in Chicago have sparked a new wave of student activism that is no longer limited to the quads or to the Hyde Park community, moving beyond issues that just affect students.&lt;br/&gt;The lack of a Level 1 adult trauma center on the southside of Chicago and the push for the UCMC to build one has been an issue that community groups have been raising for years. Most recently, the RSOStudents for Health Equity has joined community groups to protest the University's continued refusal to host a center, which they argue is the biggest obstacle in the fight to improve trauma care for southside residents. The UCMC says that a trauma center would be too costly and would take resources from other vital resources the hospital provides.&lt;br/&gt;On February 26, just three days after the CCD opened, SHE along with community groupFearless Leading by the Youth held their second protest at the site of the University's newest hospital (see "Campus Controversies"). The groups claim that SHE's projected $15 million per-year price tag for the trauma center is a small number compared to the $700 million spent to build the new facility, while the University and some community leaders claim the new hospital is doing a lot for the surrounding community.&lt;br/&gt;The subsequent discovery of an undercover UCPD officer posing as a protestor at the February 26 demonstration prompted outrage from students and from the administration, which claimed that it had no knowledge of the undercover officer before it was made public. (see "Campus Controversies").&lt;br/&gt;In response, students fromSouthside Solidarity Network launched a campaign seeking to reform certain aspects of the UCPD, including increasing transparency within the police force. The campaign culminated in a UCPD Speakout event held in late May, where students shared personal accounts of encounters with officers.&lt;br/&gt;Third-year and SSN coordinator Emma LaBounty said that the campaign for UCPD reform will continue through the upcoming school year. She feels that there is still an issue of policing on campus and that SSN would try to tackle the question of "how do we prevent instances like [the undercover UCPD officer] from happening again?"&lt;br/&gt;LaBounty also indicated that SSN, along with other groups on campuses across Chicago, would continue to fight for the University to adopt a no-loan policy, which the groups argue is vital to incoming students who must consider financial aid packages to make their choice.&lt;br/&gt;As SSN and SHE continue their campaigns this school year, others are moving on to new projects after successes last June.Students Organizing United with Labor , a group dedicated to tackling labor-related issues on campus, fought University administrators and food service provider Aramark over the fate of Pierce Dining Hall workers. They were able to secure a guarantee from Aramark that there would be no layoffs to dining hall staff as a result of the closure.&lt;br/&gt;Third-year and SOUL member Miriam Shestack said that her group would continue to look out for the rights of workers on campus. "This is an example of why a group like SOUL exists," she said. "Basically, when something is going on on campus we talk to workers to see if their concerns are being addressed by the University, and if they're not, we try to address them."&lt;br/&gt;SOUL will also join the Chicago Fight for 15 campaign, a group of Chicago fast food and retail workers who are demanding the minimum wage be raised to $15 an hour, which would affect workers across the campus.&lt;br/&gt;While some groups on campus have been fighting for issues for many years, this quarter will also see new social justice groups begin to officially organize. One such group, theSocioeconomic Diversity Alliance , began planning last year to apply for RSO status this fall.&lt;br/&gt;In the short term, SDA would like to establish a support group for low-income and first-generation students in the College, fourth-year Lynda Lopez, one of the group's main organizers, wrote in an e-mail. She said that the general consensus within SDA and on campus is that the University lacks any real resources for these students. Lopez also believes that SDA will be able to convince the University to assemble a task force to look into socioeconomic diversity on campus. This would be the group's long term goal, she said.&lt;br/&gt;Other groups continue to fight for their own issues on campus.Stop Funding Climate Change , theUChicago Climate Action Network and theGreen Campus Initiative will continue to demand that the University stop funding climate change. In April, a referendum was passed during Student Government elections, which called for the University "to shift its investment strategy to account for the environmental impact of oil, gas, and coal used by the companies it invests in." Despite student support for the referendum, the University has refrained from divesting from companies involved in political controversies in the past, saying that it is bound to be politically neutral by a document called theKalven Report.&lt;br/&gt;As both new and old students return to campus this September, they will be entering an environment of student activism that Lopez said is "alive and well."</t>
         </is>
+      </c>
+      <c r="L130" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="131">
@@ -6125,10 +6522,13 @@
           <t>Pro-Israel/Zionism</t>
         </is>
       </c>
-      <c r="J131" t="inlineStr">
+      <c r="K131" t="inlineStr">
         <is>
           <t>Dozens of student activists, student government leaders and NYU administrators gathered in room 802 of the Kimmel Center for Student Life on Thursday evening for a public town hall with President Andrew Hamilton, Student Government President Juan Manuel Calero, Senior Vice Provost for Global Programs Linda Mills and Assistant Manager of Diversity and Inclusion Initiatives Krystal McLeod.&lt;br/&gt;While the event was intended to focused on NYU's Global Network, activists from NYU's Student Labor Action Movement and NYU Divest pressed the president on issues of student representation and the university's fossil fuel investments. Hamilton also publicly announced his opposition to the decision of 51 student groups to boycott the state of Israel and other pro-Israeli student groups.&lt;br/&gt;Around 50 students and several NYU administration members turned out for the panel.&lt;br/&gt;SLAM and Divest Demand Transparency&lt;br/&gt;During the Q&amp;A session, several activists representing SLAM and NYU Divest took to the microphone to ask Hamilton questions. Despite the groups' recent streak of public activism and occupation of university buildings, the event proceeded without any major disruption from student activists.&lt;br/&gt;Attendees were largely made up of student activists and student government members, and many of SLAM's questions and commentary received snaps from the audience. When Hamilton made points that student activists disagreed with, several audience members hissed.&lt;br/&gt;"I take climate change very seriously and I have said so on many occasions," Hamilton said. "This is one of the greatest challenges facing the world in the coming decades and there are many ways of tackling it."&lt;br/&gt;Alana Beyer&lt;br/&gt;SLAM member and Gallatin senior Hannah Fullerton asked Hamilton how administrators and trustees will more effectively facilitate discussion between students, faculty and trustees.&lt;br/&gt;SLAM member and Gallatin senior Hannah Fullerton asked Hamilton how administrators and trustees will more effectively facilitate discussion between students, faculty and trustees. In response, Hamilton said that the university has made efforts to facilitate conversation in recent years and that he hopes to continue to facilitate conversation in the future.&lt;br/&gt;The audience reacted negatively to Hamilton's answer, as NYU recently denied SLAM and Divest's demand for a public town hall meeting with trustees in the room. When asked why the university turned down this demand, Hamilton cited the nature of the town hall meeting, claiming that its public and potentially hostile nature would prevent productive discussion.&lt;br/&gt;"Town halls are a different kind of format," Hamilton said. "They are not the most effective exchange of ideas."&lt;br/&gt;NYU Divest member and GLS junior Ismael Ibrahim took to the mic combatively, criticizing trustees' 2016 decision against fossil fuel divestment. Ibrahim used this example in reference to Divest's skepticism that the Board of Trustees could make decisions in line with the student body's values.&lt;br/&gt;Hamilton, saying that he is a believer in climate change and an ardent supporter of environmental research, admitted his disagreement with trustees on the matter.&lt;br/&gt;"My personal opinion is not necessarily the same as the Board of Trustees'" Hamilton says&lt;br/&gt;- Washington Sq. News (@nyunews) April 19, 2018&lt;br/&gt;However, Hamilton said that both NYU and New York City still rely on fossil fuels, and said he feels unsure that NYU could feasibly power all of its resources relying solely on renewables. Deflecting the critique of the board, he said that most of us, by using airplanes and automobiles, are contributing to the climate crisis, and that it must be each of our individual responsibilities to make habitual changes in our daily lives.&lt;br/&gt;Hamilton Denounces BDS Movement&lt;br/&gt;Near the end of the town hall meeting, Hamilton was met with hisses as he vocalized his disagreement with the Boycott, Divestment and Sanctions movement.&lt;br/&gt;"We believe the university exist to bring people together not to seperate them," Hamilton said. "For this reason I am opposed to BDS. The university will not participate in boycotting of academics based in Israel. We believe in academic freedom and the free flow of ideas. Boycotting is antithetical to that vision."&lt;br/&gt;The formal denouncement from Hamilton comes just one week after 51 students groups, led by the Jewish Voice for Peace and NYU Students for Justice in Palestine, joined together in support for the pro-Palestinian cause: Boycott, Divestment and Sanctions. The signatories call for a boycott of the state of Israel and of pro-Israeli student groups Realize Israel and TorchPac.&lt;br/&gt;"I am opposed to BDS," says President Andrew Hamilton&lt;br/&gt;- Washington Sq. News (@nyunews) April 19, 2018&lt;br/&gt;The BDS movement has sparked heated divisions on campus in the past week. Members from the Black and Brown Coalition at NYU said they have received verbal threats and harassment for their decision to support the BDS movement. Nearly 800 people have also signed on a pro-Israeli petition in opposition to the BDS movement.&lt;br/&gt;Hamilton also announced that he sent a letter to the Israeli government condemning their decision to ban groups that support BDS&lt;br/&gt;Alana Beyer&lt;br/&gt;Stern School of Business junor Essma Bengabsia, who brought up issues of explicit Islamophobia from students and faculty in Stern.&lt;br/&gt;Racism and Islamophobia in Stern&lt;br/&gt;Hamilton also addressed Stern School of Business senior Essma Bengabsia, who brought up issues of explicit Islamophobia and racism from students and faculty in Stern.&lt;br/&gt;"The use of the N-word is very frequent around Stern around students of color, sometimes to them," Bengabsia said. "On several occasions this year alone, several Muslim students have been called terrorists to their faces ... We've spoken on several occasions to administrators in Stern on many different levels and the responses we've gotten are things along the lines of, 'don't take it too emotionally,' 'don't take it personally,' 'it's your job to educate people.'"&lt;br/&gt;Hamilton said that he was aware of issues brought to administration in the past.&lt;br/&gt;NYU President Andrew Hamilton admits to knowing about claims of racism toward Muslim students at the Stern School of Business at Town Hall pic.twitter.com/XFlp1V7MNv&lt;br/&gt;- Mack DeGeurin (@MDeGeurin) April 19, 2018&lt;br/&gt;"What you've said is deeply distressing," Hamilton said to Bengabsia. "The incidents you described are completely unacceptable. I had been made aware of some of the concern and growing student unhappiness about the situation there. This is an opportunity and indeed Stern must take these concerns seriously."&lt;br/&gt;Linda Mills, who has been in dialogue with Bengabsia, also responded to the concerns expressed during the panel discussion.&lt;br/&gt;"It's very frustrating to hear that this has continued," Mills said. "We left the conversation at a key moment thinking progress had been made. The other thing I would say is that if you don't feel safe, we need to know and we need to take action."&lt;br/&gt;"We don't feel safe, I'm telling you right now," Bengabsia responded.&lt;br/&gt;In an interview with WSN, Bengabsia described her desire to have her voice heard by administration officials.&lt;br/&gt;"I've been trying to push for more diversity and inclusivity in Stern since I was a freshman, so for three years now," she said. "We came here today because we know it still goes back to the same Stern dean we're trying to reach but they don't put this as a priority until they have Andy Hamilton or Linda Mills or someone else from senior administration emailing them."&lt;br/&gt;Despite taking her concerns to senior administration, Bengabsia is still concered about the rate at which direct action will be taken. Associate Vice President for Student Affairs and Diversity Initiatives Monroe France said a 15 minute phone call between himself and NYU administration has been scheduled for Friday, April 20.&lt;br/&gt;"It was a nice response, they said they were concerned but I'm also just hoping it turns into action," Bengabsia said. "We've been having conversations like this for over three years and it's just been at a standstill."&lt;br/&gt;Stern first-year Reneen Khalil, who said she has been called a terrorist by more than one Stern student, told WSN about her feelings after the panel.&lt;br/&gt;"[Hamilton] said that town halls are not very effective, so what is the point of having this meeting if you're not listening to students," Khalil said. "I think there were a lot of passive aggressive comments being made by the [panel]. They tried to stay as general as possible and didn't answer a lot of students' questions."&lt;br/&gt;Global Mobility in Wake of Visa Denials&lt;br/&gt;When asked by WSN what steps NYU is taking to ensure global mobility of faculty and students critical of host government, Hamilton repeated many of the same points he has made in previous public statements.&lt;br/&gt;"A principal tenet of the Global network is the free flow of students and faculty throughout," he said.&lt;br/&gt;Hamilton acknowledged the visa denials of professors Mohamad Bazzi and Arang Keshavarzian to the NYU Abu Dhabi campus, but went on to say that students and faculty have also experienced a rise in visa denials to the United States under the Trump Administration.&lt;br/&gt;"We saw two faculty members unable to get visas for the Abu Dhabi campus last year," he said. "We also saw students unable to get visas to the United States and that is likely to increase in the coming years before it gets better again with this current government in Washington D.C."&lt;br/&gt;Hamilton said that the university is acting to strengthen their office for visa support, which he said will offer students and faculty better guidance and information about visas and mobility for their particular abroad sites.&lt;br/&gt;When asked why NYU's administration did not play a more active role in combating faculty visa denias, the president said that the university cannot control the laws and security clearances issued by foreign governments.&lt;br/&gt;"The university does not give out visas, governments do," he said. "We have little control over that decision making process."&lt;br/&gt;He said the university will press and do what it can to work with governments, but did not specify what these interventions would look like in practice. Hamilton said that while the university aims to address issues related to mobility, visa denials are an inevitable consequence foundational to the Global Network.&lt;br/&gt;"I can't change the world and sometimes the world can be a mean and bitter place," Hamilton said.&lt;br/&gt;Email the WSN News Desk at [email protected]&lt;br/&gt;Correction, April 22: A previous version of this incorrectly said that the phone call regarding discrimination at Stern was to be between the NYU administration and Essma Bengabsia. However, the conversation was scheduled to be between NYU's administration and Monroe France.</t>
         </is>
+      </c>
+      <c r="L131" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -6168,10 +6568,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J132" t="inlineStr">
+      <c r="K132" t="inlineStr">
         <is>
           <t>Protesters of the Keystone XL pipeline, a proposed pipeline that would carry tar sands oil from Canada to the Gulf of Mexico, lined up at the intersection of Lincoln Way and Welch Avenue on Saturday, Sept. 21.&lt;br/&gt;Tar sands oil consists of crude oil mixed with sand, clay and bitumen, a material used for road and roof surfacing.&lt;br/&gt;Approximately 30 people turned out for the "Draw the Line" rally, and about a third of them were students.&lt;br/&gt;"It was interesting that the rally participants were either young [children], college [students] or older retired people," said Terry Lowman, a member of A Mid-Iowa Organizing Strategy. "One of the issues with climate change is that it is gradual enough that it's difficult for one to personally see how things are changing."&lt;br/&gt;Yet some older people can tell there's something different. Look at the photos of the North Pole over the last 40 years. It's visibly different.&lt;br/&gt;An environmental and social justice group on campus called ActivUs participated in the event along with AMOS and Ames community members.&lt;br/&gt;AMOS and ActivUs were in charge of organizing the rally on campus; they filled out a 350.org event planner, a website dedicated to climate crisis activism that began the "Draw the Line" campaign, and reached out to those who might be interested in the event.&lt;br/&gt;AMOS focused on the off-campus community, while ActivUs focused on recruiting students for the event.&lt;br/&gt;Emails were sent to those involved with ActivUs, the graduate program in sustainable agriculture and Live Green.&lt;br/&gt;"I was impressed by the turnout," said Rivka Fidel, president of ActivUs. "We had more people come [to the rally] than sign up online."&lt;br/&gt;The Draw the Line rally is a national event. Six protest rallies were held in Iowa and many environmental activist organizations such as Better Future Project, The Climate Reality Project, Energy Action Coalition and Friends of the Earth were participants in "drawing the line" across the country.&lt;br/&gt;Participants at the Iowa State rally held signs made the previous Thursday in Sloss House.&lt;br/&gt;The signs each contained a line; when the protesters stood together, they'd connect their lines and literally "draw the line" in protest against the pipeline, asking President Barack Obama to reject it.&lt;br/&gt;Some of the signs had slogans like "Pipelines Always Spill," "Jobs for Clean Energy, Not For Dirty Oil," "KXL Equals Xtra Bad" and "Climate Justice."&lt;br/&gt;"President Obama said he would not approve the Keystone XL pipeline if it would significantly impact the climate, but he still has not rejected it outright," Fidel said in ISU's 'Draw the Line' press release. "Research shows that burning the tar sands oil will result in 0.7 degrees Fahrenheit (0.4 degrees Celsius) of warming. So the science is clear. It's time for Obama to draw the line on KXL and say 'no.'"&lt;br/&gt;The protesters caught the eyes of some onlookers.&lt;br/&gt;"Occasionally someone would come along and ask a question, at which point a few of us would break off to start a more serious discussion," Fidel said. "We were surprised that some passerby did not know what the Keystone XL pipeline was."&lt;br/&gt;Participants in the hour-long event also shared their demonstration through social media. ActivUs members took pictures and made posts on their Facebook page, bringing in approximately 50 page views.&lt;br/&gt;Opposition for the Keystone XL pipeline concurs with most of what was voiced at Saturday's rally. Those opposed are mainly concerned with climate change as the result of burning oil and its greenhouse gas emissions and the potential for environmental disasters with a pipeline running straight through the United States.&lt;br/&gt;Those encouraging the pipeline's construction are arguing it will, according to Keystone XL Pipeline website, "bring essential infrastructure to North American oil producers... provide jobs, long-term energy independence and an economic boost to Americans."&lt;br/&gt;Iowa State's ActivUs group plans to participate in a 350.org fossil fuel divestment campaign called "Fossil Free" in the future, continuing with their endeavors to halt climate change.&lt;br/&gt;"ISU represents education, especially scientific education, and it is scientific knowledge that proves climate change is happening," Fidel said. "We must act to mitigate it immediately."</t>
         </is>
+      </c>
+      <c r="L132" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="133">
@@ -6211,10 +6614,13 @@
           <t>Sexual assault/violence</t>
         </is>
       </c>
-      <c r="J133" t="inlineStr">
+      <c r="K133" t="inlineStr">
         <is>
           <t>Students hang banners in Arts and Letters Hall Wednesday decrying hate speech a week after conservative MIlo Yiannopoulos visited campus. (Brenden Moore/The DePaulia)&lt;br/&gt;Student activists decried hate speech as they dropped banners, one stating "Hate speech ? free speech" and the other asking "What would Vinny do?",  from the third and fourth floor balconies of Arts and Letters Hall this afternoon.&lt;br/&gt;The act comes after a week which saw political and racial tensions float to the surface following conservative writer Milo Yiannopoulos' visit to campus and incidents that include the drawing of an anti-Mexican slur on the Quad and the reported finding of a noose the sidewalk near a residence hall.&lt;br/&gt;Around 20 student activists, split by floor, dropped the banners around 12:50 p.m. and started chants that included, "Hate speech ain't free speech", "Can't stop the revolution" and "Black Lives Matter".&lt;br/&gt;Sources said the event had been in the works for nearly a week and that it may have been the effort of a sociology class applying the events of last week to curriculum in the classroom.&lt;br/&gt;About 10 minutes in, a university maintenance worker attempted to take the banners down, which led to chants of "Let the banner hang!" and then cheers when he indeed quit his effort.&lt;br/&gt;"Let the banner hang!" pic.twitter.com/P1mMjhqfuO&lt;br/&gt;- Brenden Moore (@brendenmoore13) June 1, 2016&lt;br/&gt;The event would continue for another 10 minutes when Public Safety eventually took the banner down. The students then marched outside the building and dispersed.&lt;br/&gt;The university appeared to have a heads up as an assortment of officials, including vice president for facilities operations Bob Janis, vice president for student affairs Gene Zdziarski and associate vice president for diversity Rico Tyler were quickly on the scene. This is the fourth banner drop in recent years. One in April 2014 brought attention to the alleged rape culture in the athletic department, one in Spring 2014 called for DePaul to divest in companies that supported Israel's occupation of Palestine by dropping a Palestinian flag and one in the Student Center two weeks ago called for former Chicago Police officer Dante Servin to be denied his pension after he killed Rekia Boyd.</t>
         </is>
+      </c>
+      <c r="L133" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -6254,10 +6660,13 @@
           <t>Anti-racism, Campus climate, University governance, admin, policies, programs, curriculum, Affirmative action (For)</t>
         </is>
       </c>
-      <c r="J134" t="inlineStr">
+      <c r="K134" t="inlineStr">
         <is>
           <t>In recent months, colleges across the country have seen a spate of demonstrations regarding issues of identity, with students demanding greater inclusivity on their campuses. Many resemble Dartmouth's April "Freedom Budget" protests, when over a dozen students occupied College President Phil Hanlon's office for two days, demanding a point-by-point response to a list of over 70 demands regarding issues of diversity.&lt;br/&gt;In the last year, students at Princeton University, Harvard University, Oberlin College, Mills College, University of Michigan, City University of New York, Mount Holyoke College and University of California at Los Angeles, among others, have initiated protests concerning similar issues. Melissa Padilla '16, who was involved in the "Freedom Budget" protest, said she communicated with her friends who were involved with similar protests at other schools, including New York University and University of Texas at Austin, during the construction of the "Freedom Budget" and the sit-in. Other Dartmouth activists spoke with friends on various campuses as well, she said. The protest at Dartmouth, she said, was not a reaction to movements at other schools but a response to discrimination at the College. "A lot of universities are looking to be more inclusive but are acting very unlike their statements," Padilla said. "There's a big gap between their mission statements and the actual reality of being a student on campus." Across the country students are demanding that administrators make structural changes to better support all students. On April 7, a coalition of students at Oberlin College, in Ohio, wrote an open letter in support of the sit-in at Dartmouth. The letter was posted in the opinion section of "Fearless and Loathing," an independent website run by Oberlin students. "We recognize the actions of our fellow students at Dartmouth as courageous, necessary steps that must be taken if institutions such as ours - ones that advertise themselves on falsified notions of diversity, inclusivity and dignity - continue to treat 'dialogue' as a synonym for structural violence," the letter states. Oberlin junior Ana Robelo, who has been a member of the coalition since its founding last fall, said several communities on Oberlin's campus worked together to compile a list of demands for their school's administration. The demands included increased administrative transparency, divestment from companies that support Israeli occupation of Palestine and scholarship funding for undocumented students. On Oct. 10, a group of Oberlin students took over the Board of Trustees meeting and discussed demands. Oberlin senior Alice Beecher said that hundreds of students dressed in red as a symbol of solidarity. Robelo said she sensed strong and immediate backlash during the meeting. Student reactions, however, were generally supportive, though some disagreed with the group's tactics and the demand to divest from companies that support Israel, Beecher said. Since the board meeting, Beecher said that some smaller communities within the coalition have met with administrators to advance individual demands. Beecher said students joined together to create a replica of the wall separating Gaza and Israel, painting it with different representations of borders in society. Students then placed pieces of the wall in front of Oberlin's main library alongside an audiotape playing students' personal stories of division within the Oberlin community, she said. Members of the coalition also stood outside a second trustee meeting in December while holding pieces of the reconstructed wall, Beecher said. Robelo said the coalition formed in part as a result of events that took place at Oberlin last spring, including the appearance of someone dressed in a Ku Klux Klan robe and racist graffiti around campus. The coalition, Beecher said, was reacting to what they perceived as the administration's non-response. On May 1, approximately 10 students sat outside a Princeton University student center wearing black shirts and white opera masks, playing a recording of their manifesto on a boombox, Princeton junior Katie Horvath said. Passersby were offered fliers outlining the group's 10 demands for change at the university, including revised mental health policies, divestment and a call for more gender neutral housing options, among others. Horvath, who participated in the demonstration but emphasized that she did not organize it, said although the protest stemmed from a queer activism movement, its demands were "intersectional" and addressed a range of issues beyond gender.&lt;br/&gt;Though the Princeton group, called Praxis Axis, placed a stack of masks next to their demonstration as an invitation for passersby to join in, few people followed suit since few knew in advance or had clothing that matched that of the protesters, which Horvarth said became a "barrier to entry." Horvath said that the Praxis Axis demands felt similar in nature to demands voiced by the "Freedom Budget," as both were intersectional efforts to address issues centered on identity. Although Praxis Axis members did not work directly with Dartmouth students to compile their demands, Horvarth said she believed demonstrators at various schools would benefit from joining forces. For those at institutions like Princeton, which tend to have less widespread student activism than more urban institutions, engaging with like-minded students at other colleges can contribute to a stronger "protest culture," she said. On April 2, Princeton freshman Tal Fortgang published an essay titled "Checking My Privilege: Character as the Basis of Privilege" in The Tory, a conservative publication at the school. The piece, in which Fortgang refused to apologize for having privilege and cited examples of difficulties faced by his family, prompted much discussion on the Princeton campus, Horvath said. "It's been helpful," she said, "in that it has made people concerned and aware who would otherwise be likely to dismiss the demands of a group like the protest group on May Day as unnecessary or absurd or over the top." Mount Holyoke, an all-women's college in Massachusetts, is in the midst of a movement that aims to address discrimination and increase student involvement in college policy, said junior Melanie Wilkerson, an active participant in the movement. The movement, known as "MoHonest," began after Mount Holyoke student Maya Wegerif, 21, wrote a blog post alleging discrimination by campus police when she was arrested following an alcohol-related incident. Wilkerson said that many students of color at Mount Holyoke related to Wegerif's experience, and the incident sparked much discussion about discrimination and the power of campus police. "We began to form an entity that wanted to specifically represent students of color on campus," she said. "And even more broadly, those who have faced discrimination on campus or were allowed to suffer discrimination and not receive adequate administrative support." Members presented a formal list of demands to the administration in April, Wilkerson said, and are currently at a "standstill." The group's demands include encouraging more active student participation in campus policy and decisions, increasing institutional support for first-generation college students, updating the policy for reporting grievances and creating educational workshops for students, faculty, staff and campus police. "We're still negotiating, but we're a little disappointed with the administration," Wilkerson said. Wilkerson said that members of the "MoHonest" movement were aware of the "Freedom Budget" and considered the Dartmouth activists' tactics when brainstorming. The sit-in at Dartmouth, she said, was "successful in its visibility." Though "MoHonest" protesters considered a sit-in, Wilkerson said they decided against it because some members felt that - unlike at Dartmouth - not enough time had elapsed since the demands had been voiced. Wilkerson said the "MoHonest" movement reflects a nationwide trend of students becoming more vocal about administrators' lack of support. "MoHonest" has supported related movements at other institutions, including Vassar College and Bryn Mawr College, she said. "I feel like the trend is catching on because people across the country are really starting to acknowledge the kind of power young people have," she said. Though "MoHonest" faced some opposition from students, Wilkerson said it has found a broad base of support among faculty and alumni. "In my three years at Mount Holyoke, I have witnessed people go through some pretty intense stuff in terms of discrimination," Wilkerson said. "Even in a very liberal, diversity-agenda-pushing institution like Mount Holyoke, there are still fundamental flaws and issues that need to be addressed." Two student movements have recently arisen at Harvard University, both aiming to increase diversity among faculty, staff and administrators and to improve resources for more diverse programming, Harvard senior Terrance Moore said. The first of these movements, a photography campaign titled "I, Too, Am Harvard," launched on Tumblr in early March. The pictures show black students holding signs with examples of racial prejudice they have experienced at Harvard, accompanied by the slogan. Once the campaign gained attention, students involved began researching other movements to see how they were successful in creating institutional change, Moore said. The second student movement, known as "The Diversity Report," spun out of the "I, Too, Am Harvard" campaign, Moore said. Students involved in "The Diversity Report" wrote a list of demands and are currently working with specific administrators to achieve them, Moore said. After contacting them, the students decided to fill out report cards evaluating administrators to hold them accountable.</t>
         </is>
+      </c>
+      <c r="L134" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -6302,10 +6711,13 @@
           <t>_Other Issue</t>
         </is>
       </c>
-      <c r="J135" t="inlineStr">
+      <c r="K135" t="inlineStr">
         <is>
           <t>Bridget R Irvine Sandra Korn '14, a leader for the Responsible Investment at Harvard Coalition, speaks to protesters gathered on the steps of Widener Library on Friday afternoon. The rally protested Harvard's management of its timber plantations in northern Argentina and ended in a protest in front of Massachusetts Hall.&lt;br/&gt;The Responsible Investment at Harvard Coalition held a rally Friday afternoon on the steps of Widener Library and Massachusetts Hall to protest the University's management of timber plantations it owns in Argentina. The rally comes after much debate over the plantations, including allegations of mismanagement in the fall and the announcement of the recertification of the plantations last week.&lt;br/&gt;Throughout the afternoon, students and community members chanted, marched, and held signs, which read "Harvard be transparent," "Faust: no more land grabs," and "We're yelling timber, you better move."&lt;br/&gt;After several members of the Harvard community, including the Undergraduate Council President and a Harvard alumnus working on the City Council, spoke to the protesters gathered in front of Widener, the group marched to Massachusetts Hall, which houses the University's central administration and President Drew G. Faust's office. A delegation from the group entered Massachusetts Hall with a petition containing 1,150 signatures, formally asking Faust to change the University's management of its plantations.&lt;br/&gt;The protests were a part of Responsible Investment at Harvard Coalition's week-long SHAME Tour, which seeks to "stop Harvard's Argentine mismanagement and exploitation," according to the organization's website. As part of the demonstration, the coalition flew two leaders from local communities in Argentina, Adrian Obregon and Emilio Spataro, 4,884 miles to Harvard's campus.&lt;br/&gt;Responsible Investment at Harvard is a coalition of students, alumni, faculty, and community members dedicated to changing the way the University manages its investments, according to its website. Members of the coalition argue that Harvard's unjust practices on the Argentine plantations include devastating local farmers, harming workers, and destroying wetlands.&lt;br/&gt;According to Responsible Investment at Harvard member Gabriel H. Bayard '15, the coalition's three basic demands are that "all new planting [has] to stop until an environmental impact study has been done in a participatory manner, all planting [must] be stopped within two kilometers of populated areas, and the Harvard Management Company [must] oblige by all legally required labor practices."&lt;br/&gt;UC president Gus A. Mayopoulos '15 spoke at the rally, voicing his support for the coalition's efforts. The UC will be hosting a forum on responsible investment with Obregon and Spataro on Tuesday.&lt;br/&gt;"It is unfortunate, it's sad, and it's embarrassing that Harvard is choosing to fund these efforts by damaging a community," Mayopoulos said.&lt;br/&gt;Cambridge City Council Member and Harvard Kennedy School graduate Leland Cheung also spoke at the rally.&lt;br/&gt;"I'm proud to be a Harvard grad, but there's so much that is making me ashamed," Cheung said, citing both the campaign for divestment and the recent unionization movement of DoubleTree hotel employees.&lt;br/&gt;"It's not enough to try to educate students to go out and change the world when Harvard is going out and damaging the world," he added.&lt;br/&gt;In addition to the protest, Responsible Investment at Harvard has already hosted several events, including one in New York and an event with the Harvard Kennedy School Progressive Caucus.&lt;br/&gt;-Staff writer Kristina D. Lorch can be reached at klorch@college.harvard.edu</t>
         </is>
+      </c>
+      <c r="L135" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="136">
@@ -6345,10 +6757,13 @@
           <t>_Other Issue</t>
         </is>
       </c>
-      <c r="J136" t="inlineStr">
+      <c r="K136" t="inlineStr">
         <is>
           <t>The practice of protesting commencement speakers is nothing new, but rarely in recent memory have these protests been as widespread and as solicitous of public attention as they have been this spring.&lt;br/&gt;It all started April 8, when administrators at Brandeis University, acting under pressure from undergraduates and faculty members, rescinded a commencement invitation to Ayaan Hirsi Ali, a noted women's rights advocate and strident critic of Islam. To most students, the rescindment seemed prudent, and the original invitation almost inexplicable. Ali, after all, had called Islam a "destructive, nihilistic cult of death" in an interview with the London Evening Standard in 2007, and many of her statements continue to be overtly Islamphobic.&lt;br/&gt;But the commencement rows that would follow in the coming weeks seemed far more frivolous, in that these protests were not based in opposition to personal bigotry, but rather in opposition to specific political policies that were not, on their face, tied to intolerance.&lt;br/&gt;On May 4, for instance, former Secretary of State Condoleezza Rice, facing student protest at Rutgers as a result of her involvement in the Iraq War and her approval of waterboarding war detainees, decided not to attend the school's ceremony, as she feared that the contentious atmosphere surrounding her visit would subtract from the collegial atmosphere of graduation. Though she withdrew voluntarily, it was clear she felt intellectually bullied. "I am honored to have served my country," she said on May 5. "I have defended America's belief in free speech and the exchange of ideas."&lt;br/&gt;Christine LaGarde: Is she really that evil? (AP/Cliff Owen)&lt;br/&gt;Christine LaGarde, the current managing director of the IMF and a noted labor and antitrust lawyer before she entered the public sector, was the next commencement speaker to come under fire. Petitioners at Smith College, students and faculty alike, rallied to disinvite her, accusing the IMF of "imperialistic" policies, while conceding that LaGarde may herself be a "good person." Soon LaGarde withdrew for the same reasons as Rice.&lt;br/&gt;A few days later, students at Haverford pressured former University of California chancellor Robert C. Birgeneau into withdrawing from its commencement ceremonies because he initially supported the police response to a heated 2011 Occupy Berkeley incident. (The fact that he condemned the police and called for an immediate investigation after seeing video footage of the altercation a few days later meant little to the protestors.)&lt;br/&gt;And, recently, a similar debate also penetrated Harvard's campus: at the Graduate School of Education, petitioners attempted a putsch against Colorado State Senator Michael C. Johnston-who fortunately did speak at commencement-on the basis of his support for "test-based accountability" for teachers.&lt;br/&gt;Among the commentariat, save in the most liberal journals, pundits and editorial boards have come down against these protesting students, describing their meta-movement as a harbinger of "rising liberal intolerance" on campus. And though student papers, including the Crimson, have defended the protests, it seems to me that the mainstream media is at least partially right. Birgeneau, who himself has a history of liberal, nonviolent protest, hardly seems like a controversial figure. Neither does LaGarde, who in many respects would be considered something of a lefty in Amercan political circles, even if the organization she now heads is associated with neoliberal economics. New York City police commissioner Ray Kelly treads more contentious ground, but the refusal of Brown students to let him speak at a forum and Q&amp;A last semester-which is far from a commencement speech-struck many, including myself, as close-minded.&lt;br/&gt;Those supporting these student protests frame the issue as one of free speech: they have a right, under this principle, to fight "speech with speech"-and their speech happens to take the form of protest. I wholeheartedly agree with this principle, but this argument misses the point.&lt;br/&gt;Though we certainly have a right, and, at times, a responsibility to protest, the issue here is the effect of the protest, not the legitimacy of the method. And here the effect is too often sealing our campuses off from the policies that vocal students disagree with-limiting our politics to a very narrow kind of campus liberalism.&lt;br/&gt;In the protestors' defense, a commencement address is not just another forum on campus; the selected speaker should not denigrate a certain people or ethnicity during their speech, as graduates of all stripes should be able to attend without their personal dignity being called into question. That's why I agree with Brandeis' rejection of Hirsi Ali.&lt;br/&gt;But specific policy disagreements-unless they are predicated on racist or overtly discriminatory sentiment-should not be a basis for disinvitation. Like most campus communities, our community is far too intellectually diverse to avoid this kind of conflict, and-as most students who've engaged in political debate with peers will attest-non-bigoted, intellectually rigorous arguments from the other side of the political spectrum are often the most informative, and almost always the most challenging.&lt;br/&gt;For me, it feels strange to oppose student protest, as I appreciate and support the work of SLAM, SJSF, Divest and a number of other activist groups on campus. In other words, I mostly share the politics of the protestors I'm critiquing. But here I do have one profound disagreement: while a commencement speaker must be intellectually accomplished and adhere to basic principles of tolerance, he or she does not need to agree with my politics.</t>
         </is>
+      </c>
+      <c r="L136" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="137">
@@ -6388,10 +6803,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J137" t="inlineStr">
+      <c r="K137" t="inlineStr">
         <is>
           <t> WASHINGTON - Hoping President Barack Obama, CC '83, was watching from his window, 13 Columbia undergraduates protesting the Keystone XL pipeline were arrested in front of the White House Sunday afternoon. The students were released later that evening.&lt;br/&gt;The group was part of XL Dissent, a student-organized march against the pipeline, which drew more than 1,000 students from 100 colleges and universities to Washington, D.C., over the weekend.&lt;br/&gt;"The point of getting arrested is that it's making a much stronger political statement," Michael Greenberg, CC '16 and founder of XL Dissent, said at a civil disobedience training session Saturday to loud cheers.&lt;br/&gt;"You just don't get media if you're just at a rally," Elana Sulakshana, CC '17 and an organizer of the Columbia delegation, said.&lt;br/&gt;Police arrested 372 protesters from 12 p.m. to 5 p.m. for "blocking passage," an infraction that carries a $50 fine.&lt;br/&gt;The XL Dissent protest started Sunday morning with a rally in Georgetown University's Red Square, after which students marched for two miles through the streets of Washington to the White House.&lt;br/&gt;Protesters laid out black tarps representing oil spills along the way, including one in front of Secretary of State John Kerry's house. The march ended with a rally in front of the White House and a demonstration in which students zip-tied themselves to the White House fence or pretended to die on top of an "oil spill."&lt;br/&gt;"The Keystone Pipeline is enormous," said Iliana Salazar-Dodge, CC '16, who was arrested Sunday along with Sulakshana and Greenberg. "Because it's so big, it could be a big turning point in the fight for climate change, or it could reaffirm our commitment to fossil fuels. The time has come where we have to do something now."&lt;br/&gt;Although the Keystone XL has brought many environmentalists together under one cause, an unwanted possible result is a fractured and fragmented movement. On Sunday, students held signs proclaiming themselves as "ecosocialists" alongside ones that said "Hope &amp; Change, not Climate Change" and "Planet over Profit."&lt;br/&gt;Many of the student protesters were involved in environmental activism groups at their schools.&lt;br/&gt;Rachel Thomas, Tufts '16, was arrested Sunday with the other students. Thomas said she is heavily involved in her school's divestment from fossil fuels-like many of the Columbia protesters.&lt;br/&gt;Chris Bangert-Drowns, University of Maryland '17, said he is a proponent of student power on a general level, because students in and around Washington do not have official representation.&lt;br/&gt;Because the proposed pipeline, which would carry crude oil from the tar sands of Northern Alberta, Canada to refineries along the Gulf Coast, cuts across the border between the United States and Canada, it must be approved by both the State Department and Obama. The Keystone XL is seen by environmentalists as a test of the president's resolve to fight climate change-a goal the president has said would be a linchpin of his second term.&lt;br/&gt;Greenberg said the goal of XL Dissent is to force Obama to refuse to allow the pipeline to be built and to begin a wave of young activism on the issue.&lt;br/&gt;From speaking with students in XL Dissent, it was clear that few had ever been arrested in an act of civil disobedience before, and some had never even been to a protest.&lt;br/&gt;Much of Saturday's civil disobedience training session involved organizers from DC Action Lab, a Washington-based activist group, and more experienced protesters giving advice ("Bring your own toilet paper.") and telling people what to bring, which was only a photo ID and exactly $50 bail ("The police do not make change.").&lt;br/&gt;"Should I zip-tie myself to the fence or die on the spill to get arrested?" Sulakshana asked other Columbia students during the rally.&lt;br/&gt;Greenberg started XL Dissent in September 2013 after he worked as a summer fellow at 350.org, a nonprofit that organizes and raises awareness for climate change movements. Sunday's march aimed to bring student voices into the debate over the proposed Keystone XL pipeline.&lt;br/&gt;"We can only afford to burn 20 percent of the conventional fuel reserves we have, and the fact that we're even considering this is absurd," Greenberg said, referring to the Intergovernmental Panel on Climate Change's prediction that disastrous climate change would be inescapable if more than 20 percent of the world's fossil fuel reserves were burned.&lt;br/&gt;A 2011 EU study said that refining oil from tar sands produced 22 percent more emissions than refining oil from more conventional sources. And according to the Alberta Ministry of Energy, around 11 percent-or 170 billion barrels-of the world's oil reserves lie in the province.&lt;br/&gt;Environmentalists are concerned that the Keystone XL pipeline would pave the way for a massive expansion in the extraction and refining of oil sands, along with potential spills and problems that could ruin habitats along the pipeline.&lt;br/&gt;But proponents of the pipeline aren't convinced that its effects will be as dire as environmentalists think. A State Department report from January concluded that oil would be extracted from the tar sands at the same rate whether the pipeline were built or not. A Feb. 21 editorial in Science written by the magazine's editor-in-chief Marcia McNutt argued that transporting oil by pipeline is at least safer than by road or rail.&lt;br/&gt;"That's like saying, 'Let's kill the world because the world's going to get killed anyway,'" Greenberg said.&lt;br/&gt;Salazar-Dodge agreed.&lt;br/&gt;"Even if they build a pipeline in Canada anyway, if Obama vetoes it, it would send a message," she said.&lt;br/&gt;XL Dissent is a rough hierarchy of organizers, campus leaders, and participants, not a leaderless movement, Greenberg said. The group's next steps are unclear as it waits for an answer from the White House.&lt;br/&gt;Greenberg, as he marched with the protesters he helped to mobilize, seemed bewildered that XL Dissent had been such a success.&lt;br/&gt;"It's a little intimidating, because people might be a little disappointed by future things that I do," he said.&lt;br/&gt;news@columbiaspectator.com  |  @theareticall</t>
         </is>
+      </c>
+      <c r="L137" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="138">
@@ -6431,10 +6849,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J138" t="inlineStr">
+      <c r="K138" t="inlineStr">
         <is>
           <t>Echoes of drummed garbage cans paired with acoustic guitars and the constant chant of "We are unstoppable, another world is possible."&lt;br/&gt;This was the scene in Washington, D.C. as UVM students protested the Keystone pipeline until arrest, March 2.&lt;br/&gt;"This was my first time getting arrested and I wanted it to be for something that was not a dumb mistake but something that I care about and did intentionally," junior Christina Fornaciari said. "I was on the fence [about participating] until we started walking with the rally.&lt;br/&gt;"It felt like most people around me were opting to get arrested and I wanted to be a part of that," she said.&lt;br/&gt;Close to 40 students from various Vermont schools took a bus to the capital over spring break to join hundreds of students at the XL Dissent Protest, Fornaciari said.&lt;br/&gt;The Vermont schools represented included UVM, Bennington College and Middlebury College.&lt;br/&gt;"I think many people when they are interested in a certain issue just talk about it but I think UVM students are more the doing type," SGA president Connor Daley said.&lt;br/&gt;Of the 18 UVM students who attended the protest, nine were arrested, senior Alex Smiley said.&lt;br/&gt;She said she organized and planned for the UVM group to attend the protest.&lt;br/&gt;"A fair number of students seem excited about engaging in some of these big picture environmental issues in a way that I haven't seen in a while," said Rob Williams, a lecturer in the Rubenstein School of environmental sciences.&lt;br/&gt;The UVM student protestors that were arrested were Smiley, Fornaciari, junior Caroline McCall, senior Katy Hellman, junior Emily Roland, senior Margaret Galka, senior Morgan Marzo, sophomore Brian Thompson and junior Claire Longyear, Smiley said.&lt;br/&gt;"I think students willing to get arrested in D.C. fits with Vermont's reputation of being a petri-dish for political, environmental and social change," Williams said.&lt;br/&gt;Smiley said she "jumped on" the opportunity to organize the protest after Ally Johnson-&lt;br/&gt;Kurts, state divestment organizer for 350Vermont, spoke in her climate justice and advocacy class, asking someone to take charge.&lt;br/&gt;The protest featured a march from Georgetown University campus to the White House, speeches on the implications of the pipeline and an acted out oil spill demonstration.&lt;br/&gt;The protest ended with the occupation of the White House fence and sidewalk until arrest, according to XLDissent.org.&lt;br/&gt;The protest urged President Barack Obama to consider his previous commitment to environmental policy and reject the pipeline's construction, according to XLDissent.org.&lt;br/&gt;The protestors were arrested on the charge of "blocking passage" and were faced with a collateral fine of $50, Sgt. Lelani Woods of the U.S. park police said.&lt;br/&gt;To "block passage" means to "impede" other visitors of the area from "viewing the north side of the White House and from walking on the sidewalk," Woods said.&lt;br/&gt;"If you are going to get arrested, don't get arrested for dealing crack, get arrested in service to the community and the planet," Williams said. "That's the best way to get arrested."&lt;br/&gt;Canada's National Energy Board plans to have the 263 mile long pipeline that currently carries "light crude oil" from Maine through Vermont to Montreal to now transport a heavier oil extracted from tar sands.&lt;br/&gt;The line travels 1,179 miles from the Canadian province of Alberta through eight American states, according to a March 6 article from VTDigger.&lt;br/&gt;Fuel derived from the tar sands extractions creates 17 percent more greenhouse gas emissions than conventional fuel, according to a March 5 article in VTDigger.&lt;br/&gt;The board recently hired the Canadian energy company, Enbridge, to reverse the flow of this crude oil, according to the articles.&lt;br/&gt;Each day 300,000 barrels of the heavy oil would move east to two Quebec refineries.&lt;br/&gt;This number is up from the previous 240,000 barrels per day that were transported in the opposite direction, according to the VTDigger articles.&lt;br/&gt;The concern that most Vermont students and local residents find with the plan is that these heavier tar sand oils may lead to leaks in the 30-inch, 63-year-old, the article stated. 12</t>
         </is>
+      </c>
+      <c r="L138" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="139">
@@ -6474,10 +6895,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J139" t="inlineStr">
+      <c r="K139" t="inlineStr">
         <is>
           <t>Gustavus students marched in the nation's capitol last week as part of a nation-wide student-led protest against the Keystone XL pipeline. Demonstrating under the name XL Dissent, 25 Gustavus students joined over 1,000 other youth from across the United States in the largest act of youth civil disobedience in a decade.&lt;br/&gt;Gustavus students represented the largest collective group of youth protesters from the state.   With 70 youth in attendance overall, Minnesota had the second-largest state representation at the protest, coming in behind Massachusetts.&lt;br/&gt;According to student reports, after marching, the protesters fastened themselves to the White House fence with plastic zip ties and staged a mock oil spill on the sidewalk outside.&lt;br/&gt;After repeated warnings, police arrested demonstrators for blocking passage of sidewalks. Nearly 400 students were arrested, including eight from Gustavus.&lt;br/&gt;The arrests have raised some eyebrows among students on campus. Some viewed the arrests as contrived and questioned the need for orchestrating them.&lt;br/&gt;Senior Political Science Major Anna McDevitt, one of the key Gustavus organizers for XL Dissent, spoke to the mechanics behind the notion of risking arrest. For her, risking arrest is a key component of effective civil disobedience.&lt;br/&gt;"Throughout history, civil disobedience has played a huge role in shaping our nation's history-and our world's history-and much of it has been student-led. Our protesting Keystone XL is our generation's way of being a part of that tradition of civil disobedience. Our willingness to be arrested is our way of saying, 'we're not afraid, we're willing to put ourselves on the line to show what is important to us,'" McDevitt said.&lt;br/&gt;Though an important statement, other students saw the arrests as a reminder of their privileged position in society. Senior Political Science and Scandinavian Studies Major Annalise Dobbelstein, one of those arrested, voiced her inner conflict.&lt;br/&gt;"I was definitely conflicted about getting arrested. I mean, I raised my own bail money and had a plan to get out of jail once I got in. I had the privilege of getting arrested and knowing that it wouldn't make a huge mark on my future, unlike so many who are wrongfully arrested and never get out of the [jail] system. I still grapple with that," Dobbelstein said.&lt;br/&gt;First-year Leigh Todd, who provided jail support for those arrested, said that from a practical standpoint, risking arrest was a way of drawing more attention to the protest by allowing them to spend more time on the streets and in the public eye.&lt;br/&gt;"The arrests were a very public way of showing people what we believe in. If we had just marched the streets, it would have just been seen as 'just another march,' and we wanted to spend as much time on the street as possible. The arrests allowed us to do that-to gain people's attention and also the president's attention," Todd said.&lt;br/&gt;Motives for Protest&lt;br/&gt;For those who protested, getting President Obama's attention was key, considering that the final approval for the pipeline's completion lies in his hands.&lt;br/&gt;For many, the president's decision serves as a test of his commitment to environmental issues. Many Gustavus protesters considered their involvement as holding the president-who many of them helped vote into office-accountable for past promises.&lt;br/&gt;"For a lot of us, the first president we voted for was Obama because he said he was going to be a climate leader, not a pipeline president. He campaigned as a climate champion and we were excited about that. This protest is us holding him accountable [for the commitment he made]. We were the young voters who elected him, and we want to see him make the right choice," McDevitt said.&lt;br/&gt;Dobbelstein echoed the political motivations behind her involvement in the protest and added a note of urgency to the impending decision.&lt;br/&gt;"He [the president] has one time to make this decision. I voted him into office twice and I am not okay having [the Keystone XL pipeline] potentially go on my record and not having done anything to stop it," Dobbelstein said.&lt;br/&gt;For other students like Todd, the pipeline would literally hit them where they live. Todd's hometown is York, Nebraska, one of the many communities that would be directly impacted by the construction of the pipeline.&lt;br/&gt;Blake VanOosbree&lt;br/&gt;Todd raised two major issues posed by the pipeline: its potential to drastically compromise the Ogallala Aquifer, a major water source in the region, and the irreparable damage the pipeline poses to farmland.&lt;br/&gt;"If the pipeline were to ever leak, it would really affect my community. [My county] is mostly corn and soybean fields, farmland, and unstable country roads. If there were a leak, not only would it tamper with the Ogallala Aquifer, it would tamper with farmer's fields by passing directly through them. Those fields represent a lot of work, and [the pipeline] would destroy that," Todd said.&lt;br/&gt;Despite the deep commitment to the issue, the forecasts regarding Obama's final decision were mixed.&lt;br/&gt;"I honestly thought [the president] was going to approve the pipeline. So, for a lot of us, [the protest] was our last chance to influence his decision. After this action, however, I feel there's no way he can accept it. Seeing the media attention [the protest] got-with it being the largest youth civil disobedience act in a decade-I really think we sent a  message," McDevitt said.&lt;br/&gt;Todd was less optimistic and said she has tried to avoid thinking about it because of the distress it causes her.&lt;br/&gt;"Right now, I would say probably yes, [the president] will approve it. Money always wins. I haven't thought about it though, because I don't want to think about it. This issue really hits home-the pipeline would destroy everything back home for me," Todd said.&lt;br/&gt;Future Predictions and Plans&lt;br/&gt;Despite mixed predictions of the president's decision, the Gustavus protesters see their trip to the capitol as momentum for rallying future engagement on issues of environmental justice.&lt;br/&gt;"I knew that once we got out there, it would be a huge motivator for us returning to campus. After our return, we all said, 'okay, what are we going to do now?" McDevitt said.&lt;br/&gt;Future initiatives include the Divest Gustavus campaign and halting the exploitation of tar sands in Minnesota.&lt;br/&gt;McDevitt hopes to organize students this spring against the Alberta Clipper, a pipeline that comes through Northern MN, which is in the process of applying for a permit to expand the pipe to a capacity even larger than Keystone XL.&lt;br/&gt;For those involved in the protest, these plans for future engagement represent what they see as a larger call to action for their generation.&lt;br/&gt;"Each generation has its own challenges and each must address them. Our protest says to the world that, right now, climate change is the most threatening thing to our future-this is what our generation's challenge is and we're going to fight it. We want a livable future and we're not going to let corporations make decisions for us," McDevitt said.&lt;br/&gt;Todd echoed the call for continued action.&lt;br/&gt;"We're not just going to protest, we're going to take this further. We're going to divest Gustavus, we're going to keep creating awareness," Todd said.&lt;br/&gt;With less than 60 days of public comment left on the Keystone XL decision, student protesters encourage those who want to voice their opinion to write letters and contact their local state representatives.&lt;br/&gt;Students wanting to get involved with future environmental justice campaigns like Divest Gustavus and the fight against tar sands should contact Divest Gustavus at divestgustavus@gustavus.edu&lt;br/&gt;What is Keystone XL?&lt;br/&gt;Keystone XL is a 1,179-mile pipeline that would carry crude oil from Canada's tar sands, in the province of Alberta, across parts of eight states and over the vast Ogallala Aquifer, to US refineries in Nebraska, Illinois and the Gulf Coast of Texas. (See map to right for proposed route of Keystone XL and existing pipeline).&lt;br/&gt;While operations in the southern leg of Keystone XL has already begun, plans for the northern section are on hold, pending presidential permit.</t>
         </is>
+      </c>
+      <c r="L139" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="140">
@@ -6517,10 +6941,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J140" t="inlineStr">
+      <c r="K140" t="inlineStr">
         <is>
           <t>The proposed Keystone XL Pipeline expansion that would run 1,700 miles between Canada and Texas caused Burlington citizens and student groups to protest its existence last week on a nationwide Day of Action.&lt;br/&gt;350VT and allies such as UVM's Student Climate Culture (SCC) demonstrated their opposition toward the pipeline at the "Draw the Line" events throughout the nation the weekend of Sept. 20.&lt;br/&gt;SCC led a Draw the Line action in South Burlington Sept. 21.&lt;br/&gt;The pipeline, which would bring 700,000 barrels of Canadian oil to American Gulf Coast refineries a day, has mainly caused the stir mainly due to its expected affect on the environment.&lt;br/&gt;The environmental and climate action group, 350VT, wrote a public letter addressed to President Obama urging him to reject the proposed Keystone XL Pipeline. The letter also attempted to dissuade the president from making any deals with Canadian government officials.&lt;br/&gt;According to the letter, "carbon pollution from the tar sands is now projected to be twice as high in 2020 as envisioned under that plan."&lt;br/&gt;"[We inspired] at least 50 folks, including students, Burlington community members, friends and supporters [to join the movement]," said sophomore and SCC club member Brian Thompson.&lt;br/&gt;Thompson was one of at least 10 people who helped organize the Draw the Line event. He said that it "went according to plan" and was a great opportunity to "gain campus momentum."&lt;br/&gt;This day of action began with 10 people gathering in front of the Waterman building on South Prospect St. to speak out against the pipeline. There were also three caricatures that mockingly supported the Keystone project and gave speeches of gratitude on behalf of CEO's of fossil fuel companies.&lt;br/&gt;The satirical supporters then carried a mock pipeline towards Church Street, where a group of environmental activists "Drew the Line" and blocked the pipeline from continuing. The collision of the pipeline into the protesters caused a symbolic oil spill.&lt;br/&gt;Protesters had the opportunity to speak about why they were there and to show their support for the national effort.&lt;br/&gt;"[This was] a chance for groups across the country to come together and have a unified voice," Thompson said.&lt;br/&gt;Activist groups, like SCC, will continue to try to empower other students to join such resistance movements, whether it's regarding fossil fuel divestment or the Keystone XL Pipeline in this case, Thompson said.</t>
         </is>
+      </c>
+      <c r="L140" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -6565,10 +6992,13 @@
           <t>_Other Issue</t>
         </is>
       </c>
-      <c r="J141" t="inlineStr">
+      <c r="K141" t="inlineStr">
         <is>
           <t>On Saturday, Nov. 16, students took part in "Tour de Fracked," a bike ride organized to peacefully protest the Vermont fracked gas pipeline that is proposed to run through Middlebury.&lt;br/&gt;The College has expressed its support for the pipeline, maintaining that it will provide an inexpensive, local form of energy for the school and residents of the town. Many students, however, are fighting the College's stance because they believe the environmental and social side effects of fracking are too high of a price to pay.&lt;br/&gt;Hydraulic fracturing is a process of obtaining natural gas by pressurizing liquids, including harmful chemical substances, to fracture rock below the earth. These chemicals have the potential to leak into groundwater near wells and thus contaminate drinking water.&lt;br/&gt;Rosalie Wright-Lapin '15, one of the organizers of the bike ride, is fearful of the social issues associated with fracking.&lt;br/&gt;"[The] pipeline poses a major ethical paradox," Wright-Lapin said. "Many argue that fracked gas will provide affordable "clean" heat for Vermonters. The importance of making heat affordable for Vermonters is undoubtedly a social justice issue - all humans (especially living in a climate like Vermont's) should have access to affordable heat. However, the mere process of fracking disrupts towns and threatens the health and environment of those communities."&lt;br/&gt;People in the residential communities near a fracking site are often put in compromising situations in which they do not usually have the power to change. This brings into question the ethics of using fracked gas.&lt;br/&gt;Zane Anthony '16.5 is another passionate orchestrator of the Tour de Frack who wants to make the possible implementation of the pipeline, and the controversy over fracking in general, more of a focus on campus. At Powershift, an environmental convention for students across the country that occurred over Fall Break, Anthony and others became motivated to do more related to the climate crisis and environmental justice movements.&lt;br/&gt;Anthony has been working with an organization called the Vermont Public Interest Research Group , which aims to bring the voice of Vermont citizens to public policy debates. Anthony's work with VPIRG helped him gain momentum for spearheading the Tour de Fracked.&lt;br/&gt;The bike ride was meant to be a symbolic showing of "Middlebury activists riding together in solidarity in opposition to the Vermont pipeline." The Tour de Fracked group had advertised for their cause. Other advertisements were more creative, such as a caution-tape patch that served as a statement of solidarity, because caution tape symbolizes the precautionary principle; a huge element in the sustainability movement. Advertisements have included flyers, notification of the local media, a planned conference and over 75 photo petitions of students holding up their statements of disapproval of the pipeline.&lt;br/&gt;Despite their efforts, Anthony feels that environmental activist groups are somewhat lacking on campus. He noted the major focus on the issues of divestment and local food, and the absence of strong activism for any other area.&lt;br/&gt;"[It's] a fallacy [that] Middlebury prides itself on its progressive nature - divestment and [local] food are longer term [issues] but the pipeline could be built in February," said Anthony. "Now is the time, before it is built, for people to see that they are opposed to it."&lt;br/&gt;According to Wright-Lapin, there are many reasons to be opposed to the construction of the pipeline.&lt;br/&gt;"Any organic farms through which the pipeline passes can no longer be organic, thus ruining the living that many hardworking Vermonters have built for themselves and their families," said Wright-Lapin.&lt;br/&gt;"Providing affordable heat for some is only a step towards social justice if it is not ruining the homes of others. Bettering people's lives is only meaningful when it is not harming people on the other end," she said.&lt;br/&gt;These students held Tour de Frack to bring the broad spectrum of environmental issues, and the effects that could result from the pipleine for both the College and the Middlebury community to the attention of the college community at large.</t>
         </is>
+      </c>
+      <c r="L141" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="142">
@@ -6608,10 +7038,13 @@
           <t>Sexual assault/violence, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J142" t="inlineStr">
+      <c r="K142" t="inlineStr">
         <is>
           <t>From student protests of the 1960s to the momentum of modern university protests, colleges have often been watersheds of student-driven activism. Dartmouth is no exception, with students from across campus pushing for change. Most recently, February's "Freedom Budget," a student-authored document of more than 70 demands related to campus diversity and inclusivity, set off a firestorm of discussion.&lt;br/&gt;Campus activism over the "Freedom Budget" continued to flare up in the following weeks, leading to a two-day occupation of College President Phil Hanlon's Parkhurst Hall office in protest of what participants characterized as an inadequate administrative response. There, a group of about 35 students demanded a point-by-point response to the document. In late March, the Dartmouth Coalition for Immigration Reform, Equality and DREAMers hosted an event seeking to eliminate the use of the word "illegal" to refer to undocumented immigrants in the U.S. CoFIRED's co-founder, Oscar Cornejo '17, said that he hopes the new support network for undocumented students will keep the College community conscious of the uncertainty often faced by undocumented students. In its six-month existence, CoFIRED has put on a campaign called "Do I Look Illegal?" in an effort to dispel stereotype of undocumented people. Cornejo said the group has started a discussion with the financial aid and admissions offices on how to communicate with undocumented students. Also, the group helped post relevant information for undocumented students on the admissions website. He said he hoped that more students will get involved in the future. Although contentious and highly visible displays of activism often dominate campus conversation, many forms of student engagement may not be as widely seen.&lt;br/&gt;This past April, students marched across campus as part of the nationwide "Take Back the Night" rally in a protest against sexual assault. These rallies have occurred at Dartmouth since 1991. While some students combat sexual assault and spread awareness through marches, others collaborate with organizations such as the Student and Presidential Committee on Sexual Assault, which drives initiatives to address sexual assault and holds symposiums on the issue. This past year, Esteban Castano '14 and Gillian O'Connell '15 helped launch Improve Dartmouth, an online forum in which Dartmouth students can propose, vote on and discuss ideas that could benefit campus. Student moderators and administrators advocate for promising suggestions. Some recently completed suggestions include modifying the College's dining plans, as well as simpler ideas like adding a new printer location and introducing reusable silverware. One of the Improve Dartmouth's campaigns contributed to the College's decision to establish a zero-tolerance policy for sexual assault. "I think the organizations like the Inter-Community Council, Student Assembly and Improve Dartmouth are very accessible, but the more voices that can be heard the better," Noah Manning '17, a member of Student Assembly and a moderator for Improve Dartmouth, said. Environmental activism is a large part of campus activity, often supported by the Dartmouth Office of Sustainability. Alisa White '17, one of 10 freshmen EcoReps in her class, said she became involved in sustainability almost as soon as she arrived on campus. White praised the Sustainability Office for its efforts to support student passions. "It's a group of people who aren't afraid to carry a spork around sometimes," she said. "We look at sustainability in a lot of different facets, as a way of life, not just a few habits like composting." Divest Dartmouth is another campus environmental activism movement, arguing that supporting companies that produce and profit from fossil fuels is not in the best interest of the College. The ability to defend one's views and arguments is key, White said, especially at a place like Dartmouth. She established a Dartmouth chapter of Rootstrikers, a national nonprofit half-activist, half-think tank group which focuses on ways to reform campaign finance. A large part of the group's work involves reading and researching briefs and court cases in order to support its proposals. "Activism can be polarizing, but if you pick issues that you really care about, it's a great thing to be involved with," White said. Ultimately, she said, being a student activist is about fighting for issues one cares about. Campus centers such as the Office of Pluralism and Leadership are instrumental in supporting student activism, Hui Cheng '16 said. She said she found herself suddenly cognizant of the socioeconomic disparities between her and different classmates her freshman fall. "There's not really a community discussion about class going on, especially how it affects people's lives at Dartmouth," she said. "It's certainly not something most people think about before going to college." Last winter, Cheng served on OPAL's intercommunity council as socioeconomic chair and eventually pitched the idea of a council on socioeconomic awareness. Cheng was hired as a socioeconomic class intern at OPAL to turn her idea into a reality. The council, which launched last winter, held a "Hidden Costs of Dartmouth" panel during Dimensions and a similar event for the summer 2014 Dartmouth Bound program. The panel highlighted students' experiences with class at Dartmouth and covered various resources available to students. "I feel like campus activism has only grown stronger as my time here progressed," Cheng said. She said she considers OPAL to be a safe space where student activists can find support. Center for Gender and Student Engagement also provides a comfortable space where students passionate about social justice can connect, said Jessica King Fredel '17. During her freshman winter, King Fredel co-directed and performed in the student-run production "Voices" as part of V-February, which was sponsored in part by the CGSE. The show focuses on the different experiences of Dartmouth women. "Voices," which touched on topics including fraternity culture, sexual assault and body image, was performed to an audience of more than 600 people in Spaulding Auditorium. The show seemed to expose people to ideas of inequality they had never before considered, King Fredel said, adding that she received numerous questions about feminism and intersectionality in the weeks following the show. "I consistently feel like this kind of performance is a great way to open a dialogue in a community without making any specific group feel attacked," she said. "It is simply a sharing of experiences." In the end, activism on campus is primarily by and for the students, Gavin Huang '14 said. Huang joined dialogue groups and volunteer programs at the Tucker Foundation as a freshman, continuing through senior year with his work on the "Freedom Budget." "These are opportunities that you create," he said. "A lot of the groups, organizations and services on campus were a result of student demand themselves." Although the aforementioned examples of activism are all important in their own ways, they only capture a slice of a constantly evolving campus, where visible change each year. "I am sure that if a member of the Class of 2018 wants to make a difference, there is a way for them to do so," Manning said. Gavin Huang is a former member of The Dartmouth Senior Staff.</t>
         </is>
+      </c>
+      <c r="L142" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="143">
@@ -6651,10 +7084,13 @@
           <t>Sexual assault/violence, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J143" t="inlineStr">
+      <c r="K143" t="inlineStr">
         <is>
           <t>From student protests of the 1960s to the momentum of modern university protests, colleges have often been watersheds of student-driven activism. Dartmouth is no exception, with students from across campus pushing for change.&lt;br/&gt;Most recently, February's "Freedom Budget," a student-authored document of more than 70 demands related to campus diversity and inclusivity, set off a firestorm of discussion.&lt;br/&gt;Campus activism over the "Freedom Budget" continued to flare up in the following weeks, leading to a two-day occupation of College President Phil Hanlon's Parkhurst Hall office in protest of what participants characterized as an inadequate administrative response. There, a group of about 35 students demanded a point-by-point response to the document.&lt;br/&gt;In late March, the Dartmouth Coalition for Immigration Reform, Equality and DREAMers hosted an event seeking to eliminate the use of the word "illegal" to refer to undocumented immigrants in the U.S.&lt;br/&gt;CoFIRED's co-founder, Oscar Cornejo '17, said that he hopes the new support network for undocumented students will keep the College community conscious of the uncertainty often faced by undocumented students.&lt;br/&gt;In its six-month existence, CoFIRED has put on a campaign called "Do I Look Illegal?" in an effort to dispel stereotype of undocumented people. Cornejo said the group has started a discussion with the financial aid and admissions offices on how to communicate with undocumented students.&lt;br/&gt;Also, the group helped post relevant information for undocumented students on the admissions website. He said he hoped that more students will get involved in the future.&lt;br/&gt;Although contentious and highly visible displays of activism often dominate campus conversation, many forms of student engagement may not be as widely seen.&lt;br/&gt;This past April, students marched across campus as part of the nationwide "Take Back the Night" rally in a protest against sexual assault. These rallies have occurred at Dartmouth since 1991.&lt;br/&gt;While some students combat sexual assault and spread awareness through marches, others collaborate with organizations such as the Student and Presidential Committee on Sexual Assault, which drives initiatives to address sexual assault and holds symposiums on the issue.&lt;br/&gt;This past year, Esteban Castano '14 and Gillian O'Connell '15 helped launch Improve Dartmouth, an online forum in which Dartmouth students can propose, vote on and discuss ideas that could benefit campus. Student moderators and administrators advocate for promising suggestions.&lt;br/&gt;Some recently completed suggestions include modifying the College's dining plans, as well as simpler ideas like adding a new printer location and introducing reusable silverware. One of the Improve Dartmouth's campaigns contributed to the College's decision to establish a zero-tolerance policy for sexual assault.&lt;br/&gt;"I think the organizations like the Inter-Community Council, Student Assembly and Improve Dartmouth are very accessible, but the more voices that can be heard the better," Noah Manning '17, a member of Student Assembly and a moderator for Improve Dartmouth, said.&lt;br/&gt;Environmental activism is a large part of campus activity, often supported by the Dartmouth Office of Sustainability.&lt;br/&gt;Alisa White '17, one of 10 freshmen EcoReps in her class, said she became involved in sustainability almost as soon as she arrived on campus.&lt;br/&gt;White praised the Sustainability Office for its efforts to support student passions.&lt;br/&gt;"It's a group of people who aren't afraid to carry a spork around sometimes," she said. "We look at sustainability in a lot of different facets, as a way of life, not just a few habits like composting."&lt;br/&gt;Divest Dartmouth is another campus environmental activism movement, arguing that supporting companies that produce and profit from fossil fuels is not in the best interest of the College.&lt;br/&gt;The ability to defend one's views and arguments is key, White said, especially at a place like Dartmouth.&lt;br/&gt;She established a Dartmouth chapter of Rootstrikers, a national nonprofit half-activist, half-think tank group which focuses on ways to reform campaign finance. A large part of the group's work involves reading and researching briefs and court cases in order to support its proposals.&lt;br/&gt;"Activism can be polarizing, but if you pick issues that you really care about, it's a great thing to be involved with," White said.&lt;br/&gt;Ultimately, she said, being a student activist is about fighting for issues one cares about.&lt;br/&gt;Campus centers such as the Office of Pluralism and Leadership are instrumental in supporting student activism, Hui Cheng '16 said.&lt;br/&gt;She said she found herself suddenly cognizant of the socioeconomic disparities between her and different classmates her freshman fall.&lt;br/&gt;"There's not really a community discussion about class going on, especially how it affects people's lives at Dartmouth," she said. "It's certainly not something most people think about before going to college."&lt;br/&gt;Last winter, Cheng served on OPAL's intercommunity council as socioeconomic chair and eventually pitched the idea of a council on socioeconomic awareness. Cheng was hired as a socioeconomic class intern at OPAL to turn her idea into a reality.&lt;br/&gt;The council, which launched last winter, held a "Hidden Costs of Dartmouth" panel during Dimensions and a similar event for the summer 2014 Dartmouth Bound program. The panel highlighted students' experiences with class at Dartmouth and covered various resources available to students.&lt;br/&gt;"I feel like campus activism has only grown stronger as my time here progressed," Cheng said.&lt;br/&gt;She said she considers OPAL to be a safe space where student activists can find support.&lt;br/&gt;Center for Gender and Student Engagement also provides a comfortable space where students passionate about social justice can connect, said Jessica King Fredel '17.&lt;br/&gt;During her freshman winter, King Fredel co-directed and performed in the student-run production "Voices" as part of V-February, which was sponsored in part by the CGSE. The show focuses on the different experiences of Dartmouth women.&lt;br/&gt;"Voices," which touched on topics including fraternity culture, sexual assault and body image, was performed to an audience of more than 600 people in Spaulding Auditorium.&lt;br/&gt;The show seemed to expose people to ideas of inequality they had never before considered, King Fredel said, adding that she received numerous questions about feminism and intersectionality in the weeks following the show.&lt;br/&gt;"I consistently feel like this kind of performance is a great way to open a dialogue in a community without making any specific group feel attacked," she said. "It is simply a sharing of experiences."&lt;br/&gt;In the end, activism on campus is primarily by and for the students, Gavin Huang '14 said. Huang joined dialogue groups and volunteer programs at the Tucker Foundation as a freshman, continuing through senior year with his work on the "Freedom Budget."&lt;br/&gt;"These are opportunities that you create," he said. "A lot of the groups, organizations and services on campus were a result of student demand themselves."&lt;br/&gt;Although the aforementioned examples of activism are all important in their own ways, they only capture a slice of a constantly evolving campus, where visible change each year.&lt;br/&gt;"I am sure that if a member of the Class of 2018 wants to make a difference, there is a way for them to do so," Manning said.&lt;br/&gt;Gavin Huang is a former member of The Dartmouth Senior Staff.</t>
         </is>
+      </c>
+      <c r="L143" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="144">
@@ -6699,10 +7135,13 @@
           <t>Anti-racism, Campus climate, Immigration (For)</t>
         </is>
       </c>
-      <c r="J144" t="inlineStr">
+      <c r="K144" t="inlineStr">
         <is>
           <t>In recent months, colleges across the country have seen a spate of demonstrations regarding issues of identity, with students demanding greater inclusivity on their campuses. Many resemble Dartmouth's April "Freedom Budget" protests, when over a dozen students occupied College President Phil Hanlon's office for two days, demanding a point-by-point response to a list of over 70 demands regarding issues of diversity.&lt;br/&gt;In the last year, students at Princeton University, Harvard University, Oberlin College, Mills College, University of Michigan, City University of New York, Mount Holyoke College and University of California at Los Angeles, among others, have initiated protests concerning similar issues. Melissa Padilla '16, who was involved in the "Freedom Budget" protest, said she communicated with her friends who were involved with similar protests at other schools, including New York University and University of Texas at Austin, during the construction of the "Freedom Budget" and the sit-in. Other Dartmouth activists spoke with friends on various campuses as well, she said. The protest at Dartmouth, she said, was not a reaction to movements at other schools but a response to discrimination at the College. "A lot of universities are looking to be more inclusive but are acting very unlike their statements," Padilla said. "There's a big gap between their mission statements and the actual reality of being a student on campus." Across the country students are demanding that administrators make structural changes to better support all students. On April 7, a coalition of students at Oberlin College, in Ohio, wrote an open letter in support of the sit-in at Dartmouth. The letter was posted in the opinion section of "Fearless and Loathing," an independent website run by Oberlin students. "We recognize the actions of our fellow students at Dartmouth as courageous, necessary steps that must be taken if institutions such as ours - ones that advertise themselves on falsified notions of diversity, inclusivity and dignity - continue to treat 'dialogue' as a synonym for structural violence," the letter states. Oberlin junior Ana Robelo, who has been a member of the coalition since its founding last fall, said several communities on Oberlin's campus worked together to compile a list of demands for their school's administration. The demands included increased administrative transparency, divestment from companies that support Israeli occupation of Palestine and scholarship funding for undocumented students. On Oct. 10, a group of Oberlin students took over the Board of Trustees meeting and discussed demands. Oberlin senior Alice Beecher said that hundreds of students dressed in red as a symbol of solidarity. Robelo said she sensed strong and immediate backlash during the meeting. Student reactions, however, were generally supportive, though some disagreed with the group's tactics and the demand to divest from companies that support Israel, Beecher said. Since the board meeting, Beecher said that some smaller communities within the coalition have met with administrators to advance individual demands. Beecher said students joined together to create a replica of the wall separating Gaza and Israel, painting it with different representations of borders in society. Students then placed pieces of the wall in front of Oberlin's main library alongside an audiotape playing students' personal stories of division within the Oberlin community, she said. Members of the coalition also stood outside a second trustee meeting in December while holding pieces of the reconstructed wall, Beecher said. Robelo said the coalition formed in part as a result of events that took place at Oberlin last spring, including the appearance of someone dressed in a Ku Klux Klan robe and racist graffiti around campus. The coalition, Beecher said, was reacting to what they perceived as the administration's non-response. On May 1, approximately 10 students sat outside a Princeton University student center wearing black shirts and white opera masks, playing a recording of their manifesto on a boombox, Princeton junior Katie Horvath said. Passersby were offered fliers outlining the group's 10 demands for change at the university, including revised mental health policies, divestment and a call for more gender neutral housing options, among others. Horvath, who participated in the demonstration but emphasized that she did not organize it, said although the protest stemmed from a queer activism movement, its demands were "intersectional" and addressed a range of issues beyond gender.&lt;br/&gt;Though the Princeton group, called Praxis Axis, placed a stack of masks next to their demonstration as an invitation for passersby to join in, few people followed suit since few knew in advance or had clothing that matched that of the protesters, which Horvarth said became a "barrier to entry." Horvath said that the Praxis Axis demands felt similar in nature to demands voiced by the "Freedom Budget," as both were intersectional efforts to address issues centered on identity. Although Praxis Axis members did not work directly with Dartmouth students to compile their demands, Horvarth said she believed demonstrators at various schools would benefit from joining forces. For those at institutions like Princeton, which tend to have less widespread student activism than more urban institutions, engaging with like-minded students at other colleges can contribute to a stronger "protest culture," she said. On April 2, Princeton freshman Tal Fortgang published an essay titled "Checking My Privilege: Character as the Basis of Privilege" in The Tory, a conservative publication at the school. The piece, in which Fortgang refused to apologize for having privilege and cited examples of difficulties faced by his family, prompted much discussion on the Princeton campus, Horvath said. "It's been helpful," she said, "in that it has made people concerned and aware who would otherwise be likely to dismiss the demands of a group like the protest group on May Day as unnecessary or absurd or over the top." Mount Holyoke, an all-women's college in Massachusetts, is in the midst of a movement that aims to address discrimination and increase student involvement in college policy, said junior Melanie Wilkerson, an active participant in the movement. The movement, known as "MoHonest," began after Mount Holyoke student Maya Wegerif, 21, wrote a blog post alleging discrimination by campus police when she was arrested following an alcohol-related incident. Wilkerson said that many students of color at Mount Holyoke related to Wegerif's experience, and the incident sparked much discussion about discrimination and the power of campus police. "We began to form an entity that wanted to specifically represent students of color on campus," she said. "And even more broadly, those who have faced discrimination on campus or were allowed to suffer discrimination and not receive adequate administrative support." Members presented a formal list of demands to the administration in April, Wilkerson said, and are currently at a "standstill." The group's demands include encouraging more active student participation in campus policy and decisions, increasing institutional support for first-generation college students, updating the policy for reporting grievances and creating educational workshops for students, faculty, staff and campus police. "We're still negotiating, but we're a little disappointed with the administration," Wilkerson said. Wilkerson said that members of the "MoHonest" movement were aware of the "Freedom Budget" and considered the Dartmouth activists' tactics when brainstorming. The sit-in at Dartmouth, she said, was "successful in its visibility." Though "MoHonest" protesters considered a sit-in, Wilkerson said they decided against it because some members felt that - unlike at Dartmouth - not enough time had elapsed since the demands had been voiced. Wilkerson said the "MoHonest" movement reflects a nationwide trend of students becoming more vocal about administrators' lack of support. "MoHonest" has supported related movements at other institutions, including Vassar College and Bryn Mawr College, she said. "I feel like the trend is catching on because people across the country are really starting to acknowledge the kind of power young people have," she said. Though "MoHonest" faced some opposition from students, Wilkerson said it has found a broad base of support among faculty and alumni. "In my three years at Mount Holyoke, I have witnessed people go through some pretty intense stuff in terms of discrimination," Wilkerson said. "Even in a very liberal, diversity-agenda-pushing institution like Mount Holyoke, there are still fundamental flaws and issues that need to be addressed." Two student movements have recently arisen at Harvard University, both aiming to increase diversity among faculty, staff and administrators and to improve resources for more diverse programming, Harvard senior Terrance Moore said. The first of these movements, a photography campaign titled "I, Too, Am Harvard," launched on Tumblr in early March. The pictures show black students holding signs with examples of racial prejudice they have experienced at Harvard, accompanied by the slogan. Once the campaign gained attention, students involved began researching other movements to see how they were successful in creating institutional change, Moore said. The second student movement, known as "The Diversity Report," spun out of the "I, Too, Am Harvard" campaign, Moore said. Students involved in "The Diversity Report" wrote a list of demands and are currently working with specific administrators to achieve them, Moore said. After contacting them, the students decided to fill out report cards evaluating administrators to hold them accountable.</t>
         </is>
+      </c>
+      <c r="L144" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -6747,10 +7186,13 @@
           <t>Anti-racism, Campus climate, Immigration (For)</t>
         </is>
       </c>
-      <c r="J145" t="inlineStr">
+      <c r="K145" t="inlineStr">
         <is>
           <t>From student protests of the 1960s to the momentum of modern university protests, colleges have often been watersheds of student-driven activism. Dartmouth is no exception, with students from across campus pushing for change. Most recently, February's "Freedom Budget," a student-authored document of more than 70 demands related to campus diversity and inclusivity, set off a firestorm of discussion.&lt;br/&gt;Campus activism over the "Freedom Budget" continued to flare up in the following weeks, leading to a two-day occupation of College President Phil Hanlon's Parkhurst Hall office in protest of what participants characterized as an inadequate administrative response. There, a group of about 35 students demanded a point-by-point response to the document. In late March, the Dartmouth Coalition for Immigration Reform, Equality and DREAMers hosted an event seeking to eliminate the use of the word "illegal" to refer to undocumented immigrants in the U.S. CoFIRED's co-founder, Oscar Cornejo '17, said that he hopes the new support network for undocumented students will keep the College community conscious of the uncertainty often faced by undocumented students. In its six-month existence, CoFIRED has put on a campaign called "Do I Look Illegal?" in an effort to dispel stereotype of undocumented people. Cornejo said the group has started a discussion with the financial aid and admissions offices on how to communicate with undocumented students. Also, the group helped post relevant information for undocumented students on the admissions website. He said he hoped that more students will get involved in the future. Although contentious and highly visible displays of activism often dominate campus conversation, many forms of student engagement may not be as widely seen.&lt;br/&gt;This past April, students marched across campus as part of the nationwide "Take Back the Night" rally in a protest against sexual assault. These rallies have occurred at Dartmouth since 1991. While some students combat sexual assault and spread awareness through marches, others collaborate with organizations such as the Student and Presidential Committee on Sexual Assault, which drives initiatives to address sexual assault and holds symposiums on the issue. This past year, Esteban Castano '14 and Gillian O'Connell '15 helped launch Improve Dartmouth, an online forum in which Dartmouth students can propose, vote on and discuss ideas that could benefit campus. Student moderators and administrators advocate for promising suggestions. Some recently completed suggestions include modifying the College's dining plans, as well as simpler ideas like adding a new printer location and introducing reusable silverware. One of the Improve Dartmouth's campaigns contributed to the College's decision to establish a zero-tolerance policy for sexual assault. "I think the organizations like the Inter-Community Council, Student Assembly and Improve Dartmouth are very accessible, but the more voices that can be heard the better," Noah Manning '17, a member of Student Assembly and a moderator for Improve Dartmouth, said. Environmental activism is a large part of campus activity, often supported by the Dartmouth Office of Sustainability. Alisa White '17, one of 10 freshmen EcoReps in her class, said she became involved in sustainability almost as soon as she arrived on campus. White praised the Sustainability Office for its efforts to support student passions. "It's a group of people who aren't afraid to carry a spork around sometimes," she said. "We look at sustainability in a lot of different facets, as a way of life, not just a few habits like composting." Divest Dartmouth is another campus environmental activism movement, arguing that supporting companies that produce and profit from fossil fuels is not in the best interest of the College. The ability to defend one's views and arguments is key, White said, especially at a place like Dartmouth. She established a Dartmouth chapter of Rootstrikers, a national nonprofit half-activist, half-think tank group which focuses on ways to reform campaign finance. A large part of the group's work involves reading and researching briefs and court cases in order to support its proposals. "Activism can be polarizing, but if you pick issues that you really care about, it's a great thing to be involved with," White said. Ultimately, she said, being a student activist is about fighting for issues one cares about. Campus centers such as the Office of Pluralism and Leadership are instrumental in supporting student activism, Hui Cheng '16 said. She said she found herself suddenly cognizant of the socioeconomic disparities between her and different classmates her freshman fall. "There's not really a community discussion about class going on, especially how it affects people's lives at Dartmouth," she said. "It's certainly not something most people think about before going to college." Last winter, Cheng served on OPAL's intercommunity council as socioeconomic chair and eventually pitched the idea of a council on socioeconomic awareness. Cheng was hired as a socioeconomic class intern at OPAL to turn her idea into a reality. The council, which launched last winter, held a "Hidden Costs of Dartmouth" panel during Dimensions and a similar event for the summer 2014 Dartmouth Bound program. The panel highlighted students' experiences with class at Dartmouth and covered various resources available to students. "I feel like campus activism has only grown stronger as my time here progressed," Cheng said. She said she considers OPAL to be a safe space where student activists can find support. Center for Gender and Student Engagement also provides a comfortable space where students passionate about social justice can connect, said Jessica King Fredel '17. During her freshman winter, King Fredel co-directed and performed in the student-run production "Voices" as part of V-February, which was sponsored in part by the CGSE. The show focuses on the different experiences of Dartmouth women. "Voices," which touched on topics including fraternity culture, sexual assault and body image, was performed to an audience of more than 600 people in Spaulding Auditorium. The show seemed to expose people to ideas of inequality they had never before considered, King Fredel said, adding that she received numerous questions about feminism and intersectionality in the weeks following the show. "I consistently feel like this kind of performance is a great way to open a dialogue in a community without making any specific group feel attacked," she said. "It is simply a sharing of experiences." In the end, activism on campus is primarily by and for the students, Gavin Huang '14 said. Huang joined dialogue groups and volunteer programs at the Tucker Foundation as a freshman, continuing through senior year with his work on the "Freedom Budget." "These are opportunities that you create," he said. "A lot of the groups, organizations and services on campus were a result of student demand themselves." Although the aforementioned examples of activism are all important in their own ways, they only capture a slice of a constantly evolving campus, where visible change each year. "I am sure that if a member of the Class of 2018 wants to make a difference, there is a way for them to do so," Manning said. Gavin Huang is a former member of The Dartmouth Senior Staff.</t>
         </is>
+      </c>
+      <c r="L145" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -6795,10 +7237,13 @@
           <t>Anti-racism, Campus climate, Immigration (For)</t>
         </is>
       </c>
-      <c r="J146" t="inlineStr">
+      <c r="K146" t="inlineStr">
         <is>
           <t>From student protests of the 1960s to the momentum of modern university protests, colleges have often been watersheds of student-driven activism. Dartmouth is no exception, with students from across campus pushing for change.&lt;br/&gt;Most recently, February's "Freedom Budget," a student-authored document of more than 70 demands related to campus diversity and inclusivity, set off a firestorm of discussion.&lt;br/&gt;Campus activism over the "Freedom Budget" continued to flare up in the following weeks, leading to a two-day occupation of College President Phil Hanlon's Parkhurst Hall office in protest of what participants characterized as an inadequate administrative response. There, a group of about 35 students demanded a point-by-point response to the document.&lt;br/&gt;In late March, the Dartmouth Coalition for Immigration Reform, Equality and DREAMers hosted an event seeking to eliminate the use of the word "illegal" to refer to undocumented immigrants in the U.S.&lt;br/&gt;CoFIRED's co-founder, Oscar Cornejo '17, said that he hopes the new support network for undocumented students will keep the College community conscious of the uncertainty often faced by undocumented students.&lt;br/&gt;In its six-month existence, CoFIRED has put on a campaign called "Do I Look Illegal?" in an effort to dispel stereotype of undocumented people. Cornejo said the group has started a discussion with the financial aid and admissions offices on how to communicate with undocumented students.&lt;br/&gt;Also, the group helped post relevant information for undocumented students on the admissions website. He said he hoped that more students will get involved in the future.&lt;br/&gt;Although contentious and highly visible displays of activism often dominate campus conversation, many forms of student engagement may not be as widely seen.&lt;br/&gt;This past April, students marched across campus as part of the nationwide "Take Back the Night" rally in a protest against sexual assault. These rallies have occurred at Dartmouth since 1991.&lt;br/&gt;While some students combat sexual assault and spread awareness through marches, others collaborate with organizations such as the Student and Presidential Committee on Sexual Assault, which drives initiatives to address sexual assault and holds symposiums on the issue.&lt;br/&gt;This past year, Esteban Castano '14 and Gillian O'Connell '15 helped launch Improve Dartmouth, an online forum in which Dartmouth students can propose, vote on and discuss ideas that could benefit campus. Student moderators and administrators advocate for promising suggestions.&lt;br/&gt;Some recently completed suggestions include modifying the College's dining plans, as well as simpler ideas like adding a new printer location and introducing reusable silverware. One of the Improve Dartmouth's campaigns contributed to the College's decision to establish a zero-tolerance policy for sexual assault.&lt;br/&gt;"I think the organizations like the Inter-Community Council, Student Assembly and Improve Dartmouth are very accessible, but the more voices that can be heard the better," Noah Manning '17, a member of Student Assembly and a moderator for Improve Dartmouth, said.&lt;br/&gt;Environmental activism is a large part of campus activity, often supported by the Dartmouth Office of Sustainability.&lt;br/&gt;Alisa White '17, one of 10 freshmen EcoReps in her class, said she became involved in sustainability almost as soon as she arrived on campus.&lt;br/&gt;White praised the Sustainability Office for its efforts to support student passions.&lt;br/&gt;"It's a group of people who aren't afraid to carry a spork around sometimes," she said. "We look at sustainability in a lot of different facets, as a way of life, not just a few habits like composting."&lt;br/&gt;Divest Dartmouth is another campus environmental activism movement, arguing that supporting companies that produce and profit from fossil fuels is not in the best interest of the College.&lt;br/&gt;The ability to defend one's views and arguments is key, White said, especially at a place like Dartmouth.&lt;br/&gt;She established a Dartmouth chapter of Rootstrikers, a national nonprofit half-activist, half-think tank group which focuses on ways to reform campaign finance. A large part of the group's work involves reading and researching briefs and court cases in order to support its proposals.&lt;br/&gt;"Activism can be polarizing, but if you pick issues that you really care about, it's a great thing to be involved with," White said.&lt;br/&gt;Ultimately, she said, being a student activist is about fighting for issues one cares about.&lt;br/&gt;Campus centers such as the Office of Pluralism and Leadership are instrumental in supporting student activism, Hui Cheng '16 said.&lt;br/&gt;She said she found herself suddenly cognizant of the socioeconomic disparities between her and different classmates her freshman fall.&lt;br/&gt;"There's not really a community discussion about class going on, especially how it affects people's lives at Dartmouth," she said. "It's certainly not something most people think about before going to college."&lt;br/&gt;Last winter, Cheng served on OPAL's intercommunity council as socioeconomic chair and eventually pitched the idea of a council on socioeconomic awareness. Cheng was hired as a socioeconomic class intern at OPAL to turn her idea into a reality.&lt;br/&gt;The council, which launched last winter, held a "Hidden Costs of Dartmouth" panel during Dimensions and a similar event for the summer 2014 Dartmouth Bound program. The panel highlighted students' experiences with class at Dartmouth and covered various resources available to students.&lt;br/&gt;"I feel like campus activism has only grown stronger as my time here progressed," Cheng said.&lt;br/&gt;She said she considers OPAL to be a safe space where student activists can find support.&lt;br/&gt;Center for Gender and Student Engagement also provides a comfortable space where students passionate about social justice can connect, said Jessica King Fredel '17.&lt;br/&gt;During her freshman winter, King Fredel co-directed and performed in the student-run production "Voices" as part of V-February, which was sponsored in part by the CGSE. The show focuses on the different experiences of Dartmouth women.&lt;br/&gt;"Voices," which touched on topics including fraternity culture, sexual assault and body image, was performed to an audience of more than 600 people in Spaulding Auditorium.&lt;br/&gt;The show seemed to expose people to ideas of inequality they had never before considered, King Fredel said, adding that she received numerous questions about feminism and intersectionality in the weeks following the show.&lt;br/&gt;"I consistently feel like this kind of performance is a great way to open a dialogue in a community without making any specific group feel attacked," she said. "It is simply a sharing of experiences."&lt;br/&gt;In the end, activism on campus is primarily by and for the students, Gavin Huang '14 said. Huang joined dialogue groups and volunteer programs at the Tucker Foundation as a freshman, continuing through senior year with his work on the "Freedom Budget."&lt;br/&gt;"These are opportunities that you create," he said. "A lot of the groups, organizations and services on campus were a result of student demand themselves."&lt;br/&gt;Although the aforementioned examples of activism are all important in their own ways, they only capture a slice of a constantly evolving campus, where visible change each year.&lt;br/&gt;"I am sure that if a member of the Class of 2018 wants to make a difference, there is a way for them to do so," Manning said.&lt;br/&gt;Gavin Huang is a former member of The Dartmouth Senior Staff.</t>
         </is>
+      </c>
+      <c r="L146" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="147">
@@ -6838,10 +7283,13 @@
           <t>University governance, admin, policies, programs, curriculum, Campus climate, Anti-racism</t>
         </is>
       </c>
-      <c r="J147" t="inlineStr">
+      <c r="K147" t="inlineStr">
         <is>
           <t>In recent months, colleges across the country have seen a spate of demonstrations regarding issues of identity, with students demanding greater inclusivity on their campuses. Many resemble Dartmouth's April "Freedom Budget" protests, when over a dozen students occupied College President Phil Hanlon's office for two days, demanding a point-by-point response to a list of over 70 demands regarding issues of diversity.&lt;br/&gt;In the last year, students at Princeton University, Harvard University, Oberlin College, Mills College, University of Michigan, City University of New York, Mount Holyoke College and University of California at Los Angeles, among others, have initiated protests concerning similar issues. Melissa Padilla '16, who was involved in the "Freedom Budget" protest, said she communicated with her friends who were involved with similar protests at other schools, including New York University and University of Texas at Austin, during the construction of the "Freedom Budget" and the sit-in. Other Dartmouth activists spoke with friends on various campuses as well, she said. The protest at Dartmouth, she said, was not a reaction to movements at other schools but a response to discrimination at the College. "A lot of universities are looking to be more inclusive but are acting very unlike their statements," Padilla said. "There's a big gap between their mission statements and the actual reality of being a student on campus." Across the country students are demanding that administrators make structural changes to better support all students. On April 7, a coalition of students at Oberlin College, in Ohio, wrote an open letter in support of the sit-in at Dartmouth. The letter was posted in the opinion section of "Fearless and Loathing," an independent website run by Oberlin students. "We recognize the actions of our fellow students at Dartmouth as courageous, necessary steps that must be taken if institutions such as ours - ones that advertise themselves on falsified notions of diversity, inclusivity and dignity - continue to treat 'dialogue' as a synonym for structural violence," the letter states. Oberlin junior Ana Robelo, who has been a member of the coalition since its founding last fall, said several communities on Oberlin's campus worked together to compile a list of demands for their school's administration. The demands included increased administrative transparency, divestment from companies that support Israeli occupation of Palestine and scholarship funding for undocumented students. On Oct. 10, a group of Oberlin students took over the Board of Trustees meeting and discussed demands. Oberlin senior Alice Beecher said that hundreds of students dressed in red as a symbol of solidarity. Robelo said she sensed strong and immediate backlash during the meeting. Student reactions, however, were generally supportive, though some disagreed with the group's tactics and the demand to divest from companies that support Israel, Beecher said. Since the board meeting, Beecher said that some smaller communities within the coalition have met with administrators to advance individual demands. Beecher said students joined together to create a replica of the wall separating Gaza and Israel, painting it with different representations of borders in society. Students then placed pieces of the wall in front of Oberlin's main library alongside an audiotape playing students' personal stories of division within the Oberlin community, she said. Members of the coalition also stood outside a second trustee meeting in December while holding pieces of the reconstructed wall, Beecher said. Robelo said the coalition formed in part as a result of events that took place at Oberlin last spring, including the appearance of someone dressed in a Ku Klux Klan robe and racist graffiti around campus. The coalition, Beecher said, was reacting to what they perceived as the administration's non-response. On May 1, approximately 10 students sat outside a Princeton University student center wearing black shirts and white opera masks, playing a recording of their manifesto on a boombox, Princeton junior Katie Horvath said. Passersby were offered fliers outlining the group's 10 demands for change at the university, including revised mental health policies, divestment and a call for more gender neutral housing options, among others. Horvath, who participated in the demonstration but emphasized that she did not organize it, said although the protest stemmed from a queer activism movement, its demands were "intersectional" and addressed a range of issues beyond gender.&lt;br/&gt;Though the Princeton group, called Praxis Axis, placed a stack of masks next to their demonstration as an invitation for passersby to join in, few people followed suit since few knew in advance or had clothing that matched that of the protesters, which Horvarth said became a "barrier to entry." Horvath said that the Praxis Axis demands felt similar in nature to demands voiced by the "Freedom Budget," as both were intersectional efforts to address issues centered on identity. Although Praxis Axis members did not work directly with Dartmouth students to compile their demands, Horvarth said she believed demonstrators at various schools would benefit from joining forces. For those at institutions like Princeton, which tend to have less widespread student activism than more urban institutions, engaging with like-minded students at other colleges can contribute to a stronger "protest culture," she said. On April 2, Princeton freshman Tal Fortgang published an essay titled "Checking My Privilege: Character as the Basis of Privilege" in The Tory, a conservative publication at the school. The piece, in which Fortgang refused to apologize for having privilege and cited examples of difficulties faced by his family, prompted much discussion on the Princeton campus, Horvath said. "It's been helpful," she said, "in that it has made people concerned and aware who would otherwise be likely to dismiss the demands of a group like the protest group on May Day as unnecessary or absurd or over the top." Mount Holyoke, an all-women's college in Massachusetts, is in the midst of a movement that aims to address discrimination and increase student involvement in college policy, said junior Melanie Wilkerson, an active participant in the movement. The movement, known as "MoHonest," began after Mount Holyoke student Maya Wegerif, 21, wrote a blog post alleging discrimination by campus police when she was arrested following an alcohol-related incident. Wilkerson said that many students of color at Mount Holyoke related to Wegerif's experience, and the incident sparked much discussion about discrimination and the power of campus police. "We began to form an entity that wanted to specifically represent students of color on campus," she said. "And even more broadly, those who have faced discrimination on campus or were allowed to suffer discrimination and not receive adequate administrative support." Members presented a formal list of demands to the administration in April, Wilkerson said, and are currently at a "standstill." The group's demands include encouraging more active student participation in campus policy and decisions, increasing institutional support for first-generation college students, updating the policy for reporting grievances and creating educational workshops for students, faculty, staff and campus police. "We're still negotiating, but we're a little disappointed with the administration," Wilkerson said. Wilkerson said that members of the "MoHonest" movement were aware of the "Freedom Budget" and considered the Dartmouth activists' tactics when brainstorming. The sit-in at Dartmouth, she said, was "successful in its visibility." Though "MoHonest" protesters considered a sit-in, Wilkerson said they decided against it because some members felt that - unlike at Dartmouth - not enough time had elapsed since the demands had been voiced. Wilkerson said the "MoHonest" movement reflects a nationwide trend of students becoming more vocal about administrators' lack of support. "MoHonest" has supported related movements at other institutions, including Vassar College and Bryn Mawr College, she said. "I feel like the trend is catching on because people across the country are really starting to acknowledge the kind of power young people have," she said. Though "MoHonest" faced some opposition from students, Wilkerson said it has found a broad base of support among faculty and alumni. "In my three years at Mount Holyoke, I have witnessed people go through some pretty intense stuff in terms of discrimination," Wilkerson said. "Even in a very liberal, diversity-agenda-pushing institution like Mount Holyoke, there are still fundamental flaws and issues that need to be addressed." Two student movements have recently arisen at Harvard University, both aiming to increase diversity among faculty, staff and administrators and to improve resources for more diverse programming, Harvard senior Terrance Moore said. The first of these movements, a photography campaign titled "I, Too, Am Harvard," launched on Tumblr in early March. The pictures show black students holding signs with examples of racial prejudice they have experienced at Harvard, accompanied by the slogan. Once the campaign gained attention, students involved began researching other movements to see how they were successful in creating institutional change, Moore said. The second student movement, known as "The Diversity Report," spun out of the "I, Too, Am Harvard" campaign, Moore said. Students involved in "The Diversity Report" wrote a list of demands and are currently working with specific administrators to achieve them, Moore said. After contacting them, the students decided to fill out report cards evaluating administrators to hold them accountable.</t>
         </is>
+      </c>
+      <c r="L147" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="148">
@@ -6881,10 +7329,13 @@
           <t>Immigration (For), University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J148" t="inlineStr">
+      <c r="K148" t="inlineStr">
         <is>
           <t>From student protests of the 1960s to the momentum of modern university protests, colleges have often been watersheds of student-driven activism. Dartmouth is no exception, with students from across campus pushing for change. Most recently, February's "Freedom Budget," a student-authored document of more than 70 demands related to campus diversity and inclusivity, set off a firestorm of discussion.&lt;br/&gt;Campus activism over the "Freedom Budget" continued to flare up in the following weeks, leading to a two-day occupation of College President Phil Hanlon's Parkhurst Hall office in protest of what participants characterized as an inadequate administrative response. There, a group of about 35 students demanded a point-by-point response to the document. In late March, the Dartmouth Coalition for Immigration Reform, Equality and DREAMers hosted an event seeking to eliminate the use of the word "illegal" to refer to undocumented immigrants in the U.S. CoFIRED's co-founder, Oscar Cornejo '17, said that he hopes the new support network for undocumented students will keep the College community conscious of the uncertainty often faced by undocumented students. In its six-month existence, CoFIRED has put on a campaign called "Do I Look Illegal?" in an effort to dispel stereotype of undocumented people. Cornejo said the group has started a discussion with the financial aid and admissions offices on how to communicate with undocumented students. Also, the group helped post relevant information for undocumented students on the admissions website. He said he hoped that more students will get involved in the future. Although contentious and highly visible displays of activism often dominate campus conversation, many forms of student engagement may not be as widely seen.&lt;br/&gt;This past April, students marched across campus as part of the nationwide "Take Back the Night" rally in a protest against sexual assault. These rallies have occurred at Dartmouth since 1991. While some students combat sexual assault and spread awareness through marches, others collaborate with organizations such as the Student and Presidential Committee on Sexual Assault, which drives initiatives to address sexual assault and holds symposiums on the issue. This past year, Esteban Castano '14 and Gillian O'Connell '15 helped launch Improve Dartmouth, an online forum in which Dartmouth students can propose, vote on and discuss ideas that could benefit campus. Student moderators and administrators advocate for promising suggestions. Some recently completed suggestions include modifying the College's dining plans, as well as simpler ideas like adding a new printer location and introducing reusable silverware. One of the Improve Dartmouth's campaigns contributed to the College's decision to establish a zero-tolerance policy for sexual assault. "I think the organizations like the Inter-Community Council, Student Assembly and Improve Dartmouth are very accessible, but the more voices that can be heard the better," Noah Manning '17, a member of Student Assembly and a moderator for Improve Dartmouth, said. Environmental activism is a large part of campus activity, often supported by the Dartmouth Office of Sustainability. Alisa White '17, one of 10 freshmen EcoReps in her class, said she became involved in sustainability almost as soon as she arrived on campus. White praised the Sustainability Office for its efforts to support student passions. "It's a group of people who aren't afraid to carry a spork around sometimes," she said. "We look at sustainability in a lot of different facets, as a way of life, not just a few habits like composting." Divest Dartmouth is another campus environmental activism movement, arguing that supporting companies that produce and profit from fossil fuels is not in the best interest of the College. The ability to defend one's views and arguments is key, White said, especially at a place like Dartmouth. She established a Dartmouth chapter of Rootstrikers, a national nonprofit half-activist, half-think tank group which focuses on ways to reform campaign finance. A large part of the group's work involves reading and researching briefs and court cases in order to support its proposals. "Activism can be polarizing, but if you pick issues that you really care about, it's a great thing to be involved with," White said. Ultimately, she said, being a student activist is about fighting for issues one cares about. Campus centers such as the Office of Pluralism and Leadership are instrumental in supporting student activism, Hui Cheng '16 said. She said she found herself suddenly cognizant of the socioeconomic disparities between her and different classmates her freshman fall. "There's not really a community discussion about class going on, especially how it affects people's lives at Dartmouth," she said. "It's certainly not something most people think about before going to college." Last winter, Cheng served on OPAL's intercommunity council as socioeconomic chair and eventually pitched the idea of a council on socioeconomic awareness. Cheng was hired as a socioeconomic class intern at OPAL to turn her idea into a reality. The council, which launched last winter, held a "Hidden Costs of Dartmouth" panel during Dimensions and a similar event for the summer 2014 Dartmouth Bound program. The panel highlighted students' experiences with class at Dartmouth and covered various resources available to students. "I feel like campus activism has only grown stronger as my time here progressed," Cheng said. She said she considers OPAL to be a safe space where student activists can find support. Center for Gender and Student Engagement also provides a comfortable space where students passionate about social justice can connect, said Jessica King Fredel '17. During her freshman winter, King Fredel co-directed and performed in the student-run production "Voices" as part of V-February, which was sponsored in part by the CGSE. The show focuses on the different experiences of Dartmouth women. "Voices," which touched on topics including fraternity culture, sexual assault and body image, was performed to an audience of more than 600 people in Spaulding Auditorium. The show seemed to expose people to ideas of inequality they had never before considered, King Fredel said, adding that she received numerous questions about feminism and intersectionality in the weeks following the show. "I consistently feel like this kind of performance is a great way to open a dialogue in a community without making any specific group feel attacked," she said. "It is simply a sharing of experiences." In the end, activism on campus is primarily by and for the students, Gavin Huang '14 said. Huang joined dialogue groups and volunteer programs at the Tucker Foundation as a freshman, continuing through senior year with his work on the "Freedom Budget." "These are opportunities that you create," he said. "A lot of the groups, organizations and services on campus were a result of student demand themselves." Although the aforementioned examples of activism are all important in their own ways, they only capture a slice of a constantly evolving campus, where visible change each year. "I am sure that if a member of the Class of 2018 wants to make a difference, there is a way for them to do so," Manning said. Gavin Huang is a former member of The Dartmouth Senior Staff.</t>
         </is>
+      </c>
+      <c r="L148" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -6924,10 +7375,13 @@
           <t>Immigration (For), University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J149" t="inlineStr">
+      <c r="K149" t="inlineStr">
         <is>
           <t>From student protests of the 1960s to the momentum of modern university protests, colleges have often been watersheds of student-driven activism. Dartmouth is no exception, with students from across campus pushing for change.&lt;br/&gt;Most recently, February's "Freedom Budget," a student-authored document of more than 70 demands related to campus diversity and inclusivity, set off a firestorm of discussion.&lt;br/&gt;Campus activism over the "Freedom Budget" continued to flare up in the following weeks, leading to a two-day occupation of College President Phil Hanlon's Parkhurst Hall office in protest of what participants characterized as an inadequate administrative response. There, a group of about 35 students demanded a point-by-point response to the document.&lt;br/&gt;In late March, the Dartmouth Coalition for Immigration Reform, Equality and DREAMers hosted an event seeking to eliminate the use of the word "illegal" to refer to undocumented immigrants in the U.S.&lt;br/&gt;CoFIRED's co-founder, Oscar Cornejo '17, said that he hopes the new support network for undocumented students will keep the College community conscious of the uncertainty often faced by undocumented students.&lt;br/&gt;In its six-month existence, CoFIRED has put on a campaign called "Do I Look Illegal?" in an effort to dispel stereotype of undocumented people. Cornejo said the group has started a discussion with the financial aid and admissions offices on how to communicate with undocumented students.&lt;br/&gt;Also, the group helped post relevant information for undocumented students on the admissions website. He said he hoped that more students will get involved in the future.&lt;br/&gt;Although contentious and highly visible displays of activism often dominate campus conversation, many forms of student engagement may not be as widely seen.&lt;br/&gt;This past April, students marched across campus as part of the nationwide "Take Back the Night" rally in a protest against sexual assault. These rallies have occurred at Dartmouth since 1991.&lt;br/&gt;While some students combat sexual assault and spread awareness through marches, others collaborate with organizations such as the Student and Presidential Committee on Sexual Assault, which drives initiatives to address sexual assault and holds symposiums on the issue.&lt;br/&gt;This past year, Esteban Castano '14 and Gillian O'Connell '15 helped launch Improve Dartmouth, an online forum in which Dartmouth students can propose, vote on and discuss ideas that could benefit campus. Student moderators and administrators advocate for promising suggestions.&lt;br/&gt;Some recently completed suggestions include modifying the College's dining plans, as well as simpler ideas like adding a new printer location and introducing reusable silverware. One of the Improve Dartmouth's campaigns contributed to the College's decision to establish a zero-tolerance policy for sexual assault.&lt;br/&gt;"I think the organizations like the Inter-Community Council, Student Assembly and Improve Dartmouth are very accessible, but the more voices that can be heard the better," Noah Manning '17, a member of Student Assembly and a moderator for Improve Dartmouth, said.&lt;br/&gt;Environmental activism is a large part of campus activity, often supported by the Dartmouth Office of Sustainability.&lt;br/&gt;Alisa White '17, one of 10 freshmen EcoReps in her class, said she became involved in sustainability almost as soon as she arrived on campus.&lt;br/&gt;White praised the Sustainability Office for its efforts to support student passions.&lt;br/&gt;"It's a group of people who aren't afraid to carry a spork around sometimes," she said. "We look at sustainability in a lot of different facets, as a way of life, not just a few habits like composting."&lt;br/&gt;Divest Dartmouth is another campus environmental activism movement, arguing that supporting companies that produce and profit from fossil fuels is not in the best interest of the College.&lt;br/&gt;The ability to defend one's views and arguments is key, White said, especially at a place like Dartmouth.&lt;br/&gt;She established a Dartmouth chapter of Rootstrikers, a national nonprofit half-activist, half-think tank group which focuses on ways to reform campaign finance. A large part of the group's work involves reading and researching briefs and court cases in order to support its proposals.&lt;br/&gt;"Activism can be polarizing, but if you pick issues that you really care about, it's a great thing to be involved with," White said.&lt;br/&gt;Ultimately, she said, being a student activist is about fighting for issues one cares about.&lt;br/&gt;Campus centers such as the Office of Pluralism and Leadership are instrumental in supporting student activism, Hui Cheng '16 said.&lt;br/&gt;She said she found herself suddenly cognizant of the socioeconomic disparities between her and different classmates her freshman fall.&lt;br/&gt;"There's not really a community discussion about class going on, especially how it affects people's lives at Dartmouth," she said. "It's certainly not something most people think about before going to college."&lt;br/&gt;Last winter, Cheng served on OPAL's intercommunity council as socioeconomic chair and eventually pitched the idea of a council on socioeconomic awareness. Cheng was hired as a socioeconomic class intern at OPAL to turn her idea into a reality.&lt;br/&gt;The council, which launched last winter, held a "Hidden Costs of Dartmouth" panel during Dimensions and a similar event for the summer 2014 Dartmouth Bound program. The panel highlighted students' experiences with class at Dartmouth and covered various resources available to students.&lt;br/&gt;"I feel like campus activism has only grown stronger as my time here progressed," Cheng said.&lt;br/&gt;She said she considers OPAL to be a safe space where student activists can find support.&lt;br/&gt;Center for Gender and Student Engagement also provides a comfortable space where students passionate about social justice can connect, said Jessica King Fredel '17.&lt;br/&gt;During her freshman winter, King Fredel co-directed and performed in the student-run production "Voices" as part of V-February, which was sponsored in part by the CGSE. The show focuses on the different experiences of Dartmouth women.&lt;br/&gt;"Voices," which touched on topics including fraternity culture, sexual assault and body image, was performed to an audience of more than 600 people in Spaulding Auditorium.&lt;br/&gt;The show seemed to expose people to ideas of inequality they had never before considered, King Fredel said, adding that she received numerous questions about feminism and intersectionality in the weeks following the show.&lt;br/&gt;"I consistently feel like this kind of performance is a great way to open a dialogue in a community without making any specific group feel attacked," she said. "It is simply a sharing of experiences."&lt;br/&gt;In the end, activism on campus is primarily by and for the students, Gavin Huang '14 said. Huang joined dialogue groups and volunteer programs at the Tucker Foundation as a freshman, continuing through senior year with his work on the "Freedom Budget."&lt;br/&gt;"These are opportunities that you create," he said. "A lot of the groups, organizations and services on campus were a result of student demand themselves."&lt;br/&gt;Although the aforementioned examples of activism are all important in their own ways, they only capture a slice of a constantly evolving campus, where visible change each year.&lt;br/&gt;"I am sure that if a member of the Class of 2018 wants to make a difference, there is a way for them to do so," Manning said.&lt;br/&gt;Gavin Huang is a former member of The Dartmouth Senior Staff.</t>
         </is>
+      </c>
+      <c r="L149" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -6972,10 +7426,13 @@
           <t>Campus climate, Anti-racism, Police violence, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J150" t="inlineStr">
+      <c r="K150" t="inlineStr">
         <is>
           <t>In recent months, colleges across the country have seen a spate of demonstrations regarding issues of identity, with students demanding greater inclusivity on their campuses. Many resemble Dartmouth's April "Freedom Budget" protests, when over a dozen students occupied College President Phil Hanlon's office for two days, demanding a point-by-point response to a list of over 70 demands regarding issues of diversity.&lt;br/&gt;In the last year, students at Princeton University, Harvard University, Oberlin College, Mills College, University of Michigan, City University of New York, Mount Holyoke College and University of California at Los Angeles, among others, have initiated protests concerning similar issues. Melissa Padilla '16, who was involved in the "Freedom Budget" protest, said she communicated with her friends who were involved with similar protests at other schools, including New York University and University of Texas at Austin, during the construction of the "Freedom Budget" and the sit-in. Other Dartmouth activists spoke with friends on various campuses as well, she said. The protest at Dartmouth, she said, was not a reaction to movements at other schools but a response to discrimination at the College. "A lot of universities are looking to be more inclusive but are acting very unlike their statements," Padilla said. "There's a big gap between their mission statements and the actual reality of being a student on campus." Across the country students are demanding that administrators make structural changes to better support all students. On April 7, a coalition of students at Oberlin College, in Ohio, wrote an open letter in support of the sit-in at Dartmouth. The letter was posted in the opinion section of "Fearless and Loathing," an independent website run by Oberlin students. "We recognize the actions of our fellow students at Dartmouth as courageous, necessary steps that must be taken if institutions such as ours - ones that advertise themselves on falsified notions of diversity, inclusivity and dignity - continue to treat 'dialogue' as a synonym for structural violence," the letter states. Oberlin junior Ana Robelo, who has been a member of the coalition since its founding last fall, said several communities on Oberlin's campus worked together to compile a list of demands for their school's administration. The demands included increased administrative transparency, divestment from companies that support Israeli occupation of Palestine and scholarship funding for undocumented students. On Oct. 10, a group of Oberlin students took over the Board of Trustees meeting and discussed demands. Oberlin senior Alice Beecher said that hundreds of students dressed in red as a symbol of solidarity. Robelo said she sensed strong and immediate backlash during the meeting. Student reactions, however, were generally supportive, though some disagreed with the group's tactics and the demand to divest from companies that support Israel, Beecher said. Since the board meeting, Beecher said that some smaller communities within the coalition have met with administrators to advance individual demands. Beecher said students joined together to create a replica of the wall separating Gaza and Israel, painting it with different representations of borders in society. Students then placed pieces of the wall in front of Oberlin's main library alongside an audiotape playing students' personal stories of division within the Oberlin community, she said. Members of the coalition also stood outside a second trustee meeting in December while holding pieces of the reconstructed wall, Beecher said. Robelo said the coalition formed in part as a result of events that took place at Oberlin last spring, including the appearance of someone dressed in a Ku Klux Klan robe and racist graffiti around campus. The coalition, Beecher said, was reacting to what they perceived as the administration's non-response. On May 1, approximately 10 students sat outside a Princeton University student center wearing black shirts and white opera masks, playing a recording of their manifesto on a boombox, Princeton junior Katie Horvath said. Passersby were offered fliers outlining the group's 10 demands for change at the university, including revised mental health policies, divestment and a call for more gender neutral housing options, among others. Horvath, who participated in the demonstration but emphasized that she did not organize it, said although the protest stemmed from a queer activism movement, its demands were "intersectional" and addressed a range of issues beyond gender.&lt;br/&gt;Though the Princeton group, called Praxis Axis, placed a stack of masks next to their demonstration as an invitation for passersby to join in, few people followed suit since few knew in advance or had clothing that matched that of the protesters, which Horvarth said became a "barrier to entry." Horvath said that the Praxis Axis demands felt similar in nature to demands voiced by the "Freedom Budget," as both were intersectional efforts to address issues centered on identity. Although Praxis Axis members did not work directly with Dartmouth students to compile their demands, Horvarth said she believed demonstrators at various schools would benefit from joining forces. For those at institutions like Princeton, which tend to have less widespread student activism than more urban institutions, engaging with like-minded students at other colleges can contribute to a stronger "protest culture," she said. On April 2, Princeton freshman Tal Fortgang published an essay titled "Checking My Privilege: Character as the Basis of Privilege" in The Tory, a conservative publication at the school. The piece, in which Fortgang refused to apologize for having privilege and cited examples of difficulties faced by his family, prompted much discussion on the Princeton campus, Horvath said. "It's been helpful," she said, "in that it has made people concerned and aware who would otherwise be likely to dismiss the demands of a group like the protest group on May Day as unnecessary or absurd or over the top." Mount Holyoke, an all-women's college in Massachusetts, is in the midst of a movement that aims to address discrimination and increase student involvement in college policy, said junior Melanie Wilkerson, an active participant in the movement. The movement, known as "MoHonest," began after Mount Holyoke student Maya Wegerif, 21, wrote a blog post alleging discrimination by campus police when she was arrested following an alcohol-related incident. Wilkerson said that many students of color at Mount Holyoke related to Wegerif's experience, and the incident sparked much discussion about discrimination and the power of campus police. "We began to form an entity that wanted to specifically represent students of color on campus," she said. "And even more broadly, those who have faced discrimination on campus or were allowed to suffer discrimination and not receive adequate administrative support." Members presented a formal list of demands to the administration in April, Wilkerson said, and are currently at a "standstill." The group's demands include encouraging more active student participation in campus policy and decisions, increasing institutional support for first-generation college students, updating the policy for reporting grievances and creating educational workshops for students, faculty, staff and campus police. "We're still negotiating, but we're a little disappointed with the administration," Wilkerson said. Wilkerson said that members of the "MoHonest" movement were aware of the "Freedom Budget" and considered the Dartmouth activists' tactics when brainstorming. The sit-in at Dartmouth, she said, was "successful in its visibility." Though "MoHonest" protesters considered a sit-in, Wilkerson said they decided against it because some members felt that - unlike at Dartmouth - not enough time had elapsed since the demands had been voiced. Wilkerson said the "MoHonest" movement reflects a nationwide trend of students becoming more vocal about administrators' lack of support. "MoHonest" has supported related movements at other institutions, including Vassar College and Bryn Mawr College, she said. "I feel like the trend is catching on because people across the country are really starting to acknowledge the kind of power young people have," she said. Though "MoHonest" faced some opposition from students, Wilkerson said it has found a broad base of support among faculty and alumni. "In my three years at Mount Holyoke, I have witnessed people go through some pretty intense stuff in terms of discrimination," Wilkerson said. "Even in a very liberal, diversity-agenda-pushing institution like Mount Holyoke, there are still fundamental flaws and issues that need to be addressed." Two student movements have recently arisen at Harvard University, both aiming to increase diversity among faculty, staff and administrators and to improve resources for more diverse programming, Harvard senior Terrance Moore said. The first of these movements, a photography campaign titled "I, Too, Am Harvard," launched on Tumblr in early March. The pictures show black students holding signs with examples of racial prejudice they have experienced at Harvard, accompanied by the slogan. Once the campaign gained attention, students involved began researching other movements to see how they were successful in creating institutional change, Moore said. The second student movement, known as "The Diversity Report," spun out of the "I, Too, Am Harvard" campaign, Moore said. Students involved in "The Diversity Report" wrote a list of demands and are currently working with specific administrators to achieve them, Moore said. After contacting them, the students decided to fill out report cards evaluating administrators to hold them accountable.</t>
         </is>
+      </c>
+      <c r="L150" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -7020,10 +7477,13 @@
           <t>Indigenous issues</t>
         </is>
       </c>
-      <c r="J151" t="inlineStr">
+      <c r="K151" t="inlineStr">
         <is>
           <t>In spite of the Tuesday afternoon drizzle, about 75 protesters lined up through Sather Gate hoisting a 90-foot inflatable Keystone XL "pipeline" above their heads to protest the contentious project that would transport crude oil from Alberta to Nebraska.&lt;br/&gt;UC Berkeley students from Cal Berkeley Democrats, CALPIRG and CalSERVE held posters and sunflowers while chanting, "Hey, Obama, we don't want no pipeline drama," during the rally. Other members of the crowd supported the inflatable black tube, which read, "No Keystone Pipeline!"&lt;br/&gt;The U.S. Department of State is in the process of finalizing an environmental review that it commissioned about the project and determining whether granting a presidential permit would be in the interest of the nation. In March, the department released a preliminary draft of the report.&lt;br/&gt;The 12:30 p.m. rally, coordinated through the ASUC Office of Environmental Sustainability, featured UC Berkeley professor of energy Daniel Kammen, who has served on the Natural Resources Canada research and study team for new technologies in the past.&lt;br/&gt;"Energy is central to our lives, but pollution is not," he said during the rally . "We need a diverse, resilient energy economy - not one tied to more polluting fuels, as are the Albertan tar sands."&lt;br/&gt;Several environmental groups, including the Center for Biological Diversity, Sunflower Alliance and 350 Bay Area, supported the event.&lt;br/&gt;Earlier this semester, the ASUC Senate instructed ASUC President DeeJay Pepito in a near-unanimous vote to write a letter to President Barack Obama to express the ASUC's formal opposition to the construction of the pipeline.&lt;br/&gt;The protesters objected to the process by which tar sands are extracted before being carried through the pipeline - a process they said damages clean water supplies and causes extensive deforestation - and see the project as a threat to the communities it will pass through.&lt;br/&gt;"It matters to me because I see environmental policies like fossil fuels as an issue of social justice," said ASUC Executive Vice President Nolan Pack, who attended the rally. "This pipeline will displace indigenous people."&lt;br/&gt;Last spring, the ASUC Senate passed a bill authored by Pack that urged the university to divest its funds from fossil fuel companies.&lt;br/&gt;"We want to raise awareness that Cal students are against the pipeline," said ASUC Director of Sustainability Haley Broder. "We want to make sure President Obama feels the pressure."&lt;br/&gt;Megan Messerly is a news editor. Contact her at [email protected] and follow her on Twitter @meganmesserly.</t>
         </is>
+      </c>
+      <c r="L151" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="152">
@@ -7068,10 +7528,13 @@
           <t>Anti-racism</t>
         </is>
       </c>
-      <c r="J152" t="inlineStr">
+      <c r="K152" t="inlineStr">
         <is>
           <t>Students protest in front of Holyoke Center&lt;br/&gt;"If you like it, keep it. If you don't, leave."&lt;br/&gt;These words of coercion oft used to intimidate powerless employees by employers are very familiar to Delmy Lemus, a housekeeper at the DoubleTree Hotel in Allston, which Harvard bought back in 2005. According to Lemus, her employers threaten her and her coworkers with these words whenever they speak up against unfair working conditions.&lt;br/&gt;Lemus has been working at the DoubleTree Hotel for the past five years. Although working conditions were tolerable when she first began the job, conditions began to decline after her first year and have continued to deteriorate ever since. Her employers verbally abuse her, having yelled at her to the point of making her cry several times. After the hotel cut down on employees, Lemus and one other housekeeper were required to complete job assignments that were originally designed for four to five workers. As a result, Lemus now performs extra duties, such as laundry and room requests, and is constantly rushing and running to complete her work. If she does not complete her daily tasks, she will receive a warning the next morning, and after three warnings, she will be fired. Due to such a burdensome workload, Lemus has suffered from several injuries from her work, including a broken nose, and now suffers from chronic back pain.&lt;br/&gt;Even when Lemus was eight months pregnant a few years ago, her employer forced her to continue her job without aid, which included bending down to make beds and lifting heavy objects, such as cots and sofa beds. Once she started to experience contractions, Lemus asked to take leave for work. However, her employer accused her of lying about her due date, told her to work for at least one more week, and threatened her that she would lose her job if she did not return within three months. In face of such threats, Lemus took leave, and a few days later, gave birth to her daughter Arianna. Astonishingly, her job has continued to get worse since then. Lemus' tragic story, however, is but one of many among the employees at the Harvard-owned DoubleTree Hotel.&lt;br/&gt; The DoubleTree Campaign&lt;br/&gt;Most, if not all, the employees at the DoubleTree Hotel in Allston at the hotel suffer from terrible working conditions, including but not limited to low wages, high accident rates, unaffordable health care, racial and gender discrimination, verbal abuse, and sexual harassment. In fact, according to a report titled "Harvard's Hotel compared [sic] to the Harvard Community Standard," 96 percent of surveyed workers said that their jobs had degraded over the past six years, while 84 percent said they could not imagine continuing to work there for the next 10 years. This is why Lemus decided to join the DoubleTree campaign. In an interview with the HPR, Lemus said, "I decided to get involved because if I don't do something, then I will have to leave my job soon. Things are getting worse."&lt;br/&gt;There are more shocking statistics. One-hundred percent of surveyed room attendants stated they suffer from pain at home, which all of them agreed interferes with their other activities. Meanwhile, 78 percent do not view their workplace as a safe environment. Furthermore, the DoubleTree Hotel employees only earn 68 cents for every dollar that Harvard University Dining Services employees who have two or more years of work experience at the university do.&lt;br/&gt;Such inhumane working conditions have fueled the DoubleTree campaign, a campaign run by Harvard' Student Labor Action Movement in concert with the employees at DoubleTree Hotel and the union with the purpose of fighting to establish fair process for employees at the hotel. According to abovementioned report, fair process is "an established, common agreement whereby the employer pledges not to retaliate while employees decide whether or not they would like to join a union." While the DoubleTree campaign may appear to be like any other fair labor campaign run by SLAM, deeper examination suggests that the campaign is a unique one, involving a more critical role on the part of students, the hotel's mixed status as property and an investment, and broader moral implications for Harvard's role in the community.&lt;br/&gt;A Brief History&lt;br/&gt;At the beginning of last semester, SLAM helped organize a supermajority of workers at DoubleTree Hotel to sign a petition stating that they would like to establish fair process. On March 12, the workers presented the petition for fair process to the DoubleTree Hotel management. Afterwards, SLAM garnered approximately 600 petition signatures by Harvard students over the next two months. When presented to Harvard University President Drew Faust, however, the petition was rejected. On May 8, Harvard Human Resources sent a letter to the union Boston's Local 26 expressing their refusal to establish fair process for DoubleTree employees.&lt;br/&gt;In early November, SLAM published a report titled "Harvard's Hotel compared to the Harvard Community Standard," outlining the abuses DoubleTree Hotel workers suffer. SLAM plans to present the report to Faust, as well as distribute copies of the report in university dining halls and obtain more petition signatures from students. SLAM member Gabriel Bayard notes that SLAM plans to hold a forum involving workers, students, and professors to discuss the importance of the campaign. Several faculty members have expressed support for the campaign, including Marshall Ganz, a Senior Lecturer at the Harvard Kennedy School, and Kirsten Weld, Assistant Professor of History at the College.&lt;br/&gt;A Triangular Force&lt;br/&gt; It is important to note the critical role students play in the campaign. While the Hilton manages the DoubleTree Hotel, Harvard owns it. As a result, even though the Hilton may face the brunt of pressure from workers, it cannot do anything without Harvard's approval. Therefore, it does not matter that Hilton hotels in Boston have a history of saying yes to unions and workers regarding labor negotiations if Harvard is not persuaded to agree to establish fair process. According to a Hilton Worldwide spokesperson, Hilton is "committed to offering a workplace environment where our team members are treated fairly and with respect, including respecting the right of our team members to choose or not choose collective bargaining representation."&lt;br/&gt; Due to the unique circumstances, it is particularly important for students to get involved in the campaign and insist Harvard to protect workers' rights. Pressure on the hotel by the workers and pressure on Harvard by the students are necessary components to the success of the campaign. In an interview with the HPR, Bayard said, "We think it's exciting because there aren't that many times that students are so central to a campaign like this, and this time students are. The workers could burn the hotel down and Harvard could say they don't care. When students and workers fight together, we can really change things."&lt;br/&gt; SLAM member Preston Craig also notes the critical role that Harvard students can play in this campaign, in comparison with other campaigns SLAM is running. In an interview with the HPR, Craig noted, "[The DoubleTree Hotel] is something that is owned by Harvard, which is different than the other campaigns that SLAM is working on. As Harvard students, we both have the responsibility and a unique position to effect change. I think the main thing is that undergraduate students educate more people about the campaign and increase pressure on the administration."&lt;br/&gt;Fellow SLAM member, Lee Hittner-Cunningham, agrees with Craig. In an interview with the HPR, she stated, "The way we're going to make progress isn't just by workers doing demonstrations or boycotts. It's about directly going to the owners. The administration has to respond to undergraduate complaints about things. If we have the undergraduate population mobilize to say they won't tolerate treating workers this way, then Harvard can become a force for good and not accept the kind of conditions that the workers are subjected to."&lt;br/&gt; Thus, the effort required for the success of the DoubleTree Campaign can be seen as triangular. Pressure from all three sides-employees, the students, and the union-is critical to achieve fair process for the workers.&lt;br/&gt;A Mixed Precedent&lt;br/&gt;There is reason to be optimistic about the DoubleTree campaign. In December 2011, a similar labor union campaign that involved ownership by Harvard and management by another company occurred at the Harvard Law School and ended up in success for SLAM. HLS dining services workers, who worked for Restaurant Associates, were non-union. About 90 percent signed a card saying they wanted a fair process, and two weeks later, Harvard agreed, providing the cafeteria workers the same contract as workers at the university dining halls. In the end, the workers voted to join Boston's Local 26. Therefore, there is a clear precedent of Harvard agreeing to fair process for subcontracted workers who work for another company.&lt;br/&gt;Yet, there is a complicating factor that may prevent the DoubleTree campaign's mission from being quite as easily accomplished as that of the HLS cafeteria. This factor has to do with the location of the hotel, which ultimately affects the value of the hotel in Harvard's self-interest. Examination of this issue sheds light on Harvard's resistance to establishing fair process for the hotel employees. In one respect, Harvard's purchase of DoubleTree Hotel can be seen as simply buying property for the university. Harvard makes approximately $20 million every year from the DoubleTree Hotel and the tax valuation for the property is between $50 and $100 million. Therefore, Harvard may be trying to maximize profits.&lt;br/&gt;However, according to Bayard, the hotel is more like an investment in that Harvard has a master plan to make Allston its second campus; owning a large span of property like the hotel provides the university flexibility in its expansion plans. A quick cost-benefit analysis regarding the slight effect increasing wages would have on the $20 million revenue Harvard makes from the hotel, in contrast to the great improvement of worker productivity and hotel reputation that comes along with happier employees, can support this theory. It is not just about revenue; it is about investment.&lt;br/&gt;Moral Implications&lt;br/&gt;This investment aspect of the DoubleTree Hotel does not only have logistical, monetary repercussions. It has deeper moral implications. According to Bayard, "Harvard is being reticent. They're afraid of allowing students to determine that their investments also have to be fair."&lt;br/&gt;This is where the DoubleTree campaign ties in with all of the other contemporary activist campaigns on campus, such as Divest Harvard led by Students for a Just and Sustainable Future and the efforts led by Responsible Investment at Harvard Coalition. Currently, the Harvard administration refuses to accept moral responsibility for its investments, in stark contrast to its normative statements of morality. For example, in President Drew Faust's speech to launch Harvard's $6.5 billion Capital Campaign, she asserted that Harvard's legacy should be "as good as it is great." In addition, in discussing employment at Harvard, the Vice President for Human Resources stated Harvard should build a " community guided by shared values."&lt;br/&gt; Despite student efforts to steer Harvard away from unethical practices, the administration continues to refuse to acknowledge that investing money in certain companies or projects has vast ethical repercussions and that such great power inherently brings the burden of moral duty. Speaking to this moral responsibility, Bayard aptly illustrates the deep impact the DoubleTree Campaign can have in shaping Harvard's attitude toward its investments: "What I think is really promising about this campaign is it opens the door that Harvard's investments have an impact on Boston and the Harvard community. Our hope for future investments is that Harvard will recognize there is a responsibility to abide by certain principles, one being labor fairness. Thirty-two billion dollars has to go somewhere, and a lot of it goes to direct investments. We're hoping that Harvard will realize these investments have a direct impact on the Harvard community and that it doesn't come at expense to Harvard."&lt;br/&gt; Predicting the Future&lt;br/&gt;Those involved in the campaign appear to be very confident about the impending success of the campaign. Bayard stated, "This will work. This will happen. I'm very confident. I think Harvard has little moral standing to say no to this. The workers have demonstrated that they are a part of the Harvard community. As such, they should be given the same rights as any of the other works in the dining halls. We think Drew Faust knows that."&lt;br/&gt; What's the overall importance of this campaign?  Lemus, perhaps, puts it in the most simple but accurate terms: "If you're human, you can understand." One of many activist campaigns on campus, the DoubleTree campaign proves critical in its exemplification of the importance of being humane and in the deep moral implications it has for humanity.</t>
         </is>
+      </c>
+      <c r="L152" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="153">
@@ -7111,10 +7574,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J153" t="inlineStr">
+      <c r="K153" t="inlineStr">
         <is>
           <t>McGill’s Petrocultures 2014 conference faced criticism last Friday, when participants were forced to relocate following an occupation of the Faculty Club by a group called “LockOut Petrocultures.” Later that day, student campaign group Divest McGill demonstrated outside the conference as well.&lt;br/&gt;At 8:00 a.m., approximately 30 members of the Montreal community group occupied the Faculty Club, interrupting nearly one and a half hours of the conference. Due to the occupation, the conference was temporarily relocated to Redpath Hall.&lt;br/&gt;Mona Luxion, an Urban Planning Ph.D. candidate and media relations officer for LockOut Petrocultures, said that the group planned the disruption to question the effectiveness of the conference.&lt;br/&gt;“Staging a debate [where] fossil fuel company executives have equal say as potential critics is reinforcing the status quo; it’s not moving us forward,” she said. “We really wanted to challenge this idea that this is a debate that should be happening, and really push towards concrete actions that gets [McGill] out of the business of fossil fuels.”&lt;br/&gt;Petrocultures was hosted by the McGill Institute for the Study of Canada (MISC), which organizes conferences on a wide variety of topics, changing from year to year. This year’s event drew participants from the arts, social sciences, sciences, and engineering from across Canada to speak on the consequences of reliance on fossil fuels and to discuss responsible alternatives&lt;br/&gt;“Petrocultures 2014 will bring together leading figures to discuss and debate the role of oil and energy in shaping social, cultural, and political life in Canada at present and in the future,” the conference program reads. “[The] event involv[es] a diverse group of speakers from across Canada.”&lt;br/&gt;Members of Divest McGill, a student campaign group against university investment in fossil fuel industries, attended the conference as participants but also expressed support for the occupiers. In the Divest McGill demonstration that same day, protestors chanted in support of divestment and invited members of the community to envision a future without reliance on fossil fuels.&lt;br/&gt;“[The conference] purport[s] to be really non-partisan, but in reality they had two hour-long sessions from people from oil companies or from energy boards, and had very clear, vested interests,” Bronwen Tucker, Divest McGill coordinator, said. “There was not a single grassroots Indigenous activist. They just didn’t do a proper job at representing the whole spectrum.”&lt;br/&gt;However, William Straw—professor and director of the MISC—noted that 17 of the 26 speakers at the conference were activists. These included five people from Indigenous communities who work on the impact of fossil fuels, although two had to withdraw at the last minute due to personal reasons.&lt;br/&gt;“To the accusation that the conference offered a false ‘balance,’ I will simply point to the overwhelming representation of environmental activists,” Straw said. “To the accusation—made before the conference had begun—that we were going to debate ‘climate change’ as if it were an unsettled issue, I will note that no one at the conference, with the possible exception of [one attendee], challenged the reality of climate change.”&lt;br/&gt;Luxion said the occupation achieved their goals of critiquing and interrupting the conference.&lt;br/&gt;“I think we led people to question the starting point [of the conference], in addition to actually having a material impact in terms of forcing the conference to move,” she said.&lt;br/&gt;Straw said that he was disappointed that attempts to communicate with the occupiers were ineffective.&lt;br/&gt;“We hoped to talk to the occupiers, and several participants […] made an effort to speak to them,” Straw said. “That wasn’t successful.”&lt;br/&gt;Straw maintained that he was pleased with the conference’s turnout this year, and that the protests would not impact future conferences.&lt;br/&gt;“Building a conference is a multi-month process of awaiting responses, last minute withdrawals, pressures from various quarters, and disappointments,” he said. “Given all this, I’m pleased with what we came up with.”&lt;br/&gt;Share this:Click to share on Twitter (Opens in new window)Click to share on Facebook (Opens in new window)Click to share on Google+ (Opens in new window)&lt;br/&gt;&lt;br/&gt;Related</t>
         </is>
+      </c>
+      <c r="L153" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="154">
@@ -7154,10 +7620,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J154" t="inlineStr">
+      <c r="K154" t="inlineStr">
         <is>
           <t>Concordia, McGill Students Hold “Die-In” to Protest Fossil Fuel Investment&lt;br/&gt;News by Noelle Didierjean — Published April 8, 2014 | Comments&lt;br/&gt;Follow @noellesolange&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Students ‘died’ at McGill to protest the university’s investment in fossil fuels  Photo Noelle Didierjean&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Students protested fossil fuel investment  Photo Noelle Didierjean&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Students ‘died’ at McGill to protest the university’s investment in fossil fuels Photo Noelle Didierjean&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Students ‘died’ at McGill to protest the university’s investment in fossil fuels Photo Noelle Didierjean&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Students protested fossil fuel investment  Photo Noelle Didierjean&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Students ‘died’ at McGill to protest the university’s investment in fossil fuels Photo Noelle Didierjean&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Students ‘died’ at McGill to protest the university’s investment in fossil fuels Photo Noelle Didierjean&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Students protested fossil fuel investment  Photo Noelle Didierjean&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;A rally culminating in a “die-in” was held on Tuesday, April 1 in protest of Concordia and McGill University’s environmental policies. &lt;br/&gt;Students met in the mezzanine floor of the Hall Building from 3 p.m. to 4 p.m., making signs and eating food provided by the organizers. &lt;br/&gt;“There are 12 [rallies] happening across Canada in the different divestment campaigns coordinated by the Canadian Youth Climate Coalition. [This is part of] a national day of action called ‘Fossil Fools’ to try and get more awareness,” explained Anthony Garoufalis-Auger, CSU VP External and Mobilization and member of Divest Concordia. &lt;br/&gt;At around 4 p.m., the participants left the Hall Building and marched down Mackay St. to St. Catherine St. W. They were escorted by several police cars. &lt;br/&gt;“For climate justice at our schools, no tar sands, no fossil fuels,” protesters chanted.&lt;br/&gt;The crowd wound its way down St. Catherine St. W. before heading down McGill Ave. &lt;br/&gt;“Last week, the British medical journal editorial board wrote that the best thing for health professionals to do for climate action is to demand that their institutions, including universities and hospitals, divest from fossil fuels,” Garoufalis-Auger told the crowd with a megaphone.  &lt;br/&gt;“We need to keep pushing, and not take no as an answer.” &lt;br/&gt;The group then made their way to a tarp in front of McGill’s central building, where ‘Fossil Fuel Fred,’ a character played by McGill student Justin Chisholm, made a satirical speech thanking ‘McSpill University’ and ‘CoalCordia’ for investing in fossil fuels.&lt;br/&gt;The character “originally came out of a mock candidate to force all the [McGill] presidential candidates to take a position on divestment,” Chisholm explained. &lt;br/&gt;“At the end of his campaign he pretended to go away to a tropical island and do something at ‘CoalCordia’ to bridge the gap there so Concordia and McGill could use the character,” he said.&lt;br/&gt;The die-in simulated an oil spill, and around 15 students ‘died’ one by one on the tarp, including CSU councillor John Talbot and Garoufalis-Auger. There were several minutes of silence for those impacted by oil spills, after which protesters dispersed. &lt;br/&gt;The 12 rallies took place following the conclusion of PowerShift, which many of the protesters attended. An annual conference held this year in Halifax, PowerShift brings youth together with the goal of promoting a “clean, just and sustainable future.”&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;By commenting on this page you agree to the terms of our Comments Policy.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Please enable JavaScript to view the comments powered by Disqus.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Related Reading&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;Feasting and Fighting Resource Extraction&lt;br/&gt;Michelle Pucci&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;GGI Crash Course&lt;br/&gt;Julia Wolfe &amp; Corey Pool&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;Decision to Change the Redmen Name Postponed&lt;br/&gt;Alexander Perez&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;Tear Gas, Stun Grenades End Anti-Austerity Protest&lt;br/&gt;Noelle Didierjean</t>
         </is>
+      </c>
+      <c r="L154" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="155">
@@ -7197,10 +7666,13 @@
           <t>Domestic foreign policy, Anti-war/peace</t>
         </is>
       </c>
-      <c r="J155" t="inlineStr">
+      <c r="K155" t="inlineStr">
         <is>
           <t>The practice of protesting commencement speakers is nothing new, but rarely in recent memory have these protests been as widespread and as solicitous of public attention as they have been this spring.&lt;br/&gt;It all started April 8, when administrators at Brandeis University, acting under pressure from undergraduates and faculty members, rescinded a commencement invitation to Ayaan Hirsi Ali, a noted women's rights advocate and strident critic of Islam. To most students, the rescindment seemed prudent, and the original invitation almost inexplicable. Ali, after all, had called Islam a "destructive, nihilistic cult of death" in an interview with the London Evening Standard in 2007, and many of her statements continue to be overtly Islamphobic.&lt;br/&gt;But the commencement rows that would follow in the coming weeks seemed far more frivolous, in that these protests were not based in opposition to personal bigotry, but rather in opposition to specific political policies that were not, on their face, tied to intolerance.&lt;br/&gt;On May 4, for instance, former Secretary of State Condoleezza Rice, facing student protest at Rutgers as a result of her involvement in the Iraq War and her approval of waterboarding war detainees, decided not to attend the school's ceremony, as she feared that the contentious atmosphere surrounding her visit would subtract from the collegial atmosphere of graduation. Though she withdrew voluntarily, it was clear she felt intellectually bullied. "I am honored to have served my country," she said on May 5. "I have defended America's belief in free speech and the exchange of ideas."&lt;br/&gt;Christine LaGarde: Is she really that evil? (AP/Cliff Owen)&lt;br/&gt;Christine LaGarde, the current managing director of the IMF and a noted labor and antitrust lawyer before she entered the public sector, was the next commencement speaker to come under fire. Petitioners at Smith College, students and faculty alike, rallied to disinvite her, accusing the IMF of "imperialistic" policies, while conceding that LaGarde may herself be a "good person." Soon LaGarde withdrew for the same reasons as Rice.&lt;br/&gt;A few days later, students at Haverford pressured former University of California chancellor Robert C. Birgeneau into withdrawing from its commencement ceremonies because he initially supported the police response to a heated 2011 Occupy Berkeley incident. (The fact that he condemned the police and called for an immediate investigation after seeing video footage of the altercation a few days later meant little to the protestors.)&lt;br/&gt;And, recently, a similar debate also penetrated Harvard's campus: at the Graduate School of Education, petitioners attempted a putsch against Colorado State Senator Michael C. Johnston-who fortunately did speak at commencement-on the basis of his support for "test-based accountability" for teachers.&lt;br/&gt;Among the commentariat, save in the most liberal journals, pundits and editorial boards have come down against these protesting students, describing their meta-movement as a harbinger of "rising liberal intolerance" on campus. And though student papers, including the Crimson, have defended the protests, it seems to me that the mainstream media is at least partially right. Birgeneau, who himself has a history of liberal, nonviolent protest, hardly seems like a controversial figure. Neither does LaGarde, who in many respects would be considered something of a lefty in Amercan political circles, even if the organization she now heads is associated with neoliberal economics. New York City police commissioner Ray Kelly treads more contentious ground, but the refusal of Brown students to let him speak at a forum and Q&amp;A last semester-which is far from a commencement speech-struck many, including myself, as close-minded.&lt;br/&gt;Those supporting these student protests frame the issue as one of free speech: they have a right, under this principle, to fight "speech with speech"-and their speech happens to take the form of protest. I wholeheartedly agree with this principle, but this argument misses the point.&lt;br/&gt;Though we certainly have a right, and, at times, a responsibility to protest, the issue here is the effect of the protest, not the legitimacy of the method. And here the effect is too often sealing our campuses off from the policies that vocal students disagree with-limiting our politics to a very narrow kind of campus liberalism.&lt;br/&gt;In the protestors' defense, a commencement address is not just another forum on campus; the selected speaker should not denigrate a certain people or ethnicity during their speech, as graduates of all stripes should be able to attend without their personal dignity being called into question. That's why I agree with Brandeis' rejection of Hirsi Ali.&lt;br/&gt;But specific policy disagreements-unless they are predicated on racist or overtly discriminatory sentiment-should not be a basis for disinvitation. Like most campus communities, our community is far too intellectually diverse to avoid this kind of conflict, and-as most students who've engaged in political debate with peers will attest-non-bigoted, intellectually rigorous arguments from the other side of the political spectrum are often the most informative, and almost always the most challenging.&lt;br/&gt;For me, it feels strange to oppose student protest, as I appreciate and support the work of SLAM, SJSF, Divest and a number of other activist groups on campus. In other words, I mostly share the politics of the protestors I'm critiquing. But here I do have one profound disagreement: while a commencement speaker must be intellectually accomplished and adhere to basic principles of tolerance, he or she does not need to agree with my politics.</t>
         </is>
+      </c>
+      <c r="L155" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="156">
@@ -7240,10 +7712,13 @@
           <t>University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J156" t="inlineStr">
+      <c r="K156" t="inlineStr">
         <is>
           <t>By XUEYING CHEN '16 and GRACE BENNETT-PIERRE '16&lt;br/&gt;Co-Editor-in-Chief and Staff Writer&lt;br/&gt;Students marched in two protests on Saturday at the Seven Sisters Latin@ Conference in Pendleton Atrium and yesterday in Green Hall. Wellesley Academic Action Movement-Siblings Leading Action for Multiculturalism (WAAM-SLAM2) organized the protests. WAAM-SLAM2 is a joint effort of Latin@s Unidas Changing Academia and students from the Ethnic Studies Conference committee. The movement actively pushes for the implementation of a Latin@ studies minor, as part of a broader effort to introduce an ethnic studies major into the academic curriculum.&lt;br/&gt;On Saturday, the College hosted the second annual Seven Sisters Latin@ Conference. The student coordinators of the conference, who are not affiliated with WAAM-SLAM2, invited President of the College H. Kim Bottomly to speak. She briefly welcomed attendees, some of whom traveled from Smith College, and thanked the conference organizers.&lt;br/&gt;"I'd just like to say that I can't stay for today, but I hope the organizers will report back to me about the things that you've discussed and really the critical issues that you are facing as you go forward as students," she said.&lt;br/&gt;After Bottomly left the podium, nearly 50 students silently marched into Pendleton Atrium carrying posters, some of which read "Where is our Latin@ house?" and "We're done waiting." The students formed a circle around Bottomly as she read all of the signs with a smile before she exited the atrium. Some students had taped their mouths shut to represent how they feel silenced at Wellesley.&lt;br/&gt;The organizers of WAAM-SLAM2 have chosen to remain anonymous because they believe any statement or action made belongs to the movement and not to any individual student.&lt;br/&gt;According to the movement organizers, the administration has stated if they introduce Latin@ studies or ethnic studies, they must also implement Queer studies or Native American studies out of fairness for other marginalized groups. They also emphasized that hiring new faculty for ethnic studies could affect financial aid.&lt;br/&gt;"The administration has promoted circular, unproductive dialogue as a tactic to put off necessary action," the student organizers wrote in a statement to The Wellesley News. "Wellesley continues attempting to appease and silence the student body by making it appear as though they are doing everything in their power."&lt;br/&gt;While Bottomly does not directly handle curriculum affairs, WAAM-SLAM2 held a protest after her remarks because they believe that such an influential overseer of the College should directly hear their concerns and know how to address them.&lt;br/&gt;WAAM-SLAM2 released its Transformation Justice and Education Bill for Wellesley College, a document of demands addressed to the administration. In the bill, student organizers of WAAM-SLAM2 asked for various commitments, including multicultural spaces, a commitment to meet the needs of students with disabilities and LGBTQ students and divestment from fossil fuels.&lt;br/&gt;A second protest took place yesterday during the lunch hour, when approximately 60 students marched to the administrative offices. The students chanted a passage from the bill describing the WAAM-SLAM2 mission as they moved from the offices of Bottomly and Provost Andrew Shennan, both of whom were attending meetings elsewhere, to the office of Richard French, dean of academic affairs.&lt;br/&gt;Student protesters asked French to read the 15-page document detailing their demands for the College and to then sign a statement committing himself to the completion of the listed goals, including the creation of Latin@ studies minor and ethnic studies major.&lt;br/&gt;French said he read the document before the students' arrived and began the exchange by stating his intention to engage in dialogue about the issues brought forth by WAAM-SLAM2.&lt;br/&gt;"My door is always open as many of you know; you said that dialogue and resistance are both legitimate. I cannot resist, but I can certainly engage in dialogue," French said.&lt;br/&gt;However, French refused to sign the final page of the document, citing his unwillingness to make an empty promise to students because he does not have the means to change the curriculum on his own. At the same time, he voiced his sympathy for the movement and mentioned that he has worked tirelessly on the possible introduction of ethnic studies for the past year.&lt;br/&gt;"I encourage people to continue to work with me, but working with me is not saying there are 40 people outside my office, and we refuse to let you leave until you sign a document I haven't read for more than 30 seconds," French said.&lt;br/&gt;When asked about the lack of multicultural spaces on campus, French emphasized that he is not solely responsible for all of the decisions made at the College, particularly those decisions unrelated to academic programs.&lt;br/&gt;"I am a member of the faculty, a member of the administration, who does not have absolute authority over almost any of these things here," French said. "I am, however, in conversation with the senior staff, with the deans of students, with other deans, and we will discuss these in a thoughtful way and respond to you, but I cannot give you a unilateral response right now."&lt;br/&gt;Following their exchange with French, a core group of students read a response summarizing their expectations for action on the part of the administration.&lt;br/&gt;"We refuse to conform to a system that is broken and inadequate, we will not accept any excuses from the administration, nor will we tolerate any further implied threats that would disproportionately affect targeted groups of students," they stated. "We demand that the claims of student prioritization and diversification be accomplished by the implementation of the action previously outlined."&lt;br/&gt;The students thanked French and began to move out of the hallway.&lt;br/&gt;Before students vacated Green Hall, Dean of Faculty Affairs Kathryn Lynch asked that students stop calling her at home with messages about the issue.&lt;br/&gt;"I have been called in the middle of the night, in my home, waking me and my entire family up and terrorizing us. Please stop," Lynch said. Lynch received phone calls in the middle of the night, which frightened her family because certain members have existing medical conditions.&lt;br/&gt;Over the weekend, the movement conducted a call campaign. The flyers distributed by WAAM-SLAM2 organizers to promote Saturday's protest also listed the phone numbers of Bottomly, Shennan, French and Lynch. Although the other phone numbers listed were office lines, Lynch's home phone number was included on the flyer.&lt;br/&gt;WAAM-SLAM2 supporters left the administrators voicemail messages urging them to establish more ethnic studies courses. The organizers did not intend to contact Lynch at home, but found the number listed as a campus number in the College directory. The original script of the messages does not include any threats and ends with, "This is a fight that is over 40 years old. We are done waiting. Thank you for your consideration."&lt;br/&gt;WAAM-SLAM2 stems from the first WAAM-SLAM movement, which occurred in 2001. More than a decade ago, Wellesley students held rallies, sit-ins, letter campaigns and meetings with the administration to secure full-time advisors for students of Asian and Latin@ descent and protest the the denial of Professor Elena Creef's tenure in women's and gender studies department. The College did not meet all the demands published by WAAM-SLAM in 2001, including the installation of a space for students of Asian descent, a demand which was first voiced in 1988.&lt;br/&gt; "It's really important to show that this is not a movement that sprung up overnight. This has happened for decades at this college, and we are simply revitalizing an old movement while adding new demands," the WAAM-SLAM2 organizers wrote in the statement.&lt;br/&gt;The student organizers believe that the movement will continue far into the future. While they will focus mainly on ethnic studies, the coordinators recognize that many other issues also exist at Wellesley.&lt;br/&gt;"Back in 2001, [we] imagine no one really thought WAAM-SLAM would continue," the organizers said. "The fact that it continues today, 14 years later, is a testament to the power of activism that is alive in all students."&lt;br/&gt;WAAM-SLAM2 will host an information session open to all members of the College community later today at 5:30 p.m. in Munger Hall.</t>
         </is>
+      </c>
+      <c r="L156" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -7288,10 +7763,13 @@
           <t>University governance, admin, policies, programs, curriculum, Campus climate</t>
         </is>
       </c>
-      <c r="J157" t="inlineStr">
+      <c r="K157" t="inlineStr">
         <is>
           <t>By XUEYING CHEN '16 and GRACE BENNETT-PIERRE '16&lt;br/&gt;Co-Editor-in-Chief and Staff Writer&lt;br/&gt;Students marched in two protests on Saturday at the Seven Sisters Latin@ Conference in Pendleton Atrium and yesterday in Green Hall. Wellesley Academic Action Movement-Siblings Leading Action for Multiculturalism (WAAM-SLAM2) organized the protests. WAAM-SLAM2 is a joint effort of Latin@s Unidas Changing Academia and students from the Ethnic Studies Conference committee. The movement actively pushes for the implementation of a Latin@ studies minor, as part of a broader effort to introduce an ethnic studies major into the academic curriculum.&lt;br/&gt;On Saturday, the College hosted the second annual Seven Sisters Latin@ Conference. The student coordinators of the conference, who are not affiliated with WAAM-SLAM2, invited President of the College H. Kim Bottomly to speak. She briefly welcomed attendees, some of whom traveled from Smith College, and thanked the conference organizers.&lt;br/&gt;"I'd just like to say that I can't stay for today, but I hope the organizers will report back to me about the things that you've discussed and really the critical issues that you are facing as you go forward as students," she said.&lt;br/&gt;After Bottomly left the podium, nearly 50 students silently marched into Pendleton Atrium carrying posters, some of which read "Where is our Latin@ house?" and "We're done waiting." The students formed a circle around Bottomly as she read all of the signs with a smile before she exited the atrium. Some students had taped their mouths shut to represent how they feel silenced at Wellesley.&lt;br/&gt;The organizers of WAAM-SLAM2 have chosen to remain anonymous because they believe any statement or action made belongs to the movement and not to any individual student.&lt;br/&gt;According to the movement organizers, the administration has stated if they introduce Latin@ studies or ethnic studies, they must also implement Queer studies or Native American studies out of fairness for other marginalized groups. They also emphasized that hiring new faculty for ethnic studies could affect financial aid.&lt;br/&gt;"The administration has promoted circular, unproductive dialogue as a tactic to put off necessary action," the student organizers wrote in a statement to The Wellesley News. "Wellesley continues attempting to appease and silence the student body by making it appear as though they are doing everything in their power."&lt;br/&gt;While Bottomly does not directly handle curriculum affairs, WAAM-SLAM2 held a protest after her remarks because they believe that such an influential overseer of the College should directly hear their concerns and know how to address them.&lt;br/&gt;WAAM-SLAM2 released its Transformation Justice and Education Bill for Wellesley College, a document of demands addressed to the administration. In the bill, student organizers of WAAM-SLAM2 asked for various commitments, including multicultural spaces, a commitment to meet the needs of students with disabilities and LGBTQ students and divestment from fossil fuels.&lt;br/&gt;A second protest took place yesterday during the lunch hour, when approximately 60 students marched to the administrative offices. The students chanted a passage from the bill describing the WAAM-SLAM2 mission as they moved from the offices of Bottomly and Provost Andrew Shennan, both of whom were attending meetings elsewhere, to the office of Richard French, dean of academic affairs.&lt;br/&gt;Student protesters asked French to read the 15-page document detailing their demands for the College and to then sign a statement committing himself to the completion of the listed goals, including the creation of Latin@ studies minor and ethnic studies major.&lt;br/&gt;French said he read the document before the students' arrived and began the exchange by stating his intention to engage in dialogue about the issues brought forth by WAAM-SLAM2.&lt;br/&gt;"My door is always open as many of you know; you said that dialogue and resistance are both legitimate. I cannot resist, but I can certainly engage in dialogue," French said.&lt;br/&gt;However, French refused to sign the final page of the document, citing his unwillingness to make an empty promise to students because he does not have the means to change the curriculum on his own. At the same time, he voiced his sympathy for the movement and mentioned that he has worked tirelessly on the possible introduction of ethnic studies for the past year.&lt;br/&gt;"I encourage people to continue to work with me, but working with me is not saying there are 40 people outside my office, and we refuse to let you leave until you sign a document I haven't read for more than 30 seconds," French said.&lt;br/&gt;When asked about the lack of multicultural spaces on campus, French emphasized that he is not solely responsible for all of the decisions made at the College, particularly those decisions unrelated to academic programs.&lt;br/&gt;"I am a member of the faculty, a member of the administration, who does not have absolute authority over almost any of these things here," French said. "I am, however, in conversation with the senior staff, with the deans of students, with other deans, and we will discuss these in a thoughtful way and respond to you, but I cannot give you a unilateral response right now."&lt;br/&gt;Following their exchange with French, a core group of students read a response summarizing their expectations for action on the part of the administration.&lt;br/&gt;"We refuse to conform to a system that is broken and inadequate, we will not accept any excuses from the administration, nor will we tolerate any further implied threats that would disproportionately affect targeted groups of students," they stated. "We demand that the claims of student prioritization and diversification be accomplished by the implementation of the action previously outlined."&lt;br/&gt;The students thanked French and began to move out of the hallway.&lt;br/&gt;Before students vacated Green Hall, Dean of Faculty Affairs Kathryn Lynch asked that students stop calling her at home with messages about the issue.&lt;br/&gt;"I have been called in the middle of the night, in my home, waking me and my entire family up and terrorizing us. Please stop," Lynch said. Lynch received phone calls in the middle of the night, which frightened her family because certain members have existing medical conditions.&lt;br/&gt;Over the weekend, the movement conducted a call campaign. The flyers distributed by WAAM-SLAM2 organizers to promote Saturday's protest also listed the phone numbers of Bottomly, Shennan, French and Lynch. Although the other phone numbers listed were office lines, Lynch's home phone number was included on the flyer.&lt;br/&gt;WAAM-SLAM2 supporters left the administrators voicemail messages urging them to establish more ethnic studies courses. The organizers did not intend to contact Lynch at home, but found the number listed as a campus number in the College directory. The original script of the messages does not include any threats and ends with, "This is a fight that is over 40 years old. We are done waiting. Thank you for your consideration."&lt;br/&gt;WAAM-SLAM2 stems from the first WAAM-SLAM movement, which occurred in 2001. More than a decade ago, Wellesley students held rallies, sit-ins, letter campaigns and meetings with the administration to secure full-time advisors for students of Asian and Latin@ descent and protest the the denial of Professor Elena Creef's tenure in women's and gender studies department. The College did not meet all the demands published by WAAM-SLAM in 2001, including the installation of a space for students of Asian descent, a demand which was first voiced in 1988.&lt;br/&gt; "It's really important to show that this is not a movement that sprung up overnight. This has happened for decades at this college, and we are simply revitalizing an old movement while adding new demands," the WAAM-SLAM2 organizers wrote in the statement.&lt;br/&gt;The student organizers believe that the movement will continue far into the future. While they will focus mainly on ethnic studies, the coordinators recognize that many other issues also exist at Wellesley.&lt;br/&gt;"Back in 2001, [we] imagine no one really thought WAAM-SLAM would continue," the organizers said. "The fact that it continues today, 14 years later, is a testament to the power of activism that is alive in all students."&lt;br/&gt;WAAM-SLAM2 will host an information session open to all members of the College community later today at 5:30 p.m. in Munger Hall.</t>
         </is>
+      </c>
+      <c r="L157" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="158">
@@ -7331,10 +7809,13 @@
           <t>University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J158" t="inlineStr">
+      <c r="K158" t="inlineStr">
         <is>
           <t>By XUEYING CHEN '16 and GRACE BENNETT-PIERRE '16&lt;br/&gt;Co-Editor-in-Chief and Staff Writer&lt;br/&gt;Students marched in two protests on Saturday at the Seven Sisters Latin@ Conference in Pendleton Atrium and yesterday in Green Hall. Wellesley Academic Action Movement-Siblings Leading Action for Multiculturalism (WAAM-SLAM2) organized the protests. WAAM-SLAM2 is a joint effort of Latin@s Unidas Changing Academia and students from the Ethnic Studies Conference committee. The movement actively pushes for the implementation of a Latin@ studies minor, as part of a broader effort to introduce an ethnic studies major into the academic curriculum.&lt;br/&gt;On Saturday, the College hosted the second annual Seven Sisters Latin@ Conference. The student coordinators of the conference, who are not affiliated with WAAM-SLAM2, invited President of the College H. Kim Bottomly to speak. She briefly welcomed attendees, some of whom traveled from Smith College, and thanked the conference organizers.&lt;br/&gt;"I'd just like to say that I can't stay for today, but I hope the organizers will report back to me about the things that you've discussed and really the critical issues that you are facing as you go forward as students," she said.&lt;br/&gt;After Bottomly left the podium, nearly 50 students silently marched into Pendleton Atrium carrying posters, some of which read "Where is our Latin@ house?" and "We're done waiting." The students formed a circle around Bottomly as she read all of the signs with a smile before she exited the atrium. Some students had taped their mouths shut to represent how they feel silenced at Wellesley.&lt;br/&gt;The organizers of WAAM-SLAM2 have chosen to remain anonymous because they believe any statement or action made belongs to the movement and not to any individual student.&lt;br/&gt;According to the movement organizers, the administration has stated if they introduce Latin@ studies or ethnic studies, they must also implement Queer studies or Native American studies out of fairness for other marginalized groups. They also emphasized that hiring new faculty for ethnic studies could affect financial aid.&lt;br/&gt;"The administration has promoted circular, unproductive dialogue as a tactic to put off necessary action," the student organizers wrote in a statement to The Wellesley News. "Wellesley continues attempting to appease and silence the student body by making it appear as though they are doing everything in their power."&lt;br/&gt;While Bottomly does not directly handle curriculum affairs, WAAM-SLAM2 held a protest after her remarks because they believe that such an influential overseer of the College should directly hear their concerns and know how to address them.&lt;br/&gt;WAAM-SLAM2 released its Transformation Justice and Education Bill for Wellesley College, a document of demands addressed to the administration. In the bill, student organizers of WAAM-SLAM2 asked for various commitments, including multicultural spaces, a commitment to meet the needs of students with disabilities and LGBTQ students and divestment from fossil fuels.&lt;br/&gt;A second protest took place yesterday during the lunch hour, when approximately 60 students marched to the administrative offices. The students chanted a passage from the bill describing the WAAM-SLAM2 mission as they moved from the offices of Bottomly and Provost Andrew Shennan, both of whom were attending meetings elsewhere, to the office of Richard French, dean of academic affairs.&lt;br/&gt;Student protesters asked French to read the 15-page document detailing their demands for the College and to then sign a statement committing himself to the completion of the listed goals, including the creation of Latin@ studies minor and ethnic studies major.&lt;br/&gt;French said he read the document before the students' arrived and began the exchange by stating his intention to engage in dialogue about the issues brought forth by WAAM-SLAM2.&lt;br/&gt;"My door is always open as many of you know; you said that dialogue and resistance are both legitimate. I cannot resist, but I can certainly engage in dialogue," French said.&lt;br/&gt;However, French refused to sign the final page of the document, citing his unwillingness to make an empty promise to students because he does not have the means to change the curriculum on his own. At the same time, he voiced his sympathy for the movement and mentioned that he has worked tirelessly on the possible introduction of ethnic studies for the past year.&lt;br/&gt;"I encourage people to continue to work with me, but working with me is not saying there are 40 people outside my office, and we refuse to let you leave until you sign a document I haven't read for more than 30 seconds," French said.&lt;br/&gt;When asked about the lack of multicultural spaces on campus, French emphasized that he is not solely responsible for all of the decisions made at the College, particularly those decisions unrelated to academic programs.&lt;br/&gt;"I am a member of the faculty, a member of the administration, who does not have absolute authority over almost any of these things here," French said. "I am, however, in conversation with the senior staff, with the deans of students, with other deans, and we will discuss these in a thoughtful way and respond to you, but I cannot give you a unilateral response right now."&lt;br/&gt;Following their exchange with French, a core group of students read a response summarizing their expectations for action on the part of the administration.&lt;br/&gt;"We refuse to conform to a system that is broken and inadequate, we will not accept any excuses from the administration, nor will we tolerate any further implied threats that would disproportionately affect targeted groups of students," they stated. "We demand that the claims of student prioritization and diversification be accomplished by the implementation of the action previously outlined."&lt;br/&gt;The students thanked French and began to move out of the hallway.&lt;br/&gt;Before students vacated Green Hall, Dean of Faculty Affairs Kathryn Lynch asked that students stop calling her at home with messages about the issue.&lt;br/&gt;"I have been called in the middle of the night, in my home, waking me and my entire family up and terrorizing us. Please stop," Lynch said. Lynch received phone calls in the middle of the night, which frightened her family because certain members have existing medical conditions.&lt;br/&gt;Over the weekend, the movement conducted a call campaign. The flyers distributed by WAAM-SLAM2 organizers to promote Saturday's protest also listed the phone numbers of Bottomly, Shennan, French and Lynch. Although the other phone numbers listed were office lines, Lynch's home phone number was included on the flyer.&lt;br/&gt;WAAM-SLAM2 supporters left the administrators voicemail messages urging them to establish more ethnic studies courses. The organizers did not intend to contact Lynch at home, but found the number listed as a campus number in the College directory. The original script of the messages does not include any threats and ends with, "This is a fight that is over 40 years old. We are done waiting. Thank you for your consideration."&lt;br/&gt;WAAM-SLAM2 stems from the first WAAM-SLAM movement, which occurred in 2001. More than a decade ago, Wellesley students held rallies, sit-ins, letter campaigns and meetings with the administration to secure full-time advisors for students of Asian and Latin@ descent and protest the the denial of Professor Elena Creef's tenure in women's and gender studies department. The College did not meet all the demands published by WAAM-SLAM in 2001, including the installation of a space for students of Asian descent, a demand which was first voiced in 1988.&lt;br/&gt; "It's really important to show that this is not a movement that sprung up overnight. This has happened for decades at this college, and we are simply revitalizing an old movement while adding new demands," the WAAM-SLAM2 organizers wrote in the statement.&lt;br/&gt;The student organizers believe that the movement will continue far into the future. While they will focus mainly on ethnic studies, the coordinators recognize that many other issues also exist at Wellesley.&lt;br/&gt;"Back in 2001, [we] imagine no one really thought WAAM-SLAM would continue," the organizers said. "The fact that it continues today, 14 years later, is a testament to the power of activism that is alive in all students."&lt;br/&gt;WAAM-SLAM2 will host an information session open to all members of the College community later today at 5:30 p.m. in Munger Hall.</t>
         </is>
+      </c>
+      <c r="L158" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="159">
@@ -7379,10 +7860,13 @@
           <t>University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J159" t="inlineStr">
+      <c r="K159" t="inlineStr">
         <is>
           <t>Student coalition brainstorms next steps&lt;br/&gt;By XUEYING CHEN '16&lt;br/&gt;Co Editor-in-Chief&lt;br/&gt;Hannah Degner '15 Staff Photographer&lt;br/&gt;WAAM-SLAM2 assembled a teach in with the College community last Friday after student representatives met with Wellesley College President H. Kim Bottomly the previous day.&lt;br/&gt;The movement protested twice last month to demand that the administration incorporate a Latin@ minor and ethnic studies major.&lt;br/&gt;At the meeting last Thursday, students from WAAM-SLAM2 presented to Bottomly the demands listed in their Transformative Justice and Education Bill for Wellesley College. Provost Andy Shennan, provost of the College; Debra DeMeis, dean of students, Robbin Chapman, associate provost and academic director of diversity; Ben Hammond, vice president for finance and administration and Jennifer Desjarlais, director of admission and financial aid, attended as well.&lt;br/&gt;The administration did not allow reporters to attend the meeting, but WAAM-SLAM2 expects to release a response at the end of next week on their Facebook page.&lt;br/&gt;The student organizers of WAAM-SLAM2 intended to inform and involve more students in the movement after meeting with Bottomly. More than 70 people attended the teach in hosted in the Clapp Library Lecture Room. The meeting opened and closed with a unity clap, which starts out slow and speeds up into collective applause and cheering. According to the organizers of WAAM-SLAM2, the College union workers use this clap to open their own meetings.&lt;br/&gt;The organizers introduced attendees to the recent history of the movement, beginning with the open letter students wrote to the administration demanding ethnic studies a little more than a year ago. Many of the letter drafters graduated, and the College did not respond. After an ethnic studies conference took place on campus, Dean of Academic Affairs Richard French established a faculty working committee in February. The committee is chaired by Professor of English and Director of American Studies Yoon Sun Lee, to explore ethnic studies in more depth.&lt;br/&gt;The faculty working group invited students to take an active part in the discussion, but disagreements arose. Some faculty members wanted to focus on ethnic minorities in other countries, instead of the students' intention to implement an interdepartmental major concentrated on the experiences of U.S. ethnic minorities.&lt;br/&gt;French released an update yesterday on the progress of the faculty working group due to the campus-wide interest.&lt;br/&gt;The faculty working group recommended the introduction of a Latin@ studies minor as well as the creation of a comparative race studies focus on U.S. ethnic minorities within the American studies program.&lt;br/&gt;"[They] recommend further consideration of a structured individual major or minor in Global/Transnational Ethnic Studies," French wrote. "Such an option would complement the U.S.-focused ethnic studies offered in American Studies."&lt;br/&gt;The working group also identified the need to create a tenure-track position to teach the Latin@ studies introductory course and to recruit existing faculty to teach other courses for the minor. Over the next academic year, the American studies department and working group plans to write a detailed proposal for the Latin@ studies minor and a comparative race studies focus, as well as to introduce an experimental introductory course on ethnic minorities around the world.&lt;br/&gt;"The time has come for a well-considered clarification and expansion of ethnic studies at Wellesley," French stated in the announcement.&lt;br/&gt;Nancy Negrete '14, a student representative of WAAM-SLAM2, expressed that the coalition responded positively to the faculty discussion, but still has issues with the recommendations in French's statement.&lt;br/&gt;She says that the announcement fails to mention who will take charge of the Latin@ studies minor proposal as well as a detailed timeline of the process. Negrete also states that the faculty working group does not elaborate on U.S.-based ethnic studies nor mention hiring a professor specialized in the field.&lt;br/&gt;"We want a U.S.-based interdepartmental ethnic studies major and welcome courses that are transnational in focus because we recognize this as an emerging focus within ethnic studies," Negrete said. "But such courses should serve to complement the study of racialized experiences of minorities in America."&lt;br/&gt;She also pointed out that students never asked for transnational ethnic studies structured individual major.&lt;br/&gt;While Negrete is speaking on behalf of WAAM-SLAM2, its organizers would like to stress that any statement or action made belongs to the movement and not as any individual student.&lt;br/&gt;"We do commend the faculty working group and administration for their work, and this response is in no means against their efforts or all the work they have put in," Negrete said.&lt;br/&gt;An attendee at the teach in also asked why the student organizers chose to incorporate fossil fuel divestment as a demand. The student organizers responded that choosing not the divest from fossil fuels equates to environmental racism because certain groups, especially marginalized communities, live in the areas most affected by pollution.&lt;br/&gt;Several students who attended the teach in wanted WAAM-SLAM2 to specify how the coalition will measure its goals.&lt;br/&gt;"The administration has continued to show a lack of willingness to actually efficiently work with students when they bring up significant problems on campus. So it becomes necessary that students to stand up for themselves," Claire Mildrum '15 said. "I support the movement but want some clarification on what determines success."&lt;br/&gt;Throughout the meeting, supporters of the movement spoke up and reminded attendees of the barriers the administration have created to slow down the implementation of ethnic studies. According to the organizers of WAAM-SLAM2, the administration has voiced doubts about being able to hire a new qualified Latin@ professor to teach Latin@ studies.&lt;br/&gt;The organizers also referenced the effectiveness of the first WAAM-SLAM movement that occurred 2001. They claimed that nearly 300 students actively supported the original coalition and completed a 24-hour sit in demonstration in Green Hall. The College satisfied some of their demands after WAAM-SLAM threatened a hunger strike by sending press releases to national media outlets.&lt;br/&gt;Near the end of the teach in, supporters broke into groups to brainstorm ideas for WAAM-SLAM2 to strengthen its visibility throughout the College community. The coalition is currently finding ways to involve student organizations across campus and seeking the support of alumni.&lt;br/&gt;Editor's note: An earlier version of this story incorrectly stated faculty recommended the introduction of a Latin@ studies major as well as the creation of a comparative race studies course focused on U.S. ethnic minorities within the American studies department. More accurately, the faculty working group recommended the introduction of a Latin@ studies minor and a comparative race studies focus in the American studies program.About these adsdiv.wpa&gt;div { margin-top: 1em; } #google_ads_div_wpcom_below_post_adsafe_ad_container { display: block !important; }</t>
         </is>
+      </c>
+      <c r="L159" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="160">
@@ -7422,10 +7906,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J160" t="inlineStr">
+      <c r="K160" t="inlineStr">
         <is>
           <t>A human oil spill spread across Dwinelle Plaza on Monday - a silent demonstration against fracking that is the first in a series of events to kick-start Earth Week 2014.&lt;br/&gt;The day after the four-year anniversary of the BP oil spill, about 20 students, clad entirely in black, circled and sprawled around a miniature wooden oil rig covered with protest signs. Protesters wanted to illustrate the environmental effects of fracking by using human bodies as symbols of the devastation.&lt;br/&gt;"An oil spill is a very visible and recognizable example of the corruption and destruction wrought by the fossil fuel industry," said Jake Soiffer, a freshman and an actions coordinator at Fossil Free Cal, in an email. "The details - lying on the floor, wearing all black - bring out the serious, pressing nature of the issue."&lt;br/&gt;Fracking, also known as hydraulic fracturing, involves extracting natural gas and oil by injecting water, sand and chemicals - many of them toxic - into underground shell rock.&lt;br/&gt;The protest, which was planned and sponsored by Students Against Fracking and by Fossil Free Cal, comes a month after a similar demonstration on Sproul to pressure Gov. Jerry Brown into banning fracking in California. Like last month's protest, students Monday aimed to raise awareness of fracking - but, this time, through a symbolic display.&lt;br/&gt;Suspended from the 12-foot-tall small-scale oil rig was a list of chemicals involved in fracking operations that are injected into bedrock to break it up. At the foot of the rig were students, quietly reclining on the ground.&lt;br/&gt;The protest then kicked into another gear as a student protester wielded a megaphone, chanting "leave the oil in the soil" and "hey hey, ho ho, Keystone XL has to go."&lt;br/&gt;The protest is the first of many events in UC Berkeley's annual Earth Week festival, sponsored and organized by the ASUC Sustainability Team. The week - which lasts through Sunday - is designed to spread awareness on environmental issues and is filled with events that promote discussions on ecological issues and teach what it means to lead a sustainable lifestyle.&lt;br/&gt;Founded at the beginning of this semester, Students Against Fracking focuses primarily on leading an educational campaign around campus. The organization will continue to work in solidarity with Fossil Free Cal, a campus group campaigning for the UC Board of Regents to divest from the fossil fuel industry.&lt;br/&gt;Kristy Drutman, a freshman and co-coordinator for Students Against Fracking, said the organization will begin to take a bigger step forward in their environmental campaign on campus by starting a petition. The petition would pressure Brown to approve a potential bill come November that would pause fracking in California to allow for further scientific research on the cost-effectiveness of fracking.&lt;br/&gt;In addition, Fossil Free Cal is now looking to broaden student support, connect with local environmental groups and pass a resolution through the ASUC.&lt;br/&gt;Contact Bo Kovitz at [email protected] and follow her on Twitter @beau_etc.</t>
         </is>
+      </c>
+      <c r="L160" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -7465,10 +7952,13 @@
           <t>Anti-colonial/political independence</t>
         </is>
       </c>
-      <c r="J161" t="inlineStr">
+      <c r="K161" t="inlineStr">
         <is>
           <t>The practice of protesting commencement speakers is nothing new, but rarely in recent memory have these protests been as widespread and as solicitous of public attention as they have been this spring.&lt;br/&gt;It all started April 8, when administrators at Brandeis University, acting under pressure from undergraduates and faculty members, rescinded a commencement invitation to Ayaan Hirsi Ali, a noted women's rights advocate and strident critic of Islam. To most students, the rescindment seemed prudent, and the original invitation almost inexplicable. Ali, after all, had called Islam a "destructive, nihilistic cult of death" in an interview with the London Evening Standard in 2007, and many of her statements continue to be overtly Islamphobic.&lt;br/&gt;But the commencement rows that would follow in the coming weeks seemed far more frivolous, in that these protests were not based in opposition to personal bigotry, but rather in opposition to specific political policies that were not, on their face, tied to intolerance.&lt;br/&gt;On May 4, for instance, former Secretary of State Condoleezza Rice, facing student protest at Rutgers as a result of her involvement in the Iraq War and her approval of waterboarding war detainees, decided not to attend the school's ceremony, as she feared that the contentious atmosphere surrounding her visit would subtract from the collegial atmosphere of graduation. Though she withdrew voluntarily, it was clear she felt intellectually bullied. "I am honored to have served my country," she said on May 5. "I have defended America's belief in free speech and the exchange of ideas."&lt;br/&gt;Christine LaGarde: Is she really that evil? (AP/Cliff Owen)&lt;br/&gt;Christine LaGarde, the current managing director of the IMF and a noted labor and antitrust lawyer before she entered the public sector, was the next commencement speaker to come under fire. Petitioners at Smith College, students and faculty alike, rallied to disinvite her, accusing the IMF of "imperialistic" policies, while conceding that LaGarde may herself be a "good person." Soon LaGarde withdrew for the same reasons as Rice.&lt;br/&gt;A few days later, students at Haverford pressured former University of California chancellor Robert C. Birgeneau into withdrawing from its commencement ceremonies because he initially supported the police response to a heated 2011 Occupy Berkeley incident. (The fact that he condemned the police and called for an immediate investigation after seeing video footage of the altercation a few days later meant little to the protestors.)&lt;br/&gt;And, recently, a similar debate also penetrated Harvard's campus: at the Graduate School of Education, petitioners attempted a putsch against Colorado State Senator Michael C. Johnston-who fortunately did speak at commencement-on the basis of his support for "test-based accountability" for teachers.&lt;br/&gt;Among the commentariat, save in the most liberal journals, pundits and editorial boards have come down against these protesting students, describing their meta-movement as a harbinger of "rising liberal intolerance" on campus. And though student papers, including the Crimson, have defended the protests, it seems to me that the mainstream media is at least partially right. Birgeneau, who himself has a history of liberal, nonviolent protest, hardly seems like a controversial figure. Neither does LaGarde, who in many respects would be considered something of a lefty in Amercan political circles, even if the organization she now heads is associated with neoliberal economics. New York City police commissioner Ray Kelly treads more contentious ground, but the refusal of Brown students to let him speak at a forum and Q&amp;A last semester-which is far from a commencement speech-struck many, including myself, as close-minded.&lt;br/&gt;Those supporting these student protests frame the issue as one of free speech: they have a right, under this principle, to fight "speech with speech"-and their speech happens to take the form of protest. I wholeheartedly agree with this principle, but this argument misses the point.&lt;br/&gt;Though we certainly have a right, and, at times, a responsibility to protest, the issue here is the effect of the protest, not the legitimacy of the method. And here the effect is too often sealing our campuses off from the policies that vocal students disagree with-limiting our politics to a very narrow kind of campus liberalism.&lt;br/&gt;In the protestors' defense, a commencement address is not just another forum on campus; the selected speaker should not denigrate a certain people or ethnicity during their speech, as graduates of all stripes should be able to attend without their personal dignity being called into question. That's why I agree with Brandeis' rejection of Hirsi Ali.&lt;br/&gt;But specific policy disagreements-unless they are predicated on racist or overtly discriminatory sentiment-should not be a basis for disinvitation. Like most campus communities, our community is far too intellectually diverse to avoid this kind of conflict, and-as most students who've engaged in political debate with peers will attest-non-bigoted, intellectually rigorous arguments from the other side of the political spectrum are often the most informative, and almost always the most challenging.&lt;br/&gt;For me, it feels strange to oppose student protest, as I appreciate and support the work of SLAM, SJSF, Divest and a number of other activist groups on campus. In other words, I mostly share the politics of the protestors I'm critiquing. But here I do have one profound disagreement: while a commencement speaker must be intellectually accomplished and adhere to basic principles of tolerance, he or she does not need to agree with my politics.</t>
         </is>
+      </c>
+      <c r="L161" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="162">
@@ -7508,10 +7998,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J162" t="inlineStr">
+      <c r="K162" t="inlineStr">
         <is>
           <t>A human oil spill spread across Dwinelle Plaza on Monday - a silent demonstration against fracking that is the first in a series of events to kick-start Earth Week 2014.&lt;br/&gt;The day after the four-year anniversary of the BP oil spill, about 20 students, clad entirely in black, circled and sprawled around a miniature wooden oil rig covered with protest signs. Protesters wanted to illustrate the environmental effects of fracking by using human bodies as symbols of the devastation.&lt;br/&gt;"An oil spill is a very visible and recognizable example of the corruption and destruction wrought by the fossil fuel industry," said Jake Soiffer, a freshman and an actions coordinator at Fossil Free Cal, in an email. "The details - lying on the floor, wearing all black - bring out the serious, pressing nature of the issue."&lt;br/&gt;Fracking, also known as hydraulic fracturing, involves extracting natural gas and oil by injecting water, sand and chemicals - many of them toxic - into underground shell rock.&lt;br/&gt;The protest, which was planned and sponsored by Students Against Fracking and by Fossil Free Cal, comes a month after a similar demonstration on Sproul to pressure Gov. Jerry Brown into banning fracking in California. Like last month's protest, students Monday aimed to raise awareness of fracking - but, this time, through a symbolic display.&lt;br/&gt;Suspended from the 12-foot-tall small-scale oil rig was a list of chemicals involved in fracking operations that are injected into bedrock to break it up. At the foot of the rig were students, quietly reclining on the ground.&lt;br/&gt;The protest then kicked into another gear as a student protester wielded a megaphone, chanting "leave the oil in the soil" and "hey hey, ho ho, Keystone XL has to go."&lt;br/&gt;The protest is the first of many events in UC Berkeley's annual Earth Week festival, sponsored and organized by the ASUC Sustainability Team. The week - which lasts through Sunday - is designed to spread awareness on environmental issues and is filled with events that promote discussions on ecological issues and teach what it means to lead a sustainable lifestyle.&lt;br/&gt;Founded at the beginning of this semester, Students Against Fracking focuses primarily on leading an educational campaign around campus. The organization will continue to work in solidarity with Fossil Free Cal, a campus group campaigning for the UC Board of Regents to divest from the fossil fuel industry.&lt;br/&gt;Kristy Drutman, a freshman and co-coordinator for Students Against Fracking, said the organization will begin to take a bigger step forward in their environmental campaign on campus by starting a petition. The petition would pressure Brown to approve a potential bill come November that would pause fracking in California to allow for further scientific research on the cost-effectiveness of fracking.&lt;br/&gt;In addition, Fossil Free Cal is now looking to broaden student support, connect with local environmental groups and pass a resolution through the ASUC.&lt;br/&gt;Contact Bo Kovitz at [email protected] and follow her on Twitter @beau_etc.</t>
         </is>
+      </c>
+      <c r="L162" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="163">
@@ -7551,10 +8044,13 @@
           <t>Pro-Palestine/BDS, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J163" t="inlineStr">
+      <c r="K163" t="inlineStr">
         <is>
           <t>In recent months, colleges across the country have seen a spate of demonstrations regarding issues of identity, with students demanding greater inclusivity on their campuses. Many resemble Dartmouth's April "Freedom Budget" protests, when over a dozen students occupied College President Phil Hanlon's office for two days, demanding a point-by-point response to a list of over 70 demands regarding issues of diversity.&lt;br/&gt;In the last year, students at Princeton University, Harvard University, Oberlin College, Mills College, University of Michigan, City University of New York, Mount Holyoke College and University of California at Los Angeles, among others, have initiated protests concerning similar issues. Melissa Padilla '16, who was involved in the "Freedom Budget" protest, said she communicated with her friends who were involved with similar protests at other schools, including New York University and University of Texas at Austin, during the construction of the "Freedom Budget" and the sit-in. Other Dartmouth activists spoke with friends on various campuses as well, she said. The protest at Dartmouth, she said, was not a reaction to movements at other schools but a response to discrimination at the College. "A lot of universities are looking to be more inclusive but are acting very unlike their statements," Padilla said. "There's a big gap between their mission statements and the actual reality of being a student on campus." Across the country students are demanding that administrators make structural changes to better support all students. On April 7, a coalition of students at Oberlin College, in Ohio, wrote an open letter in support of the sit-in at Dartmouth. The letter was posted in the opinion section of "Fearless and Loathing," an independent website run by Oberlin students. "We recognize the actions of our fellow students at Dartmouth as courageous, necessary steps that must be taken if institutions such as ours - ones that advertise themselves on falsified notions of diversity, inclusivity and dignity - continue to treat 'dialogue' as a synonym for structural violence," the letter states. Oberlin junior Ana Robelo, who has been a member of the coalition since its founding last fall, said several communities on Oberlin's campus worked together to compile a list of demands for their school's administration. The demands included increased administrative transparency, divestment from companies that support Israeli occupation of Palestine and scholarship funding for undocumented students. On Oct. 10, a group of Oberlin students took over the Board of Trustees meeting and discussed demands. Oberlin senior Alice Beecher said that hundreds of students dressed in red as a symbol of solidarity. Robelo said she sensed strong and immediate backlash during the meeting. Student reactions, however, were generally supportive, though some disagreed with the group's tactics and the demand to divest from companies that support Israel, Beecher said. Since the board meeting, Beecher said that some smaller communities within the coalition have met with administrators to advance individual demands. Beecher said students joined together to create a replica of the wall separating Gaza and Israel, painting it with different representations of borders in society. Students then placed pieces of the wall in front of Oberlin's main library alongside an audiotape playing students' personal stories of division within the Oberlin community, she said. Members of the coalition also stood outside a second trustee meeting in December while holding pieces of the reconstructed wall, Beecher said. Robelo said the coalition formed in part as a result of events that took place at Oberlin last spring, including the appearance of someone dressed in a Ku Klux Klan robe and racist graffiti around campus. The coalition, Beecher said, was reacting to what they perceived as the administration's non-response. On May 1, approximately 10 students sat outside a Princeton University student center wearing black shirts and white opera masks, playing a recording of their manifesto on a boombox, Princeton junior Katie Horvath said. Passersby were offered fliers outlining the group's 10 demands for change at the university, including revised mental health policies, divestment and a call for more gender neutral housing options, among others. Horvath, who participated in the demonstration but emphasized that she did not organize it, said although the protest stemmed from a queer activism movement, its demands were "intersectional" and addressed a range of issues beyond gender.&lt;br/&gt;Though the Princeton group, called Praxis Axis, placed a stack of masks next to their demonstration as an invitation for passersby to join in, few people followed suit since few knew in advance or had clothing that matched that of the protesters, which Horvarth said became a "barrier to entry." Horvath said that the Praxis Axis demands felt similar in nature to demands voiced by the "Freedom Budget," as both were intersectional efforts to address issues centered on identity. Although Praxis Axis members did not work directly with Dartmouth students to compile their demands, Horvarth said she believed demonstrators at various schools would benefit from joining forces. For those at institutions like Princeton, which tend to have less widespread student activism than more urban institutions, engaging with like-minded students at other colleges can contribute to a stronger "protest culture," she said. On April 2, Princeton freshman Tal Fortgang published an essay titled "Checking My Privilege: Character as the Basis of Privilege" in The Tory, a conservative publication at the school. The piece, in which Fortgang refused to apologize for having privilege and cited examples of difficulties faced by his family, prompted much discussion on the Princeton campus, Horvath said. "It's been helpful," she said, "in that it has made people concerned and aware who would otherwise be likely to dismiss the demands of a group like the protest group on May Day as unnecessary or absurd or over the top." Mount Holyoke, an all-women's college in Massachusetts, is in the midst of a movement that aims to address discrimination and increase student involvement in college policy, said junior Melanie Wilkerson, an active participant in the movement. The movement, known as "MoHonest," began after Mount Holyoke student Maya Wegerif, 21, wrote a blog post alleging discrimination by campus police when she was arrested following an alcohol-related incident. Wilkerson said that many students of color at Mount Holyoke related to Wegerif's experience, and the incident sparked much discussion about discrimination and the power of campus police. "We began to form an entity that wanted to specifically represent students of color on campus," she said. "And even more broadly, those who have faced discrimination on campus or were allowed to suffer discrimination and not receive adequate administrative support." Members presented a formal list of demands to the administration in April, Wilkerson said, and are currently at a "standstill." The group's demands include encouraging more active student participation in campus policy and decisions, increasing institutional support for first-generation college students, updating the policy for reporting grievances and creating educational workshops for students, faculty, staff and campus police. "We're still negotiating, but we're a little disappointed with the administration," Wilkerson said. Wilkerson said that members of the "MoHonest" movement were aware of the "Freedom Budget" and considered the Dartmouth activists' tactics when brainstorming. The sit-in at Dartmouth, she said, was "successful in its visibility." Though "MoHonest" protesters considered a sit-in, Wilkerson said they decided against it because some members felt that - unlike at Dartmouth - not enough time had elapsed since the demands had been voiced. Wilkerson said the "MoHonest" movement reflects a nationwide trend of students becoming more vocal about administrators' lack of support. "MoHonest" has supported related movements at other institutions, including Vassar College and Bryn Mawr College, she said. "I feel like the trend is catching on because people across the country are really starting to acknowledge the kind of power young people have," she said. Though "MoHonest" faced some opposition from students, Wilkerson said it has found a broad base of support among faculty and alumni. "In my three years at Mount Holyoke, I have witnessed people go through some pretty intense stuff in terms of discrimination," Wilkerson said. "Even in a very liberal, diversity-agenda-pushing institution like Mount Holyoke, there are still fundamental flaws and issues that need to be addressed." Two student movements have recently arisen at Harvard University, both aiming to increase diversity among faculty, staff and administrators and to improve resources for more diverse programming, Harvard senior Terrance Moore said. The first of these movements, a photography campaign titled "I, Too, Am Harvard," launched on Tumblr in early March. The pictures show black students holding signs with examples of racial prejudice they have experienced at Harvard, accompanied by the slogan. Once the campaign gained attention, students involved began researching other movements to see how they were successful in creating institutional change, Moore said. The second student movement, known as "The Diversity Report," spun out of the "I, Too, Am Harvard" campaign, Moore said. Students involved in "The Diversity Report" wrote a list of demands and are currently working with specific administrators to achieve them, Moore said. After contacting them, the students decided to fill out report cards evaluating administrators to hold them accountable.</t>
         </is>
+      </c>
+      <c r="L163" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="164">
@@ -7596,10 +8092,13 @@
           <t>University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J164" t="inlineStr">
+      <c r="K164" t="inlineStr">
         <is>
           <t>Following the announcement of the University of Maine System's $36 million budget shortfall for fiscal year 2015, there has been much speculation and fear. The prospect of cutting even more faculty positions as well as entire programs from the curriculum is something that no one wants, but in the eyes of the board of trustees, these are necessary measures that must be taken to fix the deficit.&lt;br/&gt;The University of Southern Maine was the first to feel the sting of these budget cuts, with USM president Theo Kalikow announcing four full academic programs and between 20 and 30 faculty positions would be cut in an effort to chip away at the $14 million shortfall that USM must resolve.&lt;br/&gt;In response to this announcement, around 125 students and faculty stood in protest on Monday, March 24 to show their displeasure. The group walked out of their classes midday and gathered outside of the University of Maine School of Law building on USM's Portland campus, where the administrative offices are located. This resulted in the building being closed early.&lt;br/&gt;Many of the protesters believe that the crisis is manufactured, and that the UMS has a large reserve of money saved that it isn't willing to draw from. However, Kalikow insists that the crisis is real, citing the continuing freeze of state funding, tuition rates, dropping enrollment and an aging infrastructure on some campuses as primary reasons for the situation. Kalikow has also emphasized that this is a system wide problem, with all seven UMS campuses having to make sacrifices.&lt;br/&gt;Jules Purnell is a USM student studying women and gender studies and feels that students should be more involved with decisions of this magnitude.&lt;br/&gt;"We feel like we're getting a lot of double-talk," she said at the rally. "We need them to realize we need these faculty members and programs, otherwise our campus will be gutted and we won't have any way of reaching the vision we've set forth for our university."&lt;br/&gt;Solidarity&lt;br/&gt;After having witnessed the happenings in Portland, students on the Orono campus have started taking notice, with the announcement last week that UMaine would be signing with health insurance company Cigna, replacing its employee assistance program and student housing policy changes being the first of a raft of cuts and changes made to the campus structure.&lt;br/&gt;On Tuesday, a small group of concerned students met in the Wade Center in the Memorial Union to discuss the problems facing the UMS and possible steps that could be taken. Leading members of various activist groups on campus were present, including members of the Maine Peace Action Committee and Samantha Perez, president of The Green Team. The group gathered with the intent to show solidarity with USM and support the cause of the students who are at odds with UMS administration about how things are being handled.&lt;br/&gt;Perez, who led The Green Team in a meeting with the UMS board of trustees regarding divestment from fossil fuels last month, set up a Skype chat with Meaghan Lasala, a USM student who also participated in the protest on Monday. Lasala recounted the day when protesters attempted to occupy the Provost office in Portland.&lt;br/&gt;"We feel that [the administration] stepped over students bodies rather than communicating with us," Lasala said.&lt;br/&gt;"They're an inspiring group of kids down there," Perez said of the protesters at USM. "I wasn't going to get involved until it was announced that there would be cuts here."&lt;br/&gt;Perez mirrors Lasala's thoughts regarding the way things are being handled by upper level administration.&lt;br/&gt;"I think students are starting to get motivated. We need to start being included in decisions made at the university. That's my main goal," Perez said. "I don't think we're considered as main constituents."&lt;br/&gt;Perez hopes that by working together with students from other schools, a solution can be found that would nullify the need to cut programs and faculty.&lt;br/&gt;"I think that all the departments are really important. We've been working so hard [for department collaborations]. Everything here is important or it wouldn't be here. I can't think of a single faculty member I'd like to see let go," Perez said.&lt;br/&gt;"We're still at the research stage; we're going to dive deep and get some options," Perez said. "Hopefully the budget cuts won't need to happen and the University of Maine System can have a brighter future."&lt;br/&gt;Legislative action&lt;br/&gt;With the sponsorship of Representative Ben Chimpan of Portland, USM students drafted an emergency bill that was brought before the Maine Legislature on Thursday. The bill, if passed, would institute a one-year moratorium on layoffs and budget cuts by the UMS in the hopes that another solution could be found in the meantime. It also called for the creation of a stakeholders group of students and faculty that would study the system's finances and make recommendations over the course of the moratorium.&lt;br/&gt;However, because of the last minute proposal, the bill went before a 10-member group of legislative leaders who voted 6-4 to reject the bill, with those who opposed the bill arguing that passing the bill would be overstepping the bounds of their legal power.&lt;br/&gt;"There's a crisis right now in our public university system," Chipman said at the council meeting. "Students and faculty are asking for our help, and I propose that we address this crisis now."&lt;br/&gt;Despite this setback, the student solidarity group, now called #UMaineFuture, is determined to continue its fight.&lt;br/&gt;"If they don't want to make it a legislative issue, then we'll make it an election issue." Shannon Brennan, a UMaine Orono student who is also an organizer for #UMaineFuture, said in a prepared statement after the decision.&lt;br/&gt;Orono cuts announced&lt;br/&gt;The University of Maine Orono's original budget shortfall was estimated to be $12 million. After further analysis which included imminent retirements, this number has been lowered to $9.7, still a steep climb. On Friday, the university finally announced the cuts that it would be making in order to make up for this deficit.&lt;br/&gt;Although no programs will be cut, 61 positions will be eliminated, 30 of which will be through retirements while the other 31 will be non-faculty positions with five of them being layoffs. $5.3 million will also be syphoned from a savings fund that has been built up over the course of the last decade. According to Vice President for Administration and Finance Janet Waldron, this will nearly deplete the savings fund, restricting the university's ability to react in case of further financial emergencies.</t>
         </is>
+      </c>
+      <c r="L164" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="165">
@@ -7639,10 +8138,13 @@
           <t>University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J165" t="inlineStr">
+      <c r="K165" t="inlineStr">
         <is>
           <t>Following the announcement of the University of Maine System's $36 million budget shortfall for fiscal year 2015, there has been much speculation and fear. The prospect of cutting even more faculty positions as well as entire programs from the curriculum is something that no one wants, but in the eyes of the board of trustees, these are necessary measures that must be taken to fix the deficit.&lt;br/&gt;The University of Southern Maine was the first to feel the sting of these budget cuts, with USM president Theo Kalikow announcing four full academic programs and between 20 and 30 faculty positions would be cut in an effort to chip away at the $14 million shortfall that USM must resolve.&lt;br/&gt;In response to this announcement, around 125 students and faculty stood in protest on Monday, March 24 to show their displeasure. The group walked out of their classes midday and gathered outside of the University of Maine School of Law building on USM's Portland campus, where the administrative offices are located. This resulted in the building being closed early.&lt;br/&gt;Many of the protesters believe that the crisis is manufactured, and that the UMS has a large reserve of money saved that it isn't willing to draw from. However, Kalikow insists that the crisis is real, citing the continuing freeze of state funding, tuition rates, dropping enrollment and an aging infrastructure on some campuses as primary reasons for the situation. Kalikow has also emphasized that this is a system wide problem, with all seven UMS campuses having to make sacrifices.&lt;br/&gt;Jules Purnell is a USM student studying women and gender studies and feels that students should be more involved with decisions of this magnitude.&lt;br/&gt;"We feel like we're getting a lot of double-talk," she said at the rally. "We need them to realize we need these faculty members and programs, otherwise our campus will be gutted and we won't have any way of reaching the vision we've set forth for our university."&lt;br/&gt;Solidarity&lt;br/&gt;After having witnessed the happenings in Portland, students on the Orono campus have started taking notice, with the announcement last week that UMaine would be signing with health insurance company Cigna, replacing its employee assistance program and student housing policy changes being the first of a raft of cuts and changes made to the campus structure.&lt;br/&gt;On Tuesday, a small group of concerned students met in the Wade Center in the Memorial Union to discuss the problems facing the UMS and possible steps that could be taken. Leading members of various activist groups on campus were present, including members of the Maine Peace Action Committee and Samantha Perez, president of The Green Team. The group gathered with the intent to show solidarity with USM and support the cause of the students who are at odds with UMS administration about how things are being handled.&lt;br/&gt;Perez, who led The Green Team in a meeting with the UMS board of trustees regarding divestment from fossil fuels last month, set up a Skype chat with Meaghan Lasala, a USM student who also participated in the protest on Monday. Lasala recounted the day when protesters attempted to occupy the Provost office in Portland.&lt;br/&gt;"We feel that [the administration] stepped over students bodies rather than communicating with us," Lasala said.&lt;br/&gt;"They're an inspiring group of kids down there," Perez said of the protesters at USM. "I wasn't going to get involved until it was announced that there would be cuts here."&lt;br/&gt;Perez mirrors Lasala's thoughts regarding the way things are being handled by upper level administration.&lt;br/&gt;"I think students are starting to get motivated. We need to start being included in decisions made at the university. That's my main goal," Perez said. "I don't think we're considered as main constituents."&lt;br/&gt;Perez hopes that by working together with students from other schools, a solution can be found that would nullify the need to cut programs and faculty.&lt;br/&gt;"I think that all the departments are really important. We've been working so hard [for department collaborations]. Everything here is important or it wouldn't be here. I can't think of a single faculty member I'd like to see let go," Perez said.&lt;br/&gt;"We're still at the research stage; we're going to dive deep and get some options," Perez said. "Hopefully the budget cuts won't need to happen and the University of Maine System can have a brighter future."&lt;br/&gt;Legislative action&lt;br/&gt;With the sponsorship of Representative Ben Chimpan of Portland, USM students drafted an emergency bill that was brought before the Maine Legislature on Thursday. The bill, if passed, would institute a one-year moratorium on layoffs and budget cuts by the UMS in the hopes that another solution could be found in the meantime. It also called for the creation of a stakeholders group of students and faculty that would study the system's finances and make recommendations over the course of the moratorium.&lt;br/&gt;However, because of the last minute proposal, the bill went before a 10-member group of legislative leaders who voted 6-4 to reject the bill, with those who opposed the bill arguing that passing the bill would be overstepping the bounds of their legal power.&lt;br/&gt;"There's a crisis right now in our public university system," Chipman said at the council meeting. "Students and faculty are asking for our help, and I propose that we address this crisis now."&lt;br/&gt;Despite this setback, the student solidarity group, now called #UMaineFuture, is determined to continue its fight.&lt;br/&gt;"If they don't want to make it a legislative issue, then we'll make it an election issue." Shannon Brennan, a UMaine Orono student who is also an organizer for #UMaineFuture, said in a prepared statement after the decision.&lt;br/&gt;Orono cuts announced&lt;br/&gt;The University of Maine Orono's original budget shortfall was estimated to be $12 million. After further analysis which included imminent retirements, this number has been lowered to $9.7, still a steep climb. On Friday, the university finally announced the cuts that it would be making in order to make up for this deficit.&lt;br/&gt;Although no programs will be cut, 61 positions will be eliminated, 30 of which will be through retirements while the other 31 will be non-faculty positions with five of them being layoffs. $5.3 million will also be syphoned from a savings fund that has been built up over the course of the last decade. According to Vice President for Administration and Finance Janet Waldron, this will nearly deplete the savings fund, restricting the university's ability to react in case of further financial emergencies.</t>
         </is>
+      </c>
+      <c r="L165" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="166">
@@ -7687,10 +8189,13 @@
           <t>University governance, admin, policies, programs, curriculum, Anti-racism, Police violence</t>
         </is>
       </c>
-      <c r="J166" t="inlineStr">
+      <c r="K166" t="inlineStr">
         <is>
           <t>Following the University's announcement that it will not divest from major coal companies,around 100 students gathered Sunday and Monday nights in the Underground in response to what they called the University's unwillingness to listen to student voices.&lt;br/&gt;The student organizers refused to elaborate on their specific goals to The Herald and did not allow reporters inside their meetings.&lt;br/&gt;The meeting spawned from a Facebook status by Jenny Li '14 inviting other students to join her in the Underground to discuss the University's decision not to divest from coal, Sophie Soloway '14.5 wrote in an email to The Herald. Several people shared the status and others sent email and texting chains to spread word around campus, Soloway added.&lt;br/&gt;The announcement about coal divestment "seemed like a catalyst that precipitated pre-existing feelings about other times the Corporation and administration has not been accountable to student needs," Soloway wrote.&lt;br/&gt;Representatives from student groups including Brown Divest Coal, Support for Survivors of Sexual Assault, Students for Justice in Palestine and Student Labor Alliance attended the meeting, Soloway said.&lt;br/&gt;"They were all coming together to make it more of an open discussion to talk about transparency and accountability with the school and how it was lacking and they were frustrated by it," Marguerite Suozzo-Gole '15.5 said.&lt;br/&gt;Students at the Monday meeting discussed the possibility of staging a walkout later this week, Suozzo-Gole said.&lt;br/&gt;"There were very eloquent speakers making informed and impassioned" speeches to attendees, Suozzo-Gole said.&lt;br/&gt;"I wasn't expecting it to be as big as it was. It was so well-attended," Soloway said.&lt;br/&gt;Soloway attended the meeting because she feels like there is a "critical mass of student voices saying they've done everything they can and still haven't effected change" at the University, she said.&lt;br/&gt;Brown Divest Coal, the principal group that campaigned for divestment, has worked "really hard and they have a right to be disappointed," Suozzo-Gale said. But she added that its members should not walk out on the community.&lt;br/&gt;"Both being radical and not being radical enough doesn't produce change," she said. "You kind of have to strike the right balance."&lt;br/&gt;Undergraduate Council of Students President Todd Harris '14.5 was attending a meeting of the environmental group emPOWER Sunday night to hear student concerns about the University's decision regarding coal when he found out about the initial meeting in the Underground, he said.&lt;br/&gt;"I went with emPOWER to the meeting ... to hear what students had to say," Harris said.&lt;br/&gt;Many students in attendance expressed frustration over issues including and beyond coal divestment, he added.&lt;br/&gt;These broader issues included the University not listening to student concern over queer safety and a lecture today by New York City Police Commissioner Raymond Kelly hosted by the Taubman Center for Public Policy and American Institutions, Suozzo-Gole said.&lt;br/&gt;Kelly's invitation to speak at Brown has fueled controversy due to his signature stop-and-frisk policy, with many petitioning the center to rescind his invitation.&lt;br/&gt;Several students involved in the effort to cancel the Kelly talk also attended the Monday and Sunday meetings, Soloway said.&lt;br/&gt;Many students felt the University is not listening to them, Soloway said.&lt;br/&gt;"Students are part of groups that have gone through all available channels to effect change" but they feel like they have hit brick walls, she said.&lt;br/&gt;"I think the number of students who are angry and tired of being silenced and ignored is larger and rapidly growing," wrote Emma Wohl '14, a former Herald arts and culture editor, in an email to The Herald.&lt;br/&gt;Helen McDonald '14 went to the Sunday meeting because she is "tired of the Corporation's hypocrisy," as well as the University's "horrible treatment of (Brown) Dining Service workers and its numerous actions to silence student voices," she wrote in an email to The Herald.&lt;br/&gt;"We will all be part of Brown for the rest of our lives, so we should have the power to decide on the University's moral image and impact," Josue Crowther '15 wrote in an email to the Herald. Crowther attended the Sunday meeting as part of Brown Divest Coal and as a BuDS employee with "many concerns," he wrote.&lt;br/&gt;The Sunday meeting was over two hours long, and students discussed many ideas about how to express their frustrations, Soloway said.&lt;br/&gt;Interested students will continue meeting to determine specific demands and plan future action, Crowther wrote.</t>
         </is>
+      </c>
+      <c r="L166" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="167">
@@ -7735,10 +8240,13 @@
           <t>Police violence, Anti-racism, Campus climate, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J167" t="inlineStr">
+      <c r="K167" t="inlineStr">
         <is>
           <t>This past week showed an excitement and vitality that arguably hasn't existed on Brown's campus since the struggle for need-blind admission in the 90s. Despite highs and lows and victories and frustrations, the feeling that something important is happening on this campus is undeniable.&lt;br/&gt;This feeling is largely because of two important events on campus: the Corporation's refusal to divest from coal and the protest against New York Police Commissioner Ray Kelly. The former clearly demonstrated that we students have no power in this University through the "proper channels," no matter how many students support our cause. The latter showed us that the way for students to make a difference on this campus is through action.&lt;br/&gt;What succeeded in the Kelly protest was the time-honored tactic of disruption, like that used in the protests against the Vietnam and Iraq wars, for instance. Similar to the government-sponsored forums and televised events that promoted these wars, the Kelly event was not going to be a place for equal discourse. Kelly was the one with the mic and the platform, and the other side had neither. We are kidding ourselves if we think the questions we asked would have been new to Kelly, who has spoken about these policies many times before - even if someone asked what we considered to be the perfect question.&lt;br/&gt;The protest, on the other hand, succeeded in stopping our institution from giving Kelly a platform. It succeeded in allowing those who are never given this platform a chance to speak and be heard campus-wide, if not nation-wide. The mainly black and Latino students and community members who disrupted the events were heard, even if their statements about the policies had rarely been reported before. Finally, the protest disrupted Kelly's ability to teach the Providence Police force - for whom the two front rows were reserved - how to implement these policies here in Providence.&lt;br/&gt;We need student power at the University because we should play a role in deciding how it is run, along with faculty members and staff members. We should be able to decide what the University is invested in - after all, it is investing our money. We should also be able to decide how it is run: for instance, whether constant renovations are worth continual tuition hikes.&lt;br/&gt;And because the University is a key center of knowledge production, we should have a say in whose voice our institution magnifies. Deciding to give the platform to Kelly or to those who have suffered from racist police policies - or both - is a political choice. Right now, this choice is made by whoever gives money for lectures. Money equals speech, not only in political campaigns, but also on this campus. Students, faculty members and staff members should decide whose voice we magnify with our institution, not money.&lt;br/&gt;Universities for the past few decades, at Brown and across the country, have been characterized by increasing tuition but decreasing student power, decreasing pay and tenure rates for faculty members and decreasing pay and benefits for staffers. This money is being put toward more administrators with higher salaries and toward shiny new sports facilities and dorms. While some sports struggle to obtain funding and varsity status, others bring the University prestige and revenue from ticket sales. And dorms help attract wealthier students who can afford these higher tuition rates. The decisions of this University should be based on the priorities of those studying or working here, not on revenue maximization.&lt;br/&gt;We should be fighting for greater say in the University, ways to directly influence the Corporation or greater faculty governance and tenure rates. But our main weapon as students is action.&lt;br/&gt;The Kelly event showed this most recently, but we need only look to the struggles that created need-blind admission, the Africana Studies department or the Third World Center to see how students can change the campus: through protests, disruptions of events, sit-ins and walk-outs. In the coming weeks, we expect and hope to see struggles for student power on this campus, such as the upcoming action by Brown Divest Coal, and we encourage everyone to join them.&lt;br/&gt;The Brown International Socialist Organization can be contacted at isoatbrown@gmail.com</t>
         </is>
+      </c>
+      <c r="L167" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -7783,10 +8291,13 @@
           <t>Police violence, Anti-racism, Campus climate, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J168" t="inlineStr">
+      <c r="K168" t="inlineStr">
         <is>
           <t>Enriquez '16: No, Protesters were standing for racial justice&lt;br/&gt;On Oct. 29, student activists and members of the local community stood up and spoke over New York City Police Commissioner Ray Kelly's planned lecture. Their personal narratives and quotes eventually resulted in the speech's cancellation.&lt;br/&gt;People who support the punishment of these student activists highlight the fact that the students violated the "free inquiry" clause set forth in the University's Code of Student Conduct and in our mission statement. I see where those people come from. When I heard that the lecture was canceled, I was angry and disappointed that a few students could ruin a chance for others to form opinions about Kelly. That was until I realized the issues tied to this event are larger than just listening to a single speaker - they are unavoidably tied to our fellow students. Because of the activists' personal experiences, their positive intentions and the fact that they actually facilitated greater intellectual inquiry, it would be entirely misguided for the University to punish those who stood up.&lt;br/&gt;In the days after the talk, I spoke to black and Latino students who lived in Harlem or the Bronx, and I saw them relive memories of  their teenage siblings walking the city streets. They recounted how Kelly's policies encouraged the police to treat them like criminals solely based on their race and age. I heard someone describe having siblings with strong opinions on what is right and wrong in society - who may burst at the injustice of being patted down for the alleged crime of having dark skin and walking home from school.&lt;br/&gt;I had a visceral reaction to their anecdotes, in which I imagined my friends walking back from class and a police officer pulling them aside, asking them to identify themselves, patting them down, going through their pockets and rifling through their bags. I realized that my protected suburban life never exposed me to the experiences of my minority friends and their families in New York living in constant fear of our government. Only when I saw their bodies shrink with shame as they talked about the police in their neighborhoods did I really understand what I thought I already knew. If Kelly had calmly lectured to that tiny auditorium, I would not have been able to have the impassioned conversation that led me to that realization.&lt;br/&gt;Brown's mission statement declares, "The mission of Brown University is to serve the community, the nation and the world by discovering, communicating and preserving knowledge and understanding in a spirit of free inquiry."&lt;br/&gt;For the thousands of students, faculty members and administrators in our community who were not in the auditorium as Kelly spoke, the actions of the protesters called attention to an issue that many of us would have otherwise brushed aside. Their defiance spurred our campus into weeks of discussion about "proactive policing," free speech, racism and the ethics of modern society.&lt;br/&gt;It seems to me that through the protesters' passion and experiences, they communicated something that many of us had not yet discovered for ourselves - stop and frisk is unconstitutional and harmful to communities.&lt;br/&gt;Beyond this fulfillment of the Brown mission statement, their bold actions resulted in wide media coverage of Kelly's planned speech that amplified this lesson. The New York Times, CNN, the Huffington Post, Fox News and dozens of media outlets carried stories about the protest and therefore brought this essential discussion to the nation.&lt;br/&gt;Recently, when Melissa Harris-Perry of MSNBC discussed the actions of the protesters, she launched into a lengthy debate about the ethics behind stop and frisk. Looking at statistics from the New York Attorney General's office, Harris-Perry concluded that on top of the policy being unconstitutional, "stop and frisk does not stop crime" and is "harmful to black communities." Maybe more people felt empathy for the victims of stop and frisk as a result of the news coverage. Harris-Perry's national discussion is so much more important to the health of our nation and the millions of people who have been unjustly treated in New York than 200 people sitting quietly, doing the "safe" thing and keeping our university out of the national spotlight.&lt;br/&gt;Not only did the protesters spark a national discussion, they also sent a clear message to the local community. At Kelly's talk, there were a sizable number of white male police officers seated prominently in the front two rows. Among those officers was Providence Commissioner of Public Safety Steven Pare. The presence of the commissioner and his officers was threatening to the community protesters, who feared that the University was elevating both Kelly and his controversial policies. By standing up, they sent a clear message to Providence law enforcement that our local community would not support the implementation of similar policies.&lt;br/&gt;An essential requirement to the "spirit of free inquiry" in any community is that every individual feels safe enough to venture into that community, both physically and intellectually. Those members of our community - our friends, co-workers and neighbors - who protested Kelly acted non-violently in the interest of their safety and the safety of others. They promoted a discussion that was inevitably more effective than Ray Kelly's speech. They should not be punished.&lt;br/&gt;Many people in our generation, myself included, are often too disillusioned to make their voices heard. They believe that they cannot change anything and that the powers that be will not respect their opinion. Punishing these individuals for standing up for New York's communities only feeds this disillusionment and deepens the divide between the establishment and the leaders of tomorrow. Let these brave people go.&lt;br/&gt;Nico Enriquez '16 is thankful to those in our community who stood up. He can be reached at nenriquez3@gmail.com&lt;br/&gt;Delaney '15: Yes, Protestors must be held accountable&lt;br/&gt;Over the past several weeks, Brown has been immersed in a discussion centered on the Ray Kelly incident that has brought to light many important tenets of the University, including freedom of speech, social justice and the free exchange of ideas. The Herald has printed columns and letters from students, alums and faculty members with a multitude of viewpoints and ideas regarding the matter.&lt;br/&gt;The most important point that has consistently been made is that this is not a discussion of the validity of stop and frisk. It is a discussion of how members of Brown's student body acted in response to their opinions of Kelly and his policies. Therefore, the question of punishment should be derived from examining the actions taken by the protesters, independent of what they were protesting.&lt;br/&gt;First of all, the actions of the protesters were an unacceptable form of discourse. As many have already pointed out, the disruptive protests silenced the voices of many students who wanted to challenge Kelly with questions they had prepared. It is not acceptable for some students to feel that their voices are more important than those of their peers, especially in the context of a university.&lt;br/&gt;Furthermore, the forum that was held the following day continued this unacceptable form of discourse. Several students made highly caustic remarks toward faculty members and peers, with one student accusing a Brown police officer of being a racist and another directly referring to President Christina Paxson as a terrorist. This is not an appropriate way to express grievances and underscores a lack of respect toward the student body and the University that should not be tolerated.&lt;br/&gt;Second, as many have pointed out, the students' actions were a clear violation of Brown's mission: to foster the free exchange of ideas. It is entirely acceptable that students protested outside the lecture hall - they have the right to voice their opinions through protest. But it is not acceptable that they proceeded to disrupt and ultimately force the cancellation of the lecture.&lt;br/&gt;Speakers, especially controversial ones, are an important medium of discourse and are crucial to both the exchange of ideas on campus and the promotion of students' intellectual curiosity. It is unacceptable that the group not only shut down the lecture but also potentially jeopardized Brown's ability to host controversial speakers in the future. It is possible that these speakers will be hesitant to come to Brown after hearing about the way Kelly was treated.&lt;br/&gt;If the University does nothing, it will effectively condone the protesters' behavior, which would be unacceptable for the administration to do. Nobody is forcing any Brown student to agree with, or attend, any lecture on campus. But for many students, these events are one of the great benefits of attending a university that can host such high-profile speakers. The suppression of intellectual diffusion must never be tolerated.&lt;br/&gt;Finally, aside from what Paxson referred to in her email as "the extraordinary nature of these events," the actions of the students were a clear violation of the Code of Student Conduct. In the section on "Protest and Demonstration Guidelines," unacceptable forms of protest include interrupting or halting a lecture, a debate or any public forum. All Brown students agreed to abide by this code prior to matriculating, and they must be held accountable for violating it. The extraordinary nature of these events does not provide sufficient cause for violating the code.&lt;br/&gt;One of the arguments in support of the protesters' actions is that the context of the situation required a more extreme form of action and justified what happened. Many people at the forum, including a professor, supported the protesters on this basis.&lt;br/&gt;But the emotions and opinions of this small group of people do not warrant impeding the flow of ideas, silencing the voices of other students and violating the code of conduct. And as demonstrated by a recent Herald poll, 73 percent of the student body agrees with me ("Poll shows mixed opinions on Ray Kelly, coal divestment," Nov. 6).&lt;br/&gt;The majority of the student body also agrees that stop and frisk is an unacceptable policy, one with repercussions to which many of us cannot fully relate. But the protesters crossed the line. The ends do not always justify the means, and the University must hold the protesters accountable.&lt;br/&gt;Finally, I think Brown should consider inviting Kelly back to speak. I understand that some students have visceral reactions toward the man and his ideology. But this is a step the University could take to reinforce its mission to support the free exchange of ideas, even if - or perhaps especially when - they are controversial or upsetting.&lt;br/&gt;Daniel Delaney '15 can be reached for comment at daniel_delaney@brown.edu</t>
         </is>
+      </c>
+      <c r="L168" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="169">
@@ -7826,10 +8337,13 @@
           <t>Tuition, fees, financial aid, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J169" t="inlineStr">
+      <c r="K169" t="inlineStr">
         <is>
           <t>We wake up on the hard floor of the administrative building at the University of Mary Washington for the fourth day - backs aching, emotions draining - and we question why we are here. We share one trait: we are all Virginia college students. We attend the University of Mary Washington, University of Virginia, Virginia Tech, College of William and Mary, James Madison, Old Dominion, Christopher Newport and Virginia Commonwealth Universities, but this week we all occupy the same tile floor. Why did we choose to confine ourselves in this cramped hallway, monitored by guards and physically barred from the outside world? The decision to host a sit-in at UMW was neither lighthearted nor easy. It was made by desperate students working tirelessly, through every possible avenue, to make our voices heard by our university governing boards. We have received sustained denial.&lt;br/&gt;Divest UMW is a student group dedicated to removing the university's investments in the fossil fuel industry. Our group has spent the past two years escalating their campaign, most notably with a 200 person march across the university's campus. Divest UMW has garnered support from one-fourth of the student body, over one-third of the faculty, and 3,772 (and counting) signatures on an online petition. The overwhelming support won Divest UMW a detailed presentation on divestment to the Board. Our group asked for the creation of a divestment subcommittee to explore divestment options.&lt;br/&gt;One month later, on Mar. 18, Rector Holly Cuellar rejected the proposal, dismissing the concerns of thousands of her constituents without a deliberation or a public vote. She explained her decision and then quickly moved the Board meeting onto another topic. The decision shocked not only the Divest UMW group, but it also resonated with students across the state. It was a bleak reminder that the student voice in university governance is too often overlooked. The sentiment is felt by students all over Virginia who are actively seeking student input into the decisions made by their Boards.&lt;br/&gt;This past week, students at the University of Virginia, UMW's former sister school, were yet again reminded of the lack of accountability and transparency of their Board of Visitors. Student protesters marched to the doors of the public Special Collections Library, where the Board now holds its meetings, after finding out about a decision to raise tuition over 13 percent for newly accepted in-state students as well as a 3.9 percent increase for all current undergraduates. However, the protestors were immediately met with locked doors guarded by police. Student groups such as U.Va. Students United and the Latino Student Alliance could only wait silently on the steps as the Board passed the tuition hike despite much concern over the impact this decision would have on middle- and low-income applicants.&lt;br/&gt;The voices of these student bodies were stifled by their Boards through secrecy, literal barriers of locked and guarded doors and apathy. At this point the students, who are the most important stakeholders of our universities, have no real influence on major decisions made by their governing bodies. Divestment and affordable education are just two campaigns facing the same roadblocks of indifference and rejection that have been repeatedly experienced. Erin Raderstorf, a sophomore at the University of Mary Washington, believes this lack of communication should be concerning to all university students, whatever their interests: "It does transcend divestment. This is why I am supporting this movement so much, because my voice as a student could be potentially ignored on another issue. The Board's blatant disrespect for the student voice is something that should concern all students, not just those concerned with one particular issue."&lt;br/&gt;So we sit. We have exhausted the conventional methods of connecting with our governing bodies. We have sent emails, attended meetings and given presentations, just to be met with a lackluster effort from our Boards. These issues are not trivial to us. This is not a class project or an experiment. These are our educations, our futures and our voices. We will continue making noise until we become so undeniably loud that our administrators will have no choice but to listen.&lt;br/&gt;Caroline Bray is a first-year in the College and and Jake Turner is a second-year in the Graduate School of Arts and Sciences. Colleen Cosgriff is a second-year and Sarah Kinzer is a first-year at the University of Mary Washington.</t>
         </is>
+      </c>
+      <c r="L169" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="170">
@@ -7869,10 +8383,13 @@
           <t>University governance, admin, policies, programs, curriculum, Environmental</t>
         </is>
       </c>
-      <c r="J170" t="inlineStr">
+      <c r="K170" t="inlineStr">
         <is>
           <t>Cameron Yong/HIGHLANDER&lt;br/&gt;Last week's UC regents meeting in Sacramento featured the presentation of a report examining improvements to the California community college-UC transfer pathway and the introduction of a focus group that will address issues of sexual harassment on all 10 campuses. Over 60 students, alumni and professors also protested at the regents meeting, demanding that the regents sell off the investments in fossil fuel companies from the UC's $7.7 billion endowment fund.&lt;br/&gt;Half of all UC transfer students came from about 22 community colleges&lt;br/&gt;In a report released on Wednesday May 14, the UC Office of the President proposed improving counseling services and programs at the community college level to make the transfer application process easier and reduce confusion that students face in determining which courses are required for admission.&lt;br/&gt;One-third of the students - about 15,000 students per year - transfer into the UC system. However, half of all transfer students come from less than 20 percent of the 112 community colleges across the state.&lt;br/&gt;Officials said they are aiming to pay special attention to 30 community colleges that send the fewest students to the UC. They will try to garner admission from schools in the far northern regions of California, the Central Valley and in the Inland Empire.&lt;br/&gt;"Transfer students are an important part of UC's strength as an engine of social mobility for our state," said UC President Janet Napolitano. "Put simply, if we are serving transfers well, then we are serving the state well."&lt;br/&gt;5,330 out of the 8,188 transfer students who applied to UCR in fall 2013 were admitted - a rate of 65 percent - with an overwhelming majority of 95 percent who came from California community colleges.&lt;br/&gt;Some of the recommendations highlighted in the report are: developing a targeted system of reaching out to prospective transfer students to let them know that the UC is attainable and affordable; establishing a "CCC to UC Pipeline Initiative" in partnership with 30 community colleges that do not send large numbers of students to UC; providing each new transfer student with a "Transfer Success Kit," to include such elements as guaranteed housing, earlier transfer credit evaluations, orientation and mentoring; and developing transfer-oriented curriculum pathways that clearly map courses students need to be eligible to transfer into their desired major.&lt;br/&gt;UC regents focus on systemwide sexual harassment&lt;br/&gt;UC Regent Bonnie Reiss made a request during last week's regents meeting to create a new focus group which will aim to address sexual assault cases around the UC system.&lt;br/&gt;Reiss questioned whether there is enough being done at the 10 UC campuses to communicate to the student body that there is a zero-tolerance policy when it comes to crimes of sexual assault. The U.S. Department of Education released a list earlier this month of higher education institutions containing open sexual violence investigations that potentially failed to meet Title IX. This is a federal law that prohibits sex-based discrimination in campuses that receive federal funding. UC Berkeley, along with 54 other college campuses across the nation, landed on the list and is facing an ongoing state audit of its sexual assault policies.&lt;br/&gt;"I want every chancellor, on every campus - I want to see their action plan," Reiss told San Jose Mercury News.&lt;br/&gt;According to a recent report from a White House task force, about one in five college women are victims of attempted sexual assault or sexual assault. Napolitano informed the regents that she will make it a priority to provide better training to victims advocates and make sure offenders are held responsible for their actions.&lt;br/&gt;"I think students are playing a key role to educate us and each other on this issue," said Napolitano.&lt;br/&gt;Protesters rally at regents meeting for a call to action on fossil fuel divestment&lt;br/&gt;Since January, Fossil Free UC, a group that compiles members of organizations from eight UC campuses, has met with regents to discuss the implementation of a task force that will investigate the feasibility of fossil fuel divestment.&lt;br/&gt;Last week's announcement from Stanford University declaring they would sell off their investments in coal-mining companies (with the exception of natural gas and oil) prompted Fossil Free UC members to demand more from the UC.&lt;br/&gt;During the meeting, Fossil Free UC members were granted 10 minutes to speak during public comment but seemed unsatisfied with the time appropriated and disrupted the meeting several times by chanting slogans such as "invest in education, not climate change."&lt;br/&gt;"It's important to bring forth why we are doing this," said Ophir Bruck, a student organizer with Fossil Free UC. "It's about our future. Climate change is the most serious issue that our generation has to deal with. It makes no sense that our university is invested in the destruction of our future, rather they should be investing in fulfilling our future."&lt;br/&gt;Aligning with the fossil fuel initiative, the ASUCR senate also passed a resolution urging the UCOP endowment fund to divest from the top 200 fossil fuel companies in the same week.&lt;br/&gt;The students of Fossil Free UC have secured a meeting with Chief Investment Officer Jagdeep Singh Bachher and Executive Vice President of Business Operations Nathan Brostrom at the UC Office of the President on May 21 to discuss the formation of a UC Task Force on Sustainable Investing.</t>
         </is>
+      </c>
+      <c r="L170" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -7912,10 +8429,13 @@
           <t>Tuition, fees, financial aid, Public funding for higher education</t>
         </is>
       </c>
-      <c r="J171" t="inlineStr">
+      <c r="K171" t="inlineStr">
         <is>
           <t>&lt;strong&gt;Ottawa Student Federation holds its first general assembly&lt;/strong&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;The Student Federation of University of Ottawa (SFUO) hosted it first general assembly&amp;nbsp; Nov. 17 in the Ottawa Convention Centre.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;This general assembly was an open meeting where all undergraduate students voted on items including governance, bylaws, policies, campaigns, and school budgets.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;The proposal to support general assemblies was first introduced last fall by the Marxist Students&amp;rsquo; Association (now the Revolutionary Student Movement at uOttawa) and was inspired by the experience of the Quebec student movement, according to SFUO&amp;rsquo;s website.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;General assemblies allow rank and file students to better control the decision-making process, instead of leaving all the power in the hands of student officers and university staff.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;After the launch of a petition, whose number of signatures forced the holding of a referendum, the first ballot was held in late November. A majority of voters supported the proposal, but the turnout was insufficient for the decision to be considered valid. This time however, the quorum was met. University of Ottawa has now become one of the few campuses in Ontario where the student union is subject to the authority of the general assembly.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Topics discussed in the general meeting included a plan in which SFUO publicly endorses the Fossil Free uOttawa campaign and supports their efforts to get the University of Ottawa to divest its endowment and pension funds from fossil fuel companies. Another significant topic of the meetings was a potential strike at uOttawa during Spring 2015 with demands including, but not limited to, lower tuition, the dissolution of the code of conduct, and the creation of a Racialised Student Centre.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&amp;nbsp;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;strong&gt;Alberta students protest tuition spikes&lt;/strong&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Alberta students protested a new round of proposed tuition increases as they marched onto the provincial legislature in Edmonton on Monday, Nov. 17.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Around 300 students chanted &amp;ldquo;What do we want? Funding,&amp;rdquo; looking to sway the decision of&amp;nbsp; Advanced Education Minister Don Scott to implement tuition hikes in as many as 26 different programs and to increase post-secondary institutions&amp;rsquo; budgets.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Scott said Alberta&amp;rsquo;s post-secondary institutions already spend far more than any other province, and students pay 20 to 25 per cent of the cost. He is still undecided whether or not to implement the tuition hikes.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;While most tuition increases are tied to inflation, the University of Alberta has asked for permission to increase business tuition by 50 per cent, to $34,700 from the current $23,217 for an MBA.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;In a interview with the &lt;em&gt;Edmonton Journal, &lt;/em&gt;Navneet Khinda, chair of the Council of Alberta University Students declared: &amp;ldquo;We want the government to prioritize post-secondary education.&amp;rdquo;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Navneet also stated, &amp;ldquo;Students are fed up. We want a long-term vision for post-secondary.&amp;rdquo;</t>
         </is>
+      </c>
+      <c r="L171" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="172">
@@ -7927,10 +8447,13 @@
           <t>Umbrella_Harvard_Divestment_2014-2015</t>
         </is>
       </c>
-      <c r="J172" t="inlineStr">
+      <c r="K172" t="inlineStr">
         <is>
           <t>Students from environmental activist group Divest Harvard reassumed their positions in front of Massachussetts Hall on Wednesday morning, blocking entrances to the administrative building for the second time this semester in protest of the appointment of new University Chief Financial Officer Thomas J. Hollister, who is a former oil executive.&lt;br/&gt;Around 30 protesters calling Harvard to divest its $35.9 billion endowment from fossil fuels blocked the three entrances to the building-which houses the offices of top Harvard administrators including University President Drew G. Faust-at 6:45 a.m. The group was still there late Wednesday morning.&lt;br/&gt;In April, the group staged a continuous weeklong blockade of Mass. Hall. Protesters also staged a sit-in at the Harvard Alumni Association and blocked entrances to University Hall-another administrative building in the Yard-for part of that time.&lt;br/&gt;Faust, who has been repeatedly inconvenienced by the protesters, has maintained that the University should not divest, arguing that Harvard focuses its efforts to address climate change through research and teaching.&lt;br/&gt;Hollister formerly served as the chief operating officer and chief financial officer of Fortune 500 energy distribution company Global Partners LP. He also previously served as president of Citizens Bank of Massachusetts and vice chairman of Citizens Financial Group.&lt;br/&gt;Divest Harvard co-founder Chloe S. Maxmin '15 charged that his appointment is "another example of Harvard aligning with the fossil fuel industry over students."&lt;br/&gt;Dean of the College Rakesh Khurana stopped by the blockade at about 7:15 a.m. to greet the students and talk with them.&lt;br/&gt;"As a University, we have always had values of free discourse and engagement and, at the same time, an obligation to make sure the work at the University can continue," Khurana said.&lt;br/&gt;In the middle of exam period, many students studied for finals and wrote papers during the protest. Laptops and papers scattering the yard, and several said they planned to leave the blockade to take Wednesday exams. Divest Harvard co-coordinator Jasmine P. Opie '16, who was finishing a take-home exam outside Mass. Hall, said the group wanted to protest Hollister before leaving campus for the summer.&lt;br/&gt;Faust could not be reached for comment on Wednesday morning.&lt;br/&gt;-Staff writer Mariel A. Klein can be reached at mariel.klein@thecrimson.com Follow her on Twitter @mariel_klein.&lt;br/&gt;Next in University News Faust Visits Chicago for 'Your Harvard' Alumni Event</t>
         </is>
+      </c>
+      <c r="L172" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="173">
@@ -7947,10 +8470,13 @@
           <t>"Draw the Line" events that occurred simultaneously across the U.S. in protest of the Keystone XL pipeline.</t>
         </is>
       </c>
-      <c r="J173" t="inlineStr">
+      <c r="K173" t="inlineStr">
         <is>
           <t>Fri, Sep 27 at 3:40pm&lt;br/&gt;The Claremont Colleges Divestment Campaign staged a protest against the Keystone XL pipeline project on Sept. 21, in an effort to broaden its approach to tackling climate change.&lt;br/&gt;The group continues to campaign for 5C administrations to divest their endowments from fossil fuel companies, but has shifted their attention to other environmental issues as well.&lt;br/&gt;"Divestment is only a tactic, a means to achieve an end," Claremont Colleges Divestment Campaign leader Patrick Pelegri-O'Day PO '15 said. "Our goal is climate justice. We want to show that these issues are all connected, and are all part of the same broader goal."&lt;br/&gt;At the Keystone XL protest, which was staged by 24 campaign members and drew about 30 spectators, protesters tied black string dotted with notecards from tree to tree across the 5Cs.&lt;br/&gt;Pelegri-O'Day said that they intended the string to represent the pipeline, which, if built, would bisect much of the United States while transporting tar sands oil from Canada to Texas.&lt;br/&gt;The notecards detailed some projected environmental effects of the pipeline project.&lt;br/&gt;"NASA scientist Jim Hansen has said that if Canada's tar sands are completely tapped, then it is 'game over' for the climate," one card read.&lt;br/&gt;"The Keystone XL pipeline will carry 830,000 barrels of crude oil from Canada to the U.S. every day," another read.&lt;br/&gt;One of more than 200 "Draw the Line" events that occurred simultaneously across the U.S., the Claremont Colleges Divestment Campaign protest was coordinated with environmentalist Bill McKibben's 350.org, the environmental group that has led Keystone XL protests since 2011 and inspired divestment campaigns at college campuses.&lt;br/&gt;"We need to alter our climate change trajectory, and that means persuading the American people-and therefore our politicians-that we need to change our paradigm and policies toward carbon emissions," Pelegri-O'Day said.&lt;br/&gt;"The Keystone XL pipeline ... will transport dirty tar sands oil to international markets, and pollute land and water sources in indigenous and farming communities along the route," said Jess Grady-Benson PZ '14, Claremont Colleges Divestment Campaign organizer and former 350.org intern.&lt;br/&gt;These indigenous groups include the Yankton Sioux and the Nez Perce tribes, whose lands sit in the path of the intended Keystone pipeline path.&lt;br/&gt;Grady-Benson noted that, unlike most previous actions that the Divestment Campaign has taken on campus, the Keystone protest did not seek action on the part of the 5Cs, but rather was intended to raise national awareness in solidarity with the other 350.org groups who participated in the same protest across the country.&lt;br/&gt;Still, the Claremont Colleges Divestment Campaign is continuing its efforts to encourage the schools to divest in spite of the recent veto from the Pomona College Board of Trustees (see page 1). Pelegri-O'Day said that the group is presenting its case for divestment to the Pitzer College Board of Trustees on Oct. 11.&lt;br/&gt;The organization's next enterprise will most likely aim toward a wider audience, as the Keystone protest did. He added that the group is considering a changing its name to reflect its new and broader approach to climate justice.</t>
         </is>
+      </c>
+      <c r="L173" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="174">
@@ -7990,10 +8516,13 @@
           <t>Tuition, fees, financial aid, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J174" t="inlineStr">
+      <c r="K174" t="inlineStr">
         <is>
           <t>By Jeong Park&lt;br/&gt;Students focused on protesting against the recent University of California tuition increase proposal at the Student of Color Conference, one of the biggest UC-wide conferences over the weekend.&lt;br/&gt;In addition to protesting at the UC Merced campus, where the conference took place, students talked and made signs describing ways the tuition increase would affect them. The proposal, announced by the UC last week, would raise tuition and fees by up to 5 percent for the next five years.&lt;br/&gt;"Once the conference is over, this will be the conversation we'll keep having on our campus," said Fabienne Roth, Undergraduate Students Association Council general representative 3, who attended the conference.&lt;br/&gt;The Student of Color Conference, hosted in UC Merced for the first time in its 26-year history, is meant to create a space for student advocates to gather and discuss topics that relate to underrepresented students in higher education. In recent years, students have focused on issues such as mass incarceration and college affordability.&lt;br/&gt;A few dozen students from UCLA attended the conference as part of a USAC external vice president's delegation. About 1,000 people attended the event.&lt;br/&gt;The UC Student Association, which advocates for University students in higher education issues, hosts the conference every year. The event took place at UCLA last year.&lt;br/&gt;UCSA members have voiced opposition to the tuition hike proposal since it was announced, calling it a way to hold students hostage in a battle between the University and state legislators.&lt;br/&gt;The conference featured several workshops on immigration, among other topics. It also featured guest speakers, such as Carlotta Walls LaNier, one of the first black students to attend an all-white school in Arkansas after the Brown v. Board of Education decision in 1954. The Supreme Court decision led to the desegregation of K-12 education in the country.&lt;br/&gt;Devin Murphy, USAC president, and Savannah Badalich, student wellness commissioner, led a presentation on the "All of Us" mental health campaign at UCLA and urged student leaders at other UC campuses to create their own mental health campaigns.&lt;br/&gt;At the conference, the UCSA Board of Directors also met. The board voted to table a resolution calling for the UC to divest from companies that some students say profit from the Israeli occupation of Gaza and the West Bank, Roth said.&lt;br/&gt;The board also passed a resolution calling for the University to sign a community benefits agreement with Richmond, a city in Northern California that will house the UC Berkeley Global Campus at Richmond Bay. The agreement, if established, would seek to promote investments in small businesses and education in Richmond. The agreement would also aim to prepare residents for jobs at the campus.&lt;br/&gt;Compiled by Jeong Park, Bruin senior staff.</t>
         </is>
+      </c>
+      <c r="L174" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="175">
@@ -8040,10 +8569,13 @@
           <t>Police violence, Prison/mass incarceration</t>
         </is>
       </c>
-      <c r="J175" t="inlineStr">
+      <c r="K175" t="inlineStr">
         <is>
           <t>This past Wednesday, Oct. 22, led by the student organization WOC (Women of Color), a group of students and faculty members held a silent March on campus against police brutality. Wednesday marked the National Day to Stop Police Brutality, Repression, and the Criminalization of a Generation.&lt;br/&gt;"Basically we are just having a silent march in solidarity with what's been happening over the summer, and what's been happening throughout American history," one of the student leaders, Ola Fadairo '15, said as he introduced the event.&lt;br/&gt;"It was mostly started by what was happening this summer in Ferguson with Mike Brown, [and] what happened in New York, and pretty much everywhere in the United States where men of color were gunned down by police officers for no reason. So we are just going to bring awareness. This is [going to be] a silent, peaceful march. And we are just trying to bring  moreawareness to campus because it is something that should be talked about but not talked about enough," Fadairo said.&lt;br/&gt;Around 5:30 pm, more than fifty students and three faculty members gathered in front of Ross dining hall for the march. The march started outside of the Ross Dining Hall. Protesters then passed ADK and walked down the hill to the Davis Library, then passed Old Chapel and McCullough, and ended in front of Mead Chapel. The group made stops inside Ross Dining Hall, the library and in front of Mead Chapel, where different students made speeches to express their cause and promote awareness.&lt;br/&gt;In Ross Dining Hall, after a short speech, a student speaker requested that students stand with them in silence. A few students went up first and then all the students in the dining hall stood up along with the marchers.&lt;br/&gt;During the march, many students carried banners and posters which read "Solidarity with Ferguson", "Hands Up, Don't Shoot", "Black Lives Matter", "Sagging Pants is NOT Probable cause" and "Midd Divest from White Supremacy", to name a few. The weather was cloudy with drizzle, the students walked in the rain with their posters and banners in hand, silently.&lt;br/&gt;"For two generations, black and Latino youth have been shipped to prison in numbers never before seen anywhere else in the world," President of Women of Color Jackie Park '15 said.&lt;br/&gt;"The U.S. has five percent of the world population, but 25 percent of the world prison population. More than 60 percent of those in U.S. prisons are black or Latino. How many debts will it take till we know that too many people have died? At least 215 people have been killed by cops in live enforcements since Mike Brown was killed by Darren Wilson in Ferguson. I am often viewed as a safe or non-threatening woman of color, but I am here in solidarity because I refuse to submit to white supremacy, and I also refuse to live in a society that allows incondolence and violence. I am an active member of WOC (Women of Color), the violence against women, especially queer, trans and gender-nonconforming women of color is at all-time high. And the lives and faces are not visible in the media or elsewhere. This violence against women is another way the police use brutal repression and violence to serve the heteronormative and misogynistic agenda of the state. It is so important to be in solidarity with and for one another and show up in struggle. No justice, no peace," Park said in front of the marchers in the Davis Library atrium.&lt;br/&gt;At the last stop in front of Mead Chapel, the group of students raised their hands in the air in silence and then lit candles while saying the slogan "No justice, no peace" to mark the moment of commemoration and solidarity.&lt;br/&gt;One student participant talked about her objective in joining the march. "I stand for equality and justice for everyone to have the same opportunity that I was able to have, you know, growing up with the privilege I grow up with. Being here (at Middlebury), I really think everyone should have that opportunity."&lt;br/&gt;When asked about her seemingly broad objective, she said, "It is always more broad than this, but it is important to always have moments like this when the campus can really get together and you can get an intersection of group from all across campus together to remember that even though it's easy to feel really isolated here, we are part of this broader ecosystem of injustice that has perpetuated."</t>
         </is>
+      </c>
+      <c r="L175" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="176">
@@ -8078,10 +8610,13 @@
           <t>Middlebury College</t>
         </is>
       </c>
-      <c r="J176" t="inlineStr">
+      <c r="K176" t="inlineStr">
         <is>
           <t>On Tuesday, January 13, about 45 people gathered in front of Mead Chapel for a "rejection rally" against the Keystone XL pipeline, joining over 130 rejection rallies nationwide.  Encouraged by 350.org and 350 Massachusetts, rallies took place all across the country in the wake of Nebraska's decision to allow the pipeline to pass through.&lt;br/&gt;The purpose of the 'rejection' rallies was to continue to show opposition to the Keystone XL pipeline that would carry tar sands oil from Alberta, Canada to the Gulf Coast in the hope that President Obama will veto Congress's decision to allow the pipeline.&lt;br/&gt;Middlebury's rejection rally was lead by a combination of individuals and groups on campus, including Sunday Night Group, Divest Midd, Zane Anthony '16.5 and Emma Ronai-Durning '18.&lt;br/&gt;"I helped organize this rally because I think it's really important that Middlebury be part of a national movement against the Keystone pipeline," said Michael Shrader '18. "While this one is not necessarily local, the affects are global and affect us here at Middlebury, so people have a right to know more about it."&lt;br/&gt;In addition to students, a number of protesters in the crowd were members of local communities and organizations.&lt;br/&gt;"I definitely support the cause here," said Jennifer Vyhnak, a resident of Bristol and an environmental activist. Vyhnak condemned the "dinosaur fuels" of the past, and stressed the need to usher in a new era of green energy.&lt;br/&gt;"We really need to be supporting the energies of the future, the energies that do as little harm as possible, and allow us to live on this good earth with respect for one another," she said. "It feels like its time. It's time for us to grow up."&lt;br/&gt;In contrast, Phil Hoxie '17 and the College Republicans held a rally in support of the pipeline and in support of the jobs it would create. The rally was called 'Students 4 Jobs' on its Facebook page.&lt;br/&gt;"We want to reassure people who have dissenting views that there are other people who share [them]," Hoxie said, "and that they are worth expressing - especially in an academic context."&lt;br/&gt;One of the signs that the students opposing the pipeline brandished irked Hoxie.&lt;br/&gt;"I was kind of upset by 'Middlebury College rejects Keystone XL' as a blanket statement," he said. "That's supposed to cover the whole student body. It doesn't. [We] are here to remind the students of Middlebury that there is a dissenting opinion, which is very important in any debate. It's important to have two sides."&lt;br/&gt;The rejection rally began on Mead Chapel steps with opening remarks by several students.  Michael Schrader '18 stated their purpose of the rally as "urging President Obama to stand up against the interest of foreign oil companies" by vetoing the Keystone XL pipeline.&lt;br/&gt;"Tar sands development spells increased pollution, greenhouse gasses, heavy metals, polluted aquifers, and climate chaos," Schrader said. He encouraged people to rally for the good of all Americans.&lt;br/&gt;"Not just Americans," a voice yelled from the crowd, to cheers and clapping. "All kinds of people!"&lt;br/&gt;"We've all been fighting this pipeline for a ridiculous number of years," Hannah Bristol '14.5 said in her opening remarks. "We've had the largest climate march in history - and then beat that record and had another largest climate march in history," Bristol added to laughter and more cheers.&lt;br/&gt;"Many of us here have been arrested. I don't know how we can possibly say  any louder that this pipeline is bad news. But the Republicans in Congress don't seem to get the message," Bristol said.&lt;br/&gt;Phil Hoxie '17.5 disagreed, and stated that the pipeline would relieve a strained American economy.&lt;br/&gt;"The green energy market is not a competitive market," he said when asked about funding green energy instead.&lt;br/&gt;"I want to see incentives for companies to invest in greener technologies - companies like Tesla, by boosting demand for those items, not necessarily through [direct investment]."&lt;br/&gt;Alexander Khan '17, who was unable to make the event, agreed with Hoxie in a prewritten statement: "The pipeline will provide jobs which in turn with strengthen our economy. Only with the help of a robust economy will the United States be able to solve the problems that the world faces."&lt;br/&gt;Most importantly, Hoxie stressed that no matter what the United States did, the tar sands were likely to be used regardless.&lt;br/&gt;"Whether the United States builds this pipeline or not, that oil is coming out of the ground and there's no way for anybody to stop that," Hoxie said.&lt;br/&gt;The Chinese will buy it up in a second. The Canadians are still waiting for their ideal situation - for the pipeline to go through the United States, for it to be refined in the United States, and be sold through the port of Louisiana to it's final destination, wherever that may be." Participants in the rejection rally certainly did not believe their efforts were in vain; the excitement among the demonstrators was palpable.&lt;br/&gt;Many of them were demonstrating for the first time to such an event.&lt;br/&gt;Max Greenwald '18 acknowledged that he normally doesn't show up to rallies like this, because Middlebury is such a "liberal and environmentally conscious school." However, something caused him to change his mind.&lt;br/&gt;"I saw some people were actually having a counter rally to this," he noted, referring to the 'Students 4 Jobs' rally that had occured minutes before the march began.&lt;br/&gt;"Clearly there is some division on this issue, so I thought I'd show my support.&lt;br/&gt;  You can't always expect someone else to do it. When you see crowds on TV supporting something that you care about, you have to be one of those people in the crowd if you expect your movement to gain any momentum."&lt;br/&gt;As students and townspeople milled about by Mead Chapel sharing stories of their inspiration to attend the rally, and their experiences with past climate activism at events locally and in Washington DC.  Ross Conrad, a local beekeeper, attended the rally.&lt;br/&gt;"I feel like I need to apologize for my generation because we have failed to deal with this issue and we're dumping this on your laps, and that's not right," Conrad said.  Conrad likes the format of these local rejection rallies, rather than one centralized rally.&lt;br/&gt;"Everything's going to have to be more localized, more decentralized, if we're going to be better stewards of this earth, in my view," Conrad said.&lt;br/&gt;Anthony and Ronai-Durning led the procession down Mead Chapel hill with a banner that read "Middlebury Rejects KXL" with a picture of a pipeline dripping black oil. The crowd consisting of students and members of the Middlebury community followed behind in groups of twos and threes carrying candles and signs.  As they walked down to Old Chapel, people chanted "Barack Obama, yes you can!  Stop the dirty pipeline plan!" and "Tar sands kill! Pipelines spill!"&lt;br/&gt;In front of Old Chapel, the procession stopped to for a photo with their signs, as did many other rejection rallies.  The rejection rallies across the country followed a very similar format, as most were developed from a toolkit provided by 350.org.  The picture "will join a national mosaic of these pictures, banners, et cetera to be broadcast to various larger news outlets," Anthony said.&lt;br/&gt;Following the photo, the procession walked back up Mead Chapel hill chanting and into Proctor.  The procession walked into the serving area and through the dining hall.  On Proctor Terrace, the group gathered for one last picture and dispersed.</t>
         </is>
+      </c>
+      <c r="L176" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="177">
@@ -8121,10 +8656,13 @@
           <t>University governance, admin, policies, programs, curriculum, Environmental</t>
         </is>
       </c>
-      <c r="J177" t="inlineStr">
+      <c r="K177" t="inlineStr">
         <is>
           <t>Nineteen members of Fossil Free Yale were fined and threatened with arrest after a day-long sit-in on Yale's campus, according to the Yale Daily News.&lt;br/&gt;On April 9, 48 members of Fossil Free Yale entered Woodbridge Hall in the morning to begin the day-long sit-in.&lt;br/&gt;Later that afternoon, approximately 150 people gathered around Woodbridge Hall and formed a human chain to advocate for the divestment of Yale's endowment from fossil fuels.&lt;br/&gt;The Yale Police Department Chief Ronnell Higgins issued a 5 p.m. deadline for the protestors to disperse, threatening those who did not with arrest. Nineteen students refused to leave the hall even after the deadline, and they were issued "infraction tickets" by the police.&lt;br/&gt;Infraction tickets do not appear on Department of Justice criminal records.&lt;br/&gt;Some students who remained in the building after multiple notifications to leave were individually arrested by the police.&lt;br/&gt;Chelsea Watson, a sophomore who is the communications director for Fossil Free Yale, said that though other schools have witnessed sit-ins, Yale is the first to arrest any student.</t>
         </is>
+      </c>
+      <c r="L177" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="178">
@@ -8164,10 +8702,13 @@
           <t>University governance, admin, policies, programs, curriculum, Environmental</t>
         </is>
       </c>
-      <c r="J178" t="inlineStr">
+      <c r="K178" t="inlineStr">
         <is>
           <t>This past weekend was an important one for our university- but many students might not know it. The Yale Corporation, the secretive, autocratic governing body of Yale, held their spring meeting. We never know when the meetings will occur, and we cannot know what is discussed or how it is presented. The meeting minutes are kept sealed for 50 years, and strict confidentiality policies prevent any Corporation member except the President from speaking about decisions reached during the meeting.&lt;br/&gt;According to the Yale website, the Corporation is comprised of Yale graduates, many of whom are current or former CEOs of multinational corporations. With the exception of President Peter Salovey, there is no faculty or student representation on the board. Corporation members are detached from life at Yale. They rarely step foot on this campus, and their interaction with students is limited to select Masters' Teas. This group controls everything from the university's investments to the selection of its President to the renaming of its colleges. It cannot, however, accurately reflect the interests of the students and faculty that make up the Yale community as long as it lacks their voices and representation. Instead, it represents the private interests of a select few.&lt;br/&gt;Fossil Free Yale regularly submits proposals to the Yale Corporation through an advisory committee, and thus keeps a close watch for Corporation meetings. Fossil Free Yale is just one part of a worldwide, student-led fossil fuel divestment movement that centers around climate justice. The fossil fuel industry contributes disproportionately to climate change, blocks climate change legislation through political lobbying and donations, and exploits communities that are already marginalized; most often, these are low-income communities and communities of color.&lt;br/&gt;Divestment is a symbolic action meant to morally bankrupt the fossil fuel industry. To profit from an industry dependent upon the destruction of our planet and its people is an ethical failure on all of our parts, so Fossil Free Yale has been fighting to convince the Yale Corporation to divest its $25.6 billion endowment from the fossil fuel industry. If Yale divests, it would not only have the opportunity to be a world leader on climate change, but also to make the powerful statement that we will no longer be complicit in the social impacts that climate change and fossil fuel extraction have on the world, especially in disadvantaged communities.&lt;br/&gt;But how can Yale manage its endowment in a socially responsible way if those who make its decisions are directly engaged with the unethical industries from which we must divest? The extractive fossil fuels industry is well represented on the Corporation, with seats held by tycoons such as Charles "Chip" Goodyear, the former CEO of BHP Billiton, a multinational mining, metals, and petroleum company, and Dr. Paul Joskow, who previously sat on the board of TransCanada, the energy company responsible for the infamous Keystone XL pipeline.&lt;br/&gt;The personal interests of those who sit on the Corporation clearly hold more weight than those of the students. When forced to pick a side on divestment, the Corporation sided with the corporate interests of the fossil fuel industry, rather than the faculty, alumni, and thousands of students who have called for divestment. They were able to do this in secret, without having to disclose personal ties and recuse themselves from the decision.&lt;br/&gt;When I reflect on the fact that a group of CEOs sat in a room this past weekend to discuss student grievances, demands, and proposals without actually hearing from students, let alone informing them that this discussion was happening, I question the purpose of this autocratic governing body. Fossil Free Yale has never been informed of a meeting or been contacted for clarifications, and yet the Corporation has had the final say on every proposal we have submitted.&lt;br/&gt;Consider the demands made by Next Yale, Graduate Employees and Student Organizations , New Haven Rising, Students Unite Now and other activist groups last semester. Yale's governing elite has complete control over many of these initiatives as well, despite their utter detachment from the students and issues themselves. The Corporation is so far removed from student movements that it is absurd to think their decisions are well-informed and free from conflicts of interest.&lt;br/&gt;Over the past three years, Fossil Free Yale has grown accustomed to hearing nothing but silence from the shadows in which the Corporation members sit. We spend months at a time writing new proposals to present to the administration, only to have them reject our requests for more direct engagement. We continually ask to speak directly with a Corporation member or to have observer status at the meeting on our proposal, but these requests are systematically rejected or ignored, even after massive demonstrations of student support.&lt;br/&gt;During the past three years of Fossil Free Yale's mobilization for divestment, we have tried many different tactics. We began our campaign by navigating official administrative channels. We worked with an administrative advisory committee and held a referendum with Yale College Council, in which roughly 2,900 students voted in support of divestment- 83% percent of the students who voted. After our first proposal was rejected without any further engagement, we began to escalate our efforts outside of official channels. We wanted to be so loud that they would have no choice but to truly listen and genuinely respond. We repeatedly asked the administration to listen to us. We wrote letters to the Corporation and President Salovey, and held rallies outside of Woodbridge Hall. We asked them, "Whose side are you on?"&lt;br/&gt;We were met with silence.&lt;br/&gt;Finally, on April 9, 2015 at 8:50 a.m., 50 Fossil Free Yale members walked into Woodbridge Hall and sat down. We explained that we would leave when the administration agreed to engage with us; we wanted, for once, a real conversation. One hundred and fifty students rallied outside Woodbridge in support. The University's response was cold and clear: get out of Woodbridge or get arrested. Nineteen students remained in Woodbridge Hall following this ultimatum, and, as promised, we were arrested.&lt;br/&gt;I will never forget the moment my school chose to arrest me. It was exciting to feel the love, support, and pride of those students around me who understood the significance of that day, but I also cannot forget the slow wave of nausea that washed over me as I realized that my school didn't care about me. Our request was simple: talk to us. Their response was just as simple: we'd rather not. As my arrest was processed and I was escorted out of the building, I realized that our movement could not triumph if Yale remained governed in this way.&lt;br/&gt;We did learn something from this arrest: Yale had been listening all along. But when it came down to it, they chose to take disciplinary action against their students rather than to engage with them. They heard our messages about the fossil fuel industry's involvement in political corruption and its role in the dissemination of fraudulent science. They read our letter about the social justice implications of fossil fuel extraction. They listened when we told them that climate change is an urgent crisis that affects us all, but that most immediately affects communities that are invisible to an elite institution like Yale. They knew that divesting from fossil fuels would be Yale's opportunity to acknowledge the reality of these harms, as well as to recognize that the allocation of money and investments constitutes a political statement. It was idealistic to think that if they listened, they would change. The truth is that they have heard us. They simply don't care.&lt;br/&gt;I imagine some people are unsurprised by this apathy, or will cite the necessity of pragmatism. This is what we have come to expect from those in power. Think about Flint's poisoned water, or the aftermath of the 2008 financial crisis. We have grown up in a society where our leaders are rarely held accountable for decisions that negatively impact their constituents. Perhaps a few become scapegoats. But what if we could envision a future where that is not the case? What if our university was accountable to the students it was created to serve, and to the world beyond?&lt;br/&gt;But how do you go about changing an institution whose interests are fundamentally incompatible with those of the people it represents? It is difficult, but it is possible. We, the Yale community, must hold the Corporation accountable, because if we don't, nobody will. We must speak up for the victims of the fossil fuel injustice from which Yale profits, and join together as students to fight for a more just and transparent university. The problem is greater than just individual Corporation members deciding whether or not to care about students. The elite structure and confidentiality policies of the Yale Corporation create conditions in which it is easy for members not to care. They are able to disregard Yale's students and faculty, and their detachment from the Yale community makes it exceedingly difficult to be accountable.&lt;br/&gt;If the Yale Corporation was just, transparent, and democratic, it would account for the voices of its students and faculty. It would consider the ethical implications of its investments. It would make changes that serve the community rather than Corporation members' personal connections, Yale's marketing and branding strategies, and the massive financial appetite of the University. Representatives would be held responsible if they did not fulfill these expectations.&lt;br/&gt;We need to critically question if this power structure is a legitimate, representative, and appropriate governing body for Yale. In our opinion, it is not.</t>
         </is>
+      </c>
+      <c r="L178" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="179">
@@ -8207,10 +8748,13 @@
           <t>Economy/inequality, Labor and work, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J179" t="inlineStr">
+      <c r="K179" t="inlineStr">
         <is>
           <t>It's really hard to get into Yale," Bill Hinners, the first cook in Pierson Dining Hall, told me.&lt;br/&gt;But Hinners was not talking about the standard set for the students who pass through his dining hall. Last year, 150,000 people actively sought employment at the University. Just under 500 succeeded. The acceptance rate- just under a third of a percent-is approximately 20 times smaller than the equivalent rate for undergraduates.&lt;br/&gt;Even given this selectivity, Yale is New Haven's largest employer. The University provides jobs to around 15,000 individuals across faculty and staff positions. Roughly a third are New Haven residents. This university-city relationship isn't unique to Yale and New Haven; a number of other U.S. cities such as Philadelphia and Baltimore rely disproportionately on major universities for employment. But Yale presents a particularly dramatic example, due to the wide disparity between the University's endowment and the poverty of its host city.&lt;br/&gt;Unemployment plagues New Haven. Currently, the city's unemployment rate is nearly triple the national average. The citywide rate of 14 percent jumps to over 18 percent for blacks; a fifth of Latino residents are unemployed.&lt;br/&gt;At a community meeting last April, two of the New Haven alders defiantly hoisted a binder brimming with the resumes of 500 qualified New Haven workers; these 500 were educated, trained job seekers, who still were without employment.&lt;br/&gt;Two months later, Yale pledged to hire 500 new employees over the coming two years. The announcement, which came in the form of a letter from Yale's Vice President of the Office of New Haven and State Affairs Bruce Alexander to New Haven Mayor Toni Harp, ARC '78, specified that, where possible, the hires would be New Haven residents. Four hundred of the jobs would fill staff positions-such as maintenance or clerical work-and the remaining 100 are construction positions. While many of the jobs will fill current spots, Vice President of Human Relations Mike Peel said that the construction of the two new residential colleges, set to open two years from now, will increase demand.&lt;br/&gt;It is 20 times harder to get into Yale as an employee than it is as a student. Granted, the staff's yearly turnover rate pales in comparison to that of the student body. A strong union presence actively contributes to Yale's attractiveness as an employer and bolsters these jobs' stability. While hiring rates are low, it is not news that New Haven depends on Yale as a major driver of the local economy. The viability of this relationship, though, is uncertain.&lt;br/&gt;TWO DAYS AFTER YALE ANNOUNCED THE 500 JOBS, NEW Haven Rising staged a march protesting persistent joblessness and unemployment. Just outside City Hall, Reverend Scott Marks proclaimed a "jobs crisis" in the city. The march attracted over 1,000 demonstrators across community organizations, unions, and religious institutions, shutting down the block between City Hall and the New Haven Green. The unfortunate truth is that Marks hit the nail on the head.&lt;br/&gt;Last year, the mayor's office commissioned a report on the New Haven jobs landscape. The findings were dismal. The report, released in May 2015, found that just under two-thirds of New Haven residents are employed, revealing that the unemployment rate underestimates the numbers of those out of work by nearly half. The disparity can likely be accounted for in the numbers of those who no longer actively seek work and in part-time workers seeking full-time jobs.&lt;br/&gt;For the jobs that do exist, the wage distribution tells a still-worse story. According to DataHaven's 2013 Community Index Report, there are around 82,000 jobs in New Haven. But only half pay workers $20 an hour or more, which is considered a living wage. Moreover, only one in five of employees are New Haven residents. Fewer than one in 20 living wage jobs are held by residents of low-income neighborhoods.&lt;br/&gt;The national poverty level for a family of four is $23,021; New Haven residents must make almost $80,000 to meet a secure yet modest living standard. If we assume that an employee works eight hour days, five days a week, 50 out of 52 weeks a year, that comes out to $40,000, just half of what is needed to offer financial security. It becomes clear that even living wages are not nearly enough.&lt;br/&gt;In a 2012 survey, nearly a third of adult New Haven residents described their ability to secure suitable employment as "poor." Among black residents, that number nearly doubled.&lt;br/&gt;The numbers are devastating. Many are looking for work, more are barely getting by in the jobs they have, and a huge number in both categories are people of color living in the city's poorest areas.&lt;br/&gt;Conversations about employment are often followed by ones focusing on education-it is no revelation that higher levels of education typically correlate to improved employment prospects. New Haven is no exception. Slightly less than a third of New Haven adults are considered to be at the lowest literacy levels; over the last four years, only 45 New Haven residents passed the GED. To begin to close the employment gap, education, too, must be addressed.&lt;br/&gt;Even still, only 39 percent of job seekers possess a Bachelor's degree or higher. Meanwhile, 70 percent of employers seeking candidates require that level of education. The numbers demonstrate that the jobs crisis is only exacerbated by the fact that New Haven employers are seeking employees that may not exist, while residents are searching for jobs they do not qualify for.&lt;br/&gt;In the meantime, local leaders are looking for Yale to do its part-big time. The head of Local 34, the union that represents clerical and technical workers at the University, agrees. In an email to the Herald, Laurie Kennington cut straight to the point. "Yale needs to do more," she wrote. The University employs 5,140 New Haven residents. Over half of these employees are faculty members or post doctoral candidates. Approximately 1,500 are unionized staff members. In 2014, 166 New Haven residents joined unions affiliated with Yale.&lt;br/&gt;LAST FRIDAY, I FOLLOWED UNION VETERAN ERIC SINGLETON through Pierson Dining Hall and past the serving area into the kitchen. We snaked between the large, gray plastic serving carts towards a man standing comfortably in front of the grill, where bacon for that morning's breakfast sizzled. His salt-and-pepper mustache curled as he smiled. He wiped a large hand against his apron before offering it to me. "Bill, here, has been working at Yale for 35 years," Singleton said as an introduction.&lt;br/&gt;"Actually, 34," Hinners, the first cook in Pierson Dining Hall, corrected. "It'll be 35 next November."&lt;br/&gt;What I wouldn't learn until a few hours later is that Singleton, too, has worked at the University for almost 30 years. Singleton is from New Haven, Hinners from Branford. Hinners said that he thought most of his coworkers are from New Haven. When I mentioned that only a third of the staff is local, both Hinners and Singleton were shocked. He said he would have estimated the number at closer to 75 or 80 percent.&lt;br/&gt;For locals and commuters alike, the advantages of working at Yale are innumerable. "I was going to come here for a year, but once I got here, it's such a nice place to work," Hinners said. He rattled off the advantages of being a Yale employee: the hours, the days off, the benefits, the pay, the job security.&lt;br/&gt;Singleton went as far as to say that Yale surpasses any other Ivy League school-in fact any university-in terms of pay scale and benefits. "They have so many perks. You can really make a career out of this," he said. Relations between the University and its employees, however, haven't always been so congenial. In fact, 20 years ago, hardly any of the benefits Hinners had listed even existed.&lt;br/&gt;"THE ONLY SURE THINGS IN LIFE ARE DEATH, TAXES, AND hostile labor relations at Yale University," Local 35 leader Bob Proto told the Herald in 1996.&lt;br/&gt;It wasn't until 2003 that the relationship began to stabilize. That year, the New York Times reported that Yale held "by far the worst record of labor tension of any university in the nation." Three unions-Locals 34 and 35, and 150 food workers at Yale-New Haven Hospital-and 1,000 graduate students had just coordinated a five-day walk-out that shut down dining halls, left seminar tables without section leaders, and dormitory bathrooms unclean.&lt;br/&gt;The 2003 strike was the eighth such incident in the last four decades. Two strikes, in 1974 and 1977, lasted nearly all semester. In 1984, another 10-week strike led to the creation of Local 34. "Historically, Yale has not been the most supportive employer. We can do better," former President Richard C. Levin, GRD '74, told the Times. By the end of his tenure, Levin would be credited for ameliorating decades of labor strife.&lt;br/&gt;According to Yale History professor Jennifer Klein, the University provoked the 2003 strike in an attempt to push the union back and to create jobs outside of the union's bargaining unit. The plan, however, backfired. "It really signaled to the University that the unions were not going away, that the workers supported it and they wanted a voice," she said.&lt;br/&gt;The strike ended with a major victory for the unions. Under the terms of the eight-year contract, the University would increase Local 34 wages by roughly 44 percent, while Local 35 wages would rise 32 percent. Moreover, monthly pensions would nearly double, a landmark change as pensions previously hovered around $500 per month, pushing retirees into poverty.&lt;br/&gt;Hinners attributes the superb benefits that Yale provides entirely to the union. "They're the reason we get everything we get," he said.&lt;br/&gt;Since 2003, the Local 34 and 35 union contracts have been renewed twice, both relatively seamlessly. In 2009, union members agreed to extend the 2003 contract another three years, a step that some viewed as a triumph, given the debilitated state of the nation's economy at the time. "In good times, this would be a good contract," Proto told the New Haven Independent. "In these times, it's incredible."&lt;br/&gt;Additionally, members of Local 35 were promised no layoffs, while the University vowed to enhance job security for members of Local 34. Union members again ratified a contract in 2012 without clamor. It raised wages 15 percent and 14 percent for Local 34 and 35, respectively, over four years. The unions, meanwhile, made some concessions on healthcare and pensions. The next contract is set for renewal in 2016.&lt;br/&gt;Even before the 2012 renewal, Proto said that Yale's contract was one of the top in the nation. Coupled with Hinners' and Singleton's glowing reviews, it is no surprise that 150,000 job seekers are waiting in line for their shot at employment at Yale.&lt;br/&gt;"I was lucky. I had worked with one of the cooks at a private club, so he said apply, and I did," Hinners told me. "For the most part, Yale seldom advertises jobs. It's almost like you have to be in the right place at the right time. A lot of it has to do with luck."&lt;br/&gt;SOME, UNFORTUNATELY, ARE LESS LUCKY THAN OTHERS. I met Bill McElveen just outside New Haven Works, an organization that connects unemployed New Haven residents with hiring opportunities. McElveen is an ex-offender, has a high school diploma, and was recently let go from the city's Parks and Recreation Department where he had worked for the last two years. He had made the trip to New Haven Works to reapply for a position within Parks and Rec.&lt;br/&gt;When we started talking, and I told him that Yale is adding 500 jobs, he balked. "I wouldn't mind working for Yale," he said, adding that he understands Yale to be the best employer in the city. "Hearing that information firsthand is something that motivates me to get employment." He left me the number of the supervisor at his halfway house, and asked me to call and share further details about the Yale jobs.&lt;br/&gt;Yale hires through Strategic Talent-management and Recruitment System , an online portal on its human resources website. According to the website, applying online is the only way to pursue employment for all staff positions at the University. Yale HR handles all staff hiring, while departments conduct independent hiring processes for faculty.&lt;br/&gt;In accordance with the 2012 union contract, when jobs become available, they are first offered to laid-off workers, then to inside hires, and lastly to individuals who come through the city's job pipelines, New Haven Works included.&lt;br/&gt;Less formally, a number of University employees get their foot in the door through temporary employment, better known as casuals. The unions protest this arrangement-it brings on employees outside the bargaining chip, and they can't offer those employees union benefits. Meanwhile, the university profits from the arrangement. Clearly a source of tension between the University and the unions, increasing union pressure drove Yale to transition casuals to full-time employment in the 2012 contract approval. Still, Hinners believes that casuals remain one of the major avenues to employment.&lt;br/&gt;Now, though, 500 jobs are opening up. Peel said 100 of the newly announced jobs will be for construction workers. Federal law requires that 25 percent of work hours must be performed by minority construction workers and 6.9 percent by women; meanwhile, the city mandates that projects receiving city dollars reserve 25 percent of work hours for New Haven residents. But as a privately funded project at a private institution, the University will not be held to those standards.&lt;br/&gt;While the University maintains that it still meets the federally mandated quota, local contractors contest that Yale creates a hostile environment for smaller construction management teams. L.M. Stewart is the business manager for Tri-Con Construction Managers LLC, a small construction management team that worked on numerous University projects valuing $5 million and under. The company redid the seating at the Yale Bowl and repaired the tunnel under Route 34, among other jobs."[Yale] grudgingly worked with small contractors, but I don't think their heart was really into it," Stewart told me.&lt;br/&gt;Stewart said his company closed out its last project for the University four or five years ago. He believes that, since, the University has turned to hiring larger construction management teams. "A lot of them are out of town and out of state, and they don't reach out to local contractors," he said.&lt;br/&gt;According to Stewart, Yale opens positions to local contractors, but often makes the job criteria exceedingly difficult. "Yale is a big contributor towards the New Haven economy. But when you're looking at it from a construction standpoint, it leaves much to be desired," he said.&lt;br/&gt;Yale History professor Jennifer Klein reminded me that Yale is constantly hiring. These 500 new jobs are expected to come in addition to the numbers that the University typically recruits. Given that Yale added just under 500 jobs in 2014, the commitment effectively doubles the University's hiring.&lt;br/&gt;At the New Haven Rising march in June, however, demonstrators protested that 500 is not enough. "Hire the 500 New Haven residents now, and clear the way for the thousands behind them!" Board of Alders President Tyisha Walker proclaimed.&lt;br/&gt;The 500, for now, is certainly a start. "We can debate whether it should be more-more would certainly be nice," said John Padilla, who works for a local consulting firm that has done projects for the mayor's office. "But I think if those 500 jobs went to 500 New Haveners, especially unemployed New Haveners, that would be significant. Any time you have 500 people going to work, that's significant."&lt;br/&gt;THE TOWN-GOWN RELATIONSHIP BETWEEN YALE AND New Haven represents a stark example of a national trend. Postindustrial cities across the U.S.-from Baltimore to Philadelphia to Boston-still are struggling to fully recover from the economic devastation caused by the sudden drop of industrialized labor in the 1980s.&lt;br/&gt;The term "post-industrial" first emerged in 1982, when historians Barry Bluestone and Bennett Harrison described the "widespread, systematic divestment in the nation's productive capacity." While indeed these cities are quite a bit larger than New Haven, the post-industrial narrative flows through them all.&lt;br/&gt;At its peak during WWII, New Haven's Winchester Repeating Arms factory employed roughly 19,000 New Haven residents. In years to follow, it slowly devolved, until it went bankrupt in 1989. When the doors officially closed in 2006, only 186 employees remained.&lt;br/&gt;In a list of the nation's poorest cities published by CBS last February, Baltimore, Philadelphia, and Boston all made an appearance. Each is home to some of the largest university names in the country-Johns Hopkins, University of Pennsylvania, and a host that call Boston their home.&lt;br/&gt;Earlier this year, Klein wrote that universities are far from a guarantee of economic success for the cities they dominate. "Universities and their research parks or hospitals have steadily expanded territorially and economically, while local communities have little say in how their neighborhoods are reshaped or how resources are allocated," Klein wrote. Across the country, universities and the medical complexes that accompany them have slid in to fill the gaping employment hole deindustrialization left in its wake.&lt;br/&gt;Beyond the University, Yale-New Haven Hospital is the second largest employer in the city. In fact, the city cites healthcare as one of the top two growth industries in New Haven; the number of healthcare jobs are projected to increase 20 percent in the next five years.&lt;br/&gt;But the city perhaps has undue faith in the hospital, and in healthcare more generally, to close the employment gap. Acknowledging the role of universities and their associated medical complexes in poverty stricken cities across the city is by no means to exonerate Yale of its duties. Rather, it serves as a reminder of its massive presence and responsibility in the post-industrial city.&lt;br/&gt;Indeed, Yale is a private, tax-exempt institution, and by no means a rapidly growing business. Unionized jobs are well protected, which puts turnover-as Hinners and others described-at close to none. As such, the rise of urban systems that rely on universities and healthcare for employment is untenable.&lt;br/&gt;"It's been an unequal balance of power," Klein told me. "The University has acquired significant leverage and the ability to act unilaterally." In a lot of ways, the University's role in actively combatting unemployment in Elm City is almost paradoxical. Yale should do more-it is both trite to and impossible not to return to the $26 billion endowment the University raised last year, not to mention the multi-million dollar payments to its financial advisors. But simultaneously, the balance of power Klein refers to must begin to shift. Can Yale begin to act as a partner for the benefit of the city, rather than acting singly and on the city's behalf? For the sake of those living here, it must.</t>
         </is>
+      </c>
+      <c r="L179" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="180">
@@ -8250,10 +8794,13 @@
           <t>University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J180" t="inlineStr">
+      <c r="K180" t="inlineStr">
         <is>
           <t>Ohio University's Student Senate is proposing dramatic changes for the university that would significantly affect the institution's budget, if they were ever adopted by officials.&lt;br/&gt;Senate's proposals - which will be voted on at its Wednesday meeting - can be forwarded to whomever they choose. But senate is only an advisory committee formed to represent undergraduate students on campus. Officials aren't required to make the changes it suggests.&lt;br/&gt;Senate's ideas include:&lt;br/&gt;-A $15 minimum wage that is almost double Ohio's $7.95 minimum wage.&lt;br/&gt;-Elimination of tuition increases&lt;br/&gt;-No pay raises for administrators making over $200,000&lt;br/&gt;-Transparency of OU's endowment&lt;br/&gt;-Divestment from the use of fossil fuels&lt;br/&gt;-Suspending the rules dictating how senate meetings are run&lt;br/&gt;Senate President Megan Marzec and Vice President Caitlyn McDaniel could not be reached for comment by press time.&lt;br/&gt;"Student Senate holds that all students and workers alike deserve a living wage," the resolution reads.&lt;br/&gt;The demand to implement a tuition freeze, beginning the 2015-16 academic year, is from Restart's campaign, which Marzec and McDaniel both ran on in last year's senate election.&lt;br/&gt;Marzec was also among four students arrested at a Board of Trustees meeting during the Spring Semester of the 2012-13 academic year for protesting a tuition increase.&lt;br/&gt;Senate also formed the Administrative Accountability Committee early this year to review OU administrators' salaries.&lt;br/&gt;Last week, some senators, including Will Klatt, chair of the Administrative Accountability Committee and Governmental Affairs commissioner, went to the office hours of OU President Roderick McDavis to protest his "excessive compensation."&lt;br/&gt;Some students said McDavis was "hostile" in that meeting and "yelled" at them; top university administrators disagreed, calling the meeting "tense."&lt;br/&gt;The board gave McDavis a 7.8 percent pay raise in August, increasing his base pay to $465,000, and he received a bonus of $85,000. The board said he deserved the increased compensation because of his successful fundraising, OU's record enrollment and leadership on renovating campus, among other reasons.&lt;br/&gt;Senate will also vote to support the F--kRapeCulture Homecoming March, calling for the mandatory participation of OU students in taking the Not Anymore online sexual assault education program and expanding training for the Athens and OU police departments on how to handle sexual assault cases.&lt;br/&gt;Senate will also consider suspending Robert's Rules of Order, which govern when members can speak, introduce motions or resolutions and generally control the flow of senate meetings.&lt;br/&gt;The resolution states that "most students are probably unfamiliar with Robert's Rules of Order, and therefore they pose a barrier to student participation during discussion."&lt;br/&gt;@Alisa_Warren&lt;br/&gt;aw120713@ohio.edu</t>
         </is>
+      </c>
+      <c r="L180" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="181">
@@ -8293,10 +8840,13 @@
           <t>Police violence</t>
         </is>
       </c>
-      <c r="J181" t="inlineStr">
+      <c r="K181" t="inlineStr">
         <is>
           <t>Rutgers students have remained vocal throughout the past few weeks of heated racial tension stemming from grand jury decisions. Organizing quickly, students protested on at least three separate occasions, while two of the protests have been large, organized movements incorporating hundreds of members of the Rutgers community at a time. The most recent protest took place this past Friday in response to the Eric Garner grand jury decision not to indict the officer that caused his death using an illegal chokehold. Students began gathering at the Douglass Student Center and then marched onto Route 18 during rush hour traffic, where they remained for roughly an hour. While standing on the highway, a number of student protestors participated in a die-in, laying down in solidarity with victims of police brutality, as a human chain of students formed around them.&lt;br/&gt;During the protest, students began using #RU4BlackLives to express their sentiments online. Many of those affiliated with the University have made clear their disdain for institutionalized racism and police brutality, as well as their disapproval for the two grand juries that failed to indict officers involved with the deaths of unarmed black men. This hashtag addresses student sentiment over the recent issues, but what can be said for the administration? While today marks the first official business day since students shut down Route 18, University President Robert L. Barchi and the administration have yet to release a statement addressing student protests and the cause at large.&lt;br/&gt;In the past, the Rutgers administration has heard student voices and acted accordingly. When students protested apartheid in South Africa, the administration responded by divesting from a handful of companies with holdings in the country. While those actions stemmed directly from protesting administration and staging a sit-in at a meeting of the Rutgers Board of Governors and the Board of Trustees, this is not an issue that students should have highlight to administration. The lack of response makes it seem as though they have turned a blind eye to an issue that is erupting across the nation. As an institution, Rutgers uses its vast diversity as a selling point. The number of students from a myriad of minority backgrounds and various socioeconomic classes is constantly referenced in order to attract more applicants. There are also a number of University programs that support the academic growth of minority students, but if the University does not address social issues pertaining to such a large group of students, then what can be said of the importance Rutgers really places on diversity?&lt;br/&gt;Both the Rutgers University Police Department and the New Brunswick Police Department have also failed to release statements regarding protests. Although the level of professionalism displayed by NBPD during Friday's protest was commendable, their silence speaks volumes. Claims have been made that protesting in New Brunswick does nothing and that student should go major cities in order to have their voices heard. But two years ago, New Brunswick Police officers were involved in the fatal shooting of an unarmed black man, showing that police brutality is a local issue. In September of 2011, Barry "Gene" Deloatch was shot after being approached by New Brunswick police. Students brought the issue to the police by ending their protest with a die-in at the New Brunswick Police Department, an action that merits a response.&lt;br/&gt;Faculty members and professors have come forward to stand in solidarity with student protestors and their actions have not gone unnoticed. But Barchi and the administration have so far not even released a statement of solidarity with the protestors, students and others affected by the injustices that have been made clear in our own judicial system. We hope to see more support from the administration for, at the very least, the students at this University who they so proudly present as the faces of Rutgers' diversity.</t>
         </is>
+      </c>
+      <c r="L181" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="182">
@@ -8336,10 +8886,13 @@
           <t>University governance, admin, policies, programs, curriculum, Tuition, fees, financial aid</t>
         </is>
       </c>
-      <c r="J182" t="inlineStr">
+      <c r="K182" t="inlineStr">
         <is>
           <t>In protest of the University's decision to charge all students not enrolled in the Student Health Insurance Plan a $350 fee to address Gannett Health Services' financial concerns, over 100 students occupied Day Hall Monday. The group of Cornellians, mobilized by the Save the Pass Coalition, expressed frustrations while rallying in the lobby of Willard Straight Hall before marching to the Office of the President and Provost. Although we are supportive of constructive discourse, we at The Sun are concerned by the overall lack of respect shown for administrators who, we believe, tried to have a meaningful conversation with the opposition.&lt;br/&gt;We understand the necessity for appropriate dissent in directing change across the University. Cornellians hold a long history of fighting for change, from combating in loco parentis and the Vietnam Warin the 1950s and 1960s and Apartheid in the the 1980s. In spite of this history of activism, there are still challenges facing both administrators and students at Cornell. We also agree with the protesters and the greater student body who have expressed concerns with the lack of transparency in creating the fee. Yet, we find the precedent set by those who outright disrespected administrators worrying. There are times to be disruptive in a constructive manner to garner the attention of those in charge. However, we believe once individuals gain that attention, it is imperative to hold a respectful dialogue.&lt;br/&gt;When President David Skorton first made himself available to students occupying his office, no one approached him. Instead they chose to disrupt the operations of Day Hall by playing music and encouraging "dance parties" outside Skorton's office and across the administrative building. When he returned later to try to approach students again, protesters disregarded what he said, instead heckling the President and interrupting him as he tried to justify the reasons for the health fee and other issues that were brought up. There was an opportunity for this protest to be meaningful and changing, yet protesters were disjointed in their message and lacked civility, belittling their legitimacy and cause. The protests on Monday are worryingly reminiscent of the student takeover of an April Student Assembly meeting, protesting the S.A.'s decision to table Resolution 72, which called for the University to divest from pro-Israeli corporations. The events that transpired Monday and last semester showcase the importance of a respectful democratic process in handling larger issues on campus.&lt;br/&gt;Students have the right to express their opinions and we encourage all students to find ways to make their voices heard through constructive forums and proper channels. For students to demand transparency and respect from not only administrators, but also student leaders, it is imperative that they are respectful in return.</t>
         </is>
+      </c>
+      <c r="L182" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="183">
@@ -8379,10 +8932,13 @@
           <t>Pro-Palestine/BDS</t>
         </is>
       </c>
-      <c r="J183" t="inlineStr">
+      <c r="K183" t="inlineStr">
         <is>
           <t>Jewish Organizations on campus worried about impact on students&lt;br/&gt;Photo courtesy of Eve Panagapko&lt;br/&gt;The Ontario branch of the Canadian Federation of Students (CFS) unanimously voted to boycott Israel at their latest general meeting following ongoing conflicts in the region.&lt;br/&gt;The proposal to join the Boycott, Divestment and Sanctions (BDS) movement was put forward by the Ryerson Students’ Union.&lt;br/&gt;Anna Goldfinch, an executive member of the CFS, said the motion was passed “to condemn the current actions of the state of Israel in Gaza including the bombing of two universities,” and to pressure the Harper government to “stop supplying arms to Israel and the Canada-Israel free trade agreement.”&lt;br/&gt;Conflict in Gaza was revived this summer as 2,100 Palestinians, mostly civilians, were killed. Seventy Israelis were also killed. A cease-fire was established Aug. 27.&lt;br/&gt;Each student union will decide to what extent they will implement the boycott.&lt;br/&gt;Anne-Marie Roy, president of the Student Federation of the University of Ottawa (SFUO), said they don’t currently have a student mandate on the BDS, but the SFUO supports the motion because they already have a mandate for solidarity work for Palestinians.&lt;br/&gt;Roy referred to the Right to Education campaign, which U of O students voted to join in 2009. The campaign “addresses the specific challenges around access to education for Palestinian youth,” she said.&lt;br/&gt;Members of the Jewish community on campus are troubled by the CFS’s decision.&lt;br/&gt;Chaim Boyarsky, rabbi and co-director of the Rohr Chabad Student Network of Ottawa, said he was “not surprised, but extremely pained” by the boycott.&lt;br/&gt;“America killed hundreds and thousands of people fighting in Iraq, and no one is boycotting America,” he said.&lt;br/&gt;Boyarsky said the students he has spoken to have expressed “shock, disbelief, and pain, but a strong sense of determination.”&lt;br/&gt;“It’s very disappointing to see any type of activity from groups that are supposed to be representing our students on campus adopting any type of element that makes it hostile and uncomfortable on campus,” said Scott Goldstein, executive director of the campus Jewish community Hillel Ottawa.&lt;br/&gt;However, Roy said it’s “not a religious issue, and we’re willing to support Jewish students on campus in any way.”&lt;br/&gt;The BDS movement began in 2005 when Palestinian civil society called for the boycott of Israeli products, divestment from Israeli corporations, and sanctions against Israel “until it complies with international law and Palestinian rights.”&lt;br/&gt;Goldfinch said it’s a tactic that’s been used historically “in a number of political campaigns—everything from ending apartheid in South Africa to opposing the tar sands.”&lt;br/&gt;Goldstein said that “people don’t want to be on a campus environment that is not promoting peace and not promoting dialogue,” and that the BDS “does not promote peace.”&lt;br/&gt;“This type of motion, to me, shows why and how disconnected (the CFS) is from the general student body on our university campuses,” he said.&lt;br/&gt;Last March at the U of O, the Muslim Students Association asked students to boycott Sabra hummus because of its connections to Israel.&lt;br/&gt;More recently, the University of Regina cut ties with Hebrew University in Israel last month, following protests from students and community members. However, U of R president Andrew Gaudes said the university ended the relationship only because the “course content offered by Hebrew University did not meet our needs.”&lt;br/&gt;Gaudes told the U of R’s campus newspaper the Carillon that “as a university, we do not agree with a blanket exclusion of Israeli institutions from these types of conversations.”&lt;br/&gt;Share this:Click to share on Twitter (Opens in new window)Click to share on Facebook (Opens in new window)Click to share on Google+ (Opens in new window)</t>
         </is>
+      </c>
+      <c r="L183" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="184">
@@ -8422,10 +8978,13 @@
           <t>Economy/inequality</t>
         </is>
       </c>
-      <c r="J184" t="inlineStr">
+      <c r="K184" t="inlineStr">
         <is>
           <t>Click on a title or quote to read more!&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;The Tariq Khan Drama&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;The Students’ Society of McGill University (SSMU) saw its fair share of the short-lived SSMU President Tariq Khan this year. Elections SSMU invalidated Khan’s election as SSMU President on April 1, 2014 – a week after he was elected president by a margin of only 78 votes – due to SSMU bylaw infractions committed during his campaign. The violations included the participation of individuals external to SSMU in his campaign, the sending of unsolicited text messages to the public – for which he had been censured on March 21, the last day of the campaign period –  inconsistencies in campaign expenditures, and the impingement of the spirit of a fair campaign and of the voting process.&lt;br/&gt;Following his invalidation, Khan filed an appeal with the SSMU Judicial Board (J-Board), which upheld his invalidation on April 29. Khan later took this issue to the Superior Court of Quebec and filed a request on May 29 for a preliminary injunction to reinstate him as SSMU President until the full hearing for a permanent injunction. The Court dismissed his application on June 3, reasoning that his reinstatement would have incurred additional costs and caused undue inconvenience on the part of SSMU. Khan later withdrew his court case in October before its full hearing due to financial motivations and the decreasing timeliness of the case.&lt;br/&gt;Khan resurfaced on the first day of the 2015-16 SSMU elections when screenshots of a Facebook conversation were released on reddit, revealing recently-elected SSMU President Kareem Ibrahim’s suggestion to hack Khan’s Facebook account last year. Upon news of the screenshots, he revealed his intentions to update the police report that he filed after his account was allegedly hacked on March 27, 2014.&lt;br/&gt;—Emma Noradounkian&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Campus unions get moving&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Compared with 2011’s McGill University Non-Academic Certified Association (MUNACA) strike, the past few years have been fairly quiet on the union front. This year, however, has seen a flurry of activity at McGill unions.&lt;br/&gt;Floor fellows began a union drive over a year ago in November 2013, driven by the University’s earlier push for a change in residence models. Since then, floor fellows have succeeded at forming a union, and joined the Association of McGill University Support Employees (AMUSE) last May. The process, however, has not been without hiccups: this January,collective agreement negotiations between the University and the floor fellows bargaining unit stalled over the exclusion of the “core values” of floor fellows (namely their anti-oppressive mandate and harm reduction approach) from the proposed agreement. The negotiations have started again and are currently ongoing.&lt;br/&gt;McGill’s Teaching Union, AGSEM, has also been working to unionize undergraduate teaching support staff, which include course graders, note-takers, and teaching assistants (TAs). Despite receiving support from post-grads and undergrads, the process has not been without tensions: McGill challenged AGSEM’s promotion of its own union campaign due to disputing interpretations of the Quebec Labour Code. At the date of publication, the union drive is still ongoing.&lt;br/&gt;This year also saw a merger between AMUSE and MUNACA, despite some internal trepidation over their differing sizes. Joint bylaws are on the way.&lt;br/&gt;—Molly Korab&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;“I cannot celebrate the status quo of mental health support at McGill.”&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;The mental health landscape at McGill for the 2014-15 academic year has been a disappointing one. Though a working group was struck under the purview of Senate in October 2013, most of the recommendations issued by the group in June 2014 have yet to be implemented. Of the 36 initiatives on the roster, only two have been completed, the first being the development of a student services app, and the second publicly presented only as “further [development] of a robust early alert program.”&lt;br/&gt;While both the administration and student government have been pursuing mental health services reform, they do not appear to be working closely. SSMU VP University Affairs Claire Stewart-Kanigan told The Daily in October, around the time the University announced its intention to create a ‘wellness portal,’ that the relationship between the two was “a consultative arrangement, not a partnership. Given that SSMU is named as a partner on the website, consultation is not enough.”&lt;br/&gt;There have been no updates on the ‘wellness portal,’ projected to be launched in Winter 2015.&lt;br/&gt;Most of the visible events that have taken place this year – in particular, the second annual Students In Mind conference on mental health in October and the Mental Health Awareness Week in November – were largely student-driven and student-led initiatives. Additionally, the most vocal advocates for mental health reform have been students.&lt;br/&gt;In addition to managing the planning and execution of the Mental Health Awareness Week, Stewart-Kanigan oversaw the successful launch of SSMU’s new mental health department, which involved the hire of a coordinator and the development of a mental health listserv to promote peer and professional support services for students and forward student-led anti-stigma initiatives.&lt;br/&gt;­&lt;br/&gt;—Emily Saul&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Tense debates at General Assemblies&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;After years of SSMU General Assemblies (GAs) that have failed to reach quorum or present particularly political motions, portions of this year’s GAs saw huge turnout – with over 700 students attending the Fall 2014 GA and over 500 students at the Winter 2015 GA – as well as plenty of controversy.&lt;br/&gt;Most notably, both GAs saw motions that poked at the long-dormant Israel-Palestine divide on campus. At the Fall 2014 GA, a motion to stand in solidarity with the people of the occupied Palestinian territories and condemn Israel’s violence toward Palestine over the summer was postponed indefinitely, with 402 in favour and 337 against, after hours of debate. At the Winter 2015 GA, a motion to divest from companies profiting from the illegal occupation of the Palestinian territories garnered the endorsement of many campus groups (including The Daily), but failed by only 64 votes.&lt;br/&gt;Despite the intense attention given to these two motions, a number of other political motions passed, mandating SSMU to take action on diverse issues such as unpaid internships, military research, climate change, and austerity. SSMU also saw a J-Board challenge after the contentious postponement of the Fall 2014 Palestine motion, where the judicial body ruled that simplified standing rules should be adopted and publicized at GAs to better facilitate debate.&lt;br/&gt;More broadly, this year’s GAs have prompted a campus-wide (and still ongoing) dialogue on the political role of the student union – which most notably played itself out in the recent 2015-16 SSMU executive elections – with some students questioning whether SSMU should take stances on ‘divisive’ political issues.&lt;br/&gt;—Dana Wray&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Students against austerity&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;This year has seen a whirlwind of opposition against austerity measures and budget cuts set in place by the Liberal provincial government, which have reduced funding to social services, including welfare, healthcare, and education. In the fall, as part of an ongoing push that began even before this academic year, students at UQAM organized a group to allow students and community members to work together to protest these cuts: the Comité Printemps 2015, which helped mobilize around 80,000 students to go on strike on Halloween, and over 80,000 students planned to strike against austerity during March and April. This mobilization has not evaded McGill, as French language and literature students recently voted to go on strike for a week, and other departments have planned strike votes.&lt;br/&gt;These student initiatives contrast with the stance taken by the McGill administration, which has been accommodating of austerity measures. McGill has been making cuts of its own, after undergoing $45 million in cuts from the provincial government over the last four years. The results of these cuts have been felt by workers at McGill, as the administration has set up a hiring freeze, decreasing the number of jobs available, and increasing the workloads of many employees. To combat the administration’s decrease in the number of full-time jobs at McGill, as well as the fact that many positions with benefits have been replaced with lower-paid, part-time jobs that do not receive benefits, AMURE recently voted to start a fund for counselling services for its members.&lt;br/&gt;&lt;br/&gt;In response to the austerity measures taken by both McGill and the Quebec government SSMU and the Post-Graduate Students’ Society (PGSS) have taken stances against the government’s measures and asked McGill to oppose these huge cuts. At the SSMU Fall 2014 GA, students voted to add advocating against austerity to the portfolio of the VP External, and SSMU has since hosted an anti-austerity activities night to show students just how wide-reaching the damaging effects of austerity can be.&lt;br/&gt;—Jill Bachelder&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Sustainability at McGill&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Many important initiatives that began in previous years were continued and strengthened over the course of this one. Divest McGill helped organize a bus to take McGill and Concordia students to the People’s Climate March in New York City, where over 400,000 people marched in the streets of Manhattan to protest the United Nations Climate Summit and raise awareness about global warming. Divest also submitted a new petition for McGill to divest from fossil fuel companies to the Board of Governors (BoG), making a comeback two years after its first petition was presented to, and rejected by, the BoG. In addition, over 100 faculty members signed on to an open letter submitted to the BoG in support of divestment.&lt;br/&gt;SSMU also continued its efforts to promote sustainability on campus, starting a composting program in the Shatner building, and joining Étudiant(e)s contre les oléoducs (ÉCO), after the a motion passed at the Fall 2014 GA that mandated SSMU to stand alongside groups combatting climate change.&lt;br/&gt;Finally, the McGill Office of Sustainability launched its Vision 2020 program, an initiative aiming to create a more sustainable McGill by the year 2020.&lt;br/&gt;—Jill Bachelder</t>
         </is>
+      </c>
+      <c r="L184" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="185">
@@ -8465,10 +9024,13 @@
           <t>University governance, admin, policies, programs, curriculum, Public funding for higher education</t>
         </is>
       </c>
-      <c r="J185" t="inlineStr">
+      <c r="K185" t="inlineStr">
         <is>
           <t>Hundreds of students marched to the California Capitol in Sacramento on Monday, demanding more state funding for the University of California and calling for Gov. Jerry Brown and UC President Janet Napolitano to be more ansparent in their budget negotiations.The UC Student Association, which advocates for University students on student-related issues such as tuition, held its annual Student Lobby Conference this weekend.Students lobbied legislators and went to workshops where they learned sategies about how to advocate for specific issues. They also attended workshops on UCSA's budget and legislative priorities.Undergraduate students from UCLA attended the conference, with delegates coming from all UC campuses except UC Hastings College of the Law.&lt;br/&gt;About 400 students attended the conference.In November, the UC passed a proposal to potentially increase tuition by up to 5 percent annually for the next five years, contingent on the state increasing funding for the University. Brown's proposed budget for the 2015-2016 fiscal year allocates about $120 million more in state funding, $100 million less than what the UC has asked for. The additional state funding is contingent on the University holding tuition flat.Brown and Napolitano are the two members of the Select Advisory Committee on the Cost Sucture of the University, the so-called "committee of two" formed in January to look at the University's cost sucture. They will update their committee findings at the next UC Regents meeting in May. However, students have called for them to discuss the findings further publicly.Students at the lobbying conference, calling themselves the Committee of 240,000, staged a rally on the west steps of the California Capitol on Monday. The 240,000 number was meant to represent the approximate number of students at the UC."Committee of two. We are out here; where are you?" students chanted.Students at the rally also held up signs criticizing Napolitano and Brown, with messages such as "Committee of two, shame on you" and "Brown better have my money."Students also tweeted with hashtags such as #Committeeof240000 and called for the committee to hear more student input.Napolitano told the Daily Bruin Editorial Board on April 9 that she would be open to talking with Brown about bringing students into committee meetings.At the conference, students also held an awards banquet, where Fossil Free UC received the Advocate of the Year award for its work calling for the UC to divest from companies that profit from the exaction of fossil fuels. Kevin Sabo, chair of the UCSA Board of Directors, received the award for Student Advocate of the Year.Brown will release his revised state budget for the next fiscal year in May, when students may learn more about whether the UC averted a tuition hike.Compiled by Jorge Valero, Bruin conibutor.</t>
         </is>
+      </c>
+      <c r="L185" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="186">
@@ -8508,10 +9070,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J186" t="inlineStr">
+      <c r="K186" t="inlineStr">
         <is>
           <t>SAN FRANCISCO - At its meeting Wednesday, the UC Board of Regents' Committee on Investments voted to approve a recommendation from the UC task force on sustainable investing to continue the university's investments in fossil fuel companies.&lt;br/&gt;At the meeting, members of Fossil Free UC, a coalition advocating divestment, protested the recommendation's proposal to not divest. The recommendation encourages the university to implement a framework for sustainable investment by the end of the fiscal year and invest $1 billion into green initiatives over the next five years. The full UC Board of Regents will vote on the recommendation Thursday.&lt;br/&gt;"We sought to take a truly holistic approach and make recommendations that could have meaningful long-term impacts," said Jagdeep Singh Bachher, UC chief investment officer and head of the task force.&lt;br/&gt;According to UC spokesperson Dianne Klein, the majority of the task members, after looking at research on the issue, felt that divestment would not do much to alleviate the effects of climate change. The UC system currently invests $10 billion out of the $91 billion managed by the university in energy companies.&lt;br/&gt;"(Divestment) would certainly have a negative effect on our portfolio as far as returns," Klein said.&lt;br/&gt;Student Regent Sadia Saifuddin attempted to make an amendment to the final recommendation that would insert language considering divestment from coal companies in the future, which ultimately did not pass.&lt;br/&gt;As part of the recommendation, the university would sign on to the United Nations Principles for Responsible Investment, a worldwide investor network dedicated to helping its members invest sustainably. The recommendation also proposes that the university integrate environmental, social and governance factors into its portfolio decisions.&lt;br/&gt;"We're absolutely committed to investing in our future," Bachher said. "Making that commitment is the right thing to do in the long term."&lt;br/&gt;Members of Fossil Free UC assembled in a protest that began outside and continued into the meeting. Chanting slogans, the protesters held signs reading, "We are worth more than fossil fuels" and "Students not fossil fuels."&lt;br/&gt;According to Victoria Fernandez, a UC Berkeley senior and a member of both Fossil Free UC and the task force, students were not fairly consulted during the process leading up to the task force's recommendation. She said while Greg Boyce, CEO of coal company Peabody Energy, was invited to lobby the committee, students were not given the chance to bring in experts, such as Don Gould, an asset manager and a Pitzer College trustee, to advocate divestment.&lt;br/&gt;"Industry voice was being prioritized over the voices of advocates for divestment," Fernandez said.&lt;br/&gt;This year, Stanford University divested from coal companies, and Pitzer College removed all assets in fossil fuel companies.&lt;br/&gt;Contact Hiep Nguyen at [email protected] and follow him on Twitter @_hiepn.</t>
         </is>
+      </c>
+      <c r="L186" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="187">
@@ -8551,10 +9116,13 @@
           <t>University governance, admin, policies, programs, curriculum, Labor and work, Economy/inequality</t>
         </is>
       </c>
-      <c r="J187" t="inlineStr">
+      <c r="K187" t="inlineStr">
         <is>
           <t>While the national Fight for $15 campaign focuses on raising the federal minimum wage, the300 students and professors from Columbia and other universities who gathered on Low Plaza on Wednesday also demanded an increase in the minimum wage and salaries for adjunct professors.&lt;br/&gt;Wednesday's protest coincided with a number of national Fight for $15 protests, including demonstrations in Times Square and Chicago. On Low Steps, before the protesters marched down Broadway and headed downtown, students, professors, and speakers advocated for raising the salary of adjunct professors, in addition to calling for a higher minimum wage for workers.&lt;br/&gt;"We talk about low-wage workers, we think about McDonald's employees, but what we don't think about as often are the people who teach our classes at this Ivy League University," RJ Pettersen, GSAS '15 and a master's sociology student, said.&lt;br/&gt;The protest was the first major Fight for $15 event on Columbia's campus since the nationwide campaign-which has gained local support since it began in New York City in 2012-first came to Columbia's campus in February. Students from New York University, the City University of New York, the New School, and various local high schools also attended the protest.&lt;br/&gt;"The current poverty wages and lack of unionization plaguing too many in our society-from fast-food workers to adjunct professors-are a barrier to entry for any upward mobility," Columbia University Democrats Media Director Jordana Narin, CC '17, said in a message to Spectator.&lt;br/&gt;Protesters held posters and banners during a speak-out on Low Plaza before marching to a McDonald's on West 96th Street and then heading to Times Square in order to spread awareness across the city.&lt;br/&gt;"There's so many adjuncts that I know who can't make it. They're going from school to school to school, working at three or four different schools, and they're still below poverty wage," Elizabeth Owen, TC '01 and an adjunct professor at Teachers College, said.&lt;br/&gt;Owen said that she teaches 40 to 50 students-each of whom pay more in tuition than she makes as her salary.&lt;br/&gt;"It's not fair to the students," she said. "We don't have the time to give them. We don't have the energy, we don't have office hours, we don't have an office to meet them in, we're sponsoring their master's project and we don't have the adequate time to put into it."&lt;br/&gt;An adjunct professor at Barnard College-who asked to remain anonymous out of concern for job security-said that the disparity between tuition and pay for adjuncts is upsetting.&lt;br/&gt;"I'm also a parent who's paying for a kid to go to a prestigious university much like this one," the adjunct professor said. "The disparity between what they charge me to send my kid to school and what I'm earning at the same time-it's infuriating."&lt;br/&gt;At the speakout, undergraduate students said they shared the concerns expressed by adjunct professors.&lt;br/&gt;"This is an issue for students, it's an issue for professors, and it's an issue for anyone who cares about a better economy for everyone," Ben LaZebnik, CC '18 and an organizer with Columbia Fight for 15, said.&lt;br/&gt;In addition to undergraduate student organizers from the Fight for $15 movement, many of the protest's attendees came from the CU Dems or fossil fuel divestment groups such as Barnard Columbia Divest for Climate Justice, which was formerly known as Barnard Columbia Divest.&lt;br/&gt;"Climate justice is impossible in a system that prioritizes profit over people," CDCJ organizer Elana Sulakshana, CC '17, said during the speak-out. "Communities devastated by poverty wages and mass incarceration are the most vulnerable to the effects of climate change. The fight for 15 is the fight for a livable planet."&lt;br/&gt;For others, though, the Fight for $15 movement has a more personal meaning.&lt;br/&gt;"In high school, I worked in fast food and I didn't think it was right to see my co-workers have to balance two jobs and have to work overtime in order to just barely make it," Ja'da Young, CC '17, said.&lt;br/&gt;"It's important for students to get involved because a lot of us are also workers affected by this," she added. "When we graduate as well we're inheriting this economy, so it's important to advocate for what we believe is right and what we want."&lt;br/&gt;news@columbiaspectator.com | @ColumbiaSpec.</t>
         </is>
+      </c>
+      <c r="L187" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="188">
@@ -8589,10 +9157,13 @@
           <t>Labor and work, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J188" t="inlineStr">
+      <c r="K188" t="inlineStr">
         <is>
           <t>Hasbara at York has started a campaign to highlight what they believe to be anti-Israeli politics from CUPE 3903, by taking over the union local’s social media campaign.&lt;br/&gt;On January 15, Hasbara at York, an Israeli student advocacy group, created an event on Facebook asking its members to tweet issues that would make a better York for them, highlighted around CUPE 3903’s pro-BDS stance, which Hasbara sees as racist and anti-Semetic.&lt;br/&gt;“Our grievance with CUPE is that it states that it stands for justice and equity but has been participating in racist activities. They have adopted the BDS motion (Boycott, Divestment, and Sanctions) which makes false accusations on Israel. This motion is anti-Semitic because it inequitably targets the Jewish state presenting a double standard and encourages a boycott of both Israeli citizens and Palestinian workers,” writes Ariella Daniels, president of Hasbara at York.&lt;br/&gt;“The motion is a clear violation of the Ontario Human Rights Code which forbids discrimination by the basis of place of origin. CUPE has attended anti-Israel rallies, proudly waving their flags with those who stand with the flag of Hamas, an internationally recognized terrorist organization. CUPE claims to stand for ‘safe space’ and is suppose to represent a diverse amount of people, yet they marginalize members they claim to represent.”&lt;br/&gt;Many of the tweets, as seen below, accuse CUPE of making campus an unsafe space.&lt;br/&gt;&lt;br/&gt;When asked by Excalibur on January 16 whether he has seen the negative tweets on his campaign, Faiz Ahmed, chairperson of CUPE 3903, says, “I don’t have a very big online presence, so I don’t see that.”&lt;br/&gt;When informed that many of the tweets accuse CUPE 3903 of racism, in relation to support of divestment, he says incredulously, “That CUPE is racist? Those types of allegations are clearly laughable.”&lt;br/&gt;He adds “But what does [BDS] to do with our bargaining?”&lt;br/&gt;CUPE 3903 has been running the #betteryork campaign online to drum up support from the wider York community during their bargaining period with the university. CUPE 3903 has been without a contract since August.&lt;br/&gt;Daniels says Hasbara at York decided to use #BetterYork because it is the students’ responsibility to let the decision makers know what a #BetterYork really means.&lt;br/&gt;“CUPE is encouraging the use of #BetterYork for their vote on striking, to state what a #BetterYork means. We are doing just that by exposing to Twitter users, of the true face of CUPE and their hypocrisy. A #BetterYork is without the BDS motion and support for anti-Israel activities both on campus and in the union.”&lt;br/&gt;On Twitter, CUPE 3903 has not directly responded to many of the allegations and complaints by students or by Hasbara at York.&lt;br/&gt;Likewise, Daniels says, “We are not planning on engaging with CUPE any further. Nevertheless, being that CUPE has aligned itself with Students Against Israeli Apartheid, Ontario Public Interest Research Group, York Federation of Students and Graduate Students Association, who all preach hatred against the Jewish state, it is our mandate to expose and correct this problem within CUPE and the rest of these organizations.”&lt;br/&gt;&lt;br/&gt; &lt;br/&gt;Follow along Hasbara at York’s social media campaign here: Hasbara at York targets CUPE 3903’s #BetterYork campaign&lt;br/&gt;&lt;br/&gt;Divyesh Mistry, Executive Editor (Online)&lt;br/&gt;Ryan Moore, Assistant News Editor&lt;br/&gt;Featured image courtesy of Hasbara at York on Facebook.&lt;br/&gt;Tweets courtesy of Twitter.</t>
         </is>
+      </c>
+      <c r="L188" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="189">
@@ -8632,10 +9203,13 @@
           <t>Tuition, fees, financial aid</t>
         </is>
       </c>
-      <c r="J189" t="inlineStr">
+      <c r="K189" t="inlineStr">
         <is>
           <t>A coalition of campus groups will rally at Sather Gate on Tuesday to demonstrate against the university's plan to increase tuition over the next five years, along with other protesting groups across the UC system.&lt;br/&gt;At the UC Board of Regents meeting at the UCSF Mission Bay campus Wedneday, the regents will vote on proposed 5-percent increases in tuition and fees annually over the next five years, if state funding remains at 4 percent. Students from various UC campuses will be bussed to the meeting to demonstrate against the plan.&lt;br/&gt;The rally and march, hosted by the ASUC Office of the External Affairs Vice President, will begin at 12:30 p.m. The event aims to raise awareness of the proposal, according to Margaret Mary Downey, a head steward of United Auto Workers Local 2865, the union representing UC student-workers that is participating in the rally.&lt;br/&gt;"Students are sacrificing their time and well being to let the regents know that this is not OK," said Spencer Pritchard, CalSERVE chair. "We've been able to stop fee hikes in 2011 when students protested. It's possible if enough students show up and email the regents."&lt;br/&gt;Campus spokesperson Janet Gilmore said in an email that she anticipates the rally will be peaceful.&lt;br/&gt;Before the rally, Fossil Free Cal will be hosting a mock regents meeting at noon at Sather Gate, according to Jake Soiffer, field organizer for the California Student Sustainability Coalition. At the mock meeting, Soiffer said in an email, students will dress up as regents and address students asking for decreased tuition and divestment in fossil fuels.&lt;br/&gt;Protesters will also speak and demonstrate at the Wednesday regents meeting. Students from UC Berkeley will be driven to the meeting in buses with the help of the American Federation of State, County and Municipal Employees Local 3299, said Caitlin Quinn, external affairs vice president.&lt;br/&gt;"We will also have students studying in public spaces to show that we're still students and still trying to get through all our classes despite all this," Quinn said in an email, adding that demonstrators plan to be at the scene when the regents arrive.&lt;br/&gt;According to UC Office of the President spokesperson Brooke Converse, a 30-minute public comment period will be held at the start of the meeting.&lt;br/&gt;Kevin Sabo, University of California Student Association board chair, said students from UC Davis, UC Santa Cruz, UCLA, UC Irvine, UC San Diego and UC Riverside also plan to attend.&lt;br/&gt;"We want to show the regents that students are not children and not incapable of advocating to the UC and state government that we have the organizational capacity ... to make change," Sabo said. "We hope that the regents leave the meeting knowing it was a mistake to leave students out of the process."&lt;br/&gt;UCSA created a petition against the tuition increase that garnered more than 10,000 signatures as of Monday.&lt;br/&gt;According to Olivia Lichterman, a UAW 2865 member, a general assembly will begin at Sather Gate at 5 p.m. after the regents meeting to allow community members to organize and channel frustrations regarding the tuition increase plan through an open forum.&lt;br/&gt;Rallies will also take place at other UC campuses tomorrow.&lt;br/&gt;At UC Davis, various groups plan to protest the tuition plan and occupy an administration building, said Harley Litzelman, director of the UC Davis student government's office of advocacy and student representation.&lt;br/&gt;Contact Sierra Stalcup at [email protected] and follow her on Twitter @SierraStalcup.</t>
         </is>
+      </c>
+      <c r="L189" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="190">
@@ -8675,10 +9249,13 @@
           <t>Economy/inequality</t>
         </is>
       </c>
-      <c r="J190" t="inlineStr">
+      <c r="K190" t="inlineStr">
         <is>
           <t>Students, Professors Wait for Decision After First Tribunal&lt;br/&gt;Eight Concordia Students Charged With Disruptions Call Process “Problematic”&lt;br/&gt;News by Michelle Pucci — Published December 12, 2015 | Updated December 13, 2015 | Comments&lt;br/&gt;Follow @michellempucci&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;The tribunal was for student-protesters who are accused of disrupting classes last semester.  File Photo Shaun Michaud&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Eight of the estimated 24 students accused of disrupting classes during last semester’s strikes are waiting for a decision from a tribunal last week, the latest installment in a process they call “problematic” and “abusive.”&lt;br/&gt;The original charges came after a ripple of anti-austerity protests and student strikes took place in Quebec CEGEPs and universities last spring. &lt;br/&gt;About a month after complaints were filed by professors before the summer break, Concordia agreed to join them as co-complainants. Concordia’s spokesperson Chris Mota said the university became a co-complainant in support of the professors and will support the outcome of the hearings.&lt;br/&gt;Despite hiring multiple mediators to settle the charges informally between students and professors, there are no plans for more efforts of mediation in the future.&lt;br/&gt;“Mediation is voluntary and can take place so long as all parties wish to participate,” spokesperson Chris Mota wrote in an email. “The fact that tribunals took place last week suggests that the mutual interest in continuing mediation was not present.”&lt;br/&gt;The remaining students charged will likely also be called to a tribunal. Students are calling on the university to drop the charges.&lt;br/&gt;“We feel that the university is also responsible in a major way for what happened,” said Aloyse Muller, one of the students involved in the Dec. 2 tribunal. “They’re trying to present themselves like a neutral player when they’re really not.”&lt;br/&gt;The current events stem from spring 2015 anti-austerity protest actions, when more than a dozen student associations and the faculty of fine arts student association voted to strike at least one day of classes last semester. Some associations voted to strike for several weeks.&lt;br/&gt;Concordia’s response was to cancel a day of classes for each department, whose students voted to strike or to participate in city-wide protest, either March 23 or April 2. &lt;br/&gt;On April 1, students enforcing the strike mandate entered a political science class with noise-making machines and chanted until most students walked out. An official complaint under article 29G of the Code of Rights and Responsibilities was filed by the course professor Graham Dodds. Some of the students also face complaints over other pickets from professors Michael Lipson and Travis Smith. &lt;br/&gt;The first tribunal&lt;br/&gt;The eight students presented evidence, personal statements and called forward witnesses at the tribunal last week. The university said respondents were able to request separate hearings.&lt;br/&gt;The Dec. 2 hearing lasted about eight hours, according to two respondents, and coincided with the final week of classes and final assignments. For students in third or fourth year, exams take place in the last weeks of classes and not during the exam period, says Katie Nelson, one of the eight students at the hearing.&lt;br/&gt;“It’s definitely affected my studies and probably the outcome of those classes, because I’ve either had to take time writing statements of evidence or meet with advocacy or go to the tribunal itself which is about seven or eight hours,” she said.&lt;br/&gt;At least two more tribunals are expected, one for each of the professors who filed formal complaints against students, but dates have yet to be announced.&lt;br/&gt;The university department responsible for tribunals avoids scheduling hearings during exam periods or vacation periods and tries to accommodate panelists, the chairperson, complaintants and respondents. This means the next tribunal will likely take place next semester. &lt;br/&gt;“I’m not sure why they thought it was appropriate to schedule such a long tribunal at such an inconvenient time,” Nelson said. “It definitely shows that the university has very little regard to the actual academic work coming out of students and really illustrates the political nature of the tribunal itself.”&lt;br/&gt;There was no testimony by an administrative representative at the Dec. 2 tribunal, according to Nelson. Mota previously told The Link that the university became a co-complainant to provide professors with information from campus security. Nelson said there was a representative from security at the tribunal.&lt;br/&gt;Even if the jury comes back and recommends the lowest charge, a letter of reprimand, Nelson fears her case might be sent to upper administration since this isn’t the first tribunal she’s faced, or the last. &lt;br/&gt;Following last year’s vote for Boycott Divest Sanction (BDS) of Israel by the Concordia Student Union, Nelson, who was campaigning pro-BDS, was accused of harassment and given a letter of reprimand for a different charge. &lt;br/&gt;Now she faces complaints by two professors, Graham Dodds and Michael Lipson, for disrupting classes while carrying out strike mandates to picket political science classes.&lt;br/&gt;Nelson says she is concerned that Lipson acted as an advocate for Dodds and was present at the tribunal.&lt;br/&gt;“He was privy to all the argumentation, all the personal testimony, all the witnesses presented in Dodds’s case, and now essentially has the upper hand,” she said.&lt;br/&gt;Professors Dodds and Smith declined to be interviewed, since the tribunal process is still ongoing. Lipson did not respond to a request for comment.&lt;br/&gt;Nelson called the tribunal process, a lack of communication and delays in scheduling “legally problematic” and “psychologically abusive,” and hopes the tribunals don’t move on.&lt;br/&gt;“The university should be preparing for the ramifications and consequences of doing that to its students,” she said, promising to look into civil litigation.&lt;br/&gt;Unsuccessful mediations&lt;br/&gt;Mediation, which was touted as a possible venue for resolution of the complaints, doesn’t seem to be a possibility for students and professors anymore.&lt;br/&gt;Concordia began a mediation process in the fall to encourage an informal compromise between professors and students. The first attempt began in early October, but seemingly ended without an agreement.&lt;br/&gt;All participants signed a nondisclosure agreement, which prevented them from speaking with media.&lt;br/&gt;One student has agreed to a mediated settlement, but the terms of the agreement are still unknown. Some other students have had their charges dropped because they were not directly involved in disrupting the classes of the complainants.&lt;br/&gt;About a month later, another round of mediation sessions were organized with new mediators—but the tribunal date had already been set.&lt;br/&gt;“That’s something I found problematic, to have the tribunal at the same time as the mediation—especially a few days before finals,” said Aloyse Muller, one of the students being charged.&lt;br/&gt;An administrative representative was noticeably lacking in all the meetings set up with the purpose of mediation over the semester.&lt;br/&gt;“I have to give it to Concordia, you know, a ‘real education for the real world,’” said Muller, citing the university’s old motto.&lt;br/&gt;“I’ve learned a lot about what’s the mediation process, what’s the problem of having a nine-hour discussion when you have to take caucuses all the time,” he said. “Real education, real helpful, probably better than some of my classes this term.”&lt;br/&gt;Correction: A previous version of this story stated Katie Nelson was charged with harassment. She was accused of harassment, but received a letter of reprimand for a different charge. The Link regrets the error.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;By commenting on this page you agree to the terms of our Comments Policy.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Please enable JavaScript to view the comments powered by Disqus.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Related Reading&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;First Tribunal for Student-Protesters Set for Dec. 2&lt;br/&gt;Jonathan Caragay-Cook&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Opinions&lt;br/&gt;Editorial: These Student-Protester Tribunals Are Just for Show&lt;br/&gt;The Link&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;Concordia Student-Protester Tribunals Suspended&lt;br/&gt;Jonathan Caragay-Cook&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Opinions&lt;br/&gt;Editorial: Make P-6 an Election Issue&lt;br/&gt;The Link</t>
         </is>
+      </c>
+      <c r="L190" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="191">
@@ -8718,10 +9295,13 @@
           <t>Economy/inequality, Public funding for higher education</t>
         </is>
       </c>
-      <c r="J191" t="inlineStr">
+      <c r="K191" t="inlineStr">
         <is>
           <t>Students, Professors Wait for Decision After First Tribunal&lt;br/&gt;Eight Concordia Students Charged With Disruptions Call Process “Problematic”&lt;br/&gt;News by Michelle Pucci — Published December 12, 2015 | Updated December 13, 2015 | Comments&lt;br/&gt;Follow @michellempucci&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;The tribunal was for student-protesters who are accused of disrupting classes last semester.  File Photo Shaun Michaud&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Eight of the estimated 24 students accused of disrupting classes during last semester’s strikes are waiting for a decision from a tribunal last week, the latest installment in a process they call “problematic” and “abusive.”&lt;br/&gt;The original charges came after a ripple of anti-austerity protests and student strikes took place in Quebec CEGEPs and universities last spring. &lt;br/&gt;About a month after complaints were filed by professors before the summer break, Concordia agreed to join them as co-complainants. Concordia’s spokesperson Chris Mota said the university became a co-complainant in support of the professors and will support the outcome of the hearings.&lt;br/&gt;Despite hiring multiple mediators to settle the charges informally between students and professors, there are no plans for more efforts of mediation in the future.&lt;br/&gt;“Mediation is voluntary and can take place so long as all parties wish to participate,” spokesperson Chris Mota wrote in an email. “The fact that tribunals took place last week suggests that the mutual interest in continuing mediation was not present.”&lt;br/&gt;The remaining students charged will likely also be called to a tribunal. Students are calling on the university to drop the charges.&lt;br/&gt;“We feel that the university is also responsible in a major way for what happened,” said Aloyse Muller, one of the students involved in the Dec. 2 tribunal. “They’re trying to present themselves like a neutral player when they’re really not.”&lt;br/&gt;The current events stem from spring 2015 anti-austerity protest actions, when more than a dozen student associations and the faculty of fine arts student association voted to strike at least one day of classes last semester. Some associations voted to strike for several weeks.&lt;br/&gt;Concordia’s response was to cancel a day of classes for each department, whose students voted to strike or to participate in city-wide protest, either March 23 or April 2. &lt;br/&gt;On April 1, students enforcing the strike mandate entered a political science class with noise-making machines and chanted until most students walked out. An official complaint under article 29G of the Code of Rights and Responsibilities was filed by the course professor Graham Dodds. Some of the students also face complaints over other pickets from professors Michael Lipson and Travis Smith. &lt;br/&gt;The first tribunal&lt;br/&gt;The eight students presented evidence, personal statements and called forward witnesses at the tribunal last week. The university said respondents were able to request separate hearings.&lt;br/&gt;The Dec. 2 hearing lasted about eight hours, according to two respondents, and coincided with the final week of classes and final assignments. For students in third or fourth year, exams take place in the last weeks of classes and not during the exam period, says Katie Nelson, one of the eight students at the hearing.&lt;br/&gt;“It’s definitely affected my studies and probably the outcome of those classes, because I’ve either had to take time writing statements of evidence or meet with advocacy or go to the tribunal itself which is about seven or eight hours,” she said.&lt;br/&gt;At least two more tribunals are expected, one for each of the professors who filed formal complaints against students, but dates have yet to be announced.&lt;br/&gt;The university department responsible for tribunals avoids scheduling hearings during exam periods or vacation periods and tries to accommodate panelists, the chairperson, complaintants and respondents. This means the next tribunal will likely take place next semester. &lt;br/&gt;“I’m not sure why they thought it was appropriate to schedule such a long tribunal at such an inconvenient time,” Nelson said. “It definitely shows that the university has very little regard to the actual academic work coming out of students and really illustrates the political nature of the tribunal itself.”&lt;br/&gt;There was no testimony by an administrative representative at the Dec. 2 tribunal, according to Nelson. Mota previously told The Link that the university became a co-complainant to provide professors with information from campus security. Nelson said there was a representative from security at the tribunal.&lt;br/&gt;Even if the jury comes back and recommends the lowest charge, a letter of reprimand, Nelson fears her case might be sent to upper administration since this isn’t the first tribunal she’s faced, or the last. &lt;br/&gt;Following last year’s vote for Boycott Divest Sanction (BDS) of Israel by the Concordia Student Union, Nelson, who was campaigning pro-BDS, was accused of harassment and given a letter of reprimand for a different charge. &lt;br/&gt;Now she faces complaints by two professors, Graham Dodds and Michael Lipson, for disrupting classes while carrying out strike mandates to picket political science classes.&lt;br/&gt;Nelson says she is concerned that Lipson acted as an advocate for Dodds and was present at the tribunal.&lt;br/&gt;“He was privy to all the argumentation, all the personal testimony, all the witnesses presented in Dodds’s case, and now essentially has the upper hand,” she said.&lt;br/&gt;Professors Dodds and Smith declined to be interviewed, since the tribunal process is still ongoing. Lipson did not respond to a request for comment.&lt;br/&gt;Nelson called the tribunal process, a lack of communication and delays in scheduling “legally problematic” and “psychologically abusive,” and hopes the tribunals don’t move on.&lt;br/&gt;“The university should be preparing for the ramifications and consequences of doing that to its students,” she said, promising to look into civil litigation.&lt;br/&gt;Unsuccessful mediations&lt;br/&gt;Mediation, which was touted as a possible venue for resolution of the complaints, doesn’t seem to be a possibility for students and professors anymore.&lt;br/&gt;Concordia began a mediation process in the fall to encourage an informal compromise between professors and students. The first attempt began in early October, but seemingly ended without an agreement.&lt;br/&gt;All participants signed a nondisclosure agreement, which prevented them from speaking with media.&lt;br/&gt;One student has agreed to a mediated settlement, but the terms of the agreement are still unknown. Some other students have had their charges dropped because they were not directly involved in disrupting the classes of the complainants.&lt;br/&gt;About a month later, another round of mediation sessions were organized with new mediators—but the tribunal date had already been set.&lt;br/&gt;“That’s something I found problematic, to have the tribunal at the same time as the mediation—especially a few days before finals,” said Aloyse Muller, one of the students being charged.&lt;br/&gt;An administrative representative was noticeably lacking in all the meetings set up with the purpose of mediation over the semester.&lt;br/&gt;“I have to give it to Concordia, you know, a ‘real education for the real world,’” said Muller, citing the university’s old motto.&lt;br/&gt;“I’ve learned a lot about what’s the mediation process, what’s the problem of having a nine-hour discussion when you have to take caucuses all the time,” he said. “Real education, real helpful, probably better than some of my classes this term.”&lt;br/&gt;Correction: A previous version of this story stated Katie Nelson was charged with harassment. She was accused of harassment, but received a letter of reprimand for a different charge. The Link regrets the error.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;By commenting on this page you agree to the terms of our Comments Policy.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Please enable JavaScript to view the comments powered by Disqus.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Related Reading&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;First Tribunal for Student-Protesters Set for Dec. 2&lt;br/&gt;Jonathan Caragay-Cook&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Opinions&lt;br/&gt;Editorial: These Student-Protester Tribunals Are Just for Show&lt;br/&gt;The Link&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;Concordia Student-Protester Tribunals Suspended&lt;br/&gt;Jonathan Caragay-Cook&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Opinions&lt;br/&gt;Editorial: Make P-6 an Election Issue&lt;br/&gt;The Link</t>
         </is>
+      </c>
+      <c r="L191" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="192">
@@ -8761,10 +9341,13 @@
           <t>Economy/inequality</t>
         </is>
       </c>
-      <c r="J192" t="inlineStr">
+      <c r="K192" t="inlineStr">
         <is>
           <t>Students, Professors Wait for Decision After First Tribunal&lt;br/&gt;Eight Concordia Students Charged With Disruptions Call Process “Problematic”&lt;br/&gt;News by Michelle Pucci — Published December 12, 2015 | Updated December 13, 2015 | Comments&lt;br/&gt;Follow @michellempucci&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;The tribunal was for student-protesters who are accused of disrupting classes last semester.  File Photo Shaun Michaud&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Eight of the estimated 24 students accused of disrupting classes during last semester’s strikes are waiting for a decision from a tribunal last week, the latest installment in a process they call “problematic” and “abusive.”&lt;br/&gt;The original charges came after a ripple of anti-austerity protests and student strikes took place in Quebec CEGEPs and universities last spring. &lt;br/&gt;About a month after complaints were filed by professors before the summer break, Concordia agreed to join them as co-complainants. Concordia’s spokesperson Chris Mota said the university became a co-complainant in support of the professors and will support the outcome of the hearings.&lt;br/&gt;Despite hiring multiple mediators to settle the charges informally between students and professors, there are no plans for more efforts of mediation in the future.&lt;br/&gt;“Mediation is voluntary and can take place so long as all parties wish to participate,” spokesperson Chris Mota wrote in an email. “The fact that tribunals took place last week suggests that the mutual interest in continuing mediation was not present.”&lt;br/&gt;The remaining students charged will likely also be called to a tribunal. Students are calling on the university to drop the charges.&lt;br/&gt;“We feel that the university is also responsible in a major way for what happened,” said Aloyse Muller, one of the students involved in the Dec. 2 tribunal. “They’re trying to present themselves like a neutral player when they’re really not.”&lt;br/&gt;The current events stem from spring 2015 anti-austerity protest actions, when more than a dozen student associations and the faculty of fine arts student association voted to strike at least one day of classes last semester. Some associations voted to strike for several weeks.&lt;br/&gt;Concordia’s response was to cancel a day of classes for each department, whose students voted to strike or to participate in city-wide protest, either March 23 or April 2. &lt;br/&gt;On April 1, students enforcing the strike mandate entered a political science class with noise-making machines and chanted until most students walked out. An official complaint under article 29G of the Code of Rights and Responsibilities was filed by the course professor Graham Dodds. Some of the students also face complaints over other pickets from professors Michael Lipson and Travis Smith. &lt;br/&gt;The first tribunal&lt;br/&gt;The eight students presented evidence, personal statements and called forward witnesses at the tribunal last week. The university said respondents were able to request separate hearings.&lt;br/&gt;The Dec. 2 hearing lasted about eight hours, according to two respondents, and coincided with the final week of classes and final assignments. For students in third or fourth year, exams take place in the last weeks of classes and not during the exam period, says Katie Nelson, one of the eight students at the hearing.&lt;br/&gt;“It’s definitely affected my studies and probably the outcome of those classes, because I’ve either had to take time writing statements of evidence or meet with advocacy or go to the tribunal itself which is about seven or eight hours,” she said.&lt;br/&gt;At least two more tribunals are expected, one for each of the professors who filed formal complaints against students, but dates have yet to be announced.&lt;br/&gt;The university department responsible for tribunals avoids scheduling hearings during exam periods or vacation periods and tries to accommodate panelists, the chairperson, complaintants and respondents. This means the next tribunal will likely take place next semester. &lt;br/&gt;“I’m not sure why they thought it was appropriate to schedule such a long tribunal at such an inconvenient time,” Nelson said. “It definitely shows that the university has very little regard to the actual academic work coming out of students and really illustrates the political nature of the tribunal itself.”&lt;br/&gt;There was no testimony by an administrative representative at the Dec. 2 tribunal, according to Nelson. Mota previously told The Link that the university became a co-complainant to provide professors with information from campus security. Nelson said there was a representative from security at the tribunal.&lt;br/&gt;Even if the jury comes back and recommends the lowest charge, a letter of reprimand, Nelson fears her case might be sent to upper administration since this isn’t the first tribunal she’s faced, or the last. &lt;br/&gt;Following last year’s vote for Boycott Divest Sanction (BDS) of Israel by the Concordia Student Union, Nelson, who was campaigning pro-BDS, was accused of harassment and given a letter of reprimand for a different charge. &lt;br/&gt;Now she faces complaints by two professors, Graham Dodds and Michael Lipson, for disrupting classes while carrying out strike mandates to picket political science classes.&lt;br/&gt;Nelson says she is concerned that Lipson acted as an advocate for Dodds and was present at the tribunal.&lt;br/&gt;“He was privy to all the argumentation, all the personal testimony, all the witnesses presented in Dodds’s case, and now essentially has the upper hand,” she said.&lt;br/&gt;Professors Dodds and Smith declined to be interviewed, since the tribunal process is still ongoing. Lipson did not respond to a request for comment.&lt;br/&gt;Nelson called the tribunal process, a lack of communication and delays in scheduling “legally problematic” and “psychologically abusive,” and hopes the tribunals don’t move on.&lt;br/&gt;“The university should be preparing for the ramifications and consequences of doing that to its students,” she said, promising to look into civil litigation.&lt;br/&gt;Unsuccessful mediations&lt;br/&gt;Mediation, which was touted as a possible venue for resolution of the complaints, doesn’t seem to be a possibility for students and professors anymore.&lt;br/&gt;Concordia began a mediation process in the fall to encourage an informal compromise between professors and students. The first attempt began in early October, but seemingly ended without an agreement.&lt;br/&gt;All participants signed a nondisclosure agreement, which prevented them from speaking with media.&lt;br/&gt;One student has agreed to a mediated settlement, but the terms of the agreement are still unknown. Some other students have had their charges dropped because they were not directly involved in disrupting the classes of the complainants.&lt;br/&gt;About a month later, another round of mediation sessions were organized with new mediators—but the tribunal date had already been set.&lt;br/&gt;“That’s something I found problematic, to have the tribunal at the same time as the mediation—especially a few days before finals,” said Aloyse Muller, one of the students being charged.&lt;br/&gt;An administrative representative was noticeably lacking in all the meetings set up with the purpose of mediation over the semester.&lt;br/&gt;“I have to give it to Concordia, you know, a ‘real education for the real world,’” said Muller, citing the university’s old motto.&lt;br/&gt;“I’ve learned a lot about what’s the mediation process, what’s the problem of having a nine-hour discussion when you have to take caucuses all the time,” he said. “Real education, real helpful, probably better than some of my classes this term.”&lt;br/&gt;Correction: A previous version of this story stated Katie Nelson was charged with harassment. She was accused of harassment, but received a letter of reprimand for a different charge. The Link regrets the error.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;By commenting on this page you agree to the terms of our Comments Policy.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Please enable JavaScript to view the comments powered by Disqus.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Related Reading&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;First Tribunal for Student-Protesters Set for Dec. 2&lt;br/&gt;Jonathan Caragay-Cook&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Opinions&lt;br/&gt;Editorial: These Student-Protester Tribunals Are Just for Show&lt;br/&gt;The Link&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;Concordia Student-Protester Tribunals Suspended&lt;br/&gt;Jonathan Caragay-Cook&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Opinions&lt;br/&gt;Editorial: Make P-6 an Election Issue&lt;br/&gt;The Link</t>
         </is>
+      </c>
+      <c r="L192" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="193">
@@ -8804,10 +9387,13 @@
           <t>Police violence, Anti-racism</t>
         </is>
       </c>
-      <c r="J193" t="inlineStr">
+      <c r="K193" t="inlineStr">
         <is>
           <t>Tuesday was the 26th anniversary of the day 10,000 Chinese students gathered in Beijing's Tiananmen Square to mourn reform leader Hu Yaobang in the now-infamous Tiananmen Square protests and massacre.&lt;br/&gt;As many as 1.2 million people gathered over the course of the student-led movement before the Chinese government ordered a military crackdown against the peaceful protesters, which killed an unknown number of its participants and purged as many as 10,000 of their supporters afterward. Though the Tiananmen Square protests ended in tragedy, they are remembered today as a powerful moment when young people stood up for their beliefs against an iron system.&lt;br/&gt;Though half a world away, the 40 Acres has a similarly poignant history of student activism. The first University protest took place in 1897, and there have been dozens if not hundreds of student demonstrations since.&lt;br/&gt;According to John Woodrow Storey ad Mary L. Kelley's Twentieth-Century Texas: A Social and Cultural History, student activism was the catalyst for the University's full racial integration in 1965, and the fear of Vietnam War protesters rushing the Tower brought about the installation of the hedges and groves now decorating the West Mall in the late 1960s. Last December's "die-in" for Eric Garner, the black man killed by a white police officer in New York over the summer, was another example of the bold activist spirit ingrained in the culture of the student body.&lt;br/&gt;The recent debate between Unify Texas and UTDivest is the most recent incarnation of student activism on UT's campus. On April 7, the first debate about the BDS movement, or Boycott, Divestment and Sanctions, took place in the weekly Student Government meeting between student groups UTDivest and Unify Texas. Since then, our campus and this opinion page have been alight with powerful and well argued statements to the virtues of both causes.&lt;br/&gt;The vibrancy of character, passion of purpose and dedication to an issue whose complexity frightens most away from serious consideration was a powerful and inspiring experience for me as a student. During one of the most formative times in all of our lives, where we spend our days learning and becoming our truest selves in four years devoted to self-discovery, the BDS debate often left me wondering: What more could I do for this campus, for this world?&lt;br/&gt;For this reason and many others, I feel blessed that this movement happened on campus. It is imperative that more debates on campus happen, too. Though the issue was decided by Student Government Tuesday night against the resolution, I hope that an environment of open discourse is nurtured by this University. It is important for students to be able to speak freely about the issues that matter and be challenged so that we as a student body may grow stronger in our personal convictions, which only an environment of open discourse can ensure. So, to all of my fellow students who contributed to that, please let me say thank you.&lt;br/&gt;However, in future on-campus debates, I hope participants will exercise restraint and sensitivity, which I often felt was lacking over the last two weeks. Though I admired the debaters' passion, this cause engendered more hate between students than I felt comfortable witnessing. By the time SG voted, accusations of bigotry and virulent personal character attacks on student leaders in both movements became the name of the game. For shame.&lt;br/&gt;Inspiring others and fighting for justice is noble. What this debate devolved into over the last two weeks was not. This debate mattered. Protecting the integrity of it was sacred. Hurting someone else is not the same as helping yourself.&lt;br/&gt;Now that this debate is over, it would be too easy for one side or the other to become complacent with self-satisfaction at winning or rueful of their loss. Protect yourselves from such temptation.&lt;br/&gt;As student activists, we can capture the voice of campus. We can make change happen. We can inspire our fellow students.&lt;br/&gt;Or we can hurt them, ourselves and our cause. To all of the participants in the fight over BDS, many of whom I believe did not take part in the mudslinging of the baser parts of the last few weeks, I urge you to serve our campus by holding your peers accountable to their cause when some may bow to the temptation of fighting with anything other than reason.&lt;br/&gt;Conduct yourselves with the dignity your cause demands of you as its representatives. If the cost is to the students around us and a community of openness, nothing is worth it. Fight the good fight, Longhorns. Just be wary of the repercussions.&lt;br/&gt;Smith is a history and humanities junior from Austin. Follow Smith on Twitter @claireseysmith.</t>
         </is>
+      </c>
+      <c r="L193" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="194">
@@ -8852,10 +9438,13 @@
           <t>Anti-racism, Police violence</t>
         </is>
       </c>
-      <c r="J194" t="inlineStr">
+      <c r="K194" t="inlineStr">
         <is>
           <t>Oberlin students, faculty and staff came together this week to organize and execute a variety of protests, demonstrations and actions that highlighted what they identify as the College's complicity in the systemic oppression of people of color. While these protests were not the only actions that took place this week, they were among the more heavily-attended demonstrations.&lt;br/&gt;Students Challenge Board of Trustees&lt;br/&gt;Over 100 students occupied the Board of Trustees forum in Stevenson Dining Hall on Thursday, crowding along the walls and dispersing themselves throughout the space in order to ensure that their voices would be heard.&lt;br/&gt;"I look at the disdain in your faces, and I can see that you don't respect me or the people who look like me," one student said to the trustees, many of whom were white men.&lt;br/&gt;"Don't admit students into this college just to make this college look good," said another.&lt;br/&gt;"You limit access to students of color at this school," a third said. "You limit our access into your classrooms. Why is it that the only people I know who have ever heard of Oberlin are rich and white?"&lt;br/&gt;The action, which was organized by several students of color, called attention to what many have identified as Oberlin's institutional marginalization of low-income students and people of color.&lt;br/&gt;Many of the students who spoke at the forum demanded the Board take accountability for what they viewed to be the Board's apathetic approach, as well as for the racist microaggressions that some used in their responses.&lt;br/&gt;"Hands up," several students of color shouted when they heard language they identified as violent or oppressive. "Don't shoot," the rest of the demonstrators yelled back.&lt;br/&gt;According to College junior and action organizer Kiki Acey, the chant was a way for students to express the pain that comes from destructive and dehumanizing language.&lt;br/&gt;"If they kick us, we will say ouch," said Acey.&lt;br/&gt;Other students used the forum to address specific concerns and demands. College junior Amethyst Carey asked the Board why the Multicultural Visit Program had been expanded to give even more access to white students, while College junior Lisa-Qiao MacDonald demanded that the trustees take part in anti-racist and anti- oppression trainings - a comment that garnered much support from the protesters.&lt;br/&gt;While these remarks elicited responses from several trustees, many other comments went unaddressed.&lt;br/&gt;"These issues are central to our conversations," said Board Co-chair Diane Yu, OC '73.&lt;br/&gt;Other board members agreed and stressed that their goal was to serve students.&lt;br/&gt;"We want to [allocate resources] where they can best be used," said trustee Alan Wurtzel, OC '55.&lt;br/&gt;Wurtzel went on to say that the Board was between a fiscal rock and a hard place when it came to earning revenue, as the College has very few income channels and cannot afford to vastly reallocate its assets.&lt;br/&gt;Peters Protest Denounces Respectability Politics&lt;br/&gt;While the Board of Trustees enjoyed pre-dinner drinks in the lobby of Peters Hall earlier that evening, a group of protesters were congregating upstairs.&lt;br/&gt;"Ferguson is all around us. We need to pop the bubble that insulates us from the rest of the world. We do not get to compartmentalize these issues," said Bautista.&lt;br/&gt;When the time came for the students to interrupt the dinner, they split into two groups. The white students descended the staircase first, filling the lobby with shouts and other loud vocal noises that called attention to the demonstrators. They were soon followed by students of color, who silently dispersed themselves throughout the lobby.&lt;br/&gt;According to Bautista, the demonstration was purposefully chaotic and inconvenient and was purposefully de- signed to have white students enter the lobby first.&lt;br/&gt;"We need to reverse the racial paradigm that is associated with activism," Bautista said. "Not just on campus, but nationally. It's a paradigm that allows people to be apathetic and police other students. This policing has been mostly coming from white students on this campus unfortunately, and when you see a cohort of people who look just like you, it's a little bit harder for you to criminalize them and demean them and invalidate everything they're saying because they are you."&lt;br/&gt;While the rest of the students descended into the lobby, Bautista remained on the stairwell to request the crowd take four and a half minutes honoring the memory of Michael Brown, an unarmed black teenager who was shot by white police officer Darren Wilson in Ferguson, MO, this summer.&lt;br/&gt;In demonstrations across the country, the four and a half minutes of silence was specifically chosen to represent the four and a half hours that Brown's body was left lying in the street.&lt;br/&gt;During the silence, trustees craned their necks to see the demonstrators, some of whom were holding posters of other black and brown Americans who have been murdered by white police officers. Others were holding posters of the 43 Mexican students that disappeared in southern Mexico this September.&lt;br/&gt;Other students passed out a list of demands to the trustees, which were a direct reproduction of the demands that were presented at the Board of Trustees meeting in October of 2013.&lt;br/&gt;The demands called for increased institutional transparency, divestment from companies that profit from Israel's occupation of Palestine, creation of a scholarship program for undocumented students, a ban on fracking on College-owned property and the official formation of an Asian-American studies minor.&lt;br/&gt;"We were highlighting the fact that there has been complicity and inaction [ from the trustees] despite student pro- test," Bautista said. "How will trustees wield their privilege moving forward?"&lt;br/&gt;Though the trustees and other dinner attendees were largely silent during the demonstration, Dean of Students Eric Estes said the protest had an important message.&lt;br/&gt;"I think they thought it was incredibly powerful," Estes said. "I was just talking to a trustee who actually occupied this building during the Vietnam War protests. We were having a fascinating conversation... I love and respect our students very much."&lt;br/&gt;Protesters Unite in Oberlin, Cleveland&lt;br/&gt;Nearly 200 students participated in the national Hands Up, Walk Out day of solidarity on Monday, shouting chants of "Hands up, don't shoot" and "No justice, no peace" as they marched through the campus and into town.&lt;br/&gt;Protesting against the systemic marginalization, brutalization and dehumanization of black and brown Americans and denouncing police brutality and other forms of racialized violence, the demonstrators called out Oberlin's administration for its inaction.&lt;br/&gt;The protest formally started at 1 p.m., when dozens of students walked out of their classrooms and convened in front of the Cox Administration Building. After staging a four-and-a-half minute "die-in" - in which protesters lay on the ground - they advanced toward the King Building, where they weaved in and out of classrooms in an attempt to engage their peers in the action. From there, students marched into the Science Center, through Wilder Bowl and into Bibbins Hall, where several teachers were holding music theory classes.&lt;br/&gt;While some professors allowed students to join the protest or cancelled class, others chose instead to ignore it. Many of the students, however, chose to ignore their professors, and by the time the crowd surged out of the Conservatory, it was over 100 strong.&lt;br/&gt;"No justice, no peace, no racist police," the students shouted as they headed toward the Oberlin Police Station, where they aimed to hold officers in Oberlin and nationwide accountable for police brutality enacted against black and brown Americans.&lt;br/&gt;After protesting outside the police station, students moved toward Oberlin High School, where they proceeded to inform those exiting the building of how to get transportation to several protests in Cleveland.&lt;br/&gt;Demonstrators then returned to Cox to reconvene and discuss productive ways to move forward. By the time the crowd dispersed, students had formed groups that focused on media saturation, artistic expression, direct action, decompression and community and church engagement.&lt;br/&gt;The Hands Up, Walk Out demonstration was part of many that were organized in response to the recent events in Ferguson. Many communities have been protesting police violence since the shooting, strengthening their efforts when Missouri's grand jury announced last month that the officer who killed Mike Brown would not be indicted.&lt;br/&gt;A number of Oberlin students have participated in several of these demonstrations, including one that took place last week in Cleveland. The protest, which was organized by Cleveland anti-mass-incarceration group Puncture the Silence, saw nearly 100 Oberlin students stand in solidarity with Cleveland residents who condemned the grand jury's decision not to indict Wilson, as well as the recent murder of black 12-year-old Tamir Rice by a white Cleveland police officer.&lt;br/&gt;One of the other highly attended actions on campus was Wednesday's Faculty and Student Teach-In on Ferguson, during which approximately 300 students gathered in King to hear individuals speak on the historical context of police brutality and systemic oppressions of people of color, as well as the ways that students can prioritize activism. The Multicultural Resource Center as well as the Comparative American Studies, Africana Studies and History departments organized the event.&lt;br/&gt;According to College President Marvin Krislov, these initiatives will be taken into consideration as the administration moves forward with its action. In his weekly Source column published on Wednesday, he announced the formation of a working group designed to determine the "best principles and practices for ensuring campus safety in an inclusive and equitable fashion."&lt;br/&gt;In an interview with the Review, he highlighted the importance of community.&lt;br/&gt;"We recognize that these events are very concerning and upsetting to a lot of people, and we want to be there as a community to support students and others - faculty and staff - who want to talk about this, and I hope that we can figure out educational ways in which we can think about these issues together."</t>
         </is>
+      </c>
+      <c r="L194" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="195">
@@ -8902,10 +9491,13 @@
           <t>University governance, admin, policies, programs, curriculum, Campus climate, Police violence</t>
         </is>
       </c>
-      <c r="J195" t="inlineStr">
+      <c r="K195" t="inlineStr">
         <is>
           <t>Oberlin students, faculty and staff came together this week to organize and execute a variety of protests, demonstrations and actions that highlighted what they identify as the College's complicity in the systemic oppression of people of color. While these protests were not the only actions that took place this week, they were among the more heavily-attended demonstrations.&lt;br/&gt;Students Challenge Board of Trustees&lt;br/&gt;Over 100 students occupied the Board of Trustees forum in Stevenson Dining Hall on Thursday, crowding along the walls and dispersing themselves throughout the space in order to ensure that their voices would be heard.&lt;br/&gt;"I look at the disdain in your faces, and I can see that you don't respect me or the people who look like me," one student said to the trustees, many of whom were white men.&lt;br/&gt;"Don't admit students into this college just to make this college look good," said another.&lt;br/&gt;"You limit access to students of color at this school," a third said. "You limit our access into your classrooms. Why is it that the only people I know who have ever heard of Oberlin are rich and white?"&lt;br/&gt;The action, which was organized by several students of color, called attention to what many have identified as Oberlin's institutional marginalization of low-income students and people of color.&lt;br/&gt;Many of the students who spoke at the forum demanded the Board take accountability for what they viewed to be the Board's apathetic approach, as well as for the racist microaggressions that some used in their responses.&lt;br/&gt;"Hands up," several students of color shouted when they heard language they identified as violent or oppressive. "Don't shoot," the rest of the demonstrators yelled back.&lt;br/&gt;According to College junior and action organizer Kiki Acey, the chant was a way for students to express the pain that comes from destructive and dehumanizing language.&lt;br/&gt;"If they kick us, we will say ouch," said Acey.&lt;br/&gt;Other students used the forum to address specific concerns and demands. College junior Amethyst Carey asked the Board why the Multicultural Visit Program had been expanded to give even more access to white students, while College junior Lisa-Qiao MacDonald demanded that the trustees take part in anti-racist and anti- oppression trainings - a comment that garnered much support from the protesters.&lt;br/&gt;While these remarks elicited responses from several trustees, many other comments went unaddressed.&lt;br/&gt;"These issues are central to our conversations," said Board Co-chair Diane Yu, OC '73.&lt;br/&gt;Other board members agreed and stressed that their goal was to serve students.&lt;br/&gt;"We want to [allocate resources] where they can best be used," said trustee Alan Wurtzel, OC '55.&lt;br/&gt;Wurtzel went on to say that the Board was between a fiscal rock and a hard place when it came to earning revenue, as the College has very few income channels and cannot afford to vastly reallocate its assets.&lt;br/&gt;Peters Protest Denounces Respectability Politics&lt;br/&gt;While the Board of Trustees enjoyed pre-dinner drinks in the lobby of Peters Hall earlier that evening, a group of protesters were congregating upstairs.&lt;br/&gt;"Ferguson is all around us. We need to pop the bubble that insulates us from the rest of the world. We do not get to compartmentalize these issues," said Bautista.&lt;br/&gt;When the time came for the students to interrupt the dinner, they split into two groups. The white students descended the staircase first, filling the lobby with shouts and other loud vocal noises that called attention to the demonstrators. They were soon followed by students of color, who silently dispersed themselves throughout the lobby.&lt;br/&gt;According to Bautista, the demonstration was purposefully chaotic and inconvenient and was purposefully de- signed to have white students enter the lobby first.&lt;br/&gt;"We need to reverse the racial paradigm that is associated with activism," Bautista said. "Not just on campus, but nationally. It's a paradigm that allows people to be apathetic and police other students. This policing has been mostly coming from white students on this campus unfortunately, and when you see a cohort of people who look just like you, it's a little bit harder for you to criminalize them and demean them and invalidate everything they're saying because they are you."&lt;br/&gt;While the rest of the students descended into the lobby, Bautista remained on the stairwell to request the crowd take four and a half minutes honoring the memory of Michael Brown, an unarmed black teenager who was shot by white police officer Darren Wilson in Ferguson, MO, this summer.&lt;br/&gt;In demonstrations across the country, the four and a half minutes of silence was specifically chosen to represent the four and a half hours that Brown's body was left lying in the street.&lt;br/&gt;During the silence, trustees craned their necks to see the demonstrators, some of whom were holding posters of other black and brown Americans who have been murdered by white police officers. Others were holding posters of the 43 Mexican students that disappeared in southern Mexico this September.&lt;br/&gt;Other students passed out a list of demands to the trustees, which were a direct reproduction of the demands that were presented at the Board of Trustees meeting in October of 2013.&lt;br/&gt;The demands called for increased institutional transparency, divestment from companies that profit from Israel's occupation of Palestine, creation of a scholarship program for undocumented students, a ban on fracking on College-owned property and the official formation of an Asian-American studies minor.&lt;br/&gt;"We were highlighting the fact that there has been complicity and inaction [ from the trustees] despite student pro- test," Bautista said. "How will trustees wield their privilege moving forward?"&lt;br/&gt;Though the trustees and other dinner attendees were largely silent during the demonstration, Dean of Students Eric Estes said the protest had an important message.&lt;br/&gt;"I think they thought it was incredibly powerful," Estes said. "I was just talking to a trustee who actually occupied this building during the Vietnam War protests. We were having a fascinating conversation... I love and respect our students very much."&lt;br/&gt;Protesters Unite in Oberlin, Cleveland&lt;br/&gt;Nearly 200 students participated in the national Hands Up, Walk Out day of solidarity on Monday, shouting chants of "Hands up, don't shoot" and "No justice, no peace" as they marched through the campus and into town.&lt;br/&gt;Protesting against the systemic marginalization, brutalization and dehumanization of black and brown Americans and denouncing police brutality and other forms of racialized violence, the demonstrators called out Oberlin's administration for its inaction.&lt;br/&gt;The protest formally started at 1 p.m., when dozens of students walked out of their classrooms and convened in front of the Cox Administration Building. After staging a four-and-a-half minute "die-in" - in which protesters lay on the ground - they advanced toward the King Building, where they weaved in and out of classrooms in an attempt to engage their peers in the action. From there, students marched into the Science Center, through Wilder Bowl and into Bibbins Hall, where several teachers were holding music theory classes.&lt;br/&gt;While some professors allowed students to join the protest or cancelled class, others chose instead to ignore it. Many of the students, however, chose to ignore their professors, and by the time the crowd surged out of the Conservatory, it was over 100 strong.&lt;br/&gt;"No justice, no peace, no racist police," the students shouted as they headed toward the Oberlin Police Station, where they aimed to hold officers in Oberlin and nationwide accountable for police brutality enacted against black and brown Americans.&lt;br/&gt;After protesting outside the police station, students moved toward Oberlin High School, where they proceeded to inform those exiting the building of how to get transportation to several protests in Cleveland.&lt;br/&gt;Demonstrators then returned to Cox to reconvene and discuss productive ways to move forward. By the time the crowd dispersed, students had formed groups that focused on media saturation, artistic expression, direct action, decompression and community and church engagement.&lt;br/&gt;The Hands Up, Walk Out demonstration was part of many that were organized in response to the recent events in Ferguson. Many communities have been protesting police violence since the shooting, strengthening their efforts when Missouri's grand jury announced last month that the officer who killed Mike Brown would not be indicted.&lt;br/&gt;A number of Oberlin students have participated in several of these demonstrations, including one that took place last week in Cleveland. The protest, which was organized by Cleveland anti-mass-incarceration group Puncture the Silence, saw nearly 100 Oberlin students stand in solidarity with Cleveland residents who condemned the grand jury's decision not to indict Wilson, as well as the recent murder of black 12-year-old Tamir Rice by a white Cleveland police officer.&lt;br/&gt;One of the other highly attended actions on campus was Wednesday's Faculty and Student Teach-In on Ferguson, during which approximately 300 students gathered in King to hear individuals speak on the historical context of police brutality and systemic oppressions of people of color, as well as the ways that students can prioritize activism. The Multicultural Resource Center as well as the Comparative American Studies, Africana Studies and History departments organized the event.&lt;br/&gt;According to College President Marvin Krislov, these initiatives will be taken into consideration as the administration moves forward with its action. In his weekly Source column published on Wednesday, he announced the formation of a working group designed to determine the "best principles and practices for ensuring campus safety in an inclusive and equitable fashion."&lt;br/&gt;In an interview with the Review, he highlighted the importance of community.&lt;br/&gt;"We recognize that these events are very concerning and upsetting to a lot of people, and we want to be there as a community to support students and others - faculty and staff - who want to talk about this, and I hope that we can figure out educational ways in which we can think about these issues together."</t>
         </is>
+      </c>
+      <c r="L195" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -8950,10 +9542,13 @@
           <t>Indigenous issues</t>
         </is>
       </c>
-      <c r="J196" t="inlineStr">
+      <c r="K196" t="inlineStr">
         <is>
           <t>Stephen Huber | Student Life&lt;br/&gt;Students march up Brookings Steps on Tuesday to initiate a sit-in encouraging Washington University to cut ties with Peabody Energy. Around 100 students attended a rally Wednesday afternoon to hear statements from alumni and individuals from communities where Peabody has opened mines.&lt;br/&gt;About half of those students stayed overnight, under the stars or in tents pitched in the Brookings Archway, in the first campus sit-in since 2005, when students planted themselves in South Brookings Hall for 18 days to secure higher wages for the University's contract workers.&lt;br/&gt;Now, students are pressuring the University to end its relationship with Peabody Energy, the world's largest private coal company, which participants insist is an "evil" organization actively destroying not only indigenous communities but also the environment. But years of campus protests against "clean coal" have yielded virtually no results, and the administration has given no indication that this time will be different.&lt;br/&gt;The University receives significant funding from the company for research and scholarships. In 2008, Peabody gave the University $5 million to help it create a Consortium for Clean Coal Utilization; as recently as Tuesday, the school announced that it had received a $3.4 million grant, partially funded by Peabody Energy, to find ways to make coal plants meet the carbon emission standards recently proposed by the Environmental Protection Agency. Greg Boyce, the company's CEO, was named to the University's board of trustees.&lt;br/&gt;Peabody Energy has come under fire from environmental advocacy groups in recent months for attempting to expand its mining facilities in Rocky Branch, Ill. Locals argue that the company is trying to force them out of their homes while also endangering their town by disregarding environmental regulations and working without permits.&lt;br/&gt;In an op-ed in Student Life last week, four students also blasted the company for forcing the relocation of the Navajo and Hopi tribes with its mines in Arizona's Black Mesa Plateau and supporting the American Legislative Exchange Council a conservative nonprofit group that advocates for Stand Your Ground laws.&lt;br/&gt;Many involved in the sit-in say they are willing to stay for weeks if necessary to achieve productive dialogue. Their "ask" or official goal is to cut ties with Peabody and have Boyce removed from the board of trustees, but participants said they are willing to consider other resolutions involving a University statement saying it does not support Peabody.&lt;br/&gt;The sit-in, which has been in the works for about a month, began at 6 p.m. Tuesday, with a crowd of about 50 undergraduates, alumni, students from other local universities and members of various environmental groups holding signs and rallying as organizers spoke by megaphone.&lt;br/&gt;"This University is supposed to stand for health and for justice," junior Nancy Yang said at a rally on the Brookings steps Wednesday afternoon. "It's teaching students about medicine and about how to cure people, but Peabody is a company that is doing a lot of things directly against that."&lt;br/&gt;Wednesday's rally brought nearly 100 people to the Brookings steps to hear students and community members offer remarks and read statements from alumni and individuals from communities where Peabody has opened mines.&lt;br/&gt;"I find it a little bit hypocritical that, as we're expanding the No. 1 social work school in the country and as we're building a new building for our master's in public health, that we are inextricably linked to a huge corporation that's perpetuating these problems, marginalizing communities and making people sick," senior Megan Odenthal said at the rally.&lt;br/&gt;Students participating in the sit-in have made a point to remain amicable and work with the Washington University Police Department to avoid arrest or referral to the Office of Student Conduct. They went as far as pitching their tents under the Brookings Arch, agreeing to sleep on concrete rather than the grass to avoid being charged for landscaping damage.&lt;br/&gt;The students have designated individuals to act as liaisons to the media, people who pass by and administrators walking through. Director of the First Year Center and Associate Vice Chancellor Rob Wild and Judicial Administrator Tamara King stopped by Tuesday night, and even the chancellor said he walked by on Wednesday morning, though no one noticed.&lt;br/&gt;"I went on my normal walk this morning; I guess I left my residence at about 5:30," Chancellor Mark Wrighton said. "I typically take a walk around campus including the Quadrangle; I saw the students, and they were all sleeping. I didn't disturb them and my dog didn't bark at them."&lt;br/&gt;The sit-in follows a meeting between Green Action members and Wrighton on Monday, where students discussed a Student Union resolution passed on March 19 to divest from fossil fuel companies by 2025. The resolution passed 14-2.&lt;br/&gt;At the meeting, the chancellor acknowledged their concerns but personally disagreed with their argument that the school needs to abandon coal, according to multiple individuals present. He also said that he would forward their concerns to the board of trustees at the May 1 meeting.&lt;br/&gt;"I think the students are addressing a very important concern," Wrighton said. "We're talking...about a very long-term challenge."&lt;br/&gt;He said that, while the University receives most of its research funding from the federal government, the school's involvement with companies like Peabody also helps it fund important research.&lt;br/&gt;"Corporate partners...have valuable contributions to make, and we value those partnerships," Wrighton said. "We need to prepare our students to be leaders in society, and that's a broad statement, but students who are engineers, for example...might go to work for a petroleum company. My view is we need to be able to be in a position to provide the infrastructure and support that is most helpful in fulfilling the potential of our students and faculty."&lt;br/&gt;But students disagree that the school's relationship with coal companies is aligned with the school's mission to "enhance the lives and livelihoods of students, the people of the greater St. Louis community, the country, and the world."&lt;br/&gt;"If we're not putting our actions and investments in line with our mission statement, we're ultimately not living up to our mission statement as a university," senior Rachel Goldstein, former president of Green Action, said.&lt;br/&gt;Participants hope to maintain a presence of about 15 students throughout the day under the Brookings Arch to hold the space, and they will be making decisions by consensus. They are hoping to meet with the chancellor later this week to discuss what they hope to achieve.&lt;br/&gt;Peabody Energy would not comment directly on the sit-in, but a spokesperson for the company told Student Life in a statement that "Peabody is proud to support Washington University in St. Louis and its leadership in education, as well as in clean coal research."</t>
         </is>
+      </c>
+      <c r="L196" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -8998,10 +9593,13 @@
           <t>Indigenous issues</t>
         </is>
       </c>
-      <c r="J197" t="inlineStr">
+      <c r="K197" t="inlineStr">
         <is>
           <t>Stephen Huber | Student Life&lt;br/&gt;Students march up Brookings Steps on Tuesday to initiate a sit-in encouraging Washington University to cut ties with Peabody Energy. Around 100 students attended a rally Wednesday afternoon to hear statements from alumni and individuals from communities where Peabody has opened mines.&lt;br/&gt;About half of those students stayed overnight, under the stars or in tents pitched in the Brookings Archway, in the first campus sit-in since 2005, when students planted themselves in South Brookings Hall for 18 days to secure higher wages for the University's contract workers.&lt;br/&gt;Now, students are pressuring the University to end its relationship with Peabody Energy, the world's largest private coal company, which participants insist is an "evil" organization actively destroying not only indigenous communities but also the environment. But years of campus protests against "clean coal" have yielded virtually no results, and the administration has given no indication that this time will be different.&lt;br/&gt;The University receives significant funding from the company for research and scholarships. In 2008, Peabody gave the University $5 million to help it create a Consortium for Clean Coal Utilization; as recently as Tuesday, the school announced that it had received a $3.4 million grant, partially funded by Peabody Energy, to find ways to make coal plants meet the carbon emission standards recently proposed by the Environmental Protection Agency. Greg Boyce, the company's CEO, was named to the University's board of trustees.&lt;br/&gt;Peabody Energy has come under fire from environmental advocacy groups in recent months for attempting to expand its mining facilities in Rocky Branch, Ill. Locals argue that the company is trying to force them out of their homes while also endangering their town by disregarding environmental regulations and working without permits.&lt;br/&gt;In an op-ed in Student Life last week, four students also blasted the company for forcing the relocation of the Navajo and Hopi tribes with its mines in Arizona's Black Mesa Plateau and supporting the American Legislative Exchange Council a conservative nonprofit group that advocates for Stand Your Ground laws.&lt;br/&gt;Many involved in the sit-in say they are willing to stay for weeks if necessary to achieve productive dialogue. Their "ask" or official goal is to cut ties with Peabody and have Boyce removed from the board of trustees, but participants said they are willing to consider other resolutions involving a University statement saying it does not support Peabody.&lt;br/&gt;The sit-in, which has been in the works for about a month, began at 6 p.m. Tuesday, with a crowd of about 50 undergraduates, alumni, students from other local universities and members of various environmental groups holding signs and rallying as organizers spoke by megaphone.&lt;br/&gt;"This University is supposed to stand for health and for justice," junior Nancy Yang said at a rally on the Brookings steps Wednesday afternoon. "It's teaching students about medicine and about how to cure people, but Peabody is a company that is doing a lot of things directly against that."&lt;br/&gt;Wednesday's rally brought nearly 100 people to the Brookings steps to hear students and community members offer remarks and read statements from alumni and individuals from communities where Peabody has opened mines.&lt;br/&gt;"I find it a little bit hypocritical that, as we're expanding the No. 1 social work school in the country and as we're building a new building for our master's in public health, that we are inextricably linked to a huge corporation that's perpetuating these problems, marginalizing communities and making people sick," senior Megan Odenthal said at the rally.&lt;br/&gt;Students participating in the sit-in have made a point to remain amicable and work with the Washington University Police Department to avoid arrest or referral to the Office of Student Conduct. They went as far as pitching their tents under the Brookings Arch, agreeing to sleep on concrete rather than the grass to avoid being charged for landscaping damage.&lt;br/&gt;The students have designated individuals to act as liaisons to the media, people who pass by and administrators walking through. Director of the First Year Center and Associate Vice Chancellor Rob Wild and Judicial Administrator Tamara King stopped by Tuesday night, and even the chancellor said he walked by on Wednesday morning, though no one noticed.&lt;br/&gt;"I went on my normal walk this morning; I guess I left my residence at about 5:30," Chancellor Mark Wrighton said. "I typically take a walk around campus including the Quadrangle; I saw the students, and they were all sleeping. I didn't disturb them and my dog didn't bark at them."&lt;br/&gt;The sit-in follows a meeting between Green Action members and Wrighton on Monday, where students discussed a Student Union resolution passed on March 19 to divest from fossil fuel companies by 2025. The resolution passed 14-2.&lt;br/&gt;At the meeting, the chancellor acknowledged their concerns but personally disagreed with their argument that the school needs to abandon coal, according to multiple individuals present. He also said that he would forward their concerns to the board of trustees at the May 1 meeting.&lt;br/&gt;"I think the students are addressing a very important concern," Wrighton said. "We're talking...about a very long-term challenge."&lt;br/&gt;He said that, while the University receives most of its research funding from the federal government, the school's involvement with companies like Peabody also helps it fund important research.&lt;br/&gt;"Corporate partners...have valuable contributions to make, and we value those partnerships," Wrighton said. "We need to prepare our students to be leaders in society, and that's a broad statement, but students who are engineers, for example...might go to work for a petroleum company. My view is we need to be able to be in a position to provide the infrastructure and support that is most helpful in fulfilling the potential of our students and faculty."&lt;br/&gt;But students disagree that the school's relationship with coal companies is aligned with the school's mission to "enhance the lives and livelihoods of students, the people of the greater St. Louis community, the country, and the world."&lt;br/&gt;"If we're not putting our actions and investments in line with our mission statement, we're ultimately not living up to our mission statement as a university," senior Rachel Goldstein, former president of Green Action, said.&lt;br/&gt;Participants hope to maintain a presence of about 15 students throughout the day under the Brookings Arch to hold the space, and they will be making decisions by consensus. They are hoping to meet with the chancellor later this week to discuss what they hope to achieve.&lt;br/&gt;Peabody Energy would not comment directly on the sit-in, but a spokesperson for the company told Student Life in a statement that "Peabody is proud to support Washington University in St. Louis and its leadership in education, as well as in clean coal research."</t>
         </is>
+      </c>
+      <c r="L197" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="198">
@@ -9046,10 +9644,13 @@
           <t>Indigenous issues</t>
         </is>
       </c>
-      <c r="J198" t="inlineStr">
+      <c r="K198" t="inlineStr">
         <is>
           <t>As part of Global Divestment Day, Fossil Free WashU sent a letter to Chancellor Mark Wrighton on Feb. 13 encouraging him to divest Washington University's endowment from fossil fuel companies.&lt;br/&gt;Then-senior James Cooper informs students about Peabody Energy's Rocky Branch mine using local lands to expand its facilities in Illinois. Students staged a sit-in for more than two weeks last April to protest the University's involvement with Peabody.&lt;br/&gt;Fossil Free WashU , an organization that aims to have Washington University divest its endowment from fossil fuel companies, is currently using Facebook to spread its open letter amongst the student population. The group wants the University to freeze the amount invested right now and eventually remove any money from the top 200 fossil fuel companies.&lt;br/&gt;In 2013, a survey collected data revealing that out of 1,000 students, only 6 percent would be against divestment, and in the same year, a petition for divestment gained 700 signatures. Additionally, in 2014, Student Union passed a resolution that supported divestment and outlined the processes by which the University could do so.&lt;br/&gt;The group's letter cited a study by the Aperio Investment group, which claimed that the differences in portfolios that are and aren't still invested in fossil fuels is extremely minimal, and the risk resulting from divestment is about a 0.005-percent increase. The University does not make the investment of its endowment public, but according to projections from FFWU based on comparable data from similar institutions, 3 to 5 percent of the endowment is invested in fossil fuel companies.&lt;br/&gt;"It has become clear to us as students that we cannot stand idly by while our educational institution supports companies that degrade the environment, abuse human rights, and worsen public health through its investments," FFWU wrote in its letter to Wrighton.&lt;br/&gt;Students march up Brookings Steps last April to initiate a sit-in encouraging Washington University to cut ties with Peabody Energy. The series of protest events concluded with the arrests of seven students trying to deliver a letter encouraging Peabody CEO Greg Boyce to resign from the University's board of trustees.&lt;br/&gt;The letter continues, "Wash U and other universities have a unique opportunity to stand up as responsible world leaders and motivate large-scale action for a sustainable future. This issue is only going to grow in importance."&lt;br/&gt;President of FFWU and sophomore Chloe Ames wants Wrighton and the University to consider the school's scholarly basis in making this decision.&lt;br/&gt;"By divesting in fossil fuels, that shows that not only does Wash. U. support the scientific facts that have been found and the research on fossil fuels that they have been very negative toward the environment and the greater world," Ames said. "That's definitely a step forward for the University, improving its dedication to both its students, people and just science in general as a research community."&lt;br/&gt;According to sophomore Nate Thomas, FFWU's treasurer, divestment would not affect the amount of money received by major donors such as Peabody Energy and Arch Coal.&lt;br/&gt;"If they were to stop donating and take away their support for the school, they would also lose a lot because they get a lot of this relationship, too," Thomas said. "That's not something they would likely jeopardize. Even if the University took its relatively small amount of investments in fossil fuels out, it's pretty unlikely they might be offended, might be unhappy, but the thought of them pulling out their support for our school is not really on the table."&lt;br/&gt;Although the letter has not been acknowledged publicly by the chancellor, FFWU hopes that the University considers the benefits of divesting.&lt;br/&gt;"We think divestment in fossil fuels is very important for combating climate change, and what we really think that Wash. U. could do by divesting is take a stand," Thomas said. "It would really send a strong message, and that's the main benefit of it and that's what we would like to see. We would like obviously all fossil fuels to be divested."&lt;br/&gt;Freshman Keaton Schifer, however, does not believe the University should have to listen to the requests of FFWU.&lt;br/&gt;"My general opinion is that [Washington University] is a private institution; they can really invest in whatever company they see fit that would benefit them and their interests," Schifer said. "And if that is a fossil fuels company, then that would be the right choice for them."&lt;br/&gt;Schifer added, "I've never had a problem before in supporting the oil and coal industry, so I do not have an issue with it."</t>
         </is>
+      </c>
+      <c r="L198" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -9089,10 +9690,13 @@
           <t>University governance, admin, policies, programs, curriculum, Labor and work</t>
         </is>
       </c>
-      <c r="J199" t="inlineStr">
+      <c r="K199" t="inlineStr">
         <is>
           <t>Dear Peter Dolan, Chairman, and the Board of Trustees of Tufts University,&lt;br/&gt;As you may have heard, around the time of your meeting this past Saturday morning, around 80 students gathered to show their support for fossil fuel divestment. This diverse coalition of students rallied from the Campus Center up to the pillars of Ballou Hall as speakers reiterated the moral imperative of divestment, reminding us that our investments in fossil fuels are a vote of support for industries that fuel injustice around the world. The week leading up to the rally, hundreds of students wrote what they stand to lose as a result of climate change on slips of paper. We linked these slips into a chain that we crossed over the doors of Ballou Hall. We demand that you strengthen and protect this chain, not break it.&lt;br/&gt;At Tufts, fossil fuel divestment has been endorsed by the student body through thousands of petition signatures and a public referendum, hundreds of alumni and 45 faculty members so far. When you had the opportunity to make Tufts a leader on this issue, you chose not to, instead rejecting divestment. We cannot, and will not, accept no for an answer. You told the Tufts community that divestment would not be considered at this time, but this issue cannot wait any longer. Now is the time.&lt;br/&gt;With the crushing significance of this international movement in mind, we demand that the Board take the following actions, and see no reason why you would fail to do so.&lt;br/&gt;Tufts should take this opportunity to create an investment strategy that better reflects its values. Our mission statement reads: "Tufts is a student-centered research university dedicated to the creation and application of knowledge. We are committed to providing transformational experiences for students and faculty in an inclusive and collaborative environment where creative scholars generate bold ideas, innovate in the face of complex challenges and distinguish themselves as active citizens of the world." Divestment is a bold idea that tackles the complex challenge of climate change. Tufts Climate Action wants to use the collaborative environment of our university to work with you, the Board of Trustees, to distinguish ourselves as active citizens of the world by taking a stand against fossil fuel industries.&lt;br/&gt;With love,&lt;br/&gt;Tufts Climate Action</t>
         </is>
+      </c>
+      <c r="L199" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="200">
@@ -9132,10 +9736,13 @@
           <t>Environmental</t>
         </is>
       </c>
-      <c r="J200" t="inlineStr">
+      <c r="K200" t="inlineStr">
         <is>
           <t>Photo Credit: Jennifer Lam&lt;br/&gt;A group of protestors gathered in front of the Creese Student Center at 9 a.m. Dec. 5 to object to the conference event "Philadelphia: The Next Great Energy Hub," hosted in part by Drexel University.&lt;br/&gt;The Greater Philadelphia Chamber of Commerce's CEO Council for Growth, "comprised of executives from the region's biggest corporations in the energy, chemical, and infrastructure sectors" staffs and supports the Greater Philadelphia's Energy Action Team, which hosted the protested conference. Companies which were involved in the committee to host the conference included Braskem America, the Dow Chemical Co., Exelon Corp., Monroe Energy, Philadelphia Energy Solutions, the Public Service Electric and Gas Co., Sunoco Logistics, UGI Corp. and many others.&lt;br/&gt;The conference invited natural gas investors, as well as leaders in chemical and financial groups involved with natural gas energy resources, to hear speakers about the expansion of natural gas production and usage in greater Philadelphia. The speakers for the panel discussion on the usage of the Marcellus formation were Jason Bordoff, founding director of the Center on Global Energy Policy at Columbia University, George Stark, director of external affairs at Cabot Oil &amp; Gas, and John Walsh, president and CEO of UGI Corp.&lt;br/&gt;The Facebook group organizing the Drexel student protestors states that the conference promotes activities which would "exacerbate groundwater pollution already being seen in Pennsylvania as a result of hydrofracking for natural gas ... increase air pollution in our neighborhoods from refineries and petrochemical factories ... [and] increase greenhouse gas emissions and further exacerbate global climate change."&lt;br/&gt;The group organized to demonstrate that Drexel students are against these practices. Another statement of the protesting students said, "With all of Philadelphia's leaps in sustainability and Drexel's supposed commitment to the environment, this plan represents a giant step backwards. We can only stop this destructive vision with immediate and deliberate action." Protesting groups of Drexel included the Sierra Student Coalition, the Fossil Fuel Divestment Group, the Naturalists Association and others.&lt;br/&gt;The protest included more than just Drexel students, as members and involved citizens from 19 Philadelphia and national environmental and sustainable energy groups were in attendance. Following the protest there was a counter-conference held concurrently with the disputed conference to "discuss what a sustainable Philadelphia could and should look like," according to the protestors. At the anti-conference, speakers Kevin Pool of the Grays Ferry Neighbors Association, Poune Saberi from Physicians for Social Responsibility, John Scorsone of SolareAmerica and Drexel student activist Matthew Wang provided information on Philadelphia and sustainable energy as well as information on natural gas.&lt;br/&gt;As Pennsylvania has established its dominance as the leading natural gas producing state in the United States, this conference falls in the middle of a very controversial period of policy creation and federal involvement in energy commerce. The biggest reason for this controversy is the disagreement evolving between environmentalists and economists concerning the pros and cons of natural gas production and usage. According to the Council for Growth, "the current daily gross production of natural gas from the Marcellus [shale formation] is in excess of 15 billion cubic feet - and at that level of production the formation has well over a 100-year reserve life." This huge reserve of natural gas is enticing for economists and politicians, especially in this tense period between the U.S. and the countries which provide oil imports the U.S. has relied on for the past several decades. However, environmentalists are concerned about potential pollution-causing effects of natural gas drilling and usage.&lt;br/&gt;Photo Credit: Jennifer Lam&lt;br/&gt;The ongoing disputes between the two camps on natural gas usage have yet to be affected significantly by state and federal legislation. Currently, the Pennsylvania government offers grants for alternative fuel development and deployment programs as well as projects supporting the creation and research of natural gas vehicles. The Environmental Protection Agency made its last regulatory decisions on natural gas and oil in April 2012. The latest federal legislation to govern the industry demanded certain standards on natural gas and oil containment tanks and was updated August 2013. Right now, the fighting between camps is definitely mobile only on the civilian and corporate levels, and not within legislatures.&lt;br/&gt;A final comment from the protest organizers stated that "we [the protestors] believe that with Drexel's advertised support of green technologies and sustainability, the University should not be hosting events and providing support for the expansion of the fossil fuel industry. Philadelphia itself claims to be a leader in sustainability as far as cities go, and we believe that turning the city into a natural gas hub would be a major step backwards." The protestors decidedly demonstrated an organized front against the conference to support this claim.&lt;br/&gt;Share this:&lt;br/&gt;EmailFacebookTwitterMorePrintGoogleLinkedInStumbleUponRedditTumblrPinterestPocke t&lt;br/&gt;Related</t>
         </is>
+      </c>
+      <c r="L200" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="201">
@@ -9175,10 +9782,13 @@
           <t>Labor and work</t>
         </is>
       </c>
-      <c r="J201" t="inlineStr">
+      <c r="K201" t="inlineStr">
         <is>
           <t>The College announced Wednesday that it will stop investing in HEI Hotels and Resorts, a company accused of unfair labor practices and discouraging worker unionization, according to Director of Media Relations for the College Justin Anderson.&lt;br/&gt;"For investment strategy and portfolio-specific reasons, Dartmouth has no plans to make future investments in HEI-sponsored funds," Anderson said in a statement to The Dartmouth.&lt;br/&gt;Dartmouth is the last Ivy League institution and latest school to join universities across the country in publicly renouncing future investments in HEI, according to Nathan Gusdorf '12, leader of Occupy Dartmouth and campus efforts to protest investments in HEI. Schools including Harvard University, Yale University, Vanderbilt University and Brown University have all recently stated that they will not reinvest in HEI, while Swarthmore College and Cornell University, which do not currently invest in HEI, have pledged to never invest in the company in the future, he said.&lt;br/&gt;"It's a big win for us," campaign co-organizer Janet Kim '13 said. "It took Princeton three years of campaigning to successfully get their school to disinvest, and we only took three months and applied only a couple of pressure points."&lt;br/&gt;Kim also said that the College's decision to stop investments may prove to be the "tipping point" for HEI Hotels' future.&lt;br/&gt;"HEI is heavily funded by Ivy League endowments," Kim said. "Since we are the last Ivy to pull out of investing, this means the company is going to lose a lot of funding. We're now waiting to see how HEI will respond."&lt;br/&gt;In February, Gusdorf and Kim organized a march on Parkhurst Hall to deliver a letter to College President Jim Yong Kim, the Board of Trustees, the Advisory Committee on Investor Responsibility and other administrators in protest of the College's investment in HEI.&lt;br/&gt;HEI has faced a number of labor accusations in recent years, including allegations that the company denies basic benefits to workers, Gusdorf said.&lt;br/&gt;"HEI doesn't create jobs," he said. "Their sole economic function is to fire workers and downgrade pay and benefits in order to make more money."&lt;br/&gt;In 2011, the California State Labor Commission found the company guilty of denying required rest breaks to eight employees and ordered the company to pay $41,000 in compensation, according to a press release from the labor rights group Unite Here. HEI was similarly found guilty of illegal retaliatory practices by a Massachusetts court in 2011 and received multiple National Labor Relations Board complaints in 2008, the press release said.&lt;br/&gt;Of the 10 students who delivered the letter, the majority were involved in Occupy Dartmouth, Students Stand with Staff, the Dartmouth affiliate of United Students Against Sweatshops or a combination of all three.&lt;br/&gt;Dartmouth students first came in contact with United Students Against Sweatshops during the organization's northeast regional meeting this past fall, according to Kim. After talking with Brown students who had successfully convinced their university to be the first school to publicly end all future investments in HEI, Dartmouth students began to organize a campaign.&lt;br/&gt;"This is a big victory coming out of Occupy Dartmouth," Gusdorf said. "While [the campaign] wasn't Occupy-specific, this community of activists was formed through Occupy, and it's inspiring and exciting because this is going to lead to more frequent and pronounced political actions. Let it never be said that Occupy never did anything."&lt;br/&gt;Four days after the letter was submitted, the College replied to the student group and said they would not make any further investments in HEI until the ACIR could review the matter, Gusdorf said.&lt;br/&gt;ACIR is an internal College committee composed of faculty and student representatives that meets every spring to make recommendations to the College "on how it should vote specific proxy resolutions for U.S. companies in which the College holds publicly traded shares," according to its website.&lt;br/&gt;"One of the biggest issues is that no one knows about this committee," Gusdorf said. "Even though meetings are technically open, it's not something that Dartmouth students are aware of and we have no idea how members are selected. [ACIR] is a way of satisfying or pretending to satisfy the expectation that this school practices responsible investing. It's not a real means of oversight."&lt;br/&gt;ACIR's public membership list has not been updated on its website since 2010.&lt;br/&gt;Gusdorf said he met with ACIR executive director Allegra Lubrano last term to advise the group on how to present its case to the committee.&lt;br/&gt;"We were told it wasn't fair to HEI to let us speak to the committee unless the company could also speak," Gusdorf said.&lt;br/&gt;Gusdorf said ACIR asked both HEI Hotels and the students to submit paperwork to defend their practices and their claims, respectively, for the committee's consideration.&lt;br/&gt;"I think this was incredibly silly," he said. "It suggests that we're equally as powerful as HEI, and it shows how much the system is rigged against anyone being able to change anything. Our case is a moral and a political one."&lt;br/&gt;Gusdorf said he received an email from Lubrano on the morning of May 2, the day that ACIR was scheduled to meet, with the College's decision to divest. ACIR therefore made a decision before its formal review of the matter was scheduled to start, Janet Kim said. Chief of Staff David Spalding sent a follow-up email to Gusdorf confirming the announcement, he said.&lt;br/&gt;Gusdorf said he believes the College's decision to divest was a political move made in response to the students' campaign efforts.&lt;br/&gt;"They said it was for investment strategy reasons,' and all other schools except for Brown said the same thing," he said. "But it was all about political pressure. Finance people want to remain completely insensitive because often times schools invest in unethical companies."&lt;br/&gt;Gusdorf and Kim said that the College's general reluctance to speak about its investment in HEI is a reflection of a problem of transparency in the College's administration.&lt;br/&gt;"Our school isn't a total democracy, but students and faculty should have some decision-making power and know what's going on and I don't think we meet those goals right now," Gusdorf said.&lt;br/&gt;Gusdorf said they considered various ways to express public discontent over the College's investments and "how aggressive" the group wanted to be with their protest.&lt;br/&gt;"We learned being more militant is often what's necessary to be effective," he said. "Accepting the structure of bureaucracy leads to failure when you're pressing political issues."&lt;br/&gt;In addition to the February march through Parkhurst, the students also marched throughout campus as a "general protest" on May 1, or May Day, which is considered to be International Worker's Day, Gusdorf said.&lt;br/&gt;Kim said she agreed that the group's active protesting techniques contributed to their success.&lt;br/&gt;"If we had gone directly to ACIR, we definitely would have seen a delay," she said. "The College probably would not have overturned their investment so quickly. We got a response from Spalding right after we protested with our letter. Our effectiveness comes from our tactics and the way we put out our message."&lt;br/&gt;Gusdorf and Kim said they are working on two more immediate campaigns to address other issues.&lt;br/&gt;"The HEI victory makes us excited to do more work," Kim said.&lt;br/&gt;In light of upcoming contract discussions with union workers at the College, Gusdorf said he hopes to make a "public demand" for fair contract renegotiation.&lt;br/&gt;"Unions can't engage in protests or other political actions until the negotiations break down," he said. "As I understand, the College is using delaying methods so fewer people are around to be upset with these unfair practices."&lt;br/&gt;Gusdorf said students affiliated with the Occupy movement are also pushing the College to disassociate itself with the Fair Labor Association, which includes companies that have been accused of fraudulent operations in sweatshop factories. Instead, Gusdorf said he would like the College to affiliate with the Worker's Rights Consortium, a group which he said has a "fair code of conduct for how universities source their school apparel to avoid sweatshop factories."&lt;br/&gt;"Students need to have more authority here," Gusdorf said of Dartmouth's campus culture. "We're so subservient all the time to the administration, but this becomes a significant question in light of the new College presidential search. Are students going to have actual voting power or are we always going to be stuck?"&lt;br/&gt;Lubrano could not be reached for comment by press time.</t>
         </is>
+      </c>
+      <c r="L201" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="202">
@@ -9218,10 +9828,13 @@
           <t>University governance, admin, policies, programs, curriculum, Labor and work</t>
         </is>
       </c>
-      <c r="J202" t="inlineStr">
+      <c r="K202" t="inlineStr">
         <is>
           <t>The College announced Wednesday that it will stop investing in HEI Hotels and Resorts, a company accused of unfair labor practices and discouraging worker unionization, according to Director of Media Relations for the College Justin Anderson.&lt;br/&gt;"For investment strategy and portfolio-specific reasons, Dartmouth has no plans to make future investments in HEI-sponsored funds," Anderson said in a statement to The Dartmouth.&lt;br/&gt;Dartmouth is the last Ivy League institution and latest school to join universities across the country in publicly renouncing future investments in HEI, according to Nathan Gusdorf '12, leader of Occupy Dartmouth and campus efforts to protest investments in HEI. Schools including Harvard University, Yale University, Vanderbilt University and Brown University have all recently stated that they will not reinvest in HEI, while Swarthmore College and Cornell University, which do not currently invest in HEI, have pledged to never invest in the company in the future, he said.&lt;br/&gt;"It's a big win for us," campaign co-organizer Janet Kim '13 said. "It took Princeton three years of campaigning to successfully get their school to disinvest, and we only took three months and applied only a couple of pressure points."&lt;br/&gt;Kim also said that the College's decision to stop investments may prove to be the "tipping point" for HEI Hotels' future.&lt;br/&gt;"HEI is heavily funded by Ivy League endowments," Kim said. "Since we are the last Ivy to pull out of investing, this means the company is going to lose a lot of funding. We're now waiting to see how HEI will respond."&lt;br/&gt;In February, Gusdorf and Kim organized a march on Parkhurst Hall to deliver a letter to College President Jim Yong Kim, the Board of Trustees, the Advisory Committee on Investor Responsibility and other administrators in protest of the College's investment in HEI.&lt;br/&gt;HEI has faced a number of labor accusations in recent years, including allegations that the company denies basic benefits to workers, Gusdorf said.&lt;br/&gt;"HEI doesn't create jobs," he said. "Their sole economic function is to fire workers and downgrade pay and benefits in order to make more money."&lt;br/&gt;In 2011, the California State Labor Commission found the company guilty of denying required rest breaks to eight employees and ordered the company to pay $41,000 in compensation, according to a press release from the labor rights group Unite Here. HEI was similarly found guilty of illegal retaliatory practices by a Massachusetts court in 2011 and received multiple National Labor Relations Board complaints in 2008, the press release said.&lt;br/&gt;Of the 10 students who delivered the letter, the majority were involved in Occupy Dartmouth, Students Stand with Staff, the Dartmouth affiliate of United Students Against Sweatshops or a combination of all three.&lt;br/&gt;Dartmouth students first came in contact with United Students Against Sweatshops during the organization's northeast regional meeting this past fall, according to Kim. After talking with Brown students who had successfully convinced their university to be the first school to publicly end all future investments in HEI, Dartmouth students began to organize a campaign.&lt;br/&gt;"This is a big victory coming out of Occupy Dartmouth," Gusdorf said. "While [the campaign] wasn't Occupy-specific, this community of activists was formed through Occupy, and it's inspiring and exciting because this is going to lead to more frequent and pronounced political actions. Let it never be said that Occupy never did anything."&lt;br/&gt;Four days after the letter was submitted, the College replied to the student group and said they would not make any further investments in HEI until the ACIR could review the matter, Gusdorf said.&lt;br/&gt;ACIR is an internal College committee composed of faculty and student representatives that meets every spring to make recommendations to the College "on how it should vote specific proxy resolutions for U.S. companies in which the College holds publicly traded shares," according to its website.&lt;br/&gt;"One of the biggest issues is that no one knows about this committee," Gusdorf said. "Even though meetings are technically open, it's not something that Dartmouth students are aware of and we have no idea how members are selected. [ACIR] is a way of satisfying or pretending to satisfy the expectation that this school practices responsible investing. It's not a real means of oversight."&lt;br/&gt;ACIR's public membership list has not been updated on its website since 2010.&lt;br/&gt;Gusdorf said he met with ACIR executive director Allegra Lubrano last term to advise the group on how to present its case to the committee.&lt;br/&gt;"We were told it wasn't fair to HEI to let us speak to the committee unless the company could also speak," Gusdorf said.&lt;br/&gt;Gusdorf said ACIR asked both HEI Hotels and the students to submit paperwork to defend their practices and their claims, respectively, for the committee's consideration.&lt;br/&gt;"I think this was incredibly silly," he said. "It suggests that we're equally as powerful as HEI, and it shows how much the system is rigged against anyone being able to change anything. Our case is a moral and a political one."&lt;br/&gt;Gusdorf said he received an email from Lubrano on the morning of May 2, the day that ACIR was scheduled to meet, with the College's decision to divest. ACIR therefore made a decision before its formal review of the matter was scheduled to start, Janet Kim said. Chief of Staff David Spalding sent a follow-up email to Gusdorf confirming the announcement, he said.&lt;br/&gt;Gusdorf said he believes the College's decision to divest was a political move made in response to the students' campaign efforts.&lt;br/&gt;"They said it was for investment strategy reasons,' and all other schools except for Brown said the same thing," he said. "But it was all about political pressure. Finance people want to remain completely insensitive because often times schools invest in unethical companies."&lt;br/&gt;Gusdorf and Kim said that the College's general reluctance to speak about its investment in HEI is a reflection of a problem of transparency in the College's administration.&lt;br/&gt;"Our school isn't a total democracy, but students and faculty should have some decision-making power and know what's going on and I don't think we meet those goals right now," Gusdorf said.&lt;br/&gt;Gusdorf said they considered various ways to express public discontent over the College's investments and "how aggressive" the group wanted to be with their protest.&lt;br/&gt;"We learned being more militant is often what's necessary to be effective," he said. "Accepting the structure of bureaucracy leads to failure when you're pressing political issues."&lt;br/&gt;In addition to the February march through Parkhurst, the students also marched throughout campus as a "general protest" on May 1, or May Day, which is considered to be International Worker's Day, Gusdorf said.&lt;br/&gt;Kim said she agreed that the group's active protesting techniques contributed to their success.&lt;br/&gt;"If we had gone directly to ACIR, we definitely would have seen a delay," she said. "The College probably would not have overturned their investment so quickly. We got a response from Spalding right after we protested with our letter. Our effectiveness comes from our tactics and the way we put out our message."&lt;br/&gt;Gusdorf and Kim said they are working on two more immediate campaigns to address other issues.&lt;br/&gt;"The HEI victory makes us excited to do more work," Kim said.&lt;br/&gt;In light of upcoming contract discussions with union workers at the College, Gusdorf said he hopes to make a "public demand" for fair contract renegotiation.&lt;br/&gt;"Unions can't engage in protests or other political actions until the negotiations break down," he said. "As I understand, the College is using delaying methods so fewer people are around to be upset with these unfair practices."&lt;br/&gt;Gusdorf said students affiliated with the Occupy movement are also pushing the College to disassociate itself with the Fair Labor Association, which includes companies that have been accused of fraudulent operations in sweatshop factories. Instead, Gusdorf said he would like the College to affiliate with the Worker's Rights Consortium, a group which he said has a "fair code of conduct for how universities source their school apparel to avoid sweatshop factories."&lt;br/&gt;"Students need to have more authority here," Gusdorf said of Dartmouth's campus culture. "We're so subservient all the time to the administration, but this becomes a significant question in light of the new College presidential search. Are students going to have actual voting power or are we always going to be stuck?"&lt;br/&gt;Lubrano could not be reached for comment by press time.</t>
         </is>
+      </c>
+      <c r="L202" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="203">
@@ -9262,10 +9875,13 @@
           <t>Public funding for higher education, Economy/inequality, Social services and welfare</t>
         </is>
       </c>
-      <c r="J203" t="inlineStr">
+      <c r="K203" t="inlineStr">
         <is>
           <t>Tens of thousands of people assembled on McGill College last Friday to protest the Liberal government’s austerity measures, which include severe cuts to education and healthcare. Undeterred by the fact that the demonstration was swiftly declared illegal by the police, demonstrators marched for over two and a half hours, making their way down Ste. Catherine and to Montreal’s Old Port, where the demonstration eventually dispersed.&lt;br/&gt;“It’s important to be here because austerity cuts are affecting everyone in Quebec, students included,” Kelly, a Women’s Studies student at McGill, told The Daily. “Over $200 million has been cut from university funding from the province, and that translates to over $14 million being cut at McGill.”&lt;br/&gt;Organized by a large coalition that includes the Association pour une solidarité syndicale étudiante (ASSÉ), the event drew thousands of students. Buses from CEGEPs and universities were observed picking up protesters at the demonstration’s termination point.&lt;br/&gt;“It was great seeing […] 50,000 people out on the streets,” ASSÉ co-spokesperson Camille Godbout told The Daily. “It was great to see all the groups mobilizing against the austerity cuts. We have today 82,000 students on strike across the province so [it was good] seeing other groups, unions, and community groups coming down to Montreal.”&lt;br/&gt;“It’s important to be here because austerity cuts are affecting everyone in Quebec, students included.”&lt;br/&gt;“The province, as far as I know, didn’t consult people before putting this budget forward,” said Kelly. “They didn’t give people in Quebec a choice about it, that’s why everyone’s angry about it and coming to resist and show the province that this is not the way to do things.”&lt;br/&gt;Kelly was part of a small McGill contingent of around twenty students. A larger contingent from Concordia, numbering around 100 students, was also present.&lt;br/&gt;“We [at the Concordia Graduate Students’ Association (GSA)] do have a mandate, actually, to support free education,” GSA VP External Mohammad Jawad Khan told The Daily. “So I believe right now is not the right time to [make] budget cuts [for] the university and the government. Unfortunately, Concordia has wholeheartedly accepted them.”&lt;br/&gt;Christian, a demonstrator, called the austerity measures anti-democratic. “Austerity measures are a cut at the level of social democracy,” he said. “It is not only a divestment in the [form] of money in the strictest sense, but a divestment [from] the [social] capital.”&lt;br/&gt;“[Instead of the democratic process] right now, it is the IMF [International Monetary Fund] and international banks who are [driving] national economies,” Christian noted.&lt;br/&gt;Although the protest had been declared illegal, police intervention was minimal. Contingents of officers in riot gear walked with the crowd, and a number of officers on bicycles escorted the demonstration. Demonstrators were observed conversing and interacting with the officers at the scene.&lt;br/&gt;Godbout suggested that the lighter-than-usual police presence was a product of the demonstration’s opposition to the controversial Bill 3, which would require higher contributions to the pension fund for many police officers and other public service employees in Quebec.&lt;br/&gt;“We stand in solidarity with all the workers who are touched right now by the [changes in the] pensions. Clearly we still stand against police brutality, but maybe [the pensions have] something to do with the fact that [the police] acted more lightly than usual,” she said.&lt;br/&gt;Indeed, a group of several hundred firefighters representing the Association des pompiers de Montréal (ADPM) participated in the protest. The ADPM made headlines in August when a group of its members disturbed a City of Montreal council meeting in protest of Bill 3. Six firefighters were fired and dozens more suspended following the incident.&lt;br/&gt;In order to emphasize their dissatisfaction with the government’s policies, hundreds of protesters took to the streets again on Friday night following the main demonstration. This time, several arrests were made.&lt;br/&gt;A collective organization committee called the “Comité large printemps 2015” has also been formed, through which students and workers will continue to organize and escalate pressure tactics, potentially leading up to a strike.&lt;br/&gt;“History in Quebec has shown that past strikes have been really effective in getting the government to change what they’re doing,” said Kelly.&lt;br/&gt;[flickr id=”72157649081364165″]</t>
         </is>
+      </c>
+      <c r="L203" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="204">
@@ -9306,10 +9922,13 @@
           <t>Public funding for higher education, Economy/inequality, Social services and welfare</t>
         </is>
       </c>
-      <c r="J204" t="inlineStr">
+      <c r="K204" t="inlineStr">
         <is>
           <t>Click on a title or quote to read more!&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;The Tariq Khan Drama&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;The Students’ Society of McGill University (SSMU) saw its fair share of the short-lived SSMU President Tariq Khan this year. Elections SSMU invalidated Khan’s election as SSMU President on April 1, 2014 – a week after he was elected president by a margin of only 78 votes – due to SSMU bylaw infractions committed during his campaign. The violations included the participation of individuals external to SSMU in his campaign, the sending of unsolicited text messages to the public – for which he had been censured on March 21, the last day of the campaign period –  inconsistencies in campaign expenditures, and the impingement of the spirit of a fair campaign and of the voting process.&lt;br/&gt;Following his invalidation, Khan filed an appeal with the SSMU Judicial Board (J-Board), which upheld his invalidation on April 29. Khan later took this issue to the Superior Court of Quebec and filed a request on May 29 for a preliminary injunction to reinstate him as SSMU President until the full hearing for a permanent injunction. The Court dismissed his application on June 3, reasoning that his reinstatement would have incurred additional costs and caused undue inconvenience on the part of SSMU. Khan later withdrew his court case in October before its full hearing due to financial motivations and the decreasing timeliness of the case.&lt;br/&gt;Khan resurfaced on the first day of the 2015-16 SSMU elections when screenshots of a Facebook conversation were released on reddit, revealing recently-elected SSMU President Kareem Ibrahim’s suggestion to hack Khan’s Facebook account last year. Upon news of the screenshots, he revealed his intentions to update the police report that he filed after his account was allegedly hacked on March 27, 2014.&lt;br/&gt;—Emma Noradounkian&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Campus unions get moving&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Compared with 2011’s McGill University Non-Academic Certified Association (MUNACA) strike, the past few years have been fairly quiet on the union front. This year, however, has seen a flurry of activity at McGill unions.&lt;br/&gt;Floor fellows began a union drive over a year ago in November 2013, driven by the University’s earlier push for a change in residence models. Since then, floor fellows have succeeded at forming a union, and joined the Association of McGill University Support Employees (AMUSE) last May. The process, however, has not been without hiccups: this January,collective agreement negotiations between the University and the floor fellows bargaining unit stalled over the exclusion of the “core values” of floor fellows (namely their anti-oppressive mandate and harm reduction approach) from the proposed agreement. The negotiations have started again and are currently ongoing.&lt;br/&gt;McGill’s Teaching Union, AGSEM, has also been working to unionize undergraduate teaching support staff, which include course graders, note-takers, and teaching assistants (TAs). Despite receiving support from post-grads and undergrads, the process has not been without tensions: McGill challenged AGSEM’s promotion of its own union campaign due to disputing interpretations of the Quebec Labour Code. At the date of publication, the union drive is still ongoing.&lt;br/&gt;This year also saw a merger between AMUSE and MUNACA, despite some internal trepidation over their differing sizes. Joint bylaws are on the way.&lt;br/&gt;—Molly Korab&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;“I cannot celebrate the status quo of mental health support at McGill.”&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;The mental health landscape at McGill for the 2014-15 academic year has been a disappointing one. Though a working group was struck under the purview of Senate in October 2013, most of the recommendations issued by the group in June 2014 have yet to be implemented. Of the 36 initiatives on the roster, only two have been completed, the first being the development of a student services app, and the second publicly presented only as “further [development] of a robust early alert program.”&lt;br/&gt;While both the administration and student government have been pursuing mental health services reform, they do not appear to be working closely. SSMU VP University Affairs Claire Stewart-Kanigan told The Daily in October, around the time the University announced its intention to create a ‘wellness portal,’ that the relationship between the two was “a consultative arrangement, not a partnership. Given that SSMU is named as a partner on the website, consultation is not enough.”&lt;br/&gt;There have been no updates on the ‘wellness portal,’ projected to be launched in Winter 2015.&lt;br/&gt;Most of the visible events that have taken place this year – in particular, the second annual Students In Mind conference on mental health in October and the Mental Health Awareness Week in November – were largely student-driven and student-led initiatives. Additionally, the most vocal advocates for mental health reform have been students.&lt;br/&gt;In addition to managing the planning and execution of the Mental Health Awareness Week, Stewart-Kanigan oversaw the successful launch of SSMU’s new mental health department, which involved the hire of a coordinator and the development of a mental health listserv to promote peer and professional support services for students and forward student-led anti-stigma initiatives.&lt;br/&gt;­&lt;br/&gt;—Emily Saul&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Tense debates at General Assemblies&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;After years of SSMU General Assemblies (GAs) that have failed to reach quorum or present particularly political motions, portions of this year’s GAs saw huge turnout – with over 700 students attending the Fall 2014 GA and over 500 students at the Winter 2015 GA – as well as plenty of controversy.&lt;br/&gt;Most notably, both GAs saw motions that poked at the long-dormant Israel-Palestine divide on campus. At the Fall 2014 GA, a motion to stand in solidarity with the people of the occupied Palestinian territories and condemn Israel’s violence toward Palestine over the summer was postponed indefinitely, with 402 in favour and 337 against, after hours of debate. At the Winter 2015 GA, a motion to divest from companies profiting from the illegal occupation of the Palestinian territories garnered the endorsement of many campus groups (including The Daily), but failed by only 64 votes.&lt;br/&gt;Despite the intense attention given to these two motions, a number of other political motions passed, mandating SSMU to take action on diverse issues such as unpaid internships, military research, climate change, and austerity. SSMU also saw a J-Board challenge after the contentious postponement of the Fall 2014 Palestine motion, where the judicial body ruled that simplified standing rules should be adopted and publicized at GAs to better facilitate debate.&lt;br/&gt;More broadly, this year’s GAs have prompted a campus-wide (and still ongoing) dialogue on the political role of the student union – which most notably played itself out in the recent 2015-16 SSMU executive elections – with some students questioning whether SSMU should take stances on ‘divisive’ political issues.&lt;br/&gt;—Dana Wray&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Students against austerity&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;This year has seen a whirlwind of opposition against austerity measures and budget cuts set in place by the Liberal provincial government, which have reduced funding to social services, including welfare, healthcare, and education. In the fall, as part of an ongoing push that began even before this academic year, students at UQAM organized a group to allow students and community members to work together to protest these cuts: the Comité Printemps 2015, which helped mobilize around 80,000 students to go on strike on Halloween, and over 80,000 students planned to strike against austerity during March and April. This mobilization has not evaded McGill, as French language and literature students recently voted to go on strike for a week, and other departments have planned strike votes.&lt;br/&gt;These student initiatives contrast with the stance taken by the McGill administration, which has been accommodating of austerity measures. McGill has been making cuts of its own, after undergoing $45 million in cuts from the provincial government over the last four years. The results of these cuts have been felt by workers at McGill, as the administration has set up a hiring freeze, decreasing the number of jobs available, and increasing the workloads of many employees. To combat the administration’s decrease in the number of full-time jobs at McGill, as well as the fact that many positions with benefits have been replaced with lower-paid, part-time jobs that do not receive benefits, AMURE recently voted to start a fund for counselling services for its members.&lt;br/&gt;&lt;br/&gt;In response to the austerity measures taken by both McGill and the Quebec government SSMU and the Post-Graduate Students’ Society (PGSS) have taken stances against the government’s measures and asked McGill to oppose these huge cuts. At the SSMU Fall 2014 GA, students voted to add advocating against austerity to the portfolio of the VP External, and SSMU has since hosted an anti-austerity activities night to show students just how wide-reaching the damaging effects of austerity can be.&lt;br/&gt;—Jill Bachelder&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Sustainability at McGill&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Many important initiatives that began in previous years were continued and strengthened over the course of this one. Divest McGill helped organize a bus to take McGill and Concordia students to the People’s Climate March in New York City, where over 400,000 people marched in the streets of Manhattan to protest the United Nations Climate Summit and raise awareness about global warming. Divest also submitted a new petition for McGill to divest from fossil fuel companies to the Board of Governors (BoG), making a comeback two years after its first petition was presented to, and rejected by, the BoG. In addition, over 100 faculty members signed on to an open letter submitted to the BoG in support of divestment.&lt;br/&gt;SSMU also continued its efforts to promote sustainability on campus, starting a composting program in the Shatner building, and joining Étudiant(e)s contre les oléoducs (ÉCO), after the a motion passed at the Fall 2014 GA that mandated SSMU to stand alongside groups combatting climate change.&lt;br/&gt;Finally, the McGill Office of Sustainability launched its Vision 2020 program, an initiative aiming to create a more sustainable McGill by the year 2020.&lt;br/&gt;—Jill Bachelder</t>
         </is>
+      </c>
+      <c r="L204" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="205">
@@ -9349,10 +9968,13 @@
           <t>Environmental, University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J205" t="inlineStr">
+      <c r="K205" t="inlineStr">
         <is>
           <t>SAN FRANCISCO - At its meeting Wednesday, the UC Board of Regents' Committee on Investments voted to approve a recommendation from the UC task force on sustainable investing to continue the university's investments in fossil fuel companies.&lt;br/&gt;At the meeting, members of Fossil Free UC, a coalition advocating divestment, protested the recommendation's proposal to not divest. The recommendation encourages the university to implement a framework for sustainable investment by the end of the fiscal year and invest $1 billion into green initiatives over the next five years. The full UC Board of Regents will vote on the recommendation Thursday.&lt;br/&gt;"We sought to take a truly holistic approach and make recommendations that could have meaningful long-term impacts," said Jagdeep Singh Bachher, UC chief investment officer and head of the task force.&lt;br/&gt;According to UC spokesperson Dianne Klein, the majority of the task members, after looking at research on the issue, felt that divestment would not do much to alleviate the effects of climate change. The UC system currently invests $10 billion out of the $91 billion managed by the university in energy companies.&lt;br/&gt;"(Divestment) would certainly have a negative effect on our portfolio as far as returns," Klein said.&lt;br/&gt;Student Regent Sadia Saifuddin attempted to make an amendment to the final recommendation that would insert language considering divestment from coal companies in the future, which ultimately did not pass.&lt;br/&gt;As part of the recommendation, the university would sign on to the United Nations Principles for Responsible Investment, a worldwide investor network dedicated to helping its members invest sustainably. The recommendation also proposes that the university integrate environmental, social and governance factors into its portfolio decisions.&lt;br/&gt;"We're absolutely committed to investing in our future," Bachher said. "Making that commitment is the right thing to do in the long term."&lt;br/&gt;Members of Fossil Free UC assembled in a protest that began outside and continued into the meeting. Chanting slogans, the protesters held signs reading, "We are worth more than fossil fuels" and "Students not fossil fuels."&lt;br/&gt;According to Victoria Fernandez, a UC Berkeley senior and a member of both Fossil Free UC and the task force, students were not fairly consulted during the process leading up to the task force's recommendation. She said while Greg Boyce, CEO of coal company Peabody Energy, was invited to lobby the committee, students were not given the chance to bring in experts, such as Don Gould, an asset manager and a Pitzer College trustee, to advocate divestment.&lt;br/&gt;"Industry voice was being prioritized over the voices of advocates for divestment," Fernandez said.&lt;br/&gt;This year, Stanford University divested from coal companies, and Pitzer College removed all assets in fossil fuel companies.&lt;br/&gt;Contact Hiep Nguyen at [email protected] and follow him on Twitter @_hiepn.</t>
         </is>
+      </c>
+      <c r="L205" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="206">
@@ -9392,10 +10014,13 @@
           <t>Pro-Palestine/BDS</t>
         </is>
       </c>
-      <c r="J206" t="inlineStr">
+      <c r="K206" t="inlineStr">
         <is>
           <t>An organization representing university students’ unions across the province passed a unanimous emergency motion to boycott Israel at its general meeting last month.&lt;br/&gt;The controversial resolution was submitted by the Ryerson Students’ Union at the general meeting of the Canadian Federation of Students-Ontario (CFS-O), the Canadian Press reported. The motion called on members to join the Boycott, Divestment and Sanctions Movement against Israel.&lt;br/&gt;“Students have long been at the forefront of movements against foreign occupation, in support of peace and that movement will continue on campuses across Ontario,” said Anna Goldfinch, national executive representative of CFS-O. “This motion is reflective of having a province-wide endorsement of this campaign to start working across Ontario, not just local campuses.”&lt;br/&gt;Over 30 students’ unions across Ontario–including UTMSU–are members of the CFS-O and over 100 delegates gathered to vote unanimously on the passing of the resolution. UTMSU President Hassan Havili did not respond to requests for comment; it is unconfirmed whether UTMSU sent a representative to the meeting.&lt;br/&gt;Despite being passed unanimously, the CFS-O motion has received criticism from various groups, including from the Society of Graduate and Professional Students at Queen’s University, which is a CFS-O member but was unable to attend the meeting.&lt;br/&gt;The Israel-Palestine conflict has been the subject of controversy at UTM in the past. In February of last year, UTMSU officially recognized the BDS movement. After receiving a total of 700 signatures from UTM’s Students Against Israeli Apartheid (SAIA) group, the motion was passed.&lt;br/&gt;Last March, SAIA also hosted a “Hungry for Freedom” event which featured Skype calls with and recordings of freed Palestinian prisoners. The event and its content were reviewed by university administration amid concerns over its nature. SAIA also promoted the BDS Movement at the event.&lt;br/&gt;In the past, the CFS-O has called on the Harper government to stop supplying arms to Israel and to end the Canada-Israel free trade agreement. The campaign has since moved on to advocate for the rights and freedoms of those affected by the military occupation within Gaza, along with supporting the right to education for Palestinian civil society.&lt;br/&gt;Boycott, Divestment, and Sanctions, which has supporters and critics on both political sides of the Israel-Palestine controversy, is a movement created in 2005 by Palestinian NGOs to discourage the government of Israel to stop its alleged violations of Palestinian human rights.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Tweet&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Share&lt;br/&gt;0&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Reddit&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;+1&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;LinkedIn&lt;br/&gt;0&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Email</t>
         </is>
+      </c>
+      <c r="L206" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="207">
@@ -9435,10 +10060,13 @@
           <t>Labor and work, Tuition, fees, financial aid, University governance, admin, policies, programs, curriculum, LGB+/Sexual orientation (For)</t>
         </is>
       </c>
-      <c r="J207" t="inlineStr">
+      <c r="K207" t="inlineStr">
         <is>
           <t>Israel Peace Week this year offered a pro-Israel narrative to counter what zionists allege is anti-Israel propaganda.&lt;br/&gt;The annual week of events Hasbara at York hosts which coincides with Israeli Apartheid Week is Israel Peace Week. Hasbara believes activities like IAW is detrimental to peace and coexistence on campus and beyond.&lt;br/&gt;“We want to promote dialogue on Israel and the Middle East to the students at York University,” says Ariella Daniels, Hasbara president. “The only way we can learn from each other is to provide a safe space to facilitate a discussion on the issues.”&lt;br/&gt;Due to the strike, Hasbara was unable to execute their plans this year.&lt;br/&gt;“Academics are a priority to students and they have a right to make their own decision on crossing picket lines and attending classes,” says  Daniels.&lt;br/&gt;“As for CUPE giving a platform for students to make false accusations on Israel, she says, I think it is sad that a union claiming to represent a large population of workers feel the need to marginalize Jewish and Pro-Israel students and faculty.&lt;br/&gt;“Anti-Israel sentiment has nothing to do with the issues regarding the strike. CUPE is using their position for external political agendas, but this is nothing new.”&lt;br/&gt;Daniels returned from a conference hosted by the organization StandWithUs which discussed the threats of the Boycott, Divestment and Sanctions (BDS) movement.&lt;br/&gt;She had the opportunity to hear from Palestinian activist Bassem Eid who “firmly stands against BDS.”Bassem stated that BDS is a “Prelude to Genocide to Palestinians.”&lt;br/&gt;Many people have expressed concern over the boycott, divestment, sanctions movement which has made considerable gains over the last decade.&lt;br/&gt;Over three hundred students are petitioning York over SAIA’s Israeli Apartheid Week, claiming that one of their guest speakers, Steven Salaita, is anti-Semitic.&lt;br/&gt;“SAIA is lying when they say Palestinians support the boycott movement against Israel,” says Willem Hart, fourth year social science student.&lt;br/&gt;Last year, anti-Israel activists campaigned against Soda Stream for its factory in the disputed territory, adds Hart.&lt;br/&gt;Despite the fact that the Palestinians hired by Soda Stream made the same hourly wage as the employees who commuted from Israel, says Hart, and even despite the fact that the factory had built a mosque on-sight to facilitate the Islamic prayer sessions that went on throughout the day, the factory in the West Bank was still the target of boycotts and condemnations.&lt;br/&gt;Hart says all the boycott accomplished was renewed unemployment and economic insecurity of hundreds of Palestinian workers.&lt;br/&gt;Hart cites a number of Palestinian activists who stand against BDS, such as Bassem Eid, the founder and former director of the Jerusalem-based Palestinian Human Rights Monitoring Group.&lt;br/&gt;Additionally, Zionist critics say the BDS movement singles out one country for condemnation in the complex Middle East issue.&lt;br/&gt;“It is misguided, because instead of promoting peace, it furthers the conflict,” says Meryle Lee Kates, executive director of StandWithUs.&lt;br/&gt;“BDS uses the language of social justice and human rights to mask its true goals – the elimination of Israel.”&lt;br/&gt;According to Kates, the leaders of the BDS campaign create a hostile environment by marginalizing Jewish and pro-Israel students, attempting to shut down dialogue. This, says Kates, does not allow for civil discourse that students of all races and religions have a right to expect from their institutions of higher learning.&lt;br/&gt;“We believe BDS undermines the establishment of a two-state solution,” she says. “The two-state solution that Palestinian leaders rejected in 2000, 2001 and 2008.”&lt;br/&gt;Those who do not hold the Palestinian leadership accountable are infantilizing them and perpetuating obstacles to peace, adds Kates.&lt;br/&gt;Kates says while BDS activity has increased, many students are increasingly resenting the co-option of their voices by BDS activists.&lt;br/&gt;“Jewish and pro-Israel students are becoming more vocal and united in defense of their communities, their homeland, and the Jewish people’s inalienable right to self-determination.”&lt;br/&gt;Zina Rakhamilova, StandWithUs at York, campus coordinator,  says use of the word “apartheid” applied to Israel is completely inaccurate.&lt;br/&gt;“The apartheid in South Africa was institutionalized and legalized segregation based on race,” says Rakhamilova.&lt;br/&gt;Rakhamilova cites Arab citizens of Israel who are  members of the supreme court, members of parliament (the Knesset), and leaders of academic institutions.&lt;br/&gt;In fact, Israel is the diametric opposite of South African apartheid’s legal system of oppression and discrimination based on skin color, she adds.&lt;br/&gt;“The leaders of the BDS movement have openly opposed the two-state solution that Israel and most Palestinians seek, and have condemned any aspect of Israeli-Palestinian cooperation.”&lt;br/&gt;“The agenda of this movement does not seek to challenge ideas or foster dialogue – it seeks only to demonize the one state in the Middle East that treats its minorities equally.”&lt;br/&gt;Rakhamilova and Kates challenge BDS activists who, they allege, use the apartheid screen to find ways real ways of helping the Palestinians who are held captive by their corrupt leadership.&lt;br/&gt;“University campuses should be safe places for all students to voice their views,” says Rakhamilova.&lt;br/&gt;“Equating Israel to apartheid South Africa is not only academically dishonest, it is an excuse to demonize the state of Israel and ignore the active terrorist groups that openly call for the destruction of the Jewish state and persecute their own minorities.”&lt;br/&gt;&lt;br/&gt;Ryan Moore, Assistant News Editor</t>
         </is>
+      </c>
+      <c r="L207" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="208">
@@ -9478,10 +10106,13 @@
           <t>Pro-Israel/Zionism, Faith-based discrimination</t>
         </is>
       </c>
-      <c r="J208" t="inlineStr">
+      <c r="K208" t="inlineStr">
         <is>
           <t>Israel Peace Week this year offered a pro-Israel narrative to counter what zionists allege is anti-Israel propaganda.&lt;br/&gt;The annual week of events Hasbara at York hosts which coincides with Israeli Apartheid Week is Israel Peace Week. Hasbara believes activities like IAW is detrimental to peace and coexistence on campus and beyond.&lt;br/&gt;“We want to promote dialogue on Israel and the Middle East to the students at York University,” says Ariella Daniels, Hasbara president. “The only way we can learn from each other is to provide a safe space to facilitate a discussion on the issues.”&lt;br/&gt;Due to the strike, Hasbara was unable to execute their plans this year.&lt;br/&gt;“Academics are a priority to students and they have a right to make their own decision on crossing picket lines and attending classes,” says  Daniels.&lt;br/&gt;“As for CUPE giving a platform for students to make false accusations on Israel, she says, I think it is sad that a union claiming to represent a large population of workers feel the need to marginalize Jewish and Pro-Israel students and faculty.&lt;br/&gt;“Anti-Israel sentiment has nothing to do with the issues regarding the strike. CUPE is using their position for external political agendas, but this is nothing new.”&lt;br/&gt;Daniels returned from a conference hosted by the organization StandWithUs which discussed the threats of the Boycott, Divestment and Sanctions (BDS) movement.&lt;br/&gt;She had the opportunity to hear from Palestinian activist Bassem Eid who “firmly stands against BDS.”Bassem stated that BDS is a “Prelude to Genocide to Palestinians.”&lt;br/&gt;Many people have expressed concern over the boycott, divestment, sanctions movement which has made considerable gains over the last decade.&lt;br/&gt;Over three hundred students are petitioning York over SAIA’s Israeli Apartheid Week, claiming that one of their guest speakers, Steven Salaita, is anti-Semitic.&lt;br/&gt;“SAIA is lying when they say Palestinians support the boycott movement against Israel,” says Willem Hart, fourth year social science student.&lt;br/&gt;Last year, anti-Israel activists campaigned against Soda Stream for its factory in the disputed territory, adds Hart.&lt;br/&gt;Despite the fact that the Palestinians hired by Soda Stream made the same hourly wage as the employees who commuted from Israel, says Hart, and even despite the fact that the factory had built a mosque on-sight to facilitate the Islamic prayer sessions that went on throughout the day, the factory in the West Bank was still the target of boycotts and condemnations.&lt;br/&gt;Hart says all the boycott accomplished was renewed unemployment and economic insecurity of hundreds of Palestinian workers.&lt;br/&gt;Hart cites a number of Palestinian activists who stand against BDS, such as Bassem Eid, the founder and former director of the Jerusalem-based Palestinian Human Rights Monitoring Group.&lt;br/&gt;Additionally, Zionist critics say the BDS movement singles out one country for condemnation in the complex Middle East issue.&lt;br/&gt;“It is misguided, because instead of promoting peace, it furthers the conflict,” says Meryle Lee Kates, executive director of StandWithUs.&lt;br/&gt;“BDS uses the language of social justice and human rights to mask its true goals – the elimination of Israel.”&lt;br/&gt;According to Kates, the leaders of the BDS campaign create a hostile environment by marginalizing Jewish and pro-Israel students, attempting to shut down dialogue. This, says Kates, does not allow for civil discourse that students of all races and religions have a right to expect from their institutions of higher learning.&lt;br/&gt;“We believe BDS undermines the establishment of a two-state solution,” she says. “The two-state solution that Palestinian leaders rejected in 2000, 2001 and 2008.”&lt;br/&gt;Those who do not hold the Palestinian leadership accountable are infantilizing them and perpetuating obstacles to peace, adds Kates.&lt;br/&gt;Kates says while BDS activity has increased, many students are increasingly resenting the co-option of their voices by BDS activists.&lt;br/&gt;“Jewish and pro-Israel students are becoming more vocal and united in defense of their communities, their homeland, and the Jewish people’s inalienable right to self-determination.”&lt;br/&gt;Zina Rakhamilova, StandWithUs at York, campus coordinator,  says use of the word “apartheid” applied to Israel is completely inaccurate.&lt;br/&gt;“The apartheid in South Africa was institutionalized and legalized segregation based on race,” says Rakhamilova.&lt;br/&gt;Rakhamilova cites Arab citizens of Israel who are  members of the supreme court, members of parliament (the Knesset), and leaders of academic institutions.&lt;br/&gt;In fact, Israel is the diametric opposite of South African apartheid’s legal system of oppression and discrimination based on skin color, she adds.&lt;br/&gt;“The leaders of the BDS movement have openly opposed the two-state solution that Israel and most Palestinians seek, and have condemned any aspect of Israeli-Palestinian cooperation.”&lt;br/&gt;“The agenda of this movement does not seek to challenge ideas or foster dialogue – it seeks only to demonize the one state in the Middle East that treats its minorities equally.”&lt;br/&gt;Rakhamilova and Kates challenge BDS activists who, they allege, use the apartheid screen to find ways real ways of helping the Palestinians who are held captive by their corrupt leadership.&lt;br/&gt;“University campuses should be safe places for all students to voice their views,” says Rakhamilova.&lt;br/&gt;“Equating Israel to apartheid South Africa is not only academically dishonest, it is an excuse to demonize the state of Israel and ignore the active terrorist groups that openly call for the destruction of the Jewish state and persecute their own minorities.”&lt;br/&gt;&lt;br/&gt;Ryan Moore, Assistant News Editor</t>
         </is>
+      </c>
+      <c r="L208" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="209">
@@ -9525,10 +10156,13 @@
           <t>University governance, admin, policies, programs, curriculum, Anti-racism, Racist/racialized symbols</t>
         </is>
       </c>
-      <c r="J209" t="inlineStr">
+      <c r="K209" t="inlineStr">
         <is>
           <t>Four New Haven residents were arrested Friday afternoon during a “Change the Name” rally — a final push before the Yale Corporation voted on Saturday to rename Calhoun College.&lt;br/&gt;&lt;br/&gt;The arrests came as part of a demonstration planned by Change the Name Coalition, a group of student and community activists that has held Friday protests since July demanding that Calhoun be renamed. Over 50 New Haven residents and Yale affiliates gathered at the Elm Street corner of the New Haven Green at 3 p.m. to listen to speeches from community activists and students.&lt;br/&gt;&lt;br/&gt;At approximately 3:45 p.m., activists marched across Elm Street with a large banner to block traffic, and demonstrators sat down behind it. The New Haven Police Department issued a verbal warning at 3:53 p.m. Shortly after, officers arrested the four protesters who were barring traffic, citing misdemeanor disorderly conduct.&lt;br/&gt;&lt;br/&gt;The four arrests came less than 24 hours before the University announced it was going to rename Calhoun after Grace Hopper GRD ’34. On the day of the announcement, those involved in the protest expressed happiness with the corporation’s decision to rename the college.&lt;br/&gt;&lt;br/&gt;“I am just really grateful that the Corporation and the [Yale] president stepped up and did the right thing,” said Kica Matos, director of immigrant rights and racial justice at the Center for Community Change.&lt;br/&gt;&lt;br/&gt;Matos was arrested at the protest alongside activists John Lugo, Anna Robinson-Sweet ’11 and Luna Gayeski. Matos previously helped lead other actions with the Change the Name Coalition, including the delivery of a care package to University President Peter Salovey that contained African-American literature and a letter requesting that Calhoun College be renamed.&lt;br/&gt;&lt;br/&gt;Protest organizers did not ask the public to participate in the arrests, instead requesting that they “witness it in power.” Matos explained that she, Lugo, Robinson-Sweet and Gayeski had attended a training beforehand and did not expect others to join them in being arrested. In fact, she said, the coalition coordinated their arrests with the police beforehand, and representatives from the Yale Law School’s National Lawyers Guild Legal Observer Program were present at the demonstration.&lt;br/&gt;&lt;br/&gt;As Gayeski was being arrested, they asked the police officer to loosen their cuffs. The officer immediately complied. The four arrestees were taken to the New Haven Police Station, where they called their lawyer Patricia Kane and were released the same day.&lt;br/&gt;&lt;br/&gt;Matos explained that members of the New Haven community became involved with the push to change Calhoun’s name after Yale dining hall worker Corey Menafee was arrested last summer for breaking a window depicting slavery.&lt;br/&gt;&lt;br/&gt;“This issue unites town and gown. We’ve been working with not just students but with Yale staff and faculty as well,” Matos told the News. “To me, that’s a model of what’s possible.”&lt;br/&gt;&lt;br/&gt;Still, she said credit for the name change must go to student activists, particularly students of color, who have been fighting for the change for years. Lugo, an organizer with Unidad Latina en Acción, echoed Matos and credited student activism for what he described as a victory for the whole New Haven community.&lt;br/&gt;&lt;br/&gt;Matos added that she hopes Saturday’s decision is a sign of the Corporation’s willingness to listen to both student and community voices.&lt;br/&gt;&lt;br/&gt;Those who spoke at the rally talked about the negative impacts of having a building dedicated to a white supremacist such as John C. Calhoun, class of 1804.&lt;br/&gt;&lt;br/&gt;“I want to be treated as a man, and as a young black man walking around New Haven I would appreciate if the Calhoun name was one I did not have to face,” said Justin Farmer, a student activist from Southern Connecticut State University.&lt;br/&gt;&lt;br/&gt;Farmer said Yale must go beyond simply changing the name, however, and do more to honor black history and to increase equity in the Elm City. Other attendees at the rally agreed that changing the name is not enough, citing divestment from fossil fuels and private prisons as additional steps the Yale Corporation should take.&lt;br/&gt;&lt;br/&gt;Though Menafee himself was not present at the protest, local philanthropist Wendy Hamilton read a speech he wrote for it in which he assured protesters he was with them in spirit.&lt;br/&gt;&lt;br/&gt;“Here at Yale we believe in truth and enlightenment,” the speech read. “We are here to lift each other up and set an example for the world to follow. We want the name Calhoun removed from our college and replaced with one that’s prideful and respectable.”</t>
         </is>
+      </c>
+      <c r="L209" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="210">
@@ -9568,10 +10202,13 @@
           <t>University governance, admin, policies, programs, curriculum</t>
         </is>
       </c>
-      <c r="J210" t="inlineStr">
+      <c r="K210" t="inlineStr">
         <is>
           <t>On Friday, March 17th, Associate Dean of Students Nathan Miller informed five students by email that they could face sanctions for a violation of the student code of conduct incurred during their participation in a peaceful protest last month.&lt;br/&gt;The five students are members of the student organization Mountain Justice, which held a sit-in in the office of Chief Investment Officer Mark Amstutz on Feb. 24 after President Smith informed students that the Board of Managers would stand by its decision not to divest, even though students voted on a proposal for partial divestment in a student referendum held earlier in the month.&lt;br/&gt;The Board's response continued a history of rejecting student demands for divestment. In 2013, the college refused to divest from fossil fuels after student protests prompted the Board to consider its position. In March and April of 2015, students staged a one-month long sit-in in the office of Vice President for Finance and Administration Gregory Brown in an effort to persuade the Board of Managers to reconsider divestment. Since then, the college has amended its student code of conduct to prohibit any protest that occurs in offices or disturbs the normal work of the college.&lt;br/&gt;According to the 2017 Student Handbook: "Expressions of dissent are expected in any living and learning community, but this expression must not interfere with normal College business ... Protests are permissible, except in the following locations: classrooms, offices, libraries, dining halls (including cafes), Worth Health Center, residence hall rooms, and lecture halls, ensuring that the normal work, residential experiences, and services of the College can continue. Students who disrupt the functions of the College, including violating the rights of community members and invited speakers to speak, may be subject to the judicial process."&lt;br/&gt;The students each attended a judicial hearing on March 22nd. In a statement published in the Daily Gazette on Monday, Mountain Justice revealed that the administration found the five students guilty of violating the student code of conduct. Initially, the administration had threatened a consequence as severe as fines or probation, but chose to issue the five students warnings instead. In their statement, Mountain Justice presumed that the administration backed down after it was met with student, faculty, and alumni backlash.&lt;br/&gt;At a faculty meeting on March 17th, faculty voted 53-to-9 in support of partial divestment. Following the student citations, 25 faculty members signed an open letter to Miller and Dean of Students Liz Braun outlining their objection to the administration's actions and their support of students' right to nonviolent protest.&lt;br/&gt;"We encourage [students] to think of creative ways to intervene, to raise awareness, to change mindsets, to disrupt systems, or create new ones. We encourage them to not lose faith, or to give up easily.  We encourage them to persist, and they have done so through their persistent calls for divestment from fossil fuels and reinvestment in alternative energy resources," the letter read.&lt;br/&gt;Similarly, more than 650 students and other members of the community have signed a petition urging Miller and Smith to affirm students' right to peaceful protest.&lt;br/&gt;Alumni have also expressed their disapproval with the college's decision not to divest in an op-ed open letter addressed to Smith and Miller. The letter has collected more than 200 signatures.&lt;br/&gt;Several alumni have withheld financial contributions as a result. Some have instead opted to contribute to the Responsible Endowments Fund, an alternate fund established by Mountain Justice to collect funds it will release to the college on the condition that it chooses to divest. Otherwise, the money will be used to finance students in their fight for climate justice, according to the fund's website.&lt;br/&gt;John Braxton '70 explained over email that he will withhold contributions from the college over the issue of the Board's refusal to divest.&lt;br/&gt;"Until Swarthmore divests, I will not make contributions to the college, and I encourage other alumni to join me. I will hold these funds and gladly make a contribution again when the Board of trustees [divests]," Braxton wrote.&lt;br/&gt;Lee Oxenham '72 stopped contributing to the college in 2013 when the college initially refused to engage with the divestment movement. She was further upset to learn that the college disciplined students for their participation in the protest last month.&lt;br/&gt;"I am outraged that the Swarthmore College administration would even consider taking action against nonviolent student protesters on any issue," Oxenham wrote over email.&lt;br/&gt;Peter Meyer '65 was also upset by the college's continued refusal to divest.&lt;br/&gt;"I am embarrassed for Swarthmore every time I [read] an article about divestment that mentions where the movement originated and then notes that the college has not acted," Meyer wrote in an email.&lt;br/&gt;Anne Kapuscinski '76 stated that she and other alumni sent letters to the Board in January asking members to engage in dialogue with students. In an email she sent to the Board on Jan. 23, Kapuscinski expressed her disappointment with the Board's refusal to divest and said that she stopped giving to Swarthmore as a result.&lt;br/&gt;"With tears welling, I said that I would feel morally obligated to stop my annual contributions if Swarthmore continued to avoid divestment. In December 2016, with a truly heavy heart, I did not send an annual contribution to Swarthmore because the leadership had still not committed to a plan to divest," she wrote.&lt;br/&gt;The students cited were dismayed with the college's decision to discipline them rather than engage with them on divestment.&lt;br/&gt;Stephen O'Hanlon '17, one of the students disciplined by the administration, noted his disappointment with the college's response to the protest.&lt;br/&gt;"It's really disappointing that not only is the institution refusing to engage in dialogue on divestment after the students have passed it by such a huge margin ... [but] that they're so unwilling to engage on this that they would rather cite students than sit down and engage in dialogue," O'Hanlon said.&lt;br/&gt;O'Hanlon acknowledged that he and the other protesters cited were in violation of college policy. However, he believed that they have upheld a moral code through their actions.&lt;br/&gt;"We acknowledge that we did take action that was in violation of the code of conduct, but we think that even if we broke that code, we held to a moral code that's grounded in the values of Swarthmore, and in the values that we've been taught in our classes and that we talk about with our peers," O'Hanlon said.&lt;br/&gt;September Porras '20, one of the students who received a warning, noted miscommunications between the Public Safety officers present and the students in Amstutz's office over their violation of the school policy.&lt;br/&gt;"We weren't clearly informed of what the consequences would be," Porras said.&lt;br/&gt;Director of Public Safety Michael Hill said that he informed the students that they were in violation of the student code of conduct in occupying Amstutz's office.&lt;br/&gt;"I gave all of the students who remained a chance to leave the office at that point but again made it clear that if they chose to stay they were violating college policy; I repeated this several times as well as the fact that there could be sanctions," Hill wrote in an email.&lt;br/&gt;O'Hanlon was not sitting in the office when Public Safety took student IDs. He also noted that several students who were in the office during the day were not cited.&lt;br/&gt;"I was never actually asked to leave the office but I was still cited, which seems really perplexing. I had gone into the office a few times to communicate with students but I was never sitting in the office. And there were a number of other students who were in the office throughout the day who also were not cited," O'Hanlon said.&lt;br/&gt;According to Hill, officers took IDs of five students who were either in the office or continued to enter the office.&lt;br/&gt;Lewis Fitzgerald-Holland '18, one of the students cited, said that he was unsure as to why Miller cited five students when there were more than five students in the office throughout the day. Miller could not be reached for comment.&lt;br/&gt;Fitzgerald-Holland believed that the administration targeted O'Hanlon simply because he is a coordinator of Mountain Justice.&lt;br/&gt;"As far as I'm concerned, it's pretty clear that they're going after [O'Hanlon] simply as a student leader, which is just naked political repression. It's not acceptable," Fitzgerald-Holland said.&lt;br/&gt;In response to the backlash, Smith published an op-ed article in the Daily Gazette affirming free speech and peaceful protest as values core to Swarthmore. She explained that the students who sat in Amstutz's office were disrupting his ability to do work and thus were in violation of the student code of conduct.&lt;br/&gt;O'Hanlon said that the students in the office aided Amstutz in completing menial tasks.&lt;br/&gt;"During the sit-in we made sure there weren't too many people in the office so that [Amstutz] couldn't move around and complete his tasks, and his task for the day was shredding papers. The shredding company had big bins in his office already ... He told us that was what he was going to be doing that day, and that we could help if we wanted to, and a number of students who were at the sit-in helped him do shredding and helped him with his tasks that day," O'Hanlon explained.&lt;br/&gt;Amstutz could not be reached for comment.&lt;br/&gt;Porras believed that Smith's tone toward the five students was biased.&lt;br/&gt;"[Smith] said in her op-ed article that several people left the room once they figured out what the consequences were going to be, and five remained, making us sound like five of us were obstinate, rude, and refused to leave and were disrupting what everybody else was going for at the protest, which wasn't true. We were leading the protest, so we very much knew what we were doing," Porras said.&lt;br/&gt;Fitzgerald-Holland noted that Smith's op-ed was published before the five students had been notified of the results of their hearings. The op-ed was published on Thursday, Mar. 23, and the students were informed of the results the following day. Fitzgerald-Holland believed Smith's action was unprofessional.&lt;br/&gt;"The op-ed that Val Smith put out was particularly egregious because as an administrator, she was commenting on a judicial proceeding that had not actually finished, assuming guilt, making numerous factual errors, and in that respect, it was very out of line for an administrator to do from a due process perspective. It's not acceptable in any regard," Fitzgerald-Holland said.&lt;br/&gt;Porras also noted factual inconsistencies in Smith's op-ed. One error involved the number of participants in the protest. Smith wrote that three dozen members of the community participated in the sit-in, but Porras said that this number was higher.&lt;br/&gt;"Over the course of the day, 70 people signed in, which we were very proud of considering we planned this the day before," Porras said.&lt;br/&gt;Fitzgerald-Holland believed Smith's condemnation of the student's actions as violations of college policy is contrary to her personal beliefs in the power of student activism and peaceful protest.&lt;br/&gt;"I think the hardest part for myself and a lot of people right now is seeing Val Smith come out publicly like that and condemn our actions when everything she has said and done in the past - in her inaugural speeches, in her interviews - she has so strongly pushed for this idea that you need to rely on the younger generations to expose moral challenges ... and that's why student protesters and student leaders should be respected, and then here you have Val Smith doing precisely the opposite," he said.&lt;br/&gt;O'Hanlon believed Smith and the administration have contradicted the values on which Swarthmore stands.&lt;br/&gt;"[The administration] betrayed our values as an institution, our generation that's going to be impacted by climate change, and the millions of people who are being threatened by the Trump administration's and the fossil fuel industry's disastrous climate policies. President Smith has a choice about whether she's going to stand up for students, for communities around the world impacted by climate change, and our values as an institution, or if she's going to stand with the board. And we hope that she stands with us," he said.&lt;br/&gt;Fitzgerald-Holland noted the importance of condemning the fossil fuel industry in an age in which many deny the existence of climate change.&lt;br/&gt;"I think it's more urgent than ever that independent institutions like Swarthmore take a stand against the fossil fuel industry when our president doesn't even acknowledge the existence of what I think is probably the greatest moral threat to our generation," he said.&lt;br/&gt;He also affirmed the value of nonconventional forms of protest to producing change.&lt;br/&gt;"Cookie-cutter protests aren't going to get us anywhere if all you're doing is standing at a table, giving people flyers. You're not going to actually pressure powerful organizations to change. Val Smith cannot purport to uphold these values of student leadership and students taking a moral stand and then erase that when those students actually stand up to power in any respect. You can't have it both ways," he said.</t>
         </is>
+      </c>
+      <c r="L210" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="211">
@@ -9611,10 +10248,13 @@
           <t>Economy/inequality, Public funding for higher education</t>
         </is>
       </c>
-      <c r="J211" t="inlineStr">
+      <c r="K211" t="inlineStr">
         <is>
           <t>Students, Professors Wait for Decision After First Tribunal&lt;br/&gt;Eight Concordia Students Charged With Disruptions Call Process “Problematic”&lt;br/&gt;News by Michelle Pucci — Published December 12, 2015 | Updated December 13, 2015 | Comments&lt;br/&gt;Follow @michellempucci&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;The tribunal was for student-protesters who are accused of disrupting classes last semester.  File Photo Shaun Michaud&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Eight of the estimated 24 students accused of disrupting classes during last semester’s strikes are waiting for a decision from a tribunal last week, the latest installment in a process they call “problematic” and “abusive.”&lt;br/&gt;The original charges came after a ripple of anti-austerity protests and student strikes took place in Quebec CEGEPs and universities last spring. &lt;br/&gt;About a month after complaints were filed by professors before the summer break, Concordia agreed to join them as co-complainants. Concordia’s spokesperson Chris Mota said the university became a co-complainant in support of the professors and will support the outcome of the hearings.&lt;br/&gt;Despite hiring multiple mediators to settle the charges informally between students and professors, there are no plans for more efforts of mediation in the future.&lt;br/&gt;“Mediation is voluntary and can take place so long as all parties wish to participate,” spokesperson Chris Mota wrote in an email. “The fact that tribunals took place last week suggests that the mutual interest in continuing mediation was not present.”&lt;br/&gt;The remaining students charged will likely also be called to a tribunal. Students are calling on the university to drop the charges.&lt;br/&gt;“We feel that the university is also responsible in a major way for what happened,” said Aloyse Muller, one of the students involved in the Dec. 2 tribunal. “They’re trying to present themselves like a neutral player when they’re really not.”&lt;br/&gt;The current events stem from spring 2015 anti-austerity protest actions, when more than a dozen student associations and the faculty of fine arts student association voted to strike at least one day of classes last semester. Some associations voted to strike for several weeks.&lt;br/&gt;Concordia’s response was to cancel a day of classes for each department, whose students voted to strike or to participate in city-wide protest, either March 23 or April 2. &lt;br/&gt;On April 1, students enforcing the strike mandate entered a political science class with noise-making machines and chanted until most students walked out. An official complaint under article 29G of the Code of Rights and Responsibilities was filed by the course professor Graham Dodds. Some of the students also face complaints over other pickets from professors Michael Lipson and Travis Smith. &lt;br/&gt;The first tribunal&lt;br/&gt;The eight students presented evidence, personal statements and called forward witnesses at the tribunal last week. The university said respondents were able to request separate hearings.&lt;br/&gt;The Dec. 2 hearing lasted about eight hours, according to two respondents, and coincided with the final week of classes and final assignments. For students in third or fourth year, exams take place in the last weeks of classes and not during the exam period, says Katie Nelson, one of the eight students at the hearing.&lt;br/&gt;“It’s definitely affected my studies and probably the outcome of those classes, because I’ve either had to take time writing statements of evidence or meet with advocacy or go to the tribunal itself which is about seven or eight hours,” she said.&lt;br/&gt;At least two more tribunals are expected, one for each of the professors who filed formal complaints against students, but dates have yet to be announced.&lt;br/&gt;The university department responsible for tribunals avoids scheduling hearings during exam periods or vacation periods and tries to accommodate panelists, the chairperson, complaintants and respondents. This means the next tribunal will likely take place next semester. &lt;br/&gt;“I’m not sure why they thought it was appropriate to schedule such a long tribunal at such an inconvenient time,” Nelson said. “It definitely shows that the university has very little regard to the actual academic work coming out of students and really illustrates the political nature of the tribunal itself.”&lt;br/&gt;There was no testimony by an administrative representative at the Dec. 2 tribunal, according to Nelson. Mota previously told The Link that the university became a co-complainant to provide professors with information from campus security. Nelson said there was a representative from security at the tribunal.&lt;br/&gt;Even if the jury comes back and recommends the lowest charge, a letter of reprimand, Nelson fears her case might be sent to upper administration since this isn’t the first tribunal she’s faced, or the last. &lt;br/&gt;Following last year’s vote for Boycott Divest Sanction (BDS) of Israel by the Concordia Student Union, Nelson, who was campaigning pro-BDS, was accused of harassment and given a letter of reprimand for a different charge. &lt;br/&gt;Now she faces complaints by two professors, Graham Dodds and Michael Lipson, for disrupting classes while carrying out strike mandates to picket political science classes.&lt;br/&gt;Nelson says she is concerned that Lipson acted as an advocate for Dodds and was present at the tribunal.&lt;br/&gt;“He was privy to all the argumentation, all the personal testimony, all the witnesses presented in Dodds’s case, and now essentially has the upper hand,” she said.&lt;br/&gt;Professors Dodds and Smith declined to be interviewed, since the tribunal process is still ongoing. Lipson did not respond to a request for comment.&lt;br/&gt;Nelson called the tribunal process, a lack of communication and delays in scheduling “legally problematic” and “psychologically abusive,” and hopes the tribunals don’t move on.&lt;br/&gt;“The university should be preparing for the ramifications and consequences of doing that to its students,” she said, promising to look into civil litigation.&lt;br/&gt;Unsuccessful mediations&lt;br/&gt;Mediation, which was touted as a possible venue for resolution of the complaints, doesn’t seem to be a possibility for students and professors anymore.&lt;br/&gt;Concordia began a mediation process in the fall to encourage an informal compromise between professors and students. The first attempt began in early October, but seemingly ended without an agreement.&lt;br/&gt;All participants signed a nondisclosure agreement, which prevented them from speaking with media.&lt;br/&gt;One student has agreed to a mediated settlement, but the terms of the agreement are still unknown. Some other students have had their charges dropped because they were not directly involved in disrupting the classes of the complainants.&lt;br/&gt;About a month later, another round of mediation sessions were organized with new mediators—but the tribunal date had already been set.&lt;br/&gt;“That’s something I found problematic, to have the tribunal at the same time as the mediation—especially a few days before finals,” said Aloyse Muller, one of the students being charged.&lt;br/&gt;An administrative representative was noticeably lacking in all the meetings set up with the purpose of mediation over the semester.&lt;br/&gt;“I have to give it to Concordia, you know, a ‘real education for the real world,’” said Muller, citing the university’s old motto.&lt;br/&gt;“I’ve learned a lot about what’s the mediation process, what’s the problem of having a nine-hour discussion when you have to take caucuses all the time,” he said. “Real education, real helpful, probably better than some of my classes this term.”&lt;br/&gt;Correction: A previous version of this story stated Katie Nelson was charged with harassment. She was accused of harassment, but received a letter of reprimand for a different charge. The Link regrets the error.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;By commenting on this page you agree to the terms of our Comments Policy.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Please enable JavaScript to view the comments powered by Disqus.&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Related Reading&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;First Tribunal for Student-Protesters Set for Dec. 2&lt;br/&gt;Jonathan Caragay-Cook&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Opinions&lt;br/&gt;Editorial: These Student-Protester Tribunals Are Just for Show&lt;br/&gt;The Link&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;News&lt;br/&gt;Concordia Student-Protester Tribunals Suspended&lt;br/&gt;Jonathan Caragay-Cook&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;Opinions&lt;br/&gt;Editorial: Make P-6 an Election Issue&lt;br/&gt;The Link</t>
         </is>
+      </c>
+      <c r="L211" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="212">
@@ -9656,10 +10296,13 @@
           <t>Economy/inequality, Public funding for higher education, Social services and welfare, Labor and work</t>
         </is>
       </c>
-      <c r="J212" t="inlineStr">
+      <c r="K212" t="inlineStr">
         <is>
           <t>Tens of thousands of people assembled on McGill College last Friday to protest the Liberal government’s austerity measures, which include severe cuts to education and healthcare. Undeterred by the fact that the demonstration was swiftly declared illegal by the police, demonstrators marched for over two and a half hours, making their way down Ste. Catherine and to Montreal’s Old Port, where the demonstration eventually dispersed.&lt;br/&gt;“It’s important to be here because austerity cuts are affecting everyone in Quebec, students included,” Kelly, a Women’s Studies student at McGill, told The Daily. “Over $200 million has been cut from university funding from the province, and that translates to over $14 million being cut at McGill.”&lt;br/&gt;Organized by a large coalition that includes the Association pour une solidarité syndicale étudiante (ASSÉ), the event drew thousands of students. Buses from CEGEPs and universities were observed picking up protesters at the demonstration’s termination point.&lt;br/&gt;“It was great seeing […] 50,000 people out on the streets,” ASSÉ co-spokesperson Camille Godbout told The Daily. “It was great to see all the groups mobilizing against the austerity cuts. We have today 82,000 students on strike across the province so [it was good] seeing other groups, unions, and community groups coming down to Montreal.”&lt;br/&gt;“It’s important to be here because austerity cuts are affecting everyone in Quebec, students included.”&lt;br/&gt;“The province, as far as I know, didn’t consult people before putting this budget forward,” said Kelly. “They didn’t give people in Quebec a choice about it, that’s why everyone’s angry about it and coming to resist and show the province that this is not the way to do things.”&lt;br/&gt;Kelly was part of a small McGill contingent of around twenty students. A larger contingent from Concordia, numbering around 100 students, was also present.&lt;br/&gt;“We [at the Concordia Graduate Students’ Association (GSA)] do have a mandate, actually, to support free education,” GSA VP External Mohammad Jawad Khan told The Daily. “So I believe right now is not the right time to [make] budget cuts [for] the university and the government. Unfortunately, Concordia has wholeheartedly accepted them.”&lt;br/&gt;Christian, a demonstrator, called the austerity measures anti-democratic. “Austerity measures are a cut at the level of social democracy,” he said. “It is not only a divestment in the [form] of money in the strictest sense, but a divestment [from] the [social] capital.”&lt;br/&gt;“[Instead of the democratic process] right now, it is the IMF [International Monetary Fund] and international banks who are [driving] national economies,” Christian noted.&lt;br/&gt;Although the protest had been declared illegal, police intervention was minimal. Contingents of officers in riot gear walked with the crowd, and a number of officers on bicycles escorted the demonstration. Demonstrators were observed conversing and interacting with the officers at the scene.&lt;br/&gt;Godbout suggested that the lighter-than-usual police presence was a product of the demonstration’s opposition to the controversial Bill 3, which would require higher contributions to the pension fund for many police officers and other public service employees in Quebec.&lt;br/&gt;“We stand in solidarity with all the workers who are touched right now by the [changes in the] pensions. Clearly we still stand against police brutality, but maybe [the pensions have] something to do with the fact that [the police] acted more lightly than usual,” she said.&lt;br/&gt;Indeed, a group of several hundred firefighters representing the Association des pompiers de Montréal (ADPM) participated in the protest. The ADPM made headlines in August when a group of its members disturbed a City of Montreal council meeting in protest of Bill 3. Six firefighters were fired and dozens more suspended following the incident.&lt;br/&gt;In order to emphasize their dissatisfaction with the government’s policies, hundreds of protesters took to the streets again on Friday night following the main demonstration. This time, several arrests were made.&lt;br/&gt;A collective organization committee called the “Comité large printemps 2015” has also been formed, through which students and workers will continue to organize and escalate pressure tactics, potentially leading up to a strike.&lt;br/&gt;“History in Quebec has shown that past strikes have been really effective in getting the government to change what they’re doing,” said Kelly.&lt;br/&gt;[flickr id=”72157649081364165″]</t>
         </is>
+      </c>
+      <c r="L212" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="213">
@@ -9699,10 +10342,13 @@
           <t>Economy/inequality, Public funding for higher education, Social services and welfare</t>
         </is>
       </c>
-      <c r="J213" t="inlineStr">
+      <c r="K213" t="inlineStr">
         <is>
           <t>Tens of thousands of people assembled on McGill College last Friday to protest the Liberal government’s austerity measures, which include severe cuts to education and healthcare. Undeterred by the fact that the demonstration was swiftly declared illegal by the police, demonstrators marched for over two and a half hours, making their way down Ste. Catherine and to Montreal’s Old Port, where the demonstration eventually dispersed.&lt;br/&gt;“It’s important to be here because austerity cuts are affecting everyone in Quebec, students included,” Kelly, a Women’s Studies student at McGill, told The Daily. “Over $200 million has been cut from university funding from the province, and that translates to over $14 million being cut at McGill.”&lt;br/&gt;Organized by a large coalition that includes the Association pour une solidarité syndicale étudiante (ASSÉ), the event drew thousands of students. Buses from CEGEPs and universities were observed picking up protesters at the demonstration’s termination point.&lt;br/&gt;“It was great seeing […] 50,000 people out on the streets,” ASSÉ co-spokesperson Camille Godbout told The Daily. “It was great to see all the groups mobilizing against the austerity cuts. We have today 82,000 students on strike across the province so [it was good] seeing other groups, unions, and community groups coming down to Montreal.”&lt;br/&gt;“It’s important to be here because austerity cuts are affecting everyone in Quebec, students included.”&lt;br/&gt;“The province, as far as I know, didn’t consult people before putting this budget forward,” said Kelly. “They didn’t give people in Quebec a choice about it, that’s why everyone’s angry about it and coming to resist and show the province that this is not the way to do things.”&lt;br/&gt;Kelly was part of a small McGill contingent of around twenty students. A larger contingent from Concordia, numbering around 100 students, was also present.&lt;br/&gt;“We [at the Concordia Graduate Students’ Association (GSA)] do have a mandate, actually, to support free education,” GSA VP External Mohammad Jawad Khan told The Daily. “So I believe right now is not the right time to [make] budget cuts [for] the university and the government. Unfortunately, Concordia has wholeheartedly accepted them.”&lt;br/&gt;Christian, a demonstrator, called the austerity measures anti-democratic. “Austerity measures are a cut at the level of social democracy,” he said. “It is not only a divestment in the [form] of money in the strictest sense, but a divestment [from] the [social] capital.”&lt;br/&gt;“[Instead of the democratic process] right now, it is the IMF [International Monetary Fund] and international banks who are [driving] national economies,” Christian noted.&lt;br/&gt;Although the protest had been declared illegal, police intervention was minimal. Contingents of officers in riot gear walked with the crowd, and a number of officers on bicycles escorted the demonstration. Demonstrators were observed conversing and interacting with the officers at the scene.&lt;br/&gt;Godbout suggested that the lighter-than-usual police presence was a product of the demonstration’s opposition to the controversial Bill 3, which would require higher contributions to the pension fund for many police officers and other public service employees in Quebec.&lt;br/&gt;“We stand in solidarity with all the workers who are touched right now by the [changes in the] pensions. Clearly we still stand against police brutality, but maybe [the pensions have] something to do with the fact that [the police] acted more lightly than usual,” she said.&lt;br/&gt;Indeed, a group of several hundred firefighters representing the Association des pompiers de Montréal (ADPM) participated in the protest. The ADPM made headlines in August when a group of its members disturbed a City of Montreal council meeting in protest of Bill 3. Six firefighters were fired and dozens more suspended following the incident.&lt;br/&gt;In order to emphasize their dissatisfaction with the government’s policies, hundreds of protesters took to the streets again on Friday night following the main demonstration. This time, several arrests were made.&lt;br/&gt;A collective organization committee called the “Comité large printemps 2015” has also been formed, through which students and workers will continue to organize and escalate pressure tactics, potentially leading up to a strike.&lt;br/&gt;“History in Quebec has shown that past strikes have been really effective in getting the government to change what they’re doing,” said Kelly.&lt;br/&gt;[flickr id=”72157649081364165″]</t>
         </is>
+      </c>
+      <c r="L213" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="214">
@@ -9742,10 +10388,13 @@
           <t>Racist/racialized symbols</t>
         </is>
       </c>
-      <c r="J214" t="inlineStr">
+      <c r="K214" t="inlineStr">
         <is>
           <t>Four New Haven residents were arrested Friday afternoon during a “Change the Name” rally — a final push before the Yale Corporation voted on Saturday to rename Calhoun College.&lt;br/&gt;&lt;br/&gt;The arrests came as part of a demonstration planned by Change the Name Coalition, a group of student and community activists that has held Friday protests since July demanding that Calhoun be renamed. Over 50 New Haven residents and Yale affiliates gathered at the Elm Street corner of the New Haven Green at 3 p.m. to listen to speeches from community activists and students.&lt;br/&gt;&lt;br/&gt;At approximately 3:45 p.m., activists marched across Elm Street with a large banner to block traffic, and demonstrators sat down behind it. The New Haven Police Department issued a verbal warning at 3:53 p.m. Shortly after, officers arrested the four protesters who were barring traffic, citing misdemeanor disorderly conduct.&lt;br/&gt;&lt;br/&gt;The four arrests came less than 24 hours before the University announced it was going to rename Calhoun after Grace Hopper GRD ’34. On the day of the announcement, those involved in the protest expressed happiness with the corporation’s decision to rename the college.&lt;br/&gt;&lt;br/&gt;“I am just really grateful that the Corporation and the [Yale] president stepped up and did the right thing,” said Kica Matos, director of immigrant rights and racial justice at the Center for Community Change.&lt;br/&gt;&lt;br/&gt;Matos was arrested at the protest alongside activists John Lugo, Anna Robinson-Sweet ’11 and Luna Gayeski. Matos previously helped lead other actions with the Change the Name Coalition, including the delivery of a care package to University President Peter Salovey that contained African-American literature and a letter requesting that Calhoun College be renamed.&lt;br/&gt;&lt;br/&gt;Protest organizers did not ask the public to participate in the arrests, instead requesting that they “witness it in power.” Matos explained that she, Lugo, Robinson-Sweet and Gayeski had attended a training beforehand and did not expect others to join them in being arrested. In fact, she said, the coalition coordinated their arrests with the police beforehand, and representatives from the Yale Law School’s National Lawyers Guild Legal Observer Program were present at the demonstration.&lt;br/&gt;&lt;br/&gt;As Gayeski was being arrested, they asked the police officer to loosen their cuffs. The officer immediately complied. The four arrestees were taken to the New Haven Police Station, where they called their lawyer Patricia Kane and were released the same day.&lt;br/&gt;&lt;br/&gt;Matos explained that members of the New Haven community became involved with the push to change Calhoun’s name after Yale dining hall worker Corey Menafee was arrested last summer for breaking a window depicting slavery.&lt;br/&gt;&lt;br/&gt;“This issue unites town and gown. We’ve been working with not just students but with Yale staff and faculty as well,” Matos told the News. “To me, that’s a model of what’s possible.”&lt;br/&gt;&lt;br/&gt;Still, she said credit for the name change must go to student activists, particularly students of color, who have been fighting for the change for years. Lugo, an organizer with Unidad Latina en Acción, echoed Matos and credited student activism for what he described as a victory for the whole New Haven community.&lt;br/&gt;&lt;br/&gt;Matos added that she hopes Saturday’s decision is a sign of the Corporation’s willingness to listen to both student and community voices.&lt;br/&gt;&lt;br/&gt;Those who spoke at the rally talked about the negative impacts of having a building dedicated to a white supremacist such as John C. Calhoun, class of 1804.&lt;br/&gt;&lt;br/&gt;“I want to be treated as a man, and as a young black man walking around New Haven I would appreciate if the Calhoun name was one I did not have to face,” said Justin Farmer, a student activist from Southern Connecticut State University.&lt;br/&gt;&lt;br/&gt;Farmer said Yale must go beyond simply changing the name, however, and do more to honor black history and to increase equity in the Elm City. Other attendees at the rally agreed that changing the name is not enough, citing divestment from fossil fuels and private prisons as additional steps the Yale Corporation should take.&lt;br/&gt;&lt;br/&gt;Though Menafee himself was not present at the protest, local philanthropist Wendy Hamilton read a speech he wrote for it in which he assured protesters he was with them in spirit.&lt;br/&gt;&lt;br/&gt;“Here at Yale we believe in truth and enlightenment,” the speech read. “We are here to lift each other up and set an example for the world to follow. We want the name Calhoun removed from our college and replaced with one that’s prideful and respectable.”</t>
         </is>
+      </c>
+      <c r="L214" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>